<commit_message>
added game links to the xref file. checked for missing enumeration descriptions. fixed some.
</commit_message>
<xml_diff>
--- a/src/game_params.xlsx
+++ b/src/game_params.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Activity_Data\Mancala_github\MancalaGames\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E699764B-ED80-4D43-9A59-AD66382EE6CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{803B3D97-FAD9-4625-8A15-2EEE6F94FB4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29955" yWindow="1875" windowWidth="29040" windowHeight="16200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="game_params" sheetId="1" r:id="rId1"/>
@@ -645,14 +645,6 @@
     <t>Number of end games played out from each leaf node created. One value for each difficulty level (0-3).</t>
   </si>
   <si>
-    <t>Allows specifing non-all-equal start patterns. Four patterns are supported:
-GAMACHA: starting from the third hold (from start player's left) place nbr_seeds in every other hole, the first move is prescribed move the center hole's seeds to the other side (this is done automatically).
-ALTERNATES: everyother hole is filled with nbr_seeds, no seeds end up opposite eachother. If a player has fewer seeds than their opponent, then they start.
-ALTS_WITH_1: like Alternates except the starter's 2nd from right hole with nbr_seeds is replaced with one seed.
-CLIPPEDTRIPLES: pattern of 0 S S (where S is nbr_seeds) is used to fill the holes; if a full cycle of 3 cannot be placed, the holes are left empty. The True and False sides are the same from the player's perspective, e.g. they will look reversed when viewed from one side of the game board.
-TWOEMPTY: all but the rightmost two holes for each player are filled with is nbr_seeds.</t>
-  </si>
-  <si>
     <t>child_cvt</t>
   </si>
   <si>
@@ -817,15 +809,6 @@
     <t>NONE: no additional restrictions.
 OPP_ONLY:  Only make children on the opposite side or in opponent's territory.
 NOT_1ST_OPP: Don't make a child in the first hole on the opponents side/territory with one seed.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Games with children allow players to claim holes. These child holes are an extension of the stores and seeds in them count towards a win. Making a child stops any multiple lap sowing, moves cannot start from children, and they cannot be captured.
-NORMAL: no special child rules
-WALDAS: Stores are not supported. Captures are instead moved into waldas, thus a player may not capture until they have created a walda. Child locations are limited.  Each player may create up to 6 waldas: on either end of each side of the board and the next outer hole on their own side of the board. Note that there are only 8 total places that waldas maybe created.
-ONE_CHILD: Use the tuzdek rules for children: only one child allowed on own side of the board, may not be in player's left most hole,  and may not be opposite eachother.
-WEG: children maybe created in holes owned by the opponent. Ending a sow in an opponent's weg captures the seed just sown and one more (if there is one); the player get's to play again.
-BULL: create one bull if final seed sows to CHILD_CVT, create two bulls if the final two seeds are sown to CHILD_CVT-1 and CHILD_CVT (in either order).
-</t>
   </si>
   <si>
     <t>nocaptfirst</t>
@@ -867,13 +850,6 @@
 Multi lap with multiple captures: capture when last hole sown is followed by an empty hole which is then followed by an occupied hole. Continue captures as long as the pattern of empty hole followed by an occupied hole continues.
 xxx_SOW_CAPT_ALL does not do this capture.
 OPPSIDECAPT, EVENS, CAPT_MAX, CAPT_MIN, and CAPT_ON apply only to an optional xxx_SOW_CAPT_ALL and not the final capture.</t>
-  </si>
-  <si>
-    <t>BASIC_SOWER: the first sow follows general rules of single lap sowing.  Other sow parameters will be enacted  afterward.
-MLAPS_SOWER: the first sow follows general rules of multi-lap sowing. Other sow parameters will be enacted  afterward.
-SOW1OPP: at least one seed must be sown on the opponents side of the board accomplished by sowing as normal until the final seed, then any remaining holes on the player side are skipped and the
-PLUS1MINUS1: proceed from the selected hole by moving one seed from the next hole into the following hole, next skip that hole and repeat moving seed forward. After cycling the board, capture across from the opening hole.
-ARNGE_LIMIT: the first move may be used to rearrange the seeds (opponent is same layout). If the first move is not used for rearrangement, captures and child creation are not allowed from the starter until the second player makes a child or captures.</t>
   </si>
   <si>
     <t>NOT_APPLICABLE</t>
@@ -890,18 +866,14 @@
 UMOVE: allow the loser to choose where seeds are placed. At least one seed must be placed in each hole, remaining seeds are placed in the store. The winner's layout is the same layout but reflected.</t>
   </si>
   <si>
-    <t>SOW_BLKD_DIV: Holes sown to GPARAM_ONE are closed (blocked) and the hole's seeds are removed from play. Blocked holes on own side are skipped when sowing and blocked holes on opp side are diverted out of play or captured. 
-SOW_BLKD_DIV_NR: SOW_BLKD_DIV except that each player's rightmost hole cannot be closed.
-OWN_SOW_CAPT_ALL: Capture all holes that are sown that meet the simple capture criteria: evens, min, max and  capture on. Other criteria are enforced: side of the board, unlocked, and not child.   Grand Slam rules are not applied. If the game goal TERRITORY the capturer is the hole owner; otherwise the capturer is done by side. NOCAPTFIRST prevents this capture for the first move.
-SOW_SOW_CAPT_ALL: Capture all holes that sown that meed the simple capture criteria only on the SOWER's side of the board. NOCAPTFIRST prevents this capture for the first move.
-NO_SOW_OPP_2S: Don't sow into opponents holes with 2 seeds.</t>
-  </si>
-  <si>
     <t>Defines which player starts 2nd and subsequent rounds:
 - ALTERNATE: the round starter alternates.
 - LOSER: the loser of the previous round starts the current round.
 - WINNER: the winner of the previous round starts the current round.
 - LAST_MOVER: the player that made the last move of the previous round, starts the new round.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Moves maybe made from any hole, independent of the side of the board. Moves need specify side, position and directions.  </t>
   </si>
   <si>
     <t>Allow rules limit the holes from which moves may start.  Disallowed holes are not selectable.
@@ -912,10 +884,44 @@
 SINGLE_ALL_TO_ZERO: Holes with single seeds may only be played if all holes contain single seeds and then only if the next hole is empty.
 TWO_ONLY_ALL: Holes with two seeds may only be played if all holes contain two seeds.
 TWO_ONLY_ALL_RIGHT: Holes with two seeds may not be played, unless all holes contains two seeds, in which case the rightmost hole must be played.
-FIRST_TURN_ONLY_RIGHT_TWO: The first turn must start from one of the two rightmost holes.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Moves maybe made from any hole, independent of the side of the board. Moves need specify side, position and directions.  </t>
+FIRST_TURN_ONLY_RIGHT_TWO: The first turn must start from one of the two rightmost holes.
+RIGHT_2_1ST_THEN_ALL_TWO:  The first turn must start from one of the two rightmost holes. Subsequent moves may only start from holes without 2 seeds, unless all holes contain zero or 2 seeds.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Games with children allow players to claim holes. These child holes are an extension of the stores and seeds in them count towards a win. Making a child stops any multiple lap sowing, moves cannot start from children, and they cannot be captured.
+NOCHILD: children are not used.
+NORMAL: no special child rules.
+WALDAS: Stores are not supported. Captures are instead moved into waldas, thus a player may not capture until they have created a walda. Child locations are limited.  Each player may create up to 6 waldas: on either end of each side of the board and the next outer hole on their own side of the board. Note that there are only 8 total places that waldas maybe created.
+ONE_CHILD: Use the tuzdek rules for children: only one child allowed on own side of the board, may not be in player's left most hole,  and may not be opposite eachother.
+WEG: children maybe created in holes owned by the opponent. Ending a sow in an opponent's weg captures the seed just sown and one more (if there is one); the player get's to play again.
+BULL: create one bull if final seed sows to CHILD_CVT, create two bulls if the final two seeds are sown to CHILD_CVT-1 and CHILD_CVT (in either order).
+</t>
+  </si>
+  <si>
+    <t>NONE: there is no prescribed opening move.
+BASIC_SOWER: the first sow follows general rules of single lap sowing.  Other sow parameters will be enacted  afterward.
+MLAPS_SOWER: the first sow follows general rules of multi-lap sowing. Other sow parameters will be enacted  afterward.
+SOW1OPP: at least one seed must be sown on the opponents side of the board accomplished by sowing as normal until the final seed, then any remaining holes on the player side are skipped and the
+PLUS1MINUS1: proceed from the selected hole by moving one seed from the next hole into the following hole, next skip that hole and repeat moving seed forward. After cycling the board, capture across from the opening hole.
+ARNGE_LIMIT: the first move may be used to rearrange the seeds (opponent is same layout). If the first move is not used for rearrangement, captures and child creation are not allowed from the starter until the second player makes a child or captures.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NONE: there is no special sowing rules.
+SOW_BLKD_DIV: Holes sown to GPARAM_ONE are closed (blocked) and the hole's seeds are removed from play. Blocked holes on own side are skipped when sowing and blocked holes on opp side are diverted out of play or captured. 
+SOW_BLKD_DIV_NR: SOW_BLKD_DIV except that each player's rightmost hole cannot be closed.
+OWN_SOW_CAPT_ALL: Capture all holes that are sown that meet the simple capture criteria: evens, min, max and  capture on. Other criteria are enforced: side of the board, unlocked, and not child.   Grand Slam rules are not applied. If the game goal TERRITORY the capturer is the hole owner; otherwise the capturer is done by side. NOCAPTFIRST prevents this capture for the first move.
+SOW_SOW_CAPT_ALL: Capture all holes that sown that meed the simple capture criteria only on the SOWER's side of the board. NOCAPTFIRST prevents this capture for the first move.
+NO_SOW_OPP_2S: Don't sow into opponents holes with 2 seeds.
+</t>
+  </si>
+  <si>
+    <t>Allows specifing non-all-equal start patterns. Four patterns are supported:
+ALL_EQUAL: all holes start with the same number of seeds.
+GAMACHA: starting from the third hold (from start player's left) place nbr_seeds in every other hole, the first move is prescribed move the center hole's seeds to the other side (this is done automatically).
+ALTERNATES: everyother hole is filled with nbr_seeds, no seeds end up opposite eachother. If a player has fewer seeds than their opponent, then they start.
+ALTS_WITH_1: like Alternates except the starter's 2nd from right hole with nbr_seeds is replaced with one seed.
+CLIPPEDTRIPLES: pattern of 0 S S (where S is nbr_seeds) is used to fill the holes; if a full cycle of 3 cannot be placed, the holes are left empty. The True and False sides are the same from the player's perspective, e.g. they will look reversed when viewed from one side of the game board.
+TWOEMPTY: all but the rightmost two holes for each player are filled with is nbr_seeds.</t>
   </si>
 </sst>
 </file>
@@ -1801,7 +1807,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K1" sqref="K1:K1048576"/>
+      <selection pane="bottomLeft" activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1832,7 +1838,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>4</v>
@@ -1914,15 +1920,15 @@
         <v>171</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="285" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="345" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>69</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>204</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>205</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>24</v>
@@ -1931,10 +1937,10 @@
         <v>14</v>
       </c>
       <c r="F4" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="G4" s="5" t="s">
         <v>206</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>207</v>
       </c>
       <c r="H4" s="3">
         <v>3</v>
@@ -1943,7 +1949,7 @@
         <v>0</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -2071,7 +2077,7 @@
         <v>0</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -2103,7 +2109,7 @@
         <v>0</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -2135,7 +2141,7 @@
         <v>0</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -2143,10 +2149,10 @@
         <v>106</v>
       </c>
       <c r="B11" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>221</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>222</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>24</v>
@@ -2167,7 +2173,7 @@
         <v>0</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="210" x14ac:dyDescent="0.25">
@@ -2199,7 +2205,7 @@
         <v>0</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -2231,7 +2237,7 @@
         <v>2</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -2239,10 +2245,10 @@
         <v>106</v>
       </c>
       <c r="B14" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>234</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>235</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>24</v>
@@ -2263,7 +2269,7 @@
         <v>2</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="105" x14ac:dyDescent="0.25">
@@ -2399,10 +2405,10 @@
         <v>106</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>24</v>
@@ -2423,7 +2429,7 @@
         <v>2</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2455,7 +2461,7 @@
         <v>2</v>
       </c>
       <c r="J20" s="4" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2463,10 +2469,10 @@
         <v>106</v>
       </c>
       <c r="B21" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="C21" s="3" t="s">
         <v>218</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>219</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>24</v>
@@ -2487,7 +2493,7 @@
         <v>2</v>
       </c>
       <c r="J21" s="4" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -2495,10 +2501,10 @@
         <v>106</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>24</v>
@@ -2507,10 +2513,10 @@
         <v>59</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="H22" s="3">
         <v>10</v>
@@ -2519,7 +2525,7 @@
         <v>2</v>
       </c>
       <c r="J22" s="4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2647,7 +2653,7 @@
         <v>0</v>
       </c>
       <c r="J26" s="4" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="330" x14ac:dyDescent="0.25">
@@ -2655,10 +2661,10 @@
         <v>42</v>
       </c>
       <c r="B27" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="C27" s="3" t="s">
         <v>237</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>238</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>24</v>
@@ -2667,10 +2673,10 @@
         <v>62</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="H27" s="3">
         <v>6</v>
@@ -2679,7 +2685,7 @@
         <v>0</v>
       </c>
       <c r="J27" s="4" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="105" x14ac:dyDescent="0.25">
@@ -2711,7 +2717,7 @@
         <v>0</v>
       </c>
       <c r="J28" s="4" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="120" x14ac:dyDescent="0.25">
@@ -2775,10 +2781,10 @@
         <v>2</v>
       </c>
       <c r="J30" s="4" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" ht="270" x14ac:dyDescent="0.25">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" ht="285" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>42</v>
       </c>
@@ -2807,18 +2813,18 @@
         <v>2</v>
       </c>
       <c r="J31" s="4" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" ht="240" x14ac:dyDescent="0.25">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" ht="255" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>42</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D32" s="3" t="s">
         <v>24</v>
@@ -2827,10 +2833,10 @@
         <v>60</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="G32" s="5" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="H32" s="3">
         <v>3</v>
@@ -2839,7 +2845,7 @@
         <v>2</v>
       </c>
       <c r="J32" s="4" t="s">
-        <v>259</v>
+        <v>263</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -2847,10 +2853,10 @@
         <v>42</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D33" s="3" t="s">
         <v>24</v>
@@ -2871,7 +2877,7 @@
         <v>2</v>
       </c>
       <c r="J33" s="4" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
@@ -3095,7 +3101,7 @@
         <v>0</v>
       </c>
       <c r="J40" s="4" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="41" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3135,10 +3141,10 @@
         <v>142</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D42" s="3" t="s">
         <v>162</v>
@@ -3159,7 +3165,7 @@
         <v>0</v>
       </c>
       <c r="J42" s="4" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="43" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3551,7 +3557,7 @@
         <v>9</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D55" s="3" t="s">
         <v>24</v>
@@ -3569,7 +3575,7 @@
         <v>0</v>
       </c>
       <c r="J55" s="4" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="56" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3642,7 +3648,7 @@
         <v>0</v>
       </c>
       <c r="J58" s="4" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="59" spans="1:10" ht="105" x14ac:dyDescent="0.25">
@@ -3805,15 +3811,15 @@
         <v>86</v>
       </c>
     </row>
-    <row r="64" spans="1:10" ht="255" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" ht="285" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
         <v>76</v>
       </c>
       <c r="B64" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="C64" s="3" t="s">
         <v>227</v>
-      </c>
-      <c r="C64" s="3" t="s">
-        <v>228</v>
       </c>
       <c r="D64" s="3" t="s">
         <v>24</v>
@@ -3822,10 +3828,10 @@
         <v>70</v>
       </c>
       <c r="F64" s="3" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="G64" s="5" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="H64" s="3">
         <v>6</v>
@@ -3834,7 +3840,7 @@
         <v>0</v>
       </c>
       <c r="J64" s="4" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
     </row>
     <row r="65" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -3886,10 +3892,10 @@
         <v>44</v>
       </c>
       <c r="F66" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="G66" s="5" t="s">
         <v>210</v>
-      </c>
-      <c r="G66" s="5" t="s">
-        <v>211</v>
       </c>
       <c r="H66" s="3">
         <v>0</v>
@@ -3898,7 +3904,7 @@
         <v>2</v>
       </c>
       <c r="J66" s="8" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="67" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3933,15 +3939,15 @@
         <v>99</v>
       </c>
     </row>
-    <row r="68" spans="1:10" ht="315" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" ht="330" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
         <v>76</v>
       </c>
       <c r="B68" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="C68" s="3" t="s">
         <v>199</v>
-      </c>
-      <c r="C68" s="3" t="s">
-        <v>200</v>
       </c>
       <c r="D68" s="3" t="s">
         <v>24</v>
@@ -3950,10 +3956,10 @@
         <v>27</v>
       </c>
       <c r="F68" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G68" s="5" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="H68" s="3">
         <v>3</v>
@@ -3962,7 +3968,7 @@
         <v>2</v>
       </c>
       <c r="J68" s="4" t="s">
-        <v>248</v>
+        <v>262</v>
       </c>
     </row>
     <row r="69" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3970,10 +3976,10 @@
         <v>76</v>
       </c>
       <c r="B69" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="C69" s="3" t="s">
         <v>197</v>
-      </c>
-      <c r="C69" s="3" t="s">
-        <v>198</v>
       </c>
       <c r="D69" s="3" t="s">
         <v>24</v>
@@ -3994,7 +4000,7 @@
         <v>2</v>
       </c>
       <c r="J69" s="4" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="70" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -4002,22 +4008,22 @@
         <v>76</v>
       </c>
       <c r="B70" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="C70" s="3" t="s">
         <v>244</v>
       </c>
-      <c r="C70" s="3" t="s">
+      <c r="D70" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E70" s="3">
+        <v>24</v>
+      </c>
+      <c r="F70" s="3" t="s">
         <v>245</v>
       </c>
-      <c r="D70" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E70" s="3">
-        <v>24</v>
-      </c>
-      <c r="F70" s="3" t="s">
-        <v>246</v>
-      </c>
       <c r="G70" s="3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="H70" s="3">
         <v>5</v>
@@ -4026,7 +4032,7 @@
         <v>2</v>
       </c>
       <c r="J70" s="4" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Test coverage for new_game.py to 100%
</commit_message>
<xml_diff>
--- a/src/game_params.xlsx
+++ b/src/game_params.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Activity_Data\Mancala_github\MancalaGames\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{803B3D97-FAD9-4625-8A15-2EEE6F94FB4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{766CBC3E-FC5B-40D0-89AD-A69CB3E7FB5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -530,12 +530,6 @@
     <t>The default difficulty. Can be changed at play time, even during game play, in the Mancala UI.</t>
   </si>
   <si>
-    <t>The overall goal of the game. Defines how a player wins.
-MAX_SEEDS: player with the maximum number of seeds at the end of the game wins or they collect more than half of the total seeds
-DEPRIVE: eliminate all of your opponents seeds.
-TERRITORY: claim ownership of holes. Each round the ownership of holes is determined by the number of seeds captured in the previous round.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Sow counter-clockwise.
 Capture on evens. </t>
   </si>
@@ -853,17 +847,6 @@
   </si>
   <si>
     <t>NOT_APPLICABLE</t>
-  </si>
-  <si>
-    <t>Choose how holes are filled when a new round strarts:
-NOT_APPLICABLE: round fill doesn't need to be specified: either not played in rounds or game goal is TERRITORY (all holes filled).
-LEFT_FILL: fill holes from the player's left.
-RIGHT_FILL: fill holes from the player's right. 
-OUTSIDE_FILL: fill holes from the outside ends toward the middle.
-EVEN_FILL: fill both sides with the same number of seeds per hole, determined by dividing the losers seeds by the number of holes per side. If that is not playable base on minimum move, extra seeds are put in each players leftmost hole. Any extra seeds are put in each player's store.
-SHORTEN: shorten the board so that all of the loser's holes are filled; the winner will have more seeds in their store but the same board arrangement. If the game uses children, they will not be created if the board size is reduced to 3 or less.
-UCHOOSE: allow user to choose which holes have seeds (are not blocked) when ROUNDS with BLOCKS are used.
-UMOVE: allow the loser to choose where seeds are placed. At least one seed must be placed in each hole, remaining seeds are placed in the store. The winner's layout is the same layout but reflected.</t>
   </si>
   <si>
     <t>Defines which player starts 2nd and subsequent rounds:
@@ -922,6 +905,24 @@
 ALTS_WITH_1: like Alternates except the starter's 2nd from right hole with nbr_seeds is replaced with one seed.
 CLIPPEDTRIPLES: pattern of 0 S S (where S is nbr_seeds) is used to fill the holes; if a full cycle of 3 cannot be placed, the holes are left empty. The True and False sides are the same from the player's perspective, e.g. they will look reversed when viewed from one side of the game board.
 TWOEMPTY: all but the rightmost two holes for each player are filled with is nbr_seeds.</t>
+  </si>
+  <si>
+    <t>The overall goal of the game. Defines how a player wins.
+MAX_SEEDS: player with the maximum number of seeds at the end of the game wins or they collect more than half of the total seeds
+DEPRIVE: eliminate all of your opponents seeds.
+TERRITORY: claim ownership of holes. Each round the ownership of holes is determined by the number of seeds captured in the previous round. In a TERRITORY game without rounds, the winner is the player gained the most territory during play.</t>
+  </si>
+  <si>
+    <t>Choose how holes are filled when a new round strarts:
+NOT_APPLICABLE: round fill doesn't need to be specified: either not played in rounds or game goal is TERRITORY (all holes filled).
+LEFT_FILL: fill holes from the player's left.
+RIGHT_FILL: fill holes from the player's right. 
+OUTSIDE_FILL: fill holes from the outside ends toward the middle.
+EVEN_FILL: fill both sides with the same number of seeds per hole, determined by dividing the losers seeds by the number of holes per side. If that is not playable base on minimum move, extra seeds are put in each players leftmost hole. Any extra seeds are put in each player's store.
+SHORTEN: shorten the board so that all of the loser's holes are filled; the winner will have more seeds in their store but the same board arrangement. If the game uses children, they will not be created if the board size is reduced to 3 or less.
+UCHOOSE: allow user to choose which holes have seeds (are not blocked) when ROUNDS with BLOCKS are used.
+UMOVE: allow the loser to choose where seeds are placed. At least one seed must be placed in each hole, remaining seeds are placed in the store. The winner's layout is the same layout but reflected.
+Note: These are not in numerical order.</t>
   </si>
 </sst>
 </file>
@@ -1806,8 +1807,8 @@
   <dimension ref="A1:J70"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G4" sqref="G4"/>
+      <pane ySplit="1" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1838,7 +1839,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>4</v>
@@ -1917,7 +1918,7 @@
         <v>0</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="345" x14ac:dyDescent="0.25">
@@ -1925,10 +1926,10 @@
         <v>69</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>203</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>204</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>24</v>
@@ -1937,10 +1938,10 @@
         <v>14</v>
       </c>
       <c r="F4" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="G4" s="5" t="s">
         <v>205</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>206</v>
       </c>
       <c r="H4" s="3">
         <v>3</v>
@@ -1949,7 +1950,7 @@
         <v>0</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -2077,7 +2078,7 @@
         <v>0</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -2109,7 +2110,7 @@
         <v>0</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -2141,7 +2142,7 @@
         <v>0</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -2149,10 +2150,10 @@
         <v>106</v>
       </c>
       <c r="B11" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>220</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>221</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>24</v>
@@ -2173,7 +2174,7 @@
         <v>0</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="210" x14ac:dyDescent="0.25">
@@ -2205,7 +2206,7 @@
         <v>0</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -2237,7 +2238,7 @@
         <v>2</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -2245,10 +2246,10 @@
         <v>106</v>
       </c>
       <c r="B14" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>233</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>234</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>24</v>
@@ -2269,7 +2270,7 @@
         <v>2</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="105" x14ac:dyDescent="0.25">
@@ -2301,7 +2302,7 @@
         <v>2</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="240" x14ac:dyDescent="0.25">
@@ -2333,7 +2334,7 @@
         <v>2</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2405,10 +2406,10 @@
         <v>106</v>
       </c>
       <c r="B19" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="C19" s="3" t="s">
         <v>247</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>248</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>24</v>
@@ -2429,7 +2430,7 @@
         <v>2</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2449,7 +2450,7 @@
         <v>20</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G20" s="5" t="s">
         <v>104</v>
@@ -2461,7 +2462,7 @@
         <v>2</v>
       </c>
       <c r="J20" s="4" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2469,10 +2470,10 @@
         <v>106</v>
       </c>
       <c r="B21" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="C21" s="3" t="s">
         <v>217</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>218</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>24</v>
@@ -2493,7 +2494,7 @@
         <v>2</v>
       </c>
       <c r="J21" s="4" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -2501,10 +2502,10 @@
         <v>106</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>24</v>
@@ -2513,10 +2514,10 @@
         <v>59</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="H22" s="3">
         <v>10</v>
@@ -2525,7 +2526,7 @@
         <v>2</v>
       </c>
       <c r="J22" s="4" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2653,18 +2654,18 @@
         <v>0</v>
       </c>
       <c r="J26" s="4" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" ht="330" x14ac:dyDescent="0.25">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="345" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>42</v>
       </c>
       <c r="B27" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="C27" s="3" t="s">
         <v>236</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>237</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>24</v>
@@ -2673,10 +2674,10 @@
         <v>62</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="H27" s="3">
         <v>6</v>
@@ -2685,7 +2686,7 @@
         <v>0</v>
       </c>
       <c r="J27" s="4" t="s">
-        <v>258</v>
+        <v>265</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="105" x14ac:dyDescent="0.25">
@@ -2717,10 +2718,10 @@
         <v>0</v>
       </c>
       <c r="J28" s="4" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" ht="120" x14ac:dyDescent="0.25">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="135" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>42</v>
       </c>
@@ -2749,7 +2750,7 @@
         <v>2</v>
       </c>
       <c r="J29" s="4" t="s">
-        <v>164</v>
+        <v>264</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2781,7 +2782,7 @@
         <v>2</v>
       </c>
       <c r="J30" s="4" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="31" spans="1:10" ht="285" x14ac:dyDescent="0.25">
@@ -2813,7 +2814,7 @@
         <v>2</v>
       </c>
       <c r="J31" s="4" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="255" x14ac:dyDescent="0.25">
@@ -2821,10 +2822,10 @@
         <v>42</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D32" s="3" t="s">
         <v>24</v>
@@ -2833,10 +2834,10 @@
         <v>60</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="G32" s="5" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="H32" s="3">
         <v>3</v>
@@ -2845,7 +2846,7 @@
         <v>2</v>
       </c>
       <c r="J32" s="4" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -2853,10 +2854,10 @@
         <v>42</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D33" s="3" t="s">
         <v>24</v>
@@ -2877,7 +2878,7 @@
         <v>2</v>
       </c>
       <c r="J33" s="4" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
@@ -2897,7 +2898,7 @@
         <v>28</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G34" s="5" t="s">
         <v>20</v>
@@ -2996,7 +2997,7 @@
         <v>32</v>
       </c>
       <c r="G37" s="6" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="H37" s="3">
         <v>4</v>
@@ -3069,7 +3070,7 @@
         <v>2</v>
       </c>
       <c r="J39" s="4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="40" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -3077,10 +3078,10 @@
         <v>142</v>
       </c>
       <c r="B40" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="C40" s="3" t="s">
         <v>175</v>
-      </c>
-      <c r="C40" s="3" t="s">
-        <v>176</v>
       </c>
       <c r="D40" s="3" t="s">
         <v>162</v>
@@ -3089,11 +3090,11 @@
         <v>13</v>
       </c>
       <c r="F40" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="G40" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="G40" s="3" t="s">
-        <v>177</v>
-      </c>
       <c r="H40" s="3">
         <v>0</v>
       </c>
@@ -3101,7 +3102,7 @@
         <v>0</v>
       </c>
       <c r="J40" s="4" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="41" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3141,10 +3142,10 @@
         <v>142</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D42" s="3" t="s">
         <v>162</v>
@@ -3165,7 +3166,7 @@
         <v>0</v>
       </c>
       <c r="J42" s="4" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="43" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3173,13 +3174,13 @@
         <v>142</v>
       </c>
       <c r="B43" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="C43" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="C43" s="3" t="s">
+      <c r="D43" s="3" t="s">
         <v>180</v>
-      </c>
-      <c r="D43" s="3" t="s">
-        <v>181</v>
       </c>
       <c r="E43" s="3">
         <v>46</v>
@@ -3188,7 +3189,7 @@
         <v>103</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="H43" s="3">
         <v>4</v>
@@ -3197,7 +3198,7 @@
         <v>0</v>
       </c>
       <c r="J43" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -3205,13 +3206,13 @@
         <v>142</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E44" s="3">
         <v>40</v>
@@ -3220,7 +3221,7 @@
         <v>103</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H44" s="3">
         <v>6</v>
@@ -3229,7 +3230,7 @@
         <v>0</v>
       </c>
       <c r="J44" s="4" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="45" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3237,13 +3238,13 @@
         <v>142</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E45" s="3">
         <v>41</v>
@@ -3252,7 +3253,7 @@
         <v>103</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="H45" s="3">
         <v>7</v>
@@ -3261,7 +3262,7 @@
         <v>0</v>
       </c>
       <c r="J45" s="4" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="46" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3269,13 +3270,13 @@
         <v>142</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E46" s="3">
         <v>42</v>
@@ -3284,7 +3285,7 @@
         <v>103</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="H46" s="3">
         <v>8</v>
@@ -3293,7 +3294,7 @@
         <v>0</v>
       </c>
       <c r="J46" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="47" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3325,7 +3326,7 @@
         <v>2</v>
       </c>
       <c r="J47" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
@@ -3557,7 +3558,7 @@
         <v>9</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D55" s="3" t="s">
         <v>24</v>
@@ -3575,7 +3576,7 @@
         <v>0</v>
       </c>
       <c r="J55" s="4" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="56" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3621,7 +3622,7 @@
         <v>0</v>
       </c>
       <c r="J57" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="58" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3648,7 +3649,7 @@
         <v>0</v>
       </c>
       <c r="J58" s="4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="59" spans="1:10" ht="105" x14ac:dyDescent="0.25">
@@ -3680,7 +3681,7 @@
         <v>0</v>
       </c>
       <c r="J59" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="60" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3816,10 +3817,10 @@
         <v>76</v>
       </c>
       <c r="B64" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="C64" s="3" t="s">
         <v>226</v>
-      </c>
-      <c r="C64" s="3" t="s">
-        <v>227</v>
       </c>
       <c r="D64" s="3" t="s">
         <v>24</v>
@@ -3828,10 +3829,10 @@
         <v>70</v>
       </c>
       <c r="F64" s="3" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G64" s="5" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="H64" s="3">
         <v>6</v>
@@ -3840,7 +3841,7 @@
         <v>0</v>
       </c>
       <c r="J64" s="4" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="65" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -3860,7 +3861,7 @@
         <v>75</v>
       </c>
       <c r="F65" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G65" s="5" t="s">
         <v>104</v>
@@ -3872,7 +3873,7 @@
         <v>0</v>
       </c>
       <c r="J65" s="4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="66" spans="1:10" ht="135" x14ac:dyDescent="0.25">
@@ -3892,10 +3893,10 @@
         <v>44</v>
       </c>
       <c r="F66" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="G66" s="5" t="s">
         <v>209</v>
-      </c>
-      <c r="G66" s="5" t="s">
-        <v>210</v>
       </c>
       <c r="H66" s="3">
         <v>0</v>
@@ -3904,7 +3905,7 @@
         <v>2</v>
       </c>
       <c r="J66" s="8" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="67" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3944,10 +3945,10 @@
         <v>76</v>
       </c>
       <c r="B68" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="C68" s="3" t="s">
         <v>198</v>
-      </c>
-      <c r="C68" s="3" t="s">
-        <v>199</v>
       </c>
       <c r="D68" s="3" t="s">
         <v>24</v>
@@ -3956,10 +3957,10 @@
         <v>27</v>
       </c>
       <c r="F68" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G68" s="5" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="H68" s="3">
         <v>3</v>
@@ -3968,7 +3969,7 @@
         <v>2</v>
       </c>
       <c r="J68" s="4" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="69" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3976,10 +3977,10 @@
         <v>76</v>
       </c>
       <c r="B69" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="C69" s="3" t="s">
         <v>196</v>
-      </c>
-      <c r="C69" s="3" t="s">
-        <v>197</v>
       </c>
       <c r="D69" s="3" t="s">
         <v>24</v>
@@ -4000,7 +4001,7 @@
         <v>2</v>
       </c>
       <c r="J69" s="4" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="70" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -4008,22 +4009,22 @@
         <v>76</v>
       </c>
       <c r="B70" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="C70" s="3" t="s">
         <v>243</v>
       </c>
-      <c r="C70" s="3" t="s">
+      <c r="D70" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E70" s="3">
+        <v>24</v>
+      </c>
+      <c r="F70" s="3" t="s">
         <v>244</v>
       </c>
-      <c r="D70" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E70" s="3">
-        <v>24</v>
-      </c>
-      <c r="F70" s="3" t="s">
-        <v>245</v>
-      </c>
       <c r="G70" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="H70" s="3">
         <v>5</v>
@@ -4032,7 +4033,7 @@
         <v>2</v>
       </c>
       <c r="J70" s="4" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Integration test for weg Support tools to create that test
</commit_message>
<xml_diff>
--- a/src/game_params.xlsx
+++ b/src/game_params.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Activity_Data\Mancala_github\MancalaGames\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{766CBC3E-FC5B-40D0-89AD-A69CB3E7FB5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5894903E-B278-46BC-B981-2036B6AEE6A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -871,16 +871,6 @@
 RIGHT_2_1ST_THEN_ALL_TWO:  The first turn must start from one of the two rightmost holes. Subsequent moves may only start from holes without 2 seeds, unless all holes contain zero or 2 seeds.</t>
   </si>
   <si>
-    <t xml:space="preserve">Games with children allow players to claim holes. These child holes are an extension of the stores and seeds in them count towards a win. Making a child stops any multiple lap sowing, moves cannot start from children, and they cannot be captured.
-NOCHILD: children are not used.
-NORMAL: no special child rules.
-WALDAS: Stores are not supported. Captures are instead moved into waldas, thus a player may not capture until they have created a walda. Child locations are limited.  Each player may create up to 6 waldas: on either end of each side of the board and the next outer hole on their own side of the board. Note that there are only 8 total places that waldas maybe created.
-ONE_CHILD: Use the tuzdek rules for children: only one child allowed on own side of the board, may not be in player's left most hole,  and may not be opposite eachother.
-WEG: children maybe created in holes owned by the opponent. Ending a sow in an opponent's weg captures the seed just sown and one more (if there is one); the player get's to play again.
-BULL: create one bull if final seed sows to CHILD_CVT, create two bulls if the final two seeds are sown to CHILD_CVT-1 and CHILD_CVT (in either order).
-</t>
-  </si>
-  <si>
     <t>NONE: there is no prescribed opening move.
 BASIC_SOWER: the first sow follows general rules of single lap sowing.  Other sow parameters will be enacted  afterward.
 MLAPS_SOWER: the first sow follows general rules of multi-lap sowing. Other sow parameters will be enacted  afterward.
@@ -923,6 +913,16 @@
 UCHOOSE: allow user to choose which holes have seeds (are not blocked) when ROUNDS with BLOCKS are used.
 UMOVE: allow the loser to choose where seeds are placed. At least one seed must be placed in each hole, remaining seeds are placed in the store. The winner's layout is the same layout but reflected.
 Note: These are not in numerical order.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Games with children allow players to claim holes. These child holes are an extension of the stores and seeds in them count towards a win. Making a child stops any multiple lap sowing, moves cannot start from children, and they cannot be captured.
+NOCHILD: children are not used.
+NORMAL: no special child rules.
+WALDAS: Stores are not supported. Captures are instead moved into waldas, thus a player may not capture until they have created a walda. Child locations are limited.  Each player may create up to 6 waldas: on either end of each side of the board and the next outer hole on their own side of the board. Note that there are only 8 total places that waldas maybe created.
+ONE_CHILD: Use the tuzdek rules for children: only one child allowed on own side of the board, may not be in player's left most hole,  and may not be opposite eachother.
+WEG: children maybe created in holes owned by the opponent. Ending a sow in an opponent's weg captures the seed just sown and one more (if there is one); generally, the player get's to play again (per CAPT_RTURN).
+BULL: create one bull if final seed sows to CHILD_CVT, create two bulls if the final two seeds are sown to CHILD_CVT-1 and CHILD_CVT (in either order).
+</t>
   </si>
 </sst>
 </file>
@@ -1808,7 +1808,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J27" sqref="J27"/>
+      <selection pane="bottomLeft" activeCell="J68" sqref="J68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2686,7 +2686,7 @@
         <v>0</v>
       </c>
       <c r="J27" s="4" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="105" x14ac:dyDescent="0.25">
@@ -2750,7 +2750,7 @@
         <v>2</v>
       </c>
       <c r="J29" s="4" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2814,7 +2814,7 @@
         <v>2</v>
       </c>
       <c r="J31" s="4" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="255" x14ac:dyDescent="0.25">
@@ -2846,7 +2846,7 @@
         <v>2</v>
       </c>
       <c r="J32" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -3841,7 +3841,7 @@
         <v>0</v>
       </c>
       <c r="J64" s="4" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="65" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -3940,7 +3940,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="68" spans="1:10" ht="330" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" ht="345" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
         <v>76</v>
       </c>
@@ -3969,7 +3969,7 @@
         <v>2</v>
       </c>
       <c r="J68" s="4" t="s">
-        <v>260</v>
+        <v>265</v>
       </c>
     </row>
     <row r="69" spans="1:10" ht="30" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Coverage test for weg making and capturing. Added a rule so WEGs require Goal == TERRITORY Moved make_child (not exactly a) deco to it's own file.
</commit_message>
<xml_diff>
--- a/src/game_params.xlsx
+++ b/src/game_params.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Activity_Data\Mancala_github\MancalaGames\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5894903E-B278-46BC-B981-2036B6AEE6A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE8076CE-21BD-4ECB-B819-52E43D4B6C8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="game_params" sheetId="1" r:id="rId1"/>
@@ -920,7 +920,7 @@
 NORMAL: no special child rules.
 WALDAS: Stores are not supported. Captures are instead moved into waldas, thus a player may not capture until they have created a walda. Child locations are limited.  Each player may create up to 6 waldas: on either end of each side of the board and the next outer hole on their own side of the board. Note that there are only 8 total places that waldas maybe created.
 ONE_CHILD: Use the tuzdek rules for children: only one child allowed on own side of the board, may not be in player's left most hole,  and may not be opposite eachother.
-WEG: children maybe created in holes owned by the opponent. Ending a sow in an opponent's weg captures the seed just sown and one more (if there is one); generally, the player get's to play again (per CAPT_RTURN).
+WEG: children maybe created in holes owned by the opponent. Ending a sow in an opponent's weg captures the seed just sown and one more (if there is one); generally, the player get's to play again (per CAPT_RTURN). WEGs are supported for TERRITORY games only (hole ownership required).
 BULL: create one bull if final seed sows to CHILD_CVT, create two bulls if the final two seeds are sown to CHILD_CVT-1 and CHILD_CVT (in either order).
 </t>
   </si>
@@ -3940,7 +3940,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="68" spans="1:10" ht="345" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" ht="360" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
         <v>76</v>
       </c>

</xml_diff>

<commit_message>
Coverage completed for capturer.py. Fixed documentation for xc_sown (it was wrong). make_child (is not yet 100%) also 'covered' by test_capturer. added inhibitor to not_yet because it's just not tested  (changed something that clearly seemed wrong).
</commit_message>
<xml_diff>
--- a/src/game_params.xlsx
+++ b/src/game_params.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Activity_Data\Mancala_github\MancalaGames\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE8076CE-21BD-4ECB-B819-52E43D4B6C8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F51A8478-0D4E-43E0-854E-A6124B07629F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1065" yWindow="180" windowWidth="28770" windowHeight="16170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="game_params" sheetId="1" r:id="rId1"/>
@@ -766,10 +766,6 @@
     <t>Must sow opp for xcapt</t>
   </si>
   <si>
-    <t>Don't do cross capture if have not sown into the opposite hole.
-If ending on own side of the board, but did not sow opposite hole, repeat turn.</t>
-  </si>
-  <si>
     <t>round_fill</t>
   </si>
   <si>
@@ -923,6 +919,10 @@
 WEG: children maybe created in holes owned by the opponent. Ending a sow in an opponent's weg captures the seed just sown and one more (if there is one); generally, the player get's to play again (per CAPT_RTURN). WEGs are supported for TERRITORY games only (hole ownership required).
 BULL: create one bull if final seed sows to CHILD_CVT, create two bulls if the final two seeds are sown to CHILD_CVT-1 and CHILD_CVT (in either order).
 </t>
+  </si>
+  <si>
+    <t>Only allow cross capture if the player has sown into the hole on the opposite side of board (the one to be captured from). 
+If a player ends on their own side of the board in an empty hole, but did not sow any opposite hole, the get a repeat turn.</t>
   </si>
 </sst>
 </file>
@@ -1807,8 +1807,8 @@
   <dimension ref="A1:J70"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J68" sqref="J68"/>
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1839,7 +1839,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>4</v>
@@ -1950,7 +1950,7 @@
         <v>0</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -2078,7 +2078,7 @@
         <v>0</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -2110,7 +2110,7 @@
         <v>0</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -2142,7 +2142,7 @@
         <v>0</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -2174,7 +2174,7 @@
         <v>0</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="210" x14ac:dyDescent="0.25">
@@ -2206,7 +2206,7 @@
         <v>0</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -2238,10 +2238,10 @@
         <v>2</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>106</v>
       </c>
@@ -2270,7 +2270,7 @@
         <v>2</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>234</v>
+        <v>265</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="105" x14ac:dyDescent="0.25">
@@ -2406,10 +2406,10 @@
         <v>106</v>
       </c>
       <c r="B19" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="C19" s="3" t="s">
         <v>246</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>247</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>24</v>
@@ -2430,7 +2430,7 @@
         <v>2</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2462,7 +2462,7 @@
         <v>2</v>
       </c>
       <c r="J20" s="4" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2654,7 +2654,7 @@
         <v>0</v>
       </c>
       <c r="J26" s="4" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="345" x14ac:dyDescent="0.25">
@@ -2662,10 +2662,10 @@
         <v>42</v>
       </c>
       <c r="B27" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="C27" s="3" t="s">
         <v>235</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>236</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>24</v>
@@ -2674,10 +2674,10 @@
         <v>62</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H27" s="3">
         <v>6</v>
@@ -2686,7 +2686,7 @@
         <v>0</v>
       </c>
       <c r="J27" s="4" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="105" x14ac:dyDescent="0.25">
@@ -2750,7 +2750,7 @@
         <v>2</v>
       </c>
       <c r="J29" s="4" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2782,7 +2782,7 @@
         <v>2</v>
       </c>
       <c r="J30" s="4" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="31" spans="1:10" ht="285" x14ac:dyDescent="0.25">
@@ -2814,7 +2814,7 @@
         <v>2</v>
       </c>
       <c r="J31" s="4" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="255" x14ac:dyDescent="0.25">
@@ -2846,7 +2846,7 @@
         <v>2</v>
       </c>
       <c r="J32" s="4" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -3142,10 +3142,10 @@
         <v>142</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D42" s="3" t="s">
         <v>162</v>
@@ -3166,7 +3166,7 @@
         <v>0</v>
       </c>
       <c r="J42" s="4" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="43" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3841,7 +3841,7 @@
         <v>0</v>
       </c>
       <c r="J64" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="65" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -3969,7 +3969,7 @@
         <v>2</v>
       </c>
       <c r="J68" s="4" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="69" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -4009,19 +4009,19 @@
         <v>76</v>
       </c>
       <c r="B70" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="C70" s="3" t="s">
         <v>242</v>
       </c>
-      <c r="C70" s="3" t="s">
+      <c r="D70" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E70" s="3">
+        <v>24</v>
+      </c>
+      <c r="F70" s="3" t="s">
         <v>243</v>
-      </c>
-      <c r="D70" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E70" s="3">
-        <v>24</v>
-      </c>
-      <c r="F70" s="3" t="s">
-        <v>244</v>
       </c>
       <c r="G70" s="3" t="s">
         <v>205</v>
@@ -4033,7 +4033,7 @@
         <v>2</v>
       </c>
       <c r="J70" s="4" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Coverage for make_child.py Test for inhibitor.py
</commit_message>
<xml_diff>
--- a/src/game_params.xlsx
+++ b/src/game_params.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Activity_Data\Mancala_github\MancalaGames\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F51A8478-0D4E-43E0-854E-A6124B07629F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D53D65F-D36E-4A2E-9AB9-8D0F540C1115}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1065" yWindow="180" windowWidth="28770" windowHeight="16170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-75" yWindow="75" windowWidth="28770" windowHeight="16170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="game_params" sheetId="1" r:id="rId1"/>
@@ -911,18 +911,18 @@
 Note: These are not in numerical order.</t>
   </si>
   <si>
+    <t>Only allow cross capture if the player has sown into the hole on the opposite side of board (the one to be captured from). 
+If a player ends on their own side of the board in an empty hole, but did not sow any opposite hole, the get a repeat turn.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Games with children allow players to claim holes. These child holes are an extension of the stores and seeds in them count towards a win. Making a child stops any multiple lap sowing, moves cannot start from children, and they cannot be captured.
 NOCHILD: children are not used.
-NORMAL: no special child rules.
+NORMAL: children are made when a final seeds sows a hole to CHILD_CVT.
 WALDAS: Stores are not supported. Captures are instead moved into waldas, thus a player may not capture until they have created a walda. Child locations are limited.  Each player may create up to 6 waldas: on either end of each side of the board and the next outer hole on their own side of the board. Note that there are only 8 total places that waldas maybe created.
-ONE_CHILD: Use the tuzdek rules for children: only one child allowed on own side of the board, may not be in player's left most hole,  and may not be opposite eachother.
+ONE_CHILD: Use the tuzdek rules for children: only one child allowed on opponent's side of the board, may not be in player's left most hole,  and may not be opposite eachother.
 WEG: children maybe created in holes owned by the opponent. Ending a sow in an opponent's weg captures the seed just sown and one more (if there is one); generally, the player get's to play again (per CAPT_RTURN). WEGs are supported for TERRITORY games only (hole ownership required).
 BULL: create one bull if final seed sows to CHILD_CVT, create two bulls if the final two seeds are sown to CHILD_CVT-1 and CHILD_CVT (in either order).
 </t>
-  </si>
-  <si>
-    <t>Only allow cross capture if the player has sown into the hole on the opposite side of board (the one to be captured from). 
-If a player ends on their own side of the board in an empty hole, but did not sow any opposite hole, the get a repeat turn.</t>
   </si>
 </sst>
 </file>
@@ -1808,7 +1808,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J16" sqref="J16"/>
+      <selection pane="bottomLeft" activeCell="J68" sqref="J68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2270,7 +2270,7 @@
         <v>2</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="105" x14ac:dyDescent="0.25">
@@ -3940,7 +3940,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="68" spans="1:10" ht="360" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" ht="375" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
         <v>76</v>
       </c>
@@ -3969,7 +3969,7 @@
         <v>2</v>
       </c>
       <c r="J68" s="4" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="69" spans="1:10" ht="30" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
tested and corrected min_occupy and cant_occupy_more
</commit_message>
<xml_diff>
--- a/src/game_params.xlsx
+++ b/src/game_params.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Activity_Data\Mancala_github\MancalaGames\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D53D65F-D36E-4A2E-9AB9-8D0F540C1115}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C40320D4-7033-470F-91FF-F60CBEB1712C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-75" yWindow="75" windowWidth="28770" windowHeight="16170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28830" yWindow="30" windowWidth="28770" windowHeight="16170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="game_params" sheetId="1" r:id="rId1"/>
@@ -875,15 +875,6 @@
 ARNGE_LIMIT: the first move may be used to rearrange the seeds (opponent is same layout). If the first move is not used for rearrangement, captures and child creation are not allowed from the starter until the second player makes a child or captures.</t>
   </si>
   <si>
-    <t xml:space="preserve">NONE: there is no special sowing rules.
-SOW_BLKD_DIV: Holes sown to GPARAM_ONE are closed (blocked) and the hole's seeds are removed from play. Blocked holes on own side are skipped when sowing and blocked holes on opp side are diverted out of play or captured. 
-SOW_BLKD_DIV_NR: SOW_BLKD_DIV except that each player's rightmost hole cannot be closed.
-OWN_SOW_CAPT_ALL: Capture all holes that are sown that meet the simple capture criteria: evens, min, max and  capture on. Other criteria are enforced: side of the board, unlocked, and not child.   Grand Slam rules are not applied. If the game goal TERRITORY the capturer is the hole owner; otherwise the capturer is done by side. NOCAPTFIRST prevents this capture for the first move.
-SOW_SOW_CAPT_ALL: Capture all holes that sown that meed the simple capture criteria only on the SOWER's side of the board. NOCAPTFIRST prevents this capture for the first move.
-NO_SOW_OPP_2S: Don't sow into opponents holes with 2 seeds.
-</t>
-  </si>
-  <si>
     <t>Allows specifing non-all-equal start patterns. Four patterns are supported:
 ALL_EQUAL: all holes start with the same number of seeds.
 GAMACHA: starting from the third hold (from start player's left) place nbr_seeds in every other hole, the first move is prescribed move the center hole's seeds to the other side (this is done automatically).
@@ -923,6 +914,15 @@
 WEG: children maybe created in holes owned by the opponent. Ending a sow in an opponent's weg captures the seed just sown and one more (if there is one); generally, the player get's to play again (per CAPT_RTURN). WEGs are supported for TERRITORY games only (hole ownership required).
 BULL: create one bull if final seed sows to CHILD_CVT, create two bulls if the final two seeds are sown to CHILD_CVT-1 and CHILD_CVT (in either order).
 </t>
+  </si>
+  <si>
+    <t>NONE: there is no special sowing rules.
+SOW_BLKD_DIV: Holes sown to GPARAM_ONE are closed (blocked) and the hole's seeds are removed from play. Blocked holes on own side are skipped when sowing and blocked holes on opp side are diverted out of play or captured. GOAL must be DEPRIVE.
+SOW_BLKD_DIV_NR: SOW_BLKD_DIV except that each player's rightmost hole cannot be closed. GOAL must be DEPRIVE.
+OWN_SOW_CAPT_ALL: Capture all holes that are sown that meet the simple capture criteria: evens, min, max and  capture on. Other criteria are enforced: side of the board, unlocked, and not child.   Grand Slam rules are not applied. If the game goal TERRITORY the capturer is the hole owner; otherwise the capturer is done by side. NOCAPTFIRST prevents this capture for the first move.
+SOW_SOW_CAPT_ALL: Capture all holes that sown that meed the simple capture criteria only on the SOWER's side of the board. NOCAPTFIRST prevents this capture for the first move.
+NO_SOW_OPP_2S: Don't sow into opponents holes with 2 seeds.
+Note: These are not in numerical order.</t>
   </si>
 </sst>
 </file>
@@ -1807,8 +1807,8 @@
   <dimension ref="A1:J70"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J68" sqref="J68"/>
+      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J64" sqref="J64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2270,7 +2270,7 @@
         <v>2</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="105" x14ac:dyDescent="0.25">
@@ -2686,7 +2686,7 @@
         <v>0</v>
       </c>
       <c r="J27" s="4" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="105" x14ac:dyDescent="0.25">
@@ -2750,7 +2750,7 @@
         <v>2</v>
       </c>
       <c r="J29" s="4" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2814,7 +2814,7 @@
         <v>2</v>
       </c>
       <c r="J31" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="255" x14ac:dyDescent="0.25">
@@ -3812,7 +3812,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="64" spans="1:10" ht="285" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" ht="300" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
         <v>76</v>
       </c>
@@ -3841,7 +3841,7 @@
         <v>0</v>
       </c>
       <c r="J64" s="4" t="s">
-        <v>260</v>
+        <v>265</v>
       </c>
     </row>
     <row r="65" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -3969,7 +3969,7 @@
         <v>2</v>
       </c>
       <c r="J68" s="4" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="69" spans="1:10" ht="30" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
end_move coverage to 99%.  errors found were fixed.
</commit_message>
<xml_diff>
--- a/src/game_params.xlsx
+++ b/src/game_params.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Activity_Data\Mancala_github\MancalaGames\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C40320D4-7033-470F-91FF-F60CBEB1712C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AAFEB24-2F2A-4854-9077-5A25E1ED4C54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28830" yWindow="30" windowWidth="28770" windowHeight="16170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -884,12 +884,6 @@
 TWOEMPTY: all but the rightmost two holes for each player are filled with is nbr_seeds.</t>
   </si>
   <si>
-    <t>The overall goal of the game. Defines how a player wins.
-MAX_SEEDS: player with the maximum number of seeds at the end of the game wins or they collect more than half of the total seeds
-DEPRIVE: eliminate all of your opponents seeds.
-TERRITORY: claim ownership of holes. Each round the ownership of holes is determined by the number of seeds captured in the previous round. In a TERRITORY game without rounds, the winner is the player gained the most territory during play.</t>
-  </si>
-  <si>
     <t>Choose how holes are filled when a new round strarts:
 NOT_APPLICABLE: round fill doesn't need to be specified: either not played in rounds or game goal is TERRITORY (all holes filled).
 LEFT_FILL: fill holes from the player's left.
@@ -923,6 +917,16 @@
 SOW_SOW_CAPT_ALL: Capture all holes that sown that meed the simple capture criteria only on the SOWER's side of the board. NOCAPTFIRST prevents this capture for the first move.
 NO_SOW_OPP_2S: Don't sow into opponents holes with 2 seeds.
 Note: These are not in numerical order.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The overall goal of the game. Defines how a player wins.
+- MAX_SEEDS: player with the maximum number of seeds at the end of the game wins or they collect more than half of the total seeds
+- DEPRIVE: eliminate all of your opponents seeds. 
+GRAND_SLAM must be legal for DEPRIVE games.
+The following options are incompatible with DEPRIVE games: MOVEUNLOCK, MUSTPASS, MUSTSHARE, ROUNDS, ROUND_STARTER, ROUND_FILL, NO_SIDES, SKIP_START, SOW_OWN_STORE, STORES, SOW_START, VISIT_OPP. 
+- TERRITORY: claim ownership of holes. Each round the ownership of holes is determined by the number of seeds captured in the previous round. In a TERRITORY game without rounds, the winner is the player that gained the most territory during play. 
+TERRITORY games require STORES and that GPARAM_ONE be set to a value between the number of holes and two times the number of holes.
+TERRITORY games are incompatible with NO_SIDES, START_PATTERN, GRANDSLAM of NOT_LEGAL, ALLOW_RULE of OPP_OR_EMPTY, </t>
   </si>
 </sst>
 </file>
@@ -1807,8 +1811,8 @@
   <dimension ref="A1:J70"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J64" sqref="J64"/>
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2270,7 +2274,7 @@
         <v>2</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="105" x14ac:dyDescent="0.25">
@@ -2686,7 +2690,7 @@
         <v>0</v>
       </c>
       <c r="J27" s="4" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="105" x14ac:dyDescent="0.25">
@@ -2721,7 +2725,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="135" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" ht="315" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>42</v>
       </c>
@@ -2750,7 +2754,7 @@
         <v>2</v>
       </c>
       <c r="J29" s="4" t="s">
-        <v>261</v>
+        <v>265</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3841,7 +3845,7 @@
         <v>0</v>
       </c>
       <c r="J64" s="4" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="65" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -3969,7 +3973,7 @@
         <v>2</v>
       </c>
       <c r="J68" s="4" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="69" spans="1:10" ht="30" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Implemented ChildType QUR. Defined Leyla-Gobale which uses it. Updated help files. Wrote tests, bringing capturer and make_child coverage back to 100%.
</commit_message>
<xml_diff>
--- a/src/game_params.xlsx
+++ b/src/game_params.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Activity_Data\Mancala_github\MancalaGames\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9124671-49F9-4392-AC32-B06FDEDCFE2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0D6EEA3-4458-4AAD-AC6F-7858806E5F6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28830" yWindow="30" windowWidth="28770" windowHeight="16170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28800" yWindow="30" windowWidth="28770" windowHeight="16170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="game_params" sheetId="1" r:id="rId1"/>
@@ -796,11 +796,6 @@
     <t>ChildRule</t>
   </si>
   <si>
-    <t>NONE: no additional restrictions.
-OPP_ONLY:  Only make children on the opposite side or in opponent's territory.
-NOT_1ST_OPP: Don't make a child in the first hole on the opponents side/territory with one seed.</t>
-  </si>
-  <si>
     <t>nocaptfirst</t>
   </si>
   <si>
@@ -900,16 +895,6 @@
 If a player ends on their own side of the board in an empty hole, but did not sow any opposite hole, the get a repeat turn.</t>
   </si>
   <si>
-    <t xml:space="preserve">Games with children allow players to claim holes. These child holes are an extension of the stores and seeds in them count towards a win. Making a child stops any multiple lap sowing, moves cannot start from children, and they cannot be captured.
-NOCHILD: children are not used.
-NORMAL: children are made when a final seeds sows a hole to CHILD_CVT.
-WALDAS: Stores are not supported. Captures are instead moved into waldas, thus a player may not capture until they have created a walda. Child locations are limited.  Each player may create up to 6 waldas: on either end of each side of the board and the next outer hole on their own side of the board. Note that there are only 8 total places that waldas maybe created.
-ONE_CHILD: Use the tuzdek rules for children: only one child allowed on opponent's side of the board, may not be in player's left most hole,  and may not be opposite eachother.
-WEG: children maybe created in holes owned by the opponent. Ending a sow in an opponent's weg captures the seed just sown and one more (if there is one); generally, the player get's to play again (per CAPT_RTURN). WEGs are supported for TERRITORY games only (hole ownership required).
-BULL: create one bull if final seed sows to CHILD_CVT, create two bulls if the final two seeds are sown to CHILD_CVT-1 and CHILD_CVT (in either order).
-</t>
-  </si>
-  <si>
     <t>NONE: there is no special sowing rules.
 SOW_BLKD_DIV: Holes sown to GPARAM_ONE are closed (blocked) and the hole's seeds are removed from play. Blocked holes on own side are skipped when sowing and blocked holes on opp side are diverted out of play or captured. GOAL must be DEPRIVE.
 SOW_BLKD_DIV_NR: SOW_BLKD_DIV except that each player's rightmost hole cannot be closed. GOAL must be DEPRIVE.
@@ -927,6 +912,22 @@
 - TERRITORY: claim ownership of holes. Each round the ownership of holes is determined by the number of seeds captured in the previous round. In a TERRITORY game without rounds, the winner is the player that gained the most territory during play. 
 TERRITORY games require STORES and that GPARAM_ONE be set to a value between the number of holes and two times the number of holes.
 TERRITORY games are incompatible with NO_SIDES, START_PATTERN, GRANDSLAM of NOT_LEGAL, ALLOW_RULE of OPP_OR_EMPTY, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Games with children allow players to claim holes. These child holes are an extension of the stores and seeds in them count towards a win. Making a child stops any multiple lap sowing, moves cannot start from children, and they cannot be captured.
+NOCHILD: children are not used.
+NORMAL: children are made when a final seeds sows a hole to CHILD_CVT.
+WALDA: Stores are not supported. Captures are instead moved into waldas, thus a player may not capture until they have created a walda. Child locations are limited.  Each player may create up to 6 waldas: on either end of each side of the board and the next outer hole on their own side of the board. Note that there are only 8 total places that waldas maybe created.
+ONE_CHILD: Use the tuzdek rules for children: only one child allowed on opponent's side of the board, may not be in player's left most hole,  and may not be opposite eachother.
+WEG: children maybe created in holes owned by the opponent. Ending a sow in an opponent's weg captures the seed just sown and one more (if there is one); generally, the player get's to play again (per CAPT_RTURN). WEGs are supported for TERRITORY games only (hole ownership required).
+BULL: create one bull if final seed sows to CHILD_CVT, create two bulls if the final two seeds are sown to CHILD_CVT-1 and CHILD_CVT (in either order).
+QUR: when a seed is sown into an empty hole on the player's side of the board and the opposite hole contains CHILD_CVT, create children in both holes: final seed location and opposite.
+</t>
+  </si>
+  <si>
+    <t>NONE: no additional restrictions.
+OPP_ONLY:  Only make children on the opposite side or in opponent's territory. Incompatible with BULL, QUR, and WEG child types.
+NOT_1ST_OPP: Don't make a child in the first hole on the opponents side/territory with one seed.</t>
   </si>
 </sst>
 </file>
@@ -1811,8 +1812,8 @@
   <dimension ref="A1:J70"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J29" sqref="J29"/>
+      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N68" sqref="N68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1954,7 +1955,7 @@
         <v>0</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -2082,7 +2083,7 @@
         <v>0</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -2114,7 +2115,7 @@
         <v>0</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -2146,7 +2147,7 @@
         <v>0</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -2178,7 +2179,7 @@
         <v>0</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="210" x14ac:dyDescent="0.25">
@@ -2210,7 +2211,7 @@
         <v>0</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -2242,7 +2243,7 @@
         <v>2</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -2274,7 +2275,7 @@
         <v>2</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="105" x14ac:dyDescent="0.25">
@@ -2410,10 +2411,10 @@
         <v>106</v>
       </c>
       <c r="B19" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="C19" s="3" t="s">
         <v>245</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>246</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>24</v>
@@ -2434,7 +2435,7 @@
         <v>2</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2466,7 +2467,7 @@
         <v>2</v>
       </c>
       <c r="J20" s="4" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2658,7 +2659,7 @@
         <v>0</v>
       </c>
       <c r="J26" s="4" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="345" x14ac:dyDescent="0.25">
@@ -2681,7 +2682,7 @@
         <v>236</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="H27" s="3">
         <v>6</v>
@@ -2690,7 +2691,7 @@
         <v>0</v>
       </c>
       <c r="J27" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="105" x14ac:dyDescent="0.25">
@@ -2754,7 +2755,7 @@
         <v>2</v>
       </c>
       <c r="J29" s="4" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2786,7 +2787,7 @@
         <v>2</v>
       </c>
       <c r="J30" s="4" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="31" spans="1:10" ht="285" x14ac:dyDescent="0.25">
@@ -2818,7 +2819,7 @@
         <v>2</v>
       </c>
       <c r="J31" s="4" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="255" x14ac:dyDescent="0.25">
@@ -2850,7 +2851,7 @@
         <v>2</v>
       </c>
       <c r="J32" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -3845,7 +3846,7 @@
         <v>0</v>
       </c>
       <c r="J64" s="4" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="65" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -3944,7 +3945,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="68" spans="1:10" ht="375" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
         <v>76</v>
       </c>
@@ -3973,7 +3974,7 @@
         <v>2</v>
       </c>
       <c r="J68" s="4" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
     <row r="69" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -4008,7 +4009,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="70" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
         <v>76</v>
       </c>
@@ -4037,7 +4038,7 @@
         <v>2</v>
       </c>
       <c r="J70" s="4" t="s">
-        <v>244</v>
+        <v>265</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added code to format parameter descriptions, but GOAL is ugly. Add cross references for games (text names) and parameters (when in upper case). The code for handling of multiword game names is also ugly, but the result is good. Game descriptions need to be updated to be consistent.
</commit_message>
<xml_diff>
--- a/src/game_params.xlsx
+++ b/src/game_params.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Activity_Data\Mancala_github\MancalaGames\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0D6EEA3-4458-4AAD-AC6F-7858806E5F6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBE57CD2-5654-466B-91C6-2304A51FB51F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28800" yWindow="30" windowWidth="28770" windowHeight="16170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="game_params" sheetId="1" r:id="rId1"/>
@@ -113,9 +113,6 @@
     <t>game_info _</t>
   </si>
   <si>
-    <t>The game name, may have spaces. Used for the config filename and the window title.</t>
-  </si>
-  <si>
     <t>help_file</t>
   </si>
   <si>
@@ -125,9 +122,6 @@
     <t>mancala_help.html</t>
   </si>
   <si>
-    <t>An html help file describing the game.</t>
-  </si>
-  <si>
     <t>about</t>
   </si>
   <si>
@@ -137,9 +131,6 @@
     <t>multi_str</t>
   </si>
   <si>
-    <t>Short string describing the game possibly in multiple lines. Enough to remind the player what the game options are.</t>
-  </si>
-  <si>
     <t>holes</t>
   </si>
   <si>
@@ -152,9 +143,6 @@
     <t>3</t>
   </si>
   <si>
-    <t>Number of holes on each side of the board. Start Pattern may use this number differently.</t>
-  </si>
-  <si>
     <t>nbr_start</t>
   </si>
   <si>
@@ -179,18 +167,12 @@
     <t>False</t>
   </si>
   <si>
-    <t>If a player has no allowable moves on their turn they must pass, until they have allowable moves. The game is over when neither play has an allowable move.</t>
-  </si>
-  <si>
     <t>rounds</t>
   </si>
   <si>
     <t>Rounds</t>
   </si>
   <si>
-    <t>Is the game played in rounds?</t>
-  </si>
-  <si>
     <t>round_starter</t>
   </si>
   <si>
@@ -218,9 +200,6 @@
     <t>True</t>
   </si>
   <si>
-    <t>Are stores present on the UI. Stores might not be on the UI but used if seeds are taken out of play.</t>
-  </si>
-  <si>
     <t>goal</t>
   </si>
   <si>
@@ -296,9 +275,6 @@
     <t>Move One Seed</t>
   </si>
   <si>
-    <t>Only valid when sow_start is set. Changes the sow_start behavior so that if there is only one seed in the hole, it is moved in the sow direction one hole.</t>
-  </si>
-  <si>
     <t>skip_start</t>
   </si>
   <si>
@@ -314,9 +290,6 @@
     <t>Sow Own Store</t>
   </si>
   <si>
-    <t>Sow seeds into your own store when passing it. Do not sow into your opponents store.</t>
-  </si>
-  <si>
     <t>blocks</t>
   </si>
   <si>
@@ -335,9 +308,6 @@
     <t>Visit Opp for Mlaps</t>
   </si>
   <si>
-    <t>Sow is multiplap only if the first sow reaches the opponents side of the board.</t>
-  </si>
-  <si>
     <t>0</t>
   </si>
   <si>
@@ -365,9 +335,6 @@
     <t>Capture in Sow Direction</t>
   </si>
   <si>
-    <t>Only meaninful, with multicapt. Captures are done in the same direction as the sowing, i.e. following the final hole sown. If not set, captures are done from the holes just sown.</t>
-  </si>
-  <si>
     <t>oppsidecapt</t>
   </si>
   <si>
@@ -381,9 +348,6 @@
   </si>
   <si>
     <t>Move Unlock for Capture</t>
-  </si>
-  <si>
-    <t>Captures may not be made from locked holes. Starting a sow from a hole unlocks it.</t>
   </si>
   <si>
     <t>evens</t>
@@ -532,13 +496,6 @@
   <si>
     <t xml:space="preserve">Sow counter-clockwise.
 Capture on evens. </t>
-  </si>
-  <si>
-    <t>Direction of sow:
-- CW: clockwise
-- CCW: counter-clockwise
-- SPLIT: left holes sow counter-clockwise and right holes sow clockwise, an odd middle hole must be set as udir_hole
-Any hole can be set as udir_hole to aloow the user to override the sow_direct setting.</t>
   </si>
   <si>
     <t>A list of holes that the user can control the sow direction from. Control is via the mouse button: left is clockwise and right is counter-clockwise.
@@ -554,22 +511,7 @@
     <t xml:space="preserve">The minimax scorer will use this as a multiplier to maximize the bottom players stores versus the top player's. </t>
   </si>
   <si>
-    <t>The number of seeds in each hole at the start of a game, unless the sow pattern is not ALL_EQUAL. Other sow patterns use this as the number of seeds for some holes in the associated patterns.</t>
-  </si>
-  <si>
-    <t>If an opponent has no moves at the start of your turn, you must make seeds available to them if you can.</t>
-  </si>
-  <si>
     <t>An init only parameter that used to check the consistency of the game info. Errors and warnings are raised as the rules are processed.</t>
-  </si>
-  <si>
-    <t>A grandslam is when your opponent has seeds at the start of your turn and you capture them all. This option selects what to do:
-LEGAL: the seeds are captured
-NOT_LEGAL: you may not capture all of your opponents seeds, a move which would do so is not allowed
-NO_CAPT: you may sow the seeds, but the capture is not performed
-OPP_GETS_REMAIN: if you capture all your opponents seeds, they capture all of your remaining seeds and the game is over. Winner is determined by game goal.
-LEAVE_LEFT: the capture is performed from all but the leftmost hole from the sower perspective. This might leave your oppenents without seeds or might not capture any seeds.
-LEAVE_RIGHT: the capture is performed from all but the rightmost hole from the sower perspective. This might leave your oppenents without seeds.</t>
   </si>
   <si>
     <t>GameClasses</t>
@@ -684,11 +626,6 @@
   </si>
   <si>
     <t>OFF</t>
-  </si>
-  <si>
-    <t>OFF: Single lap sowing.
-LAPPER:  If the first sow ends in a hole with more than one seed, pickup all the seeds and continue sowing another lap. Continue until the final seed of a lap reaches an empty hole, unless there is another rule that stops the sowing (e.g. making a child).
-LAPPER_NEXT:  If the first sow ends in a hole preceeding a hole with any seeds, pick up the seeds from that next hole and continue sowing another lap. Continue until the hole after the laps final seed is empty.</t>
   </si>
   <si>
     <t>gparam_one</t>
@@ -714,9 +651,6 @@
     <t>Repeat Turn on Capture</t>
   </si>
   <si>
-    <t>Repeat turn if there was a capture. Making children is not currently considered making a capture.</t>
-  </si>
-  <si>
     <t>capt_next</t>
   </si>
   <si>
@@ -755,11 +689,6 @@
     <t>On Capture, Take More Rule</t>
   </si>
   <si>
-    <t>NONE: Nothing extra
-PICKCROSS: Take the seeds from the opposite side of the board. 
-PICKTWOS: Take seeds from all holes containing two seeds but only after the first move.</t>
-  </si>
-  <si>
     <t>xc_sown</t>
   </si>
   <si>
@@ -800,41 +729,6 @@
   </si>
   <si>
     <t>No Capture First Move</t>
-  </si>
-  <si>
-    <t>Don't allow captures on the first move.</t>
-  </si>
-  <si>
-    <t>Capture when a hole contains an even number of seeds, greater than 0.
-xxx_SOW_CAPT_ALL does this capture.</t>
-  </si>
-  <si>
-    <t>Capture when the contents of the hole are less than or equal to capt_max.
-xxx_SOW_CAPT_ALL does this capture.</t>
-  </si>
-  <si>
-    <t>Capture when the contents of the hole are greater than or equal to capt_min.
-xxx_SOW_CAPT_ALL does this capture.</t>
-  </si>
-  <si>
-    <t>If the last sown seed is put in an empty hole, any seeds on the opposite side of the board are captured.
-xxx_SOW_CAPT_ALL does not do this capture.</t>
-  </si>
-  <si>
-    <t>Capture when the contents of the hole is in the capt_on list. 
-xxx_SOW_CAPT_ALL does this capture.</t>
-  </si>
-  <si>
-    <t>Capture from the hole after the final seed sown into an empty hole. 
-xxx_SOW_CAPT_ALL does not do this capture.</t>
-  </si>
-  <si>
-    <t>There are three flavors of capture two out:
-Single Lap: capture if sow ends in occupied hole, then an empty hole, followed by an occupied hole (this is hole captured).
-Multi lap but single capture: capture when last hole sown is followed by an empty hole which is then followed by an occupied hole.
-Multi lap with multiple captures: capture when last hole sown is followed by an empty hole which is then followed by an occupied hole. Continue captures as long as the pattern of empty hole followed by an occupied hole continues.
-xxx_SOW_CAPT_ALL does not do this capture.
-OPPSIDECAPT, EVENS, CAPT_MAX, CAPT_MIN, and CAPT_ON apply only to an optional xxx_SOW_CAPT_ALL and not the final capture.</t>
   </si>
   <si>
     <t>NOT_APPLICABLE</t>
@@ -848,18 +742,6 @@
   </si>
   <si>
     <t xml:space="preserve">Moves maybe made from any hole, independent of the side of the board. Moves need specify side, position and directions.  </t>
-  </si>
-  <si>
-    <t>Allow rules limit the holes from which moves may start.  Disallowed holes are not selectable.
-NONE: no special rule
-OPP_OR_EMPTY:  Limit the allowable holes to those that end in an empty hole or reach the opponents side of the board.
-SINGLE_TO_ZERO: Holes with single seeds may only be played if the next hole is empty.
-SINGLE_ONLY_ALL: Holes with single seeds may only be played if all holes contain single seeds.
-SINGLE_ALL_TO_ZERO: Holes with single seeds may only be played if all holes contain single seeds and then only if the next hole is empty.
-TWO_ONLY_ALL: Holes with two seeds may only be played if all holes contain two seeds.
-TWO_ONLY_ALL_RIGHT: Holes with two seeds may not be played, unless all holes contains two seeds, in which case the rightmost hole must be played.
-FIRST_TURN_ONLY_RIGHT_TWO: The first turn must start from one of the two rightmost holes.
-RIGHT_2_1ST_THEN_ALL_TWO:  The first turn must start from one of the two rightmost holes. Subsequent moves may only start from holes without 2 seeds, unless all holes contain zero or 2 seeds.</t>
   </si>
   <si>
     <t>NONE: there is no prescribed opening move.
@@ -879,29 +761,8 @@
 TWOEMPTY: all but the rightmost two holes for each player are filled with is nbr_seeds.</t>
   </si>
   <si>
-    <t>Choose how holes are filled when a new round strarts:
-NOT_APPLICABLE: round fill doesn't need to be specified: either not played in rounds or game goal is TERRITORY (all holes filled).
-LEFT_FILL: fill holes from the player's left.
-RIGHT_FILL: fill holes from the player's right. 
-OUTSIDE_FILL: fill holes from the outside ends toward the middle.
-EVEN_FILL: fill both sides with the same number of seeds per hole, determined by dividing the losers seeds by the number of holes per side. If that is not playable base on minimum move, extra seeds are put in each players leftmost hole. Any extra seeds are put in each player's store.
-SHORTEN: shorten the board so that all of the loser's holes are filled; the winner will have more seeds in their store but the same board arrangement. If the game uses children, they will not be created if the board size is reduced to 3 or less.
-UCHOOSE: allow user to choose which holes have seeds (are not blocked) when ROUNDS with BLOCKS are used.
-UMOVE: allow the loser to choose where seeds are placed. At least one seed must be placed in each hole, remaining seeds are placed in the store. The winner's layout is the same layout but reflected.
-Note: These are not in numerical order.</t>
-  </si>
-  <si>
     <t>Only allow cross capture if the player has sown into the hole on the opposite side of board (the one to be captured from). 
 If a player ends on their own side of the board in an empty hole, but did not sow any opposite hole, the get a repeat turn.</t>
-  </si>
-  <si>
-    <t>NONE: there is no special sowing rules.
-SOW_BLKD_DIV: Holes sown to GPARAM_ONE are closed (blocked) and the hole's seeds are removed from play. Blocked holes on own side are skipped when sowing and blocked holes on opp side are diverted out of play or captured. GOAL must be DEPRIVE.
-SOW_BLKD_DIV_NR: SOW_BLKD_DIV except that each player's rightmost hole cannot be closed. GOAL must be DEPRIVE.
-OWN_SOW_CAPT_ALL: Capture all holes that are sown that meet the simple capture criteria: evens, min, max and  capture on. Other criteria are enforced: side of the board, unlocked, and not child.   Grand Slam rules are not applied. If the game goal TERRITORY the capturer is the hole owner; otherwise the capturer is done by side. NOCAPTFIRST prevents this capture for the first move.
-SOW_SOW_CAPT_ALL: Capture all holes that sown that meed the simple capture criteria only on the SOWER's side of the board. NOCAPTFIRST prevents this capture for the first move.
-NO_SOW_OPP_2S: Don't sow into opponents holes with 2 seeds.
-Note: These are not in numerical order.</t>
   </si>
   <si>
     <t xml:space="preserve">The overall goal of the game. Defines how a player wins.
@@ -914,20 +775,164 @@
 TERRITORY games are incompatible with NO_SIDES, START_PATTERN, GRANDSLAM of NOT_LEGAL, ALLOW_RULE of OPP_OR_EMPTY, </t>
   </si>
   <si>
+    <t>An html help file describing the game (mancala_help.html is the main help file).</t>
+  </si>
+  <si>
+    <t>The game name, may have spaces. Used for the window title and the filename (with spaces replaced with underscores).</t>
+  </si>
+  <si>
+    <t>The number of seeds in each hole at the start of a game when START_PATTERN is ALL_EQUAL. Other sow patterns use this as the number of seeds for some holes in the associated patterns.</t>
+  </si>
+  <si>
+    <t>A description of the game, typically enough to remind the player what the game options are.
+New lines can be inserted with \n.</t>
+  </si>
+  <si>
+    <t>Number of holes on each side of the board.</t>
+  </si>
+  <si>
+    <t>Are stores present on the game board?</t>
+  </si>
+  <si>
+    <t>When a player has no allowable moves on their turn, they must pass, and continue to do so until they have allowable moves or the game is over. The game is over when there is a clear winner or tie condition, or when neither player has an allowable move.</t>
+  </si>
+  <si>
+    <t>Choose how holes are filled when a new round strarts:
+- NOT_APPLICABLE: round fill doesn't need to be specified: either not played in rounds or game goal is TERRITORY (all holes filled).
+- LEFT_FILL: fill holes from the player's left.
+- RIGHT_FILL: fill holes from the player's right. 
+- OUTSIDE_FILL: fill holes from the outside ends toward the middle.
+- EVEN_FILL: fill both sides with the same number of seeds per hole, determined by dividing the losers seeds by the number of holes per side. If that is not playable base on minimum move, extra seeds are put in each players leftmost hole. Any extra seeds are put in each player's store.
+- SHORTEN: shorten the board so that all of the loser's holes are filled; the winner will have more seeds in their store but the same board arrangement. If the game uses children, they will not be created if the board size is reduced to 3 or less.
+- UCHOOSE: allow user to choose which holes have seeds (are not blocked) when ROUNDS and BLOCKS are used.
+- UMOVE: allow the loser to choose where seeds are placed. At least one seed must be placed in each hole, remaining seeds are placed in the store. The winner's layout is the same layout but reflected.
+Note: These are not in numerical order.</t>
+  </si>
+  <si>
+    <t>Is the game played in a series of rounds? In the case of a round win or tie  a new starter is determined via ROUND_STARTER and  the board is reset according to ROUND_FILL. BLOCKS are used in many games and set between rounds based on the seed placement.</t>
+  </si>
+  <si>
+    <t>If an opponent has no moves at the start of your turn, you must make seeds available to them if you can. This condition is enforced by only activating holes on the UI will make seeds available.</t>
+  </si>
+  <si>
+    <t>Allow rules limit the holes from which moves may start.  Disallowed holes are not selectable.
+- NONE: no special rule
+- OPP_OR_EMPTY:  Limit the allowable holes to those that end in an empty hole or reach the opponents side of the board.
+- SINGLE_TO_ZERO: Holes with single seeds may only be played if the next hole is empty.
+- SINGLE_ONLY_ALL: Holes with single seeds may only be played if all holes contain single seeds.
+- SINGLE_ALL_TO_ZERO: Holes with single seeds may only be played if all holes contain single seeds and then only if the next hole is empty.
+- TWO_ONLY_ALL: Holes with two seeds may only be played if all holes contain two seeds.
+- TWO_ONLY_ALL_RIGHT: Holes with two seeds may not be played, unless all holes contains two seeds, in which case the rightmost hole must be played.
+- FIRST_TURN_ONLY_RIGHT_TWO: The first turn must start from one of the two rightmost holes.
+- RIGHT_2_1ST_THEN_ALL_TWO:  The first turn must start from one of the two rightmost holes. Subsequent moves may only start from holes without 2 seeds, unless all holes contain zero or 2 seeds.</t>
+  </si>
+  <si>
+    <t>Sow seeds into your own store when passing it. Do not sow into your opponents store. Sow the final seed of a move into the store, results in a repeat turn.</t>
+  </si>
+  <si>
+    <t>Direction of sow:
+- CW: clockwise
+- CCW: counter-clockwise
+- SPLIT: left side holes sow counter-clockwise and right side holes sow clockwise, an odd middle hole must be set as UDIR_HOLE. 
+Any hole can be set as UDIR_HOLE to allow the user to override the sow_direct setting.</t>
+  </si>
+  <si>
+    <t>Only valid when SOW_START is set. Changes the SOW_START behavior so that if there is only one seed in the hole, it is moved in the sow direction by one hole.</t>
+  </si>
+  <si>
+    <t>Special sow rules may additional behavior or restrictions to the sowing phase:
+- NONE: there is no special sowing rules.
+- SOW_BLKD_DIV: Holes sown to GPARAM_ONE are closed (blocked) and the hole's seeds are removed from play. Blocked holes on own side are skipped when sowing and blocked holes on opp side are diverted out of play or captured. GOAL must be DEPRIVE.
+- SOW_BLKD_DIV_NR: Behaves the same as SOW_BLKD_DIV except that each player's rightmost hole cannot be closed. GOAL must be DEPRIVE.
+- OWN_SOW_CAPT_ALL: Capture all holes that are sown that meet the simple capture criteria: evens, min, max and  capture on. Other criteria are enforced: side of the board, unlocked, and not child.   GRANDSLAM rules are not applied. If the game GOAL is TERRITORY the capturer is the hole owner; otherwise the capturer is done by side. NOCAPTFIRST prevents this capture for the first move.
+- SOW_SOW_CAPT_ALL: Capture all holes that sown that meed the simple capture criteria only on the SOWER's side of the board. NOCAPTFIRST prevents this capture for the first move.
+- NO_SOW_OPP_2S: Don't sow into opponents holes with 2 seeds.
+Note: These are not in numerical order.</t>
+  </si>
+  <si>
+    <t>Sow is multiplap only if the first sow (seeds from the starting hole) reaches the opponents side of the board.</t>
+  </si>
+  <si>
+    <t>Addiitonal child creation requirements may be set:
+- NONE: no additional restrictions.
+- OPP_ONLY:  Only make children on the opposite side or in opponent's territory. Incompatible with BULL, QUR, and WEG child types.
+- NOT_1ST_OPP: Don't make a child in the first hole on the opponents side/territory with one seed.</t>
+  </si>
+  <si>
+    <t>Determines if seeds from more the start hole are picked up and sown:
+- OFF: Single lap sowing. Seeds from the start hole are sown, typically, one per hole until expened.
+- LAPPER:  If the first sow ends in a hole with more than one seed, pickup all the seeds and continue sowing another lap. Continue until the final seed of a lap reaches an empty hole, unless there is another rule that stops the sowing (e.g. making a child).
+- LAPPER_NEXT:  If the first sow ends in a hole preceeding a hole with any seeds, pick up the seeds from that next hole and continue sowing another lap. Continue until the hole after the laps final seed is empty.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Games with children allow players to claim holes. These child holes are an extension of the stores and seeds in them count towards a win. Making a child stops any multiple lap sowing, moves cannot start from children, and they cannot be captured.
-NOCHILD: children are not used.
-NORMAL: children are made when a final seeds sows a hole to CHILD_CVT.
-WALDA: Stores are not supported. Captures are instead moved into waldas, thus a player may not capture until they have created a walda. Child locations are limited.  Each player may create up to 6 waldas: on either end of each side of the board and the next outer hole on their own side of the board. Note that there are only 8 total places that waldas maybe created.
-ONE_CHILD: Use the tuzdek rules for children: only one child allowed on opponent's side of the board, may not be in player's left most hole,  and may not be opposite eachother.
-WEG: children maybe created in holes owned by the opponent. Ending a sow in an opponent's weg captures the seed just sown and one more (if there is one); generally, the player get's to play again (per CAPT_RTURN). WEGs are supported for TERRITORY games only (hole ownership required).
-BULL: create one bull if final seed sows to CHILD_CVT, create two bulls if the final two seeds are sown to CHILD_CVT-1 and CHILD_CVT (in either order).
-QUR: when a seed is sown into an empty hole on the player's side of the board and the opposite hole contains CHILD_CVT, create children in both holes: final seed location and opposite.
+- NOCHILD: children are not used.
+- NORMAL: children are made when a final seeds sows a hole to CHILD_CVT.
+- WALDA: Stores are not supported. Captures are instead moved into waldas, thus a player may not capture until they have created a walda. Child locations are limited.  Each player may create up to 6 waldas: on either end of each side of the board and the next outer hole on their own side of the board. Note that there are only 8 total places that waldas maybe created.
+- ONE_CHILD: Use the tuzdek rules for children: only one child allowed on opponent's side of the board, may not be in player's left most hole,  and may not be opposite eachother.
+- WEG: children maybe created in holes owned by the opponent. Ending a sow in an opponent's weg captures the seed just sown and one more (if there is one); generally, the player get's to play again (per CAPT_RTURN). WEGs are supported for TERRITORY games only (hole ownership required).
+- BULL: create one bull if final seed sows to CHILD_CVT, create two bulls if the final two seeds are sown to CHILD_CVT-1 and CHILD_CVT (in either order).
+- QUR: when a seed is sown into an empty hole on the player's side of the board and the opposite hole contains CHILD_CVT, create children in both holes: final seed location and opposite.
 </t>
   </si>
   <si>
-    <t>NONE: no additional restrictions.
-OPP_ONLY:  Only make children on the opposite side or in opponent's territory. Incompatible with BULL, QUR, and WEG child types.
-NOT_1ST_OPP: Don't make a child in the first hole on the opponents side/territory with one seed.</t>
+    <t>Only meaninful, with MULTICAPT. Captures are done in the same direction as the sowing, i.e. following the final hole sown. If not set, captures are done from the holes just sown.</t>
+  </si>
+  <si>
+    <t>Capture when a hole contains an even number of seeds, greater than 0.
+Additionally, a SOWRULE of OWN_SOW_CAPT_ALL or SOW_SOW_CAPT_ALL includes this capture mechanism.</t>
+  </si>
+  <si>
+    <t>Capture when the contents of the hole are less than or equal to capt_max.
+Additionally, a SOWRULE of OWN_SOW_CAPT_ALL or SOW_SOW_CAPT_ALL includes this capture mechanism.</t>
+  </si>
+  <si>
+    <t>Capture when the contents of the hole are greater than or equal to capt_min.
+Additionally, a SOWRULE of OWN_SOW_CAPT_ALL or SOW_SOW_CAPT_ALL includes this capture mechanism.</t>
+  </si>
+  <si>
+    <t>Capture from the hole after the final seed sown into an empty hole. 
+Additionally, a SOWRULE of OWN_SOW_CAPT_ALL or SOW_SOW_CAPT_ALL includes this capture mechanism.</t>
+  </si>
+  <si>
+    <t>There are three flavors of capture two out:
+Single Lap: capture if sow ends in occupied hole, then an empty hole, followed by an occupied hole (this is hole captured).
+Multi lap but single capture: capture when last hole sown is followed by an empty hole which is then followed by an occupied hole.
+Multi lap with multiple captures: capture when last hole sown is followed by an empty hole which is then followed by an occupied hole. Continue captures as long as the pattern of empty hole followed by an occupied hole continues.
+Additionally, a SOWRULE of OWN_SOW_CAPT_ALL or SOW_SOW_CAPT_ALL includes this capture mechanism.
+OPPSIDECAPT, EVENS, CAPT_MAX, CAPT_MIN, and CAPT_ON apply only to an optional xxx_SOW_CAPT_ALL and not the final capture.</t>
+  </si>
+  <si>
+    <t>If the last sown seed is put in an empty hole, any seeds on the opposite side of the board are captured.
+SOW_RULE of either SOW_CAPT_ALL do not do this capture.</t>
+  </si>
+  <si>
+    <t>A grandslam is when your opponent has seeds at the start of your turn and you capture them all. This option selects what to do:
+- LEGAL: the seeds are captured
+- NOT_LEGAL: you may not capture all of your opponents seeds, a move which would do so is not allowed
+- NO_CAPT: you may sow the seeds, but the capture is not performed
+- OPP_GETS_REMAIN: if you capture all your opponents seeds, they capture all of your remaining seeds and the game is over. Winner is determined by game goal.
+- LEAVE_LEFT: the capture is performed from all but the leftmost hole from the sower perspective. This might leave your oppenents without seeds or might not capture any seeds.
+- LEAVE_RIGHT: the capture is performed from all but the rightmost hole from the sower perspective. This might leave your oppenents without seeds.</t>
+  </si>
+  <si>
+    <t>Holes in the game start each round locked. Captures may not be made from locked holes. Starting a sow from a hole unlocks it.</t>
+  </si>
+  <si>
+    <t>Don't allow captures on the first move of the game or round.</t>
+  </si>
+  <si>
+    <t>Capture when the contents of the hole is in the capt_on list. 
+Additionally, a SOWRULE of OWN_SOW_CAPT_ALL or SOW_SOW_CAPT_ALL includes this capture mechanism.</t>
+  </si>
+  <si>
+    <t>Repeat turn if there was a capture. Making children is not a capture.</t>
+  </si>
+  <si>
+    <t>Rules to allow taking of more than otherwise captured or picked seeds:
+- NONE: Nothing extra
+- PICKCROSS: Take the seeds from the opposite side of the board. 
+- PICKTWOS: Take seeds from all holes containing two seeds but only after the first move.</t>
   </si>
 </sst>
 </file>
@@ -1811,9 +1816,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:J70"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N68" sqref="N68"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1844,7 +1849,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>239</v>
+        <v>220</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>4</v>
@@ -1864,13 +1869,13 @@
     </row>
     <row r="2" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>24</v>
@@ -1882,7 +1887,7 @@
         <v>11</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="H2" s="3">
         <v>0</v>
@@ -1891,18 +1896,18 @@
         <v>0</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>24</v>
@@ -1911,10 +1916,10 @@
         <v>51</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="H3" s="3">
         <v>1</v>
@@ -1923,18 +1928,18 @@
         <v>0</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>170</v>
+        <v>243</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="345" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>202</v>
+        <v>186</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>203</v>
+        <v>187</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>24</v>
@@ -1943,10 +1948,10 @@
         <v>14</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>204</v>
+        <v>188</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>205</v>
+        <v>189</v>
       </c>
       <c r="H4" s="3">
         <v>3</v>
@@ -1955,18 +1960,18 @@
         <v>0</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>257</v>
+        <v>244</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>24</v>
@@ -1975,10 +1980,10 @@
         <v>16</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="H5" s="3">
         <v>0</v>
@@ -1987,18 +1992,18 @@
         <v>0</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>109</v>
+        <v>253</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>24</v>
@@ -2007,10 +2012,10 @@
         <v>58</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="H6" s="3">
         <v>1</v>
@@ -2019,18 +2024,18 @@
         <v>0</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>132</v>
+        <v>120</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>24</v>
@@ -2039,10 +2044,10 @@
         <v>49</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="H7" s="3">
         <v>2</v>
@@ -2051,18 +2056,18 @@
         <v>0</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>116</v>
+        <v>104</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>24</v>
@@ -2071,10 +2076,10 @@
         <v>33</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="H8" s="3">
         <v>3</v>
@@ -2083,18 +2088,18 @@
         <v>0</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>118</v>
-      </c>
       <c r="C9" s="3" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>24</v>
@@ -2106,7 +2111,7 @@
         <v>11</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="H9" s="3">
         <v>4</v>
@@ -2115,18 +2120,18 @@
         <v>0</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>24</v>
@@ -2138,7 +2143,7 @@
         <v>11</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="H10" s="3">
         <v>5</v>
@@ -2147,18 +2152,18 @@
         <v>0</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>219</v>
+        <v>201</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>220</v>
+        <v>202</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>24</v>
@@ -2167,10 +2172,10 @@
         <v>19</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="H11" s="3">
         <v>6</v>
@@ -2179,18 +2184,18 @@
         <v>0</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="210" x14ac:dyDescent="0.25">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="225" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>24</v>
@@ -2199,10 +2204,10 @@
         <v>22</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="H12" s="3">
         <v>7</v>
@@ -2211,18 +2216,18 @@
         <v>0</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>253</v>
+        <v>258</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>126</v>
+        <v>114</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>24</v>
@@ -2231,10 +2236,10 @@
         <v>29</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="H13" s="3">
         <v>0</v>
@@ -2243,18 +2248,18 @@
         <v>2</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>250</v>
+        <v>259</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>232</v>
+        <v>213</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>233</v>
+        <v>214</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>24</v>
@@ -2263,10 +2268,10 @@
         <v>78</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="H14" s="3">
         <v>1</v>
@@ -2275,18 +2280,18 @@
         <v>2</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>261</v>
+        <v>232</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>127</v>
+        <v>115</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>128</v>
+        <v>116</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>24</v>
@@ -2295,10 +2300,10 @@
         <v>79</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>129</v>
+        <v>117</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>130</v>
+        <v>118</v>
       </c>
       <c r="H15" s="3">
         <v>2</v>
@@ -2307,18 +2312,18 @@
         <v>2</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>167</v>
+        <v>154</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="240" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>134</v>
+        <v>122</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>135</v>
+        <v>123</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>24</v>
@@ -2327,10 +2332,10 @@
         <v>37</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
       <c r="H16" s="3">
         <v>3</v>
@@ -2339,18 +2344,18 @@
         <v>2</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>172</v>
+        <v>260</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>24</v>
@@ -2359,10 +2364,10 @@
         <v>48</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="H17" s="3">
         <v>4</v>
@@ -2371,18 +2376,18 @@
         <v>2</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>115</v>
+        <v>261</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>123</v>
+        <v>111</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>24</v>
@@ -2391,10 +2396,10 @@
         <v>57</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="H18" s="3">
         <v>5</v>
@@ -2403,18 +2408,18 @@
         <v>2</v>
       </c>
       <c r="J18" s="4" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>244</v>
+        <v>225</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>245</v>
+        <v>226</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>24</v>
@@ -2423,10 +2428,10 @@
         <v>56</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="H19" s="3">
         <v>6</v>
@@ -2435,18 +2440,18 @@
         <v>2</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>24</v>
@@ -2455,10 +2460,10 @@
         <v>20</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>177</v>
+        <v>161</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
       <c r="H20" s="3">
         <v>8</v>
@@ -2467,18 +2472,18 @@
         <v>2</v>
       </c>
       <c r="J20" s="4" t="s">
-        <v>251</v>
+        <v>263</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>216</v>
+        <v>199</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>217</v>
+        <v>200</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>24</v>
@@ -2487,10 +2492,10 @@
         <v>21</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="H21" s="3">
         <v>9</v>
@@ -2499,18 +2504,18 @@
         <v>2</v>
       </c>
       <c r="J21" s="4" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>228</v>
+        <v>210</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>230</v>
+        <v>212</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>24</v>
@@ -2519,10 +2524,10 @@
         <v>59</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>229</v>
+        <v>211</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>205</v>
+        <v>189</v>
       </c>
       <c r="H22" s="3">
         <v>10</v>
@@ -2531,18 +2536,18 @@
         <v>2</v>
       </c>
       <c r="J22" s="4" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>24</v>
@@ -2551,10 +2556,10 @@
         <v>73</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="H23" s="3">
         <v>0</v>
@@ -2563,18 +2568,18 @@
         <v>0</v>
       </c>
       <c r="J23" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>24</v>
@@ -2583,10 +2588,10 @@
         <v>50</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="H24" s="3">
         <v>1</v>
@@ -2595,18 +2600,18 @@
         <v>0</v>
       </c>
       <c r="J24" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>24</v>
@@ -2615,10 +2620,10 @@
         <v>64</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="H25" s="3">
         <v>4</v>
@@ -2627,18 +2632,18 @@
         <v>0</v>
       </c>
       <c r="J25" s="4" t="s">
-        <v>50</v>
+        <v>242</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>24</v>
@@ -2647,10 +2652,10 @@
         <v>63</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="G26" s="5" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="H26" s="3">
         <v>5</v>
@@ -2659,18 +2664,18 @@
         <v>0</v>
       </c>
       <c r="J26" s="4" t="s">
-        <v>255</v>
+        <v>228</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="345" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>234</v>
+        <v>215</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>235</v>
+        <v>216</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>24</v>
@@ -2679,10 +2684,10 @@
         <v>62</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>236</v>
+        <v>217</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>254</v>
+        <v>227</v>
       </c>
       <c r="H27" s="3">
         <v>6</v>
@@ -2691,18 +2696,18 @@
         <v>0</v>
       </c>
       <c r="J27" s="4" t="s">
-        <v>260</v>
+        <v>241</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>24</v>
@@ -2711,10 +2716,10 @@
         <v>15</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="G28" s="5" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="H28" s="3">
         <v>7</v>
@@ -2723,18 +2728,18 @@
         <v>0</v>
       </c>
       <c r="J28" s="4" t="s">
-        <v>221</v>
+        <v>203</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="315" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="D29" s="3" t="s">
         <v>24</v>
@@ -2743,10 +2748,10 @@
         <v>35</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="G29" s="5" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="H29" s="3">
         <v>0</v>
@@ -2755,18 +2760,18 @@
         <v>2</v>
       </c>
       <c r="J29" s="4" t="s">
-        <v>263</v>
+        <v>233</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="D30" s="3" t="s">
         <v>24</v>
@@ -2775,10 +2780,10 @@
         <v>55</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="G30" s="5" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="H30" s="3">
         <v>1</v>
@@ -2787,18 +2792,18 @@
         <v>2</v>
       </c>
       <c r="J30" s="4" t="s">
-        <v>256</v>
+        <v>229</v>
       </c>
     </row>
     <row r="31" spans="1:10" ht="285" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="D31" s="3" t="s">
         <v>24</v>
@@ -2807,10 +2812,10 @@
         <v>72</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="G31" s="5" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="H31" s="3">
         <v>2</v>
@@ -2819,18 +2824,18 @@
         <v>2</v>
       </c>
       <c r="J31" s="4" t="s">
-        <v>259</v>
+        <v>231</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="255" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>223</v>
+        <v>205</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>222</v>
+        <v>204</v>
       </c>
       <c r="D32" s="3" t="s">
         <v>24</v>
@@ -2839,10 +2844,10 @@
         <v>60</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>224</v>
+        <v>206</v>
       </c>
       <c r="G32" s="5" t="s">
-        <v>205</v>
+        <v>189</v>
       </c>
       <c r="H32" s="3">
         <v>3</v>
@@ -2851,18 +2856,18 @@
         <v>2</v>
       </c>
       <c r="J32" s="4" t="s">
-        <v>258</v>
+        <v>230</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>211</v>
+        <v>194</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>206</v>
+        <v>190</v>
       </c>
       <c r="D33" s="3" t="s">
         <v>24</v>
@@ -2874,7 +2879,7 @@
         <v>11</v>
       </c>
       <c r="G33" s="5" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="H33" s="3">
         <v>5</v>
@@ -2883,7 +2888,7 @@
         <v>2</v>
       </c>
       <c r="J33" s="4" t="s">
-        <v>207</v>
+        <v>191</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
@@ -2903,7 +2908,7 @@
         <v>28</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>173</v>
+        <v>157</v>
       </c>
       <c r="G34" s="5" t="s">
         <v>20</v>
@@ -2918,18 +2923,18 @@
         <v>21</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E35" s="3">
         <v>39</v>
@@ -2938,7 +2943,7 @@
         <v>11</v>
       </c>
       <c r="G35" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H35" s="3">
         <v>2</v>
@@ -2947,18 +2952,18 @@
         <v>0</v>
       </c>
       <c r="J35" s="4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B36" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C36" s="3" t="s">
         <v>26</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>27</v>
       </c>
       <c r="D36" s="3" t="s">
         <v>24</v>
@@ -2970,7 +2975,7 @@
         <v>19</v>
       </c>
       <c r="G36" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H36" s="3">
         <v>3</v>
@@ -2979,7 +2984,7 @@
         <v>0</v>
       </c>
       <c r="J36" s="4" t="s">
-        <v>29</v>
+        <v>234</v>
       </c>
     </row>
     <row r="37" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -2987,10 +2992,10 @@
         <v>15</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D37" s="3" t="s">
         <v>24</v>
@@ -2999,10 +3004,10 @@
         <v>2</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G37" s="6" t="s">
-        <v>164</v>
+        <v>152</v>
       </c>
       <c r="H37" s="3">
         <v>4</v>
@@ -3011,7 +3016,7 @@
         <v>0</v>
       </c>
       <c r="J37" s="4" t="s">
-        <v>33</v>
+        <v>237</v>
       </c>
     </row>
     <row r="38" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3043,7 +3048,7 @@
         <v>2</v>
       </c>
       <c r="J38" s="4" t="s">
-        <v>25</v>
+        <v>235</v>
       </c>
     </row>
     <row r="39" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -3051,13 +3056,13 @@
         <v>15</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E39" s="3">
         <v>54</v>
@@ -3066,7 +3071,7 @@
         <v>11</v>
       </c>
       <c r="G39" s="5" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="H39" s="3">
         <v>2</v>
@@ -3075,30 +3080,30 @@
         <v>2</v>
       </c>
       <c r="J39" s="4" t="s">
-        <v>169</v>
+        <v>236</v>
       </c>
     </row>
     <row r="40" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>174</v>
+        <v>158</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>175</v>
+        <v>159</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>162</v>
+        <v>150</v>
       </c>
       <c r="E40" s="3">
         <v>13</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>175</v>
+        <v>159</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>176</v>
+        <v>160</v>
       </c>
       <c r="H40" s="3">
         <v>0</v>
@@ -3107,21 +3112,21 @@
         <v>0</v>
       </c>
       <c r="J40" s="4" t="s">
-        <v>215</v>
+        <v>198</v>
       </c>
     </row>
     <row r="41" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>160</v>
+        <v>148</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>162</v>
+        <v>150</v>
       </c>
       <c r="E41" s="3">
         <v>30</v>
@@ -3130,7 +3135,7 @@
         <v>11</v>
       </c>
       <c r="G41" s="5" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="H41" s="3">
         <v>1</v>
@@ -3139,30 +3144,30 @@
         <v>0</v>
       </c>
       <c r="J41" s="4" t="s">
-        <v>163</v>
+        <v>151</v>
       </c>
     </row>
     <row r="42" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>240</v>
+        <v>221</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>237</v>
+        <v>218</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>162</v>
+        <v>150</v>
       </c>
       <c r="E42" s="3">
         <v>12</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="G42" s="5" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="H42" s="3">
         <v>2</v>
@@ -3171,30 +3176,30 @@
         <v>0</v>
       </c>
       <c r="J42" s="4" t="s">
-        <v>238</v>
+        <v>219</v>
       </c>
     </row>
     <row r="43" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>178</v>
+        <v>162</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>179</v>
+        <v>163</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>180</v>
+        <v>164</v>
       </c>
       <c r="E43" s="3">
         <v>46</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>181</v>
+        <v>165</v>
       </c>
       <c r="H43" s="3">
         <v>4</v>
@@ -3203,30 +3208,30 @@
         <v>0</v>
       </c>
       <c r="J43" s="4" t="s">
-        <v>191</v>
+        <v>175</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>182</v>
+        <v>166</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>186</v>
+        <v>170</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>180</v>
+        <v>164</v>
       </c>
       <c r="E44" s="3">
         <v>40</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>190</v>
+        <v>174</v>
       </c>
       <c r="H44" s="3">
         <v>6</v>
@@ -3235,30 +3240,30 @@
         <v>0</v>
       </c>
       <c r="J44" s="4" t="s">
-        <v>192</v>
+        <v>176</v>
       </c>
     </row>
     <row r="45" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>183</v>
+        <v>167</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>185</v>
+        <v>169</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>180</v>
+        <v>164</v>
       </c>
       <c r="E45" s="3">
         <v>41</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>189</v>
+        <v>173</v>
       </c>
       <c r="H45" s="3">
         <v>7</v>
@@ -3267,30 +3272,30 @@
         <v>0</v>
       </c>
       <c r="J45" s="4" t="s">
-        <v>193</v>
+        <v>177</v>
       </c>
     </row>
     <row r="46" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>184</v>
+        <v>168</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>187</v>
+        <v>171</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>180</v>
+        <v>164</v>
       </c>
       <c r="E46" s="3">
         <v>42</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>188</v>
+        <v>172</v>
       </c>
       <c r="H46" s="3">
         <v>8</v>
@@ -3299,21 +3304,21 @@
         <v>0</v>
       </c>
       <c r="J46" s="4" t="s">
-        <v>194</v>
+        <v>178</v>
       </c>
     </row>
     <row r="47" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>143</v>
+        <v>131</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>144</v>
+        <v>132</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>145</v>
+        <v>133</v>
       </c>
       <c r="E47" s="3">
         <v>74</v>
@@ -3322,7 +3327,7 @@
         <v>11</v>
       </c>
       <c r="G47" s="5" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="H47" s="3">
         <v>0</v>
@@ -3331,21 +3336,21 @@
         <v>2</v>
       </c>
       <c r="J47" s="4" t="s">
-        <v>168</v>
+        <v>155</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>146</v>
+        <v>134</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>147</v>
+        <v>135</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>145</v>
+        <v>133</v>
       </c>
       <c r="E48" s="3">
         <v>11</v>
@@ -3354,7 +3359,7 @@
         <v>11</v>
       </c>
       <c r="G48" s="5" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="H48" s="3">
         <v>1</v>
@@ -3363,21 +3368,21 @@
         <v>2</v>
       </c>
       <c r="J48" s="4" t="s">
-        <v>147</v>
+        <v>135</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>145</v>
+        <v>133</v>
       </c>
       <c r="E49" s="3">
         <v>66</v>
@@ -3386,7 +3391,7 @@
         <v>11</v>
       </c>
       <c r="G49" s="5" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="H49" s="3">
         <v>2</v>
@@ -3395,21 +3400,21 @@
         <v>2</v>
       </c>
       <c r="J49" s="4" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>150</v>
+        <v>138</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>151</v>
+        <v>139</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>145</v>
+        <v>133</v>
       </c>
       <c r="E50" s="3">
         <v>32</v>
@@ -3418,7 +3423,7 @@
         <v>11</v>
       </c>
       <c r="G50" s="5" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="H50" s="3">
         <v>3</v>
@@ -3427,21 +3432,21 @@
         <v>2</v>
       </c>
       <c r="J50" s="4" t="s">
-        <v>151</v>
+        <v>139</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>152</v>
+        <v>140</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>153</v>
+        <v>141</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>145</v>
+        <v>133</v>
       </c>
       <c r="E51" s="3">
         <v>25</v>
@@ -3450,7 +3455,7 @@
         <v>11</v>
       </c>
       <c r="G51" s="5" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="H51" s="3">
         <v>4</v>
@@ -3459,21 +3464,21 @@
         <v>2</v>
       </c>
       <c r="J51" s="4" t="s">
-        <v>153</v>
+        <v>141</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="B52" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="B52" s="3" t="s">
-        <v>154</v>
-      </c>
       <c r="C52" s="3" t="s">
-        <v>155</v>
+        <v>143</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>145</v>
+        <v>133</v>
       </c>
       <c r="E52" s="3">
         <v>34</v>
@@ -3482,7 +3487,7 @@
         <v>11</v>
       </c>
       <c r="G52" s="5" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="H52" s="3">
         <v>5</v>
@@ -3491,21 +3496,21 @@
         <v>2</v>
       </c>
       <c r="J52" s="4" t="s">
-        <v>155</v>
+        <v>143</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>156</v>
+        <v>144</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>145</v>
+        <v>133</v>
       </c>
       <c r="E53" s="3">
         <v>31</v>
@@ -3514,7 +3519,7 @@
         <v>11</v>
       </c>
       <c r="G53" s="5" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="H53" s="3">
         <v>6</v>
@@ -3523,21 +3528,21 @@
         <v>2</v>
       </c>
       <c r="J53" s="4" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>158</v>
+        <v>146</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>145</v>
+        <v>133</v>
       </c>
       <c r="E54" s="3">
         <v>61</v>
@@ -3546,7 +3551,7 @@
         <v>11</v>
       </c>
       <c r="G54" s="5" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="H54" s="3">
         <v>7</v>
@@ -3555,7 +3560,7 @@
         <v>2</v>
       </c>
       <c r="J54" s="4" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
     </row>
     <row r="55" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3563,7 +3568,7 @@
         <v>9</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>212</v>
+        <v>195</v>
       </c>
       <c r="D55" s="3" t="s">
         <v>24</v>
@@ -3581,7 +3586,7 @@
         <v>0</v>
       </c>
       <c r="J55" s="4" t="s">
-        <v>214</v>
+        <v>197</v>
       </c>
     </row>
     <row r="56" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3627,7 +3632,7 @@
         <v>0</v>
       </c>
       <c r="J57" s="4" t="s">
-        <v>171</v>
+        <v>156</v>
       </c>
     </row>
     <row r="58" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3635,7 +3640,7 @@
         <v>9</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="D58" s="3" t="s">
         <v>24</v>
@@ -3644,7 +3649,7 @@
         <v>76</v>
       </c>
       <c r="F58" s="3" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="G58" s="5"/>
       <c r="H58" s="3">
@@ -3654,18 +3659,18 @@
         <v>0</v>
       </c>
       <c r="J58" s="4" t="s">
-        <v>213</v>
+        <v>196</v>
       </c>
     </row>
     <row r="59" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="D59" s="3" t="s">
         <v>24</v>
@@ -3674,10 +3679,10 @@
         <v>68</v>
       </c>
       <c r="F59" s="3" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="G59" s="5" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="H59" s="3">
         <v>0</v>
@@ -3686,18 +3691,18 @@
         <v>0</v>
       </c>
       <c r="J59" s="4" t="s">
-        <v>165</v>
+        <v>246</v>
       </c>
     </row>
     <row r="60" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="D60" s="3" t="s">
         <v>24</v>
@@ -3706,10 +3711,10 @@
         <v>71</v>
       </c>
       <c r="F60" s="3" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="G60" s="5" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="H60" s="3">
         <v>1</v>
@@ -3718,18 +3723,18 @@
         <v>0</v>
       </c>
       <c r="J60" s="4" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
     </row>
     <row r="61" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="D61" s="3" t="s">
         <v>24</v>
@@ -3738,10 +3743,10 @@
         <v>67</v>
       </c>
       <c r="F61" s="3" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="G61" s="5" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="H61" s="3">
         <v>2</v>
@@ -3750,18 +3755,18 @@
         <v>0</v>
       </c>
       <c r="J61" s="4" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="62" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="D62" s="3" t="s">
         <v>24</v>
@@ -3770,10 +3775,10 @@
         <v>69</v>
       </c>
       <c r="F62" s="3" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="G62" s="5" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="H62" s="3">
         <v>3</v>
@@ -3782,18 +3787,18 @@
         <v>0</v>
       </c>
       <c r="J62" s="4" t="s">
-        <v>92</v>
+        <v>245</v>
       </c>
     </row>
     <row r="63" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="D63" s="3" t="s">
         <v>24</v>
@@ -3802,10 +3807,10 @@
         <v>47</v>
       </c>
       <c r="F63" s="3" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="G63" s="5" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="H63" s="3">
         <v>5</v>
@@ -3814,18 +3819,18 @@
         <v>0</v>
       </c>
       <c r="J63" s="4" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="64" spans="1:10" ht="300" x14ac:dyDescent="0.25">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" ht="360" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>225</v>
+        <v>207</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>226</v>
+        <v>208</v>
       </c>
       <c r="D64" s="3" t="s">
         <v>24</v>
@@ -3834,10 +3839,10 @@
         <v>70</v>
       </c>
       <c r="F64" s="3" t="s">
-        <v>227</v>
+        <v>209</v>
       </c>
       <c r="G64" s="5" t="s">
-        <v>205</v>
+        <v>189</v>
       </c>
       <c r="H64" s="3">
         <v>6</v>
@@ -3846,18 +3851,18 @@
         <v>0</v>
       </c>
       <c r="J64" s="4" t="s">
-        <v>262</v>
+        <v>248</v>
       </c>
     </row>
     <row r="65" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="D65" s="3" t="s">
         <v>24</v>
@@ -3866,10 +3871,10 @@
         <v>75</v>
       </c>
       <c r="F65" s="3" t="s">
-        <v>177</v>
+        <v>161</v>
       </c>
       <c r="G65" s="5" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
       <c r="H65" s="3">
         <v>8</v>
@@ -3878,18 +3883,18 @@
         <v>0</v>
       </c>
       <c r="J65" s="4" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="66" spans="1:10" ht="135" x14ac:dyDescent="0.25">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" ht="195" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="D66" s="3" t="s">
         <v>24</v>
@@ -3898,10 +3903,10 @@
         <v>44</v>
       </c>
       <c r="F66" s="3" t="s">
-        <v>208</v>
+        <v>192</v>
       </c>
       <c r="G66" s="5" t="s">
-        <v>209</v>
+        <v>193</v>
       </c>
       <c r="H66" s="3">
         <v>0</v>
@@ -3910,18 +3915,18 @@
         <v>2</v>
       </c>
       <c r="J66" s="8" t="s">
-        <v>210</v>
+        <v>251</v>
       </c>
     </row>
     <row r="67" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="D67" s="3" t="s">
         <v>24</v>
@@ -3930,10 +3935,10 @@
         <v>77</v>
       </c>
       <c r="F67" s="3" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="G67" s="5" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="H67" s="3">
         <v>1</v>
@@ -3942,18 +3947,18 @@
         <v>2</v>
       </c>
       <c r="J67" s="4" t="s">
-        <v>99</v>
+        <v>249</v>
       </c>
     </row>
     <row r="68" spans="1:10" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>197</v>
+        <v>181</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>198</v>
+        <v>182</v>
       </c>
       <c r="D68" s="3" t="s">
         <v>24</v>
@@ -3962,10 +3967,10 @@
         <v>27</v>
       </c>
       <c r="F68" s="3" t="s">
-        <v>200</v>
+        <v>184</v>
       </c>
       <c r="G68" s="5" t="s">
-        <v>199</v>
+        <v>183</v>
       </c>
       <c r="H68" s="3">
         <v>3</v>
@@ -3974,18 +3979,18 @@
         <v>2</v>
       </c>
       <c r="J68" s="4" t="s">
-        <v>264</v>
+        <v>252</v>
       </c>
     </row>
     <row r="69" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>195</v>
+        <v>179</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>196</v>
+        <v>180</v>
       </c>
       <c r="D69" s="3" t="s">
         <v>24</v>
@@ -3997,7 +4002,7 @@
         <v>11</v>
       </c>
       <c r="G69" s="5" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="H69" s="3">
         <v>4</v>
@@ -4006,18 +4011,18 @@
         <v>2</v>
       </c>
       <c r="J69" s="4" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="70" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>241</v>
+        <v>222</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>242</v>
+        <v>223</v>
       </c>
       <c r="D70" s="3" t="s">
         <v>24</v>
@@ -4026,10 +4031,10 @@
         <v>24</v>
       </c>
       <c r="F70" s="3" t="s">
-        <v>243</v>
+        <v>224</v>
       </c>
       <c r="G70" s="3" t="s">
-        <v>205</v>
+        <v>189</v>
       </c>
       <c r="H70" s="3">
         <v>5</v>
@@ -4038,7 +4043,7 @@
         <v>2</v>
       </c>
       <c r="J70" s="4" t="s">
-        <v>265</v>
+        <v>250</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Improved UMOVE and UCHOOSE issues: Changed MancalaUI::_refresh to activate all holes on non-players side (holes for which allowables was false were not being activated for seed movement). Changed RndChooseButtonBehavior::set_props to used the provided 'disable' instead of comparing to blocked property.
</commit_message>
<xml_diff>
--- a/src/game_params.xlsx
+++ b/src/game_params.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Activity_Data\Mancala_github\MancalaGames\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBE57CD2-5654-466B-91C6-2304A51FB51F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38E47652-3301-4DEE-AECC-EA08E89AE595}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -797,18 +797,6 @@
     <t>When a player has no allowable moves on their turn, they must pass, and continue to do so until they have allowable moves or the game is over. The game is over when there is a clear winner or tie condition, or when neither player has an allowable move.</t>
   </si>
   <si>
-    <t>Choose how holes are filled when a new round strarts:
-- NOT_APPLICABLE: round fill doesn't need to be specified: either not played in rounds or game goal is TERRITORY (all holes filled).
-- LEFT_FILL: fill holes from the player's left.
-- RIGHT_FILL: fill holes from the player's right. 
-- OUTSIDE_FILL: fill holes from the outside ends toward the middle.
-- EVEN_FILL: fill both sides with the same number of seeds per hole, determined by dividing the losers seeds by the number of holes per side. If that is not playable base on minimum move, extra seeds are put in each players leftmost hole. Any extra seeds are put in each player's store.
-- SHORTEN: shorten the board so that all of the loser's holes are filled; the winner will have more seeds in their store but the same board arrangement. If the game uses children, they will not be created if the board size is reduced to 3 or less.
-- UCHOOSE: allow user to choose which holes have seeds (are not blocked) when ROUNDS and BLOCKS are used.
-- UMOVE: allow the loser to choose where seeds are placed. At least one seed must be placed in each hole, remaining seeds are placed in the store. The winner's layout is the same layout but reflected.
-Note: These are not in numerical order.</t>
-  </si>
-  <si>
     <t>Is the game played in a series of rounds? In the case of a round win or tie  a new starter is determined via ROUND_STARTER and  the board is reset according to ROUND_FILL. BLOCKS are used in many games and set between rounds based on the seed placement.</t>
   </si>
   <si>
@@ -933,6 +921,18 @@
 - NONE: Nothing extra
 - PICKCROSS: Take the seeds from the opposite side of the board. 
 - PICKTWOS: Take seeds from all holes containing two seeds but only after the first move.</t>
+  </si>
+  <si>
+    <t>Choose how holes are filled when a new round strarts:
+- NOT_APPLICABLE: round fill doesn't need to be specified: either not played in rounds or game goal is TERRITORY (all holes filled).
+- LEFT_FILL: fill the round loser's holes from the player's left with NBR_START seeds each.  Holes that cannot be filled with NBR_START seeds (on the loser's side) are left empty; if BLOCKS is selected they are out of play for the round. All winner's holes are filled and are in play.
+- RIGHT_FILL: fill holes from the player's right. Other dynamics mimic left_fill.
+- OUTSIDE_FILL: fill holes from the outside ends toward the middle. Other dynamics mimic left_fill.
+- EVEN_FILL: fill all holes (both sides) with the same number of seeds; determined by dividing the losers seeds by the number of holes per side. If that is not playable based on the minimum number of seeds required for a move (MIN_MOVE); extra seeds are put in each players leftmost hole. Any extra seeds are put in each player's store.
+- SHORTEN: the number of holes that the round loser can fill with NBR_START seeds are fill on both sides, other holes are left empty. Holes are filled opposite eachother. If BLOCKS is selected, the board is shortened to the number of holes filled (empty holes are blocked and out of play). If the game uses children, they will not be created if the board size is reduced to 3 or less.
+- UCHOOSE: allow user to choose which holes have seeds (are not blocked) when ROUNDS and BLOCKS are used.
+- UMOVE: allow the loser to choose where seeds are placed. At least one seed must be placed in each hole and the game must be playable (at least one hole has MIN_MOVE seeds), remaining seeds are placed in the store. The winner's layout is the same layout but reflected.
+Note: These are not in numerical order.</t>
   </si>
 </sst>
 </file>
@@ -1817,8 +1817,8 @@
   <dimension ref="A1:J70"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F22" sqref="F22"/>
+      <pane ySplit="1" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K27" sqref="K27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1928,7 +1928,7 @@
         <v>0</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="345" x14ac:dyDescent="0.25">
@@ -1960,7 +1960,7 @@
         <v>0</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -1992,7 +1992,7 @@
         <v>0</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -2088,7 +2088,7 @@
         <v>0</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -2120,7 +2120,7 @@
         <v>0</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -2152,7 +2152,7 @@
         <v>0</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -2184,7 +2184,7 @@
         <v>0</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="225" x14ac:dyDescent="0.25">
@@ -2216,7 +2216,7 @@
         <v>0</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -2248,7 +2248,7 @@
         <v>2</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -2344,7 +2344,7 @@
         <v>2</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2376,7 +2376,7 @@
         <v>2</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2440,7 +2440,7 @@
         <v>2</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -2472,7 +2472,7 @@
         <v>2</v>
       </c>
       <c r="J20" s="4" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2504,7 +2504,7 @@
         <v>2</v>
       </c>
       <c r="J21" s="4" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -2536,7 +2536,7 @@
         <v>2</v>
       </c>
       <c r="J22" s="4" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
@@ -2632,7 +2632,7 @@
         <v>0</v>
       </c>
       <c r="J25" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="105" x14ac:dyDescent="0.25">
@@ -2667,7 +2667,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="345" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>38</v>
       </c>
@@ -2696,7 +2696,7 @@
         <v>0</v>
       </c>
       <c r="J27" s="4" t="s">
-        <v>241</v>
+        <v>265</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="105" x14ac:dyDescent="0.25">
@@ -3691,7 +3691,7 @@
         <v>0</v>
       </c>
       <c r="J59" s="4" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="60" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3787,7 +3787,7 @@
         <v>0</v>
       </c>
       <c r="J62" s="4" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="63" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -3819,7 +3819,7 @@
         <v>0</v>
       </c>
       <c r="J63" s="4" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="64" spans="1:10" ht="360" x14ac:dyDescent="0.25">
@@ -3851,7 +3851,7 @@
         <v>0</v>
       </c>
       <c r="J64" s="4" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="65" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -3915,7 +3915,7 @@
         <v>2</v>
       </c>
       <c r="J66" s="8" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="67" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3947,7 +3947,7 @@
         <v>2</v>
       </c>
       <c r="J67" s="4" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="68" spans="1:10" ht="409.5" x14ac:dyDescent="0.25">
@@ -3979,7 +3979,7 @@
         <v>2</v>
       </c>
       <c r="J68" s="4" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="69" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -4043,7 +4043,7 @@
         <v>2</v>
       </c>
       <c r="J70" s="4" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed ChildType.OneChild to not enforce the OPP_ONLY rule. Added OPP_ONLY rule to tuzdek game and tests. Changed ChildType.Walda to use the make_child deco, so that opp_only can be used with it. Opp_only with WALDAs severely limits potential walda locations.
</commit_message>
<xml_diff>
--- a/src/game_params.xlsx
+++ b/src/game_params.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Activity_Data\Mancala_github\MancalaGames\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38E47652-3301-4DEE-AECC-EA08E89AE595}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{231E9220-471E-4484-A8B4-A7335D7425CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -841,27 +841,10 @@
     <t>Sow is multiplap only if the first sow (seeds from the starting hole) reaches the opponents side of the board.</t>
   </si>
   <si>
-    <t>Addiitonal child creation requirements may be set:
-- NONE: no additional restrictions.
-- OPP_ONLY:  Only make children on the opposite side or in opponent's territory. Incompatible with BULL, QUR, and WEG child types.
-- NOT_1ST_OPP: Don't make a child in the first hole on the opponents side/territory with one seed.</t>
-  </si>
-  <si>
     <t>Determines if seeds from more the start hole are picked up and sown:
 - OFF: Single lap sowing. Seeds from the start hole are sown, typically, one per hole until expened.
 - LAPPER:  If the first sow ends in a hole with more than one seed, pickup all the seeds and continue sowing another lap. Continue until the final seed of a lap reaches an empty hole, unless there is another rule that stops the sowing (e.g. making a child).
 - LAPPER_NEXT:  If the first sow ends in a hole preceeding a hole with any seeds, pick up the seeds from that next hole and continue sowing another lap. Continue until the hole after the laps final seed is empty.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Games with children allow players to claim holes. These child holes are an extension of the stores and seeds in them count towards a win. Making a child stops any multiple lap sowing, moves cannot start from children, and they cannot be captured.
-- NOCHILD: children are not used.
-- NORMAL: children are made when a final seeds sows a hole to CHILD_CVT.
-- WALDA: Stores are not supported. Captures are instead moved into waldas, thus a player may not capture until they have created a walda. Child locations are limited.  Each player may create up to 6 waldas: on either end of each side of the board and the next outer hole on their own side of the board. Note that there are only 8 total places that waldas maybe created.
-- ONE_CHILD: Use the tuzdek rules for children: only one child allowed on opponent's side of the board, may not be in player's left most hole,  and may not be opposite eachother.
-- WEG: children maybe created in holes owned by the opponent. Ending a sow in an opponent's weg captures the seed just sown and one more (if there is one); generally, the player get's to play again (per CAPT_RTURN). WEGs are supported for TERRITORY games only (hole ownership required).
-- BULL: create one bull if final seed sows to CHILD_CVT, create two bulls if the final two seeds are sown to CHILD_CVT-1 and CHILD_CVT (in either order).
-- QUR: when a seed is sown into an empty hole on the player's side of the board and the opposite hole contains CHILD_CVT, create children in both holes: final seed location and opposite.
-</t>
   </si>
   <si>
     <t>Only meaninful, with MULTICAPT. Captures are done in the same direction as the sowing, i.e. following the final hole sown. If not set, captures are done from the holes just sown.</t>
@@ -933,6 +916,23 @@
 - UCHOOSE: allow user to choose which holes have seeds (are not blocked) when ROUNDS and BLOCKS are used.
 - UMOVE: allow the loser to choose where seeds are placed. At least one seed must be placed in each hole and the game must be playable (at least one hole has MIN_MOVE seeds), remaining seeds are placed in the store. The winner's layout is the same layout but reflected.
 Note: These are not in numerical order.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Games with children allow players to claim holes. These child holes are an extension of the stores and seeds in them count towards a win. Making a child stops any multiple lap sowing, moves cannot start from children, and they cannot be captured.
+- NOCHILD: children are not used.
+- NORMAL: children are made when a final seeds sows a hole to CHILD_CVT.
+- WALDA: Stores are not supported. Captures are instead moved into waldas, thus a player may not capture until they have created a walda. Child locations are limited.  Each player may create up to 6 waldas: on either end of each side of the board and the next outer hole on their own side of the board. Note that there are only 8 total places that waldas maybe created.
+- ONE_CHILD: only one child allowed per player, may not be in player's left most hole,  and may not be opposite eachother. Used to create tuzdek style children along with CHILD_RULE of OPP_ONLY.
+- WEG: children maybe created in holes owned by the opponent. Ending a sow in an opponent's weg captures the seed just sown and one more (if there is one); generally, the player get's to play again (per CAPT_RTURN). WEGs are supported for TERRITORY games only (hole ownership required).
+- BULL: create one bull if final seed sows to CHILD_CVT, create two bulls if the final two seeds are sown to CHILD_CVT-1 and CHILD_CVT (in either order).
+- QUR: when a seed is sown into an empty hole on the player's side of the board and the opposite hole contains CHILD_CVT, create children in both holes: final seed location and opposite.
+</t>
+  </si>
+  <si>
+    <t>Addiitonal child creation requirements may be set:
+- NONE: no additional restrictions.
+- OPP_ONLY:  Only make children on the opposite side of the board. Incompatible with BULL, QUR, and WEG child types.
+- NOT_1ST_OPP: Don't make a child in the first hole on the opponents side/territory with one seed.</t>
   </si>
 </sst>
 </file>
@@ -1817,8 +1817,8 @@
   <dimension ref="A1:J70"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K27" sqref="K27"/>
+      <pane ySplit="1" topLeftCell="A67" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J70" sqref="J70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1992,7 +1992,7 @@
         <v>0</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -2088,7 +2088,7 @@
         <v>0</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -2120,7 +2120,7 @@
         <v>0</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -2152,7 +2152,7 @@
         <v>0</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -2184,7 +2184,7 @@
         <v>0</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="225" x14ac:dyDescent="0.25">
@@ -2216,7 +2216,7 @@
         <v>0</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -2248,7 +2248,7 @@
         <v>2</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -2344,7 +2344,7 @@
         <v>2</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2376,7 +2376,7 @@
         <v>2</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2440,7 +2440,7 @@
         <v>2</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -2472,7 +2472,7 @@
         <v>2</v>
       </c>
       <c r="J20" s="4" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2504,7 +2504,7 @@
         <v>2</v>
       </c>
       <c r="J21" s="4" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -2536,7 +2536,7 @@
         <v>2</v>
       </c>
       <c r="J22" s="4" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
@@ -2696,7 +2696,7 @@
         <v>0</v>
       </c>
       <c r="J27" s="4" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="105" x14ac:dyDescent="0.25">
@@ -3915,7 +3915,7 @@
         <v>2</v>
       </c>
       <c r="J66" s="8" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="67" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3979,7 +3979,7 @@
         <v>2</v>
       </c>
       <c r="J68" s="4" t="s">
-        <v>251</v>
+        <v>264</v>
       </c>
     </row>
     <row r="69" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -4014,7 +4014,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="70" spans="1:10" ht="105" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
         <v>69</v>
       </c>
@@ -4043,7 +4043,7 @@
         <v>2</v>
       </c>
       <c r="J70" s="4" t="s">
-        <v>249</v>
+        <v>265</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Reordered RoundFill to be in a logical order.
</commit_message>
<xml_diff>
--- a/src/game_params.xlsx
+++ b/src/game_params.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Activity_Data\Mancala_github\MancalaGames\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{231E9220-471E-4484-A8B4-A7335D7425CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E57753B7-0AD8-49C0-8ED2-F4781E7F678B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-45" yWindow="30" windowWidth="28770" windowHeight="16170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="game_params" sheetId="1" r:id="rId1"/>
@@ -906,18 +906,6 @@
 - PICKTWOS: Take seeds from all holes containing two seeds but only after the first move.</t>
   </si>
   <si>
-    <t>Choose how holes are filled when a new round strarts:
-- NOT_APPLICABLE: round fill doesn't need to be specified: either not played in rounds or game goal is TERRITORY (all holes filled).
-- LEFT_FILL: fill the round loser's holes from the player's left with NBR_START seeds each.  Holes that cannot be filled with NBR_START seeds (on the loser's side) are left empty; if BLOCKS is selected they are out of play for the round. All winner's holes are filled and are in play.
-- RIGHT_FILL: fill holes from the player's right. Other dynamics mimic left_fill.
-- OUTSIDE_FILL: fill holes from the outside ends toward the middle. Other dynamics mimic left_fill.
-- EVEN_FILL: fill all holes (both sides) with the same number of seeds; determined by dividing the losers seeds by the number of holes per side. If that is not playable based on the minimum number of seeds required for a move (MIN_MOVE); extra seeds are put in each players leftmost hole. Any extra seeds are put in each player's store.
-- SHORTEN: the number of holes that the round loser can fill with NBR_START seeds are fill on both sides, other holes are left empty. Holes are filled opposite eachother. If BLOCKS is selected, the board is shortened to the number of holes filled (empty holes are blocked and out of play). If the game uses children, they will not be created if the board size is reduced to 3 or less.
-- UCHOOSE: allow user to choose which holes have seeds (are not blocked) when ROUNDS and BLOCKS are used.
-- UMOVE: allow the loser to choose where seeds are placed. At least one seed must be placed in each hole and the game must be playable (at least one hole has MIN_MOVE seeds), remaining seeds are placed in the store. The winner's layout is the same layout but reflected.
-Note: These are not in numerical order.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Games with children allow players to claim holes. These child holes are an extension of the stores and seeds in them count towards a win. Making a child stops any multiple lap sowing, moves cannot start from children, and they cannot be captured.
 - NOCHILD: children are not used.
 - NORMAL: children are made when a final seeds sows a hole to CHILD_CVT.
@@ -933,6 +921,17 @@
 - NONE: no additional restrictions.
 - OPP_ONLY:  Only make children on the opposite side of the board. Incompatible with BULL, QUR, and WEG child types.
 - NOT_1ST_OPP: Don't make a child in the first hole on the opponents side/territory with one seed.</t>
+  </si>
+  <si>
+    <t>Choose how holes are filled when a new round strarts:
+- NOT_APPLICABLE: round fill doesn't need to be specified: either not played in rounds or game goal is TERRITORY (all holes filled).
+- LEFT_FILL: fill the round loser's holes from the player's left with NBR_START seeds each.  Holes that cannot be filled with NBR_START seeds (on the loser's side) are left empty; if BLOCKS is selected they are out of play for the round. All winner's holes are filled and are in play.
+- RIGHT_FILL: fill holes from the player's right. Other dynamics mimic left_fill.
+- OUTSIDE_FILL: fill holes from the outside ends toward the middle. Other dynamics mimic left_fill.
+- EVEN_FILL: fill all holes (both sides) with the same number of seeds; determined by dividing the losers seeds by the number of holes per side. If that is not playable based on the minimum number of seeds required for a move (MIN_MOVE); extra seeds are put in each players leftmost hole. Any extra seeds are put in each player's store.
+- SHORTEN: the number of holes that the round loser can fill with NBR_START seeds are fill on both sides, other holes are left empty. Holes are filled opposite eachother. If BLOCKS is selected, the board is shortened to the number of holes filled (empty holes are blocked and out of play). If the game uses children, they will not be created if the board size is reduced to 3 or less.
+- UCHOOSE: allow user to choose which holes have seeds (are not blocked) when ROUNDS and BLOCKS are used.
+- UMOVE: allow the loser to choose where seeds are placed. At least one seed must be placed in each hole and the game must be playable (at least one hole has MIN_MOVE seeds), remaining seeds are placed in the store. The winner's layout is the same layout but reflected.</t>
   </si>
 </sst>
 </file>
@@ -1817,8 +1816,8 @@
   <dimension ref="A1:J70"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A67" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J70" sqref="J70"/>
+      <pane ySplit="1" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2696,7 +2695,7 @@
         <v>0</v>
       </c>
       <c r="J27" s="4" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="105" x14ac:dyDescent="0.25">
@@ -3979,7 +3978,7 @@
         <v>2</v>
       </c>
       <c r="J68" s="4" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="69" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -4043,7 +4042,7 @@
         <v>2</v>
       </c>
       <c r="J70" s="4" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Reordered SowRule to be in a logical order and completed parameter description.
</commit_message>
<xml_diff>
--- a/src/game_params.xlsx
+++ b/src/game_params.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Activity_Data\Mancala_github\MancalaGames\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E57753B7-0AD8-49C0-8ED2-F4781E7F678B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A479626-805B-4E25-A6DD-8F084D079356}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-45" yWindow="30" windowWidth="28770" windowHeight="16170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="735" yWindow="195" windowWidth="28770" windowHeight="16170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="game_params" sheetId="1" r:id="rId1"/>
@@ -828,16 +828,6 @@
     <t>Only valid when SOW_START is set. Changes the SOW_START behavior so that if there is only one seed in the hole, it is moved in the sow direction by one hole.</t>
   </si>
   <si>
-    <t>Special sow rules may additional behavior or restrictions to the sowing phase:
-- NONE: there is no special sowing rules.
-- SOW_BLKD_DIV: Holes sown to GPARAM_ONE are closed (blocked) and the hole's seeds are removed from play. Blocked holes on own side are skipped when sowing and blocked holes on opp side are diverted out of play or captured. GOAL must be DEPRIVE.
-- SOW_BLKD_DIV_NR: Behaves the same as SOW_BLKD_DIV except that each player's rightmost hole cannot be closed. GOAL must be DEPRIVE.
-- OWN_SOW_CAPT_ALL: Capture all holes that are sown that meet the simple capture criteria: evens, min, max and  capture on. Other criteria are enforced: side of the board, unlocked, and not child.   GRANDSLAM rules are not applied. If the game GOAL is TERRITORY the capturer is the hole owner; otherwise the capturer is done by side. NOCAPTFIRST prevents this capture for the first move.
-- SOW_SOW_CAPT_ALL: Capture all holes that sown that meed the simple capture criteria only on the SOWER's side of the board. NOCAPTFIRST prevents this capture for the first move.
-- NO_SOW_OPP_2S: Don't sow into opponents holes with 2 seeds.
-Note: These are not in numerical order.</t>
-  </si>
-  <si>
     <t>Sow is multiplap only if the first sow (seeds from the starting hole) reaches the opponents side of the board.</t>
   </si>
   <si>
@@ -932,6 +922,16 @@
 - SHORTEN: the number of holes that the round loser can fill with NBR_START seeds are fill on both sides, other holes are left empty. Holes are filled opposite eachother. If BLOCKS is selected, the board is shortened to the number of holes filled (empty holes are blocked and out of play). If the game uses children, they will not be created if the board size is reduced to 3 or less.
 - UCHOOSE: allow user to choose which holes have seeds (are not blocked) when ROUNDS and BLOCKS are used.
 - UMOVE: allow the loser to choose where seeds are placed. At least one seed must be placed in each hole and the game must be playable (at least one hole has MIN_MOVE seeds), remaining seeds are placed in the store. The winner's layout is the same layout but reflected.</t>
+  </si>
+  <si>
+    <t>Special sow rules may additional behavior or restrictions to the sowing phase:
+- NONE: there is no special sowing rules.
+- SOW_BLKD_DIV: Holes sown to GPARAM_ONE are closed (blocked) and the hole's seeds are removed from play. Blocked holes on own side are skipped when sowing and blocked holes on opp side are diverted out of play or captured. GOAL must be DEPRIVE.
+- SOW_BLKD_DIV_NR: Behaves the same as SOW_BLKD_DIV except that each player's rightmost hole cannot be closed. GOAL must be DEPRIVE.
+- OWN_SOW_CAPT_ALL: Capture all holes that are sown that meet the simple capture criteria: evens, min, max and  capture on. Other criteria are enforced: side of the board, unlocked, and not child.   GRANDSLAM rules are not applied. If the game GOAL is TERRITORY the capturer is the hole owner; otherwise the capturer is done by side. NOCAPTFIRST prevents this capture for the first move.
+- SOW_SOW_CAPT_ALL: Capture all holes that sown that meed the simple capture criteria only on the SOWER's side of the board. NOCAPTFIRST prevents this capture for the first move.
+- NO_SOW_OPP_2S: Don't sow into opponents holes with 2 seeds.
+- CHANGE_DIR_LAP: Change the direction for each lap sown. Generally used with UDIR_HOLES so the player may choose the first direction.</t>
   </si>
 </sst>
 </file>
@@ -1816,8 +1816,8 @@
   <dimension ref="A1:J70"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J27" sqref="J27"/>
+      <pane ySplit="1" topLeftCell="A61" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J64" sqref="J64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1991,7 +1991,7 @@
         <v>0</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -2087,7 +2087,7 @@
         <v>0</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -2119,7 +2119,7 @@
         <v>0</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -2151,7 +2151,7 @@
         <v>0</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -2183,7 +2183,7 @@
         <v>0</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="225" x14ac:dyDescent="0.25">
@@ -2215,7 +2215,7 @@
         <v>0</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -2247,7 +2247,7 @@
         <v>2</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -2343,7 +2343,7 @@
         <v>2</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2375,7 +2375,7 @@
         <v>2</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2439,7 +2439,7 @@
         <v>2</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -2471,7 +2471,7 @@
         <v>2</v>
       </c>
       <c r="J20" s="4" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2503,7 +2503,7 @@
         <v>2</v>
       </c>
       <c r="J21" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -2535,7 +2535,7 @@
         <v>2</v>
       </c>
       <c r="J22" s="4" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
@@ -2695,7 +2695,7 @@
         <v>0</v>
       </c>
       <c r="J27" s="4" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="105" x14ac:dyDescent="0.25">
@@ -3821,7 +3821,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="64" spans="1:10" ht="360" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" ht="390" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
         <v>69</v>
       </c>
@@ -3850,7 +3850,7 @@
         <v>0</v>
       </c>
       <c r="J64" s="4" t="s">
-        <v>247</v>
+        <v>265</v>
       </c>
     </row>
     <row r="65" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -3914,7 +3914,7 @@
         <v>2</v>
       </c>
       <c r="J66" s="8" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="67" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3946,7 +3946,7 @@
         <v>2</v>
       </c>
       <c r="J67" s="4" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="68" spans="1:10" ht="409.5" x14ac:dyDescent="0.25">
@@ -3978,7 +3978,7 @@
         <v>2</v>
       </c>
       <c r="J68" s="4" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="69" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -4042,7 +4042,7 @@
         <v>2</v>
       </c>
       <c r="J70" s="4" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Corrected xc_sown to only require that the opposite side of the board has been sown (not the cross hole as the previous incorrect implementation).
</commit_message>
<xml_diff>
--- a/src/game_params.xlsx
+++ b/src/game_params.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Activity_Data\Mancala_github\MancalaGames\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A479626-805B-4E25-A6DD-8F084D079356}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BA855D8-C75E-434F-A368-44E9509FD01A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="735" yWindow="195" windowWidth="28770" windowHeight="16170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29190" yWindow="30" windowWidth="24690" windowHeight="16170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="game_params" sheetId="1" r:id="rId1"/>
@@ -761,10 +761,6 @@
 TWOEMPTY: all but the rightmost two holes for each player are filled with is nbr_seeds.</t>
   </si>
   <si>
-    <t>Only allow cross capture if the player has sown into the hole on the opposite side of board (the one to be captured from). 
-If a player ends on their own side of the board in an empty hole, but did not sow any opposite hole, the get a repeat turn.</t>
-  </si>
-  <si>
     <t xml:space="preserve">The overall goal of the game. Defines how a player wins.
 - MAX_SEEDS: player with the maximum number of seeds at the end of the game wins or they collect more than half of the total seeds
 - DEPRIVE: eliminate all of your opponents seeds. 
@@ -932,6 +928,10 @@
 - SOW_SOW_CAPT_ALL: Capture all holes that sown that meed the simple capture criteria only on the SOWER's side of the board. NOCAPTFIRST prevents this capture for the first move.
 - NO_SOW_OPP_2S: Don't sow into opponents holes with 2 seeds.
 - CHANGE_DIR_LAP: Change the direction for each lap sown. Generally used with UDIR_HOLES so the player may choose the first direction.</t>
+  </si>
+  <si>
+    <t>Only allow cross capture if the player has sown onto the opposite side of board. 
+If a player ends on their own side of the board in an empty hole, but did not sow any opposite hole, they get a repeat turn.</t>
   </si>
 </sst>
 </file>
@@ -1816,8 +1816,8 @@
   <dimension ref="A1:J70"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A61" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J64" sqref="J64"/>
+      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1927,7 +1927,7 @@
         <v>0</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="345" x14ac:dyDescent="0.25">
@@ -1959,7 +1959,7 @@
         <v>0</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -1991,7 +1991,7 @@
         <v>0</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -2087,7 +2087,7 @@
         <v>0</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -2119,7 +2119,7 @@
         <v>0</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -2151,7 +2151,7 @@
         <v>0</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -2183,7 +2183,7 @@
         <v>0</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="225" x14ac:dyDescent="0.25">
@@ -2215,7 +2215,7 @@
         <v>0</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -2247,7 +2247,7 @@
         <v>2</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -2279,7 +2279,7 @@
         <v>2</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>232</v>
+        <v>265</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="105" x14ac:dyDescent="0.25">
@@ -2343,7 +2343,7 @@
         <v>2</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2375,7 +2375,7 @@
         <v>2</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2439,7 +2439,7 @@
         <v>2</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -2471,7 +2471,7 @@
         <v>2</v>
       </c>
       <c r="J20" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2503,7 +2503,7 @@
         <v>2</v>
       </c>
       <c r="J21" s="4" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -2535,7 +2535,7 @@
         <v>2</v>
       </c>
       <c r="J22" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
@@ -2567,7 +2567,7 @@
         <v>0</v>
       </c>
       <c r="J23" s="4" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -2599,7 +2599,7 @@
         <v>0</v>
       </c>
       <c r="J24" s="4" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -2631,7 +2631,7 @@
         <v>0</v>
       </c>
       <c r="J25" s="4" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="105" x14ac:dyDescent="0.25">
@@ -2695,7 +2695,7 @@
         <v>0</v>
       </c>
       <c r="J27" s="4" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="105" x14ac:dyDescent="0.25">
@@ -2759,7 +2759,7 @@
         <v>2</v>
       </c>
       <c r="J29" s="4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2951,7 +2951,7 @@
         <v>0</v>
       </c>
       <c r="J35" s="4" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="36" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2983,7 +2983,7 @@
         <v>0</v>
       </c>
       <c r="J36" s="4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="37" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -3015,7 +3015,7 @@
         <v>0</v>
       </c>
       <c r="J37" s="4" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="38" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3047,7 +3047,7 @@
         <v>2</v>
       </c>
       <c r="J38" s="4" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="39" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -3079,7 +3079,7 @@
         <v>2</v>
       </c>
       <c r="J39" s="4" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="40" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -3690,7 +3690,7 @@
         <v>0</v>
       </c>
       <c r="J59" s="4" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="60" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3786,7 +3786,7 @@
         <v>0</v>
       </c>
       <c r="J62" s="4" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="63" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -3818,7 +3818,7 @@
         <v>0</v>
       </c>
       <c r="J63" s="4" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="64" spans="1:10" ht="390" x14ac:dyDescent="0.25">
@@ -3850,7 +3850,7 @@
         <v>0</v>
       </c>
       <c r="J64" s="4" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="65" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -3914,7 +3914,7 @@
         <v>2</v>
       </c>
       <c r="J66" s="8" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="67" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3946,7 +3946,7 @@
         <v>2</v>
       </c>
       <c r="J67" s="4" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="68" spans="1:10" ht="409.5" x14ac:dyDescent="0.25">
@@ -3978,7 +3978,7 @@
         <v>2</v>
       </c>
       <c r="J68" s="4" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="69" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -4042,7 +4042,7 @@
         <v>2</v>
       </c>
       <c r="J70" s="4" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Giuthi and Pandi game tests (full game level integration tests). Pandi test revealed errors and missing implementation in SowRule for OWN_SOW_CAPT_ALL and SOW_SOW_CAPT_ALL. Fixed coded and updated unit tests. Added separate paragraphs to bulleted lists build_docs.py and cleaned up some of the parameter descriptions with them.
</commit_message>
<xml_diff>
--- a/src/game_params.xlsx
+++ b/src/game_params.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Activity_Data\Mancala_github\MancalaGames\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BA855D8-C75E-434F-A368-44E9509FD01A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{487355B8-0AD8-4EDE-B84D-DF21D2B51367}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29190" yWindow="30" windowWidth="24690" windowHeight="16170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4335" yWindow="555" windowWidth="23415" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="game_params" sheetId="1" r:id="rId1"/>
@@ -761,16 +761,6 @@
 TWOEMPTY: all but the rightmost two holes for each player are filled with is nbr_seeds.</t>
   </si>
   <si>
-    <t xml:space="preserve">The overall goal of the game. Defines how a player wins.
-- MAX_SEEDS: player with the maximum number of seeds at the end of the game wins or they collect more than half of the total seeds
-- DEPRIVE: eliminate all of your opponents seeds. 
-GRAND_SLAM must be legal for DEPRIVE games.
-The following options are incompatible with DEPRIVE games: MOVEUNLOCK, MUSTPASS, MUSTSHARE, ROUNDS, ROUND_STARTER, ROUND_FILL, NO_SIDES, SKIP_START, SOW_OWN_STORE, STORES, SOW_START, VISIT_OPP. 
-- TERRITORY: claim ownership of holes. Each round the ownership of holes is determined by the number of seeds captured in the previous round. In a TERRITORY game without rounds, the winner is the player that gained the most territory during play. 
-TERRITORY games require STORES and that GPARAM_ONE be set to a value between the number of holes and two times the number of holes.
-TERRITORY games are incompatible with NO_SIDES, START_PATTERN, GRANDSLAM of NOT_LEGAL, ALLOW_RULE of OPP_OR_EMPTY, </t>
-  </si>
-  <si>
     <t>An html help file describing the game (mancala_help.html is the main help file).</t>
   </si>
   <si>
@@ -892,17 +882,6 @@
 - PICKTWOS: Take seeds from all holes containing two seeds but only after the first move.</t>
   </si>
   <si>
-    <t xml:space="preserve">Games with children allow players to claim holes. These child holes are an extension of the stores and seeds in them count towards a win. Making a child stops any multiple lap sowing, moves cannot start from children, and they cannot be captured.
-- NOCHILD: children are not used.
-- NORMAL: children are made when a final seeds sows a hole to CHILD_CVT.
-- WALDA: Stores are not supported. Captures are instead moved into waldas, thus a player may not capture until they have created a walda. Child locations are limited.  Each player may create up to 6 waldas: on either end of each side of the board and the next outer hole on their own side of the board. Note that there are only 8 total places that waldas maybe created.
-- ONE_CHILD: only one child allowed per player, may not be in player's left most hole,  and may not be opposite eachother. Used to create tuzdek style children along with CHILD_RULE of OPP_ONLY.
-- WEG: children maybe created in holes owned by the opponent. Ending a sow in an opponent's weg captures the seed just sown and one more (if there is one); generally, the player get's to play again (per CAPT_RTURN). WEGs are supported for TERRITORY games only (hole ownership required).
-- BULL: create one bull if final seed sows to CHILD_CVT, create two bulls if the final two seeds are sown to CHILD_CVT-1 and CHILD_CVT (in either order).
-- QUR: when a seed is sown into an empty hole on the player's side of the board and the opposite hole contains CHILD_CVT, create children in both holes: final seed location and opposite.
-</t>
-  </si>
-  <si>
     <t>Addiitonal child creation requirements may be set:
 - NONE: no additional restrictions.
 - OPP_ONLY:  Only make children on the opposite side of the board. Incompatible with BULL, QUR, and WEG child types.
@@ -920,18 +899,45 @@
 - UMOVE: allow the loser to choose where seeds are placed. At least one seed must be placed in each hole and the game must be playable (at least one hole has MIN_MOVE seeds), remaining seeds are placed in the store. The winner's layout is the same layout but reflected.</t>
   </si>
   <si>
+    <t>Only allow cross capture if the player has sown onto the opposite side of board. 
+If a player ends on their own side of the board in an empty hole, but did not sow any opposite hole, they get a repeat turn.</t>
+  </si>
+  <si>
     <t>Special sow rules may additional behavior or restrictions to the sowing phase:
 - NONE: there is no special sowing rules.
 - SOW_BLKD_DIV: Holes sown to GPARAM_ONE are closed (blocked) and the hole's seeds are removed from play. Blocked holes on own side are skipped when sowing and blocked holes on opp side are diverted out of play or captured. GOAL must be DEPRIVE.
 - SOW_BLKD_DIV_NR: Behaves the same as SOW_BLKD_DIV except that each player's rightmost hole cannot be closed. GOAL must be DEPRIVE.
-- OWN_SOW_CAPT_ALL: Capture all holes that are sown that meet the simple capture criteria: evens, min, max and  capture on. Other criteria are enforced: side of the board, unlocked, and not child.   GRANDSLAM rules are not applied. If the game GOAL is TERRITORY the capturer is the hole owner; otherwise the capturer is done by side. NOCAPTFIRST prevents this capture for the first move.
-- SOW_SOW_CAPT_ALL: Capture all holes that sown that meed the simple capture criteria only on the SOWER's side of the board. NOCAPTFIRST prevents this capture for the first move.
+- OWN_SOW_CAPT_ALL: The hole OWNer captures all holes that are sown to meet the simple capture criteria: evens, min, max and capture on. Other criteria are enforced: side of the board, unlocked, and not child.
+  + The capture is done by the hole owner, so the non-sower may capture seeds during their opponents sowing. If the game GOAL is TERRITORY the capturer is the hole owner; otherwise each player captures from their own side of the board no matter who is sowing. 
+  + If mlaps is LAPPER and the final seed sown for any lap meets the capture criteria, the contents of the hole are captured by the sower and not the hole owner and the turn is over.
+  + GRANDSLAM rules are not applied. NOCAPTFIRST prevents this capture for the first move.
+- SOW_SOW_CAPT_ALL: Similar to OWN_SOW_CAPT_ALL but only the SOWer captures seeds from their opponent's holes. 
+  + If mlaps is LAPPER and the final seed sown for any lap meets the capture criteria, the contents of the hole are captured by the sower and not the hole owner and the turn is over.
+  + GRANDSLAM rules are not applied. NOCAPTFIRST prevents this capture for the first move.
 - NO_SOW_OPP_2S: Don't sow into opponents holes with 2 seeds.
 - CHANGE_DIR_LAP: Change the direction for each lap sown. Generally used with UDIR_HOLES so the player may choose the first direction.</t>
   </si>
   <si>
-    <t>Only allow cross capture if the player has sown onto the opposite side of board. 
-If a player ends on their own side of the board in an empty hole, but did not sow any opposite hole, they get a repeat turn.</t>
+    <t xml:space="preserve">The overall goal of the game. Defines how a player wins.
+- MAX_SEEDS: player with the maximum number of seeds at the end of the game wins or they collect more than half of the total seeds
+- DEPRIVE: eliminate all of your opponents seeds. 
+  + GRAND_SLAM must be legal for DEPRIVE games.
+  + The following options are incompatible with DEPRIVE games: MOVEUNLOCK, MUSTPASS, MUSTSHARE, ROUNDS, ROUND_STARTER, ROUND_FILL, NO_SIDES, SKIP_START, SOW_OWN_STORE, STORES, SOW_START, VISIT_OPP. 
+- TERRITORY: claim ownership of holes. Each round the ownership of holes is determined by the number of seeds captured in the previous round. In a TERRITORY game without rounds, the winner is the player that gained the most territory during play. 
+  + TERRITORY games require STORES and that GPARAM_ONE be set to a value between the number of holes and two times the number of holes.
+  + TERRITORY games are incompatible with NO_SIDES, START_PATTERN, GRANDSLAM of NOT_LEGAL, ALLOW_RULE of OPP_OR_EMPTY, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Games with children allow players to claim holes. These child holes are an extension of the stores and seeds in them count towards a win. Making a child stops any multiple lap sowing, moves cannot start from children, and they cannot be captured.
+- NOCHILD: children are not used.
+- NORMAL: children are made when a final seeds sows a hole to CHILD_CVT.
+- WALDA: STORES are not supported. Captures are instead moved into waldas, thus a player may not capture until they have created a walda. 
+  + Walda locations are limited.  Each player may create up to 6 waldas: on either end of each side of the board and the next outer hole on their own side of the board. Note that there are only 8 total places that waldas maybe created.
+- ONE_CHILD: only one child allowed per player, may not be in player's left most hole,  and may not be opposite eachother. Used to create tuzdek style children along with CHILD_RULE of OPP_ONLY.
+- WEG: children maybe created in holes owned by the opponent. Ending a sow in an opponent's weg captures the seed just sown and one more (if there is one); generally, the player gets to play again (per CAPT_RTURN). WEGs are supported for TERRITORY games only (hole ownership required).
+- BULL: create one bull if final seed sows to CHILD_CVT, create two bulls if the final two seeds are sown to CHILD_CVT-1 and CHILD_CVT (in either order).
+- QUR: when a seed is sown into an empty hole on the player's side of the board and the opposite hole contains CHILD_CVT, create children in both holes: final seed location and opposite.
+</t>
   </si>
 </sst>
 </file>
@@ -1816,8 +1822,8 @@
   <dimension ref="A1:J70"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G14" sqref="G14"/>
+      <pane ySplit="1" topLeftCell="A67" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G68" sqref="G68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1927,7 +1933,7 @@
         <v>0</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="345" x14ac:dyDescent="0.25">
@@ -1959,7 +1965,7 @@
         <v>0</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -1991,7 +1997,7 @@
         <v>0</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -2087,7 +2093,7 @@
         <v>0</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -2119,7 +2125,7 @@
         <v>0</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -2151,7 +2157,7 @@
         <v>0</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -2183,7 +2189,7 @@
         <v>0</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="225" x14ac:dyDescent="0.25">
@@ -2215,7 +2221,7 @@
         <v>0</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -2247,7 +2253,7 @@
         <v>2</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -2279,7 +2285,7 @@
         <v>2</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="105" x14ac:dyDescent="0.25">
@@ -2343,7 +2349,7 @@
         <v>2</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2375,7 +2381,7 @@
         <v>2</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2439,7 +2445,7 @@
         <v>2</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -2471,7 +2477,7 @@
         <v>2</v>
       </c>
       <c r="J20" s="4" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2503,7 +2509,7 @@
         <v>2</v>
       </c>
       <c r="J21" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -2535,7 +2541,7 @@
         <v>2</v>
       </c>
       <c r="J22" s="4" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
@@ -2567,7 +2573,7 @@
         <v>0</v>
       </c>
       <c r="J23" s="4" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -2599,7 +2605,7 @@
         <v>0</v>
       </c>
       <c r="J24" s="4" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -2631,7 +2637,7 @@
         <v>0</v>
       </c>
       <c r="J25" s="4" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="105" x14ac:dyDescent="0.25">
@@ -2695,7 +2701,7 @@
         <v>0</v>
       </c>
       <c r="J27" s="4" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="105" x14ac:dyDescent="0.25">
@@ -2759,7 +2765,7 @@
         <v>2</v>
       </c>
       <c r="J29" s="4" t="s">
-        <v>232</v>
+        <v>264</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2951,7 +2957,7 @@
         <v>0</v>
       </c>
       <c r="J35" s="4" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="36" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2983,7 +2989,7 @@
         <v>0</v>
       </c>
       <c r="J36" s="4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="37" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -3015,7 +3021,7 @@
         <v>0</v>
       </c>
       <c r="J37" s="4" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="38" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3047,7 +3053,7 @@
         <v>2</v>
       </c>
       <c r="J38" s="4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="39" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -3079,7 +3085,7 @@
         <v>2</v>
       </c>
       <c r="J39" s="4" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="40" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -3690,7 +3696,7 @@
         <v>0</v>
       </c>
       <c r="J59" s="4" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="60" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3786,7 +3792,7 @@
         <v>0</v>
       </c>
       <c r="J62" s="4" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="63" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -3818,10 +3824,10 @@
         <v>0</v>
       </c>
       <c r="J63" s="4" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="64" spans="1:10" ht="390" x14ac:dyDescent="0.25">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
         <v>69</v>
       </c>
@@ -3850,7 +3856,7 @@
         <v>0</v>
       </c>
       <c r="J64" s="4" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="65" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -3914,7 +3920,7 @@
         <v>2</v>
       </c>
       <c r="J66" s="8" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="67" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3946,7 +3952,7 @@
         <v>2</v>
       </c>
       <c r="J67" s="4" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="68" spans="1:10" ht="409.5" x14ac:dyDescent="0.25">
@@ -3978,7 +3984,7 @@
         <v>2</v>
       </c>
       <c r="J68" s="4" t="s">
-        <v>261</v>
+        <v>265</v>
       </c>
     </row>
     <row r="69" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -4042,7 +4048,7 @@
         <v>2</v>
       </c>
       <c r="J70" s="4" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deka updated to include no first move closures; test_gm_ removed for now. Two small bugs fixed: 1. clear_if for InhibitorCaptN should test >= 2. the lap continuer was wrong for SOW_BLKD_DIV_NR New capability: nocaptfirst prevents closing holes on the first turn for SOW_BLKD_DIV* games. Really big change: inhibitor moved out of decos, because it maintains state. Game state handling changed to save the inhibitor's state.
</commit_message>
<xml_diff>
--- a/src/game_params.xlsx
+++ b/src/game_params.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Activity_Data\Mancala_github\MancalaGames\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{487355B8-0AD8-4EDE-B84D-DF21D2B51367}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FAC17F5-7968-4379-8DD5-749EB8A3ED0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4335" yWindow="555" windowWidth="23415" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1950" yWindow="930" windowWidth="23415" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="game_params" sheetId="1" r:id="rId1"/>
@@ -866,9 +866,6 @@
     <t>Holes in the game start each round locked. Captures may not be made from locked holes. Starting a sow from a hole unlocks it.</t>
   </si>
   <si>
-    <t>Don't allow captures on the first move of the game or round.</t>
-  </si>
-  <si>
     <t>Capture when the contents of the hole is in the capt_on list. 
 Additionally, a SOWRULE of OWN_SOW_CAPT_ALL or SOW_SOW_CAPT_ALL includes this capture mechanism.</t>
   </si>
@@ -901,21 +898,6 @@
   <si>
     <t>Only allow cross capture if the player has sown onto the opposite side of board. 
 If a player ends on their own side of the board in an empty hole, but did not sow any opposite hole, they get a repeat turn.</t>
-  </si>
-  <si>
-    <t>Special sow rules may additional behavior or restrictions to the sowing phase:
-- NONE: there is no special sowing rules.
-- SOW_BLKD_DIV: Holes sown to GPARAM_ONE are closed (blocked) and the hole's seeds are removed from play. Blocked holes on own side are skipped when sowing and blocked holes on opp side are diverted out of play or captured. GOAL must be DEPRIVE.
-- SOW_BLKD_DIV_NR: Behaves the same as SOW_BLKD_DIV except that each player's rightmost hole cannot be closed. GOAL must be DEPRIVE.
-- OWN_SOW_CAPT_ALL: The hole OWNer captures all holes that are sown to meet the simple capture criteria: evens, min, max and capture on. Other criteria are enforced: side of the board, unlocked, and not child.
-  + The capture is done by the hole owner, so the non-sower may capture seeds during their opponents sowing. If the game GOAL is TERRITORY the capturer is the hole owner; otherwise each player captures from their own side of the board no matter who is sowing. 
-  + If mlaps is LAPPER and the final seed sown for any lap meets the capture criteria, the contents of the hole are captured by the sower and not the hole owner and the turn is over.
-  + GRANDSLAM rules are not applied. NOCAPTFIRST prevents this capture for the first move.
-- SOW_SOW_CAPT_ALL: Similar to OWN_SOW_CAPT_ALL but only the SOWer captures seeds from their opponent's holes. 
-  + If mlaps is LAPPER and the final seed sown for any lap meets the capture criteria, the contents of the hole are captured by the sower and not the hole owner and the turn is over.
-  + GRANDSLAM rules are not applied. NOCAPTFIRST prevents this capture for the first move.
-- NO_SOW_OPP_2S: Don't sow into opponents holes with 2 seeds.
-- CHANGE_DIR_LAP: Change the direction for each lap sown. Generally used with UDIR_HOLES so the player may choose the first direction.</t>
   </si>
   <si>
     <t xml:space="preserve">The overall goal of the game. Defines how a player wins.
@@ -938,6 +920,26 @@
 - BULL: create one bull if final seed sows to CHILD_CVT, create two bulls if the final two seeds are sown to CHILD_CVT-1 and CHILD_CVT (in either order).
 - QUR: when a seed is sown into an empty hole on the player's side of the board and the opposite hole contains CHILD_CVT, create children in both holes: final seed location and opposite.
 </t>
+  </si>
+  <si>
+    <t>Don't allow captures or closing of holes (SOW_RULE of SOW_BLKD_DIV) on the first move of the game or round.</t>
+  </si>
+  <si>
+    <t>Special sow rules may additional behavior or restrictions to the sowing phase:
+- NONE: there is no special sowing rule.
+- SOW_BLKD_DIV: If the final seed of an individual sow bring the contents of a hole to GPARAM_ONE seeds, the hole is closed closed (blocked). In single lap games, the hole's seeds are removed from play. In multilap games, the seeds are used to continue sowing.
+  + When sowing, blocked holes on your own side of the board are skipped  and blocked holes on opponent's side are diverted out of play or captured.
+  +NOCAPTFIRST prevents closing holes on the first move. Game GOAL must be DEPRIVE. 
+- SOW_BLKD_DIV_NR: Behaves the same as SOW_BLKD_DIV except that each player's rightmost hole cannot be closed. 
+- OWN_SOW_CAPT_ALL: The hole OWNer captures all holes that are sown to meet the simple capture criteria: evens, min, max and capture on. Other criteria are enforced: side of the board, unlocked, and not child.
+  + The capture is done by the hole owner, so the non-sower may capture seeds during their opponents sowing. If the game GOAL is TERRITORY the capturer is the hole owner; otherwise each player captures from their own side of the board no matter who is sowing. 
+  + If mlaps is LAPPER and the final seed sown for any lap meets the capture criteria, the contents of the hole are captured by the sower and not the hole owner and the turn is over.
+  + GRANDSLAM rules are not applied. NOCAPTFIRST prevents this capture for the first move.
+- SOW_SOW_CAPT_ALL: Similar to OWN_SOW_CAPT_ALL but only the SOWer captures seeds from their opponent's holes. 
+  + If mlaps is LAPPER and the final seed sown for any lap meets the capture criteria, the contents of the hole are captured by the sower and not the hole owner and the turn is over.
+  + GRANDSLAM rules are not applied. NOCAPTFIRST prevents this capture for the first move.
+- NO_SOW_OPP_2S: Don't sow into opponents holes with 2 seeds.
+- CHANGE_DIR_LAP: Change the direction for each lap sown. Generally used with UDIR_HOLES so the player may choose the first direction.</t>
   </si>
 </sst>
 </file>
@@ -1822,8 +1824,8 @@
   <dimension ref="A1:J70"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A67" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G68" sqref="G68"/>
+      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J64" sqref="J64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2285,7 +2287,7 @@
         <v>2</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="105" x14ac:dyDescent="0.25">
@@ -2416,7 +2418,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>96</v>
       </c>
@@ -2445,7 +2447,7 @@
         <v>2</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>256</v>
+        <v>264</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -2477,7 +2479,7 @@
         <v>2</v>
       </c>
       <c r="J20" s="4" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2509,7 +2511,7 @@
         <v>2</v>
       </c>
       <c r="J21" s="4" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -2541,7 +2543,7 @@
         <v>2</v>
       </c>
       <c r="J22" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
@@ -2701,7 +2703,7 @@
         <v>0</v>
       </c>
       <c r="J27" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="105" x14ac:dyDescent="0.25">
@@ -2765,7 +2767,7 @@
         <v>2</v>
       </c>
       <c r="J29" s="4" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3856,7 +3858,7 @@
         <v>0</v>
       </c>
       <c r="J64" s="4" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
     </row>
     <row r="65" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -3984,7 +3986,7 @@
         <v>2</v>
       </c>
       <c r="J68" s="4" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="69" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -4048,7 +4050,7 @@
         <v>2</v>
       </c>
       <c r="J70" s="4" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added missing ai player rules: stores_scorer and no_repeat_scorer Updated montecarlo_ts in main help. Added text to ai parameters. Sprinkled some questions as TODOs around the ai player.
</commit_message>
<xml_diff>
--- a/src/game_params.xlsx
+++ b/src/game_params.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Activity_Data\Mancala_github\MancalaGames\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FAC17F5-7968-4379-8DD5-749EB8A3ED0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{140F7FD2-074F-4228-9910-B675713AD6C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="930" windowWidth="23415" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="game_params" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="273">
   <si>
     <t>tab</t>
   </si>
@@ -489,9 +489,6 @@
   </si>
   <si>
     <t>player _</t>
-  </si>
-  <si>
-    <t>The default difficulty. Can be changed at play time, even during game play, in the Mancala UI.</t>
   </si>
   <si>
     <t xml:space="preserve">Sow counter-clockwise.
@@ -508,9 +505,6 @@
 - ALWAYS_PICK: always pick (capture) the seed, even if there was not a capture"</t>
   </si>
   <si>
-    <t xml:space="preserve">The minimax scorer will use this as a multiplier to maximize the bottom players stores versus the top player's. </t>
-  </si>
-  <si>
     <t>An init only parameter that used to check the consistency of the game info. Errors and warnings are raised as the rules are processed.</t>
   </si>
   <si>
@@ -566,19 +560,6 @@
   </si>
   <si>
     <t>[400, 400, 400, 400]</t>
-  </si>
-  <si>
-    <t>For each difficulty [0-3], the depth that the minimaxer will search to.</t>
-  </si>
-  <si>
-    <t>Bias for the Monte Carlo Tree seach algorithm for each difficulty level (0-3). 
-Value is divided by 1000.</t>
-  </si>
-  <si>
-    <t>Number of leaf nodes to create each time we pick a new move. One value for each difficulty level (0-3).</t>
-  </si>
-  <si>
-    <t>Number of end games played out from each leaf node created. One value for each difficulty level (0-3).</t>
   </si>
   <si>
     <t>child_cvt</t>
@@ -638,11 +619,6 @@
   </si>
   <si>
     <t>A derived parameter. Do not include in config files. Set during game construction length of moves: 1 (int) or 2, 3 (tuple).</t>
-  </si>
-  <si>
-    <t>minimaxer: an Alpha-Beta Pruning MiniMaxer
-negamaxer: minimaxer with a very minor optimization for alternating turn games (no repeat turns). Uses minimaxer depths for difficulties.
-montecarlo_ts: a Monte Carlo Tree Search player (that is likely implemented wrong).</t>
   </si>
   <si>
     <t>capt_rturn</t>
@@ -705,9 +681,6 @@
   </si>
   <si>
     <t>Start Active</t>
-  </si>
-  <si>
-    <t>Automatically activate the AI player. The AI player can be manually deactivated.</t>
   </si>
   <si>
     <t>order</t>
@@ -940,6 +913,68 @@
   + GRANDSLAM rules are not applied. NOCAPTFIRST prevents this capture for the first move.
 - NO_SOW_OPP_2S: Don't sow into opponents holes with 2 seeds.
 - CHANGE_DIR_LAP: Change the direction for each lap sown. Generally used with UDIR_HOLES so the player may choose the first direction.</t>
+  </si>
+  <si>
+    <t>minimaxer: an Alpha-Beta Pruning MiniMaxer
+negamaxer: minimaxer with a very minor optimization for alternating turn games (no repeat turns). Uses minimaxer depths for difficulties.
+montecarlo_ts: a Monte Carlo Tree Search player.</t>
+  </si>
+  <si>
+    <t>Number of end games played out from each expanded node. One value for each difficulty level (0-3).</t>
+  </si>
+  <si>
+    <t>Number of game tree expansions to perform each time we pick a new move. One value for each difficulty level (0-3).</t>
+  </si>
+  <si>
+    <t>Bias for the Monte Carlo Tree seach algorithm for each difficulty level (0-3).  A larger bias encourages move game tree exploration, but defocuses the exploration from the best choices. This is critical in avoiding getting stuck in sub-obtimal move choices.
+Value is divided by 1000.</t>
+  </si>
+  <si>
+    <t>The default difficulty for the game. The difficulty can be changed at play time,  even during game play, in the Mancala UI.</t>
+  </si>
+  <si>
+    <t>Automatically activate the AI player. The AI player can be manually deactivated, but it is selected for the starter it will start the game.</t>
+  </si>
+  <si>
+    <t>There are four game difficulties. Each select a set of parameters give the algorithm choosen.</t>
+  </si>
+  <si>
+    <t>If the game is being played on easy mode (game difficult of easy/0), a random value may be added to the static evaluation. This can be done to induce errors into the ai player's game play. A random value is selected between -easy_rand and + easy_rand.
+The specific value for this should be selected based on the ranges of the paremeters and multiplier.
+Used only for minimax &amp; negamax players.</t>
+  </si>
+  <si>
+    <t>The multiplier for the even scorer. The even scorer counts the number of holes with an even number of seeds. This is useful to use when the capture mechanism is evens.
+Used only for minimax &amp; negamax players.</t>
+  </si>
+  <si>
+    <t>The multiplier for the child scorer. The child scorer counts the number children each player has.
+The child scorer may only be used on games with children. If the game does not include child the multiplier must be zero.
+Used only for the minimax &amp; negamax players.</t>
+  </si>
+  <si>
+    <t>The multiplier for the stores scorer. It is applied to the difference of the seeds in each players store.
+The stores scorer may not be used in games with STORES. A zero multiplier disables the stores scorer.
+Used only for  minimax &amp; negamax players.</t>
+  </si>
+  <si>
+    <t>The multiplier for the seeds scorer. The seeds scorer computes how many seeds each player has on the game board.
+TODO does this properly deal with children or hole owners?
+Used only for minimax &amp; negamax players.</t>
+  </si>
+  <si>
+    <t>The multiplier for the empties scorer. The empties scorer counts the number empty holes each player has on the board.
+Used only for minimax &amp; negamax players.</t>
+  </si>
+  <si>
+    <t>The multiplier for the access scorer. The access scorer computes how many of the opponents holes can be accessed for the given game state.
+The access scorer is slow and therefore is prohibited from being used in multilap games (MLAPS); games with user choice of move direction (UDIR_HOLES); and games where hole owners are not predefined (NO_SIDES). In these game configurations, the multiplier must be zero to disable the access scorer.
+Used only for minimax &amp; negamax players.</t>
+  </si>
+  <si>
+    <t>A value used to encourage or discourage repeat turns. The value is added in for the current player and subtracted off the score for the opposing playing. Use a positive value to encourage the AI player to repeat turns.
+This parameter may only be used for games in which repeated turns are possible (SOW_OWN_STORE, CAPT_RTURN or XC_SOWN).
+Used only for minimax &amp; negamax players.</t>
   </si>
 </sst>
 </file>
@@ -1824,8 +1859,8 @@
   <dimension ref="A1:J70"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J64" sqref="J64"/>
+      <pane ySplit="1" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G54" sqref="G54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1856,7 +1891,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>220</v>
+        <v>212</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>4</v>
@@ -1935,7 +1970,7 @@
         <v>0</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="345" x14ac:dyDescent="0.25">
@@ -1943,10 +1978,10 @@
         <v>62</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>24</v>
@@ -1955,10 +1990,10 @@
         <v>14</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="H4" s="3">
         <v>3</v>
@@ -1967,7 +2002,7 @@
         <v>0</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -1999,7 +2034,7 @@
         <v>0</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -2095,7 +2130,7 @@
         <v>0</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -2127,7 +2162,7 @@
         <v>0</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -2159,7 +2194,7 @@
         <v>0</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -2167,10 +2202,10 @@
         <v>96</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>24</v>
@@ -2191,7 +2226,7 @@
         <v>0</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="225" x14ac:dyDescent="0.25">
@@ -2223,7 +2258,7 @@
         <v>0</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -2255,7 +2290,7 @@
         <v>2</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -2263,10 +2298,10 @@
         <v>96</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>24</v>
@@ -2287,7 +2322,7 @@
         <v>2</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>261</v>
+        <v>253</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="105" x14ac:dyDescent="0.25">
@@ -2319,7 +2354,7 @@
         <v>2</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="240" x14ac:dyDescent="0.25">
@@ -2351,7 +2386,7 @@
         <v>2</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2383,7 +2418,7 @@
         <v>2</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2423,10 +2458,10 @@
         <v>96</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>226</v>
+        <v>218</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>24</v>
@@ -2447,7 +2482,7 @@
         <v>2</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -2467,7 +2502,7 @@
         <v>20</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="G20" s="5" t="s">
         <v>94</v>
@@ -2479,7 +2514,7 @@
         <v>2</v>
       </c>
       <c r="J20" s="4" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2487,10 +2522,10 @@
         <v>96</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>24</v>
@@ -2511,7 +2546,7 @@
         <v>2</v>
       </c>
       <c r="J21" s="4" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -2519,10 +2554,10 @@
         <v>96</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>24</v>
@@ -2531,10 +2566,10 @@
         <v>59</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="H22" s="3">
         <v>10</v>
@@ -2543,7 +2578,7 @@
         <v>2</v>
       </c>
       <c r="J22" s="4" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
@@ -2575,7 +2610,7 @@
         <v>0</v>
       </c>
       <c r="J23" s="4" t="s">
-        <v>237</v>
+        <v>229</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -2607,7 +2642,7 @@
         <v>0</v>
       </c>
       <c r="J24" s="4" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -2639,7 +2674,7 @@
         <v>0</v>
       </c>
       <c r="J25" s="4" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="105" x14ac:dyDescent="0.25">
@@ -2671,7 +2706,7 @@
         <v>0</v>
       </c>
       <c r="J26" s="4" t="s">
-        <v>228</v>
+        <v>220</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="409.5" x14ac:dyDescent="0.25">
@@ -2679,10 +2714,10 @@
         <v>38</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>24</v>
@@ -2691,10 +2726,10 @@
         <v>62</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
       <c r="H27" s="3">
         <v>6</v>
@@ -2703,7 +2738,7 @@
         <v>0</v>
       </c>
       <c r="J27" s="4" t="s">
-        <v>260</v>
+        <v>252</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="105" x14ac:dyDescent="0.25">
@@ -2735,7 +2770,7 @@
         <v>0</v>
       </c>
       <c r="J28" s="4" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="315" x14ac:dyDescent="0.25">
@@ -2767,7 +2802,7 @@
         <v>2</v>
       </c>
       <c r="J29" s="4" t="s">
-        <v>262</v>
+        <v>254</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2799,7 +2834,7 @@
         <v>2</v>
       </c>
       <c r="J30" s="4" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
     </row>
     <row r="31" spans="1:10" ht="285" x14ac:dyDescent="0.25">
@@ -2831,7 +2866,7 @@
         <v>2</v>
       </c>
       <c r="J31" s="4" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="255" x14ac:dyDescent="0.25">
@@ -2839,10 +2874,10 @@
         <v>38</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="D32" s="3" t="s">
         <v>24</v>
@@ -2851,10 +2886,10 @@
         <v>60</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="G32" s="5" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="H32" s="3">
         <v>3</v>
@@ -2863,7 +2898,7 @@
         <v>2</v>
       </c>
       <c r="J32" s="4" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -2871,10 +2906,10 @@
         <v>38</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="D33" s="3" t="s">
         <v>24</v>
@@ -2895,7 +2930,7 @@
         <v>2</v>
       </c>
       <c r="J33" s="4" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
@@ -2915,7 +2950,7 @@
         <v>28</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="G34" s="5" t="s">
         <v>20</v>
@@ -2959,7 +2994,7 @@
         <v>0</v>
       </c>
       <c r="J35" s="4" t="s">
-        <v>236</v>
+        <v>228</v>
       </c>
     </row>
     <row r="36" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2991,7 +3026,7 @@
         <v>0</v>
       </c>
       <c r="J36" s="4" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
     </row>
     <row r="37" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -3014,7 +3049,7 @@
         <v>30</v>
       </c>
       <c r="G37" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="H37" s="3">
         <v>4</v>
@@ -3023,7 +3058,7 @@
         <v>0</v>
       </c>
       <c r="J37" s="4" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
     </row>
     <row r="38" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3055,7 +3090,7 @@
         <v>2</v>
       </c>
       <c r="J38" s="4" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
     </row>
     <row r="39" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -3087,18 +3122,18 @@
         <v>2</v>
       </c>
       <c r="J39" s="4" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>130</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D40" s="3" t="s">
         <v>150</v>
@@ -3107,10 +3142,10 @@
         <v>13</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="H40" s="3">
         <v>0</v>
@@ -3119,7 +3154,7 @@
         <v>0</v>
       </c>
       <c r="J40" s="4" t="s">
-        <v>198</v>
+        <v>258</v>
       </c>
     </row>
     <row r="41" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3151,18 +3186,18 @@
         <v>0</v>
       </c>
       <c r="J41" s="4" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>130</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="D42" s="3" t="s">
         <v>150</v>
@@ -3183,7 +3218,7 @@
         <v>0</v>
       </c>
       <c r="J42" s="4" t="s">
-        <v>219</v>
+        <v>263</v>
       </c>
     </row>
     <row r="43" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3191,13 +3226,13 @@
         <v>130</v>
       </c>
       <c r="B43" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="D43" s="3" t="s">
         <v>162</v>
-      </c>
-      <c r="C43" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="D43" s="3" t="s">
-        <v>164</v>
       </c>
       <c r="E43" s="3">
         <v>46</v>
@@ -3206,7 +3241,7 @@
         <v>93</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="H43" s="3">
         <v>4</v>
@@ -3215,21 +3250,21 @@
         <v>0</v>
       </c>
       <c r="J43" s="4" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>130</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E44" s="3">
         <v>40</v>
@@ -3238,7 +3273,7 @@
         <v>93</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="H44" s="3">
         <v>6</v>
@@ -3247,7 +3282,7 @@
         <v>0</v>
       </c>
       <c r="J44" s="4" t="s">
-        <v>176</v>
+        <v>261</v>
       </c>
     </row>
     <row r="45" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3255,13 +3290,13 @@
         <v>130</v>
       </c>
       <c r="B45" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="C45" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="C45" s="3" t="s">
-        <v>169</v>
-      </c>
       <c r="D45" s="3" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E45" s="3">
         <v>41</v>
@@ -3270,7 +3305,7 @@
         <v>93</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="H45" s="3">
         <v>7</v>
@@ -3279,7 +3314,7 @@
         <v>0</v>
       </c>
       <c r="J45" s="4" t="s">
-        <v>177</v>
+        <v>260</v>
       </c>
     </row>
     <row r="46" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3287,13 +3322,13 @@
         <v>130</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E46" s="3">
         <v>42</v>
@@ -3302,7 +3337,7 @@
         <v>93</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="H46" s="3">
         <v>8</v>
@@ -3311,10 +3346,10 @@
         <v>0</v>
       </c>
       <c r="J46" s="4" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
         <v>130</v>
       </c>
@@ -3343,10 +3378,10 @@
         <v>2</v>
       </c>
       <c r="J47" s="4" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" ht="135" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
         <v>130</v>
       </c>
@@ -3375,10 +3410,10 @@
         <v>2</v>
       </c>
       <c r="J48" s="4" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
         <v>130</v>
       </c>
@@ -3407,10 +3442,10 @@
         <v>2</v>
       </c>
       <c r="J49" s="4" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
         <v>130</v>
       </c>
@@ -3439,10 +3474,10 @@
         <v>2</v>
       </c>
       <c r="J50" s="4" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
         <v>130</v>
       </c>
@@ -3471,10 +3506,10 @@
         <v>2</v>
       </c>
       <c r="J51" s="4" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
         <v>130</v>
       </c>
@@ -3503,10 +3538,10 @@
         <v>2</v>
       </c>
       <c r="J52" s="4" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
         <v>130</v>
       </c>
@@ -3535,10 +3570,10 @@
         <v>2</v>
       </c>
       <c r="J53" s="4" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
         <v>130</v>
       </c>
@@ -3567,7 +3602,7 @@
         <v>2</v>
       </c>
       <c r="J54" s="4" t="s">
-        <v>147</v>
+        <v>272</v>
       </c>
     </row>
     <row r="55" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3575,7 +3610,7 @@
         <v>9</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="D55" s="3" t="s">
         <v>24</v>
@@ -3593,7 +3628,7 @@
         <v>0</v>
       </c>
       <c r="J55" s="4" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
     </row>
     <row r="56" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3639,7 +3674,7 @@
         <v>0</v>
       </c>
       <c r="J57" s="4" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="58" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3666,7 +3701,7 @@
         <v>0</v>
       </c>
       <c r="J58" s="4" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
     </row>
     <row r="59" spans="1:10" ht="105" x14ac:dyDescent="0.25">
@@ -3698,7 +3733,7 @@
         <v>0</v>
       </c>
       <c r="J59" s="4" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
     </row>
     <row r="60" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3794,7 +3829,7 @@
         <v>0</v>
       </c>
       <c r="J62" s="4" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
     </row>
     <row r="63" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -3826,7 +3861,7 @@
         <v>0</v>
       </c>
       <c r="J63" s="4" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
     </row>
     <row r="64" spans="1:10" ht="409.5" x14ac:dyDescent="0.25">
@@ -3834,10 +3869,10 @@
         <v>69</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="D64" s="3" t="s">
         <v>24</v>
@@ -3846,10 +3881,10 @@
         <v>70</v>
       </c>
       <c r="F64" s="3" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="G64" s="5" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="H64" s="3">
         <v>6</v>
@@ -3858,7 +3893,7 @@
         <v>0</v>
       </c>
       <c r="J64" s="4" t="s">
-        <v>265</v>
+        <v>257</v>
       </c>
     </row>
     <row r="65" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -3878,7 +3913,7 @@
         <v>75</v>
       </c>
       <c r="F65" s="3" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="G65" s="5" t="s">
         <v>94</v>
@@ -3890,7 +3925,7 @@
         <v>0</v>
       </c>
       <c r="J65" s="4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="66" spans="1:10" ht="195" x14ac:dyDescent="0.25">
@@ -3910,10 +3945,10 @@
         <v>44</v>
       </c>
       <c r="F66" s="3" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="G66" s="5" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="H66" s="3">
         <v>0</v>
@@ -3922,7 +3957,7 @@
         <v>2</v>
       </c>
       <c r="J66" s="8" t="s">
-        <v>246</v>
+        <v>238</v>
       </c>
     </row>
     <row r="67" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3954,7 +3989,7 @@
         <v>2</v>
       </c>
       <c r="J67" s="4" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
     </row>
     <row r="68" spans="1:10" ht="409.5" x14ac:dyDescent="0.25">
@@ -3962,10 +3997,10 @@
         <v>69</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="D68" s="3" t="s">
         <v>24</v>
@@ -3974,10 +4009,10 @@
         <v>27</v>
       </c>
       <c r="F68" s="3" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="G68" s="5" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="H68" s="3">
         <v>3</v>
@@ -3986,7 +4021,7 @@
         <v>2</v>
       </c>
       <c r="J68" s="4" t="s">
-        <v>263</v>
+        <v>255</v>
       </c>
     </row>
     <row r="69" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3994,10 +4029,10 @@
         <v>69</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="D69" s="3" t="s">
         <v>24</v>
@@ -4018,7 +4053,7 @@
         <v>2</v>
       </c>
       <c r="J69" s="4" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
     </row>
     <row r="70" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -4026,10 +4061,10 @@
         <v>69</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>222</v>
+        <v>214</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
       <c r="D70" s="3" t="s">
         <v>24</v>
@@ -4038,10 +4073,10 @@
         <v>24</v>
       </c>
       <c r="F70" s="3" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
       <c r="G70" s="3" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="H70" s="3">
         <v>5</v>
@@ -4050,7 +4085,7 @@
         <v>2</v>
       </c>
       <c r="J70" s="4" t="s">
-        <v>259</v>
+        <v>251</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix grammar in parameter description.
</commit_message>
<xml_diff>
--- a/src/game_params.xlsx
+++ b/src/game_params.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Activity_Data\Mancala_github\MancalaGames\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{140F7FD2-074F-4228-9910-B675713AD6C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E4CED72-7B7A-4A94-BF2E-52AEFD0D370B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="game_params" sheetId="1" r:id="rId1"/>
@@ -898,7 +898,69 @@
     <t>Don't allow captures or closing of holes (SOW_RULE of SOW_BLKD_DIV) on the first move of the game or round.</t>
   </si>
   <si>
-    <t>Special sow rules may additional behavior or restrictions to the sowing phase:
+    <t>minimaxer: an Alpha-Beta Pruning MiniMaxer
+negamaxer: minimaxer with a very minor optimization for alternating turn games (no repeat turns). Uses minimaxer depths for difficulties.
+montecarlo_ts: a Monte Carlo Tree Search player.</t>
+  </si>
+  <si>
+    <t>Number of end games played out from each expanded node. One value for each difficulty level (0-3).</t>
+  </si>
+  <si>
+    <t>Number of game tree expansions to perform each time we pick a new move. One value for each difficulty level (0-3).</t>
+  </si>
+  <si>
+    <t>Bias for the Monte Carlo Tree seach algorithm for each difficulty level (0-3).  A larger bias encourages move game tree exploration, but defocuses the exploration from the best choices. This is critical in avoiding getting stuck in sub-obtimal move choices.
+Value is divided by 1000.</t>
+  </si>
+  <si>
+    <t>The default difficulty for the game. The difficulty can be changed at play time,  even during game play, in the Mancala UI.</t>
+  </si>
+  <si>
+    <t>Automatically activate the AI player. The AI player can be manually deactivated, but it is selected for the starter it will start the game.</t>
+  </si>
+  <si>
+    <t>There are four game difficulties. Each select a set of parameters give the algorithm choosen.</t>
+  </si>
+  <si>
+    <t>If the game is being played on easy mode (game difficult of easy/0), a random value may be added to the static evaluation. This can be done to induce errors into the ai player's game play. A random value is selected between -easy_rand and + easy_rand.
+The specific value for this should be selected based on the ranges of the paremeters and multiplier.
+Used only for minimax &amp; negamax players.</t>
+  </si>
+  <si>
+    <t>The multiplier for the even scorer. The even scorer counts the number of holes with an even number of seeds. This is useful to use when the capture mechanism is evens.
+Used only for minimax &amp; negamax players.</t>
+  </si>
+  <si>
+    <t>The multiplier for the child scorer. The child scorer counts the number children each player has.
+The child scorer may only be used on games with children. If the game does not include child the multiplier must be zero.
+Used only for the minimax &amp; negamax players.</t>
+  </si>
+  <si>
+    <t>The multiplier for the stores scorer. It is applied to the difference of the seeds in each players store.
+The stores scorer may not be used in games with STORES. A zero multiplier disables the stores scorer.
+Used only for  minimax &amp; negamax players.</t>
+  </si>
+  <si>
+    <t>The multiplier for the seeds scorer. The seeds scorer computes how many seeds each player has on the game board.
+TODO does this properly deal with children or hole owners?
+Used only for minimax &amp; negamax players.</t>
+  </si>
+  <si>
+    <t>The multiplier for the empties scorer. The empties scorer counts the number empty holes each player has on the board.
+Used only for minimax &amp; negamax players.</t>
+  </si>
+  <si>
+    <t>The multiplier for the access scorer. The access scorer computes how many of the opponents holes can be accessed for the given game state.
+The access scorer is slow and therefore is prohibited from being used in multilap games (MLAPS); games with user choice of move direction (UDIR_HOLES); and games where hole owners are not predefined (NO_SIDES). In these game configurations, the multiplier must be zero to disable the access scorer.
+Used only for minimax &amp; negamax players.</t>
+  </si>
+  <si>
+    <t>A value used to encourage or discourage repeat turns. The value is added in for the current player and subtracted off the score for the opposing playing. Use a positive value to encourage the AI player to repeat turns.
+This parameter may only be used for games in which repeated turns are possible (SOW_OWN_STORE, CAPT_RTURN or XC_SOWN).
+Used only for minimax &amp; negamax players.</t>
+  </si>
+  <si>
+    <t>Special sow rules add additional behavior or restrictions to the sowing phase:
 - NONE: there is no special sowing rule.
 - SOW_BLKD_DIV: If the final seed of an individual sow bring the contents of a hole to GPARAM_ONE seeds, the hole is closed closed (blocked). In single lap games, the hole's seeds are removed from play. In multilap games, the seeds are used to continue sowing.
   + When sowing, blocked holes on your own side of the board are skipped  and blocked holes on opponent's side are diverted out of play or captured.
@@ -913,68 +975,6 @@
   + GRANDSLAM rules are not applied. NOCAPTFIRST prevents this capture for the first move.
 - NO_SOW_OPP_2S: Don't sow into opponents holes with 2 seeds.
 - CHANGE_DIR_LAP: Change the direction for each lap sown. Generally used with UDIR_HOLES so the player may choose the first direction.</t>
-  </si>
-  <si>
-    <t>minimaxer: an Alpha-Beta Pruning MiniMaxer
-negamaxer: minimaxer with a very minor optimization for alternating turn games (no repeat turns). Uses minimaxer depths for difficulties.
-montecarlo_ts: a Monte Carlo Tree Search player.</t>
-  </si>
-  <si>
-    <t>Number of end games played out from each expanded node. One value for each difficulty level (0-3).</t>
-  </si>
-  <si>
-    <t>Number of game tree expansions to perform each time we pick a new move. One value for each difficulty level (0-3).</t>
-  </si>
-  <si>
-    <t>Bias for the Monte Carlo Tree seach algorithm for each difficulty level (0-3).  A larger bias encourages move game tree exploration, but defocuses the exploration from the best choices. This is critical in avoiding getting stuck in sub-obtimal move choices.
-Value is divided by 1000.</t>
-  </si>
-  <si>
-    <t>The default difficulty for the game. The difficulty can be changed at play time,  even during game play, in the Mancala UI.</t>
-  </si>
-  <si>
-    <t>Automatically activate the AI player. The AI player can be manually deactivated, but it is selected for the starter it will start the game.</t>
-  </si>
-  <si>
-    <t>There are four game difficulties. Each select a set of parameters give the algorithm choosen.</t>
-  </si>
-  <si>
-    <t>If the game is being played on easy mode (game difficult of easy/0), a random value may be added to the static evaluation. This can be done to induce errors into the ai player's game play. A random value is selected between -easy_rand and + easy_rand.
-The specific value for this should be selected based on the ranges of the paremeters and multiplier.
-Used only for minimax &amp; negamax players.</t>
-  </si>
-  <si>
-    <t>The multiplier for the even scorer. The even scorer counts the number of holes with an even number of seeds. This is useful to use when the capture mechanism is evens.
-Used only for minimax &amp; negamax players.</t>
-  </si>
-  <si>
-    <t>The multiplier for the child scorer. The child scorer counts the number children each player has.
-The child scorer may only be used on games with children. If the game does not include child the multiplier must be zero.
-Used only for the minimax &amp; negamax players.</t>
-  </si>
-  <si>
-    <t>The multiplier for the stores scorer. It is applied to the difference of the seeds in each players store.
-The stores scorer may not be used in games with STORES. A zero multiplier disables the stores scorer.
-Used only for  minimax &amp; negamax players.</t>
-  </si>
-  <si>
-    <t>The multiplier for the seeds scorer. The seeds scorer computes how many seeds each player has on the game board.
-TODO does this properly deal with children or hole owners?
-Used only for minimax &amp; negamax players.</t>
-  </si>
-  <si>
-    <t>The multiplier for the empties scorer. The empties scorer counts the number empty holes each player has on the board.
-Used only for minimax &amp; negamax players.</t>
-  </si>
-  <si>
-    <t>The multiplier for the access scorer. The access scorer computes how many of the opponents holes can be accessed for the given game state.
-The access scorer is slow and therefore is prohibited from being used in multilap games (MLAPS); games with user choice of move direction (UDIR_HOLES); and games where hole owners are not predefined (NO_SIDES). In these game configurations, the multiplier must be zero to disable the access scorer.
-Used only for minimax &amp; negamax players.</t>
-  </si>
-  <si>
-    <t>A value used to encourage or discourage repeat turns. The value is added in for the current player and subtracted off the score for the opposing playing. Use a positive value to encourage the AI player to repeat turns.
-This parameter may only be used for games in which repeated turns are possible (SOW_OWN_STORE, CAPT_RTURN or XC_SOWN).
-Used only for minimax &amp; negamax players.</t>
   </si>
 </sst>
 </file>
@@ -1859,8 +1859,8 @@
   <dimension ref="A1:J70"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G54" sqref="G54"/>
+      <pane ySplit="1" topLeftCell="A64" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J64" sqref="J64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3154,7 +3154,7 @@
         <v>0</v>
       </c>
       <c r="J40" s="4" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="41" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3186,7 +3186,7 @@
         <v>0</v>
       </c>
       <c r="J41" s="4" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="42" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -3218,7 +3218,7 @@
         <v>0</v>
       </c>
       <c r="J42" s="4" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="43" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3250,7 +3250,7 @@
         <v>0</v>
       </c>
       <c r="J43" s="4" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -3282,7 +3282,7 @@
         <v>0</v>
       </c>
       <c r="J44" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="45" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3314,7 +3314,7 @@
         <v>0</v>
       </c>
       <c r="J45" s="4" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="46" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3346,7 +3346,7 @@
         <v>0</v>
       </c>
       <c r="J46" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="47" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -3378,7 +3378,7 @@
         <v>2</v>
       </c>
       <c r="J47" s="4" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="48" spans="1:10" ht="135" x14ac:dyDescent="0.25">
@@ -3410,7 +3410,7 @@
         <v>2</v>
       </c>
       <c r="J48" s="4" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="49" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -3442,7 +3442,7 @@
         <v>2</v>
       </c>
       <c r="J49" s="4" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="50" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -3474,7 +3474,7 @@
         <v>2</v>
       </c>
       <c r="J50" s="4" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="51" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -3506,7 +3506,7 @@
         <v>2</v>
       </c>
       <c r="J51" s="4" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="52" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -3538,7 +3538,7 @@
         <v>2</v>
       </c>
       <c r="J52" s="4" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="53" spans="1:10" ht="105" x14ac:dyDescent="0.25">
@@ -3570,7 +3570,7 @@
         <v>2</v>
       </c>
       <c r="J53" s="4" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="54" spans="1:10" ht="120" x14ac:dyDescent="0.25">
@@ -3602,7 +3602,7 @@
         <v>2</v>
       </c>
       <c r="J54" s="4" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="55" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3893,7 +3893,7 @@
         <v>0</v>
       </c>
       <c r="J64" s="4" t="s">
-        <v>257</v>
+        <v>272</v>
       </c>
     </row>
     <row r="65" spans="1:10" ht="90" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated the stores scorer to be usable with child games w/o stores. Configure Qelat to use the stores scorer. Fixed how the scorers for evens, seeds & empties work with territory and no_sides games. Count should only be used for no_sides and a difference based on hole owner was created for territory games.
</commit_message>
<xml_diff>
--- a/src/game_params.xlsx
+++ b/src/game_params.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Activity_Data\Mancala_github\MancalaGames\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E4CED72-7B7A-4A94-BF2E-52AEFD0D370B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CD16CD8-1A11-4CC9-95E0-2AC99C564C14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="645" yWindow="480" windowWidth="23415" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="game_params" sheetId="1" r:id="rId1"/>
@@ -434,9 +434,6 @@
     <t>stores_m</t>
   </si>
   <si>
-    <t>Stores mult</t>
-  </si>
-  <si>
     <t>player scorer _</t>
   </si>
   <si>
@@ -919,9 +916,6 @@
     <t>Automatically activate the AI player. The AI player can be manually deactivated, but it is selected for the starter it will start the game.</t>
   </si>
   <si>
-    <t>There are four game difficulties. Each select a set of parameters give the algorithm choosen.</t>
-  </si>
-  <si>
     <t>If the game is being played on easy mode (game difficult of easy/0), a random value may be added to the static evaluation. This can be done to induce errors into the ai player's game play. A random value is selected between -easy_rand and + easy_rand.
 The specific value for this should be selected based on the ranges of the paremeters and multiplier.
 Used only for minimax &amp; negamax players.</t>
@@ -934,11 +928,6 @@
     <t>The multiplier for the child scorer. The child scorer counts the number children each player has.
 The child scorer may only be used on games with children. If the game does not include child the multiplier must be zero.
 Used only for the minimax &amp; negamax players.</t>
-  </si>
-  <si>
-    <t>The multiplier for the stores scorer. It is applied to the difference of the seeds in each players store.
-The stores scorer may not be used in games with STORES. A zero multiplier disables the stores scorer.
-Used only for  minimax &amp; negamax players.</t>
   </si>
   <si>
     <t>The multiplier for the seeds scorer. The seeds scorer computes how many seeds each player has on the game board.
@@ -975,6 +964,17 @@
   + GRANDSLAM rules are not applied. NOCAPTFIRST prevents this capture for the first move.
 - NO_SOW_OPP_2S: Don't sow into opponents holes with 2 seeds.
 - CHANGE_DIR_LAP: Change the direction for each lap sown. Generally used with UDIR_HOLES so the player may choose the first direction.</t>
+  </si>
+  <si>
+    <t>The multiplier for the stores scorer. Seeds in stores and children are included.
+The stores scorer may not be used in games without STORES or CHILDREN. A zero multiplier disables the stores scorer.
+Used only for  minimax &amp; negamax players.</t>
+  </si>
+  <si>
+    <t>Stores (captured) mult</t>
+  </si>
+  <si>
+    <t>The depth that the minimaxer or negamaxer will search the game tree from the current node. One value for each difficulty.</t>
   </si>
 </sst>
 </file>
@@ -1859,8 +1859,8 @@
   <dimension ref="A1:J70"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A64" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J64" sqref="J64"/>
+      <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J48" sqref="J48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1891,7 +1891,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>4</v>
@@ -1970,7 +1970,7 @@
         <v>0</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="345" x14ac:dyDescent="0.25">
@@ -1978,10 +1978,10 @@
         <v>62</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>180</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>181</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>24</v>
@@ -1990,10 +1990,10 @@
         <v>14</v>
       </c>
       <c r="F4" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="G4" s="5" t="s">
         <v>182</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>183</v>
       </c>
       <c r="H4" s="3">
         <v>3</v>
@@ -2002,7 +2002,7 @@
         <v>0</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -2034,7 +2034,7 @@
         <v>0</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -2130,7 +2130,7 @@
         <v>0</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -2162,7 +2162,7 @@
         <v>0</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -2194,7 +2194,7 @@
         <v>0</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -2202,10 +2202,10 @@
         <v>96</v>
       </c>
       <c r="B11" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>194</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>195</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>24</v>
@@ -2226,7 +2226,7 @@
         <v>0</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="225" x14ac:dyDescent="0.25">
@@ -2258,7 +2258,7 @@
         <v>0</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -2290,7 +2290,7 @@
         <v>2</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -2298,10 +2298,10 @@
         <v>96</v>
       </c>
       <c r="B14" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>206</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>207</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>24</v>
@@ -2322,7 +2322,7 @@
         <v>2</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="105" x14ac:dyDescent="0.25">
@@ -2354,7 +2354,7 @@
         <v>2</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="240" x14ac:dyDescent="0.25">
@@ -2386,7 +2386,7 @@
         <v>2</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2418,7 +2418,7 @@
         <v>2</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2458,10 +2458,10 @@
         <v>96</v>
       </c>
       <c r="B19" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="C19" s="3" t="s">
         <v>217</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>218</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>24</v>
@@ -2482,7 +2482,7 @@
         <v>2</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -2502,7 +2502,7 @@
         <v>20</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="G20" s="5" t="s">
         <v>94</v>
@@ -2514,7 +2514,7 @@
         <v>2</v>
       </c>
       <c r="J20" s="4" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2522,10 +2522,10 @@
         <v>96</v>
       </c>
       <c r="B21" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="C21" s="3" t="s">
         <v>192</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>193</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>24</v>
@@ -2546,7 +2546,7 @@
         <v>2</v>
       </c>
       <c r="J21" s="4" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -2554,10 +2554,10 @@
         <v>96</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>24</v>
@@ -2566,10 +2566,10 @@
         <v>59</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="H22" s="3">
         <v>10</v>
@@ -2578,7 +2578,7 @@
         <v>2</v>
       </c>
       <c r="J22" s="4" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
@@ -2610,7 +2610,7 @@
         <v>0</v>
       </c>
       <c r="J23" s="4" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -2642,7 +2642,7 @@
         <v>0</v>
       </c>
       <c r="J24" s="4" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -2674,7 +2674,7 @@
         <v>0</v>
       </c>
       <c r="J25" s="4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="105" x14ac:dyDescent="0.25">
@@ -2706,7 +2706,7 @@
         <v>0</v>
       </c>
       <c r="J26" s="4" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="409.5" x14ac:dyDescent="0.25">
@@ -2714,10 +2714,10 @@
         <v>38</v>
       </c>
       <c r="B27" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="C27" s="3" t="s">
         <v>208</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>209</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>24</v>
@@ -2726,10 +2726,10 @@
         <v>62</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="H27" s="3">
         <v>6</v>
@@ -2738,7 +2738,7 @@
         <v>0</v>
       </c>
       <c r="J27" s="4" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="105" x14ac:dyDescent="0.25">
@@ -2770,7 +2770,7 @@
         <v>0</v>
       </c>
       <c r="J28" s="4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="315" x14ac:dyDescent="0.25">
@@ -2802,7 +2802,7 @@
         <v>2</v>
       </c>
       <c r="J29" s="4" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2834,7 +2834,7 @@
         <v>2</v>
       </c>
       <c r="J30" s="4" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="31" spans="1:10" ht="285" x14ac:dyDescent="0.25">
@@ -2866,7 +2866,7 @@
         <v>2</v>
       </c>
       <c r="J31" s="4" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="255" x14ac:dyDescent="0.25">
@@ -2874,10 +2874,10 @@
         <v>38</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D32" s="3" t="s">
         <v>24</v>
@@ -2886,10 +2886,10 @@
         <v>60</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="G32" s="5" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="H32" s="3">
         <v>3</v>
@@ -2898,7 +2898,7 @@
         <v>2</v>
       </c>
       <c r="J32" s="4" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -2906,10 +2906,10 @@
         <v>38</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D33" s="3" t="s">
         <v>24</v>
@@ -2930,7 +2930,7 @@
         <v>2</v>
       </c>
       <c r="J33" s="4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
@@ -2950,7 +2950,7 @@
         <v>28</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G34" s="5" t="s">
         <v>20</v>
@@ -2994,7 +2994,7 @@
         <v>0</v>
       </c>
       <c r="J35" s="4" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="36" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3026,7 +3026,7 @@
         <v>0</v>
       </c>
       <c r="J36" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="37" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -3049,7 +3049,7 @@
         <v>30</v>
       </c>
       <c r="G37" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H37" s="3">
         <v>4</v>
@@ -3058,7 +3058,7 @@
         <v>0</v>
       </c>
       <c r="J37" s="4" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="38" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3090,7 +3090,7 @@
         <v>2</v>
       </c>
       <c r="J38" s="4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="39" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -3122,7 +3122,7 @@
         <v>2</v>
       </c>
       <c r="J39" s="4" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="40" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -3130,23 +3130,23 @@
         <v>130</v>
       </c>
       <c r="B40" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="C40" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="C40" s="3" t="s">
-        <v>157</v>
-      </c>
       <c r="D40" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E40" s="3">
         <v>13</v>
       </c>
       <c r="F40" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="G40" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="G40" s="3" t="s">
-        <v>158</v>
-      </c>
       <c r="H40" s="3">
         <v>0</v>
       </c>
@@ -3154,7 +3154,7 @@
         <v>0</v>
       </c>
       <c r="J40" s="4" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="41" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3162,13 +3162,13 @@
         <v>130</v>
       </c>
       <c r="B41" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="C41" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="C41" s="3" t="s">
+      <c r="D41" s="3" t="s">
         <v>149</v>
-      </c>
-      <c r="D41" s="3" t="s">
-        <v>150</v>
       </c>
       <c r="E41" s="3">
         <v>30</v>
@@ -3186,7 +3186,7 @@
         <v>0</v>
       </c>
       <c r="J41" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="42" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -3194,13 +3194,13 @@
         <v>130</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E42" s="3">
         <v>12</v>
@@ -3218,7 +3218,7 @@
         <v>0</v>
       </c>
       <c r="J42" s="4" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="43" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3226,13 +3226,13 @@
         <v>130</v>
       </c>
       <c r="B43" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="C43" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="C43" s="3" t="s">
+      <c r="D43" s="3" t="s">
         <v>161</v>
-      </c>
-      <c r="D43" s="3" t="s">
-        <v>162</v>
       </c>
       <c r="E43" s="3">
         <v>46</v>
@@ -3241,7 +3241,7 @@
         <v>93</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H43" s="3">
         <v>4</v>
@@ -3250,7 +3250,7 @@
         <v>0</v>
       </c>
       <c r="J43" s="4" t="s">
-        <v>263</v>
+        <v>272</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -3258,13 +3258,13 @@
         <v>130</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E44" s="3">
         <v>40</v>
@@ -3273,7 +3273,7 @@
         <v>93</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="H44" s="3">
         <v>6</v>
@@ -3282,7 +3282,7 @@
         <v>0</v>
       </c>
       <c r="J44" s="4" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="45" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3290,13 +3290,13 @@
         <v>130</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E45" s="3">
         <v>41</v>
@@ -3305,7 +3305,7 @@
         <v>93</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="H45" s="3">
         <v>7</v>
@@ -3314,7 +3314,7 @@
         <v>0</v>
       </c>
       <c r="J45" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="46" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3322,13 +3322,13 @@
         <v>130</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E46" s="3">
         <v>42</v>
@@ -3337,7 +3337,7 @@
         <v>93</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H46" s="3">
         <v>8</v>
@@ -3346,7 +3346,7 @@
         <v>0</v>
       </c>
       <c r="J46" s="4" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="47" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -3357,10 +3357,10 @@
         <v>131</v>
       </c>
       <c r="C47" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="D47" s="3" t="s">
         <v>132</v>
-      </c>
-      <c r="D47" s="3" t="s">
-        <v>133</v>
       </c>
       <c r="E47" s="3">
         <v>74</v>
@@ -3378,7 +3378,7 @@
         <v>2</v>
       </c>
       <c r="J47" s="4" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
     </row>
     <row r="48" spans="1:10" ht="135" x14ac:dyDescent="0.25">
@@ -3386,13 +3386,13 @@
         <v>130</v>
       </c>
       <c r="B48" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="C48" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="C48" s="3" t="s">
-        <v>135</v>
-      </c>
       <c r="D48" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E48" s="3">
         <v>11</v>
@@ -3410,7 +3410,7 @@
         <v>2</v>
       </c>
       <c r="J48" s="4" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
     </row>
     <row r="49" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -3418,13 +3418,13 @@
         <v>130</v>
       </c>
       <c r="B49" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="C49" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="C49" s="3" t="s">
-        <v>137</v>
-      </c>
       <c r="D49" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E49" s="3">
         <v>66</v>
@@ -3442,7 +3442,7 @@
         <v>2</v>
       </c>
       <c r="J49" s="4" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
     </row>
     <row r="50" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -3450,13 +3450,13 @@
         <v>130</v>
       </c>
       <c r="B50" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="C50" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="C50" s="3" t="s">
-        <v>139</v>
-      </c>
       <c r="D50" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E50" s="3">
         <v>32</v>
@@ -3474,7 +3474,7 @@
         <v>2</v>
       </c>
       <c r="J50" s="4" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
     </row>
     <row r="51" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -3482,13 +3482,13 @@
         <v>130</v>
       </c>
       <c r="B51" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="C51" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="C51" s="3" t="s">
-        <v>141</v>
-      </c>
       <c r="D51" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E51" s="3">
         <v>25</v>
@@ -3506,7 +3506,7 @@
         <v>2</v>
       </c>
       <c r="J51" s="4" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="52" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -3514,13 +3514,13 @@
         <v>130</v>
       </c>
       <c r="B52" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="C52" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="C52" s="3" t="s">
-        <v>143</v>
-      </c>
       <c r="D52" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E52" s="3">
         <v>34</v>
@@ -3538,7 +3538,7 @@
         <v>2</v>
       </c>
       <c r="J52" s="4" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="53" spans="1:10" ht="105" x14ac:dyDescent="0.25">
@@ -3546,13 +3546,13 @@
         <v>130</v>
       </c>
       <c r="B53" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="C53" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="C53" s="3" t="s">
-        <v>145</v>
-      </c>
       <c r="D53" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E53" s="3">
         <v>31</v>
@@ -3570,7 +3570,7 @@
         <v>2</v>
       </c>
       <c r="J53" s="4" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="54" spans="1:10" ht="120" x14ac:dyDescent="0.25">
@@ -3578,13 +3578,13 @@
         <v>130</v>
       </c>
       <c r="B54" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="C54" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="C54" s="3" t="s">
-        <v>147</v>
-      </c>
       <c r="D54" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E54" s="3">
         <v>61</v>
@@ -3602,7 +3602,7 @@
         <v>2</v>
       </c>
       <c r="J54" s="4" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="55" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3610,7 +3610,7 @@
         <v>9</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D55" s="3" t="s">
         <v>24</v>
@@ -3628,7 +3628,7 @@
         <v>0</v>
       </c>
       <c r="J55" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="56" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3674,7 +3674,7 @@
         <v>0</v>
       </c>
       <c r="J57" s="4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="58" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3701,7 +3701,7 @@
         <v>0</v>
       </c>
       <c r="J58" s="4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="59" spans="1:10" ht="105" x14ac:dyDescent="0.25">
@@ -3733,7 +3733,7 @@
         <v>0</v>
       </c>
       <c r="J59" s="4" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="60" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3829,7 +3829,7 @@
         <v>0</v>
       </c>
       <c r="J62" s="4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="63" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -3861,7 +3861,7 @@
         <v>0</v>
       </c>
       <c r="J63" s="4" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="64" spans="1:10" ht="409.5" x14ac:dyDescent="0.25">
@@ -3869,10 +3869,10 @@
         <v>69</v>
       </c>
       <c r="B64" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="C64" s="3" t="s">
         <v>200</v>
-      </c>
-      <c r="C64" s="3" t="s">
-        <v>201</v>
       </c>
       <c r="D64" s="3" t="s">
         <v>24</v>
@@ -3881,10 +3881,10 @@
         <v>70</v>
       </c>
       <c r="F64" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G64" s="5" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="H64" s="3">
         <v>6</v>
@@ -3893,7 +3893,7 @@
         <v>0</v>
       </c>
       <c r="J64" s="4" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
     </row>
     <row r="65" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -3913,7 +3913,7 @@
         <v>75</v>
       </c>
       <c r="F65" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="G65" s="5" t="s">
         <v>94</v>
@@ -3925,7 +3925,7 @@
         <v>0</v>
       </c>
       <c r="J65" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="66" spans="1:10" ht="195" x14ac:dyDescent="0.25">
@@ -3945,10 +3945,10 @@
         <v>44</v>
       </c>
       <c r="F66" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="G66" s="5" t="s">
         <v>186</v>
-      </c>
-      <c r="G66" s="5" t="s">
-        <v>187</v>
       </c>
       <c r="H66" s="3">
         <v>0</v>
@@ -3957,7 +3957,7 @@
         <v>2</v>
       </c>
       <c r="J66" s="8" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="67" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3989,7 +3989,7 @@
         <v>2</v>
       </c>
       <c r="J67" s="4" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="68" spans="1:10" ht="409.5" x14ac:dyDescent="0.25">
@@ -3997,10 +3997,10 @@
         <v>69</v>
       </c>
       <c r="B68" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="C68" s="3" t="s">
         <v>175</v>
-      </c>
-      <c r="C68" s="3" t="s">
-        <v>176</v>
       </c>
       <c r="D68" s="3" t="s">
         <v>24</v>
@@ -4009,10 +4009,10 @@
         <v>27</v>
       </c>
       <c r="F68" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G68" s="5" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="H68" s="3">
         <v>3</v>
@@ -4021,7 +4021,7 @@
         <v>2</v>
       </c>
       <c r="J68" s="4" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="69" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -4029,10 +4029,10 @@
         <v>69</v>
       </c>
       <c r="B69" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="C69" s="3" t="s">
         <v>173</v>
-      </c>
-      <c r="C69" s="3" t="s">
-        <v>174</v>
       </c>
       <c r="D69" s="3" t="s">
         <v>24</v>
@@ -4053,7 +4053,7 @@
         <v>2</v>
       </c>
       <c r="J69" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="70" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -4061,22 +4061,22 @@
         <v>69</v>
       </c>
       <c r="B70" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="C70" s="3" t="s">
         <v>214</v>
       </c>
-      <c r="C70" s="3" t="s">
+      <c r="D70" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E70" s="3">
+        <v>24</v>
+      </c>
+      <c r="F70" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="D70" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E70" s="3">
-        <v>24</v>
-      </c>
-      <c r="F70" s="3" t="s">
-        <v>216</v>
-      </c>
       <c r="G70" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="H70" s="3">
         <v>5</v>
@@ -4085,7 +4085,7 @@
         <v>2</v>
       </c>
       <c r="J70" s="4" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added PickLastSeeds to allow games to end when they should. Two options for PICKLASTSEEDS and PICK2XLASTSEEDS. Updated NumNum to use PICKLASTSEEDS. Updated Lam Waladach to use PICK2XLASTSEEDS and other differences from documented rules -- to make it a playable game. Both games now pass stress tests.
</commit_message>
<xml_diff>
--- a/src/game_params.xlsx
+++ b/src/game_params.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Activity_Data\Mancala_github\MancalaGames\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CD16CD8-1A11-4CC9-95E0-2AC99C564C14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4C239DA-480A-4606-A681-E8A9D521132F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="645" yWindow="480" windowWidth="23415" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4455" yWindow="480" windowWidth="23415" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="game_params" sheetId="1" r:id="rId1"/>
@@ -843,12 +843,6 @@
     <t>Repeat turn if there was a capture. Making children is not a capture.</t>
   </si>
   <si>
-    <t>Rules to allow taking of more than otherwise captured or picked seeds:
-- NONE: Nothing extra
-- PICKCROSS: Take the seeds from the opposite side of the board. 
-- PICKTWOS: Take seeds from all holes containing two seeds but only after the first move.</t>
-  </si>
-  <si>
     <t>Addiitonal child creation requirements may be set:
 - NONE: no additional restrictions.
 - OPP_ONLY:  Only make children on the opposite side of the board. Incompatible with BULL, QUR, and WEG child types.
@@ -975,6 +969,14 @@
   </si>
   <si>
     <t>The depth that the minimaxer or negamaxer will search the game tree from the current node. One value for each difficulty.</t>
+  </si>
+  <si>
+    <t>Rules to allow taking of more than otherwise captured or picked seeds:
+- NONE: Nothing extra
+- PICKCROSS: Take the seeds from the opposite side of the board. 
+- PICKTWOS: Take seeds from all holes containing two seeds but only after the first move.
+- PICKLASTSEEDS: If there are the number of starts seeds or fewer left,  the current player collects them and the game is over. This rule is applied at the end of each turn, even if there is not a capture because the sow phase may have reduced the seed count.
+- PICK2XLASTSEEDS: if there are 2 times the number of start seeds or fewer, the round starter picks them. This rule is applied at the end of each turn, even if there is not a capture because the sow phase may have reduced the seed count.</t>
   </si>
 </sst>
 </file>
@@ -1859,8 +1861,8 @@
   <dimension ref="A1:J70"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J48" sqref="J48"/>
+      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2322,7 +2324,7 @@
         <v>2</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="105" x14ac:dyDescent="0.25">
@@ -2482,7 +2484,7 @@
         <v>2</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -2549,7 +2551,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" ht="225" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>96</v>
       </c>
@@ -2578,7 +2580,7 @@
         <v>2</v>
       </c>
       <c r="J22" s="4" t="s">
-        <v>249</v>
+        <v>272</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
@@ -2738,7 +2740,7 @@
         <v>0</v>
       </c>
       <c r="J27" s="4" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="105" x14ac:dyDescent="0.25">
@@ -2802,7 +2804,7 @@
         <v>2</v>
       </c>
       <c r="J29" s="4" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3154,7 +3156,7 @@
         <v>0</v>
       </c>
       <c r="J40" s="4" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="41" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3186,7 +3188,7 @@
         <v>0</v>
       </c>
       <c r="J41" s="4" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="42" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -3218,7 +3220,7 @@
         <v>0</v>
       </c>
       <c r="J42" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="43" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3250,7 +3252,7 @@
         <v>0</v>
       </c>
       <c r="J43" s="4" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -3282,7 +3284,7 @@
         <v>0</v>
       </c>
       <c r="J44" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="45" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3314,7 +3316,7 @@
         <v>0</v>
       </c>
       <c r="J45" s="4" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="46" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3346,7 +3348,7 @@
         <v>0</v>
       </c>
       <c r="J46" s="4" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="47" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -3357,7 +3359,7 @@
         <v>131</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D47" s="3" t="s">
         <v>132</v>
@@ -3378,7 +3380,7 @@
         <v>2</v>
       </c>
       <c r="J47" s="4" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="48" spans="1:10" ht="135" x14ac:dyDescent="0.25">
@@ -3410,7 +3412,7 @@
         <v>2</v>
       </c>
       <c r="J48" s="4" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="49" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -3442,7 +3444,7 @@
         <v>2</v>
       </c>
       <c r="J49" s="4" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="50" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -3474,7 +3476,7 @@
         <v>2</v>
       </c>
       <c r="J50" s="4" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="51" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -3506,7 +3508,7 @@
         <v>2</v>
       </c>
       <c r="J51" s="4" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="52" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -3538,7 +3540,7 @@
         <v>2</v>
       </c>
       <c r="J52" s="4" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="53" spans="1:10" ht="105" x14ac:dyDescent="0.25">
@@ -3570,7 +3572,7 @@
         <v>2</v>
       </c>
       <c r="J53" s="4" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="54" spans="1:10" ht="120" x14ac:dyDescent="0.25">
@@ -3602,7 +3604,7 @@
         <v>2</v>
       </c>
       <c r="J54" s="4" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="55" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3893,7 +3895,7 @@
         <v>0</v>
       </c>
       <c r="J64" s="4" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="65" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -4021,7 +4023,7 @@
         <v>2</v>
       </c>
       <c r="J68" s="4" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="69" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -4085,7 +4087,7 @@
         <v>2</v>
       </c>
       <c r="J70" s="4" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Improved Cow, Goat, Mbangbi & split sow help text.
</commit_message>
<xml_diff>
--- a/src/game_params.xlsx
+++ b/src/game_params.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Activity_Data\Mancala_github\MancalaGames\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4C239DA-480A-4606-A681-E8A9D521132F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B9F48C3-D746-48ED-81B9-DC0232F96F05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4455" yWindow="480" windowWidth="23415" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -774,13 +774,6 @@
     <t>Sow seeds into your own store when passing it. Do not sow into your opponents store. Sow the final seed of a move into the store, results in a repeat turn.</t>
   </si>
   <si>
-    <t>Direction of sow:
-- CW: clockwise
-- CCW: counter-clockwise
-- SPLIT: left side holes sow counter-clockwise and right side holes sow clockwise, an odd middle hole must be set as UDIR_HOLE. 
-Any hole can be set as UDIR_HOLE to allow the user to override the sow_direct setting.</t>
-  </si>
-  <si>
     <t>Only valid when SOW_START is set. Changes the SOW_START behavior so that if there is only one seed in the hole, it is moved in the sow direction by one hole.</t>
   </si>
   <si>
@@ -977,6 +970,14 @@
 - PICKTWOS: Take seeds from all holes containing two seeds but only after the first move.
 - PICKLASTSEEDS: If there are the number of starts seeds or fewer left,  the current player collects them and the game is over. This rule is applied at the end of each turn, even if there is not a capture because the sow phase may have reduced the seed count.
 - PICK2XLASTSEEDS: if there are 2 times the number of start seeds or fewer, the round starter picks them. This rule is applied at the end of each turn, even if there is not a capture because the sow phase may have reduced the seed count.</t>
+  </si>
+  <si>
+    <t>Direction of sow:
+- CW: clockwise
+- CCW: counter-clockwise
+- SPLIT: left side holes sow counter-clockwise and right side holes sow clockwise, an odd middle hole must be set in UDIR_HOLES.
+Both mouse buttons will start a move no matter the sow direction. If the hole is marked as UDIR_HOLES, the button selects sow direction. On the other hand, if the hole is not marked as UDIR_HOLES, either button will sow in the prescribed direction. This can be useful, mechanism to remind yourself that on SPLIT sow, the left holes go CW by using the left button and the right holes go CCW by using the right button.
+Any hole can be set as UDIR_HOLES to allow the user to override the sow_direct setting.</t>
   </si>
 </sst>
 </file>
@@ -1861,8 +1862,8 @@
   <dimension ref="A1:J70"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J22" sqref="J22"/>
+      <pane ySplit="1" topLeftCell="A54" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J59" sqref="J59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2036,7 +2037,7 @@
         <v>0</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -2132,7 +2133,7 @@
         <v>0</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -2164,7 +2165,7 @@
         <v>0</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -2196,7 +2197,7 @@
         <v>0</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -2228,7 +2229,7 @@
         <v>0</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="225" x14ac:dyDescent="0.25">
@@ -2260,7 +2261,7 @@
         <v>0</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -2292,7 +2293,7 @@
         <v>2</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -2324,7 +2325,7 @@
         <v>2</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="105" x14ac:dyDescent="0.25">
@@ -2388,7 +2389,7 @@
         <v>2</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2420,7 +2421,7 @@
         <v>2</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2484,7 +2485,7 @@
         <v>2</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -2516,7 +2517,7 @@
         <v>2</v>
       </c>
       <c r="J20" s="4" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2548,7 +2549,7 @@
         <v>2</v>
       </c>
       <c r="J21" s="4" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="225" x14ac:dyDescent="0.25">
@@ -2580,7 +2581,7 @@
         <v>2</v>
       </c>
       <c r="J22" s="4" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
@@ -2740,7 +2741,7 @@
         <v>0</v>
       </c>
       <c r="J27" s="4" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="105" x14ac:dyDescent="0.25">
@@ -2804,7 +2805,7 @@
         <v>2</v>
       </c>
       <c r="J29" s="4" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3156,7 +3157,7 @@
         <v>0</v>
       </c>
       <c r="J40" s="4" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="41" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3188,7 +3189,7 @@
         <v>0</v>
       </c>
       <c r="J41" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="42" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -3220,7 +3221,7 @@
         <v>0</v>
       </c>
       <c r="J42" s="4" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="43" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3252,7 +3253,7 @@
         <v>0</v>
       </c>
       <c r="J43" s="4" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -3284,7 +3285,7 @@
         <v>0</v>
       </c>
       <c r="J44" s="4" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="45" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3316,7 +3317,7 @@
         <v>0</v>
       </c>
       <c r="J45" s="4" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="46" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3348,7 +3349,7 @@
         <v>0</v>
       </c>
       <c r="J46" s="4" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="47" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -3359,7 +3360,7 @@
         <v>131</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D47" s="3" t="s">
         <v>132</v>
@@ -3380,7 +3381,7 @@
         <v>2</v>
       </c>
       <c r="J47" s="4" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="48" spans="1:10" ht="135" x14ac:dyDescent="0.25">
@@ -3412,7 +3413,7 @@
         <v>2</v>
       </c>
       <c r="J48" s="4" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="49" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -3444,7 +3445,7 @@
         <v>2</v>
       </c>
       <c r="J49" s="4" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="50" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -3476,7 +3477,7 @@
         <v>2</v>
       </c>
       <c r="J50" s="4" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="51" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -3508,7 +3509,7 @@
         <v>2</v>
       </c>
       <c r="J51" s="4" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="52" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -3540,7 +3541,7 @@
         <v>2</v>
       </c>
       <c r="J52" s="4" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="53" spans="1:10" ht="105" x14ac:dyDescent="0.25">
@@ -3572,7 +3573,7 @@
         <v>2</v>
       </c>
       <c r="J53" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="54" spans="1:10" ht="120" x14ac:dyDescent="0.25">
@@ -3604,7 +3605,7 @@
         <v>2</v>
       </c>
       <c r="J54" s="4" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="55" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3706,7 +3707,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="59" spans="1:10" ht="105" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" ht="210" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
         <v>69</v>
       </c>
@@ -3735,7 +3736,7 @@
         <v>0</v>
       </c>
       <c r="J59" s="4" t="s">
-        <v>234</v>
+        <v>272</v>
       </c>
     </row>
     <row r="60" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3863,7 +3864,7 @@
         <v>0</v>
       </c>
       <c r="J63" s="4" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="64" spans="1:10" ht="409.5" x14ac:dyDescent="0.25">
@@ -3895,7 +3896,7 @@
         <v>0</v>
       </c>
       <c r="J64" s="4" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="65" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -3959,7 +3960,7 @@
         <v>2</v>
       </c>
       <c r="J66" s="8" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="67" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3991,7 +3992,7 @@
         <v>2</v>
       </c>
       <c r="J67" s="4" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="68" spans="1:10" ht="409.5" x14ac:dyDescent="0.25">
@@ -4023,7 +4024,7 @@
         <v>2</v>
       </c>
       <c r="J68" s="4" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="69" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -4087,7 +4088,7 @@
         <v>2</v>
       </c>
       <c r="J70" s="4" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated capture related parameter descriptions.
</commit_message>
<xml_diff>
--- a/src/game_params.xlsx
+++ b/src/game_params.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Activity_Data\Mancala_github\MancalaGames\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B9F48C3-D746-48ED-81B9-DC0232F96F05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55051D06-49DF-4E44-9F9C-4B4279703F17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4455" yWindow="480" windowWidth="23415" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="game_params" sheetId="1" r:id="rId1"/>
@@ -401,9 +401,6 @@
     <t>Multiple Captures</t>
   </si>
   <si>
-    <t>After the initial capture, continue capturing as long as the capture conditions are met.</t>
-  </si>
-  <si>
     <t>grandslam</t>
   </si>
   <si>
@@ -786,37 +783,6 @@
 - LAPPER_NEXT:  If the first sow ends in a hole preceeding a hole with any seeds, pick up the seeds from that next hole and continue sowing another lap. Continue until the hole after the laps final seed is empty.</t>
   </si>
   <si>
-    <t>Only meaninful, with MULTICAPT. Captures are done in the same direction as the sowing, i.e. following the final hole sown. If not set, captures are done from the holes just sown.</t>
-  </si>
-  <si>
-    <t>Capture when a hole contains an even number of seeds, greater than 0.
-Additionally, a SOWRULE of OWN_SOW_CAPT_ALL or SOW_SOW_CAPT_ALL includes this capture mechanism.</t>
-  </si>
-  <si>
-    <t>Capture when the contents of the hole are less than or equal to capt_max.
-Additionally, a SOWRULE of OWN_SOW_CAPT_ALL or SOW_SOW_CAPT_ALL includes this capture mechanism.</t>
-  </si>
-  <si>
-    <t>Capture when the contents of the hole are greater than or equal to capt_min.
-Additionally, a SOWRULE of OWN_SOW_CAPT_ALL or SOW_SOW_CAPT_ALL includes this capture mechanism.</t>
-  </si>
-  <si>
-    <t>Capture from the hole after the final seed sown into an empty hole. 
-Additionally, a SOWRULE of OWN_SOW_CAPT_ALL or SOW_SOW_CAPT_ALL includes this capture mechanism.</t>
-  </si>
-  <si>
-    <t>There are three flavors of capture two out:
-Single Lap: capture if sow ends in occupied hole, then an empty hole, followed by an occupied hole (this is hole captured).
-Multi lap but single capture: capture when last hole sown is followed by an empty hole which is then followed by an occupied hole.
-Multi lap with multiple captures: capture when last hole sown is followed by an empty hole which is then followed by an occupied hole. Continue captures as long as the pattern of empty hole followed by an occupied hole continues.
-Additionally, a SOWRULE of OWN_SOW_CAPT_ALL or SOW_SOW_CAPT_ALL includes this capture mechanism.
-OPPSIDECAPT, EVENS, CAPT_MAX, CAPT_MIN, and CAPT_ON apply only to an optional xxx_SOW_CAPT_ALL and not the final capture.</t>
-  </si>
-  <si>
-    <t>If the last sown seed is put in an empty hole, any seeds on the opposite side of the board are captured.
-SOW_RULE of either SOW_CAPT_ALL do not do this capture.</t>
-  </si>
-  <si>
     <t>A grandslam is when your opponent has seeds at the start of your turn and you capture them all. This option selects what to do:
 - LEGAL: the seeds are captured
 - NOT_LEGAL: you may not capture all of your opponents seeds, a move which would do so is not allowed
@@ -824,13 +790,6 @@
 - OPP_GETS_REMAIN: if you capture all your opponents seeds, they capture all of your remaining seeds and the game is over. Winner is determined by game goal.
 - LEAVE_LEFT: the capture is performed from all but the leftmost hole from the sower perspective. This might leave your oppenents without seeds or might not capture any seeds.
 - LEAVE_RIGHT: the capture is performed from all but the rightmost hole from the sower perspective. This might leave your oppenents without seeds.</t>
-  </si>
-  <si>
-    <t>Holes in the game start each round locked. Captures may not be made from locked holes. Starting a sow from a hole unlocks it.</t>
-  </si>
-  <si>
-    <t>Capture when the contents of the hole is in the capt_on list. 
-Additionally, a SOWRULE of OWN_SOW_CAPT_ALL or SOW_SOW_CAPT_ALL includes this capture mechanism.</t>
   </si>
   <si>
     <t>Repeat turn if there was a capture. Making children is not a capture.</t>
@@ -865,18 +824,6 @@
 - TERRITORY: claim ownership of holes. Each round the ownership of holes is determined by the number of seeds captured in the previous round. In a TERRITORY game without rounds, the winner is the player that gained the most territory during play. 
   + TERRITORY games require STORES and that GPARAM_ONE be set to a value between the number of holes and two times the number of holes.
   + TERRITORY games are incompatible with NO_SIDES, START_PATTERN, GRANDSLAM of NOT_LEGAL, ALLOW_RULE of OPP_OR_EMPTY, </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Games with children allow players to claim holes. These child holes are an extension of the stores and seeds in them count towards a win. Making a child stops any multiple lap sowing, moves cannot start from children, and they cannot be captured.
-- NOCHILD: children are not used.
-- NORMAL: children are made when a final seeds sows a hole to CHILD_CVT.
-- WALDA: STORES are not supported. Captures are instead moved into waldas, thus a player may not capture until they have created a walda. 
-  + Walda locations are limited.  Each player may create up to 6 waldas: on either end of each side of the board and the next outer hole on their own side of the board. Note that there are only 8 total places that waldas maybe created.
-- ONE_CHILD: only one child allowed per player, may not be in player's left most hole,  and may not be opposite eachother. Used to create tuzdek style children along with CHILD_RULE of OPP_ONLY.
-- WEG: children maybe created in holes owned by the opponent. Ending a sow in an opponent's weg captures the seed just sown and one more (if there is one); generally, the player gets to play again (per CAPT_RTURN). WEGs are supported for TERRITORY games only (hole ownership required).
-- BULL: create one bull if final seed sows to CHILD_CVT, create two bulls if the final two seeds are sown to CHILD_CVT-1 and CHILD_CVT (in either order).
-- QUR: when a seed is sown into an empty hole on the player's side of the board and the opposite hole contains CHILD_CVT, create children in both holes: final seed location and opposite.
-</t>
   </si>
   <si>
     <t>Don't allow captures or closing of holes (SOW_RULE of SOW_BLKD_DIV) on the first move of the game or round.</t>
@@ -964,20 +911,80 @@
     <t>The depth that the minimaxer or negamaxer will search the game tree from the current node. One value for each difficulty.</t>
   </si>
   <si>
-    <t>Rules to allow taking of more than otherwise captured or picked seeds:
-- NONE: Nothing extra
-- PICKCROSS: Take the seeds from the opposite side of the board. 
-- PICKTWOS: Take seeds from all holes containing two seeds but only after the first move.
-- PICKLASTSEEDS: If there are the number of starts seeds or fewer left,  the current player collects them and the game is over. This rule is applied at the end of each turn, even if there is not a capture because the sow phase may have reduced the seed count.
-- PICK2XLASTSEEDS: if there are 2 times the number of start seeds or fewer, the round starter picks them. This rule is applied at the end of each turn, even if there is not a capture because the sow phase may have reduced the seed count.</t>
-  </si>
-  <si>
     <t>Direction of sow:
 - CW: clockwise
 - CCW: counter-clockwise
 - SPLIT: left side holes sow counter-clockwise and right side holes sow clockwise, an odd middle hole must be set in UDIR_HOLES.
 Both mouse buttons will start a move no matter the sow direction. If the hole is marked as UDIR_HOLES, the button selects sow direction. On the other hand, if the hole is not marked as UDIR_HOLES, either button will sow in the prescribed direction. This can be useful, mechanism to remind yourself that on SPLIT sow, the left holes go CW by using the left button and the right holes go CCW by using the right button.
 Any hole can be set as UDIR_HOLES to allow the user to override the sow_direct setting.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Capture from the hole after the final seed sown into an empty hole. 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">There are three flavors of capture two out:
+Single Lap: capture if sow ends in occupied hole, then an empty hole, followed by an occupied hole (this is hole captured).
+Multi lap but single capture: capture when last hole sown is followed by an empty hole which is then followed by an occupied hole.
+Multi lap with multiple captures: capture when last hole sown is followed by an empty hole which is then followed by an occupied hole. Continue captures as long as the pattern of empty hole followed by an occupied hole continues.
+</t>
+  </si>
+  <si>
+    <t>After the initial capture, continue capturing as long as the capture conditions are met. This multiple capture may happen in the sow direction (unsown holes) or in the opposite direction (sown holes) as determined by CAPSAMEDIR.
+See individual capture mechanism for any special requirements.</t>
+  </si>
+  <si>
+    <t>Only meaninful with MULTICAPT. Captures are done in the same direction as the sowing, i.e. following the final hole sown. If not set, captures are done from the holes just sown.</t>
+  </si>
+  <si>
+    <t>Capture when a hole contains an even number of seeds, greater than 0. When selected with other basic capture mechanisms, the capture mechanism are ANDed (all must be true for capture). Basic capture mechanisms are: CAPT_MAX, CAPT_MIN, CAPT_ON and EVENS with restrictions from OPPSIDECAPT, MOVEUNLOCK and not child holes of any type.
+MLAPS LAPPER sowing will stop the sowing on a final seed that would capture based on the selected basic capture mechanisms.
+Either SOW_RULE of OWN_SOW_CAPT_ALL or SOW_SOW_CAPT_ALL includes the basic capture mechanisms.</t>
+  </si>
+  <si>
+    <t>Capture when the contents of the hole are less than or equal to capt_max.
+When selected with other basic capture mechanisms, the capture mechanism are ANDed (all must be true for capture). Basic capture mechanisms are: CAPT_MAX, CAPT_MIN, CAPT_ON and EVENS  with restrictions from OPPSIDECAPT, MOVEUNLOCK and not child holes of any type.
+MLAPS LAPPER sowing will stop the sowing on a final seed that would capture based on the selected basic capture mechanisms.
+Either SOW_RULE of OWN_SOW_CAPT_ALL or SOW_SOW_CAPT_ALL includes the basic capture mechanisms.</t>
+  </si>
+  <si>
+    <t>Capture when the contents of the hole are greater than or equal to capt_min.
+When selected with other basic capture mechanisms, the capture mechanism are ANDed (all must be true for capture). Basic capture mechanisms are: CAPT_MAX, CAPT_MIN, CAPT_ON and EVENS  with restrictions from OPPSIDECAPT, MOVEUNLOCK and not child holes of any type.
+MLAP LAPPER sowing will stop the sowing on a final seed that would capture based on the selected basic capture mechanisms.
+Either SOW_RULE of OWN_SOW_CAPT_ALL or SOW_SOW_CAPT_ALL includes the basic capture mechanisms.</t>
+  </si>
+  <si>
+    <t>If the last sown seed is put in an empty hole, seeds on the opposite side of the board are captured. The capture of those seeds can be limited by CAPT_MAX, CAPT_MIN, CAPT_ON, EVENS, MOVEUNLOCK, OPPSIDECAPT. For example, crosscapt with evens will only capture when there are an even number of seeds in the opposite hole.
+SOW_RULE of either SOW_CAPT_ALL do not do this capture.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Games with children allow players to claim holes. These child holes are an extension of the stores and seeds in them count towards a win. Making a child stops any multiple lap sowing, moves cannot start from children, and they cannot be captured (except for special rules associated with WEGs).
+- NOCHILD: children are not used.
+- NORMAL: children are made when a final seeds sows a hole to CHILD_CVT.
+- WALDA: STORES are not supported. Captures are instead moved into waldas, thus a player may not capture until they have created a walda. 
+  + Walda locations are limited.  Each player may create up to 6 waldas: on either end of each side of the board and the next outer hole on their own side of the board. Note that there are only 8 total places that waldas maybe created.
+- ONE_CHILD: only one child allowed per player, may not be in player's left most hole,  and may not be opposite eachother. Used to create tuzdek style children along with CHILD_RULE of OPP_ONLY.
+- WEG: children maybe created in holes owned by the opponent. Ending a sow in an opponent's weg captures the seed just sown and one more (if there is one); generally, the player gets to play again (per CAPT_RTURN). WEGs are supported for TERRITORY games only (hole ownership required).
+- BULL: create one bull if final seed sows to CHILD_CVT, create two bulls if the final two seeds are sown to CHILD_CVT-1 and CHILD_CVT (in either order).
+- QUR: when a seed is sown into an empty hole on the player's side of the board and the opposite hole contains CHILD_CVT, create children in both holes: final seed location and opposite.
+</t>
+  </si>
+  <si>
+    <t>Holes in the game start each game and round locked. Captures may not be made from locked holes. Starting a sow from a hole unlocks it allowing future captures.</t>
+  </si>
+  <si>
+    <t>Capture when the contents of the hole is in the capt_on list. 
+When selected with other basic capture mechanisms, the capture mechanism are ANDed (all must be true for capture). Basic capture mechanisms are: CAPT_MAX, CAPT_MIN, CAPT_ON and EVENS   with restrictions from OPPSIDECAPT, MOVEUNLOCK and not child holes of any type.
+MLAP LAPPER sowing will stop the sowing on a final seed that would capture based on the selected basic capture mechanisms.
+Either SOWRULE of OWN_SOW_CAPT_ALL or SOW_SOW_CAPT_ALL includes the basic capture mechanisms.</t>
+  </si>
+  <si>
+    <t>Rules to allow taking of more than otherwise captured or picked seeds:
+- NONE: Nothing extra
+- PICKCROSS: Take the seeds from the opposite side of the board. 
+- PICKTWOS: Take seeds from all holes containing two seeds but only after the first move.
+- PICKLASTSEEDS: If there are the number of starts seeds or fewer left,  the current player collects them and the game is over. This rule is applied at the end of each turn, even if there is not a capture because the sow phase may have reduced the seed count.
+- PICK2XLASTSEEDS: If there are 2 times the number of start seeds or fewer, the round starter picks them. This rule is applied at the end of each turn, even if there is not a capture because the sow phase may have reduced the seed count.</t>
   </si>
 </sst>
 </file>
@@ -1862,8 +1869,8 @@
   <dimension ref="A1:J70"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A54" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J59" sqref="J59"/>
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1894,7 +1901,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>4</v>
@@ -1973,7 +1980,7 @@
         <v>0</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="345" x14ac:dyDescent="0.25">
@@ -1981,10 +1988,10 @@
         <v>62</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>179</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>180</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>24</v>
@@ -1993,10 +2000,10 @@
         <v>14</v>
       </c>
       <c r="F4" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="G4" s="5" t="s">
         <v>181</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>182</v>
       </c>
       <c r="H4" s="3">
         <v>3</v>
@@ -2005,7 +2012,7 @@
         <v>0</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -2037,7 +2044,7 @@
         <v>0</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>237</v>
+        <v>264</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -2072,7 +2079,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>96</v>
       </c>
@@ -2101,10 +2108,10 @@
         <v>0</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="150" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>96</v>
       </c>
@@ -2133,10 +2140,10 @@
         <v>0</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="165" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>96</v>
       </c>
@@ -2165,10 +2172,10 @@
         <v>0</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="165" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>96</v>
       </c>
@@ -2197,18 +2204,18 @@
         <v>0</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>96</v>
       </c>
       <c r="B11" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>193</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>194</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>24</v>
@@ -2229,18 +2236,18 @@
         <v>0</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="225" x14ac:dyDescent="0.25">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="165" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>96</v>
       </c>
       <c r="B12" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>128</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>129</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>24</v>
@@ -2261,10 +2268,10 @@
         <v>0</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>96</v>
       </c>
@@ -2293,7 +2300,7 @@
         <v>2</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>243</v>
+        <v>268</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -2301,10 +2308,10 @@
         <v>96</v>
       </c>
       <c r="B14" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>205</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>206</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>24</v>
@@ -2325,7 +2332,7 @@
         <v>2</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>250</v>
+        <v>240</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="105" x14ac:dyDescent="0.25">
@@ -2357,7 +2364,7 @@
         <v>2</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="240" x14ac:dyDescent="0.25">
@@ -2365,10 +2372,10 @@
         <v>96</v>
       </c>
       <c r="B16" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>122</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>123</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>24</v>
@@ -2377,10 +2384,10 @@
         <v>37</v>
       </c>
       <c r="F16" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="G16" s="5" t="s">
         <v>124</v>
-      </c>
-      <c r="G16" s="5" t="s">
-        <v>125</v>
       </c>
       <c r="H16" s="3">
         <v>3</v>
@@ -2389,10 +2396,10 @@
         <v>2</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>96</v>
       </c>
@@ -2421,7 +2428,7 @@
         <v>2</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>245</v>
+        <v>270</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2461,10 +2468,10 @@
         <v>96</v>
       </c>
       <c r="B19" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="C19" s="3" t="s">
         <v>216</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>217</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>24</v>
@@ -2485,18 +2492,18 @@
         <v>2</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="150" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>96</v>
       </c>
       <c r="B20" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="C20" s="3" t="s">
         <v>126</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>127</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>24</v>
@@ -2505,7 +2512,7 @@
         <v>20</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G20" s="5" t="s">
         <v>94</v>
@@ -2517,7 +2524,7 @@
         <v>2</v>
       </c>
       <c r="J20" s="4" t="s">
-        <v>246</v>
+        <v>271</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2525,10 +2532,10 @@
         <v>96</v>
       </c>
       <c r="B21" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="C21" s="3" t="s">
         <v>191</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>192</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>24</v>
@@ -2549,7 +2556,7 @@
         <v>2</v>
       </c>
       <c r="J21" s="4" t="s">
-        <v>247</v>
+        <v>237</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="225" x14ac:dyDescent="0.25">
@@ -2557,10 +2564,10 @@
         <v>96</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>24</v>
@@ -2569,10 +2576,10 @@
         <v>59</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="H22" s="3">
         <v>10</v>
@@ -2581,7 +2588,7 @@
         <v>2</v>
       </c>
       <c r="J22" s="4" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
@@ -2613,7 +2620,7 @@
         <v>0</v>
       </c>
       <c r="J23" s="4" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -2645,7 +2652,7 @@
         <v>0</v>
       </c>
       <c r="J24" s="4" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -2677,7 +2684,7 @@
         <v>0</v>
       </c>
       <c r="J25" s="4" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="105" x14ac:dyDescent="0.25">
@@ -2709,7 +2716,7 @@
         <v>0</v>
       </c>
       <c r="J26" s="4" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="409.5" x14ac:dyDescent="0.25">
@@ -2717,10 +2724,10 @@
         <v>38</v>
       </c>
       <c r="B27" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="C27" s="3" t="s">
         <v>207</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>208</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>24</v>
@@ -2729,10 +2736,10 @@
         <v>62</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="H27" s="3">
         <v>6</v>
@@ -2741,7 +2748,7 @@
         <v>0</v>
       </c>
       <c r="J27" s="4" t="s">
-        <v>249</v>
+        <v>239</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="105" x14ac:dyDescent="0.25">
@@ -2773,7 +2780,7 @@
         <v>0</v>
       </c>
       <c r="J28" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="315" x14ac:dyDescent="0.25">
@@ -2805,7 +2812,7 @@
         <v>2</v>
       </c>
       <c r="J29" s="4" t="s">
-        <v>251</v>
+        <v>241</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2837,7 +2844,7 @@
         <v>2</v>
       </c>
       <c r="J30" s="4" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="31" spans="1:10" ht="285" x14ac:dyDescent="0.25">
@@ -2869,7 +2876,7 @@
         <v>2</v>
       </c>
       <c r="J31" s="4" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="255" x14ac:dyDescent="0.25">
@@ -2877,10 +2884,10 @@
         <v>38</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D32" s="3" t="s">
         <v>24</v>
@@ -2889,10 +2896,10 @@
         <v>60</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G32" s="5" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="H32" s="3">
         <v>3</v>
@@ -2901,7 +2908,7 @@
         <v>2</v>
       </c>
       <c r="J32" s="4" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -2909,10 +2916,10 @@
         <v>38</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D33" s="3" t="s">
         <v>24</v>
@@ -2933,7 +2940,7 @@
         <v>2</v>
       </c>
       <c r="J33" s="4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
@@ -2953,7 +2960,7 @@
         <v>28</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G34" s="5" t="s">
         <v>20</v>
@@ -2997,7 +3004,7 @@
         <v>0</v>
       </c>
       <c r="J35" s="4" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="36" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3029,7 +3036,7 @@
         <v>0</v>
       </c>
       <c r="J36" s="4" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="37" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -3052,7 +3059,7 @@
         <v>30</v>
       </c>
       <c r="G37" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H37" s="3">
         <v>4</v>
@@ -3061,7 +3068,7 @@
         <v>0</v>
       </c>
       <c r="J37" s="4" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="38" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3093,7 +3100,7 @@
         <v>2</v>
       </c>
       <c r="J38" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="39" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -3125,31 +3132,31 @@
         <v>2</v>
       </c>
       <c r="J39" s="4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="40" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B40" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="C40" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="C40" s="3" t="s">
-        <v>156</v>
-      </c>
       <c r="D40" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E40" s="3">
         <v>13</v>
       </c>
       <c r="F40" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="G40" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="G40" s="3" t="s">
-        <v>157</v>
-      </c>
       <c r="H40" s="3">
         <v>0</v>
       </c>
@@ -3157,21 +3164,21 @@
         <v>0</v>
       </c>
       <c r="J40" s="4" t="s">
-        <v>254</v>
+        <v>243</v>
       </c>
     </row>
     <row r="41" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B41" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="C41" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="C41" s="3" t="s">
+      <c r="D41" s="3" t="s">
         <v>148</v>
-      </c>
-      <c r="D41" s="3" t="s">
-        <v>149</v>
       </c>
       <c r="E41" s="3">
         <v>30</v>
@@ -3189,21 +3196,21 @@
         <v>0</v>
       </c>
       <c r="J41" s="4" t="s">
-        <v>258</v>
+        <v>247</v>
       </c>
     </row>
     <row r="42" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E42" s="3">
         <v>12</v>
@@ -3221,21 +3228,21 @@
         <v>0</v>
       </c>
       <c r="J42" s="4" t="s">
-        <v>259</v>
+        <v>248</v>
       </c>
     </row>
     <row r="43" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B43" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="C43" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="C43" s="3" t="s">
+      <c r="D43" s="3" t="s">
         <v>160</v>
-      </c>
-      <c r="D43" s="3" t="s">
-        <v>161</v>
       </c>
       <c r="E43" s="3">
         <v>46</v>
@@ -3244,7 +3251,7 @@
         <v>93</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="H43" s="3">
         <v>4</v>
@@ -3253,21 +3260,21 @@
         <v>0</v>
       </c>
       <c r="J43" s="4" t="s">
-        <v>270</v>
+        <v>259</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E44" s="3">
         <v>40</v>
@@ -3276,7 +3283,7 @@
         <v>93</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="H44" s="3">
         <v>6</v>
@@ -3285,21 +3292,21 @@
         <v>0</v>
       </c>
       <c r="J44" s="4" t="s">
-        <v>257</v>
+        <v>246</v>
       </c>
     </row>
     <row r="45" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E45" s="3">
         <v>41</v>
@@ -3308,7 +3315,7 @@
         <v>93</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H45" s="3">
         <v>7</v>
@@ -3317,21 +3324,21 @@
         <v>0</v>
       </c>
       <c r="J45" s="4" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
     </row>
     <row r="46" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E46" s="3">
         <v>42</v>
@@ -3340,7 +3347,7 @@
         <v>93</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H46" s="3">
         <v>8</v>
@@ -3349,21 +3356,21 @@
         <v>0</v>
       </c>
       <c r="J46" s="4" t="s">
-        <v>255</v>
+        <v>244</v>
       </c>
     </row>
     <row r="47" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="B47" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="B47" s="3" t="s">
+      <c r="C47" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="D47" s="3" t="s">
         <v>131</v>
-      </c>
-      <c r="C47" s="3" t="s">
-        <v>269</v>
-      </c>
-      <c r="D47" s="3" t="s">
-        <v>132</v>
       </c>
       <c r="E47" s="3">
         <v>74</v>
@@ -3381,21 +3388,21 @@
         <v>2</v>
       </c>
       <c r="J47" s="4" t="s">
-        <v>268</v>
+        <v>257</v>
       </c>
     </row>
     <row r="48" spans="1:10" ht="135" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B48" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="C48" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="C48" s="3" t="s">
-        <v>134</v>
-      </c>
       <c r="D48" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E48" s="3">
         <v>11</v>
@@ -3413,21 +3420,21 @@
         <v>2</v>
       </c>
       <c r="J48" s="4" t="s">
-        <v>265</v>
+        <v>254</v>
       </c>
     </row>
     <row r="49" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B49" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="C49" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="C49" s="3" t="s">
-        <v>136</v>
-      </c>
       <c r="D49" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E49" s="3">
         <v>66</v>
@@ -3445,21 +3452,21 @@
         <v>2</v>
       </c>
       <c r="J49" s="4" t="s">
-        <v>263</v>
+        <v>252</v>
       </c>
     </row>
     <row r="50" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B50" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="C50" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="C50" s="3" t="s">
-        <v>138</v>
-      </c>
       <c r="D50" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E50" s="3">
         <v>32</v>
@@ -3477,21 +3484,21 @@
         <v>2</v>
       </c>
       <c r="J50" s="4" t="s">
-        <v>264</v>
+        <v>253</v>
       </c>
     </row>
     <row r="51" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B51" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="C51" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="C51" s="3" t="s">
-        <v>140</v>
-      </c>
       <c r="D51" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E51" s="3">
         <v>25</v>
@@ -3509,21 +3516,21 @@
         <v>2</v>
       </c>
       <c r="J51" s="4" t="s">
-        <v>262</v>
+        <v>251</v>
       </c>
     </row>
     <row r="52" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B52" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="C52" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="C52" s="3" t="s">
-        <v>142</v>
-      </c>
       <c r="D52" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E52" s="3">
         <v>34</v>
@@ -3541,21 +3548,21 @@
         <v>2</v>
       </c>
       <c r="J52" s="4" t="s">
-        <v>261</v>
+        <v>250</v>
       </c>
     </row>
     <row r="53" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B53" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="C53" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="C53" s="3" t="s">
-        <v>144</v>
-      </c>
       <c r="D53" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E53" s="3">
         <v>31</v>
@@ -3573,21 +3580,21 @@
         <v>2</v>
       </c>
       <c r="J53" s="4" t="s">
-        <v>260</v>
+        <v>249</v>
       </c>
     </row>
     <row r="54" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B54" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="C54" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="C54" s="3" t="s">
-        <v>146</v>
-      </c>
       <c r="D54" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E54" s="3">
         <v>61</v>
@@ -3605,7 +3612,7 @@
         <v>2</v>
       </c>
       <c r="J54" s="4" t="s">
-        <v>266</v>
+        <v>255</v>
       </c>
     </row>
     <row r="55" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3613,7 +3620,7 @@
         <v>9</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D55" s="3" t="s">
         <v>24</v>
@@ -3631,7 +3638,7 @@
         <v>0</v>
       </c>
       <c r="J55" s="4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="56" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3677,7 +3684,7 @@
         <v>0</v>
       </c>
       <c r="J57" s="4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="58" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3704,7 +3711,7 @@
         <v>0</v>
       </c>
       <c r="J58" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="59" spans="1:10" ht="210" x14ac:dyDescent="0.25">
@@ -3736,7 +3743,7 @@
         <v>0</v>
       </c>
       <c r="J59" s="4" t="s">
-        <v>272</v>
+        <v>260</v>
       </c>
     </row>
     <row r="60" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3832,7 +3839,7 @@
         <v>0</v>
       </c>
       <c r="J62" s="4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="63" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -3864,7 +3871,7 @@
         <v>0</v>
       </c>
       <c r="J63" s="4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="64" spans="1:10" ht="409.5" x14ac:dyDescent="0.25">
@@ -3872,10 +3879,10 @@
         <v>69</v>
       </c>
       <c r="B64" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="C64" s="3" t="s">
         <v>199</v>
-      </c>
-      <c r="C64" s="3" t="s">
-        <v>200</v>
       </c>
       <c r="D64" s="3" t="s">
         <v>24</v>
@@ -3884,10 +3891,10 @@
         <v>70</v>
       </c>
       <c r="F64" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G64" s="5" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="H64" s="3">
         <v>6</v>
@@ -3896,7 +3903,7 @@
         <v>0</v>
       </c>
       <c r="J64" s="4" t="s">
-        <v>267</v>
+        <v>256</v>
       </c>
     </row>
     <row r="65" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -3916,7 +3923,7 @@
         <v>75</v>
       </c>
       <c r="F65" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G65" s="5" t="s">
         <v>94</v>
@@ -3928,7 +3935,7 @@
         <v>0</v>
       </c>
       <c r="J65" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="66" spans="1:10" ht="195" x14ac:dyDescent="0.25">
@@ -3948,10 +3955,10 @@
         <v>44</v>
       </c>
       <c r="F66" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="G66" s="5" t="s">
         <v>185</v>
-      </c>
-      <c r="G66" s="5" t="s">
-        <v>186</v>
       </c>
       <c r="H66" s="3">
         <v>0</v>
@@ -3960,7 +3967,7 @@
         <v>2</v>
       </c>
       <c r="J66" s="8" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="67" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3992,7 +3999,7 @@
         <v>2</v>
       </c>
       <c r="J67" s="4" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="68" spans="1:10" ht="409.5" x14ac:dyDescent="0.25">
@@ -4000,10 +4007,10 @@
         <v>69</v>
       </c>
       <c r="B68" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="C68" s="3" t="s">
         <v>174</v>
-      </c>
-      <c r="C68" s="3" t="s">
-        <v>175</v>
       </c>
       <c r="D68" s="3" t="s">
         <v>24</v>
@@ -4012,10 +4019,10 @@
         <v>27</v>
       </c>
       <c r="F68" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="G68" s="5" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="H68" s="3">
         <v>3</v>
@@ -4024,7 +4031,7 @@
         <v>2</v>
       </c>
       <c r="J68" s="4" t="s">
-        <v>252</v>
+        <v>269</v>
       </c>
     </row>
     <row r="69" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -4032,10 +4039,10 @@
         <v>69</v>
       </c>
       <c r="B69" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="C69" s="3" t="s">
         <v>172</v>
-      </c>
-      <c r="C69" s="3" t="s">
-        <v>173</v>
       </c>
       <c r="D69" s="3" t="s">
         <v>24</v>
@@ -4056,7 +4063,7 @@
         <v>2</v>
       </c>
       <c r="J69" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="70" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -4064,22 +4071,22 @@
         <v>69</v>
       </c>
       <c r="B70" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="C70" s="3" t="s">
         <v>213</v>
       </c>
-      <c r="C70" s="3" t="s">
+      <c r="D70" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E70" s="3">
+        <v>24</v>
+      </c>
+      <c r="F70" s="3" t="s">
         <v>214</v>
       </c>
-      <c r="D70" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E70" s="3">
-        <v>24</v>
-      </c>
-      <c r="F70" s="3" t="s">
-        <v>215</v>
-      </c>
       <c r="G70" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="H70" s="3">
         <v>5</v>
@@ -4088,7 +4095,7 @@
         <v>2</v>
       </c>
       <c r="J70" s="4" t="s">
-        <v>248</v>
+        <v>238</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Created a new class of tests for demo composites (test_cmp_...) to test odd ways the decos might or might not work together. Started writing sower deco composite tests (including starter), found some problems, generated rules to avoid or fixed the code (several assumptions in PLUS1MINUS1 were eliminated).
</commit_message>
<xml_diff>
--- a/src/game_params.xlsx
+++ b/src/game_params.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Activity_Data\Mancala_github\MancalaGames\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55051D06-49DF-4E44-9F9C-4B4279703F17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22A7A753-6654-47AF-8A3F-4836F3A5B6F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4755" yWindow="435" windowWidth="23415" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="game_params" sheetId="1" r:id="rId1"/>
@@ -711,23 +711,6 @@
     <t xml:space="preserve">Moves maybe made from any hole, independent of the side of the board. Moves need specify side, position and directions.  </t>
   </si>
   <si>
-    <t>NONE: there is no prescribed opening move.
-BASIC_SOWER: the first sow follows general rules of single lap sowing.  Other sow parameters will be enacted  afterward.
-MLAPS_SOWER: the first sow follows general rules of multi-lap sowing. Other sow parameters will be enacted  afterward.
-SOW1OPP: at least one seed must be sown on the opponents side of the board accomplished by sowing as normal until the final seed, then any remaining holes on the player side are skipped and the
-PLUS1MINUS1: proceed from the selected hole by moving one seed from the next hole into the following hole, next skip that hole and repeat moving seed forward. After cycling the board, capture across from the opening hole.
-ARNGE_LIMIT: the first move may be used to rearrange the seeds (opponent is same layout). If the first move is not used for rearrangement, captures and child creation are not allowed from the starter until the second player makes a child or captures.</t>
-  </si>
-  <si>
-    <t>Allows specifing non-all-equal start patterns. Four patterns are supported:
-ALL_EQUAL: all holes start with the same number of seeds.
-GAMACHA: starting from the third hold (from start player's left) place nbr_seeds in every other hole, the first move is prescribed move the center hole's seeds to the other side (this is done automatically).
-ALTERNATES: everyother hole is filled with nbr_seeds, no seeds end up opposite eachother. If a player has fewer seeds than their opponent, then they start.
-ALTS_WITH_1: like Alternates except the starter's 2nd from right hole with nbr_seeds is replaced with one seed.
-CLIPPEDTRIPLES: pattern of 0 S S (where S is nbr_seeds) is used to fill the holes; if a full cycle of 3 cannot be placed, the holes are left empty. The True and False sides are the same from the player's perspective, e.g. they will look reversed when viewed from one side of the game board.
-TWOEMPTY: all but the rightmost two holes for each player are filled with is nbr_seeds.</t>
-  </si>
-  <si>
     <t>An html help file describing the game (mancala_help.html is the main help file).</t>
   </si>
   <si>
@@ -772,9 +755,6 @@
   </si>
   <si>
     <t>Only valid when SOW_START is set. Changes the SOW_START behavior so that if there is only one seed in the hole, it is moved in the sow direction by one hole.</t>
-  </si>
-  <si>
-    <t>Sow is multiplap only if the first sow (seeds from the starting hole) reaches the opponents side of the board.</t>
   </si>
   <si>
     <t>Determines if seeds from more the start hole are picked up and sown:
@@ -923,13 +903,6 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">There are three flavors of capture two out:
-Single Lap: capture if sow ends in occupied hole, then an empty hole, followed by an occupied hole (this is hole captured).
-Multi lap but single capture: capture when last hole sown is followed by an empty hole which is then followed by an occupied hole.
-Multi lap with multiple captures: capture when last hole sown is followed by an empty hole which is then followed by an occupied hole. Continue captures as long as the pattern of empty hole followed by an occupied hole continues.
-</t>
-  </si>
-  <si>
     <t>After the initial capture, continue capturing as long as the capture conditions are met. This multiple capture may happen in the sow direction (unsown holes) or in the opposite direction (sown holes) as determined by CAPSAMEDIR.
 See individual capture mechanism for any special requirements.</t>
   </si>
@@ -985,6 +958,34 @@
 - PICKTWOS: Take seeds from all holes containing two seeds but only after the first move.
 - PICKLASTSEEDS: If there are the number of starts seeds or fewer left,  the current player collects them and the game is over. This rule is applied at the end of each turn, even if there is not a capture because the sow phase may have reduced the seed count.
 - PICK2XLASTSEEDS: If there are 2 times the number of start seeds or fewer, the round starter picks them. This rule is applied at the end of each turn, even if there is not a capture because the sow phase may have reduced the seed count.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Requires MLAPS. If the first 'lap' does not reach the opponent's side of the board, the sowing ends after the first lap. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">There are three flavors of capture two out:
+Single Lap: capture if sow ends in occupied hole, then an empty hole, followed by an occupied hole the contents of this are hole captured.
+Multi lap but single capture: capture when last hole sown is followed by an empty hole which is then followed by an occupied hole.
+Multi lap with multiple captures: capture when last hole sown is followed by an empty hole which is then followed by an occupied hole. Continue captures as long as the pattern of empty hole followed by an occupied hole continues.
+</t>
+  </si>
+  <si>
+    <t>Allows specifing non-all-equal start patterns. The following patterns are supported:
+- ALL_EQUAL: all holes start with the same number of seeds.
+- GAMACHA: starting from the third hold (from start player's left) place nbr_seeds in every other hole, the first move is prescribed move the center hole's seeds to the other side (this is done automatically).
+- ALTERNATES: everyother hole is filled with nbr_seeds, no seeds end up opposite eachother. If a player has fewer seeds than their opponent, then they start.
+- ALTS_WITH_1: like Alternates except the starter's 2nd from right hole with nbr_seeds is replaced with one seed.
+- CLIPPEDTRIPLES: pattern of 0 S S (where S is nbr_seeds) is used to fill the holes; if a full cycle of 3 cannot be placed, the holes are left empty. The True and False sides are the same from the player's perspective, e.g. they will look reversed when viewed from one side of the game board.
+- TWOEMPTY: all but the rightmost two holes for each player are filled with is nbr_seeds.</t>
+  </si>
+  <si>
+    <t>The first sow of the game maybe defined by a specific rule. Prescribed openings are different than start patterns because the player may choose the sow start point. SOW_OWN_STORE and SOW_RULE are ignored during the prescribed openings.
+- NONE: there is no prescribed opening move.
+- BASIC_SOWER: the first sow is a very basic pickup the seeds and drop them one at a time in each hole ignoring any other sow parameters. Other sow parameters will be enacted  afterward. This can be used to force the first sow of an MLAPS game to be a single sow. 
+- MLAPS_SOWER: the first sow follows basic rules of multi-lap sowing (LAPPER). Other sow parameters will be enacted  afterward. 
+- SOW1OPP: at least one seed must be sown on the opponents side of the board which is accomplished by sowing as normal until the final seed, then any remaining holes on the player's side are skipped and the last seed is sown in the oppenents first hole (based on current sow direction).
+- PLUS1MINUS1: proceed from the selected hole by moving one seed from the next hole into the following hole, next skip that hole and repeat moving seed forward. After cycling the board, capture across from the opening hole. 
+- ARNGE_LIMIT: the first move may be used to rearrange the seeds (opponent is same layout). If the first move is not used for rearrangement, captures and child creation are not allowed from the starter until the second player makes a child or captures.</t>
   </si>
 </sst>
 </file>
@@ -1869,8 +1870,8 @@
   <dimension ref="A1:J70"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J22" sqref="J22"/>
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1980,7 +1981,7 @@
         <v>0</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="345" x14ac:dyDescent="0.25">
@@ -2012,7 +2013,7 @@
         <v>0</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -2044,7 +2045,7 @@
         <v>0</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -2108,7 +2109,7 @@
         <v>0</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="150" x14ac:dyDescent="0.25">
@@ -2140,7 +2141,7 @@
         <v>0</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="165" x14ac:dyDescent="0.25">
@@ -2172,7 +2173,7 @@
         <v>0</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="165" x14ac:dyDescent="0.25">
@@ -2204,7 +2205,7 @@
         <v>0</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -2236,10 +2237,10 @@
         <v>0</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="165" x14ac:dyDescent="0.25">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="180" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>96</v>
       </c>
@@ -2268,7 +2269,7 @@
         <v>0</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>262</v>
+        <v>270</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="105" x14ac:dyDescent="0.25">
@@ -2300,7 +2301,7 @@
         <v>2</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -2332,7 +2333,7 @@
         <v>2</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="105" x14ac:dyDescent="0.25">
@@ -2396,7 +2397,7 @@
         <v>2</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -2428,7 +2429,7 @@
         <v>2</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2492,7 +2493,7 @@
         <v>2</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="150" x14ac:dyDescent="0.25">
@@ -2524,7 +2525,7 @@
         <v>2</v>
       </c>
       <c r="J20" s="4" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2556,7 +2557,7 @@
         <v>2</v>
       </c>
       <c r="J21" s="4" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="225" x14ac:dyDescent="0.25">
@@ -2588,7 +2589,7 @@
         <v>2</v>
       </c>
       <c r="J22" s="4" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
@@ -2620,7 +2621,7 @@
         <v>0</v>
       </c>
       <c r="J23" s="4" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -2652,7 +2653,7 @@
         <v>0</v>
       </c>
       <c r="J24" s="4" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -2684,7 +2685,7 @@
         <v>0</v>
       </c>
       <c r="J25" s="4" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="105" x14ac:dyDescent="0.25">
@@ -2748,7 +2749,7 @@
         <v>0</v>
       </c>
       <c r="J27" s="4" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="105" x14ac:dyDescent="0.25">
@@ -2812,7 +2813,7 @@
         <v>2</v>
       </c>
       <c r="J29" s="4" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2876,10 +2877,10 @@
         <v>2</v>
       </c>
       <c r="J31" s="4" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" ht="255" x14ac:dyDescent="0.25">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" ht="390" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>38</v>
       </c>
@@ -2908,7 +2909,7 @@
         <v>2</v>
       </c>
       <c r="J32" s="4" t="s">
-        <v>220</v>
+        <v>272</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -3004,7 +3005,7 @@
         <v>0</v>
       </c>
       <c r="J35" s="4" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="36" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3036,7 +3037,7 @@
         <v>0</v>
       </c>
       <c r="J36" s="4" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="37" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -3068,7 +3069,7 @@
         <v>0</v>
       </c>
       <c r="J37" s="4" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="38" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3100,7 +3101,7 @@
         <v>2</v>
       </c>
       <c r="J38" s="4" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="39" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -3132,7 +3133,7 @@
         <v>2</v>
       </c>
       <c r="J39" s="4" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="40" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -3164,7 +3165,7 @@
         <v>0</v>
       </c>
       <c r="J40" s="4" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="41" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3196,7 +3197,7 @@
         <v>0</v>
       </c>
       <c r="J41" s="4" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
     </row>
     <row r="42" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -3228,7 +3229,7 @@
         <v>0</v>
       </c>
       <c r="J42" s="4" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
     </row>
     <row r="43" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3260,7 +3261,7 @@
         <v>0</v>
       </c>
       <c r="J43" s="4" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -3292,7 +3293,7 @@
         <v>0</v>
       </c>
       <c r="J44" s="4" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
     </row>
     <row r="45" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3324,7 +3325,7 @@
         <v>0</v>
       </c>
       <c r="J45" s="4" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="46" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3356,7 +3357,7 @@
         <v>0</v>
       </c>
       <c r="J46" s="4" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="47" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -3367,7 +3368,7 @@
         <v>130</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="D47" s="3" t="s">
         <v>131</v>
@@ -3388,7 +3389,7 @@
         <v>2</v>
       </c>
       <c r="J47" s="4" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
     </row>
     <row r="48" spans="1:10" ht="135" x14ac:dyDescent="0.25">
@@ -3420,7 +3421,7 @@
         <v>2</v>
       </c>
       <c r="J48" s="4" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="49" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -3452,7 +3453,7 @@
         <v>2</v>
       </c>
       <c r="J49" s="4" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
     </row>
     <row r="50" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -3484,7 +3485,7 @@
         <v>2</v>
       </c>
       <c r="J50" s="4" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
     </row>
     <row r="51" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -3516,7 +3517,7 @@
         <v>2</v>
       </c>
       <c r="J51" s="4" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="52" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -3548,7 +3549,7 @@
         <v>2</v>
       </c>
       <c r="J52" s="4" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
     </row>
     <row r="53" spans="1:10" ht="105" x14ac:dyDescent="0.25">
@@ -3580,7 +3581,7 @@
         <v>2</v>
       </c>
       <c r="J53" s="4" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
     </row>
     <row r="54" spans="1:10" ht="120" x14ac:dyDescent="0.25">
@@ -3612,7 +3613,7 @@
         <v>2</v>
       </c>
       <c r="J54" s="4" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="55" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3743,7 +3744,7 @@
         <v>0</v>
       </c>
       <c r="J59" s="4" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
     </row>
     <row r="60" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3839,7 +3840,7 @@
         <v>0</v>
       </c>
       <c r="J62" s="4" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="63" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -3871,7 +3872,7 @@
         <v>0</v>
       </c>
       <c r="J63" s="4" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="64" spans="1:10" ht="409.5" x14ac:dyDescent="0.25">
@@ -3903,7 +3904,7 @@
         <v>0</v>
       </c>
       <c r="J64" s="4" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
     </row>
     <row r="65" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -3967,7 +3968,7 @@
         <v>2</v>
       </c>
       <c r="J66" s="8" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
     </row>
     <row r="67" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3999,7 +4000,7 @@
         <v>2</v>
       </c>
       <c r="J67" s="4" t="s">
-        <v>234</v>
+        <v>269</v>
       </c>
     </row>
     <row r="68" spans="1:10" ht="409.5" x14ac:dyDescent="0.25">
@@ -4031,7 +4032,7 @@
         <v>2</v>
       </c>
       <c r="J68" s="4" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
     </row>
     <row r="69" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -4095,7 +4096,7 @@
         <v>2</v>
       </c>
       <c r="J70" s="4" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added numbering control for enumerations in help doc. Added numbering for Direct.
</commit_message>
<xml_diff>
--- a/src/game_params.xlsx
+++ b/src/game_params.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Activity_Data\Mancala_github\MancalaGames\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22A7A753-6654-47AF-8A3F-4836F3A5B6F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08CBD0C8-41D4-4BAF-A3D2-309469804B19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4755" yWindow="435" windowWidth="23415" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -891,14 +891,6 @@
     <t>The depth that the minimaxer or negamaxer will search the game tree from the current node. One value for each difficulty.</t>
   </si>
   <si>
-    <t>Direction of sow:
-- CW: clockwise
-- CCW: counter-clockwise
-- SPLIT: left side holes sow counter-clockwise and right side holes sow clockwise, an odd middle hole must be set in UDIR_HOLES.
-Both mouse buttons will start a move no matter the sow direction. If the hole is marked as UDIR_HOLES, the button selects sow direction. On the other hand, if the hole is not marked as UDIR_HOLES, either button will sow in the prescribed direction. This can be useful, mechanism to remind yourself that on SPLIT sow, the left holes go CW by using the left button and the right holes go CCW by using the right button.
-Any hole can be set as UDIR_HOLES to allow the user to override the sow_direct setting.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Capture from the hole after the final seed sown into an empty hole. 
 </t>
   </si>
@@ -986,6 +978,14 @@
 - SOW1OPP: at least one seed must be sown on the opponents side of the board which is accomplished by sowing as normal until the final seed, then any remaining holes on the player's side are skipped and the last seed is sown in the oppenents first hole (based on current sow direction).
 - PLUS1MINUS1: proceed from the selected hole by moving one seed from the next hole into the following hole, next skip that hole and repeat moving seed forward. After cycling the board, capture across from the opening hole. 
 - ARNGE_LIMIT: the first move may be used to rearrange the seeds (opponent is same layout). If the first move is not used for rearrangement, captures and child creation are not allowed from the starter until the second player makes a child or captures.</t>
+  </si>
+  <si>
+    <t>Direction of sow:
+- CW: clockwise
+- SPLIT: left side holes sow counter-clockwise and right side holes sow clockwise, an odd middle hole must be set in UDIR_HOLES.
+- CCW: counter-clockwise
+Both mouse buttons will start a move no matter the sow direction. If the hole is marked as UDIR_HOLES, the button selects sow direction. On the other hand, if the hole is not marked as UDIR_HOLES, either button will sow in the prescribed direction. This can be useful, mechanism to remind yourself that on SPLIT sow, the left holes go CW by using the left button and the right holes go CCW by using the right button.
+Any hole can be set as UDIR_HOLES to allow the user to override the sow_direct setting.</t>
   </si>
 </sst>
 </file>
@@ -1870,8 +1870,8 @@
   <dimension ref="A1:J70"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J32" sqref="J32"/>
+      <pane ySplit="1" topLeftCell="A54" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J59" sqref="J59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2045,7 +2045,7 @@
         <v>0</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -2109,7 +2109,7 @@
         <v>0</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="150" x14ac:dyDescent="0.25">
@@ -2141,7 +2141,7 @@
         <v>0</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="165" x14ac:dyDescent="0.25">
@@ -2173,7 +2173,7 @@
         <v>0</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="165" x14ac:dyDescent="0.25">
@@ -2205,7 +2205,7 @@
         <v>0</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -2237,7 +2237,7 @@
         <v>0</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="180" x14ac:dyDescent="0.25">
@@ -2269,7 +2269,7 @@
         <v>0</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="105" x14ac:dyDescent="0.25">
@@ -2301,7 +2301,7 @@
         <v>2</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -2429,7 +2429,7 @@
         <v>2</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2525,7 +2525,7 @@
         <v>2</v>
       </c>
       <c r="J20" s="4" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2589,7 +2589,7 @@
         <v>2</v>
       </c>
       <c r="J22" s="4" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
@@ -2877,7 +2877,7 @@
         <v>2</v>
       </c>
       <c r="J31" s="4" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="390" x14ac:dyDescent="0.25">
@@ -2909,7 +2909,7 @@
         <v>2</v>
       </c>
       <c r="J32" s="4" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -3744,7 +3744,7 @@
         <v>0</v>
       </c>
       <c r="J59" s="4" t="s">
-        <v>257</v>
+        <v>272</v>
       </c>
     </row>
     <row r="60" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -4000,7 +4000,7 @@
         <v>2</v>
       </c>
       <c r="J67" s="4" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="68" spans="1:10" ht="409.5" x14ac:dyDescent="0.25">
@@ -4032,7 +4032,7 @@
         <v>2</v>
       </c>
       <c r="J68" s="4" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="69" spans="1:10" ht="30" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Cleaned up the deprive versus sow_blkd_div options and rules, more consistent and allow more options for deprive games that are not sow_blkd_div. Fixed problems with deprive end move. Added game outcome logic to the parameter help file.
</commit_message>
<xml_diff>
--- a/src/game_params.xlsx
+++ b/src/game_params.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Activity_Data\Mancala_github\MancalaGames\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08CBD0C8-41D4-4BAF-A3D2-309469804B19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEA70319-37B5-4C59-8635-FB0D8818DE2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4755" yWindow="435" windowWidth="23415" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="game_params" sheetId="1" r:id="rId1"/>
@@ -281,9 +281,6 @@
     <t>Skip Start on Lap</t>
   </si>
   <si>
-    <t>When sowing a second or subsequent circuit of the board, skip the start hole. This will leave the start hole empty for single lap games.</t>
-  </si>
-  <si>
     <t>sow_own_store</t>
   </si>
   <si>
@@ -796,16 +793,6 @@
 If a player ends on their own side of the board in an empty hole, but did not sow any opposite hole, they get a repeat turn.</t>
   </si>
   <si>
-    <t xml:space="preserve">The overall goal of the game. Defines how a player wins.
-- MAX_SEEDS: player with the maximum number of seeds at the end of the game wins or they collect more than half of the total seeds
-- DEPRIVE: eliminate all of your opponents seeds. 
-  + GRAND_SLAM must be legal for DEPRIVE games.
-  + The following options are incompatible with DEPRIVE games: MOVEUNLOCK, MUSTPASS, MUSTSHARE, ROUNDS, ROUND_STARTER, ROUND_FILL, NO_SIDES, SKIP_START, SOW_OWN_STORE, STORES, SOW_START, VISIT_OPP. 
-- TERRITORY: claim ownership of holes. Each round the ownership of holes is determined by the number of seeds captured in the previous round. In a TERRITORY game without rounds, the winner is the player that gained the most territory during play. 
-  + TERRITORY games require STORES and that GPARAM_ONE be set to a value between the number of holes and two times the number of holes.
-  + TERRITORY games are incompatible with NO_SIDES, START_PATTERN, GRANDSLAM of NOT_LEGAL, ALLOW_RULE of OPP_OR_EMPTY, </t>
-  </si>
-  <si>
     <t>Don't allow captures or closing of holes (SOW_RULE of SOW_BLKD_DIV) on the first move of the game or round.</t>
   </si>
   <si>
@@ -861,23 +848,6 @@
     <t>A value used to encourage or discourage repeat turns. The value is added in for the current player and subtracted off the score for the opposing playing. Use a positive value to encourage the AI player to repeat turns.
 This parameter may only be used for games in which repeated turns are possible (SOW_OWN_STORE, CAPT_RTURN or XC_SOWN).
 Used only for minimax &amp; negamax players.</t>
-  </si>
-  <si>
-    <t>Special sow rules add additional behavior or restrictions to the sowing phase:
-- NONE: there is no special sowing rule.
-- SOW_BLKD_DIV: If the final seed of an individual sow bring the contents of a hole to GPARAM_ONE seeds, the hole is closed closed (blocked). In single lap games, the hole's seeds are removed from play. In multilap games, the seeds are used to continue sowing.
-  + When sowing, blocked holes on your own side of the board are skipped  and blocked holes on opponent's side are diverted out of play or captured.
-  +NOCAPTFIRST prevents closing holes on the first move. Game GOAL must be DEPRIVE. 
-- SOW_BLKD_DIV_NR: Behaves the same as SOW_BLKD_DIV except that each player's rightmost hole cannot be closed. 
-- OWN_SOW_CAPT_ALL: The hole OWNer captures all holes that are sown to meet the simple capture criteria: evens, min, max and capture on. Other criteria are enforced: side of the board, unlocked, and not child.
-  + The capture is done by the hole owner, so the non-sower may capture seeds during their opponents sowing. If the game GOAL is TERRITORY the capturer is the hole owner; otherwise each player captures from their own side of the board no matter who is sowing. 
-  + If mlaps is LAPPER and the final seed sown for any lap meets the capture criteria, the contents of the hole are captured by the sower and not the hole owner and the turn is over.
-  + GRANDSLAM rules are not applied. NOCAPTFIRST prevents this capture for the first move.
-- SOW_SOW_CAPT_ALL: Similar to OWN_SOW_CAPT_ALL but only the SOWer captures seeds from their opponent's holes. 
-  + If mlaps is LAPPER and the final seed sown for any lap meets the capture criteria, the contents of the hole are captured by the sower and not the hole owner and the turn is over.
-  + GRANDSLAM rules are not applied. NOCAPTFIRST prevents this capture for the first move.
-- NO_SOW_OPP_2S: Don't sow into opponents holes with 2 seeds.
-- CHANGE_DIR_LAP: Change the direction for each lap sown. Generally used with UDIR_HOLES so the player may choose the first direction.</t>
   </si>
   <si>
     <t>The multiplier for the stores scorer. Seeds in stores and children are included.
@@ -986,6 +956,38 @@
 - CCW: counter-clockwise
 Both mouse buttons will start a move no matter the sow direction. If the hole is marked as UDIR_HOLES, the button selects sow direction. On the other hand, if the hole is not marked as UDIR_HOLES, either button will sow in the prescribed direction. This can be useful, mechanism to remind yourself that on SPLIT sow, the left holes go CW by using the left button and the right holes go CCW by using the right button.
 Any hole can be set as UDIR_HOLES to allow the user to override the sow_direct setting.</t>
+  </si>
+  <si>
+    <t>When sowing a second or subsequent circuit of the board, skip the start hole. This will leave the start hole empty for single lap games.
+In multilap games, the start hole for the current lap is skipped. Second or subsequent laps may sow into the original start hole.</t>
+  </si>
+  <si>
+    <t>Special sow rules add additional behavior or restrictions to the sowing phase:
+- NONE: there is no special sowing rule.
+- SOW_BLKD_DIV: If the final seed of an individual sow lands on the opposite side of the board and brings the contents of that hole to GPARAM_ONE seeds, the hole is closed closed (blocked). In single lap games, the hole's seeds are removed from play. In multilap games, the seeds are used to continue sowing. MLAPS of LAPPER_NEXT is not supported with SOW_BLKD_DIV(_NR).
+  + When sowing, blocked holes on your own side of the board are skipped  and blocked holes on opponent's side are diverted out of play or captured.
+  +  Game GOAL must be DEPRIVE and all of the associated restrictions apply. NOCAPTFIRST maybe used to prevent closing holes on the first move. Capture mechanisms other than closing holes are not supported. The minimum move must be 1 and thus SOW_START is incompatible.  ALLOW_RULE may not be used to limit allowable moves.  SKIP_START and VISIT_OPP are not supported with SOW_BLKD_DIV. 
+- SOW_BLKD_DIV_NR: Behaves the same as SOW_BLKD_DIV except that each player's rightmost hole cannot be closed. 
+- OWN_SOW_CAPT_ALL: The hole OWNer captures all holes that are sown to meet the simple capture criteria: evens, min, max and capture on. Other criteria are enforced: side of the board, unlocked, and not child.
+  + The capture is done by the hole owner, so the non-sower may capture seeds during their opponents sowing. If the game GOAL is TERRITORY the capturer is the hole owner; otherwise each player captures from their own side of the board no matter who is sowing. 
+  + If MLAPS is LAPPER and the final seed sown for any lap meets the capture criteria, the contents of the hole are captured by the sower and not the hole owner and the turn is over.
+  + GRANDSLAM rules are not applied. NOCAPTFIRST prevents this capture for the first move.
+- SOW_SOW_CAPT_ALL: Similar to OWN_SOW_CAPT_ALL but only the SOWer captures seeds from their opponent's holes. 
+  + If mlaps is LAPPER and the final seed sown for any lap meets the capture criteria, the contents of the hole are captured by the sower and not the hole owner and the turn is over.
+  + GRANDSLAM rules are not applied. NOCAPTFIRST prevents this capture for the first move.
+- NO_SOW_OPP_2S: Don't sow into opponents holes with 2 seeds.
+- CHANGE_DIR_LAP: Change the direction for each lap sown. Generally used with UDIR_HOLES so the player may choose the first direction.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The overall goal of the game. Defines how a player wins.
+- MAX_SEEDS: player with the maximum number of seeds at the end of the game wins or they collect more than half of the total seeds
+- DEPRIVE: eliminate all of your opponents seeds.
+  + If a player has no seeds at the start of their turn, they loose. If a player has no moves at the start of their turn, then the game outcome is determined by who has seeds: If both players have seeds, the game ends in a tie. If the current player has seeds, but the previous player does not, then the current player wins because they forced the previous player to give away all their seeds.
+  + GRAND_SLAM must be legal for DEPRIVE games.
+  + Deprive games cannot be played in ROUNDS, use STORES, or use children. Additionally, the following options are incompatible with DEPRIVE games: MOVEUNLOCK, MUSTPASS, MUSTSHARE and NO_SIDES.
+- TERRITORY: claim ownership of holes. Each round the ownership of holes is determined by the number of seeds captured in the previous round. In a TERRITORY game without rounds, the winner is the player that gained the most territory during play. 
+  + TERRITORY games require STORES and that GPARAM_ONE be set to a value between the number of holes and two times the number of holes.
+  + TERRITORY games are incompatible with NO_SIDES, START_PATTERN, GRANDSLAM of NOT_LEGAL, ALLOW_RULE of OPP_OR_EMPTY, </t>
   </si>
 </sst>
 </file>
@@ -1870,8 +1872,8 @@
   <dimension ref="A1:J70"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A54" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J59" sqref="J59"/>
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1884,7 +1886,7 @@
     <col min="6" max="6" width="14.7109375" style="3" customWidth="1"/>
     <col min="7" max="7" width="21.140625" style="3" customWidth="1"/>
     <col min="8" max="9" width="9.140625" style="3" customWidth="1"/>
-    <col min="10" max="10" width="60.28515625" style="4" customWidth="1"/>
+    <col min="10" max="10" width="114.85546875" style="4" customWidth="1"/>
     <col min="11" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
@@ -1902,7 +1904,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>4</v>
@@ -1981,7 +1983,7 @@
         <v>0</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="345" x14ac:dyDescent="0.25">
@@ -1989,10 +1991,10 @@
         <v>62</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>178</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>179</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>24</v>
@@ -2001,10 +2003,10 @@
         <v>14</v>
       </c>
       <c r="F4" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="G4" s="5" t="s">
         <v>180</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>181</v>
       </c>
       <c r="H4" s="3">
         <v>3</v>
@@ -2013,18 +2015,18 @@
         <v>0</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="C5" s="3" t="s">
         <v>97</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>98</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>24</v>
@@ -2045,18 +2047,18 @@
         <v>0</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>99</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>100</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>24</v>
@@ -2077,18 +2079,18 @@
         <v>0</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>119</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>120</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>24</v>
@@ -2109,18 +2111,18 @@
         <v>0</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="150" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B8" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>104</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>105</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>24</v>
@@ -2141,18 +2143,18 @@
         <v>0</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="165" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B9" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>106</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>107</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>24</v>
@@ -2164,7 +2166,7 @@
         <v>11</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H9" s="3">
         <v>4</v>
@@ -2173,18 +2175,18 @@
         <v>0</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="165" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B10" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>108</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>109</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>24</v>
@@ -2196,7 +2198,7 @@
         <v>11</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H10" s="3">
         <v>5</v>
@@ -2205,18 +2207,18 @@
         <v>0</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B11" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>192</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>193</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>24</v>
@@ -2237,18 +2239,18 @@
         <v>0</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="180" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B12" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>127</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>128</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>24</v>
@@ -2269,18 +2271,18 @@
         <v>0</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B13" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>113</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>114</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>24</v>
@@ -2301,18 +2303,18 @@
         <v>2</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B14" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>204</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>205</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>24</v>
@@ -2333,18 +2335,18 @@
         <v>2</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B15" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="C15" s="3" t="s">
         <v>115</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>116</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>24</v>
@@ -2353,10 +2355,10 @@
         <v>79</v>
       </c>
       <c r="F15" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="G15" s="5" t="s">
         <v>117</v>
-      </c>
-      <c r="G15" s="5" t="s">
-        <v>118</v>
       </c>
       <c r="H15" s="3">
         <v>2</v>
@@ -2365,18 +2367,18 @@
         <v>2</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="240" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B16" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>121</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>122</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>24</v>
@@ -2385,10 +2387,10 @@
         <v>37</v>
       </c>
       <c r="F16" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="G16" s="5" t="s">
         <v>123</v>
-      </c>
-      <c r="G16" s="5" t="s">
-        <v>124</v>
       </c>
       <c r="H16" s="3">
         <v>3</v>
@@ -2397,18 +2399,18 @@
         <v>2</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B17" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="C17" s="3" t="s">
         <v>102</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>103</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>24</v>
@@ -2429,18 +2431,18 @@
         <v>2</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B18" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="C18" s="3" t="s">
         <v>110</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>111</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>24</v>
@@ -2461,18 +2463,18 @@
         <v>2</v>
       </c>
       <c r="J18" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B19" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="C19" s="3" t="s">
         <v>215</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>216</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>24</v>
@@ -2493,18 +2495,18 @@
         <v>2</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="150" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B20" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="C20" s="3" t="s">
         <v>125</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>126</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>24</v>
@@ -2513,10 +2515,10 @@
         <v>20</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H20" s="3">
         <v>8</v>
@@ -2525,18 +2527,18 @@
         <v>2</v>
       </c>
       <c r="J20" s="4" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B21" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="C21" s="3" t="s">
         <v>190</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>191</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>24</v>
@@ -2557,18 +2559,18 @@
         <v>2</v>
       </c>
       <c r="J21" s="4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="225" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>24</v>
@@ -2577,10 +2579,10 @@
         <v>59</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H22" s="3">
         <v>10</v>
@@ -2589,7 +2591,7 @@
         <v>2</v>
       </c>
       <c r="J22" s="4" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
@@ -2621,7 +2623,7 @@
         <v>0</v>
       </c>
       <c r="J23" s="4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -2653,7 +2655,7 @@
         <v>0</v>
       </c>
       <c r="J24" s="4" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -2685,7 +2687,7 @@
         <v>0</v>
       </c>
       <c r="J25" s="4" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="105" x14ac:dyDescent="0.25">
@@ -2717,7 +2719,7 @@
         <v>0</v>
       </c>
       <c r="J26" s="4" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="409.5" x14ac:dyDescent="0.25">
@@ -2725,10 +2727,10 @@
         <v>38</v>
       </c>
       <c r="B27" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="C27" s="3" t="s">
         <v>206</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>207</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>24</v>
@@ -2737,10 +2739,10 @@
         <v>62</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="H27" s="3">
         <v>6</v>
@@ -2749,7 +2751,7 @@
         <v>0</v>
       </c>
       <c r="J27" s="4" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="105" x14ac:dyDescent="0.25">
@@ -2757,10 +2759,10 @@
         <v>38</v>
       </c>
       <c r="B28" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C28" s="3" t="s">
         <v>84</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>85</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>24</v>
@@ -2781,10 +2783,10 @@
         <v>0</v>
       </c>
       <c r="J28" s="4" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" ht="315" x14ac:dyDescent="0.25">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="255" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>38</v>
       </c>
@@ -2813,7 +2815,7 @@
         <v>2</v>
       </c>
       <c r="J29" s="4" t="s">
-        <v>238</v>
+        <v>272</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2845,10 +2847,10 @@
         <v>2</v>
       </c>
       <c r="J30" s="4" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" ht="285" x14ac:dyDescent="0.25">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" ht="210" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>38</v>
       </c>
@@ -2877,18 +2879,18 @@
         <v>2</v>
       </c>
       <c r="J31" s="4" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" ht="390" x14ac:dyDescent="0.25">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" ht="285" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>38</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D32" s="3" t="s">
         <v>24</v>
@@ -2897,10 +2899,10 @@
         <v>60</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="G32" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H32" s="3">
         <v>3</v>
@@ -2909,7 +2911,7 @@
         <v>2</v>
       </c>
       <c r="J32" s="4" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -2917,10 +2919,10 @@
         <v>38</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D33" s="3" t="s">
         <v>24</v>
@@ -2932,7 +2934,7 @@
         <v>11</v>
       </c>
       <c r="G33" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H33" s="3">
         <v>5</v>
@@ -2941,7 +2943,7 @@
         <v>2</v>
       </c>
       <c r="J33" s="4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
@@ -2961,7 +2963,7 @@
         <v>28</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G34" s="5" t="s">
         <v>20</v>
@@ -3005,7 +3007,7 @@
         <v>0</v>
       </c>
       <c r="J35" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="36" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3037,7 +3039,7 @@
         <v>0</v>
       </c>
       <c r="J36" s="4" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="37" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -3060,7 +3062,7 @@
         <v>30</v>
       </c>
       <c r="G37" s="6" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="H37" s="3">
         <v>4</v>
@@ -3069,7 +3071,7 @@
         <v>0</v>
       </c>
       <c r="J37" s="4" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="38" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3101,7 +3103,7 @@
         <v>2</v>
       </c>
       <c r="J38" s="4" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="39" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -3133,31 +3135,31 @@
         <v>2</v>
       </c>
       <c r="J39" s="4" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="40" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B40" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="C40" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="C40" s="3" t="s">
-        <v>155</v>
-      </c>
       <c r="D40" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E40" s="3">
         <v>13</v>
       </c>
       <c r="F40" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="G40" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="G40" s="3" t="s">
-        <v>156</v>
-      </c>
       <c r="H40" s="3">
         <v>0</v>
       </c>
@@ -3165,21 +3167,21 @@
         <v>0</v>
       </c>
       <c r="J40" s="4" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="41" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B41" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="C41" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="C41" s="3" t="s">
+      <c r="D41" s="3" t="s">
         <v>147</v>
-      </c>
-      <c r="D41" s="3" t="s">
-        <v>148</v>
       </c>
       <c r="E41" s="3">
         <v>30</v>
@@ -3197,21 +3199,21 @@
         <v>0</v>
       </c>
       <c r="J41" s="4" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="42" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E42" s="3">
         <v>12</v>
@@ -3229,30 +3231,30 @@
         <v>0</v>
       </c>
       <c r="J42" s="4" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="43" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B43" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="C43" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="C43" s="3" t="s">
+      <c r="D43" s="3" t="s">
         <v>159</v>
-      </c>
-      <c r="D43" s="3" t="s">
-        <v>160</v>
       </c>
       <c r="E43" s="3">
         <v>46</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="H43" s="3">
         <v>4</v>
@@ -3261,30 +3263,30 @@
         <v>0</v>
       </c>
       <c r="J43" s="4" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E44" s="3">
         <v>40</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H44" s="3">
         <v>6</v>
@@ -3293,30 +3295,30 @@
         <v>0</v>
       </c>
       <c r="J44" s="4" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="45" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E45" s="3">
         <v>41</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H45" s="3">
         <v>7</v>
@@ -3325,30 +3327,30 @@
         <v>0</v>
       </c>
       <c r="J45" s="4" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="46" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E46" s="3">
         <v>42</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H46" s="3">
         <v>8</v>
@@ -3357,21 +3359,21 @@
         <v>0</v>
       </c>
       <c r="J46" s="4" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="47" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="B47" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="B47" s="3" t="s">
+      <c r="C47" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="D47" s="3" t="s">
         <v>130</v>
-      </c>
-      <c r="C47" s="3" t="s">
-        <v>255</v>
-      </c>
-      <c r="D47" s="3" t="s">
-        <v>131</v>
       </c>
       <c r="E47" s="3">
         <v>74</v>
@@ -3389,21 +3391,21 @@
         <v>2</v>
       </c>
       <c r="J47" s="4" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="48" spans="1:10" ht="135" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B48" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="C48" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="C48" s="3" t="s">
-        <v>133</v>
-      </c>
       <c r="D48" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E48" s="3">
         <v>11</v>
@@ -3412,7 +3414,7 @@
         <v>11</v>
       </c>
       <c r="G48" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H48" s="3">
         <v>1</v>
@@ -3421,21 +3423,21 @@
         <v>2</v>
       </c>
       <c r="J48" s="4" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="49" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B49" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="C49" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="C49" s="3" t="s">
-        <v>135</v>
-      </c>
       <c r="D49" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E49" s="3">
         <v>66</v>
@@ -3444,7 +3446,7 @@
         <v>11</v>
       </c>
       <c r="G49" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H49" s="3">
         <v>2</v>
@@ -3453,21 +3455,21 @@
         <v>2</v>
       </c>
       <c r="J49" s="4" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="50" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B50" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="C50" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="C50" s="3" t="s">
-        <v>137</v>
-      </c>
       <c r="D50" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E50" s="3">
         <v>32</v>
@@ -3476,7 +3478,7 @@
         <v>11</v>
       </c>
       <c r="G50" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H50" s="3">
         <v>3</v>
@@ -3485,21 +3487,21 @@
         <v>2</v>
       </c>
       <c r="J50" s="4" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="51" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B51" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="C51" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="C51" s="3" t="s">
-        <v>139</v>
-      </c>
       <c r="D51" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E51" s="3">
         <v>25</v>
@@ -3508,7 +3510,7 @@
         <v>11</v>
       </c>
       <c r="G51" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H51" s="3">
         <v>4</v>
@@ -3517,21 +3519,21 @@
         <v>2</v>
       </c>
       <c r="J51" s="4" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="52" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B52" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="C52" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="C52" s="3" t="s">
-        <v>141</v>
-      </c>
       <c r="D52" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E52" s="3">
         <v>34</v>
@@ -3540,7 +3542,7 @@
         <v>11</v>
       </c>
       <c r="G52" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H52" s="3">
         <v>5</v>
@@ -3549,21 +3551,21 @@
         <v>2</v>
       </c>
       <c r="J52" s="4" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="53" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B53" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="C53" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="C53" s="3" t="s">
-        <v>143</v>
-      </c>
       <c r="D53" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E53" s="3">
         <v>31</v>
@@ -3572,7 +3574,7 @@
         <v>11</v>
       </c>
       <c r="G53" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H53" s="3">
         <v>6</v>
@@ -3581,21 +3583,21 @@
         <v>2</v>
       </c>
       <c r="J53" s="4" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="54" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B54" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="C54" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="C54" s="3" t="s">
-        <v>145</v>
-      </c>
       <c r="D54" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E54" s="3">
         <v>61</v>
@@ -3604,7 +3606,7 @@
         <v>11</v>
       </c>
       <c r="G54" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H54" s="3">
         <v>7</v>
@@ -3613,7 +3615,7 @@
         <v>2</v>
       </c>
       <c r="J54" s="4" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="55" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3621,7 +3623,7 @@
         <v>9</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D55" s="3" t="s">
         <v>24</v>
@@ -3639,7 +3641,7 @@
         <v>0</v>
       </c>
       <c r="J55" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="56" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3685,7 +3687,7 @@
         <v>0</v>
       </c>
       <c r="J57" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="58" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3693,7 +3695,7 @@
         <v>9</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D58" s="3" t="s">
         <v>24</v>
@@ -3712,7 +3714,7 @@
         <v>0</v>
       </c>
       <c r="J58" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="59" spans="1:10" ht="210" x14ac:dyDescent="0.25">
@@ -3744,7 +3746,7 @@
         <v>0</v>
       </c>
       <c r="J59" s="4" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
     </row>
     <row r="60" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3779,7 +3781,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="61" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
         <v>69</v>
       </c>
@@ -3808,7 +3810,7 @@
         <v>0</v>
       </c>
       <c r="J61" s="4" t="s">
-        <v>81</v>
+        <v>270</v>
       </c>
     </row>
     <row r="62" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -3816,10 +3818,10 @@
         <v>69</v>
       </c>
       <c r="B62" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C62" s="3" t="s">
         <v>82</v>
-      </c>
-      <c r="C62" s="3" t="s">
-        <v>83</v>
       </c>
       <c r="D62" s="3" t="s">
         <v>24</v>
@@ -3840,7 +3842,7 @@
         <v>0</v>
       </c>
       <c r="J62" s="4" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="63" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -3872,7 +3874,7 @@
         <v>0</v>
       </c>
       <c r="J63" s="4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="64" spans="1:10" ht="409.5" x14ac:dyDescent="0.25">
@@ -3880,10 +3882,10 @@
         <v>69</v>
       </c>
       <c r="B64" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="C64" s="3" t="s">
         <v>198</v>
-      </c>
-      <c r="C64" s="3" t="s">
-        <v>199</v>
       </c>
       <c r="D64" s="3" t="s">
         <v>24</v>
@@ -3892,10 +3894,10 @@
         <v>70</v>
       </c>
       <c r="F64" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="G64" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H64" s="3">
         <v>6</v>
@@ -3904,7 +3906,7 @@
         <v>0</v>
       </c>
       <c r="J64" s="4" t="s">
-        <v>253</v>
+        <v>271</v>
       </c>
     </row>
     <row r="65" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -3912,10 +3914,10 @@
         <v>69</v>
       </c>
       <c r="B65" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C65" s="3" t="s">
         <v>91</v>
-      </c>
-      <c r="C65" s="3" t="s">
-        <v>92</v>
       </c>
       <c r="D65" s="3" t="s">
         <v>24</v>
@@ -3924,10 +3926,10 @@
         <v>75</v>
       </c>
       <c r="F65" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G65" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H65" s="3">
         <v>8</v>
@@ -3936,7 +3938,7 @@
         <v>0</v>
       </c>
       <c r="J65" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="66" spans="1:10" ht="195" x14ac:dyDescent="0.25">
@@ -3944,10 +3946,10 @@
         <v>69</v>
       </c>
       <c r="B66" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C66" s="3" t="s">
         <v>86</v>
-      </c>
-      <c r="C66" s="3" t="s">
-        <v>87</v>
       </c>
       <c r="D66" s="3" t="s">
         <v>24</v>
@@ -3956,10 +3958,10 @@
         <v>44</v>
       </c>
       <c r="F66" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="G66" s="5" t="s">
         <v>184</v>
-      </c>
-      <c r="G66" s="5" t="s">
-        <v>185</v>
       </c>
       <c r="H66" s="3">
         <v>0</v>
@@ -3968,7 +3970,7 @@
         <v>2</v>
       </c>
       <c r="J66" s="8" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="67" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3976,10 +3978,10 @@
         <v>69</v>
       </c>
       <c r="B67" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C67" s="3" t="s">
         <v>88</v>
-      </c>
-      <c r="C67" s="3" t="s">
-        <v>89</v>
       </c>
       <c r="D67" s="3" t="s">
         <v>24</v>
@@ -4000,7 +4002,7 @@
         <v>2</v>
       </c>
       <c r="J67" s="4" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
     </row>
     <row r="68" spans="1:10" ht="409.5" x14ac:dyDescent="0.25">
@@ -4008,10 +4010,10 @@
         <v>69</v>
       </c>
       <c r="B68" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="C68" s="3" t="s">
         <v>173</v>
-      </c>
-      <c r="C68" s="3" t="s">
-        <v>174</v>
       </c>
       <c r="D68" s="3" t="s">
         <v>24</v>
@@ -4020,10 +4022,10 @@
         <v>27</v>
       </c>
       <c r="F68" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G68" s="5" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="H68" s="3">
         <v>3</v>
@@ -4032,7 +4034,7 @@
         <v>2</v>
       </c>
       <c r="J68" s="4" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
     </row>
     <row r="69" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -4040,10 +4042,10 @@
         <v>69</v>
       </c>
       <c r="B69" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="C69" s="3" t="s">
         <v>171</v>
-      </c>
-      <c r="C69" s="3" t="s">
-        <v>172</v>
       </c>
       <c r="D69" s="3" t="s">
         <v>24</v>
@@ -4055,7 +4057,7 @@
         <v>11</v>
       </c>
       <c r="G69" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H69" s="3">
         <v>4</v>
@@ -4064,30 +4066,30 @@
         <v>2</v>
       </c>
       <c r="J69" s="4" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="70" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
         <v>69</v>
       </c>
       <c r="B70" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="C70" s="3" t="s">
         <v>212</v>
       </c>
-      <c r="C70" s="3" t="s">
+      <c r="D70" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E70" s="3">
+        <v>24</v>
+      </c>
+      <c r="F70" s="3" t="s">
         <v>213</v>
       </c>
-      <c r="D70" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E70" s="3">
-        <v>24</v>
-      </c>
-      <c r="F70" s="3" t="s">
-        <v>214</v>
-      </c>
       <c r="G70" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H70" s="3">
         <v>5</v>
@@ -4096,7 +4098,7 @@
         <v>2</v>
       </c>
       <c r="J70" s="4" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Minor changes. doc updates
</commit_message>
<xml_diff>
--- a/src/game_params.xlsx
+++ b/src/game_params.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Activity_Data\Mancala_github\MancalaGames\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEA70319-37B5-4C59-8635-FB0D8818DE2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA821CA0-B836-4C90-A22D-5E1E24E385C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -831,11 +831,6 @@
 Used only for the minimax &amp; negamax players.</t>
   </si>
   <si>
-    <t>The multiplier for the seeds scorer. The seeds scorer computes how many seeds each player has on the game board.
-TODO does this properly deal with children or hole owners?
-Used only for minimax &amp; negamax players.</t>
-  </si>
-  <si>
     <t>The multiplier for the empties scorer. The empties scorer counts the number empty holes each player has on the board.
 Used only for minimax &amp; negamax players.</t>
   </si>
@@ -988,6 +983,10 @@
 - TERRITORY: claim ownership of holes. Each round the ownership of holes is determined by the number of seeds captured in the previous round. In a TERRITORY game without rounds, the winner is the player that gained the most territory during play. 
   + TERRITORY games require STORES and that GPARAM_ONE be set to a value between the number of holes and two times the number of holes.
   + TERRITORY games are incompatible with NO_SIDES, START_PATTERN, GRANDSLAM of NOT_LEGAL, ALLOW_RULE of OPP_OR_EMPTY, </t>
+  </si>
+  <si>
+    <t>The multiplier for the seeds scorer. The seeds scorer computes how many seeds each player has on the game board that are not in children.
+Used only for minimax &amp; negamax players.</t>
   </si>
 </sst>
 </file>
@@ -1872,8 +1871,8 @@
   <dimension ref="A1:J70"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G29" sqref="G29"/>
+      <pane ySplit="1" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J49" sqref="J49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2047,7 +2046,7 @@
         <v>0</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -2111,7 +2110,7 @@
         <v>0</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="150" x14ac:dyDescent="0.25">
@@ -2143,7 +2142,7 @@
         <v>0</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="165" x14ac:dyDescent="0.25">
@@ -2175,7 +2174,7 @@
         <v>0</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="165" x14ac:dyDescent="0.25">
@@ -2207,7 +2206,7 @@
         <v>0</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -2239,7 +2238,7 @@
         <v>0</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="180" x14ac:dyDescent="0.25">
@@ -2271,7 +2270,7 @@
         <v>0</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="105" x14ac:dyDescent="0.25">
@@ -2303,7 +2302,7 @@
         <v>2</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -2431,7 +2430,7 @@
         <v>2</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2527,7 +2526,7 @@
         <v>2</v>
       </c>
       <c r="J20" s="4" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2591,7 +2590,7 @@
         <v>2</v>
       </c>
       <c r="J22" s="4" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
@@ -2815,7 +2814,7 @@
         <v>2</v>
       </c>
       <c r="J29" s="4" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2879,7 +2878,7 @@
         <v>2</v>
       </c>
       <c r="J31" s="4" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="285" x14ac:dyDescent="0.25">
@@ -2911,7 +2910,7 @@
         <v>2</v>
       </c>
       <c r="J32" s="4" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -3263,7 +3262,7 @@
         <v>0</v>
       </c>
       <c r="J43" s="4" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -3370,7 +3369,7 @@
         <v>129</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D47" s="3" t="s">
         <v>130</v>
@@ -3391,7 +3390,7 @@
         <v>2</v>
       </c>
       <c r="J47" s="4" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="48" spans="1:10" ht="135" x14ac:dyDescent="0.25">
@@ -3423,10 +3422,10 @@
         <v>2</v>
       </c>
       <c r="J48" s="4" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
         <v>128</v>
       </c>
@@ -3455,7 +3454,7 @@
         <v>2</v>
       </c>
       <c r="J49" s="4" t="s">
-        <v>247</v>
+        <v>272</v>
       </c>
     </row>
     <row r="50" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -3487,7 +3486,7 @@
         <v>2</v>
       </c>
       <c r="J50" s="4" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="51" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -3615,7 +3614,7 @@
         <v>2</v>
       </c>
       <c r="J54" s="4" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="55" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3746,7 +3745,7 @@
         <v>0</v>
       </c>
       <c r="J59" s="4" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="60" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3810,7 +3809,7 @@
         <v>0</v>
       </c>
       <c r="J61" s="4" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="62" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -3906,7 +3905,7 @@
         <v>0</v>
       </c>
       <c r="J64" s="4" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="65" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -4002,7 +4001,7 @@
         <v>2</v>
       </c>
       <c r="J67" s="4" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="68" spans="1:10" ht="409.5" x14ac:dyDescent="0.25">
@@ -4034,7 +4033,7 @@
         <v>2</v>
       </c>
       <c r="J68" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="69" spans="1:10" ht="30" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added an option for players sowing in opposite directions. Added rules for Olinda and a demonstration game SowOpDirs.
</commit_message>
<xml_diff>
--- a/src/game_params.xlsx
+++ b/src/game_params.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Activity_Data\Mancala_github\MancalaGames\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA821CA0-B836-4C90-A22D-5E1E24E385C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23A569A8-6357-4E48-A530-F898EA87D43A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -486,10 +486,6 @@
 Capture on evens. </t>
   </si>
   <si>
-    <t>A list of holes that the user can control the sow direction from. Control is via the mouse button: left is clockwise and right is counter-clockwise.
-Note: all holes respond to both mouse buttons, but if the hole is not in udir_holes, the sow direction will be that prescribed by sow_direct with either button.</t>
-  </si>
-  <si>
     <t>When crosscapt is set, defines what to do with the single seed initiating the cross capture.
 - LEAVE: always leave the signle seed
 - PICK_ON_CAPTURE: only pick (capture) the seed if there was a capture.
@@ -943,14 +939,6 @@
 - SOW1OPP: at least one seed must be sown on the opponents side of the board which is accomplished by sowing as normal until the final seed, then any remaining holes on the player's side are skipped and the last seed is sown in the oppenents first hole (based on current sow direction).
 - PLUS1MINUS1: proceed from the selected hole by moving one seed from the next hole into the following hole, next skip that hole and repeat moving seed forward. After cycling the board, capture across from the opening hole. 
 - ARNGE_LIMIT: the first move may be used to rearrange the seeds (opponent is same layout). If the first move is not used for rearrangement, captures and child creation are not allowed from the starter until the second player makes a child or captures.</t>
-  </si>
-  <si>
-    <t>Direction of sow:
-- CW: clockwise
-- SPLIT: left side holes sow counter-clockwise and right side holes sow clockwise, an odd middle hole must be set in UDIR_HOLES.
-- CCW: counter-clockwise
-Both mouse buttons will start a move no matter the sow direction. If the hole is marked as UDIR_HOLES, the button selects sow direction. On the other hand, if the hole is not marked as UDIR_HOLES, either button will sow in the prescribed direction. This can be useful, mechanism to remind yourself that on SPLIT sow, the left holes go CW by using the left button and the right holes go CCW by using the right button.
-Any hole can be set as UDIR_HOLES to allow the user to override the sow_direct setting.</t>
   </si>
   <si>
     <t>When sowing a second or subsequent circuit of the board, skip the start hole. This will leave the start hole empty for single lap games.
@@ -987,6 +975,20 @@
   <si>
     <t>The multiplier for the seeds scorer. The seeds scorer computes how many seeds each player has on the game board that are not in children.
 Used only for minimax &amp; negamax players.</t>
+  </si>
+  <si>
+    <t>A list of holes from which the user can choose the sow direction. Control is via the mouse button: left is clockwise and right is counter-clockwise.
+Note: all holes respond to both mouse buttons, but if the hole is not in udir_holes, the sow direction will be that prescribed by sow_direct with either button.
+Games with any hole set to user chooses direction must not use MUSTSHARE; GRANDSLAM must be LEGAL; and no special ALLOW_RULE is supported.</t>
+  </si>
+  <si>
+    <t>Direction of sow:
+- CW: clockwise
+- SPLIT: left side holes sow counter-clockwise and right side holes sow clockwise, an odd middle hole must be set in UDIR_HOLES.
+- CCW: counter-clockwise
+- PLAYALTDIR: on the first move of the game, the first player chooses their sow direction using the UDIR_HOLES method (by mouse button). The second player will sow their moves in the opposite direction. Once the first player makes their first move, both player's sow directions are set for the duration of the game no matter which button is used.  All UDIR_HOLES will apply to the game configuration.
+Both mouse buttons will start a move no matter the sow direction. If the hole is marked as UDIR_HOLES, the button selects sow direction. On the other hand, if the hole is not marked as UDIR_HOLES, either button will sow in the prescribed direction. This can be useful, mechanism to remind yourself that on SPLIT sow, the left holes go CW by using the left button and the right holes go CCW by using the right button.
+When PLAYALTDIR is not selected, any hole can be set as UDIR_HOLES to allow the user to override the sow_direct setting.</t>
   </si>
 </sst>
 </file>
@@ -1871,8 +1873,8 @@
   <dimension ref="A1:J70"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J49" sqref="J49"/>
+      <pane ySplit="1" topLeftCell="A54" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J59" sqref="J59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1903,7 +1905,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>4</v>
@@ -1982,7 +1984,7 @@
         <v>0</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="345" x14ac:dyDescent="0.25">
@@ -1990,10 +1992,10 @@
         <v>62</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>177</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>178</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>24</v>
@@ -2002,10 +2004,10 @@
         <v>14</v>
       </c>
       <c r="F4" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="G4" s="5" t="s">
         <v>179</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>180</v>
       </c>
       <c r="H4" s="3">
         <v>3</v>
@@ -2014,7 +2016,7 @@
         <v>0</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -2046,7 +2048,7 @@
         <v>0</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -2110,7 +2112,7 @@
         <v>0</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="150" x14ac:dyDescent="0.25">
@@ -2142,7 +2144,7 @@
         <v>0</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="165" x14ac:dyDescent="0.25">
@@ -2174,7 +2176,7 @@
         <v>0</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="165" x14ac:dyDescent="0.25">
@@ -2206,7 +2208,7 @@
         <v>0</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -2214,10 +2216,10 @@
         <v>95</v>
       </c>
       <c r="B11" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>191</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>192</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>24</v>
@@ -2238,7 +2240,7 @@
         <v>0</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="180" x14ac:dyDescent="0.25">
@@ -2270,7 +2272,7 @@
         <v>0</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="105" x14ac:dyDescent="0.25">
@@ -2302,7 +2304,7 @@
         <v>2</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -2310,10 +2312,10 @@
         <v>95</v>
       </c>
       <c r="B14" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>203</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>204</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>24</v>
@@ -2334,7 +2336,7 @@
         <v>2</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="105" x14ac:dyDescent="0.25">
@@ -2366,7 +2368,7 @@
         <v>2</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="240" x14ac:dyDescent="0.25">
@@ -2398,7 +2400,7 @@
         <v>2</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -2430,7 +2432,7 @@
         <v>2</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2470,10 +2472,10 @@
         <v>95</v>
       </c>
       <c r="B19" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="C19" s="3" t="s">
         <v>214</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>215</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>24</v>
@@ -2494,7 +2496,7 @@
         <v>2</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="150" x14ac:dyDescent="0.25">
@@ -2514,7 +2516,7 @@
         <v>20</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G20" s="5" t="s">
         <v>93</v>
@@ -2526,7 +2528,7 @@
         <v>2</v>
       </c>
       <c r="J20" s="4" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2534,10 +2536,10 @@
         <v>95</v>
       </c>
       <c r="B21" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="C21" s="3" t="s">
         <v>189</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>190</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>24</v>
@@ -2558,7 +2560,7 @@
         <v>2</v>
       </c>
       <c r="J21" s="4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="225" x14ac:dyDescent="0.25">
@@ -2566,10 +2568,10 @@
         <v>95</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>24</v>
@@ -2578,10 +2580,10 @@
         <v>59</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H22" s="3">
         <v>10</v>
@@ -2590,7 +2592,7 @@
         <v>2</v>
       </c>
       <c r="J22" s="4" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
@@ -2622,7 +2624,7 @@
         <v>0</v>
       </c>
       <c r="J23" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -2654,7 +2656,7 @@
         <v>0</v>
       </c>
       <c r="J24" s="4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -2686,7 +2688,7 @@
         <v>0</v>
       </c>
       <c r="J25" s="4" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="105" x14ac:dyDescent="0.25">
@@ -2718,7 +2720,7 @@
         <v>0</v>
       </c>
       <c r="J26" s="4" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="409.5" x14ac:dyDescent="0.25">
@@ -2726,10 +2728,10 @@
         <v>38</v>
       </c>
       <c r="B27" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="C27" s="3" t="s">
         <v>205</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>206</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>24</v>
@@ -2738,10 +2740,10 @@
         <v>62</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="H27" s="3">
         <v>6</v>
@@ -2750,7 +2752,7 @@
         <v>0</v>
       </c>
       <c r="J27" s="4" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="105" x14ac:dyDescent="0.25">
@@ -2782,7 +2784,7 @@
         <v>0</v>
       </c>
       <c r="J28" s="4" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="255" x14ac:dyDescent="0.25">
@@ -2814,7 +2816,7 @@
         <v>2</v>
       </c>
       <c r="J29" s="4" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2846,7 +2848,7 @@
         <v>2</v>
       </c>
       <c r="J30" s="4" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="31" spans="1:10" ht="210" x14ac:dyDescent="0.25">
@@ -2878,7 +2880,7 @@
         <v>2</v>
       </c>
       <c r="J31" s="4" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="285" x14ac:dyDescent="0.25">
@@ -2886,10 +2888,10 @@
         <v>38</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D32" s="3" t="s">
         <v>24</v>
@@ -2898,10 +2900,10 @@
         <v>60</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="G32" s="5" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H32" s="3">
         <v>3</v>
@@ -2910,7 +2912,7 @@
         <v>2</v>
       </c>
       <c r="J32" s="4" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -2918,10 +2920,10 @@
         <v>38</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D33" s="3" t="s">
         <v>24</v>
@@ -2942,7 +2944,7 @@
         <v>2</v>
       </c>
       <c r="J33" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
@@ -2962,7 +2964,7 @@
         <v>28</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G34" s="5" t="s">
         <v>20</v>
@@ -3006,7 +3008,7 @@
         <v>0</v>
       </c>
       <c r="J35" s="4" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="36" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3038,7 +3040,7 @@
         <v>0</v>
       </c>
       <c r="J36" s="4" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="37" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -3070,7 +3072,7 @@
         <v>0</v>
       </c>
       <c r="J37" s="4" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="38" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3102,7 +3104,7 @@
         <v>2</v>
       </c>
       <c r="J38" s="4" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="39" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -3134,7 +3136,7 @@
         <v>2</v>
       </c>
       <c r="J39" s="4" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="40" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -3142,10 +3144,10 @@
         <v>128</v>
       </c>
       <c r="B40" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="C40" s="3" t="s">
         <v>153</v>
-      </c>
-      <c r="C40" s="3" t="s">
-        <v>154</v>
       </c>
       <c r="D40" s="3" t="s">
         <v>147</v>
@@ -3154,11 +3156,11 @@
         <v>13</v>
       </c>
       <c r="F40" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="G40" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="G40" s="3" t="s">
-        <v>155</v>
-      </c>
       <c r="H40" s="3">
         <v>0</v>
       </c>
@@ -3166,7 +3168,7 @@
         <v>0</v>
       </c>
       <c r="J40" s="4" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="41" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3198,7 +3200,7 @@
         <v>0</v>
       </c>
       <c r="J41" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="42" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -3206,10 +3208,10 @@
         <v>128</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D42" s="3" t="s">
         <v>147</v>
@@ -3230,7 +3232,7 @@
         <v>0</v>
       </c>
       <c r="J42" s="4" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="43" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3238,13 +3240,13 @@
         <v>128</v>
       </c>
       <c r="B43" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="C43" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="C43" s="3" t="s">
+      <c r="D43" s="3" t="s">
         <v>158</v>
-      </c>
-      <c r="D43" s="3" t="s">
-        <v>159</v>
       </c>
       <c r="E43" s="3">
         <v>46</v>
@@ -3253,7 +3255,7 @@
         <v>92</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H43" s="3">
         <v>4</v>
@@ -3262,7 +3264,7 @@
         <v>0</v>
       </c>
       <c r="J43" s="4" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -3270,13 +3272,13 @@
         <v>128</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E44" s="3">
         <v>40</v>
@@ -3285,7 +3287,7 @@
         <v>92</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H44" s="3">
         <v>6</v>
@@ -3294,7 +3296,7 @@
         <v>0</v>
       </c>
       <c r="J44" s="4" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="45" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3302,13 +3304,13 @@
         <v>128</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E45" s="3">
         <v>41</v>
@@ -3317,7 +3319,7 @@
         <v>92</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H45" s="3">
         <v>7</v>
@@ -3326,7 +3328,7 @@
         <v>0</v>
       </c>
       <c r="J45" s="4" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="46" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3334,13 +3336,13 @@
         <v>128</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E46" s="3">
         <v>42</v>
@@ -3349,7 +3351,7 @@
         <v>92</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="H46" s="3">
         <v>8</v>
@@ -3358,7 +3360,7 @@
         <v>0</v>
       </c>
       <c r="J46" s="4" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="47" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -3369,7 +3371,7 @@
         <v>129</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D47" s="3" t="s">
         <v>130</v>
@@ -3390,7 +3392,7 @@
         <v>2</v>
       </c>
       <c r="J47" s="4" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="48" spans="1:10" ht="135" x14ac:dyDescent="0.25">
@@ -3422,7 +3424,7 @@
         <v>2</v>
       </c>
       <c r="J48" s="4" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="49" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -3454,7 +3456,7 @@
         <v>2</v>
       </c>
       <c r="J49" s="4" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
     </row>
     <row r="50" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -3486,7 +3488,7 @@
         <v>2</v>
       </c>
       <c r="J50" s="4" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="51" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -3518,7 +3520,7 @@
         <v>2</v>
       </c>
       <c r="J51" s="4" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="52" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -3550,7 +3552,7 @@
         <v>2</v>
       </c>
       <c r="J52" s="4" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="53" spans="1:10" ht="105" x14ac:dyDescent="0.25">
@@ -3582,7 +3584,7 @@
         <v>2</v>
       </c>
       <c r="J53" s="4" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="54" spans="1:10" ht="120" x14ac:dyDescent="0.25">
@@ -3614,15 +3616,15 @@
         <v>2</v>
       </c>
       <c r="J54" s="4" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="55" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D55" s="3" t="s">
         <v>24</v>
@@ -3640,10 +3642,10 @@
         <v>0</v>
       </c>
       <c r="J55" s="4" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="56" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
         <v>9</v>
       </c>
@@ -3666,7 +3668,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="57" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
         <v>9</v>
       </c>
@@ -3686,10 +3688,10 @@
         <v>0</v>
       </c>
       <c r="J57" s="4" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="58" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
         <v>9</v>
       </c>
@@ -3713,7 +3715,7 @@
         <v>0</v>
       </c>
       <c r="J58" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="59" spans="1:10" ht="210" x14ac:dyDescent="0.25">
@@ -3745,10 +3747,10 @@
         <v>0</v>
       </c>
       <c r="J59" s="4" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="60" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
         <v>69</v>
       </c>
@@ -3809,10 +3811,10 @@
         <v>0</v>
       </c>
       <c r="J61" s="4" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="62" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
         <v>69</v>
       </c>
@@ -3841,10 +3843,10 @@
         <v>0</v>
       </c>
       <c r="J62" s="4" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="63" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
         <v>69</v>
       </c>
@@ -3873,7 +3875,7 @@
         <v>0</v>
       </c>
       <c r="J63" s="4" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="64" spans="1:10" ht="409.5" x14ac:dyDescent="0.25">
@@ -3881,10 +3883,10 @@
         <v>69</v>
       </c>
       <c r="B64" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="C64" s="3" t="s">
         <v>197</v>
-      </c>
-      <c r="C64" s="3" t="s">
-        <v>198</v>
       </c>
       <c r="D64" s="3" t="s">
         <v>24</v>
@@ -3893,10 +3895,10 @@
         <v>70</v>
       </c>
       <c r="F64" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="G64" s="5" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H64" s="3">
         <v>6</v>
@@ -3905,7 +3907,7 @@
         <v>0</v>
       </c>
       <c r="J64" s="4" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="65" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -3925,7 +3927,7 @@
         <v>75</v>
       </c>
       <c r="F65" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G65" s="5" t="s">
         <v>93</v>
@@ -3937,10 +3939,10 @@
         <v>0</v>
       </c>
       <c r="J65" s="4" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="66" spans="1:10" ht="195" x14ac:dyDescent="0.25">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
         <v>69</v>
       </c>
@@ -3957,10 +3959,10 @@
         <v>44</v>
       </c>
       <c r="F66" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="G66" s="5" t="s">
         <v>183</v>
-      </c>
-      <c r="G66" s="5" t="s">
-        <v>184</v>
       </c>
       <c r="H66" s="3">
         <v>0</v>
@@ -3969,10 +3971,10 @@
         <v>2</v>
       </c>
       <c r="J66" s="8" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="67" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
         <v>69</v>
       </c>
@@ -4001,18 +4003,18 @@
         <v>2</v>
       </c>
       <c r="J67" s="4" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="68" spans="1:10" ht="409.5" x14ac:dyDescent="0.25">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" ht="285" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
         <v>69</v>
       </c>
       <c r="B68" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="C68" s="3" t="s">
         <v>172</v>
-      </c>
-      <c r="C68" s="3" t="s">
-        <v>173</v>
       </c>
       <c r="D68" s="3" t="s">
         <v>24</v>
@@ -4021,10 +4023,10 @@
         <v>27</v>
       </c>
       <c r="F68" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="G68" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H68" s="3">
         <v>3</v>
@@ -4033,7 +4035,7 @@
         <v>2</v>
       </c>
       <c r="J68" s="4" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="69" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -4041,10 +4043,10 @@
         <v>69</v>
       </c>
       <c r="B69" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="C69" s="3" t="s">
         <v>170</v>
-      </c>
-      <c r="C69" s="3" t="s">
-        <v>171</v>
       </c>
       <c r="D69" s="3" t="s">
         <v>24</v>
@@ -4065,30 +4067,30 @@
         <v>2</v>
       </c>
       <c r="J69" s="4" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="70" spans="1:10" ht="23.25" x14ac:dyDescent="0.25">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
         <v>69</v>
       </c>
       <c r="B70" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="C70" s="3" t="s">
         <v>211</v>
       </c>
-      <c r="C70" s="3" t="s">
+      <c r="D70" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E70" s="3">
+        <v>24</v>
+      </c>
+      <c r="F70" s="3" t="s">
         <v>212</v>
       </c>
-      <c r="D70" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E70" s="3">
-        <v>24</v>
-      </c>
-      <c r="F70" s="3" t="s">
-        <v>213</v>
-      </c>
       <c r="G70" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H70" s="3">
         <v>5</v>
@@ -4097,7 +4099,7 @@
         <v>2</v>
       </c>
       <c r="J70" s="4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
OWN_SOW_CAPT_ALL games reviewed. Rules made consistent with Russ's descriptions. Game descriptions improved. Improved some parameter descriptions. Correct cross reference links in the build_docs.py for game with multiple word names.
</commit_message>
<xml_diff>
--- a/src/game_params.xlsx
+++ b/src/game_params.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Activity_Data\Mancala_github\MancalaGames\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23A569A8-6357-4E48-A530-F898EA87D43A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{672D44C2-9F4F-46A7-A23D-3BFA33041F70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -726,9 +726,6 @@
     <t>When a player has no allowable moves on their turn, they must pass, and continue to do so until they have allowable moves or the game is over. The game is over when there is a clear winner or tie condition, or when neither player has an allowable move.</t>
   </si>
   <si>
-    <t>Is the game played in a series of rounds? In the case of a round win or tie  a new starter is determined via ROUND_STARTER and  the board is reset according to ROUND_FILL. BLOCKS are used in many games and set between rounds based on the seed placement.</t>
-  </si>
-  <si>
     <t>If an opponent has no moves at the start of your turn, you must make seeds available to them if you can. This condition is enforced by only activating holes on the UI will make seeds available.</t>
   </si>
   <si>
@@ -750,12 +747,6 @@
     <t>Only valid when SOW_START is set. Changes the SOW_START behavior so that if there is only one seed in the hole, it is moved in the sow direction by one hole.</t>
   </si>
   <si>
-    <t>Determines if seeds from more the start hole are picked up and sown:
-- OFF: Single lap sowing. Seeds from the start hole are sown, typically, one per hole until expened.
-- LAPPER:  If the first sow ends in a hole with more than one seed, pickup all the seeds and continue sowing another lap. Continue until the final seed of a lap reaches an empty hole, unless there is another rule that stops the sowing (e.g. making a child).
-- LAPPER_NEXT:  If the first sow ends in a hole preceeding a hole with any seeds, pick up the seeds from that next hole and continue sowing another lap. Continue until the hole after the laps final seed is empty.</t>
-  </si>
-  <si>
     <t>A grandslam is when your opponent has seeds at the start of your turn and you capture them all. This option selects what to do:
 - LEGAL: the seeds are captured
 - NOT_LEGAL: you may not capture all of your opponents seeds, a move which would do so is not allowed
@@ -945,23 +936,6 @@
 In multilap games, the start hole for the current lap is skipped. Second or subsequent laps may sow into the original start hole.</t>
   </si>
   <si>
-    <t>Special sow rules add additional behavior or restrictions to the sowing phase:
-- NONE: there is no special sowing rule.
-- SOW_BLKD_DIV: If the final seed of an individual sow lands on the opposite side of the board and brings the contents of that hole to GPARAM_ONE seeds, the hole is closed closed (blocked). In single lap games, the hole's seeds are removed from play. In multilap games, the seeds are used to continue sowing. MLAPS of LAPPER_NEXT is not supported with SOW_BLKD_DIV(_NR).
-  + When sowing, blocked holes on your own side of the board are skipped  and blocked holes on opponent's side are diverted out of play or captured.
-  +  Game GOAL must be DEPRIVE and all of the associated restrictions apply. NOCAPTFIRST maybe used to prevent closing holes on the first move. Capture mechanisms other than closing holes are not supported. The minimum move must be 1 and thus SOW_START is incompatible.  ALLOW_RULE may not be used to limit allowable moves.  SKIP_START and VISIT_OPP are not supported with SOW_BLKD_DIV. 
-- SOW_BLKD_DIV_NR: Behaves the same as SOW_BLKD_DIV except that each player's rightmost hole cannot be closed. 
-- OWN_SOW_CAPT_ALL: The hole OWNer captures all holes that are sown to meet the simple capture criteria: evens, min, max and capture on. Other criteria are enforced: side of the board, unlocked, and not child.
-  + The capture is done by the hole owner, so the non-sower may capture seeds during their opponents sowing. If the game GOAL is TERRITORY the capturer is the hole owner; otherwise each player captures from their own side of the board no matter who is sowing. 
-  + If MLAPS is LAPPER and the final seed sown for any lap meets the capture criteria, the contents of the hole are captured by the sower and not the hole owner and the turn is over.
-  + GRANDSLAM rules are not applied. NOCAPTFIRST prevents this capture for the first move.
-- SOW_SOW_CAPT_ALL: Similar to OWN_SOW_CAPT_ALL but only the SOWer captures seeds from their opponent's holes. 
-  + If mlaps is LAPPER and the final seed sown for any lap meets the capture criteria, the contents of the hole are captured by the sower and not the hole owner and the turn is over.
-  + GRANDSLAM rules are not applied. NOCAPTFIRST prevents this capture for the first move.
-- NO_SOW_OPP_2S: Don't sow into opponents holes with 2 seeds.
-- CHANGE_DIR_LAP: Change the direction for each lap sown. Generally used with UDIR_HOLES so the player may choose the first direction.</t>
-  </si>
-  <si>
     <t xml:space="preserve">The overall goal of the game. Defines how a player wins.
 - MAX_SEEDS: player with the maximum number of seeds at the end of the game wins or they collect more than half of the total seeds
 - DEPRIVE: eliminate all of your opponents seeds.
@@ -989,6 +963,35 @@
 - PLAYALTDIR: on the first move of the game, the first player chooses their sow direction using the UDIR_HOLES method (by mouse button). The second player will sow their moves in the opposite direction. Once the first player makes their first move, both player's sow directions are set for the duration of the game no matter which button is used.  All UDIR_HOLES will apply to the game configuration.
 Both mouse buttons will start a move no matter the sow direction. If the hole is marked as UDIR_HOLES, the button selects sow direction. On the other hand, if the hole is not marked as UDIR_HOLES, either button will sow in the prescribed direction. This can be useful, mechanism to remind yourself that on SPLIT sow, the left holes go CW by using the left button and the right holes go CCW by using the right button.
 When PLAYALTDIR is not selected, any hole can be set as UDIR_HOLES to allow the user to override the sow_direct setting.</t>
+  </si>
+  <si>
+    <t>Special sow rules add additional behavior or restrictions to the sowing phase:
+- NONE: there is no special sowing rule.
+- SOW_BLKD_DIV: If the final seed of an individual sow lands on the opposite side of the board and brings the contents of that hole to GPARAM_ONE seeds, the hole is closed closed (blocked). In single lap games, the hole's seeds are removed from play. In multilap games, the seeds are used to continue sowing. MLAPS of LAPPER_NEXT is not supported with SOW_BLKD_DIV(_NR).
+  + When sowing, blocked holes on your own side of the board are skipped  and blocked holes on opponent's side are diverted out of play or captured.
+  +  Game GOAL must be DEPRIVE and all of the associated restrictions apply. NOCAPTFIRST maybe used to prevent closing holes on the first move. Capture mechanisms other than closing holes are not supported. The minimum move must be 1 and thus SOW_START is incompatible.  ALLOW_RULE may not be used to limit allowable moves.  SKIP_START and VISIT_OPP are not supported with SOW_BLKD_DIV. 
+- SOW_BLKD_DIV_NR: Behaves the same as SOW_BLKD_DIV except that each player's rightmost hole cannot be closed. 
+- OWN_SOW_CAPT_ALL: The hole OWNer captures all holes that are sown to meet the simple capture criteria no matter who sowed them.  The simple capture criteria are: evens, min, max and capture on. Other criteria are enforced: side of the board, unlocked, and not child.
+  + The capture is done by the hole owner, so the non-sower may capture seeds while their opponents sows. If the game GOAL is TERRITORY the capturer is the hole owner; otherwise each player captures from their own side of the board no matter who is sowing. 
+  + If MLAPS is LAPPER and the final seed sown for any lap meets the simple capture criteria for that hole, the contents of the hole are captured by the sower and not the hole owner and the turn is over. For CAPTTWOOUT, CAPT_NEXT and CROSSCAPT captures, the sower always does the final capture.
+  + GRANDSLAM rules are not applied. NOCAPTFIRST prevents these capture for the first move.
+- SOW_SOW_CAPT_ALL: Similar to OWN_SOW_CAPT_ALL but only the SOWer captures seeds from their opponent's holes. 
+  + If mlaps is LAPPER and the final seed sown for any lap meets the capture criteria, the contents of the hole are captured by the sower and not the hole owner and the turn is over.
+  + GRANDSLAM rules are not applied. NOCAPTFIRST prevents this capture for the first move.
+- NO_SOW_OPP_2S: Don't sow into opponents holes with 2 seeds.
+- CHANGE_DIR_LAP: Change the direction for each lap sown. Generally used with UDIR_HOLES so the player may choose the first direction.</t>
+  </si>
+  <si>
+    <t>Is the game played in a series of rounds? When rounds are employed, each round may end under conditions that do not win the overall game. The board is then setup again per the game rules, generally with some feature changed based on the previous round: hole ownership, holes out of play, a shortened board. Play continues in rounds until either player meets the overall game winning condition.
+For example: In Weg each round ends when neither player has a valid move. The board is then set up again after determining who owns what territory (holes). Rounds continue until one player has claimed sufficient territory to be declared the game winner (e.g. ownership of 10 or more holes).
+In the case of a round win or tie  a new starter is determined via ROUND_STARTER and  the board is reset according to ROUND_FILL.
+BLOCKS are used in many games and set between rounds based on the seed placement. TERRITORY GOAL games adjust hole ownership between rounds.</t>
+  </si>
+  <si>
+    <t>Determines if seeds from more the start hole are picked up and sown:
+- OFF: Single lap sowing. Seeds from the start hole are sown, typically, one per hole until expened.
+- LAPPER:  If the first sow ends in a hole with more than one seed, pickup all the seeds and continue sowing another "lap". Note that lap here does not mean a full cicuit of the board, only an individual sow operation. In general, sowing laps continues in this manner until the final seed of a lap reaches an empty hole. There are games with other conditions for ending a multilap low such as making a capture or making a child.
+- LAPPER_NEXT:  For lapper_next sowing, the number of seeds in the last sown hole of lap do not matter. Instead, if the hole after the last sown hole has any seeds, those seeds are used to continue sowing the next lap. Sowing continues until the hole after the lap's final seed is empty. There are games with other conditions for ending a multilap low such as making a capture or making a child.</t>
   </si>
 </sst>
 </file>
@@ -1873,8 +1876,8 @@
   <dimension ref="A1:J70"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A54" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J59" sqref="J59"/>
+      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J66" sqref="J66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1984,7 +1987,7 @@
         <v>0</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="345" x14ac:dyDescent="0.25">
@@ -2016,7 +2019,7 @@
         <v>0</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -2048,7 +2051,7 @@
         <v>0</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -2112,7 +2115,7 @@
         <v>0</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="150" x14ac:dyDescent="0.25">
@@ -2144,7 +2147,7 @@
         <v>0</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="165" x14ac:dyDescent="0.25">
@@ -2176,7 +2179,7 @@
         <v>0</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="165" x14ac:dyDescent="0.25">
@@ -2208,7 +2211,7 @@
         <v>0</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -2240,7 +2243,7 @@
         <v>0</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="180" x14ac:dyDescent="0.25">
@@ -2272,7 +2275,7 @@
         <v>0</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="105" x14ac:dyDescent="0.25">
@@ -2304,7 +2307,7 @@
         <v>2</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -2336,7 +2339,7 @@
         <v>2</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="105" x14ac:dyDescent="0.25">
@@ -2400,7 +2403,7 @@
         <v>2</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -2432,7 +2435,7 @@
         <v>2</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2496,7 +2499,7 @@
         <v>2</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="150" x14ac:dyDescent="0.25">
@@ -2528,7 +2531,7 @@
         <v>2</v>
       </c>
       <c r="J20" s="4" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2560,7 +2563,7 @@
         <v>2</v>
       </c>
       <c r="J21" s="4" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="225" x14ac:dyDescent="0.25">
@@ -2592,7 +2595,7 @@
         <v>2</v>
       </c>
       <c r="J22" s="4" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
@@ -2659,7 +2662,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" ht="165" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>38</v>
       </c>
@@ -2688,7 +2691,7 @@
         <v>0</v>
       </c>
       <c r="J25" s="4" t="s">
-        <v>225</v>
+        <v>271</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="105" x14ac:dyDescent="0.25">
@@ -2752,7 +2755,7 @@
         <v>0</v>
       </c>
       <c r="J27" s="4" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="105" x14ac:dyDescent="0.25">
@@ -2816,7 +2819,7 @@
         <v>2</v>
       </c>
       <c r="J29" s="4" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2880,7 +2883,7 @@
         <v>2</v>
       </c>
       <c r="J31" s="4" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="285" x14ac:dyDescent="0.25">
@@ -2912,7 +2915,7 @@
         <v>2</v>
       </c>
       <c r="J32" s="4" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -3168,7 +3171,7 @@
         <v>0</v>
       </c>
       <c r="J40" s="4" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="41" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3200,7 +3203,7 @@
         <v>0</v>
       </c>
       <c r="J41" s="4" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="42" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -3232,7 +3235,7 @@
         <v>0</v>
       </c>
       <c r="J42" s="4" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="43" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3264,7 +3267,7 @@
         <v>0</v>
       </c>
       <c r="J43" s="4" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -3296,7 +3299,7 @@
         <v>0</v>
       </c>
       <c r="J44" s="4" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="45" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3328,7 +3331,7 @@
         <v>0</v>
       </c>
       <c r="J45" s="4" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="46" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3360,7 +3363,7 @@
         <v>0</v>
       </c>
       <c r="J46" s="4" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="47" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -3371,7 +3374,7 @@
         <v>129</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="D47" s="3" t="s">
         <v>130</v>
@@ -3392,7 +3395,7 @@
         <v>2</v>
       </c>
       <c r="J47" s="4" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="48" spans="1:10" ht="135" x14ac:dyDescent="0.25">
@@ -3424,7 +3427,7 @@
         <v>2</v>
       </c>
       <c r="J48" s="4" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="49" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -3456,7 +3459,7 @@
         <v>2</v>
       </c>
       <c r="J49" s="4" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
     </row>
     <row r="50" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -3488,7 +3491,7 @@
         <v>2</v>
       </c>
       <c r="J50" s="4" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="51" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -3520,7 +3523,7 @@
         <v>2</v>
       </c>
       <c r="J51" s="4" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="52" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -3552,7 +3555,7 @@
         <v>2</v>
       </c>
       <c r="J52" s="4" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="53" spans="1:10" ht="105" x14ac:dyDescent="0.25">
@@ -3584,7 +3587,7 @@
         <v>2</v>
       </c>
       <c r="J53" s="4" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="54" spans="1:10" ht="120" x14ac:dyDescent="0.25">
@@ -3616,7 +3619,7 @@
         <v>2</v>
       </c>
       <c r="J54" s="4" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
@@ -3747,7 +3750,7 @@
         <v>0</v>
       </c>
       <c r="J59" s="4" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
@@ -3811,7 +3814,7 @@
         <v>0</v>
       </c>
       <c r="J61" s="4" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="62" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3843,7 +3846,7 @@
         <v>0</v>
       </c>
       <c r="J62" s="4" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="63" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3875,7 +3878,7 @@
         <v>0</v>
       </c>
       <c r="J63" s="4" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="64" spans="1:10" ht="409.5" x14ac:dyDescent="0.25">
@@ -3907,7 +3910,7 @@
         <v>0</v>
       </c>
       <c r="J64" s="4" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="65" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -3939,10 +3942,10 @@
         <v>0</v>
       </c>
       <c r="J65" s="4" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="66" spans="1:10" ht="105" x14ac:dyDescent="0.25">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" ht="150" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
         <v>69</v>
       </c>
@@ -3971,7 +3974,7 @@
         <v>2</v>
       </c>
       <c r="J66" s="8" t="s">
-        <v>230</v>
+        <v>272</v>
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.25">
@@ -4003,7 +4006,7 @@
         <v>2</v>
       </c>
       <c r="J67" s="4" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="68" spans="1:10" ht="285" x14ac:dyDescent="0.25">
@@ -4035,7 +4038,7 @@
         <v>2</v>
       </c>
       <c r="J68" s="4" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="69" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -4099,7 +4102,7 @@
         <v>2</v>
       </c>
       <c r="J70" s="4" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update Kalah game text and switched to monte carlo ts. Updated documents - wording, etc.
</commit_message>
<xml_diff>
--- a/src/game_params.xlsx
+++ b/src/game_params.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Activity_Data\Mancala_github\MancalaGames\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{672D44C2-9F4F-46A7-A23D-3BFA33041F70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9AC8701-ED2A-4CE6-A944-AFDB59883E01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="600" windowWidth="27990" windowHeight="14880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="game_params" sheetId="1" r:id="rId1"/>
@@ -434,33 +434,18 @@
     <t>access_m</t>
   </si>
   <si>
-    <t>Access mult</t>
-  </si>
-  <si>
     <t>seeds_m</t>
   </si>
   <si>
-    <t>Seeds mult</t>
-  </si>
-  <si>
     <t>empties_m</t>
   </si>
   <si>
-    <t>Empties mult</t>
-  </si>
-  <si>
     <t>child_cnt_m</t>
   </si>
   <si>
-    <t>Child Count mult</t>
-  </si>
-  <si>
     <t>evens_m</t>
   </si>
   <si>
-    <t>Evens mult</t>
-  </si>
-  <si>
     <t>easy_rand</t>
   </si>
   <si>
@@ -468,9 +453,6 @@
   </si>
   <si>
     <t>repeat_turn</t>
-  </si>
-  <si>
-    <t>Repeat Turn mult</t>
   </si>
   <si>
     <t>difficulty</t>
@@ -581,13 +563,6 @@
   </si>
   <si>
     <t>NONE</t>
-  </si>
-  <si>
-    <t>General input</t>
-  </si>
-  <si>
-    <t>Goal of Territory: defines the number of holes needed for a win.
-Goal of Deprive and Blocked Divert Sower: defines the number of seeds needed to close/block holes (sow_blkd_div).</t>
   </si>
   <si>
     <t>LapSower</t>
@@ -701,9 +676,6 @@
 - LAST_MOVER: the player that made the last move of the previous round, starts the new round.</t>
   </si>
   <si>
-    <t xml:space="preserve">Moves maybe made from any hole, independent of the side of the board. Moves need specify side, position and directions.  </t>
-  </si>
-  <si>
     <t>An html help file describing the game (mancala_help.html is the main help file).</t>
   </si>
   <si>
@@ -724,9 +696,6 @@
   </si>
   <si>
     <t>When a player has no allowable moves on their turn, they must pass, and continue to do so until they have allowable moves or the game is over. The game is over when there is a clear winner or tie condition, or when neither player has an allowable move.</t>
-  </si>
-  <si>
-    <t>If an opponent has no moves at the start of your turn, you must make seeds available to them if you can. This condition is enforced by only activating holes on the UI will make seeds available.</t>
   </si>
   <si>
     <t>Allow rules limit the holes from which moves may start.  Disallowed holes are not selectable.
@@ -741,9 +710,6 @@
 - RIGHT_2_1ST_THEN_ALL_TWO:  The first turn must start from one of the two rightmost holes. Subsequent moves may only start from holes without 2 seeds, unless all holes contain zero or 2 seeds.</t>
   </si>
   <si>
-    <t>Sow seeds into your own store when passing it. Do not sow into your opponents store. Sow the final seed of a move into the store, results in a repeat turn.</t>
-  </si>
-  <si>
     <t>Only valid when SOW_START is set. Changes the SOW_START behavior so that if there is only one seed in the hole, it is moved in the sow direction by one hole.</t>
   </si>
   <si>
@@ -757,12 +723,6 @@
   </si>
   <si>
     <t>Repeat turn if there was a capture. Making children is not a capture.</t>
-  </si>
-  <si>
-    <t>Addiitonal child creation requirements may be set:
-- NONE: no additional restrictions.
-- OPP_ONLY:  Only make children on the opposite side of the board. Incompatible with BULL, QUR, and WEG child types.
-- NOT_1ST_OPP: Don't make a child in the first hole on the opponents side/territory with one seed.</t>
   </si>
   <si>
     <t>Choose how holes are filled when a new round strarts:
@@ -783,11 +743,6 @@
     <t>Don't allow captures or closing of holes (SOW_RULE of SOW_BLKD_DIV) on the first move of the game or round.</t>
   </si>
   <si>
-    <t>minimaxer: an Alpha-Beta Pruning MiniMaxer
-negamaxer: minimaxer with a very minor optimization for alternating turn games (no repeat turns). Uses minimaxer depths for difficulties.
-montecarlo_ts: a Monte Carlo Tree Search player.</t>
-  </si>
-  <si>
     <t>Number of end games played out from each expanded node. One value for each difficulty level (0-3).</t>
   </si>
   <si>
@@ -835,9 +790,6 @@
     <t>The multiplier for the stores scorer. Seeds in stores and children are included.
 The stores scorer may not be used in games without STORES or CHILDREN. A zero multiplier disables the stores scorer.
 Used only for  minimax &amp; negamax players.</t>
-  </si>
-  <si>
-    <t>Stores (captured) mult</t>
   </si>
   <si>
     <t>The depth that the minimaxer or negamaxer will search the game tree from the current node. One value for each difficulty.</t>
@@ -907,13 +859,6 @@
     <t xml:space="preserve">Requires MLAPS. If the first 'lap' does not reach the opponent's side of the board, the sowing ends after the first lap. </t>
   </si>
   <si>
-    <t xml:space="preserve">There are three flavors of capture two out:
-Single Lap: capture if sow ends in occupied hole, then an empty hole, followed by an occupied hole the contents of this are hole captured.
-Multi lap but single capture: capture when last hole sown is followed by an empty hole which is then followed by an occupied hole.
-Multi lap with multiple captures: capture when last hole sown is followed by an empty hole which is then followed by an occupied hole. Continue captures as long as the pattern of empty hole followed by an occupied hole continues.
-</t>
-  </si>
-  <si>
     <t>Allows specifing non-all-equal start patterns. The following patterns are supported:
 - ALL_EQUAL: all holes start with the same number of seeds.
 - GAMACHA: starting from the third hold (from start player's left) place nbr_seeds in every other hole, the first move is prescribed move the center hole's seeds to the other side (this is done automatically).
@@ -934,17 +879,6 @@
   <si>
     <t>When sowing a second or subsequent circuit of the board, skip the start hole. This will leave the start hole empty for single lap games.
 In multilap games, the start hole for the current lap is skipped. Second or subsequent laps may sow into the original start hole.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The overall goal of the game. Defines how a player wins.
-- MAX_SEEDS: player with the maximum number of seeds at the end of the game wins or they collect more than half of the total seeds
-- DEPRIVE: eliminate all of your opponents seeds.
-  + If a player has no seeds at the start of their turn, they loose. If a player has no moves at the start of their turn, then the game outcome is determined by who has seeds: If both players have seeds, the game ends in a tie. If the current player has seeds, but the previous player does not, then the current player wins because they forced the previous player to give away all their seeds.
-  + GRAND_SLAM must be legal for DEPRIVE games.
-  + Deprive games cannot be played in ROUNDS, use STORES, or use children. Additionally, the following options are incompatible with DEPRIVE games: MOVEUNLOCK, MUSTPASS, MUSTSHARE and NO_SIDES.
-- TERRITORY: claim ownership of holes. Each round the ownership of holes is determined by the number of seeds captured in the previous round. In a TERRITORY game without rounds, the winner is the player that gained the most territory during play. 
-  + TERRITORY games require STORES and that GPARAM_ONE be set to a value between the number of holes and two times the number of holes.
-  + TERRITORY games are incompatible with NO_SIDES, START_PATTERN, GRANDSLAM of NOT_LEGAL, ALLOW_RULE of OPP_OR_EMPTY, </t>
   </si>
   <si>
     <t>The multiplier for the seeds scorer. The seeds scorer computes how many seeds each player has on the game board that are not in children.
@@ -992,6 +926,73 @@
 - OFF: Single lap sowing. Seeds from the start hole are sown, typically, one per hole until expened.
 - LAPPER:  If the first sow ends in a hole with more than one seed, pickup all the seeds and continue sowing another "lap". Note that lap here does not mean a full cicuit of the board, only an individual sow operation. In general, sowing laps continues in this manner until the final seed of a lap reaches an empty hole. There are games with other conditions for ending a multilap low such as making a capture or making a child.
 - LAPPER_NEXT:  For lapper_next sowing, the number of seeds in the last sown hole of lap do not matter. Instead, if the hole after the last sown hole has any seeds, those seeds are used to continue sowing the next lap. Sowing continues until the hole after the lap's final seed is empty. There are games with other conditions for ending a multilap low such as making a capture or making a child.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Moves maybe made from any hole, independent of the side of the board. Moves need to specify side, position and directions.  </t>
+  </si>
+  <si>
+    <t>General Input</t>
+  </si>
+  <si>
+    <t>GOAL of Territory: defines the number of holes needed for a win.
+GOAL of Deprive and Blocked Divert Sower: defines the number of seeds needed to close/block holes (sow_blkd_div).</t>
+  </si>
+  <si>
+    <t>If an opponent has no moves at the start of your turn, you must make seeds available to them if you can. This condition is enforced by only activating holes on the UI which will make seeds available to the opponent.</t>
+  </si>
+  <si>
+    <t>Sow seeds into your own store when passing it. Do not sow into your opponents store. When the final seed is sown into the store, the sower gets another turn.</t>
+  </si>
+  <si>
+    <t>Additional child creation requirements may be set:
+- NONE: no additional restrictions.
+- OPP_ONLY:  Only make children on the opposite side of the board. Incompatible with BULL, QUR, and WEG child types.
+- NOT_1ST_OPP: Don't make a child in the first hole on the opponents side/territory with one seed.</t>
+  </si>
+  <si>
+    <t>Evens Multiplier</t>
+  </si>
+  <si>
+    <t>Repeat Turn Multiplier</t>
+  </si>
+  <si>
+    <t>Child Count Multiplier</t>
+  </si>
+  <si>
+    <t>Empties Multiplier</t>
+  </si>
+  <si>
+    <t>Seeds Multiplier</t>
+  </si>
+  <si>
+    <t>Access Multiplier</t>
+  </si>
+  <si>
+    <t>Stores (captured) Multiplier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The overall goal of the game. Defines how a player wins.
+- MAX_SEEDS: player with the maximum number of seeds at the end of the game wins or they collect more than half of the total seeds
+- DEPRIVE: eliminate all of your opponents seeds.
+  + If a player has no seeds at the start of their turn, they loose. If a player has no moves at the start of their turn, then the game outcome is determined by who has seeds: If both players have seeds, the game ends in a tie. If the current player has seeds, but the previous player does not, then the current player wins because they forced the previous player to give away all their seeds.
+  + GRANDSLAM must be legal for DEPRIVE games.
+  + Deprive games cannot be played in ROUNDS, use STORES, or use children. Additionally, the following options are incompatible with DEPRIVE games: MOVEUNLOCK, MUSTPASS, MUSTSHARE and NO_SIDES.
+- TERRITORY: claim ownership of holes. Each round the ownership of holes is determined by the number of seeds captured in the previous round. In a TERRITORY game without rounds, the winner is the player that gained the most territory during play. 
+  + TERRITORY games require STORES and that GPARAM_ONE be set to a value between the number of holes and two times the number of holes.
+  + TERRITORY games are incompatible with NO_SIDES, START_PATTERN, GRANDSLAM of NOT_LEGAL, ALLOW_RULE of OPP_OR_EMPTY, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">There are three flavors of capture two out:
+Single lap game: capture if sow ends in occupied hole, then an empty hole, followed by an occupied hole the contents of this are hole captured.
+Multi lap game but single capture: capture when last hole sown is followed by an empty hole which is then followed by an occupied hole.
+Multi lap game with multiple captures: capture when last hole sown is followed by an empty hole which is then followed by an occupied hole. Continue captures as long as the pattern of empty hole followed by an occupied hole continues.
+</t>
+  </si>
+  <si>
+    <t>The algorithm value is the name of the AI player algorithm (a string):
+minimaxer: an Alpha-Beta Pruning MiniMaxer
+negamaxer: minimaxer with a very minor optimization for alternating turn games (no repeat turns). Uses minimaxer depths for difficulties.
+montecarlo_ts: a Monte Carlo Tree Search player.</t>
   </si>
 </sst>
 </file>
@@ -1876,8 +1877,8 @@
   <dimension ref="A1:J70"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J66" sqref="J66"/>
+      <pane ySplit="1" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J40" sqref="J40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1908,7 +1909,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>4</v>
@@ -1958,7 +1959,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>62</v>
       </c>
@@ -1987,7 +1988,7 @@
         <v>0</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>225</v>
+        <v>260</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="345" x14ac:dyDescent="0.25">
@@ -1995,10 +1996,10 @@
         <v>62</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>24</v>
@@ -2007,10 +2008,10 @@
         <v>14</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="H4" s="3">
         <v>3</v>
@@ -2019,7 +2020,7 @@
         <v>0</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>226</v>
+        <v>216</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -2051,7 +2052,7 @@
         <v>0</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>252</v>
+        <v>238</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -2115,7 +2116,7 @@
         <v>0</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>251</v>
+        <v>237</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="150" x14ac:dyDescent="0.25">
@@ -2147,7 +2148,7 @@
         <v>0</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>253</v>
+        <v>239</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="165" x14ac:dyDescent="0.25">
@@ -2179,7 +2180,7 @@
         <v>0</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>254</v>
+        <v>240</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="165" x14ac:dyDescent="0.25">
@@ -2211,7 +2212,7 @@
         <v>0</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>255</v>
+        <v>241</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -2219,10 +2220,10 @@
         <v>95</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>24</v>
@@ -2243,10 +2244,10 @@
         <v>0</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="180" x14ac:dyDescent="0.25">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>95</v>
       </c>
@@ -2275,7 +2276,7 @@
         <v>0</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>262</v>
+        <v>271</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="105" x14ac:dyDescent="0.25">
@@ -2307,7 +2308,7 @@
         <v>2</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>256</v>
+        <v>242</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -2315,10 +2316,10 @@
         <v>95</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>24</v>
@@ -2339,7 +2340,7 @@
         <v>2</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>233</v>
+        <v>221</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="105" x14ac:dyDescent="0.25">
@@ -2371,7 +2372,7 @@
         <v>2</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="240" x14ac:dyDescent="0.25">
@@ -2403,7 +2404,7 @@
         <v>2</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>229</v>
+        <v>218</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -2435,7 +2436,7 @@
         <v>2</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>258</v>
+        <v>244</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2475,10 +2476,10 @@
         <v>95</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>24</v>
@@ -2499,7 +2500,7 @@
         <v>2</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>234</v>
+        <v>222</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="150" x14ac:dyDescent="0.25">
@@ -2519,7 +2520,7 @@
         <v>20</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="G20" s="5" t="s">
         <v>93</v>
@@ -2531,7 +2532,7 @@
         <v>2</v>
       </c>
       <c r="J20" s="4" t="s">
-        <v>259</v>
+        <v>245</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2539,10 +2540,10 @@
         <v>95</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>24</v>
@@ -2563,7 +2564,7 @@
         <v>2</v>
       </c>
       <c r="J21" s="4" t="s">
-        <v>230</v>
+        <v>219</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="225" x14ac:dyDescent="0.25">
@@ -2571,10 +2572,10 @@
         <v>95</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>24</v>
@@ -2583,10 +2584,10 @@
         <v>59</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="H22" s="3">
         <v>10</v>
@@ -2595,7 +2596,7 @@
         <v>2</v>
       </c>
       <c r="J22" s="4" t="s">
-        <v>260</v>
+        <v>246</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
@@ -2627,7 +2628,7 @@
         <v>0</v>
       </c>
       <c r="J23" s="4" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -2659,7 +2660,7 @@
         <v>0</v>
       </c>
       <c r="J24" s="4" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="165" x14ac:dyDescent="0.25">
@@ -2691,7 +2692,7 @@
         <v>0</v>
       </c>
       <c r="J25" s="4" t="s">
-        <v>271</v>
+        <v>255</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="105" x14ac:dyDescent="0.25">
@@ -2723,7 +2724,7 @@
         <v>0</v>
       </c>
       <c r="J26" s="4" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="409.5" x14ac:dyDescent="0.25">
@@ -2731,10 +2732,10 @@
         <v>38</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>24</v>
@@ -2743,10 +2744,10 @@
         <v>62</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
       <c r="H27" s="3">
         <v>6</v>
@@ -2755,7 +2756,7 @@
         <v>0</v>
       </c>
       <c r="J27" s="4" t="s">
-        <v>232</v>
+        <v>220</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="105" x14ac:dyDescent="0.25">
@@ -2787,7 +2788,7 @@
         <v>0</v>
       </c>
       <c r="J28" s="4" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="255" x14ac:dyDescent="0.25">
@@ -2819,7 +2820,7 @@
         <v>2</v>
       </c>
       <c r="J29" s="4" t="s">
-        <v>266</v>
+        <v>270</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2851,7 +2852,7 @@
         <v>2</v>
       </c>
       <c r="J30" s="4" t="s">
-        <v>217</v>
+        <v>257</v>
       </c>
     </row>
     <row r="31" spans="1:10" ht="210" x14ac:dyDescent="0.25">
@@ -2883,7 +2884,7 @@
         <v>2</v>
       </c>
       <c r="J31" s="4" t="s">
-        <v>263</v>
+        <v>248</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="285" x14ac:dyDescent="0.25">
@@ -2891,10 +2892,10 @@
         <v>38</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="D32" s="3" t="s">
         <v>24</v>
@@ -2903,10 +2904,10 @@
         <v>60</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="G32" s="5" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="H32" s="3">
         <v>3</v>
@@ -2915,18 +2916,18 @@
         <v>2</v>
       </c>
       <c r="J32" s="4" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>38</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>180</v>
+        <v>258</v>
       </c>
       <c r="D33" s="3" t="s">
         <v>24</v>
@@ -2947,7 +2948,7 @@
         <v>2</v>
       </c>
       <c r="J33" s="4" t="s">
-        <v>181</v>
+        <v>259</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
@@ -2967,7 +2968,7 @@
         <v>28</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="G34" s="5" t="s">
         <v>20</v>
@@ -3011,7 +3012,7 @@
         <v>0</v>
       </c>
       <c r="J35" s="4" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
     </row>
     <row r="36" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3043,7 +3044,7 @@
         <v>0</v>
       </c>
       <c r="J36" s="4" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
     </row>
     <row r="37" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -3066,7 +3067,7 @@
         <v>30</v>
       </c>
       <c r="G37" s="6" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="H37" s="3">
         <v>4</v>
@@ -3075,7 +3076,7 @@
         <v>0</v>
       </c>
       <c r="J37" s="4" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
     </row>
     <row r="38" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3107,7 +3108,7 @@
         <v>2</v>
       </c>
       <c r="J38" s="4" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
     </row>
     <row r="39" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -3139,7 +3140,7 @@
         <v>2</v>
       </c>
       <c r="J39" s="4" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
     </row>
     <row r="40" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -3147,22 +3148,22 @@
         <v>128</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="E40" s="3">
         <v>13</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="H40" s="3">
         <v>0</v>
@@ -3171,7 +3172,7 @@
         <v>0</v>
       </c>
       <c r="J40" s="4" t="s">
-        <v>235</v>
+        <v>272</v>
       </c>
     </row>
     <row r="41" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3179,13 +3180,13 @@
         <v>128</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="E41" s="3">
         <v>30</v>
@@ -3203,7 +3204,7 @@
         <v>0</v>
       </c>
       <c r="J41" s="4" t="s">
-        <v>239</v>
+        <v>226</v>
       </c>
     </row>
     <row r="42" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -3211,13 +3212,13 @@
         <v>128</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="E42" s="3">
         <v>12</v>
@@ -3235,7 +3236,7 @@
         <v>0</v>
       </c>
       <c r="J42" s="4" t="s">
-        <v>240</v>
+        <v>227</v>
       </c>
     </row>
     <row r="43" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3243,13 +3244,13 @@
         <v>128</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="E43" s="3">
         <v>46</v>
@@ -3258,7 +3259,7 @@
         <v>92</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="H43" s="3">
         <v>4</v>
@@ -3267,7 +3268,7 @@
         <v>0</v>
       </c>
       <c r="J43" s="4" t="s">
-        <v>249</v>
+        <v>235</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -3275,13 +3276,13 @@
         <v>128</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="E44" s="3">
         <v>40</v>
@@ -3290,7 +3291,7 @@
         <v>92</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="H44" s="3">
         <v>6</v>
@@ -3299,7 +3300,7 @@
         <v>0</v>
       </c>
       <c r="J44" s="4" t="s">
-        <v>238</v>
+        <v>225</v>
       </c>
     </row>
     <row r="45" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3307,13 +3308,13 @@
         <v>128</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="E45" s="3">
         <v>41</v>
@@ -3322,7 +3323,7 @@
         <v>92</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="H45" s="3">
         <v>7</v>
@@ -3331,7 +3332,7 @@
         <v>0</v>
       </c>
       <c r="J45" s="4" t="s">
-        <v>237</v>
+        <v>224</v>
       </c>
     </row>
     <row r="46" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3339,13 +3340,13 @@
         <v>128</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="E46" s="3">
         <v>42</v>
@@ -3354,7 +3355,7 @@
         <v>92</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="H46" s="3">
         <v>8</v>
@@ -3363,7 +3364,7 @@
         <v>0</v>
       </c>
       <c r="J46" s="4" t="s">
-        <v>236</v>
+        <v>223</v>
       </c>
     </row>
     <row r="47" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -3374,7 +3375,7 @@
         <v>129</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>248</v>
+        <v>269</v>
       </c>
       <c r="D47" s="3" t="s">
         <v>130</v>
@@ -3395,7 +3396,7 @@
         <v>2</v>
       </c>
       <c r="J47" s="4" t="s">
-        <v>247</v>
+        <v>234</v>
       </c>
     </row>
     <row r="48" spans="1:10" ht="135" x14ac:dyDescent="0.25">
@@ -3406,7 +3407,7 @@
         <v>131</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>132</v>
+        <v>268</v>
       </c>
       <c r="D48" s="3" t="s">
         <v>130</v>
@@ -3427,7 +3428,7 @@
         <v>2</v>
       </c>
       <c r="J48" s="4" t="s">
-        <v>245</v>
+        <v>232</v>
       </c>
     </row>
     <row r="49" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -3435,10 +3436,10 @@
         <v>128</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>134</v>
+        <v>267</v>
       </c>
       <c r="D49" s="3" t="s">
         <v>130</v>
@@ -3459,7 +3460,7 @@
         <v>2</v>
       </c>
       <c r="J49" s="4" t="s">
-        <v>267</v>
+        <v>251</v>
       </c>
     </row>
     <row r="50" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -3467,10 +3468,10 @@
         <v>128</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>136</v>
+        <v>266</v>
       </c>
       <c r="D50" s="3" t="s">
         <v>130</v>
@@ -3491,7 +3492,7 @@
         <v>2</v>
       </c>
       <c r="J50" s="4" t="s">
-        <v>244</v>
+        <v>231</v>
       </c>
     </row>
     <row r="51" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -3499,10 +3500,10 @@
         <v>128</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>138</v>
+        <v>265</v>
       </c>
       <c r="D51" s="3" t="s">
         <v>130</v>
@@ -3523,7 +3524,7 @@
         <v>2</v>
       </c>
       <c r="J51" s="4" t="s">
-        <v>243</v>
+        <v>230</v>
       </c>
     </row>
     <row r="52" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -3531,10 +3532,10 @@
         <v>128</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>140</v>
+        <v>263</v>
       </c>
       <c r="D52" s="3" t="s">
         <v>130</v>
@@ -3555,7 +3556,7 @@
         <v>2</v>
       </c>
       <c r="J52" s="4" t="s">
-        <v>242</v>
+        <v>229</v>
       </c>
     </row>
     <row r="53" spans="1:10" ht="105" x14ac:dyDescent="0.25">
@@ -3563,10 +3564,10 @@
         <v>128</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="D53" s="3" t="s">
         <v>130</v>
@@ -3587,7 +3588,7 @@
         <v>2</v>
       </c>
       <c r="J53" s="4" t="s">
-        <v>241</v>
+        <v>228</v>
       </c>
     </row>
     <row r="54" spans="1:10" ht="120" x14ac:dyDescent="0.25">
@@ -3595,10 +3596,10 @@
         <v>128</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>144</v>
+        <v>264</v>
       </c>
       <c r="D54" s="3" t="s">
         <v>130</v>
@@ -3619,7 +3620,7 @@
         <v>2</v>
       </c>
       <c r="J54" s="4" t="s">
-        <v>246</v>
+        <v>233</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
@@ -3627,7 +3628,7 @@
         <v>9</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="D55" s="3" t="s">
         <v>24</v>
@@ -3645,7 +3646,7 @@
         <v>0</v>
       </c>
       <c r="J55" s="4" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
@@ -3691,7 +3692,7 @@
         <v>0</v>
       </c>
       <c r="J57" s="4" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
@@ -3718,7 +3719,7 @@
         <v>0</v>
       </c>
       <c r="J58" s="4" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
     </row>
     <row r="59" spans="1:10" ht="210" x14ac:dyDescent="0.25">
@@ -3750,7 +3751,7 @@
         <v>0</v>
       </c>
       <c r="J59" s="4" t="s">
-        <v>269</v>
+        <v>253</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
@@ -3814,7 +3815,7 @@
         <v>0</v>
       </c>
       <c r="J61" s="4" t="s">
-        <v>265</v>
+        <v>250</v>
       </c>
     </row>
     <row r="62" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3846,7 +3847,7 @@
         <v>0</v>
       </c>
       <c r="J62" s="4" t="s">
-        <v>227</v>
+        <v>261</v>
       </c>
     </row>
     <row r="63" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3878,7 +3879,7 @@
         <v>0</v>
       </c>
       <c r="J63" s="4" t="s">
-        <v>228</v>
+        <v>217</v>
       </c>
     </row>
     <row r="64" spans="1:10" ht="409.5" x14ac:dyDescent="0.25">
@@ -3886,10 +3887,10 @@
         <v>69</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D64" s="3" t="s">
         <v>24</v>
@@ -3898,10 +3899,10 @@
         <v>70</v>
       </c>
       <c r="F64" s="3" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="G64" s="5" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="H64" s="3">
         <v>6</v>
@@ -3910,7 +3911,7 @@
         <v>0</v>
       </c>
       <c r="J64" s="4" t="s">
-        <v>270</v>
+        <v>254</v>
       </c>
     </row>
     <row r="65" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -3930,7 +3931,7 @@
         <v>75</v>
       </c>
       <c r="F65" s="3" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="G65" s="5" t="s">
         <v>93</v>
@@ -3942,7 +3943,7 @@
         <v>0</v>
       </c>
       <c r="J65" s="4" t="s">
-        <v>268</v>
+        <v>252</v>
       </c>
     </row>
     <row r="66" spans="1:10" ht="150" x14ac:dyDescent="0.25">
@@ -3962,10 +3963,10 @@
         <v>44</v>
       </c>
       <c r="F66" s="3" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="G66" s="5" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="H66" s="3">
         <v>0</v>
@@ -3974,7 +3975,7 @@
         <v>2</v>
       </c>
       <c r="J66" s="8" t="s">
-        <v>272</v>
+        <v>256</v>
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.25">
@@ -4006,7 +4007,7 @@
         <v>2</v>
       </c>
       <c r="J67" s="4" t="s">
-        <v>261</v>
+        <v>247</v>
       </c>
     </row>
     <row r="68" spans="1:10" ht="285" x14ac:dyDescent="0.25">
@@ -4014,10 +4015,10 @@
         <v>69</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="D68" s="3" t="s">
         <v>24</v>
@@ -4026,10 +4027,10 @@
         <v>27</v>
       </c>
       <c r="F68" s="3" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="G68" s="5" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="H68" s="3">
         <v>3</v>
@@ -4038,7 +4039,7 @@
         <v>2</v>
       </c>
       <c r="J68" s="4" t="s">
-        <v>257</v>
+        <v>243</v>
       </c>
     </row>
     <row r="69" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -4046,10 +4047,10 @@
         <v>69</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="D69" s="3" t="s">
         <v>24</v>
@@ -4070,7 +4071,7 @@
         <v>2</v>
       </c>
       <c r="J69" s="4" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
     </row>
     <row r="70" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -4078,10 +4079,10 @@
         <v>69</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="D70" s="3" t="s">
         <v>24</v>
@@ -4090,10 +4091,10 @@
         <v>24</v>
       </c>
       <c r="F70" s="3" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="G70" s="3" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="H70" s="3">
         <v>5</v>
@@ -4102,7 +4103,7 @@
         <v>2</v>
       </c>
       <c r="J70" s="4" t="s">
-        <v>231</v>
+        <v>262</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added sow tests in test_cmp_sow.py added log statement to sower.py updates to some help files
</commit_message>
<xml_diff>
--- a/src/game_params.xlsx
+++ b/src/game_params.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Activity_Data\Mancala_github\MancalaGames\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9AC8701-ED2A-4CE6-A944-AFDB59883E01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{400E2958-8A68-4BC8-B7A2-1312D3808540}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="600" windowWidth="27990" windowHeight="14880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28695" yWindow="480" windowWidth="27990" windowHeight="14880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="game_params" sheetId="1" r:id="rId1"/>
@@ -899,11 +899,84 @@
 When PLAYALTDIR is not selected, any hole can be set as UDIR_HOLES to allow the user to override the sow_direct setting.</t>
   </si>
   <si>
+    <t>Is the game played in a series of rounds? When rounds are employed, each round may end under conditions that do not win the overall game. The board is then setup again per the game rules, generally with some feature changed based on the previous round: hole ownership, holes out of play, a shortened board. Play continues in rounds until either player meets the overall game winning condition.
+For example: In Weg each round ends when neither player has a valid move. The board is then set up again after determining who owns what territory (holes). Rounds continue until one player has claimed sufficient territory to be declared the game winner (e.g. ownership of 10 or more holes).
+In the case of a round win or tie  a new starter is determined via ROUND_STARTER and  the board is reset according to ROUND_FILL.
+BLOCKS are used in many games and set between rounds based on the seed placement. TERRITORY GOAL games adjust hole ownership between rounds.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Moves maybe made from any hole, independent of the side of the board. Moves need to specify side, position and directions.  </t>
+  </si>
+  <si>
+    <t>General Input</t>
+  </si>
+  <si>
+    <t>GOAL of Territory: defines the number of holes needed for a win.
+GOAL of Deprive and Blocked Divert Sower: defines the number of seeds needed to close/block holes (sow_blkd_div).</t>
+  </si>
+  <si>
+    <t>If an opponent has no moves at the start of your turn, you must make seeds available to them if you can. This condition is enforced by only activating holes on the UI which will make seeds available to the opponent.</t>
+  </si>
+  <si>
+    <t>Sow seeds into your own store when passing it. Do not sow into your opponents store. When the final seed is sown into the store, the sower gets another turn.</t>
+  </si>
+  <si>
+    <t>Additional child creation requirements may be set:
+- NONE: no additional restrictions.
+- OPP_ONLY:  Only make children on the opposite side of the board. Incompatible with BULL, QUR, and WEG child types.
+- NOT_1ST_OPP: Don't make a child in the first hole on the opponents side/territory with one seed.</t>
+  </si>
+  <si>
+    <t>Evens Multiplier</t>
+  </si>
+  <si>
+    <t>Repeat Turn Multiplier</t>
+  </si>
+  <si>
+    <t>Child Count Multiplier</t>
+  </si>
+  <si>
+    <t>Empties Multiplier</t>
+  </si>
+  <si>
+    <t>Seeds Multiplier</t>
+  </si>
+  <si>
+    <t>Access Multiplier</t>
+  </si>
+  <si>
+    <t>Stores (captured) Multiplier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The overall goal of the game. Defines how a player wins.
+- MAX_SEEDS: player with the maximum number of seeds at the end of the game wins or they collect more than half of the total seeds
+- DEPRIVE: eliminate all of your opponents seeds.
+  + If a player has no seeds at the start of their turn, they loose. If a player has no moves at the start of their turn, then the game outcome is determined by who has seeds: If both players have seeds, the game ends in a tie. If the current player has seeds, but the previous player does not, then the current player wins because they forced the previous player to give away all their seeds.
+  + GRANDSLAM must be legal for DEPRIVE games.
+  + Deprive games cannot be played in ROUNDS, use STORES, or use children. Additionally, the following options are incompatible with DEPRIVE games: MOVEUNLOCK, MUSTPASS, MUSTSHARE and NO_SIDES.
+- TERRITORY: claim ownership of holes. Each round the ownership of holes is determined by the number of seeds captured in the previous round. In a TERRITORY game without rounds, the winner is the player that gained the most territory during play. 
+  + TERRITORY games require STORES and that GPARAM_ONE be set to a value between the number of holes and two times the number of holes.
+  + TERRITORY games are incompatible with NO_SIDES, START_PATTERN, GRANDSLAM of NOT_LEGAL, ALLOW_RULE of OPP_OR_EMPTY, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">There are three flavors of capture two out:
+Single lap game: capture if sow ends in occupied hole, then an empty hole, followed by an occupied hole the contents of this are hole captured.
+Multi lap game but single capture: capture when last hole sown is followed by an empty hole which is then followed by an occupied hole.
+Multi lap game with multiple captures: capture when last hole sown is followed by an empty hole which is then followed by an occupied hole. Continue captures as long as the pattern of empty hole followed by an occupied hole continues.
+</t>
+  </si>
+  <si>
+    <t>The algorithm value is the name of the AI player algorithm (a string):
+minimaxer: an Alpha-Beta Pruning MiniMaxer
+negamaxer: minimaxer with a very minor optimization for alternating turn games (no repeat turns). Uses minimaxer depths for difficulties.
+montecarlo_ts: a Monte Carlo Tree Search player.</t>
+  </si>
+  <si>
     <t>Special sow rules add additional behavior or restrictions to the sowing phase:
 - NONE: there is no special sowing rule.
-- SOW_BLKD_DIV: If the final seed of an individual sow lands on the opposite side of the board and brings the contents of that hole to GPARAM_ONE seeds, the hole is closed closed (blocked). In single lap games, the hole's seeds are removed from play. In multilap games, the seeds are used to continue sowing. MLAPS of LAPPER_NEXT is not supported with SOW_BLKD_DIV(_NR).
+- SOW_BLKD_DIV: If the final seed of an individual sow lands on the opposite side of the board and brings the contents of that hole to GPARAM_ONE seeds, the hole is closed closed (blocked). In single lap games, the hole's seeds are removed from play. In multilap games, the seeds are used to continue sowing.
   + When sowing, blocked holes on your own side of the board are skipped  and blocked holes on opponent's side are diverted out of play or captured.
-  +  Game GOAL must be DEPRIVE and all of the associated restrictions apply. NOCAPTFIRST maybe used to prevent closing holes on the first move. Capture mechanisms other than closing holes are not supported. The minimum move must be 1 and thus SOW_START is incompatible.  ALLOW_RULE may not be used to limit allowable moves.  SKIP_START and VISIT_OPP are not supported with SOW_BLKD_DIV. 
+  +  Game GOAL must be DEPRIVE and all of the associated restrictions apply. NOCAPTFIRST maybe used to prevent closing holes on the first move. Capture mechanisms other than closing holes are not supported. The minimum move must be 1 and thus SOW_START is incompatible.  ALLOW_RULE may not be used to limit allowable moves.  SKIP_START and VISIT_OPP are not supported with SOW_BLKD_DIV.  MLAPS of LAPPER_NEXT is not supported with SOW_BLKD_DIV(_NR).
 - SOW_BLKD_DIV_NR: Behaves the same as SOW_BLKD_DIV except that each player's rightmost hole cannot be closed. 
 - OWN_SOW_CAPT_ALL: The hole OWNer captures all holes that are sown to meet the simple capture criteria no matter who sowed them.  The simple capture criteria are: evens, min, max and capture on. Other criteria are enforced: side of the board, unlocked, and not child.
   + The capture is done by the hole owner, so the non-sower may capture seeds while their opponents sows. If the game GOAL is TERRITORY the capturer is the hole owner; otherwise each player captures from their own side of the board no matter who is sowing. 
@@ -916,83 +989,12 @@
 - CHANGE_DIR_LAP: Change the direction for each lap sown. Generally used with UDIR_HOLES so the player may choose the first direction.</t>
   </si>
   <si>
-    <t>Is the game played in a series of rounds? When rounds are employed, each round may end under conditions that do not win the overall game. The board is then setup again per the game rules, generally with some feature changed based on the previous round: hole ownership, holes out of play, a shortened board. Play continues in rounds until either player meets the overall game winning condition.
-For example: In Weg each round ends when neither player has a valid move. The board is then set up again after determining who owns what territory (holes). Rounds continue until one player has claimed sufficient territory to be declared the game winner (e.g. ownership of 10 or more holes).
-In the case of a round win or tie  a new starter is determined via ROUND_STARTER and  the board is reset according to ROUND_FILL.
-BLOCKS are used in many games and set between rounds based on the seed placement. TERRITORY GOAL games adjust hole ownership between rounds.</t>
-  </si>
-  <si>
     <t>Determines if seeds from more the start hole are picked up and sown:
 - OFF: Single lap sowing. Seeds from the start hole are sown, typically, one per hole until expened.
-- LAPPER:  If the first sow ends in a hole with more than one seed, pickup all the seeds and continue sowing another "lap". Note that lap here does not mean a full cicuit of the board, only an individual sow operation. In general, sowing laps continues in this manner until the final seed of a lap reaches an empty hole. There are games with other conditions for ending a multilap low such as making a capture or making a child.
-- LAPPER_NEXT:  For lapper_next sowing, the number of seeds in the last sown hole of lap do not matter. Instead, if the hole after the last sown hole has any seeds, those seeds are used to continue sowing the next lap. Sowing continues until the hole after the lap's final seed is empty. There are games with other conditions for ending a multilap low such as making a capture or making a child.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Moves maybe made from any hole, independent of the side of the board. Moves need to specify side, position and directions.  </t>
-  </si>
-  <si>
-    <t>General Input</t>
-  </si>
-  <si>
-    <t>GOAL of Territory: defines the number of holes needed for a win.
-GOAL of Deprive and Blocked Divert Sower: defines the number of seeds needed to close/block holes (sow_blkd_div).</t>
-  </si>
-  <si>
-    <t>If an opponent has no moves at the start of your turn, you must make seeds available to them if you can. This condition is enforced by only activating holes on the UI which will make seeds available to the opponent.</t>
-  </si>
-  <si>
-    <t>Sow seeds into your own store when passing it. Do not sow into your opponents store. When the final seed is sown into the store, the sower gets another turn.</t>
-  </si>
-  <si>
-    <t>Additional child creation requirements may be set:
-- NONE: no additional restrictions.
-- OPP_ONLY:  Only make children on the opposite side of the board. Incompatible with BULL, QUR, and WEG child types.
-- NOT_1ST_OPP: Don't make a child in the first hole on the opponents side/territory with one seed.</t>
-  </si>
-  <si>
-    <t>Evens Multiplier</t>
-  </si>
-  <si>
-    <t>Repeat Turn Multiplier</t>
-  </si>
-  <si>
-    <t>Child Count Multiplier</t>
-  </si>
-  <si>
-    <t>Empties Multiplier</t>
-  </si>
-  <si>
-    <t>Seeds Multiplier</t>
-  </si>
-  <si>
-    <t>Access Multiplier</t>
-  </si>
-  <si>
-    <t>Stores (captured) Multiplier</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The overall goal of the game. Defines how a player wins.
-- MAX_SEEDS: player with the maximum number of seeds at the end of the game wins or they collect more than half of the total seeds
-- DEPRIVE: eliminate all of your opponents seeds.
-  + If a player has no seeds at the start of their turn, they loose. If a player has no moves at the start of their turn, then the game outcome is determined by who has seeds: If both players have seeds, the game ends in a tie. If the current player has seeds, but the previous player does not, then the current player wins because they forced the previous player to give away all their seeds.
-  + GRANDSLAM must be legal for DEPRIVE games.
-  + Deprive games cannot be played in ROUNDS, use STORES, or use children. Additionally, the following options are incompatible with DEPRIVE games: MOVEUNLOCK, MUSTPASS, MUSTSHARE and NO_SIDES.
-- TERRITORY: claim ownership of holes. Each round the ownership of holes is determined by the number of seeds captured in the previous round. In a TERRITORY game without rounds, the winner is the player that gained the most territory during play. 
-  + TERRITORY games require STORES and that GPARAM_ONE be set to a value between the number of holes and two times the number of holes.
-  + TERRITORY games are incompatible with NO_SIDES, START_PATTERN, GRANDSLAM of NOT_LEGAL, ALLOW_RULE of OPP_OR_EMPTY, </t>
-  </si>
-  <si>
-    <t xml:space="preserve">There are three flavors of capture two out:
-Single lap game: capture if sow ends in occupied hole, then an empty hole, followed by an occupied hole the contents of this are hole captured.
-Multi lap game but single capture: capture when last hole sown is followed by an empty hole which is then followed by an occupied hole.
-Multi lap game with multiple captures: capture when last hole sown is followed by an empty hole which is then followed by an occupied hole. Continue captures as long as the pattern of empty hole followed by an occupied hole continues.
-</t>
-  </si>
-  <si>
-    <t>The algorithm value is the name of the AI player algorithm (a string):
-minimaxer: an Alpha-Beta Pruning MiniMaxer
-negamaxer: minimaxer with a very minor optimization for alternating turn games (no repeat turns). Uses minimaxer depths for difficulties.
-montecarlo_ts: a Monte Carlo Tree Search player.</t>
+- LAPPER:  If the first sow ends in a hole with more than one seed, pickup all the seeds and continue sowing another "lap". Note that lap here does not mean a full cicuit of the board, only an individual sow operation. In general, sowing laps continues in this manner until the final seed of a lap reaches an empty hole. There are games with other conditions for ending a multilap low such as making a capture or making a child. 
+  + Several values of SOW_RULE perform an operation after each lap sown: SOW_CLKD_DIV(_NR) closes the final hole and CHANGE_DIR_LAP changes the direction of sowing after each lap.
+- LAPPER_NEXT:  For lapper_next sowing, the number of seeds in the last sown hole of lap do not matter. Instead, if the hole after the last sown hole has any seeds, those seeds are used to continue sowing the next lap. Sowing continues until the hole after the lap's final seed is empty. There are games with other conditions for ending a multilap low such as making a capture or making a child.
+  + A SOW_RULE of CHANGE_DIR_LAP changes the direction of sowing after each lap. SOW_BLKD_DIV(_NR) is not supported for LAPPER_NEXT.</t>
   </si>
 </sst>
 </file>
@@ -1877,8 +1879,8 @@
   <dimension ref="A1:J70"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J40" sqref="J40"/>
+      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J66" sqref="J66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1988,7 +1990,7 @@
         <v>0</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="345" x14ac:dyDescent="0.25">
@@ -2276,7 +2278,7 @@
         <v>0</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="105" x14ac:dyDescent="0.25">
@@ -2692,7 +2694,7 @@
         <v>0</v>
       </c>
       <c r="J25" s="4" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="105" x14ac:dyDescent="0.25">
@@ -2820,7 +2822,7 @@
         <v>2</v>
       </c>
       <c r="J29" s="4" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2852,7 +2854,7 @@
         <v>2</v>
       </c>
       <c r="J30" s="4" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="31" spans="1:10" ht="210" x14ac:dyDescent="0.25">
@@ -2927,7 +2929,7 @@
         <v>176</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="D33" s="3" t="s">
         <v>24</v>
@@ -2948,7 +2950,7 @@
         <v>2</v>
       </c>
       <c r="J33" s="4" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
@@ -3172,7 +3174,7 @@
         <v>0</v>
       </c>
       <c r="J40" s="4" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
     </row>
     <row r="41" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3367,7 +3369,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="47" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
         <v>128</v>
       </c>
@@ -3375,7 +3377,7 @@
         <v>129</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="D47" s="3" t="s">
         <v>130</v>
@@ -3399,7 +3401,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="48" spans="1:10" ht="135" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
         <v>128</v>
       </c>
@@ -3407,7 +3409,7 @@
         <v>131</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D48" s="3" t="s">
         <v>130</v>
@@ -3439,7 +3441,7 @@
         <v>132</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D49" s="3" t="s">
         <v>130</v>
@@ -3463,7 +3465,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="50" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
         <v>128</v>
       </c>
@@ -3471,7 +3473,7 @@
         <v>133</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="D50" s="3" t="s">
         <v>130</v>
@@ -3495,7 +3497,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="51" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
         <v>128</v>
       </c>
@@ -3503,7 +3505,7 @@
         <v>134</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="D51" s="3" t="s">
         <v>130</v>
@@ -3527,7 +3529,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="52" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
         <v>128</v>
       </c>
@@ -3535,7 +3537,7 @@
         <v>135</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="D52" s="3" t="s">
         <v>130</v>
@@ -3559,7 +3561,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="53" spans="1:10" ht="105" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
         <v>128</v>
       </c>
@@ -3591,7 +3593,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="54" spans="1:10" ht="120" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
         <v>128</v>
       </c>
@@ -3599,7 +3601,7 @@
         <v>138</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="D54" s="3" t="s">
         <v>130</v>
@@ -3847,7 +3849,7 @@
         <v>0</v>
       </c>
       <c r="J62" s="4" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="63" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3911,7 +3913,7 @@
         <v>0</v>
       </c>
       <c r="J64" s="4" t="s">
-        <v>254</v>
+        <v>271</v>
       </c>
     </row>
     <row r="65" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -3946,7 +3948,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="66" spans="1:10" ht="150" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10" ht="210" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
         <v>69</v>
       </c>
@@ -3975,7 +3977,7 @@
         <v>2</v>
       </c>
       <c r="J66" s="8" t="s">
-        <v>256</v>
+        <v>272</v>
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.25">
@@ -4103,7 +4105,7 @@
         <v>2</v>
       </c>
       <c r="J70" s="4" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Move "easy addin" back to bottom of minimaxer parameters.
</commit_message>
<xml_diff>
--- a/src/game_params.xlsx
+++ b/src/game_params.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Activity_Data\Mancala_github\MancalaGames\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{400E2958-8A68-4BC8-B7A2-1312D3808540}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D61BE2E8-1255-451A-A2B9-2845D2C19A20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28695" yWindow="480" windowWidth="27990" windowHeight="14880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="game_params" sheetId="1" r:id="rId1"/>
@@ -1879,8 +1879,8 @@
   <dimension ref="A1:J70"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J66" sqref="J66"/>
+      <pane ySplit="1" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H54" sqref="H54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3584,7 +3584,7 @@
         <v>89</v>
       </c>
       <c r="H53" s="3">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I53" s="3">
         <v>2</v>
@@ -3616,7 +3616,7 @@
         <v>89</v>
       </c>
       <c r="H54" s="3">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I54" s="3">
         <v>2</v>

</xml_diff>

<commit_message>
Added Set Defaults command to mancala_games.pyw. Deleted most keys with default values from config files when writing them, except when writing the all_params.txt file. all_params.txt now contains the actual construction defaults. Re-ordered the game parameters for the config files. Added UI Defaults to the parameter help; when it is different than the construction default. Noted which parameters are required to be in config file in the parameters help. Updated ai_params UI default to match construction defaults.
</commit_message>
<xml_diff>
--- a/src/game_params.xlsx
+++ b/src/game_params.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Activity_Data\Mancala_github\MancalaGames\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D61BE2E8-1255-451A-A2B9-2845D2C19A20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2C6050F-E8F3-495D-AD47-E3143F958858}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="game_params" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="272">
   <si>
     <t>tab</t>
   </si>
@@ -84,9 +84,6 @@
   </si>
   <si>
     <t>Game</t>
-  </si>
-  <si>
-    <t>class</t>
   </si>
   <si>
     <t>Game Class</t>
@@ -501,9 +498,6 @@
     <t>player ai_params _</t>
   </si>
   <si>
-    <t>[1, 3, 5, 7]</t>
-  </si>
-  <si>
     <t>mcts_bias</t>
   </si>
   <si>
@@ -523,12 +517,6 @@
   </si>
   <si>
     <t>[1, 1, 1, 1]</t>
-  </si>
-  <si>
-    <t>[30, 50, 80, 110]</t>
-  </si>
-  <si>
-    <t>[400, 400, 400, 400]</t>
   </si>
   <si>
     <t>child_cvt</t>
@@ -811,18 +799,6 @@
 Either SOW_RULE of OWN_SOW_CAPT_ALL or SOW_SOW_CAPT_ALL includes the basic capture mechanisms.</t>
   </si>
   <si>
-    <t>Capture when the contents of the hole are less than or equal to capt_max.
-When selected with other basic capture mechanisms, the capture mechanism are ANDed (all must be true for capture). Basic capture mechanisms are: CAPT_MAX, CAPT_MIN, CAPT_ON and EVENS  with restrictions from OPPSIDECAPT, MOVEUNLOCK and not child holes of any type.
-MLAPS LAPPER sowing will stop the sowing on a final seed that would capture based on the selected basic capture mechanisms.
-Either SOW_RULE of OWN_SOW_CAPT_ALL or SOW_SOW_CAPT_ALL includes the basic capture mechanisms.</t>
-  </si>
-  <si>
-    <t>Capture when the contents of the hole are greater than or equal to capt_min.
-When selected with other basic capture mechanisms, the capture mechanism are ANDed (all must be true for capture). Basic capture mechanisms are: CAPT_MAX, CAPT_MIN, CAPT_ON and EVENS  with restrictions from OPPSIDECAPT, MOVEUNLOCK and not child holes of any type.
-MLAP LAPPER sowing will stop the sowing on a final seed that would capture based on the selected basic capture mechanisms.
-Either SOW_RULE of OWN_SOW_CAPT_ALL or SOW_SOW_CAPT_ALL includes the basic capture mechanisms.</t>
-  </si>
-  <si>
     <t>If the last sown seed is put in an empty hole, seeds on the opposite side of the board are captured. The capture of those seeds can be limited by CAPT_MAX, CAPT_MIN, CAPT_ON, EVENS, MOVEUNLOCK, OPPSIDECAPT. For example, crosscapt with evens will only capture when there are an even number of seeds in the opposite hole.
 SOW_RULE of either SOW_CAPT_ALL do not do this capture.</t>
   </si>
@@ -840,12 +816,6 @@
   </si>
   <si>
     <t>Holes in the game start each game and round locked. Captures may not be made from locked holes. Starting a sow from a hole unlocks it allowing future captures.</t>
-  </si>
-  <si>
-    <t>Capture when the contents of the hole is in the capt_on list. 
-When selected with other basic capture mechanisms, the capture mechanism are ANDed (all must be true for capture). Basic capture mechanisms are: CAPT_MAX, CAPT_MIN, CAPT_ON and EVENS   with restrictions from OPPSIDECAPT, MOVEUNLOCK and not child holes of any type.
-MLAP LAPPER sowing will stop the sowing on a final seed that would capture based on the selected basic capture mechanisms.
-Either SOWRULE of OWN_SOW_CAPT_ALL or SOW_SOW_CAPT_ALL includes the basic capture mechanisms.</t>
   </si>
   <si>
     <t>Rules to allow taking of more than otherwise captured or picked seeds:
@@ -995,6 +965,33 @@
   + Several values of SOW_RULE perform an operation after each lap sown: SOW_CLKD_DIV(_NR) closes the final hole and CHANGE_DIR_LAP changes the direction of sowing after each lap.
 - LAPPER_NEXT:  For lapper_next sowing, the number of seeds in the last sown hole of lap do not matter. Instead, if the hole after the last sown hole has any seeds, those seeds are used to continue sowing the next lap. Sowing continues until the hole after the lap's final seed is empty. There are games with other conditions for ending a multilap low such as making a capture or making a child.
   + A SOW_RULE of CHANGE_DIR_LAP changes the direction of sowing after each lap. SOW_BLKD_DIV(_NR) is not supported for LAPPER_NEXT.</t>
+  </si>
+  <si>
+    <t>Capture when the contents of the hole is in the capt_on list. The Mancala Games UI only has checkboxes for 1 to 5 seeds, but any number may be put into the configuration file.
+When selected with other basic capture mechanisms, the capture mechanism are ANDed (all must be true for capture). Basic capture mechanisms are: CAPT_MAX, CAPT_MIN, CAPT_ON and EVENS   with restrictions from OPPSIDECAPT, MOVEUNLOCK and not child holes of any type.
+MLAP LAPPER sowing will stop the sowing on a final seed that would capture based on the selected basic capture mechanisms.
+Either SOWRULE of OWN_SOW_CAPT_ALL or SOW_SOW_CAPT_ALL includes the basic capture mechanisms.</t>
+  </si>
+  <si>
+    <t>[100, 300, 500, 800]</t>
+  </si>
+  <si>
+    <t>[1, 1, 3, 5]</t>
+  </si>
+  <si>
+    <t>[300, 200, 100, 100]</t>
+  </si>
+  <si>
+    <t>Capture when the contents of the hole are greater than or equal to capt_min. Disable with 0 value.
+When selected with other basic capture mechanisms, the capture mechanism are ANDed (all must be true for capture). Basic capture mechanisms are: CAPT_MAX, CAPT_MIN, CAPT_ON and EVENS  with restrictions from OPPSIDECAPT, MOVEUNLOCK and not child holes of any type.
+MLAP LAPPER sowing will stop the sowing on a final seed that would capture based on the selected basic capture mechanisms.
+Either SOW_RULE of OWN_SOW_CAPT_ALL or SOW_SOW_CAPT_ALL includes the basic capture mechanisms.</t>
+  </si>
+  <si>
+    <t>Capture when the contents of the hole are less than or equal to capt_max.  Disable with 0 value.
+When selected with other basic capture mechanisms, the capture mechanism are ANDed (all must be true for capture). Basic capture mechanisms are: CAPT_MAX, CAPT_MIN, CAPT_ON and EVENS  with restrictions from OPPSIDECAPT, MOVEUNLOCK and not child holes of any type.
+MLAPS LAPPER sowing will stop the sowing on a final seed that would capture based on the selected basic capture mechanisms.
+Either SOW_RULE of OWN_SOW_CAPT_ALL or SOW_SOW_CAPT_ALL includes the basic capture mechanisms.</t>
   </si>
 </sst>
 </file>
@@ -1879,8 +1876,8 @@
   <dimension ref="A1:J70"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H54" sqref="H54"/>
+      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1911,7 +1908,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>4</v>
@@ -1929,59 +1926,59 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C2" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>64</v>
-      </c>
       <c r="D2" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E2" s="3">
-        <v>43</v>
+        <v>119</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>11</v>
       </c>
       <c r="G2" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="H2" s="3">
+        <v>0</v>
+      </c>
+      <c r="I2" s="3">
+        <v>0</v>
+      </c>
+      <c r="J2" s="4" t="s">
         <v>65</v>
-      </c>
-      <c r="H2" s="3">
-        <v>0</v>
-      </c>
-      <c r="I2" s="3">
-        <v>0</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>68</v>
-      </c>
       <c r="D3" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E3" s="3">
-        <v>51</v>
+        <v>126</v>
       </c>
       <c r="F3" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="G3" s="5" t="s">
         <v>41</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>42</v>
       </c>
       <c r="H3" s="3">
         <v>1</v>
@@ -1990,30 +1987,30 @@
         <v>0</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="345" x14ac:dyDescent="0.25">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="195" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E4" s="3">
-        <v>14</v>
+        <v>101</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="H4" s="3">
         <v>3</v>
@@ -2022,31 +2019,31 @@
         <v>0</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="C5" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>97</v>
-      </c>
       <c r="D5" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E5" s="3">
-        <v>16</v>
+        <v>103</v>
       </c>
       <c r="F5" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="G5" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="G5" s="5" t="s">
-        <v>42</v>
-      </c>
       <c r="H5" s="3">
         <v>0</v>
       </c>
@@ -2054,30 +2051,30 @@
         <v>0</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>99</v>
-      </c>
       <c r="D6" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E6" s="3">
-        <v>58</v>
+        <v>130</v>
       </c>
       <c r="F6" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="G6" s="5" t="s">
         <v>41</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>42</v>
       </c>
       <c r="H6" s="3">
         <v>1</v>
@@ -2086,30 +2083,30 @@
         <v>0</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>119</v>
-      </c>
       <c r="D7" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E7" s="3">
-        <v>49</v>
+        <v>124</v>
       </c>
       <c r="F7" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="G7" s="5" t="s">
         <v>41</v>
-      </c>
-      <c r="G7" s="5" t="s">
-        <v>42</v>
       </c>
       <c r="H7" s="3">
         <v>2</v>
@@ -2118,30 +2115,30 @@
         <v>0</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="150" x14ac:dyDescent="0.25">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B8" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>104</v>
-      </c>
       <c r="D8" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E8" s="3">
-        <v>33</v>
+        <v>114</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H8" s="3">
         <v>3</v>
@@ -2150,30 +2147,30 @@
         <v>0</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="165" x14ac:dyDescent="0.25">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B9" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>106</v>
-      </c>
       <c r="D9" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E9" s="3">
-        <v>17</v>
+        <v>104</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>11</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H9" s="3">
         <v>4</v>
@@ -2182,30 +2179,30 @@
         <v>0</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="165" x14ac:dyDescent="0.25">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B10" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>108</v>
-      </c>
       <c r="D10" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E10" s="3">
-        <v>18</v>
+        <v>105</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>11</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H10" s="3">
         <v>5</v>
@@ -2214,30 +2211,30 @@
         <v>0</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E11" s="3">
-        <v>19</v>
+        <v>106</v>
       </c>
       <c r="F11" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="G11" s="5" t="s">
         <v>41</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>42</v>
       </c>
       <c r="H11" s="3">
         <v>6</v>
@@ -2246,30 +2243,30 @@
         <v>0</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B12" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="C12" s="3" t="s">
-        <v>127</v>
-      </c>
       <c r="D12" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E12" s="3">
-        <v>22</v>
+        <v>109</v>
       </c>
       <c r="F12" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="G12" s="5" t="s">
         <v>41</v>
-      </c>
-      <c r="G12" s="5" t="s">
-        <v>42</v>
       </c>
       <c r="H12" s="3">
         <v>7</v>
@@ -2278,30 +2275,30 @@
         <v>0</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="105" x14ac:dyDescent="0.25">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B13" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="D13" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E13" s="3">
         <v>113</v>
       </c>
-      <c r="D13" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E13" s="3">
-        <v>29</v>
-      </c>
       <c r="F13" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="G13" s="5" t="s">
         <v>41</v>
-      </c>
-      <c r="G13" s="5" t="s">
-        <v>42</v>
       </c>
       <c r="H13" s="3">
         <v>0</v>
@@ -2310,30 +2307,30 @@
         <v>2</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E14" s="3">
-        <v>78</v>
+        <v>146</v>
       </c>
       <c r="F14" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="G14" s="5" t="s">
         <v>41</v>
-      </c>
-      <c r="G14" s="5" t="s">
-        <v>42</v>
       </c>
       <c r="H14" s="3">
         <v>1</v>
@@ -2342,30 +2339,30 @@
         <v>2</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="105" x14ac:dyDescent="0.25">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B15" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="C15" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="D15" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E15" s="3">
+        <v>147</v>
+      </c>
+      <c r="F15" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="D15" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E15" s="3">
-        <v>79</v>
-      </c>
-      <c r="F15" s="3" t="s">
+      <c r="G15" s="5" t="s">
         <v>116</v>
-      </c>
-      <c r="G15" s="5" t="s">
-        <v>117</v>
       </c>
       <c r="H15" s="3">
         <v>2</v>
@@ -2374,30 +2371,30 @@
         <v>2</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="240" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="165" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B16" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="D16" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E16" s="3">
+        <v>117</v>
+      </c>
+      <c r="F16" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="D16" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E16" s="3">
-        <v>37</v>
-      </c>
-      <c r="F16" s="3" t="s">
+      <c r="G16" s="5" t="s">
         <v>122</v>
-      </c>
-      <c r="G16" s="5" t="s">
-        <v>123</v>
       </c>
       <c r="H16" s="3">
         <v>3</v>
@@ -2406,30 +2403,30 @@
         <v>2</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B17" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C17" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="C17" s="3" t="s">
-        <v>102</v>
-      </c>
       <c r="D17" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E17" s="3">
-        <v>48</v>
+        <v>123</v>
       </c>
       <c r="F17" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="G17" s="5" t="s">
         <v>41</v>
-      </c>
-      <c r="G17" s="5" t="s">
-        <v>42</v>
       </c>
       <c r="H17" s="3">
         <v>4</v>
@@ -2438,30 +2435,30 @@
         <v>2</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B18" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="C18" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="C18" s="3" t="s">
-        <v>110</v>
-      </c>
       <c r="D18" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E18" s="3">
-        <v>57</v>
+        <v>129</v>
       </c>
       <c r="F18" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="G18" s="5" t="s">
         <v>41</v>
-      </c>
-      <c r="G18" s="5" t="s">
-        <v>42</v>
       </c>
       <c r="H18" s="3">
         <v>5</v>
@@ -2470,30 +2467,30 @@
         <v>2</v>
       </c>
       <c r="J18" s="4" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E19" s="3">
-        <v>56</v>
+        <v>128</v>
       </c>
       <c r="F19" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="G19" s="5" t="s">
         <v>41</v>
-      </c>
-      <c r="G19" s="5" t="s">
-        <v>42</v>
       </c>
       <c r="H19" s="3">
         <v>6</v>
@@ -2502,30 +2499,30 @@
         <v>2</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="150" x14ac:dyDescent="0.25">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B20" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="C20" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="C20" s="3" t="s">
-        <v>125</v>
-      </c>
       <c r="D20" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E20" s="3">
-        <v>20</v>
+        <v>107</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H20" s="3">
         <v>8</v>
@@ -2534,30 +2531,30 @@
         <v>2</v>
       </c>
       <c r="J20" s="4" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E21" s="3">
-        <v>21</v>
+        <v>108</v>
       </c>
       <c r="F21" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="G21" s="5" t="s">
         <v>41</v>
-      </c>
-      <c r="G21" s="5" t="s">
-        <v>42</v>
       </c>
       <c r="H21" s="3">
         <v>9</v>
@@ -2566,30 +2563,30 @@
         <v>2</v>
       </c>
       <c r="J21" s="4" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" ht="225" x14ac:dyDescent="0.25">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="135" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E22" s="3">
-        <v>59</v>
+        <v>131</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="H22" s="3">
         <v>10</v>
@@ -2598,62 +2595,62 @@
         <v>2</v>
       </c>
       <c r="J22" s="4" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E23" s="3">
+        <v>142</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="G23" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="H23" s="3">
+        <v>0</v>
+      </c>
+      <c r="I23" s="3">
+        <v>0</v>
+      </c>
+      <c r="J23" s="4" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B24" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B23" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E23" s="3">
-        <v>73</v>
-      </c>
-      <c r="F23" s="3" t="s">
+      <c r="C24" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E24" s="3">
+        <v>125</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="G24" s="5" t="s">
         <v>41</v>
-      </c>
-      <c r="G23" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="H23" s="3">
-        <v>0</v>
-      </c>
-      <c r="I23" s="3">
-        <v>0</v>
-      </c>
-      <c r="J23" s="4" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E24" s="3">
-        <v>50</v>
-      </c>
-      <c r="F24" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="G24" s="5" t="s">
-        <v>42</v>
       </c>
       <c r="H24" s="3">
         <v>1</v>
@@ -2662,30 +2659,30 @@
         <v>0</v>
       </c>
       <c r="J24" s="4" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="165" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B25" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C25" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C25" s="3" t="s">
-        <v>44</v>
-      </c>
       <c r="D25" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E25" s="3">
-        <v>64</v>
+        <v>135</v>
       </c>
       <c r="F25" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="G25" s="5" t="s">
         <v>41</v>
-      </c>
-      <c r="G25" s="5" t="s">
-        <v>42</v>
       </c>
       <c r="H25" s="3">
         <v>4</v>
@@ -2694,30 +2691,30 @@
         <v>0</v>
       </c>
       <c r="J25" s="4" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" ht="105" x14ac:dyDescent="0.25">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B26" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C26" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="D26" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E26" s="3">
+        <v>134</v>
+      </c>
+      <c r="F26" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="D26" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E26" s="3">
-        <v>63</v>
-      </c>
-      <c r="F26" s="3" t="s">
+      <c r="G26" s="5" t="s">
         <v>47</v>
-      </c>
-      <c r="G26" s="5" t="s">
-        <v>48</v>
       </c>
       <c r="H26" s="3">
         <v>5</v>
@@ -2726,30 +2723,30 @@
         <v>0</v>
       </c>
       <c r="J26" s="4" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" ht="409.5" x14ac:dyDescent="0.25">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="285" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E27" s="3">
-        <v>62</v>
+        <v>133</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="H27" s="3">
         <v>6</v>
@@ -2758,30 +2755,30 @@
         <v>0</v>
       </c>
       <c r="J27" s="4" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" ht="105" x14ac:dyDescent="0.25">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B28" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C28" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="C28" s="3" t="s">
-        <v>84</v>
-      </c>
       <c r="D28" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E28" s="3">
-        <v>15</v>
+        <v>102</v>
       </c>
       <c r="F28" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="G28" s="5" t="s">
         <v>41</v>
-      </c>
-      <c r="G28" s="5" t="s">
-        <v>42</v>
       </c>
       <c r="H28" s="3">
         <v>7</v>
@@ -2790,30 +2787,30 @@
         <v>0</v>
       </c>
       <c r="J28" s="4" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="255" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B29" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C29" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="C29" s="3" t="s">
+      <c r="D29" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E29" s="3">
+        <v>115</v>
+      </c>
+      <c r="F29" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D29" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E29" s="3">
-        <v>35</v>
-      </c>
-      <c r="F29" s="3" t="s">
+      <c r="G29" s="5" t="s">
         <v>56</v>
-      </c>
-      <c r="G29" s="5" t="s">
-        <v>57</v>
       </c>
       <c r="H29" s="3">
         <v>0</v>
@@ -2822,30 +2819,30 @@
         <v>2</v>
       </c>
       <c r="J29" s="4" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B30" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C30" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C30" s="3" t="s">
-        <v>50</v>
-      </c>
       <c r="D30" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E30" s="3">
-        <v>55</v>
+        <v>127</v>
       </c>
       <c r="F30" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="G30" s="5" t="s">
         <v>41</v>
-      </c>
-      <c r="G30" s="5" t="s">
-        <v>42</v>
       </c>
       <c r="H30" s="3">
         <v>1</v>
@@ -2854,30 +2851,30 @@
         <v>2</v>
       </c>
       <c r="J30" s="4" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" ht="210" x14ac:dyDescent="0.25">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" ht="165" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B31" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C31" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="C31" s="3" t="s">
+      <c r="D31" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E31" s="3">
+        <v>141</v>
+      </c>
+      <c r="F31" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="D31" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E31" s="3">
-        <v>72</v>
-      </c>
-      <c r="F31" s="3" t="s">
+      <c r="G31" s="5" t="s">
         <v>60</v>
-      </c>
-      <c r="G31" s="5" t="s">
-        <v>61</v>
       </c>
       <c r="H31" s="3">
         <v>2</v>
@@ -2886,30 +2883,30 @@
         <v>2</v>
       </c>
       <c r="J31" s="4" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" ht="285" x14ac:dyDescent="0.25">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" ht="240" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E32" s="3">
-        <v>60</v>
+        <v>132</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="G32" s="5" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="H32" s="3">
         <v>3</v>
@@ -2918,30 +2915,30 @@
         <v>2</v>
       </c>
       <c r="J32" s="4" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>256</v>
+        <v>249</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E33" s="3">
-        <v>36</v>
+        <v>116</v>
       </c>
       <c r="F33" s="3" t="s">
         <v>11</v>
       </c>
       <c r="G33" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H33" s="3">
         <v>5</v>
@@ -2950,7 +2947,7 @@
         <v>2</v>
       </c>
       <c r="J33" s="4" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
@@ -2958,31 +2955,31 @@
         <v>15</v>
       </c>
       <c r="B34" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C34" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C34" s="3" t="s">
+      <c r="D34" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D34" s="3" t="s">
-        <v>18</v>
-      </c>
       <c r="E34" s="3">
-        <v>28</v>
+        <v>1</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G34" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="H34" s="3">
+        <v>0</v>
+      </c>
+      <c r="I34" s="3">
+        <v>0</v>
+      </c>
+      <c r="J34" s="4" t="s">
         <v>20</v>
-      </c>
-      <c r="H34" s="3">
-        <v>0</v>
-      </c>
-      <c r="I34" s="3">
-        <v>0</v>
-      </c>
-      <c r="J34" s="4" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
@@ -2990,22 +2987,22 @@
         <v>15</v>
       </c>
       <c r="B35" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C35" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C35" s="3" t="s">
+      <c r="D35" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D35" s="3" t="s">
-        <v>33</v>
-      </c>
       <c r="E35" s="3">
-        <v>39</v>
+        <v>2</v>
       </c>
       <c r="F35" s="3" t="s">
         <v>11</v>
       </c>
       <c r="G35" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H35" s="3">
         <v>2</v>
@@ -3014,30 +3011,30 @@
         <v>0</v>
       </c>
       <c r="J35" s="4" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B36" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C36" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C36" s="3" t="s">
+      <c r="D36" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E36" s="3">
+        <v>118</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G36" s="5" t="s">
         <v>26</v>
-      </c>
-      <c r="D36" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E36" s="3">
-        <v>38</v>
-      </c>
-      <c r="F36" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G36" s="5" t="s">
-        <v>27</v>
       </c>
       <c r="H36" s="3">
         <v>3</v>
@@ -3046,7 +3043,7 @@
         <v>0</v>
       </c>
       <c r="J36" s="4" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
     </row>
     <row r="37" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -3054,22 +3051,22 @@
         <v>15</v>
       </c>
       <c r="B37" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C37" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C37" s="3" t="s">
+      <c r="D37" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E37" s="3">
+        <v>5</v>
+      </c>
+      <c r="F37" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D37" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E37" s="3">
-        <v>2</v>
-      </c>
-      <c r="F37" s="3" t="s">
-        <v>30</v>
-      </c>
       <c r="G37" s="6" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H37" s="3">
         <v>4</v>
@@ -3078,30 +3075,30 @@
         <v>0</v>
       </c>
       <c r="J37" s="4" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B38" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C38" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C38" s="3" t="s">
-        <v>23</v>
-      </c>
       <c r="D38" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E38" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F38" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G38" s="5" t="s">
         <v>19</v>
-      </c>
-      <c r="G38" s="5" t="s">
-        <v>20</v>
       </c>
       <c r="H38" s="3">
         <v>0</v>
@@ -3110,30 +3107,30 @@
         <v>2</v>
       </c>
       <c r="J38" s="4" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B39" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C39" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C39" s="3" t="s">
-        <v>36</v>
-      </c>
       <c r="D39" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E39" s="3">
-        <v>54</v>
+        <v>3</v>
       </c>
       <c r="F39" s="3" t="s">
         <v>11</v>
       </c>
       <c r="G39" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H39" s="3">
         <v>2</v>
@@ -3142,31 +3139,31 @@
         <v>2</v>
       </c>
       <c r="J39" s="4" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
     </row>
     <row r="40" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B40" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="C40" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="C40" s="3" t="s">
+      <c r="D40" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="E40" s="3">
+        <v>201</v>
+      </c>
+      <c r="F40" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="G40" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="D40" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="E40" s="3">
-        <v>13</v>
-      </c>
-      <c r="F40" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="G40" s="3" t="s">
-        <v>148</v>
-      </c>
       <c r="H40" s="3">
         <v>0</v>
       </c>
@@ -3174,30 +3171,30 @@
         <v>0</v>
       </c>
       <c r="J40" s="4" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B41" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="C41" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="C41" s="3" t="s">
+      <c r="D41" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="D41" s="3" t="s">
-        <v>141</v>
-      </c>
       <c r="E41" s="3">
-        <v>30</v>
+        <v>203</v>
       </c>
       <c r="F41" s="3" t="s">
         <v>11</v>
       </c>
       <c r="G41" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H41" s="3">
         <v>1</v>
@@ -3206,30 +3203,30 @@
         <v>0</v>
       </c>
       <c r="J41" s="4" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E42" s="3">
-        <v>12</v>
+        <v>202</v>
       </c>
       <c r="F42" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="G42" s="5" t="s">
         <v>41</v>
-      </c>
-      <c r="G42" s="5" t="s">
-        <v>42</v>
       </c>
       <c r="H42" s="3">
         <v>2</v>
@@ -3238,30 +3235,30 @@
         <v>0</v>
       </c>
       <c r="J42" s="4" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B43" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="C43" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="C43" s="3" t="s">
+      <c r="D43" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="D43" s="3" t="s">
-        <v>152</v>
-      </c>
       <c r="E43" s="3">
-        <v>46</v>
+        <v>213</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>153</v>
+        <v>268</v>
       </c>
       <c r="H43" s="3">
         <v>4</v>
@@ -3270,30 +3267,30 @@
         <v>0</v>
       </c>
       <c r="J43" s="4" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E44" s="3">
-        <v>40</v>
+        <v>210</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>162</v>
+        <v>269</v>
       </c>
       <c r="H44" s="3">
         <v>6</v>
@@ -3302,30 +3299,30 @@
         <v>0</v>
       </c>
       <c r="J44" s="4" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B45" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="C45" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="C45" s="3" t="s">
-        <v>157</v>
-      </c>
       <c r="D45" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E45" s="3">
-        <v>41</v>
+        <v>211</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>161</v>
+        <v>267</v>
       </c>
       <c r="H45" s="3">
         <v>7</v>
@@ -3334,30 +3331,30 @@
         <v>0</v>
       </c>
       <c r="J45" s="4" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E46" s="3">
-        <v>42</v>
+        <v>212</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="H46" s="3">
         <v>8</v>
@@ -3366,30 +3363,30 @@
         <v>0</v>
       </c>
       <c r="J46" s="4" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
     </row>
     <row r="47" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="B47" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="B47" s="3" t="s">
+      <c r="C47" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="D47" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="C47" s="3" t="s">
-        <v>267</v>
-      </c>
-      <c r="D47" s="3" t="s">
-        <v>130</v>
-      </c>
       <c r="E47" s="3">
-        <v>74</v>
+        <v>220</v>
       </c>
       <c r="F47" s="3" t="s">
         <v>11</v>
       </c>
       <c r="G47" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H47" s="3">
         <v>0</v>
@@ -3398,30 +3395,30 @@
         <v>2</v>
       </c>
       <c r="J47" s="4" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
     </row>
     <row r="48" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>266</v>
+        <v>259</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E48" s="3">
-        <v>11</v>
+        <v>221</v>
       </c>
       <c r="F48" s="3" t="s">
         <v>11</v>
       </c>
       <c r="G48" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H48" s="3">
         <v>1</v>
@@ -3430,30 +3427,30 @@
         <v>2</v>
       </c>
       <c r="J48" s="4" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
     </row>
     <row r="49" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>265</v>
+        <v>258</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E49" s="3">
-        <v>66</v>
+        <v>222</v>
       </c>
       <c r="F49" s="3" t="s">
         <v>11</v>
       </c>
       <c r="G49" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H49" s="3">
         <v>2</v>
@@ -3462,30 +3459,30 @@
         <v>2</v>
       </c>
       <c r="J49" s="4" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
     </row>
     <row r="50" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>264</v>
+        <v>257</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E50" s="3">
-        <v>32</v>
+        <v>223</v>
       </c>
       <c r="F50" s="3" t="s">
         <v>11</v>
       </c>
       <c r="G50" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H50" s="3">
         <v>3</v>
@@ -3494,30 +3491,30 @@
         <v>2</v>
       </c>
       <c r="J50" s="4" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
     </row>
     <row r="51" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E51" s="3">
-        <v>25</v>
+        <v>224</v>
       </c>
       <c r="F51" s="3" t="s">
         <v>11</v>
       </c>
       <c r="G51" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H51" s="3">
         <v>4</v>
@@ -3526,30 +3523,30 @@
         <v>2</v>
       </c>
       <c r="J51" s="4" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
     </row>
     <row r="52" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E52" s="3">
-        <v>34</v>
+        <v>225</v>
       </c>
       <c r="F52" s="3" t="s">
         <v>11</v>
       </c>
       <c r="G52" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H52" s="3">
         <v>5</v>
@@ -3558,71 +3555,71 @@
         <v>2</v>
       </c>
       <c r="J52" s="4" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
     </row>
     <row r="53" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>137</v>
+        <v>255</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E53" s="3">
-        <v>31</v>
+        <v>226</v>
       </c>
       <c r="F53" s="3" t="s">
         <v>11</v>
       </c>
       <c r="G53" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H53" s="3">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I53" s="3">
         <v>2</v>
       </c>
       <c r="J53" s="4" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="54" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>262</v>
+        <v>136</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E54" s="3">
-        <v>61</v>
+        <v>227</v>
       </c>
       <c r="F54" s="3" t="s">
         <v>11</v>
       </c>
       <c r="G54" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H54" s="3">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I54" s="3">
         <v>2</v>
       </c>
       <c r="J54" s="4" t="s">
-        <v>233</v>
+        <v>224</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
@@ -3630,13 +3627,13 @@
         <v>9</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E55" s="3">
-        <v>45</v>
+        <v>121</v>
       </c>
       <c r="F55" s="3" t="s">
         <v>11</v>
@@ -3648,7 +3645,7 @@
         <v>0</v>
       </c>
       <c r="J55" s="4" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
@@ -3656,14 +3653,18 @@
         <v>9</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>10</v>
+        <v>93</v>
+      </c>
+      <c r="D56" s="3" t="s">
+        <v>23</v>
       </c>
       <c r="E56" s="3">
-        <v>53</v>
+        <v>144</v>
       </c>
       <c r="F56" s="3" t="s">
-        <v>11</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="G56" s="5"/>
       <c r="H56" s="3">
         <v>0</v>
       </c>
@@ -3671,7 +3672,7 @@
         <v>0</v>
       </c>
       <c r="J56" s="4" t="s">
-        <v>12</v>
+        <v>174</v>
       </c>
     </row>
     <row r="57" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3682,7 +3683,7 @@
         <v>13</v>
       </c>
       <c r="E57" s="3">
-        <v>65</v>
+        <v>500</v>
       </c>
       <c r="F57" s="3" t="s">
         <v>14</v>
@@ -3694,7 +3695,7 @@
         <v>0</v>
       </c>
       <c r="J57" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
@@ -3702,18 +3703,14 @@
         <v>9</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="D58" s="3" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="E58" s="3">
-        <v>76</v>
+        <v>501</v>
       </c>
       <c r="F58" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="G58" s="5"/>
+        <v>11</v>
+      </c>
       <c r="H58" s="3">
         <v>0</v>
       </c>
@@ -3721,31 +3718,31 @@
         <v>0</v>
       </c>
       <c r="J58" s="4" t="s">
-        <v>178</v>
+        <v>12</v>
       </c>
     </row>
     <row r="59" spans="1:10" ht="210" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B59" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="B59" s="3" t="s">
+      <c r="C59" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="C59" s="3" t="s">
+      <c r="D59" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E59" s="3">
+        <v>137</v>
+      </c>
+      <c r="F59" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="D59" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E59" s="3">
-        <v>68</v>
-      </c>
-      <c r="F59" s="3" t="s">
+      <c r="G59" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="G59" s="5" t="s">
-        <v>73</v>
-      </c>
       <c r="H59" s="3">
         <v>0</v>
       </c>
@@ -3753,30 +3750,30 @@
         <v>0</v>
       </c>
       <c r="J59" s="4" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B60" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C60" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="C60" s="3" t="s">
-        <v>75</v>
-      </c>
       <c r="D60" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E60" s="3">
-        <v>71</v>
+        <v>140</v>
       </c>
       <c r="F60" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="G60" s="5" t="s">
         <v>41</v>
-      </c>
-      <c r="G60" s="5" t="s">
-        <v>42</v>
       </c>
       <c r="H60" s="3">
         <v>1</v>
@@ -3785,30 +3782,30 @@
         <v>0</v>
       </c>
       <c r="J60" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="61" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B61" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C61" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="C61" s="3" t="s">
-        <v>80</v>
-      </c>
       <c r="D61" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E61" s="3">
-        <v>67</v>
+        <v>136</v>
       </c>
       <c r="F61" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="G61" s="5" t="s">
         <v>41</v>
-      </c>
-      <c r="G61" s="5" t="s">
-        <v>42</v>
       </c>
       <c r="H61" s="3">
         <v>2</v>
@@ -3817,30 +3814,30 @@
         <v>0</v>
       </c>
       <c r="J61" s="4" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
     </row>
     <row r="62" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B62" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C62" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="C62" s="3" t="s">
-        <v>82</v>
-      </c>
       <c r="D62" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E62" s="3">
-        <v>69</v>
+        <v>138</v>
       </c>
       <c r="F62" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="G62" s="5" t="s">
         <v>41</v>
-      </c>
-      <c r="G62" s="5" t="s">
-        <v>42</v>
       </c>
       <c r="H62" s="3">
         <v>3</v>
@@ -3849,30 +3846,30 @@
         <v>0</v>
       </c>
       <c r="J62" s="4" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
     </row>
     <row r="63" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B63" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C63" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="C63" s="3" t="s">
-        <v>78</v>
-      </c>
       <c r="D63" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E63" s="3">
-        <v>47</v>
+        <v>122</v>
       </c>
       <c r="F63" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="G63" s="5" t="s">
         <v>41</v>
-      </c>
-      <c r="G63" s="5" t="s">
-        <v>42</v>
       </c>
       <c r="H63" s="3">
         <v>5</v>
@@ -3881,30 +3878,30 @@
         <v>0</v>
       </c>
       <c r="J63" s="4" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
     </row>
     <row r="64" spans="1:10" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E64" s="3">
-        <v>70</v>
+        <v>139</v>
       </c>
       <c r="F64" s="3" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="G64" s="5" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="H64" s="3">
         <v>6</v>
@@ -3913,30 +3910,30 @@
         <v>0</v>
       </c>
       <c r="J64" s="4" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
     </row>
     <row r="65" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B65" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C65" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="C65" s="3" t="s">
-        <v>91</v>
-      </c>
       <c r="D65" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E65" s="3">
-        <v>75</v>
+        <v>143</v>
       </c>
       <c r="F65" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G65" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H65" s="3">
         <v>8</v>
@@ -3945,30 +3942,30 @@
         <v>0</v>
       </c>
       <c r="J65" s="4" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
     </row>
     <row r="66" spans="1:10" ht="210" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B66" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C66" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="C66" s="3" t="s">
-        <v>86</v>
-      </c>
       <c r="D66" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E66" s="3">
-        <v>44</v>
+        <v>120</v>
       </c>
       <c r="F66" s="3" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="G66" s="5" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="H66" s="3">
         <v>0</v>
@@ -3977,30 +3974,30 @@
         <v>2</v>
       </c>
       <c r="J66" s="8" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B67" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C67" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="C67" s="3" t="s">
-        <v>88</v>
-      </c>
       <c r="D67" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E67" s="3">
-        <v>77</v>
+        <v>145</v>
       </c>
       <c r="F67" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="G67" s="5" t="s">
         <v>41</v>
-      </c>
-      <c r="G67" s="5" t="s">
-        <v>42</v>
       </c>
       <c r="H67" s="3">
         <v>1</v>
@@ -4009,30 +4006,30 @@
         <v>2</v>
       </c>
       <c r="J67" s="4" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
     </row>
     <row r="68" spans="1:10" ht="285" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E68" s="3">
-        <v>27</v>
+        <v>112</v>
       </c>
       <c r="F68" s="3" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="G68" s="5" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="H68" s="3">
         <v>3</v>
@@ -4041,30 +4038,30 @@
         <v>2</v>
       </c>
       <c r="J68" s="4" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
     </row>
     <row r="69" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E69" s="3">
-        <v>26</v>
+        <v>110</v>
       </c>
       <c r="F69" s="3" t="s">
         <v>11</v>
       </c>
       <c r="G69" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H69" s="3">
         <v>4</v>
@@ -4073,30 +4070,30 @@
         <v>2</v>
       </c>
       <c r="J69" s="4" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="70" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E70" s="3">
-        <v>24</v>
+        <v>111</v>
       </c>
       <c r="F70" s="3" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="G70" s="3" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="H70" s="3">
         <v>5</v>
@@ -4105,7 +4102,7 @@
         <v>2</v>
       </c>
       <c r="J70" s="4" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Made grand slam with pickers behave consistently. Updated docs to clarify behavior of gs with pickers. Check locks for PickLastSeeds. Don't log Picked if we didn't actually pick seeds. Added some cross capture and picker rules. Added tests to test_cmp_allow.py and test_cmp_capt.py.
</commit_message>
<xml_diff>
--- a/src/game_params.xlsx
+++ b/src/game_params.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Activity_Data\Mancala_github\MancalaGames\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2C6050F-E8F3-495D-AD47-E3143F958858}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AE5F7D0-9F40-46C5-BD81-D56B0AB0CD18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="game_params" sheetId="1" r:id="rId1"/>
@@ -465,12 +465,6 @@
 Capture on evens. </t>
   </si>
   <si>
-    <t>When crosscapt is set, defines what to do with the single seed initiating the cross capture.
-- LEAVE: always leave the signle seed
-- PICK_ON_CAPTURE: only pick (capture) the seed if there was a capture.
-- ALWAYS_PICK: always pick (capture) the seed, even if there was not a capture"</t>
-  </si>
-  <si>
     <t>An init only parameter that used to check the consistency of the game info. Errors and warnings are raised as the rules are processed.</t>
   </si>
   <si>
@@ -701,15 +695,6 @@
     <t>Only valid when SOW_START is set. Changes the SOW_START behavior so that if there is only one seed in the hole, it is moved in the sow direction by one hole.</t>
   </si>
   <si>
-    <t>A grandslam is when your opponent has seeds at the start of your turn and you capture them all. This option selects what to do:
-- LEGAL: the seeds are captured
-- NOT_LEGAL: you may not capture all of your opponents seeds, a move which would do so is not allowed
-- NO_CAPT: you may sow the seeds, but the capture is not performed
-- OPP_GETS_REMAIN: if you capture all your opponents seeds, they capture all of your remaining seeds and the game is over. Winner is determined by game goal.
-- LEAVE_LEFT: the capture is performed from all but the leftmost hole from the sower perspective. This might leave your oppenents without seeds or might not capture any seeds.
-- LEAVE_RIGHT: the capture is performed from all but the rightmost hole from the sower perspective. This might leave your oppenents without seeds.</t>
-  </si>
-  <si>
     <t>Repeat turn if there was a capture. Making children is not a capture.</t>
   </si>
   <si>
@@ -816,14 +801,6 @@
   </si>
   <si>
     <t>Holes in the game start each game and round locked. Captures may not be made from locked holes. Starting a sow from a hole unlocks it allowing future captures.</t>
-  </si>
-  <si>
-    <t>Rules to allow taking of more than otherwise captured or picked seeds:
-- NONE: Nothing extra
-- PICKCROSS: Take the seeds from the opposite side of the board. 
-- PICKTWOS: Take seeds from all holes containing two seeds but only after the first move.
-- PICKLASTSEEDS: If there are the number of starts seeds or fewer left,  the current player collects them and the game is over. This rule is applied at the end of each turn, even if there is not a capture because the sow phase may have reduced the seed count.
-- PICK2XLASTSEEDS: If there are 2 times the number of start seeds or fewer, the round starter picks them. This rule is applied at the end of each turn, even if there is not a capture because the sow phase may have reduced the seed count.</t>
   </si>
   <si>
     <t xml:space="preserve">Requires MLAPS. If the first 'lap' does not reach the opponent's side of the board, the sowing ends after the first lap. </t>
@@ -992,6 +969,30 @@
 When selected with other basic capture mechanisms, the capture mechanism are ANDed (all must be true for capture). Basic capture mechanisms are: CAPT_MAX, CAPT_MIN, CAPT_ON and EVENS  with restrictions from OPPSIDECAPT, MOVEUNLOCK and not child holes of any type.
 MLAPS LAPPER sowing will stop the sowing on a final seed that would capture based on the selected basic capture mechanisms.
 Either SOW_RULE of OWN_SOW_CAPT_ALL or SOW_SOW_CAPT_ALL includes the basic capture mechanisms.</t>
+  </si>
+  <si>
+    <t>When crosscapt is set, defines what to do with the single seed initiating the cross capture.
+- LEAVE: always leave the signle seed
+- PICK_ON_CAPT: only pick (capture) the seed if there was a capture
+- ALWAYS_PICK: always pick (capture) the final single seed, even if there was not a capture</t>
+  </si>
+  <si>
+    <t>Rules to allow taking of more than otherwise captured or picked seeds:
+- NONE: Nothing extra
+- PICKCROSS: Take the seeds from the opposite side of the board. 
+- PICKTWOS: Take seeds from opponents holes containing two seeds.
+- PICKLASTSEEDS: If there are the number of starts seeds or fewer left,  the current player collects them and the game is over. This rule is applied at the end of each turn, even if there is not a capture because the sow phase may have reduced the seed count.
+- PICK2XLASTSEEDS: If there are 2 times the number of start seeds or fewer, the round starter picks them. This rule is applied at the end of each turn, even if there is not a capture because the sow phase may have reduced the seed count.
+In terms of GRANDSLAM, these picks are considered captures.</t>
+  </si>
+  <si>
+    <t>A grandslam is when your opponent has seeds at the start of your turn and you capture them all. This option selects what to do:
+- LEGAL: the seeds are captured
+- NOT_LEGAL: you may not capture all of your opponents seeds, a move which would do so is not allowed
+- NO_CAPT: you may sow the seeds, but the capture is not performed
+- OPP_GETS_REMAIN: if you capture all your opponents seeds, they capture all of your remaining seeds and the game is over. Winner is determined by game goal. Seeds picked because of PICKEXTRA PICK*LASTSEEDS go the current player and not the opponent.
+- LEAVE_LEFT: the capture is performed from all but the leftmost hole from the sower perspective. This might leave your oppenents without seeds or might not capture any seeds.
+- LEAVE_RIGHT: the capture is performed from all but the rightmost hole from the sower perspective. This might leave your oppenents without seeds.</t>
   </si>
 </sst>
 </file>
@@ -1877,7 +1878,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J9" sqref="J9"/>
+      <selection pane="bottomLeft" activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1908,7 +1909,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>4</v>
@@ -1987,7 +1988,7 @@
         <v>0</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="195" x14ac:dyDescent="0.25">
@@ -1995,10 +1996,10 @@
         <v>61</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>166</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>167</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>23</v>
@@ -2007,10 +2008,10 @@
         <v>101</v>
       </c>
       <c r="F4" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="G4" s="5" t="s">
         <v>168</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>169</v>
       </c>
       <c r="H4" s="3">
         <v>3</v>
@@ -2019,7 +2020,7 @@
         <v>0</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2051,7 +2052,7 @@
         <v>0</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -2115,7 +2116,7 @@
         <v>0</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -2147,7 +2148,7 @@
         <v>0</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="105" x14ac:dyDescent="0.25">
@@ -2179,7 +2180,7 @@
         <v>0</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="105" x14ac:dyDescent="0.25">
@@ -2211,7 +2212,7 @@
         <v>0</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2219,10 +2220,10 @@
         <v>94</v>
       </c>
       <c r="B11" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>178</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>179</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>23</v>
@@ -2243,7 +2244,7 @@
         <v>0</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="120" x14ac:dyDescent="0.25">
@@ -2275,7 +2276,7 @@
         <v>0</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -2307,7 +2308,7 @@
         <v>2</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2315,10 +2316,10 @@
         <v>94</v>
       </c>
       <c r="B14" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>190</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>191</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>23</v>
@@ -2339,7 +2340,7 @@
         <v>2</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -2371,10 +2372,10 @@
         <v>2</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="165" x14ac:dyDescent="0.25">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="180" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>94</v>
       </c>
@@ -2403,7 +2404,7 @@
         <v>2</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>214</v>
+        <v>271</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2435,7 +2436,7 @@
         <v>2</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
@@ -2475,10 +2476,10 @@
         <v>94</v>
       </c>
       <c r="B19" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="C19" s="3" t="s">
         <v>201</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>202</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>23</v>
@@ -2499,7 +2500,7 @@
         <v>2</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="120" x14ac:dyDescent="0.25">
@@ -2519,7 +2520,7 @@
         <v>107</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G20" s="5" t="s">
         <v>92</v>
@@ -2531,7 +2532,7 @@
         <v>2</v>
       </c>
       <c r="J20" s="4" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -2539,10 +2540,10 @@
         <v>94</v>
       </c>
       <c r="B21" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="C21" s="3" t="s">
         <v>176</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>177</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>23</v>
@@ -2563,18 +2564,18 @@
         <v>2</v>
       </c>
       <c r="J21" s="4" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" ht="135" x14ac:dyDescent="0.25">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="150" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>94</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>23</v>
@@ -2583,10 +2584,10 @@
         <v>131</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H22" s="3">
         <v>10</v>
@@ -2595,7 +2596,7 @@
         <v>2</v>
       </c>
       <c r="J22" s="4" t="s">
-        <v>239</v>
+        <v>270</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
@@ -2627,7 +2628,7 @@
         <v>0</v>
       </c>
       <c r="J23" s="4" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -2659,7 +2660,7 @@
         <v>0</v>
       </c>
       <c r="J24" s="4" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="165" x14ac:dyDescent="0.25">
@@ -2691,7 +2692,7 @@
         <v>0</v>
       </c>
       <c r="J25" s="4" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -2723,7 +2724,7 @@
         <v>0</v>
       </c>
       <c r="J26" s="4" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="285" x14ac:dyDescent="0.25">
@@ -2731,10 +2732,10 @@
         <v>37</v>
       </c>
       <c r="B27" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="C27" s="3" t="s">
         <v>192</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>193</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>23</v>
@@ -2743,10 +2744,10 @@
         <v>133</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="H27" s="3">
         <v>6</v>
@@ -2755,7 +2756,7 @@
         <v>0</v>
       </c>
       <c r="J27" s="4" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -2787,7 +2788,7 @@
         <v>0</v>
       </c>
       <c r="J28" s="4" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="255" x14ac:dyDescent="0.25">
@@ -2819,7 +2820,7 @@
         <v>2</v>
       </c>
       <c r="J29" s="4" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2851,7 +2852,7 @@
         <v>2</v>
       </c>
       <c r="J30" s="4" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
     </row>
     <row r="31" spans="1:10" ht="165" x14ac:dyDescent="0.25">
@@ -2883,7 +2884,7 @@
         <v>2</v>
       </c>
       <c r="J31" s="4" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="240" x14ac:dyDescent="0.25">
@@ -2891,10 +2892,10 @@
         <v>37</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D32" s="3" t="s">
         <v>23</v>
@@ -2903,10 +2904,10 @@
         <v>132</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G32" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H32" s="3">
         <v>3</v>
@@ -2915,7 +2916,7 @@
         <v>2</v>
       </c>
       <c r="J32" s="4" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2923,10 +2924,10 @@
         <v>37</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="D33" s="3" t="s">
         <v>23</v>
@@ -2947,7 +2948,7 @@
         <v>2</v>
       </c>
       <c r="J33" s="4" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
@@ -2967,7 +2968,7 @@
         <v>1</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G34" s="5" t="s">
         <v>19</v>
@@ -3011,7 +3012,7 @@
         <v>0</v>
       </c>
       <c r="J35" s="4" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
@@ -3043,7 +3044,7 @@
         <v>0</v>
       </c>
       <c r="J36" s="4" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="37" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -3075,7 +3076,7 @@
         <v>0</v>
       </c>
       <c r="J37" s="4" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
@@ -3107,7 +3108,7 @@
         <v>2</v>
       </c>
       <c r="J38" s="4" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="39" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3139,7 +3140,7 @@
         <v>2</v>
       </c>
       <c r="J39" s="4" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="40" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -3147,10 +3148,10 @@
         <v>127</v>
       </c>
       <c r="B40" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="C40" s="3" t="s">
         <v>145</v>
-      </c>
-      <c r="C40" s="3" t="s">
-        <v>146</v>
       </c>
       <c r="D40" s="3" t="s">
         <v>140</v>
@@ -3159,11 +3160,11 @@
         <v>201</v>
       </c>
       <c r="F40" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="G40" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="G40" s="3" t="s">
-        <v>147</v>
-      </c>
       <c r="H40" s="3">
         <v>0</v>
       </c>
@@ -3171,7 +3172,7 @@
         <v>0</v>
       </c>
       <c r="J40" s="4" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
@@ -3203,7 +3204,7 @@
         <v>0</v>
       </c>
       <c r="J41" s="4" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="42" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3211,10 +3212,10 @@
         <v>127</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D42" s="3" t="s">
         <v>140</v>
@@ -3235,7 +3236,7 @@
         <v>0</v>
       </c>
       <c r="J42" s="4" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
@@ -3243,13 +3244,13 @@
         <v>127</v>
       </c>
       <c r="B43" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="C43" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="C43" s="3" t="s">
+      <c r="D43" s="3" t="s">
         <v>150</v>
-      </c>
-      <c r="D43" s="3" t="s">
-        <v>151</v>
       </c>
       <c r="E43" s="3">
         <v>213</v>
@@ -3258,7 +3259,7 @@
         <v>91</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="H43" s="3">
         <v>4</v>
@@ -3267,7 +3268,7 @@
         <v>0</v>
       </c>
       <c r="J43" s="4" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -3275,13 +3276,13 @@
         <v>127</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E44" s="3">
         <v>210</v>
@@ -3290,7 +3291,7 @@
         <v>91</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="H44" s="3">
         <v>6</v>
@@ -3299,7 +3300,7 @@
         <v>0</v>
       </c>
       <c r="J44" s="4" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
@@ -3307,13 +3308,13 @@
         <v>127</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E45" s="3">
         <v>211</v>
@@ -3322,7 +3323,7 @@
         <v>91</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="H45" s="3">
         <v>7</v>
@@ -3331,7 +3332,7 @@
         <v>0</v>
       </c>
       <c r="J45" s="4" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
@@ -3339,13 +3340,13 @@
         <v>127</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E46" s="3">
         <v>212</v>
@@ -3354,7 +3355,7 @@
         <v>91</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H46" s="3">
         <v>8</v>
@@ -3363,7 +3364,7 @@
         <v>0</v>
       </c>
       <c r="J46" s="4" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="47" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -3374,7 +3375,7 @@
         <v>128</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="D47" s="3" t="s">
         <v>129</v>
@@ -3395,7 +3396,7 @@
         <v>2</v>
       </c>
       <c r="J47" s="4" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="48" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -3406,7 +3407,7 @@
         <v>130</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="D48" s="3" t="s">
         <v>129</v>
@@ -3427,7 +3428,7 @@
         <v>2</v>
       </c>
       <c r="J48" s="4" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="49" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -3438,7 +3439,7 @@
         <v>131</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="D49" s="3" t="s">
         <v>129</v>
@@ -3459,7 +3460,7 @@
         <v>2</v>
       </c>
       <c r="J49" s="4" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="50" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3470,7 +3471,7 @@
         <v>132</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="D50" s="3" t="s">
         <v>129</v>
@@ -3491,7 +3492,7 @@
         <v>2</v>
       </c>
       <c r="J50" s="4" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="51" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -3502,7 +3503,7 @@
         <v>133</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="D51" s="3" t="s">
         <v>129</v>
@@ -3523,7 +3524,7 @@
         <v>2</v>
       </c>
       <c r="J51" s="4" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="52" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -3534,7 +3535,7 @@
         <v>134</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="D52" s="3" t="s">
         <v>129</v>
@@ -3555,7 +3556,7 @@
         <v>2</v>
       </c>
       <c r="J52" s="4" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="53" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -3566,7 +3567,7 @@
         <v>137</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="D53" s="3" t="s">
         <v>129</v>
@@ -3587,7 +3588,7 @@
         <v>2</v>
       </c>
       <c r="J53" s="4" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="54" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -3619,7 +3620,7 @@
         <v>2</v>
       </c>
       <c r="J54" s="4" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
@@ -3627,7 +3628,7 @@
         <v>9</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D55" s="3" t="s">
         <v>23</v>
@@ -3645,7 +3646,7 @@
         <v>0</v>
       </c>
       <c r="J55" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
@@ -3672,7 +3673,7 @@
         <v>0</v>
       </c>
       <c r="J56" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="57" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3695,7 +3696,7 @@
         <v>0</v>
       </c>
       <c r="J57" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
@@ -3750,7 +3751,7 @@
         <v>0</v>
       </c>
       <c r="J59" s="4" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
@@ -3814,7 +3815,7 @@
         <v>0</v>
       </c>
       <c r="J61" s="4" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="62" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3846,7 +3847,7 @@
         <v>0</v>
       </c>
       <c r="J62" s="4" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
     </row>
     <row r="63" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3878,7 +3879,7 @@
         <v>0</v>
       </c>
       <c r="J63" s="4" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="64" spans="1:10" ht="409.5" x14ac:dyDescent="0.25">
@@ -3886,10 +3887,10 @@
         <v>68</v>
       </c>
       <c r="B64" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="C64" s="3" t="s">
         <v>184</v>
-      </c>
-      <c r="C64" s="3" t="s">
-        <v>185</v>
       </c>
       <c r="D64" s="3" t="s">
         <v>23</v>
@@ -3898,10 +3899,10 @@
         <v>139</v>
       </c>
       <c r="F64" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G64" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H64" s="3">
         <v>6</v>
@@ -3910,7 +3911,7 @@
         <v>0</v>
       </c>
       <c r="J64" s="4" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
     </row>
     <row r="65" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -3930,7 +3931,7 @@
         <v>143</v>
       </c>
       <c r="F65" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G65" s="5" t="s">
         <v>92</v>
@@ -3942,7 +3943,7 @@
         <v>0</v>
       </c>
       <c r="J65" s="4" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="66" spans="1:10" ht="210" x14ac:dyDescent="0.25">
@@ -3962,10 +3963,10 @@
         <v>120</v>
       </c>
       <c r="F66" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="G66" s="5" t="s">
         <v>170</v>
-      </c>
-      <c r="G66" s="5" t="s">
-        <v>171</v>
       </c>
       <c r="H66" s="3">
         <v>0</v>
@@ -3974,7 +3975,7 @@
         <v>2</v>
       </c>
       <c r="J66" s="8" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.25">
@@ -4006,7 +4007,7 @@
         <v>2</v>
       </c>
       <c r="J67" s="4" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
     </row>
     <row r="68" spans="1:10" ht="285" x14ac:dyDescent="0.25">
@@ -4014,10 +4015,10 @@
         <v>68</v>
       </c>
       <c r="B68" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="C68" s="3" t="s">
         <v>161</v>
-      </c>
-      <c r="C68" s="3" t="s">
-        <v>162</v>
       </c>
       <c r="D68" s="3" t="s">
         <v>23</v>
@@ -4026,10 +4027,10 @@
         <v>112</v>
       </c>
       <c r="F68" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G68" s="5" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H68" s="3">
         <v>3</v>
@@ -4038,7 +4039,7 @@
         <v>2</v>
       </c>
       <c r="J68" s="4" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="69" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -4046,10 +4047,10 @@
         <v>68</v>
       </c>
       <c r="B69" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="C69" s="3" t="s">
         <v>159</v>
-      </c>
-      <c r="C69" s="3" t="s">
-        <v>160</v>
       </c>
       <c r="D69" s="3" t="s">
         <v>23</v>
@@ -4070,7 +4071,7 @@
         <v>2</v>
       </c>
       <c r="J69" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="70" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -4078,10 +4079,10 @@
         <v>68</v>
       </c>
       <c r="B70" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="C70" s="3" t="s">
         <v>198</v>
-      </c>
-      <c r="C70" s="3" t="s">
-        <v>199</v>
       </c>
       <c r="D70" s="3" t="s">
         <v>23</v>
@@ -4090,10 +4091,10 @@
         <v>111</v>
       </c>
       <c r="F70" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="G70" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H70" s="3">
         <v>5</v>
@@ -4102,7 +4103,7 @@
         <v>2</v>
       </c>
       <c r="J70" s="4" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Correct round end handling: only Erherhe should be > half the seeds, all the rest should end when player(s) don't have moves. ROUNDS parameter changed to an enum to describe round end condition. GPARAM_ONE may now be used in MAX_SEEDS/ROUNDS games to define the number of holes required to keep playing. This keeps some games from getting excessively long. Congklak was not implemented correctly--store ownership should be swapped-- which will not be implemented. The name was changed to Lagerung.txt with the same general game play (sow own store and sow CW). test_gm_bechi.py and test_gm_pandi.py have game tests skipped because of the rule change.
</commit_message>
<xml_diff>
--- a/src/game_params.xlsx
+++ b/src/game_params.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Activity_Data\Mancala_github\MancalaGames\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AE5F7D0-9F40-46C5-BD81-D56B0AB0CD18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6C7D6EA-DE80-46D1-9D9C-20B27A8253A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="game_params" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="273">
   <si>
     <t>tab</t>
   </si>
@@ -846,20 +846,10 @@
 When PLAYALTDIR is not selected, any hole can be set as UDIR_HOLES to allow the user to override the sow_direct setting.</t>
   </si>
   <si>
-    <t>Is the game played in a series of rounds? When rounds are employed, each round may end under conditions that do not win the overall game. The board is then setup again per the game rules, generally with some feature changed based on the previous round: hole ownership, holes out of play, a shortened board. Play continues in rounds until either player meets the overall game winning condition.
-For example: In Weg each round ends when neither player has a valid move. The board is then set up again after determining who owns what territory (holes). Rounds continue until one player has claimed sufficient territory to be declared the game winner (e.g. ownership of 10 or more holes).
-In the case of a round win or tie  a new starter is determined via ROUND_STARTER and  the board is reset according to ROUND_FILL.
-BLOCKS are used in many games and set between rounds based on the seed placement. TERRITORY GOAL games adjust hole ownership between rounds.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Moves maybe made from any hole, independent of the side of the board. Moves need to specify side, position and directions.  </t>
   </si>
   <si>
     <t>General Input</t>
-  </si>
-  <si>
-    <t>GOAL of Territory: defines the number of holes needed for a win.
-GOAL of Deprive and Blocked Divert Sower: defines the number of seeds needed to close/block holes (sow_blkd_div).</t>
   </si>
   <si>
     <t>If an opponent has no moves at the start of your turn, you must make seeds available to them if you can. This condition is enforced by only activating holes on the UI which will make seeds available to the opponent.</t>
@@ -893,17 +883,6 @@
   </si>
   <si>
     <t>Stores (captured) Multiplier</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The overall goal of the game. Defines how a player wins.
-- MAX_SEEDS: player with the maximum number of seeds at the end of the game wins or they collect more than half of the total seeds
-- DEPRIVE: eliminate all of your opponents seeds.
-  + If a player has no seeds at the start of their turn, they loose. If a player has no moves at the start of their turn, then the game outcome is determined by who has seeds: If both players have seeds, the game ends in a tie. If the current player has seeds, but the previous player does not, then the current player wins because they forced the previous player to give away all their seeds.
-  + GRANDSLAM must be legal for DEPRIVE games.
-  + Deprive games cannot be played in ROUNDS, use STORES, or use children. Additionally, the following options are incompatible with DEPRIVE games: MOVEUNLOCK, MUSTPASS, MUSTSHARE and NO_SIDES.
-- TERRITORY: claim ownership of holes. Each round the ownership of holes is determined by the number of seeds captured in the previous round. In a TERRITORY game without rounds, the winner is the player that gained the most territory during play. 
-  + TERRITORY games require STORES and that GPARAM_ONE be set to a value between the number of holes and two times the number of holes.
-  + TERRITORY games are incompatible with NO_SIDES, START_PATTERN, GRANDSLAM of NOT_LEGAL, ALLOW_RULE of OPP_OR_EMPTY, </t>
   </si>
   <si>
     <t xml:space="preserve">There are three flavors of capture two out:
@@ -993,6 +972,38 @@
 - OPP_GETS_REMAIN: if you capture all your opponents seeds, they capture all of your remaining seeds and the game is over. Winner is determined by game goal. Seeds picked because of PICKEXTRA PICK*LASTSEEDS go the current player and not the opponent.
 - LEAVE_LEFT: the capture is performed from all but the leftmost hole from the sower perspective. This might leave your oppenents without seeds or might not capture any seeds.
 - LEAVE_RIGHT: the capture is performed from all but the rightmost hole from the sower perspective. This might leave your oppenents without seeds.</t>
+  </si>
+  <si>
+    <t>GOAL of Territory: defines the number of holes needed for a win.
+GOAL of Deprive and Blocked Divert Sower: defines the number of seeds needed to close/block holes (sow_blkd_div).
+GOAL of Max Seeds and ROUNDS: define the minimum number of holes each player must have to continue the game.</t>
+  </si>
+  <si>
+    <t>NO_ROUNDS</t>
+  </si>
+  <si>
+    <t>When rounds are employed, each round may end under conditions that do not win the overall game. The board is then setup again per the game rules, generally with some feature changed based on the previous round: hole ownership, holes out of play, a shortened board. Play continues in rounds until either player meets the overall game winning condition.
+If the game is played in round, defines how each round ends: 
+- NO_ROUNDS: the game is not played in rounds
+- HALF_SEEDS: each round ends when one player has more that half the seeds
+- NO_MOVES: When MUSTSHARE is set, each round ends when neither player has a valid move.  When MUSTSHARE is not set, each round ends when a  player does have not a valid move at the start of their turn.
+For example: In Weg each round ends when neither player has a valid move. The board is then set up again after determining who owns what territory (holes). Rounds continue until one player has claimed sufficient territory to be declared the game winner (e.g. ownership of 10 or more holes).
+In the case of a round win or tie  a new starter is determined via ROUND_STARTER and  the board is reset according to ROUND_FILL.
+BLOCKS are used in many games and set between rounds based on the seed placement. TERRITORY GOAL games adjust hole ownership between rounds.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The overall goal of the game. Defines how a player wins.
+- MAX_SEEDS: The goal is to collect the maximum number of seeds.
+  + If the game is not played in rounds, the game will end when one player has more than half of the total seeds.
+  + If the game is played in rounds, the round end condition is determined by ROUNDS. These games end when one player has collected sufficient seeds to prevent the opponent from filling the required number of holes. Generally, the required number of holes is one but this may be increased by setting GPARAM_ONE. 
+  + In MAX_SEEDS/ROUNDS games the player only controls the holes on their side of the board, where as, in TERRITORY games a player may control holes on either side of the board.
+- DEPRIVE: eliminate all of your opponents seeds.
+  + If a player has no seeds at the start of their turn, they loose. If a player has no moves at the start of their turn, then the game outcome is determined by who has seeds: If both players have seeds, the game ends in a tie. If the current player has seeds, but the previous player does not, then the current player wins because they forced the previous player to give away all their seeds.
+  + GRANDSLAM must be legal for DEPRIVE games.
+  + Deprive games cannot be played in ROUNDS, use STORES, or use children. Additionally, the following options are incompatible with DEPRIVE games: MOVEUNLOCK, MUSTPASS, MUSTSHARE and NO_SIDES.
+- TERRITORY: claim ownership of holes. Each round the ownership of holes is determined by the number of seeds captured in the previous round. In a TERRITORY game without rounds, the winner is the player that gained the most territory during play. 
+  + TERRITORY games require STORES and that GPARAM_ONE be set to a value between the number of holes and two times the number of holes.
+  + TERRITORY games are incompatible with NO_SIDES, START_PATTERN, GRANDSLAM of NOT_LEGAL, ALLOW_RULE of OPP_OR_EMPTY, </t>
   </si>
 </sst>
 </file>
@@ -1877,8 +1888,8 @@
   <dimension ref="A1:J70"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G22" sqref="G22"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1988,7 +1999,7 @@
         <v>0</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="195" x14ac:dyDescent="0.25">
@@ -2180,7 +2191,7 @@
         <v>0</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="105" x14ac:dyDescent="0.25">
@@ -2212,7 +2223,7 @@
         <v>0</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2276,7 +2287,7 @@
         <v>0</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -2372,7 +2383,7 @@
         <v>2</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="180" x14ac:dyDescent="0.25">
@@ -2404,7 +2415,7 @@
         <v>2</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2532,7 +2543,7 @@
         <v>2</v>
       </c>
       <c r="J20" s="4" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -2596,7 +2607,7 @@
         <v>2</v>
       </c>
       <c r="J22" s="4" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
@@ -2663,7 +2674,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="165" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" ht="225" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>37</v>
       </c>
@@ -2680,10 +2691,10 @@
         <v>135</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>41</v>
+        <v>270</v>
       </c>
       <c r="H25" s="3">
         <v>4</v>
@@ -2692,7 +2703,7 @@
         <v>0</v>
       </c>
       <c r="J25" s="4" t="s">
-        <v>244</v>
+        <v>271</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -2791,7 +2802,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="255" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" ht="330" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>37</v>
       </c>
@@ -2820,7 +2831,7 @@
         <v>2</v>
       </c>
       <c r="J29" s="4" t="s">
-        <v>258</v>
+        <v>272</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2852,7 +2863,7 @@
         <v>2</v>
       </c>
       <c r="J30" s="4" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="31" spans="1:10" ht="165" x14ac:dyDescent="0.25">
@@ -2919,7 +2930,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>37</v>
       </c>
@@ -2927,7 +2938,7 @@
         <v>171</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D33" s="3" t="s">
         <v>23</v>
@@ -2948,7 +2959,7 @@
         <v>2</v>
       </c>
       <c r="J33" s="4" t="s">
-        <v>247</v>
+        <v>269</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
@@ -3172,7 +3183,7 @@
         <v>0</v>
       </c>
       <c r="J40" s="4" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
@@ -3259,7 +3270,7 @@
         <v>91</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="H43" s="3">
         <v>4</v>
@@ -3291,7 +3302,7 @@
         <v>91</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="H44" s="3">
         <v>6</v>
@@ -3323,7 +3334,7 @@
         <v>91</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="H45" s="3">
         <v>7</v>
@@ -3375,7 +3386,7 @@
         <v>128</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="D47" s="3" t="s">
         <v>129</v>
@@ -3407,7 +3418,7 @@
         <v>130</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D48" s="3" t="s">
         <v>129</v>
@@ -3439,7 +3450,7 @@
         <v>131</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="D49" s="3" t="s">
         <v>129</v>
@@ -3471,7 +3482,7 @@
         <v>132</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="D50" s="3" t="s">
         <v>129</v>
@@ -3503,7 +3514,7 @@
         <v>133</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="D51" s="3" t="s">
         <v>129</v>
@@ -3535,7 +3546,7 @@
         <v>134</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="D52" s="3" t="s">
         <v>129</v>
@@ -3567,7 +3578,7 @@
         <v>137</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="D53" s="3" t="s">
         <v>129</v>
@@ -3847,7 +3858,7 @@
         <v>0</v>
       </c>
       <c r="J62" s="4" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="63" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3911,7 +3922,7 @@
         <v>0</v>
       </c>
       <c r="J64" s="4" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
     </row>
     <row r="65" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -3975,7 +3986,7 @@
         <v>2</v>
       </c>
       <c r="J66" s="8" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.25">
@@ -4103,7 +4114,7 @@
         <v>2</v>
       </c>
       <c r="J70" s="4" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Bechi had the wrong number of start seeds! Updated game tests for Bechi and Pandi. Improved game text for the pick 4 games (Pandi, etc). Changed test approach for game tests: each game move is a separate test method which are collected into a single class. The class is marked incremental. If one these tests fail, all remaining tests in the class will be marked expected fail (by the test hooks in conftest.py). This keeps from reporting hundred of lines of output on test fails.
</commit_message>
<xml_diff>
--- a/src/game_params.xlsx
+++ b/src/game_params.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Activity_Data\Mancala_github\MancalaGames\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6C7D6EA-DE80-46D1-9D9C-20B27A8253A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE38A75E-AD4A-4EE6-8029-0B67BB2B87B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -698,17 +698,6 @@
     <t>Repeat turn if there was a capture. Making children is not a capture.</t>
   </si>
   <si>
-    <t>Choose how holes are filled when a new round strarts:
-- NOT_APPLICABLE: round fill doesn't need to be specified: either not played in rounds or game goal is TERRITORY (all holes filled).
-- LEFT_FILL: fill the round loser's holes from the player's left with NBR_START seeds each.  Holes that cannot be filled with NBR_START seeds (on the loser's side) are left empty; if BLOCKS is selected they are out of play for the round. All winner's holes are filled and are in play.
-- RIGHT_FILL: fill holes from the player's right. Other dynamics mimic left_fill.
-- OUTSIDE_FILL: fill holes from the outside ends toward the middle. Other dynamics mimic left_fill.
-- EVEN_FILL: fill all holes (both sides) with the same number of seeds; determined by dividing the losers seeds by the number of holes per side. If that is not playable based on the minimum number of seeds required for a move (MIN_MOVE); extra seeds are put in each players leftmost hole. Any extra seeds are put in each player's store.
-- SHORTEN: the number of holes that the round loser can fill with NBR_START seeds are fill on both sides, other holes are left empty. Holes are filled opposite eachother. If BLOCKS is selected, the board is shortened to the number of holes filled (empty holes are blocked and out of play). If the game uses children, they will not be created if the board size is reduced to 3 or less.
-- UCHOOSE: allow user to choose which holes have seeds (are not blocked) when ROUNDS and BLOCKS are used.
-- UMOVE: allow the loser to choose where seeds are placed. At least one seed must be placed in each hole and the game must be playable (at least one hole has MIN_MOVE seeds), remaining seeds are placed in the store. The winner's layout is the same layout but reflected.</t>
-  </si>
-  <si>
     <t>Only allow cross capture if the player has sown onto the opposite side of board. 
 If a player ends on their own side of the board in an empty hole, but did not sow any opposite hole, they get a repeat turn.</t>
   </si>
@@ -1004,6 +993,20 @@
 - TERRITORY: claim ownership of holes. Each round the ownership of holes is determined by the number of seeds captured in the previous round. In a TERRITORY game without rounds, the winner is the player that gained the most territory during play. 
   + TERRITORY games require STORES and that GPARAM_ONE be set to a value between the number of holes and two times the number of holes.
   + TERRITORY games are incompatible with NO_SIDES, START_PATTERN, GRANDSLAM of NOT_LEGAL, ALLOW_RULE of OPP_OR_EMPTY, </t>
+  </si>
+  <si>
+    <t>The round fill method determines which holes are filled and how many seeds they are filled with when setting up for a new round.
+Several round fill mechanisms use the same general approach called the Empty Hole Method. The loser of the previous round will end up with empty holes. These holes are not playable if BLOCKS are used; otherwise they are playable.
+The seeds each player accummulated in the previous round are distributed into holes with exactly the same number in each. That number of seeds is NBR_START. The winner will fill all of their holes and put any remaining seeds into their own store. The loser will fill as many holes as they can with nbr_start seeds and put any remaining seeds (fewer than nbr_start) into their own store.
+LEFT_FILE, RIGHT_FILL and OUTSIDE_FILL define which holes that the loser must fill. UCHOOSE allows the loser to choose which holes have seeds.
+- NOT_APPLICABLE: round fill doesn't need to be specified: either the game not played in rounds (DEPRIVE game included) or game goal is TERRITORY (all holes filled).
+- LEFT_FILL: fill the round loser's holes from the player's left with nbr_start seeds each.  
+- RIGHT_FILL: fill the round loser's holes from the player's right with nbr_start seeds each. 
+- OUTSIDE_FILL: fill the round loser's holes from the outside ends toward the middle with nbr_start seeds each. Leftmost, rightmost, 2nd leftmost, 2nd rightmost, etc. until the seeds are used up.
+- EVEN_FILL: fill all holes (both sides) with the same number of seeds; determined by dividing the losers seeds by the number of holes per side. If that is not playable based on the minimum number of seeds required for a move (MIN_MOVE); extra seeds are put in each players leftmost hole. Any extra seeds are put in each player's store.
+- SHORTEN: the number of holes that the round loser can fill with NBR_START seeds are fill on both sides, other holes are left empty. Holes are filled opposite eachother. If BLOCKS is selected, the board is shortened to the number of holes filled (empty holes are blocked and out of play). If the game uses children, they will not be created if the board size is reduced to 3 or less.
+- UCHOOSE: allow user to choose which holes have seeds (are not blocked) when ROUNDS and BLOCKS are used.
+- UMOVE: allow the loser to choose where seeds are placed. At least one seed must be placed in each hole and the game must be playable (at least one hole has MIN_MOVE seeds), remaining seeds are placed in the store. The winner's layout is the same layout but reflected.</t>
   </si>
 </sst>
 </file>
@@ -1889,7 +1892,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J29" sqref="J29"/>
+      <selection pane="bottomLeft" activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1999,7 +2002,7 @@
         <v>0</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="195" x14ac:dyDescent="0.25">
@@ -2063,7 +2066,7 @@
         <v>0</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -2127,7 +2130,7 @@
         <v>0</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -2159,7 +2162,7 @@
         <v>0</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="105" x14ac:dyDescent="0.25">
@@ -2191,7 +2194,7 @@
         <v>0</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="105" x14ac:dyDescent="0.25">
@@ -2223,7 +2226,7 @@
         <v>0</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2255,7 +2258,7 @@
         <v>0</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="120" x14ac:dyDescent="0.25">
@@ -2287,7 +2290,7 @@
         <v>0</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -2319,7 +2322,7 @@
         <v>2</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2351,7 +2354,7 @@
         <v>2</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -2383,7 +2386,7 @@
         <v>2</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="180" x14ac:dyDescent="0.25">
@@ -2415,7 +2418,7 @@
         <v>2</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2447,7 +2450,7 @@
         <v>2</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
@@ -2511,7 +2514,7 @@
         <v>2</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="120" x14ac:dyDescent="0.25">
@@ -2543,7 +2546,7 @@
         <v>2</v>
       </c>
       <c r="J20" s="4" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -2607,7 +2610,7 @@
         <v>2</v>
       </c>
       <c r="J22" s="4" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
@@ -2694,7 +2697,7 @@
         <v>43</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="H25" s="3">
         <v>4</v>
@@ -2703,7 +2706,7 @@
         <v>0</v>
       </c>
       <c r="J25" s="4" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -2738,7 +2741,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="285" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" ht="405" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>37</v>
       </c>
@@ -2767,7 +2770,7 @@
         <v>0</v>
       </c>
       <c r="J27" s="4" t="s">
-        <v>214</v>
+        <v>272</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -2831,7 +2834,7 @@
         <v>2</v>
       </c>
       <c r="J29" s="4" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2863,7 +2866,7 @@
         <v>2</v>
       </c>
       <c r="J30" s="4" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="31" spans="1:10" ht="165" x14ac:dyDescent="0.25">
@@ -2895,7 +2898,7 @@
         <v>2</v>
       </c>
       <c r="J31" s="4" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="240" x14ac:dyDescent="0.25">
@@ -2927,7 +2930,7 @@
         <v>2</v>
       </c>
       <c r="J32" s="4" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -2938,7 +2941,7 @@
         <v>171</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D33" s="3" t="s">
         <v>23</v>
@@ -2959,7 +2962,7 @@
         <v>2</v>
       </c>
       <c r="J33" s="4" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
@@ -3183,7 +3186,7 @@
         <v>0</v>
       </c>
       <c r="J40" s="4" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
@@ -3215,7 +3218,7 @@
         <v>0</v>
       </c>
       <c r="J41" s="4" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="42" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3247,7 +3250,7 @@
         <v>0</v>
       </c>
       <c r="J42" s="4" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
@@ -3270,7 +3273,7 @@
         <v>91</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="H43" s="3">
         <v>4</v>
@@ -3279,7 +3282,7 @@
         <v>0</v>
       </c>
       <c r="J43" s="4" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -3302,7 +3305,7 @@
         <v>91</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="H44" s="3">
         <v>6</v>
@@ -3311,7 +3314,7 @@
         <v>0</v>
       </c>
       <c r="J44" s="4" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
@@ -3334,7 +3337,7 @@
         <v>91</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="H45" s="3">
         <v>7</v>
@@ -3343,7 +3346,7 @@
         <v>0</v>
       </c>
       <c r="J45" s="4" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
@@ -3375,7 +3378,7 @@
         <v>0</v>
       </c>
       <c r="J46" s="4" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="47" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -3386,7 +3389,7 @@
         <v>128</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D47" s="3" t="s">
         <v>129</v>
@@ -3407,7 +3410,7 @@
         <v>2</v>
       </c>
       <c r="J47" s="4" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="48" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -3418,7 +3421,7 @@
         <v>130</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D48" s="3" t="s">
         <v>129</v>
@@ -3439,7 +3442,7 @@
         <v>2</v>
       </c>
       <c r="J48" s="4" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="49" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -3450,7 +3453,7 @@
         <v>131</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D49" s="3" t="s">
         <v>129</v>
@@ -3471,7 +3474,7 @@
         <v>2</v>
       </c>
       <c r="J49" s="4" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="50" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3482,7 +3485,7 @@
         <v>132</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D50" s="3" t="s">
         <v>129</v>
@@ -3503,7 +3506,7 @@
         <v>2</v>
       </c>
       <c r="J50" s="4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="51" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -3514,7 +3517,7 @@
         <v>133</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D51" s="3" t="s">
         <v>129</v>
@@ -3535,7 +3538,7 @@
         <v>2</v>
       </c>
       <c r="J51" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="52" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -3546,7 +3549,7 @@
         <v>134</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D52" s="3" t="s">
         <v>129</v>
@@ -3567,7 +3570,7 @@
         <v>2</v>
       </c>
       <c r="J52" s="4" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="53" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -3578,7 +3581,7 @@
         <v>137</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D53" s="3" t="s">
         <v>129</v>
@@ -3599,7 +3602,7 @@
         <v>2</v>
       </c>
       <c r="J53" s="4" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="54" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -3631,7 +3634,7 @@
         <v>2</v>
       </c>
       <c r="J54" s="4" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
@@ -3762,7 +3765,7 @@
         <v>0</v>
       </c>
       <c r="J59" s="4" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
@@ -3826,7 +3829,7 @@
         <v>0</v>
       </c>
       <c r="J61" s="4" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="62" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3858,7 +3861,7 @@
         <v>0</v>
       </c>
       <c r="J62" s="4" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="63" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3922,7 +3925,7 @@
         <v>0</v>
       </c>
       <c r="J64" s="4" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="65" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -3954,7 +3957,7 @@
         <v>0</v>
       </c>
       <c r="J65" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="66" spans="1:10" ht="210" x14ac:dyDescent="0.25">
@@ -3986,7 +3989,7 @@
         <v>2</v>
       </c>
       <c r="J66" s="8" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.25">
@@ -4018,7 +4021,7 @@
         <v>2</v>
       </c>
       <c r="J67" s="4" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="68" spans="1:10" ht="285" x14ac:dyDescent="0.25">
@@ -4050,7 +4053,7 @@
         <v>2</v>
       </c>
       <c r="J68" s="4" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="69" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -4114,7 +4117,7 @@
         <v>2</v>
       </c>
       <c r="J70" s="4" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Corrected bugs in make_child.py OneChild: it was assuming that children could only be made opposite side (could end up with >1 child depending on side of 1st child) and the exclusion holes were wrong. Added tests specific to OneChild. Changed OneChild to also support Toguz Korgool (slight variant of Toguz Xorgol). Removed the rule requiring that OneChild only be used with stores. Updated parameter child_type description.
</commit_message>
<xml_diff>
--- a/src/game_params.xlsx
+++ b/src/game_params.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Activity_Data\Mancala_github\MancalaGames\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE38A75E-AD4A-4EE6-8029-0B67BB2B87B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6616181F-3AD9-4059-B316-CBF6708A2EBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -777,18 +777,6 @@
 SOW_RULE of either SOW_CAPT_ALL do not do this capture.</t>
   </si>
   <si>
-    <t xml:space="preserve">Games with children allow players to claim holes. These child holes are an extension of the stores and seeds in them count towards a win. Making a child stops any multiple lap sowing, moves cannot start from children, and they cannot be captured (except for special rules associated with WEGs).
-- NOCHILD: children are not used.
-- NORMAL: children are made when a final seeds sows a hole to CHILD_CVT.
-- WALDA: STORES are not supported. Captures are instead moved into waldas, thus a player may not capture until they have created a walda. 
-  + Walda locations are limited.  Each player may create up to 6 waldas: on either end of each side of the board and the next outer hole on their own side of the board. Note that there are only 8 total places that waldas maybe created.
-- ONE_CHILD: only one child allowed per player, may not be in player's left most hole,  and may not be opposite eachother. Used to create tuzdek style children along with CHILD_RULE of OPP_ONLY.
-- WEG: children maybe created in holes owned by the opponent. Ending a sow in an opponent's weg captures the seed just sown and one more (if there is one); generally, the player gets to play again (per CAPT_RTURN). WEGs are supported for TERRITORY games only (hole ownership required).
-- BULL: create one bull if final seed sows to CHILD_CVT, create two bulls if the final two seeds are sown to CHILD_CVT-1 and CHILD_CVT (in either order).
-- QUR: when a seed is sown into an empty hole on the player's side of the board and the opposite hole contains CHILD_CVT, create children in both holes: final seed location and opposite.
-</t>
-  </si>
-  <si>
     <t>Holes in the game start each game and round locked. Captures may not be made from locked holes. Starting a sow from a hole unlocks it allowing future captures.</t>
   </si>
   <si>
@@ -1007,6 +995,21 @@
 - SHORTEN: the number of holes that the round loser can fill with NBR_START seeds are fill on both sides, other holes are left empty. Holes are filled opposite eachother. If BLOCKS is selected, the board is shortened to the number of holes filled (empty holes are blocked and out of play). If the game uses children, they will not be created if the board size is reduced to 3 or less.
 - UCHOOSE: allow user to choose which holes have seeds (are not blocked) when ROUNDS and BLOCKS are used.
 - UMOVE: allow the loser to choose where seeds are placed. At least one seed must be placed in each hole and the game must be playable (at least one hole has MIN_MOVE seeds), remaining seeds are placed in the store. The winner's layout is the same layout but reflected.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Games with children allow players to claim holes. These child holes are an extension of the stores and seeds in them count towards a win. Making a child stops any multiple lap sowing, moves cannot start from children, and they cannot be captured (except for special rules associated with WEGs).
+- NOCHILD: children are not used.
+- NORMAL: children are made when a final seeds sows a hole to CHILD_CVT.
+- WALDA: STORES are not supported. Captures are instead moved into waldas, thus a player may not capture until they have created a walda. 
+  + Walda locations are limited.  Each player may create up to 6 waldas: on either end of each side of the board and the next two outer holes on their own side of the board. Note that there are only 8 total places that waldas maybe created.
+- ONE_CHILD: only one child allowed per player  and may not be opposite eachother. Depending on sow direction some holes are prohibited from being made children: 
+  + CW &amp; CCW:  the last of your opponents holes that you would sow into may not be made a child.
+  + SPLIT: no end holes may be made children.
+  + Used to create tuzdek style children along with CHILD_RULE of OPP_ONLY.
+- WEG: children maybe created in holes owned by the opponent. Ending a sow in an opponent's weg captures the seed just sown and one more (if there is one); generally, the player gets to play again (per CAPT_RTURN). WEGs are supported for TERRITORY games only (hole ownership required).
+- BULL: create one bull if final seed sows to CHILD_CVT, create two bulls if the final two seeds are sown to CHILD_CVT-1 and CHILD_CVT (in either order).
+- QUR: when a seed is sown into an empty hole on the player's side of the board and the opposite hole contains CHILD_CVT, create children in both holes: final seed location and opposite.
+</t>
   </si>
 </sst>
 </file>
@@ -1891,8 +1894,8 @@
   <dimension ref="A1:J70"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C27" sqref="C27"/>
+      <pane ySplit="1" topLeftCell="A66" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J68" sqref="J68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2002,7 +2005,7 @@
         <v>0</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="195" x14ac:dyDescent="0.25">
@@ -2194,7 +2197,7 @@
         <v>0</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="105" x14ac:dyDescent="0.25">
@@ -2226,7 +2229,7 @@
         <v>0</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2290,7 +2293,7 @@
         <v>0</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -2386,7 +2389,7 @@
         <v>2</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="180" x14ac:dyDescent="0.25">
@@ -2418,7 +2421,7 @@
         <v>2</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2450,7 +2453,7 @@
         <v>2</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
@@ -2546,7 +2549,7 @@
         <v>2</v>
       </c>
       <c r="J20" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -2610,7 +2613,7 @@
         <v>2</v>
       </c>
       <c r="J22" s="4" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
@@ -2697,7 +2700,7 @@
         <v>43</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="H25" s="3">
         <v>4</v>
@@ -2706,7 +2709,7 @@
         <v>0</v>
       </c>
       <c r="J25" s="4" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -2770,7 +2773,7 @@
         <v>0</v>
       </c>
       <c r="J27" s="4" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -2834,7 +2837,7 @@
         <v>2</v>
       </c>
       <c r="J29" s="4" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2866,7 +2869,7 @@
         <v>2</v>
       </c>
       <c r="J30" s="4" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="31" spans="1:10" ht="165" x14ac:dyDescent="0.25">
@@ -2898,7 +2901,7 @@
         <v>2</v>
       </c>
       <c r="J31" s="4" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="240" x14ac:dyDescent="0.25">
@@ -2930,7 +2933,7 @@
         <v>2</v>
       </c>
       <c r="J32" s="4" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -2941,7 +2944,7 @@
         <v>171</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D33" s="3" t="s">
         <v>23</v>
@@ -2962,7 +2965,7 @@
         <v>2</v>
       </c>
       <c r="J33" s="4" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
@@ -3186,7 +3189,7 @@
         <v>0</v>
       </c>
       <c r="J40" s="4" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
@@ -3273,7 +3276,7 @@
         <v>91</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="H43" s="3">
         <v>4</v>
@@ -3305,7 +3308,7 @@
         <v>91</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="H44" s="3">
         <v>6</v>
@@ -3337,7 +3340,7 @@
         <v>91</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="H45" s="3">
         <v>7</v>
@@ -3389,7 +3392,7 @@
         <v>128</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D47" s="3" t="s">
         <v>129</v>
@@ -3421,7 +3424,7 @@
         <v>130</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D48" s="3" t="s">
         <v>129</v>
@@ -3453,7 +3456,7 @@
         <v>131</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D49" s="3" t="s">
         <v>129</v>
@@ -3474,7 +3477,7 @@
         <v>2</v>
       </c>
       <c r="J49" s="4" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="50" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3485,7 +3488,7 @@
         <v>132</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D50" s="3" t="s">
         <v>129</v>
@@ -3517,7 +3520,7 @@
         <v>133</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D51" s="3" t="s">
         <v>129</v>
@@ -3549,7 +3552,7 @@
         <v>134</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D52" s="3" t="s">
         <v>129</v>
@@ -3581,7 +3584,7 @@
         <v>137</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D53" s="3" t="s">
         <v>129</v>
@@ -3765,7 +3768,7 @@
         <v>0</v>
       </c>
       <c r="J59" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
@@ -3829,7 +3832,7 @@
         <v>0</v>
       </c>
       <c r="J61" s="4" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="62" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3861,7 +3864,7 @@
         <v>0</v>
       </c>
       <c r="J62" s="4" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="63" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3925,7 +3928,7 @@
         <v>0</v>
       </c>
       <c r="J64" s="4" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="65" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -3957,7 +3960,7 @@
         <v>0</v>
       </c>
       <c r="J65" s="4" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="66" spans="1:10" ht="210" x14ac:dyDescent="0.25">
@@ -3989,7 +3992,7 @@
         <v>2</v>
       </c>
       <c r="J66" s="8" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.25">
@@ -4021,10 +4024,10 @@
         <v>2</v>
       </c>
       <c r="J67" s="4" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="68" spans="1:10" ht="285" x14ac:dyDescent="0.25">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" ht="330" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
         <v>68</v>
       </c>
@@ -4053,7 +4056,7 @@
         <v>2</v>
       </c>
       <c r="J68" s="4" t="s">
-        <v>234</v>
+        <v>272</v>
       </c>
     </row>
     <row r="69" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -4117,7 +4120,7 @@
         <v>2</v>
       </c>
       <c r="J70" s="4" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Correct OneChild no opposite to no symmetric opposite children. Added log entry if child not made solely because not symmetric. Updated tests. Updated Toguz Xorgol text. Updated OneChild param description. pytest.ini removed xfail and xpass from summary.
</commit_message>
<xml_diff>
--- a/src/game_params.xlsx
+++ b/src/game_params.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Activity_Data\Mancala_github\MancalaGames\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6616181F-3AD9-4059-B316-CBF6708A2EBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EF5D9A4-379D-49DF-9985-41AA7D73AA6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="0" windowWidth="25755" windowHeight="15180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="game_params" sheetId="1" r:id="rId1"/>
@@ -1002,8 +1002,12 @@
 - NORMAL: children are made when a final seeds sows a hole to CHILD_CVT.
 - WALDA: STORES are not supported. Captures are instead moved into waldas, thus a player may not capture until they have created a walda. 
   + Walda locations are limited.  Each player may create up to 6 waldas: on either end of each side of the board and the next two outer holes on their own side of the board. Note that there are only 8 total places that waldas maybe created.
-- ONE_CHILD: only one child allowed per player  and may not be opposite eachother. Depending on sow direction some holes are prohibited from being made children: 
-  + CW &amp; CCW:  the last of your opponents holes that you would sow into may not be made a child.
+- ONE_CHILD: only one child allowed per player.
+  + Children must not be symmetrically opposite eachother. For example,  in a 9 hole per side game with holes numbered as follows, tuzdeks may not be in the same numbered holes:
+  + 9 8 7 6 5 4 3 2 1
+  + 1 2 3 4 5 6 7 8 9 
+  + Depending on sow direction some holes are prohibited from being made children: 
+  + CW &amp; CCW:  the last of your opponents holes that you would sow into may not be made a child. CW holes numbered 1 above and CCW holes numberd 9 above.
   + SPLIT: no end holes may be made children.
   + Used to create tuzdek style children along with CHILD_RULE of OPP_ONLY.
 - WEG: children maybe created in holes owned by the opponent. Ending a sow in an opponent's weg captures the seed just sown and one more (if there is one); generally, the player gets to play again (per CAPT_RTURN). WEGs are supported for TERRITORY games only (hole ownership required).
@@ -1893,8 +1897,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:J70"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A66" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A67" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="J68" sqref="J68"/>
     </sheetView>
   </sheetViews>
@@ -4027,7 +4031,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="68" spans="1:10" ht="330" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" ht="405" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
         <v>68</v>
       </c>

</xml_diff>

<commit_message>
added weg test_cmd_end_move test cases. tidy claimer code. resolve pylint warning. clarify Bechi multicapt stops for locked hole.
</commit_message>
<xml_diff>
--- a/src/game_params.xlsx
+++ b/src/game_params.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Activity_Data\Mancala_github\MancalaGames\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EF5D9A4-379D-49DF-9985-41AA7D73AA6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F190110-932C-4BF2-985E-40A3B0FBD266}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="0" windowWidth="25755" windowHeight="15180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="game_params" sheetId="1" r:id="rId1"/>
@@ -951,11 +951,6 @@
 - LEAVE_RIGHT: the capture is performed from all but the rightmost hole from the sower perspective. This might leave your oppenents without seeds.</t>
   </si>
   <si>
-    <t>GOAL of Territory: defines the number of holes needed for a win.
-GOAL of Deprive and Blocked Divert Sower: defines the number of seeds needed to close/block holes (sow_blkd_div).
-GOAL of Max Seeds and ROUNDS: define the minimum number of holes each player must have to continue the game.</t>
-  </si>
-  <si>
     <t>NO_ROUNDS</t>
   </si>
   <si>
@@ -1014,6 +1009,11 @@
 - BULL: create one bull if final seed sows to CHILD_CVT, create two bulls if the final two seeds are sown to CHILD_CVT-1 and CHILD_CVT (in either order).
 - QUR: when a seed is sown into an empty hole on the player's side of the board and the opposite hole contains CHILD_CVT, create children in both holes: final seed location and opposite.
 </t>
+  </si>
+  <si>
+    <t>GOAL of Territory: defines the number of holes needed for a win. The number of holes for each player are computed by rounding the number of seeds collected divided by the number of start seeds per hole.
+GOAL of Deprive and Blocked Divert Sower: defines the number of seeds needed to close/block holes (sow_blkd_div).
+GOAL of Max Seeds and ROUNDS: defines the minimum number of holes each player must have to continue the game. The player with fewer seeds must have enough seeds to fill gparam_one holes each with start_seeds in order to continue playing.  There is no rounding of seed counts as in territory games.</t>
   </si>
 </sst>
 </file>
@@ -1897,9 +1897,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:J70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A67" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J68" sqref="J68"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J33" sqref="J33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2704,7 +2704,7 @@
         <v>43</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="H25" s="3">
         <v>4</v>
@@ -2713,7 +2713,7 @@
         <v>0</v>
       </c>
       <c r="J25" s="4" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -2777,7 +2777,7 @@
         <v>0</v>
       </c>
       <c r="J27" s="4" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -2841,7 +2841,7 @@
         <v>2</v>
       </c>
       <c r="J29" s="4" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2940,7 +2940,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>37</v>
       </c>
@@ -2969,7 +2969,7 @@
         <v>2</v>
       </c>
       <c r="J33" s="4" t="s">
-        <v>267</v>
+        <v>272</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
@@ -4060,7 +4060,7 @@
         <v>2</v>
       </c>
       <c r="J68" s="4" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="69" spans="1:10" ht="30" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added a new class for Diffusion: marksteeregames.com Rules Copyright (c) January 2006 by Mark Steere
</commit_message>
<xml_diff>
--- a/src/game_params.xlsx
+++ b/src/game_params.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Activity_Data\Mancala_github\MancalaGames\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F190110-932C-4BF2-985E-40A3B0FBD266}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0D50BB2-5B39-4AE7-9527-66ECF58E4FF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="966" uniqueCount="274">
   <si>
     <t>tab</t>
   </si>
@@ -96,9 +96,6 @@
   </si>
   <si>
     <t>Mancala</t>
-  </si>
-  <si>
-    <t>The name of the Game Class. Currently only Mancala.</t>
   </si>
   <si>
     <t>name</t>
@@ -1014,6 +1011,16 @@
     <t>GOAL of Territory: defines the number of holes needed for a win. The number of holes for each player are computed by rounding the number of seeds collected divided by the number of start seeds per hole.
 GOAL of Deprive and Blocked Divert Sower: defines the number of seeds needed to close/block holes (sow_blkd_div).
 GOAL of Max Seeds and ROUNDS: defines the minimum number of holes each player must have to continue the game. The player with fewer seeds must have enough seeds to fill gparam_one holes each with start_seeds in order to continue playing.  There is no rounding of seed counts as in territory games.</t>
+  </si>
+  <si>
+    <t>The name of the Game Class. Currently one of:
+Mancala: allows setting all parameters though there are limited combinations.
+Diffusion: has unique sow method and win conditions. Only very limited parameters may be changed from defaults.</t>
+  </si>
+  <si>
+    <t>The name of the Game Class. One of:
+Mancala: allows setting all parameters though there are limited combinations.
+Diffusion: has unique sow method and win conditions. Only very limited parameters may be changed from defaults.</t>
   </si>
 </sst>
 </file>
@@ -1898,8 +1905,8 @@
   <dimension ref="A1:J70"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J33" sqref="J33"/>
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J34" sqref="J34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1930,7 +1937,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>4</v>
@@ -1950,16 +1957,16 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C2" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>63</v>
-      </c>
       <c r="D2" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E2" s="3">
         <v>119</v>
@@ -1968,39 +1975,39 @@
         <v>11</v>
       </c>
       <c r="G2" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="H2" s="3">
+        <v>0</v>
+      </c>
+      <c r="I2" s="3">
+        <v>0</v>
+      </c>
+      <c r="J2" s="4" t="s">
         <v>64</v>
-      </c>
-      <c r="H2" s="3">
-        <v>0</v>
-      </c>
-      <c r="I2" s="3">
-        <v>0</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>67</v>
-      </c>
       <c r="D3" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E3" s="3">
         <v>126</v>
       </c>
       <c r="F3" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G3" s="5" t="s">
         <v>40</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>41</v>
       </c>
       <c r="H3" s="3">
         <v>1</v>
@@ -2009,30 +2016,30 @@
         <v>0</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="195" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>166</v>
-      </c>
       <c r="D4" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E4" s="3">
         <v>101</v>
       </c>
       <c r="F4" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="G4" s="5" t="s">
         <v>167</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>168</v>
       </c>
       <c r="H4" s="3">
         <v>3</v>
@@ -2041,31 +2048,31 @@
         <v>0</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="C5" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>96</v>
-      </c>
       <c r="D5" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E5" s="3">
         <v>103</v>
       </c>
       <c r="F5" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G5" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="G5" s="5" t="s">
-        <v>41</v>
-      </c>
       <c r="H5" s="3">
         <v>0</v>
       </c>
@@ -2073,30 +2080,30 @@
         <v>0</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>98</v>
-      </c>
       <c r="D6" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E6" s="3">
         <v>130</v>
       </c>
       <c r="F6" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G6" s="5" t="s">
         <v>40</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>41</v>
       </c>
       <c r="H6" s="3">
         <v>1</v>
@@ -2105,30 +2112,30 @@
         <v>0</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>118</v>
-      </c>
       <c r="D7" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E7" s="3">
         <v>124</v>
       </c>
       <c r="F7" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G7" s="5" t="s">
         <v>40</v>
-      </c>
-      <c r="G7" s="5" t="s">
-        <v>41</v>
       </c>
       <c r="H7" s="3">
         <v>2</v>
@@ -2137,30 +2144,30 @@
         <v>0</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B8" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>103</v>
-      </c>
       <c r="D8" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E8" s="3">
         <v>114</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H8" s="3">
         <v>3</v>
@@ -2169,21 +2176,21 @@
         <v>0</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B9" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>105</v>
-      </c>
       <c r="D9" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E9" s="3">
         <v>104</v>
@@ -2192,7 +2199,7 @@
         <v>11</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H9" s="3">
         <v>4</v>
@@ -2201,21 +2208,21 @@
         <v>0</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B10" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>107</v>
-      </c>
       <c r="D10" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E10" s="3">
         <v>105</v>
@@ -2224,7 +2231,7 @@
         <v>11</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H10" s="3">
         <v>5</v>
@@ -2233,30 +2240,30 @@
         <v>0</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B11" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>178</v>
-      </c>
       <c r="D11" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E11" s="3">
         <v>106</v>
       </c>
       <c r="F11" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G11" s="5" t="s">
         <v>40</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>41</v>
       </c>
       <c r="H11" s="3">
         <v>6</v>
@@ -2265,30 +2272,30 @@
         <v>0</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B12" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="C12" s="3" t="s">
-        <v>126</v>
-      </c>
       <c r="D12" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E12" s="3">
         <v>109</v>
       </c>
       <c r="F12" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G12" s="5" t="s">
         <v>40</v>
-      </c>
-      <c r="G12" s="5" t="s">
-        <v>41</v>
       </c>
       <c r="H12" s="3">
         <v>7</v>
@@ -2297,30 +2304,30 @@
         <v>0</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B13" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="C13" s="3" t="s">
-        <v>112</v>
-      </c>
       <c r="D13" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E13" s="3">
         <v>113</v>
       </c>
       <c r="F13" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G13" s="5" t="s">
         <v>40</v>
-      </c>
-      <c r="G13" s="5" t="s">
-        <v>41</v>
       </c>
       <c r="H13" s="3">
         <v>0</v>
@@ -2329,30 +2336,30 @@
         <v>2</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B14" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="C14" s="3" t="s">
-        <v>190</v>
-      </c>
       <c r="D14" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E14" s="3">
         <v>146</v>
       </c>
       <c r="F14" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G14" s="5" t="s">
         <v>40</v>
-      </c>
-      <c r="G14" s="5" t="s">
-        <v>41</v>
       </c>
       <c r="H14" s="3">
         <v>1</v>
@@ -2361,30 +2368,30 @@
         <v>2</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B15" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="C15" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="C15" s="3" t="s">
-        <v>114</v>
-      </c>
       <c r="D15" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E15" s="3">
         <v>147</v>
       </c>
       <c r="F15" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="G15" s="5" t="s">
         <v>115</v>
-      </c>
-      <c r="G15" s="5" t="s">
-        <v>116</v>
       </c>
       <c r="H15" s="3">
         <v>2</v>
@@ -2393,30 +2400,30 @@
         <v>2</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="180" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B16" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="C16" s="3" t="s">
-        <v>120</v>
-      </c>
       <c r="D16" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E16" s="3">
         <v>117</v>
       </c>
       <c r="F16" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="G16" s="5" t="s">
         <v>121</v>
-      </c>
-      <c r="G16" s="5" t="s">
-        <v>122</v>
       </c>
       <c r="H16" s="3">
         <v>3</v>
@@ -2425,30 +2432,30 @@
         <v>2</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B17" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="C17" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="C17" s="3" t="s">
-        <v>101</v>
-      </c>
       <c r="D17" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E17" s="3">
         <v>123</v>
       </c>
       <c r="F17" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G17" s="5" t="s">
         <v>40</v>
-      </c>
-      <c r="G17" s="5" t="s">
-        <v>41</v>
       </c>
       <c r="H17" s="3">
         <v>4</v>
@@ -2457,30 +2464,30 @@
         <v>2</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B18" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="C18" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="C18" s="3" t="s">
-        <v>109</v>
-      </c>
       <c r="D18" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E18" s="3">
         <v>129</v>
       </c>
       <c r="F18" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G18" s="5" t="s">
         <v>40</v>
-      </c>
-      <c r="G18" s="5" t="s">
-        <v>41</v>
       </c>
       <c r="H18" s="3">
         <v>5</v>
@@ -2489,30 +2496,30 @@
         <v>2</v>
       </c>
       <c r="J18" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B19" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="C19" s="3" t="s">
         <v>200</v>
       </c>
-      <c r="C19" s="3" t="s">
-        <v>201</v>
-      </c>
       <c r="D19" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E19" s="3">
         <v>128</v>
       </c>
       <c r="F19" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G19" s="5" t="s">
         <v>40</v>
-      </c>
-      <c r="G19" s="5" t="s">
-        <v>41</v>
       </c>
       <c r="H19" s="3">
         <v>6</v>
@@ -2521,30 +2528,30 @@
         <v>2</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B20" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="C20" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="C20" s="3" t="s">
-        <v>124</v>
-      </c>
       <c r="D20" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E20" s="3">
         <v>107</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H20" s="3">
         <v>8</v>
@@ -2553,30 +2560,30 @@
         <v>2</v>
       </c>
       <c r="J20" s="4" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B21" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="C21" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="C21" s="3" t="s">
-        <v>176</v>
-      </c>
       <c r="D21" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E21" s="3">
         <v>108</v>
       </c>
       <c r="F21" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G21" s="5" t="s">
         <v>40</v>
-      </c>
-      <c r="G21" s="5" t="s">
-        <v>41</v>
       </c>
       <c r="H21" s="3">
         <v>9</v>
@@ -2585,30 +2592,30 @@
         <v>2</v>
       </c>
       <c r="J21" s="4" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="150" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E22" s="3">
         <v>131</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H22" s="3">
         <v>10</v>
@@ -2617,30 +2624,30 @@
         <v>2</v>
       </c>
       <c r="J22" s="4" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B23" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C23" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C23" s="3" t="s">
-        <v>51</v>
-      </c>
       <c r="D23" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E23" s="3">
         <v>142</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H23" s="3">
         <v>0</v>
@@ -2649,30 +2656,30 @@
         <v>0</v>
       </c>
       <c r="J23" s="4" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B24" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="C24" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C24" s="3" t="s">
-        <v>39</v>
-      </c>
       <c r="D24" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E24" s="3">
         <v>125</v>
       </c>
       <c r="F24" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G24" s="5" t="s">
         <v>40</v>
-      </c>
-      <c r="G24" s="5" t="s">
-        <v>41</v>
       </c>
       <c r="H24" s="3">
         <v>1</v>
@@ -2681,30 +2688,30 @@
         <v>0</v>
       </c>
       <c r="J24" s="4" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="225" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B25" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C25" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C25" s="3" t="s">
-        <v>43</v>
-      </c>
       <c r="D25" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E25" s="3">
         <v>135</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="H25" s="3">
         <v>4</v>
@@ -2713,30 +2720,30 @@
         <v>0</v>
       </c>
       <c r="J25" s="4" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B26" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C26" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C26" s="3" t="s">
-        <v>45</v>
-      </c>
       <c r="D26" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E26" s="3">
         <v>134</v>
       </c>
       <c r="F26" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="G26" s="5" t="s">
         <v>46</v>
-      </c>
-      <c r="G26" s="5" t="s">
-        <v>47</v>
       </c>
       <c r="H26" s="3">
         <v>5</v>
@@ -2745,30 +2752,30 @@
         <v>0</v>
       </c>
       <c r="J26" s="4" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="405" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B27" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="C27" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="C27" s="3" t="s">
-        <v>192</v>
-      </c>
       <c r="D27" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E27" s="3">
         <v>133</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="H27" s="3">
         <v>6</v>
@@ -2777,30 +2784,30 @@
         <v>0</v>
       </c>
       <c r="J27" s="4" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B28" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C28" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="C28" s="3" t="s">
-        <v>83</v>
-      </c>
       <c r="D28" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E28" s="3">
         <v>102</v>
       </c>
       <c r="F28" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G28" s="5" t="s">
         <v>40</v>
-      </c>
-      <c r="G28" s="5" t="s">
-        <v>41</v>
       </c>
       <c r="H28" s="3">
         <v>7</v>
@@ -2809,30 +2816,30 @@
         <v>0</v>
       </c>
       <c r="J28" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="330" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B29" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C29" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C29" s="3" t="s">
-        <v>54</v>
-      </c>
       <c r="D29" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E29" s="3">
         <v>115</v>
       </c>
       <c r="F29" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="G29" s="5" t="s">
         <v>55</v>
-      </c>
-      <c r="G29" s="5" t="s">
-        <v>56</v>
       </c>
       <c r="H29" s="3">
         <v>0</v>
@@ -2841,30 +2848,30 @@
         <v>2</v>
       </c>
       <c r="J29" s="4" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B30" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C30" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="C30" s="3" t="s">
-        <v>49</v>
-      </c>
       <c r="D30" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E30" s="3">
         <v>127</v>
       </c>
       <c r="F30" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G30" s="5" t="s">
         <v>40</v>
-      </c>
-      <c r="G30" s="5" t="s">
-        <v>41</v>
       </c>
       <c r="H30" s="3">
         <v>1</v>
@@ -2873,30 +2880,30 @@
         <v>2</v>
       </c>
       <c r="J30" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="31" spans="1:10" ht="165" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B31" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C31" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C31" s="3" t="s">
-        <v>58</v>
-      </c>
       <c r="D31" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E31" s="3">
         <v>141</v>
       </c>
       <c r="F31" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="G31" s="5" t="s">
         <v>59</v>
-      </c>
-      <c r="G31" s="5" t="s">
-        <v>60</v>
       </c>
       <c r="H31" s="3">
         <v>2</v>
@@ -2905,30 +2912,30 @@
         <v>2</v>
       </c>
       <c r="J31" s="4" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="240" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E32" s="3">
         <v>132</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G32" s="5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H32" s="3">
         <v>3</v>
@@ -2937,21 +2944,21 @@
         <v>2</v>
       </c>
       <c r="J32" s="4" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E33" s="3">
         <v>116</v>
@@ -2960,7 +2967,7 @@
         <v>11</v>
       </c>
       <c r="G33" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H33" s="3">
         <v>5</v>
@@ -2969,10 +2976,10 @@
         <v>2</v>
       </c>
       <c r="J33" s="4" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>15</v>
       </c>
@@ -2989,7 +2996,7 @@
         <v>1</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G34" s="5" t="s">
         <v>19</v>
@@ -3001,7 +3008,7 @@
         <v>0</v>
       </c>
       <c r="J34" s="4" t="s">
-        <v>20</v>
+        <v>273</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
@@ -3009,13 +3016,13 @@
         <v>15</v>
       </c>
       <c r="B35" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C35" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C35" s="3" t="s">
+      <c r="D35" s="3" t="s">
         <v>31</v>
-      </c>
-      <c r="D35" s="3" t="s">
-        <v>32</v>
       </c>
       <c r="E35" s="3">
         <v>2</v>
@@ -3024,7 +3031,7 @@
         <v>11</v>
       </c>
       <c r="G35" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H35" s="3">
         <v>2</v>
@@ -3033,7 +3040,7 @@
         <v>0</v>
       </c>
       <c r="J35" s="4" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
@@ -3041,13 +3048,13 @@
         <v>15</v>
       </c>
       <c r="B36" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C36" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C36" s="3" t="s">
-        <v>25</v>
-      </c>
       <c r="D36" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E36" s="3">
         <v>118</v>
@@ -3056,7 +3063,7 @@
         <v>18</v>
       </c>
       <c r="G36" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H36" s="3">
         <v>3</v>
@@ -3065,7 +3072,7 @@
         <v>0</v>
       </c>
       <c r="J36" s="4" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="37" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -3073,22 +3080,22 @@
         <v>15</v>
       </c>
       <c r="B37" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C37" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C37" s="3" t="s">
-        <v>28</v>
-      </c>
       <c r="D37" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E37" s="3">
         <v>5</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G37" s="6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H37" s="3">
         <v>4</v>
@@ -3097,7 +3104,7 @@
         <v>0</v>
       </c>
       <c r="J37" s="4" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
@@ -3105,13 +3112,13 @@
         <v>15</v>
       </c>
       <c r="B38" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C38" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C38" s="3" t="s">
-        <v>22</v>
-      </c>
       <c r="D38" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E38" s="3">
         <v>4</v>
@@ -3129,7 +3136,7 @@
         <v>2</v>
       </c>
       <c r="J38" s="4" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="39" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3137,13 +3144,13 @@
         <v>15</v>
       </c>
       <c r="B39" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C39" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C39" s="3" t="s">
-        <v>35</v>
-      </c>
       <c r="D39" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E39" s="3">
         <v>3</v>
@@ -3152,7 +3159,7 @@
         <v>11</v>
       </c>
       <c r="G39" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H39" s="3">
         <v>2</v>
@@ -3161,31 +3168,31 @@
         <v>2</v>
       </c>
       <c r="J39" s="4" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="40" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B40" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="C40" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="C40" s="3" t="s">
-        <v>145</v>
-      </c>
       <c r="D40" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E40" s="3">
         <v>201</v>
       </c>
       <c r="F40" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="G40" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="G40" s="3" t="s">
-        <v>146</v>
-      </c>
       <c r="H40" s="3">
         <v>0</v>
       </c>
@@ -3193,21 +3200,21 @@
         <v>0</v>
       </c>
       <c r="J40" s="4" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B41" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="C41" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="C41" s="3" t="s">
+      <c r="D41" s="3" t="s">
         <v>139</v>
-      </c>
-      <c r="D41" s="3" t="s">
-        <v>140</v>
       </c>
       <c r="E41" s="3">
         <v>203</v>
@@ -3216,7 +3223,7 @@
         <v>11</v>
       </c>
       <c r="G41" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H41" s="3">
         <v>1</v>
@@ -3225,30 +3232,30 @@
         <v>0</v>
       </c>
       <c r="J41" s="4" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="42" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E42" s="3">
         <v>202</v>
       </c>
       <c r="F42" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G42" s="5" t="s">
         <v>40</v>
-      </c>
-      <c r="G42" s="5" t="s">
-        <v>41</v>
       </c>
       <c r="H42" s="3">
         <v>2</v>
@@ -3257,30 +3264,30 @@
         <v>0</v>
       </c>
       <c r="J42" s="4" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B43" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="C43" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="C43" s="3" t="s">
+      <c r="D43" s="3" t="s">
         <v>149</v>
-      </c>
-      <c r="D43" s="3" t="s">
-        <v>150</v>
       </c>
       <c r="E43" s="3">
         <v>213</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="H43" s="3">
         <v>4</v>
@@ -3289,30 +3296,30 @@
         <v>0</v>
       </c>
       <c r="J43" s="4" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E44" s="3">
         <v>210</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="H44" s="3">
         <v>6</v>
@@ -3321,30 +3328,30 @@
         <v>0</v>
       </c>
       <c r="J44" s="4" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E45" s="3">
         <v>211</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="H45" s="3">
         <v>7</v>
@@ -3353,30 +3360,30 @@
         <v>0</v>
       </c>
       <c r="J45" s="4" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E46" s="3">
         <v>212</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H46" s="3">
         <v>8</v>
@@ -3385,21 +3392,21 @@
         <v>0</v>
       </c>
       <c r="J46" s="4" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="47" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="B47" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="B47" s="3" t="s">
+      <c r="C47" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="D47" s="3" t="s">
         <v>128</v>
-      </c>
-      <c r="C47" s="3" t="s">
-        <v>253</v>
-      </c>
-      <c r="D47" s="3" t="s">
-        <v>129</v>
       </c>
       <c r="E47" s="3">
         <v>220</v>
@@ -3408,7 +3415,7 @@
         <v>11</v>
       </c>
       <c r="G47" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H47" s="3">
         <v>0</v>
@@ -3417,21 +3424,21 @@
         <v>2</v>
       </c>
       <c r="J47" s="4" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="48" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E48" s="3">
         <v>221</v>
@@ -3440,7 +3447,7 @@
         <v>11</v>
       </c>
       <c r="G48" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H48" s="3">
         <v>1</v>
@@ -3449,21 +3456,21 @@
         <v>2</v>
       </c>
       <c r="J48" s="4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="49" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E49" s="3">
         <v>222</v>
@@ -3472,7 +3479,7 @@
         <v>11</v>
       </c>
       <c r="G49" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H49" s="3">
         <v>2</v>
@@ -3481,21 +3488,21 @@
         <v>2</v>
       </c>
       <c r="J49" s="4" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="50" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E50" s="3">
         <v>223</v>
@@ -3504,7 +3511,7 @@
         <v>11</v>
       </c>
       <c r="G50" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H50" s="3">
         <v>3</v>
@@ -3513,21 +3520,21 @@
         <v>2</v>
       </c>
       <c r="J50" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="51" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E51" s="3">
         <v>224</v>
@@ -3536,7 +3543,7 @@
         <v>11</v>
       </c>
       <c r="G51" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H51" s="3">
         <v>4</v>
@@ -3545,21 +3552,21 @@
         <v>2</v>
       </c>
       <c r="J51" s="4" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="52" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E52" s="3">
         <v>225</v>
@@ -3568,7 +3575,7 @@
         <v>11</v>
       </c>
       <c r="G52" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H52" s="3">
         <v>5</v>
@@ -3577,21 +3584,21 @@
         <v>2</v>
       </c>
       <c r="J52" s="4" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="53" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E53" s="3">
         <v>226</v>
@@ -3600,7 +3607,7 @@
         <v>11</v>
       </c>
       <c r="G53" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H53" s="3">
         <v>6</v>
@@ -3609,21 +3616,21 @@
         <v>2</v>
       </c>
       <c r="J53" s="4" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="54" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B54" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="C54" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="C54" s="3" t="s">
-        <v>136</v>
-      </c>
       <c r="D54" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E54" s="3">
         <v>227</v>
@@ -3632,7 +3639,7 @@
         <v>11</v>
       </c>
       <c r="G54" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H54" s="3">
         <v>7</v>
@@ -3641,7 +3648,7 @@
         <v>2</v>
       </c>
       <c r="J54" s="4" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
@@ -3649,10 +3656,10 @@
         <v>9</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E55" s="3">
         <v>121</v>
@@ -3667,7 +3674,7 @@
         <v>0</v>
       </c>
       <c r="J55" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
@@ -3675,16 +3682,16 @@
         <v>9</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E56" s="3">
         <v>144</v>
       </c>
       <c r="F56" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G56" s="5"/>
       <c r="H56" s="3">
@@ -3694,7 +3701,7 @@
         <v>0</v>
       </c>
       <c r="J56" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="57" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3717,7 +3724,7 @@
         <v>0</v>
       </c>
       <c r="J57" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
@@ -3745,26 +3752,26 @@
     </row>
     <row r="59" spans="1:10" ht="210" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B59" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="B59" s="3" t="s">
+      <c r="C59" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="C59" s="3" t="s">
-        <v>70</v>
-      </c>
       <c r="D59" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E59" s="3">
         <v>137</v>
       </c>
       <c r="F59" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="G59" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="G59" s="5" t="s">
-        <v>72</v>
-      </c>
       <c r="H59" s="3">
         <v>0</v>
       </c>
@@ -3772,30 +3779,30 @@
         <v>0</v>
       </c>
       <c r="J59" s="4" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B60" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C60" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C60" s="3" t="s">
-        <v>74</v>
-      </c>
       <c r="D60" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E60" s="3">
         <v>140</v>
       </c>
       <c r="F60" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G60" s="5" t="s">
         <v>40</v>
-      </c>
-      <c r="G60" s="5" t="s">
-        <v>41</v>
       </c>
       <c r="H60" s="3">
         <v>1</v>
@@ -3804,30 +3811,30 @@
         <v>0</v>
       </c>
       <c r="J60" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="61" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B61" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C61" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="C61" s="3" t="s">
-        <v>79</v>
-      </c>
       <c r="D61" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E61" s="3">
         <v>136</v>
       </c>
       <c r="F61" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G61" s="5" t="s">
         <v>40</v>
-      </c>
-      <c r="G61" s="5" t="s">
-        <v>41</v>
       </c>
       <c r="H61" s="3">
         <v>2</v>
@@ -3836,30 +3843,30 @@
         <v>0</v>
       </c>
       <c r="J61" s="4" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="62" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B62" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C62" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="C62" s="3" t="s">
-        <v>81</v>
-      </c>
       <c r="D62" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E62" s="3">
         <v>138</v>
       </c>
       <c r="F62" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G62" s="5" t="s">
         <v>40</v>
-      </c>
-      <c r="G62" s="5" t="s">
-        <v>41</v>
       </c>
       <c r="H62" s="3">
         <v>3</v>
@@ -3868,30 +3875,30 @@
         <v>0</v>
       </c>
       <c r="J62" s="4" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="63" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B63" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C63" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="C63" s="3" t="s">
-        <v>77</v>
-      </c>
       <c r="D63" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E63" s="3">
         <v>122</v>
       </c>
       <c r="F63" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G63" s="5" t="s">
         <v>40</v>
-      </c>
-      <c r="G63" s="5" t="s">
-        <v>41</v>
       </c>
       <c r="H63" s="3">
         <v>5</v>
@@ -3900,30 +3907,30 @@
         <v>0</v>
       </c>
       <c r="J63" s="4" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="64" spans="1:10" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B64" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="C64" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="C64" s="3" t="s">
-        <v>184</v>
-      </c>
       <c r="D64" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E64" s="3">
         <v>139</v>
       </c>
       <c r="F64" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G64" s="5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H64" s="3">
         <v>6</v>
@@ -3932,30 +3939,30 @@
         <v>0</v>
       </c>
       <c r="J64" s="4" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="65" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B65" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C65" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="C65" s="3" t="s">
-        <v>90</v>
-      </c>
       <c r="D65" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E65" s="3">
         <v>143</v>
       </c>
       <c r="F65" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G65" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H65" s="3">
         <v>8</v>
@@ -3964,30 +3971,30 @@
         <v>0</v>
       </c>
       <c r="J65" s="4" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="66" spans="1:10" ht="210" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B66" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C66" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="C66" s="3" t="s">
-        <v>85</v>
-      </c>
       <c r="D66" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E66" s="3">
         <v>120</v>
       </c>
       <c r="F66" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="G66" s="5" t="s">
         <v>169</v>
-      </c>
-      <c r="G66" s="5" t="s">
-        <v>170</v>
       </c>
       <c r="H66" s="3">
         <v>0</v>
@@ -3996,30 +4003,30 @@
         <v>2</v>
       </c>
       <c r="J66" s="8" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B67" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C67" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="C67" s="3" t="s">
-        <v>87</v>
-      </c>
       <c r="D67" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E67" s="3">
         <v>145</v>
       </c>
       <c r="F67" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G67" s="5" t="s">
         <v>40</v>
-      </c>
-      <c r="G67" s="5" t="s">
-        <v>41</v>
       </c>
       <c r="H67" s="3">
         <v>1</v>
@@ -4028,30 +4035,30 @@
         <v>2</v>
       </c>
       <c r="J67" s="4" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="68" spans="1:10" ht="405" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B68" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="C68" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="C68" s="3" t="s">
-        <v>161</v>
-      </c>
       <c r="D68" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E68" s="3">
         <v>112</v>
       </c>
       <c r="F68" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G68" s="5" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="H68" s="3">
         <v>3</v>
@@ -4060,21 +4067,21 @@
         <v>2</v>
       </c>
       <c r="J68" s="4" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="69" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B69" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="C69" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="C69" s="3" t="s">
-        <v>159</v>
-      </c>
       <c r="D69" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E69" s="3">
         <v>110</v>
@@ -4083,7 +4090,7 @@
         <v>11</v>
       </c>
       <c r="G69" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H69" s="3">
         <v>4</v>
@@ -4092,30 +4099,30 @@
         <v>2</v>
       </c>
       <c r="J69" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="70" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B70" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="C70" s="3" t="s">
         <v>197</v>
       </c>
-      <c r="C70" s="3" t="s">
-        <v>198</v>
-      </c>
       <c r="D70" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E70" s="3">
         <v>111</v>
       </c>
       <c r="F70" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="G70" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H70" s="3">
         <v>5</v>
@@ -4124,7 +4131,7 @@
         <v>2</v>
       </c>
       <c r="J70" s="4" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add a new goal of CLEAR - give away all of your own seeds. Correct an error with the Diffusion sower. Added Diffusion V2 game. Changed stores behavior, so that it may be used in CLEAR and DEPRIVE games to show whose turn it is without showing seed counts. Added Enlightenment game. Updated tests and documentation.
</commit_message>
<xml_diff>
--- a/src/game_params.xlsx
+++ b/src/game_params.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Activity_Data\Mancala_github\MancalaGames\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0D50BB2-5B39-4AE7-9527-66ECF58E4FF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FB7ACB9-A9AB-4E67-9F39-FE2BBACE4F89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="966" uniqueCount="274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="273">
   <si>
     <t>tab</t>
   </si>
@@ -669,9 +669,6 @@
   </si>
   <si>
     <t>Number of holes on each side of the board.</t>
-  </si>
-  <si>
-    <t>Are stores present on the game board?</t>
   </si>
   <si>
     <t>When a player has no allowable moves on their turn, they must pass, and continue to do so until they have allowable moves or the game is over. The game is over when there is a clear winner or tie condition, or when neither player has an allowable move.</t>
@@ -959,20 +956,6 @@
 For example: In Weg each round ends when neither player has a valid move. The board is then set up again after determining who owns what territory (holes). Rounds continue until one player has claimed sufficient territory to be declared the game winner (e.g. ownership of 10 or more holes).
 In the case of a round win or tie  a new starter is determined via ROUND_STARTER and  the board is reset according to ROUND_FILL.
 BLOCKS are used in many games and set between rounds based on the seed placement. TERRITORY GOAL games adjust hole ownership between rounds.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The overall goal of the game. Defines how a player wins.
-- MAX_SEEDS: The goal is to collect the maximum number of seeds.
-  + If the game is not played in rounds, the game will end when one player has more than half of the total seeds.
-  + If the game is played in rounds, the round end condition is determined by ROUNDS. These games end when one player has collected sufficient seeds to prevent the opponent from filling the required number of holes. Generally, the required number of holes is one but this may be increased by setting GPARAM_ONE. 
-  + In MAX_SEEDS/ROUNDS games the player only controls the holes on their side of the board, where as, in TERRITORY games a player may control holes on either side of the board.
-- DEPRIVE: eliminate all of your opponents seeds.
-  + If a player has no seeds at the start of their turn, they loose. If a player has no moves at the start of their turn, then the game outcome is determined by who has seeds: If both players have seeds, the game ends in a tie. If the current player has seeds, but the previous player does not, then the current player wins because they forced the previous player to give away all their seeds.
-  + GRANDSLAM must be legal for DEPRIVE games.
-  + Deprive games cannot be played in ROUNDS, use STORES, or use children. Additionally, the following options are incompatible with DEPRIVE games: MOVEUNLOCK, MUSTPASS, MUSTSHARE and NO_SIDES.
-- TERRITORY: claim ownership of holes. Each round the ownership of holes is determined by the number of seeds captured in the previous round. In a TERRITORY game without rounds, the winner is the player that gained the most territory during play. 
-  + TERRITORY games require STORES and that GPARAM_ONE be set to a value between the number of holes and two times the number of holes.
-  + TERRITORY games are incompatible with NO_SIDES, START_PATTERN, GRANDSLAM of NOT_LEGAL, ALLOW_RULE of OPP_OR_EMPTY, </t>
   </si>
   <si>
     <t>The round fill method determines which holes are filled and how many seeds they are filled with when setting up for a new round.
@@ -1013,14 +996,29 @@
 GOAL of Max Seeds and ROUNDS: defines the minimum number of holes each player must have to continue the game. The player with fewer seeds must have enough seeds to fill gparam_one holes each with start_seeds in order to continue playing.  There is no rounding of seed counts as in territory games.</t>
   </si>
   <si>
-    <t>The name of the Game Class. Currently one of:
-Mancala: allows setting all parameters though there are limited combinations.
-Diffusion: has unique sow method and win conditions. Only very limited parameters may be changed from defaults.</t>
-  </si>
-  <si>
     <t>The name of the Game Class. One of:
 Mancala: allows setting all parameters though there are limited combinations.
 Diffusion: has unique sow method and win conditions. Only very limited parameters may be changed from defaults.</t>
+  </si>
+  <si>
+    <t>True when stores are present on the game board. For games with GOAL of DEPRIVE or CLEAR, stores can be used to show whose turn it is (seed counts will not be sown).</t>
+  </si>
+  <si>
+    <t>The overall goal of the game. Defines how a player wins.
+- MAX_SEEDS: The goal is to collect the maximum number of seeds.
+  + If the game is not played in rounds, the game will end when one player has more than half of the total seeds.
+  + If the game is played in rounds, the round end condition is determined by ROUNDS. These games end when one player has collected sufficient seeds to prevent the opponent from filling the required number of holes. Generally, the required number of holes is one but this may be increased by setting GPARAM_ONE. 
+  + In MAX_SEEDS/ROUNDS games the player only controls the holes on their side of the board, where as, in TERRITORY games a player may control holes on either side of the board.
+- DEPRIVE: eliminate all of your opponents seeds.
+  + If a player has no seeds at the start of their turn, they loose. If a player has no moves at the start of their turn, then the game outcome is determined by who has seeds: If both players have seeds, the game ends in a tie. If the current player has seeds, but the previous player does not, then the current player wins because they forced the previous player to give away all their seeds.
+  + GRANDSLAM must be legal for DEPRIVE games.
+  + Deprive games cannot be played in ROUNDS or use children. Additionally, the following options are incompatible with DEPRIVE games: MOVEUNLOCK, MUSTPASS and MUSTSHARE.
+- TERRITORY: claim ownership of holes. Each round the ownership of holes is determined by the number of seeds captured in the previous round. In a TERRITORY game without rounds, the winner is the player that gained the most territory during play. 
+  + TERRITORY games require STORES and that GPARAM_ONE be set to a value between the number of holes and two times the number of holes.
+  + TERRITORY games are incompatible with NO_SIDES, START_PATTERN, GRANDSLAM of NOT_LEGAL, ALLOW_RULE of OPP_OR_EMPTY.
+- CLEAR: clear seeds from your own holes.
+  + Moves must always be possible so MIN_MOVE must be 1 and ALLOW_RULE single_all_to_zero may not be used.
+  + GRANDSLAM must be legal for DEPRIVE games.  Deprive games cannot be played in ROUNDS or use children. Additionally, the following options are incompatible with DEPRIVE games: MOVEUNLOCK, MUSTPASS and MUSTSHARE.</t>
   </si>
 </sst>
 </file>
@@ -1905,8 +1903,8 @@
   <dimension ref="A1:J70"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J34" sqref="J34"/>
+      <pane ySplit="1" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2016,7 +2014,7 @@
         <v>0</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="195" x14ac:dyDescent="0.25">
@@ -2048,7 +2046,7 @@
         <v>0</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2080,7 +2078,7 @@
         <v>0</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -2144,7 +2142,7 @@
         <v>0</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -2176,7 +2174,7 @@
         <v>0</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="105" x14ac:dyDescent="0.25">
@@ -2208,7 +2206,7 @@
         <v>0</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="105" x14ac:dyDescent="0.25">
@@ -2240,7 +2238,7 @@
         <v>0</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2272,7 +2270,7 @@
         <v>0</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="120" x14ac:dyDescent="0.25">
@@ -2304,7 +2302,7 @@
         <v>0</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -2336,7 +2334,7 @@
         <v>2</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2368,7 +2366,7 @@
         <v>2</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -2400,7 +2398,7 @@
         <v>2</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="180" x14ac:dyDescent="0.25">
@@ -2432,7 +2430,7 @@
         <v>2</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2464,7 +2462,7 @@
         <v>2</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
@@ -2528,7 +2526,7 @@
         <v>2</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="120" x14ac:dyDescent="0.25">
@@ -2560,7 +2558,7 @@
         <v>2</v>
       </c>
       <c r="J20" s="4" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -2592,7 +2590,7 @@
         <v>2</v>
       </c>
       <c r="J21" s="4" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="150" x14ac:dyDescent="0.25">
@@ -2624,10 +2622,10 @@
         <v>2</v>
       </c>
       <c r="J22" s="4" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>36</v>
       </c>
@@ -2656,7 +2654,7 @@
         <v>0</v>
       </c>
       <c r="J23" s="4" t="s">
-        <v>208</v>
+        <v>271</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -2688,7 +2686,7 @@
         <v>0</v>
       </c>
       <c r="J24" s="4" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="225" x14ac:dyDescent="0.25">
@@ -2711,7 +2709,7 @@
         <v>42</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="H25" s="3">
         <v>4</v>
@@ -2720,7 +2718,7 @@
         <v>0</v>
       </c>
       <c r="J25" s="4" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -2784,7 +2782,7 @@
         <v>0</v>
       </c>
       <c r="J27" s="4" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -2819,7 +2817,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="330" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" ht="390" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>36</v>
       </c>
@@ -2848,7 +2846,7 @@
         <v>2</v>
       </c>
       <c r="J29" s="4" t="s">
-        <v>268</v>
+        <v>272</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2880,7 +2878,7 @@
         <v>2</v>
       </c>
       <c r="J30" s="4" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="31" spans="1:10" ht="165" x14ac:dyDescent="0.25">
@@ -2912,7 +2910,7 @@
         <v>2</v>
       </c>
       <c r="J31" s="4" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="240" x14ac:dyDescent="0.25">
@@ -2944,7 +2942,7 @@
         <v>2</v>
       </c>
       <c r="J32" s="4" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -2955,7 +2953,7 @@
         <v>170</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D33" s="3" t="s">
         <v>22</v>
@@ -2976,7 +2974,7 @@
         <v>2</v>
       </c>
       <c r="J33" s="4" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="34" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -3008,7 +3006,7 @@
         <v>0</v>
       </c>
       <c r="J34" s="4" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
@@ -3200,7 +3198,7 @@
         <v>0</v>
       </c>
       <c r="J40" s="4" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
@@ -3232,7 +3230,7 @@
         <v>0</v>
       </c>
       <c r="J41" s="4" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="42" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3264,7 +3262,7 @@
         <v>0</v>
       </c>
       <c r="J42" s="4" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
@@ -3287,7 +3285,7 @@
         <v>90</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="H43" s="3">
         <v>4</v>
@@ -3296,7 +3294,7 @@
         <v>0</v>
       </c>
       <c r="J43" s="4" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -3319,7 +3317,7 @@
         <v>90</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="H44" s="3">
         <v>6</v>
@@ -3328,7 +3326,7 @@
         <v>0</v>
       </c>
       <c r="J44" s="4" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
@@ -3351,7 +3349,7 @@
         <v>90</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="H45" s="3">
         <v>7</v>
@@ -3360,7 +3358,7 @@
         <v>0</v>
       </c>
       <c r="J45" s="4" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
@@ -3392,7 +3390,7 @@
         <v>0</v>
       </c>
       <c r="J46" s="4" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="47" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -3403,7 +3401,7 @@
         <v>127</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D47" s="3" t="s">
         <v>128</v>
@@ -3424,7 +3422,7 @@
         <v>2</v>
       </c>
       <c r="J47" s="4" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="48" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -3435,7 +3433,7 @@
         <v>129</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D48" s="3" t="s">
         <v>128</v>
@@ -3456,7 +3454,7 @@
         <v>2</v>
       </c>
       <c r="J48" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="49" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -3467,7 +3465,7 @@
         <v>130</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D49" s="3" t="s">
         <v>128</v>
@@ -3488,7 +3486,7 @@
         <v>2</v>
       </c>
       <c r="J49" s="4" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="50" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3499,7 +3497,7 @@
         <v>131</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D50" s="3" t="s">
         <v>128</v>
@@ -3520,7 +3518,7 @@
         <v>2</v>
       </c>
       <c r="J50" s="4" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="51" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -3531,7 +3529,7 @@
         <v>132</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D51" s="3" t="s">
         <v>128</v>
@@ -3552,7 +3550,7 @@
         <v>2</v>
       </c>
       <c r="J51" s="4" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="52" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -3563,7 +3561,7 @@
         <v>133</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D52" s="3" t="s">
         <v>128</v>
@@ -3584,7 +3582,7 @@
         <v>2</v>
       </c>
       <c r="J52" s="4" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="53" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -3595,7 +3593,7 @@
         <v>136</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D53" s="3" t="s">
         <v>128</v>
@@ -3616,7 +3614,7 @@
         <v>2</v>
       </c>
       <c r="J53" s="4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="54" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -3648,7 +3646,7 @@
         <v>2</v>
       </c>
       <c r="J54" s="4" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
@@ -3779,7 +3777,7 @@
         <v>0</v>
       </c>
       <c r="J59" s="4" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
@@ -3843,7 +3841,7 @@
         <v>0</v>
       </c>
       <c r="J61" s="4" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="62" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3875,7 +3873,7 @@
         <v>0</v>
       </c>
       <c r="J62" s="4" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="63" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3907,7 +3905,7 @@
         <v>0</v>
       </c>
       <c r="J63" s="4" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="64" spans="1:10" ht="409.5" x14ac:dyDescent="0.25">
@@ -3939,7 +3937,7 @@
         <v>0</v>
       </c>
       <c r="J64" s="4" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="65" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -3971,7 +3969,7 @@
         <v>0</v>
       </c>
       <c r="J65" s="4" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="66" spans="1:10" ht="210" x14ac:dyDescent="0.25">
@@ -4003,7 +4001,7 @@
         <v>2</v>
       </c>
       <c r="J66" s="8" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.25">
@@ -4035,7 +4033,7 @@
         <v>2</v>
       </c>
       <c r="J67" s="4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="68" spans="1:10" ht="405" x14ac:dyDescent="0.25">
@@ -4067,7 +4065,7 @@
         <v>2</v>
       </c>
       <c r="J68" s="4" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="69" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -4131,7 +4129,7 @@
         <v>2</v>
       </c>
       <c r="J70" s="4" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updates to Enlightenment, Kalah and Valah. Clarified repeat_turn as addin not multiplier.
</commit_message>
<xml_diff>
--- a/src/game_params.xlsx
+++ b/src/game_params.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Activity_Data\Mancala_github\MancalaGames\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FB7ACB9-A9AB-4E67-9F39-FE2BBACE4F89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{620EE7FF-6317-4DAD-9365-2B8A6F2FF363}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4365" yWindow="1725" windowWidth="23295" windowHeight="13800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="game_params" sheetId="1" r:id="rId1"/>
@@ -838,9 +838,6 @@
     <t>Evens Multiplier</t>
   </si>
   <si>
-    <t>Repeat Turn Multiplier</t>
-  </si>
-  <si>
     <t>Child Count Multiplier</t>
   </si>
   <si>
@@ -1019,6 +1016,9 @@
 - CLEAR: clear seeds from your own holes.
   + Moves must always be possible so MIN_MOVE must be 1 and ALLOW_RULE single_all_to_zero may not be used.
   + GRANDSLAM must be legal for DEPRIVE games.  Deprive games cannot be played in ROUNDS or use children. Additionally, the following options are incompatible with DEPRIVE games: MOVEUNLOCK, MUSTPASS and MUSTSHARE.</t>
+  </si>
+  <si>
+    <t>Repeat Turn Addin</t>
   </si>
 </sst>
 </file>
@@ -1903,8 +1903,8 @@
   <dimension ref="A1:J70"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J29" sqref="J29"/>
+      <pane ySplit="1" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C53" sqref="C53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2206,7 +2206,7 @@
         <v>0</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="105" x14ac:dyDescent="0.25">
@@ -2238,7 +2238,7 @@
         <v>0</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2302,7 +2302,7 @@
         <v>0</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -2398,7 +2398,7 @@
         <v>2</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="180" x14ac:dyDescent="0.25">
@@ -2430,7 +2430,7 @@
         <v>2</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2558,7 +2558,7 @@
         <v>2</v>
       </c>
       <c r="J20" s="4" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -2622,7 +2622,7 @@
         <v>2</v>
       </c>
       <c r="J22" s="4" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2654,7 +2654,7 @@
         <v>0</v>
       </c>
       <c r="J23" s="4" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -2709,7 +2709,7 @@
         <v>42</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="H25" s="3">
         <v>4</v>
@@ -2718,7 +2718,7 @@
         <v>0</v>
       </c>
       <c r="J25" s="4" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -2782,7 +2782,7 @@
         <v>0</v>
       </c>
       <c r="J27" s="4" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -2846,7 +2846,7 @@
         <v>2</v>
       </c>
       <c r="J29" s="4" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2974,7 +2974,7 @@
         <v>2</v>
       </c>
       <c r="J33" s="4" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="34" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -3006,7 +3006,7 @@
         <v>0</v>
       </c>
       <c r="J34" s="4" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
@@ -3198,7 +3198,7 @@
         <v>0</v>
       </c>
       <c r="J40" s="4" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
@@ -3285,7 +3285,7 @@
         <v>90</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="H43" s="3">
         <v>4</v>
@@ -3317,7 +3317,7 @@
         <v>90</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="H44" s="3">
         <v>6</v>
@@ -3349,7 +3349,7 @@
         <v>90</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="H45" s="3">
         <v>7</v>
@@ -3401,7 +3401,7 @@
         <v>127</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D47" s="3" t="s">
         <v>128</v>
@@ -3433,7 +3433,7 @@
         <v>129</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D48" s="3" t="s">
         <v>128</v>
@@ -3465,7 +3465,7 @@
         <v>130</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D49" s="3" t="s">
         <v>128</v>
@@ -3497,7 +3497,7 @@
         <v>131</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D50" s="3" t="s">
         <v>128</v>
@@ -3529,7 +3529,7 @@
         <v>132</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D51" s="3" t="s">
         <v>128</v>
@@ -3593,7 +3593,7 @@
         <v>136</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>246</v>
+        <v>272</v>
       </c>
       <c r="D53" s="3" t="s">
         <v>128</v>
@@ -3937,7 +3937,7 @@
         <v>0</v>
       </c>
       <c r="J64" s="4" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="65" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -4001,7 +4001,7 @@
         <v>2</v>
       </c>
       <c r="J66" s="8" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.25">
@@ -4065,7 +4065,7 @@
         <v>2</v>
       </c>
       <c r="J68" s="4" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="69" spans="1:10" ht="30" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added RoundTally - games played in rounds where a specific win condition is used for the game win (other than control of holes). Configured with new goals. Broke up the ender into a few files (was > 1000). A few missing bits from renaming the drawer are included. New win parameter is not yet on the UI. Test coverage not complete. GameClass document not updated. No preconfigured games use the new goals.
</commit_message>
<xml_diff>
--- a/src/game_params.xlsx
+++ b/src/game_params.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Activity_Data\Mancala_github\MancalaGames\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{620EE7FF-6317-4DAD-9365-2B8A6F2FF363}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93AD0942-26A1-4B42-BA75-E51BA9CD5C86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4365" yWindow="1725" windowWidth="23295" windowHeight="13800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="game_params" sheetId="1" r:id="rId1"/>
@@ -955,20 +955,6 @@
 BLOCKS are used in many games and set between rounds based on the seed placement. TERRITORY GOAL games adjust hole ownership between rounds.</t>
   </si>
   <si>
-    <t>The round fill method determines which holes are filled and how many seeds they are filled with when setting up for a new round.
-Several round fill mechanisms use the same general approach called the Empty Hole Method. The loser of the previous round will end up with empty holes. These holes are not playable if BLOCKS are used; otherwise they are playable.
-The seeds each player accummulated in the previous round are distributed into holes with exactly the same number in each. That number of seeds is NBR_START. The winner will fill all of their holes and put any remaining seeds into their own store. The loser will fill as many holes as they can with nbr_start seeds and put any remaining seeds (fewer than nbr_start) into their own store.
-LEFT_FILE, RIGHT_FILL and OUTSIDE_FILL define which holes that the loser must fill. UCHOOSE allows the loser to choose which holes have seeds.
-- NOT_APPLICABLE: round fill doesn't need to be specified: either the game not played in rounds (DEPRIVE game included) or game goal is TERRITORY (all holes filled).
-- LEFT_FILL: fill the round loser's holes from the player's left with nbr_start seeds each.  
-- RIGHT_FILL: fill the round loser's holes from the player's right with nbr_start seeds each. 
-- OUTSIDE_FILL: fill the round loser's holes from the outside ends toward the middle with nbr_start seeds each. Leftmost, rightmost, 2nd leftmost, 2nd rightmost, etc. until the seeds are used up.
-- EVEN_FILL: fill all holes (both sides) with the same number of seeds; determined by dividing the losers seeds by the number of holes per side. If that is not playable based on the minimum number of seeds required for a move (MIN_MOVE); extra seeds are put in each players leftmost hole. Any extra seeds are put in each player's store.
-- SHORTEN: the number of holes that the round loser can fill with NBR_START seeds are fill on both sides, other holes are left empty. Holes are filled opposite eachother. If BLOCKS is selected, the board is shortened to the number of holes filled (empty holes are blocked and out of play). If the game uses children, they will not be created if the board size is reduced to 3 or less.
-- UCHOOSE: allow user to choose which holes have seeds (are not blocked) when ROUNDS and BLOCKS are used.
-- UMOVE: allow the loser to choose where seeds are placed. At least one seed must be placed in each hole and the game must be playable (at least one hole has MIN_MOVE seeds), remaining seeds are placed in the store. The winner's layout is the same layout but reflected.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Games with children allow players to claim holes. These child holes are an extension of the stores and seeds in them count towards a win. Making a child stops any multiple lap sowing, moves cannot start from children, and they cannot be captured (except for special rules associated with WEGs).
 - NOCHILD: children are not used.
 - NORMAL: children are made when a final seeds sows a hole to CHILD_CVT.
@@ -1001,6 +987,9 @@
     <t>True when stores are present on the game board. For games with GOAL of DEPRIVE or CLEAR, stores can be used to show whose turn it is (seed counts will not be sown).</t>
   </si>
   <si>
+    <t>Repeat Turn Addin</t>
+  </si>
+  <si>
     <t>The overall goal of the game. Defines how a player wins.
 - MAX_SEEDS: The goal is to collect the maximum number of seeds.
   + If the game is not played in rounds, the game will end when one player has more than half of the total seeds.
@@ -1015,10 +1004,25 @@
   + TERRITORY games are incompatible with NO_SIDES, START_PATTERN, GRANDSLAM of NOT_LEGAL, ALLOW_RULE of OPP_OR_EMPTY.
 - CLEAR: clear seeds from your own holes.
   + Moves must always be possible so MIN_MOVE must be 1 and ALLOW_RULE single_all_to_zero may not be used.
-  + GRANDSLAM must be legal for DEPRIVE games.  Deprive games cannot be played in ROUNDS or use children. Additionally, the following options are incompatible with DEPRIVE games: MOVEUNLOCK, MUSTPASS and MUSTSHARE.</t>
-  </si>
-  <si>
-    <t>Repeat Turn Addin</t>
+  + GRANDSLAM must be legal for DEPRIVE games.  Deprive games cannot be played in ROUNDS or use children. Additionally, the following options are incompatible with DEPRIVE games: MOVEUNLOCK, MUSTPASS and MUSTSHARE.
+- RND_WIN_COUNT:  win gparam_one rounds. ROUND_FILL is not used; each round is setup as the start of the game.
+- RND_SEED_COUNT: collect gparam_one across several rounds. ROUND_FILL is not used; each round is setup as the start of the game.
+- RND_EXTRA_SEEDS: collect gparam_one extra seeds (winner - loser seeds).  ROUND_FILL is not used; each round is setup as the start of the game.
+- RND_POINTS:  score gparam_one points. WIN is 1 point. WIN and skunk (&gt; 3/4 of seeds) is 2 points.  ROUND_FILL is not used; each round is setup as the start of the game.</t>
+  </si>
+  <si>
+    <t>The round fill method determines which holes are filled and how many seeds they are filled with when setting up for a new round.
+Several round fill mechanisms use the same general approach called the Empty Hole Method. The loser of the previous round will end up with empty holes. These holes are not playable if BLOCKS are used; otherwise they are playable. This method is not used for RND_ GOAL games.
+The seeds each player accummulated in the previous round are distributed into holes with exactly the same number in each. That number of seeds is NBR_START. The winner will fill all of their holes and put any remaining seeds into their own store. The loser will fill as many holes as they can with nbr_start seeds and put any remaining seeds (fewer than nbr_start) into their own store.
+LEFT_FILE, RIGHT_FILL and OUTSIDE_FILL define which holes that the loser must fill. UCHOOSE allows the loser to choose which holes have seeds.
+- NOT_APPLICABLE: round fill doesn't need to be specified: either the game not played in rounds (DEPRIVE game included) or game goal is TERRITORY (all holes filled).
+- LEFT_FILL: fill the round loser's holes from the player's left with nbr_start seeds each.  
+- RIGHT_FILL: fill the round loser's holes from the player's right with nbr_start seeds each. 
+- OUTSIDE_FILL: fill the round loser's holes from the outside ends toward the middle with nbr_start seeds each. Leftmost, rightmost, 2nd leftmost, 2nd rightmost, etc. until the seeds are used up.
+- EVEN_FILL: fill all holes (both sides) with the same number of seeds; determined by dividing the losers seeds by the number of holes per side. If that is not playable based on the minimum number of seeds required for a move (MIN_MOVE); extra seeds are put in each players leftmost hole. Any extra seeds are put in each player's store.
+- SHORTEN: the number of holes that the round loser can fill with NBR_START seeds are fill on both sides, other holes are left empty. Holes are filled opposite eachother. If BLOCKS is selected, the board is shortened to the number of holes filled (empty holes are blocked and out of play). If the game uses children, they will not be created if the board size is reduced to 3 or less.
+- UCHOOSE: allow user to choose which holes have seeds (are not blocked) when ROUNDS and BLOCKS are used.
+- UMOVE: allow the loser to choose where seeds are placed. At least one seed must be placed in each hole and the game must be playable (at least one hole has MIN_MOVE seeds), remaining seeds are placed in the store. The winner's layout is the same layout but reflected.</t>
   </si>
 </sst>
 </file>
@@ -1903,8 +1907,8 @@
   <dimension ref="A1:J70"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C53" sqref="C53"/>
+      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1912,12 +1916,13 @@
     <col min="1" max="1" width="11.5703125" style="3" customWidth="1"/>
     <col min="2" max="2" width="16" style="3" customWidth="1"/>
     <col min="3" max="3" width="24.42578125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="22.5703125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="16.5703125" style="3" customWidth="1"/>
     <col min="5" max="5" width="11.5703125" style="3" customWidth="1"/>
     <col min="6" max="6" width="14.7109375" style="3" customWidth="1"/>
-    <col min="7" max="7" width="21.140625" style="3" customWidth="1"/>
-    <col min="8" max="9" width="9.140625" style="3" customWidth="1"/>
-    <col min="10" max="10" width="114.85546875" style="4" customWidth="1"/>
+    <col min="7" max="7" width="16.42578125" style="3" customWidth="1"/>
+    <col min="8" max="8" width="6.7109375" style="3" customWidth="1"/>
+    <col min="9" max="9" width="7.28515625" style="3" customWidth="1"/>
+    <col min="10" max="10" width="136.42578125" style="4" customWidth="1"/>
     <col min="11" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
@@ -2654,7 +2659,7 @@
         <v>0</v>
       </c>
       <c r="J23" s="4" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -2753,7 +2758,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="405" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" ht="330" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>36</v>
       </c>
@@ -2782,7 +2787,7 @@
         <v>0</v>
       </c>
       <c r="J27" s="4" t="s">
-        <v>266</v>
+        <v>272</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -2817,7 +2822,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="390" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>36</v>
       </c>
@@ -2974,7 +2979,7 @@
         <v>2</v>
       </c>
       <c r="J33" s="4" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="34" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -3006,7 +3011,7 @@
         <v>0</v>
       </c>
       <c r="J34" s="4" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
@@ -3593,7 +3598,7 @@
         <v>136</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="D53" s="3" t="s">
         <v>128</v>
@@ -4065,7 +4070,7 @@
         <v>2</v>
       </c>
       <c r="J68" s="4" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="69" spans="1:10" ht="30" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Integrated round tally progress onto MancalaUI. Clarified comments. Unit test code for RoundTallyWinner and QuitRoundTally. Unit test coverage to 100% Corrected some bugs found.
</commit_message>
<xml_diff>
--- a/src/game_params.xlsx
+++ b/src/game_params.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Activity_Data\Mancala_github\MancalaGames\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93AD0942-26A1-4B42-BA75-E51BA9CD5C86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5461F3BC-4544-41BE-B8E5-7428B7118B0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -974,11 +974,6 @@
 </t>
   </si>
   <si>
-    <t>GOAL of Territory: defines the number of holes needed for a win. The number of holes for each player are computed by rounding the number of seeds collected divided by the number of start seeds per hole.
-GOAL of Deprive and Blocked Divert Sower: defines the number of seeds needed to close/block holes (sow_blkd_div).
-GOAL of Max Seeds and ROUNDS: defines the minimum number of holes each player must have to continue the game. The player with fewer seeds must have enough seeds to fill gparam_one holes each with start_seeds in order to continue playing.  There is no rounding of seed counts as in territory games.</t>
-  </si>
-  <si>
     <t>The name of the Game Class. One of:
 Mancala: allows setting all parameters though there are limited combinations.
 Diffusion: has unique sow method and win conditions. Only very limited parameters may be changed from defaults.</t>
@@ -988,6 +983,20 @@
   </si>
   <si>
     <t>Repeat Turn Addin</t>
+  </si>
+  <si>
+    <t>The round fill method determines which holes are filled and how many seeds they are filled with when setting up for a new round.
+Several round fill mechanisms use the same general approach called the Empty Hole Method. The loser of the previous round will end up with empty holes. These holes are not playable if BLOCKS are used; otherwise they are playable. This method is not used for RND_ GOAL games.
+The seeds each player accummulated in the previous round are distributed into holes with exactly the same number in each. That number of seeds is NBR_START. The winner will fill all of their holes and put any remaining seeds into their own store. The loser will fill as many holes as they can with nbr_start seeds and put any remaining seeds (fewer than nbr_start) into their own store.
+LEFT_FILE, RIGHT_FILL and OUTSIDE_FILL define which holes that the loser must fill. UCHOOSE allows the loser to choose which holes have seeds.
+- NOT_APPLICABLE: round fill doesn't need to be specified: either the game not played in rounds (DEPRIVE game included) or game goal is TERRITORY (all holes filled).
+- LEFT_FILL: fill the round loser's holes from the player's left with nbr_start seeds each.  
+- RIGHT_FILL: fill the round loser's holes from the player's right with nbr_start seeds each. 
+- OUTSIDE_FILL: fill the round loser's holes from the outside ends toward the middle with nbr_start seeds each. Leftmost, rightmost, 2nd leftmost, 2nd rightmost, etc. until the seeds are used up.
+- EVEN_FILL: fill all holes (both sides) with the same number of seeds; determined by dividing the losers seeds by the number of holes per side. If that is not playable based on the minimum number of seeds required for a move (MIN_MOVE); extra seeds are put in each players leftmost hole. Any extra seeds are put in each player's store.
+- SHORTEN: the number of holes that the round loser can fill with NBR_START seeds are fill on both sides, other holes are left empty. Holes are filled opposite eachother. If BLOCKS is selected, the board is shortened to the number of holes filled (empty holes are blocked and out of play). If the game uses children, they will not be created if the board size is reduced to 3 or less.
+- UCHOOSE: allow user to choose which holes have seeds (are not blocked) when ROUNDS and BLOCKS are used.
+- UMOVE: allow the loser to choose where seeds are placed. At least one seed must be placed in each hole and the game must be playable (at least one hole has MIN_MOVE seeds), remaining seeds are placed in the store. The winner's layout is the same layout but reflected.</t>
   </si>
   <si>
     <t>The overall goal of the game. Defines how a player wins.
@@ -1006,23 +1015,15 @@
   + Moves must always be possible so MIN_MOVE must be 1 and ALLOW_RULE single_all_to_zero may not be used.
   + GRANDSLAM must be legal for DEPRIVE games.  Deprive games cannot be played in ROUNDS or use children. Additionally, the following options are incompatible with DEPRIVE games: MOVEUNLOCK, MUSTPASS and MUSTSHARE.
 - RND_WIN_COUNT:  win gparam_one rounds. ROUND_FILL is not used; each round is setup as the start of the game.
-- RND_SEED_COUNT: collect gparam_one across several rounds. ROUND_FILL is not used; each round is setup as the start of the game.
+- RND_SEED_COUNT: collect gparam_one seeds across several rounds. ROUND_FILL is not used; each round is setup as the start of the game.
 - RND_EXTRA_SEEDS: collect gparam_one extra seeds (winner - loser seeds).  ROUND_FILL is not used; each round is setup as the start of the game.
-- RND_POINTS:  score gparam_one points. WIN is 1 point. WIN and skunk (&gt; 3/4 of seeds) is 2 points.  ROUND_FILL is not used; each round is setup as the start of the game.</t>
-  </si>
-  <si>
-    <t>The round fill method determines which holes are filled and how many seeds they are filled with when setting up for a new round.
-Several round fill mechanisms use the same general approach called the Empty Hole Method. The loser of the previous round will end up with empty holes. These holes are not playable if BLOCKS are used; otherwise they are playable. This method is not used for RND_ GOAL games.
-The seeds each player accummulated in the previous round are distributed into holes with exactly the same number in each. That number of seeds is NBR_START. The winner will fill all of their holes and put any remaining seeds into their own store. The loser will fill as many holes as they can with nbr_start seeds and put any remaining seeds (fewer than nbr_start) into their own store.
-LEFT_FILE, RIGHT_FILL and OUTSIDE_FILL define which holes that the loser must fill. UCHOOSE allows the loser to choose which holes have seeds.
-- NOT_APPLICABLE: round fill doesn't need to be specified: either the game not played in rounds (DEPRIVE game included) or game goal is TERRITORY (all holes filled).
-- LEFT_FILL: fill the round loser's holes from the player's left with nbr_start seeds each.  
-- RIGHT_FILL: fill the round loser's holes from the player's right with nbr_start seeds each. 
-- OUTSIDE_FILL: fill the round loser's holes from the outside ends toward the middle with nbr_start seeds each. Leftmost, rightmost, 2nd leftmost, 2nd rightmost, etc. until the seeds are used up.
-- EVEN_FILL: fill all holes (both sides) with the same number of seeds; determined by dividing the losers seeds by the number of holes per side. If that is not playable based on the minimum number of seeds required for a move (MIN_MOVE); extra seeds are put in each players leftmost hole. Any extra seeds are put in each player's store.
-- SHORTEN: the number of holes that the round loser can fill with NBR_START seeds are fill on both sides, other holes are left empty. Holes are filled opposite eachother. If BLOCKS is selected, the board is shortened to the number of holes filled (empty holes are blocked and out of play). If the game uses children, they will not be created if the board size is reduced to 3 or less.
-- UCHOOSE: allow user to choose which holes have seeds (are not blocked) when ROUNDS and BLOCKS are used.
-- UMOVE: allow the loser to choose where seeds are placed. At least one seed must be placed in each hole and the game must be playable (at least one hole has MIN_MOVE seeds), remaining seeds are placed in the store. The winner's layout is the same layout but reflected.</t>
+- RND_POINTS:  score gparam_one points. WIN is 1 point. WIN and skunk (&gt; 3/4 of total seeds) is 2 points.  ROUND_FILL is not used; each round is setup as the start of the game.</t>
+  </si>
+  <si>
+    <t>GOAL of Territory: defines the number of holes needed for a win. The number of holes for each player are computed by rounding the number of seeds collected divided by the number of start seeds per hole.
+Goal of Deprive and Blocked Divert Sower: defines the number of seeds needed to close/block holes (sow_blkd_div).
+Goal of Max Seeds and ROUNDS: defines the minimum number of holes each player must have to continue the game. The player with fewer seeds must have enough seeds to fill gparam_one holes each with start_seeds in order to continue playing.  There is no rounding of seed counts as in territory games.
+RND_* Goals: number of specified parameter for win.</t>
   </si>
 </sst>
 </file>
@@ -1907,8 +1908,8 @@
   <dimension ref="A1:J70"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J27" sqref="J27"/>
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J33" sqref="J33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2659,7 +2660,7 @@
         <v>0</v>
       </c>
       <c r="J23" s="4" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -2787,7 +2788,7 @@
         <v>0</v>
       </c>
       <c r="J27" s="4" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -2950,7 +2951,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>36</v>
       </c>
@@ -2979,7 +2980,7 @@
         <v>2</v>
       </c>
       <c r="J33" s="4" t="s">
-        <v>267</v>
+        <v>272</v>
       </c>
     </row>
     <row r="34" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -3011,7 +3012,7 @@
         <v>0</v>
       </c>
       <c r="J34" s="4" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
@@ -3598,7 +3599,7 @@
         <v>136</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D53" s="3" t="s">
         <v>128</v>

</xml_diff>

<commit_message>
Corrected interface issue with MancalaUI and Mancala for round tally tie to game tally UI and some crashes when round tally wasn't created. Change gparam_one to goal_param because that is all it can be used for. Added variant description to Dabuda and Kalah. Added Waurie.
</commit_message>
<xml_diff>
--- a/src/game_params.xlsx
+++ b/src/game_params.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Activity_Data\Mancala_github\MancalaGames\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5461F3BC-4544-41BE-B8E5-7428B7118B0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24C3AD39-BCA4-408B-BD4B-1C9D341332B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33225" yWindow="585" windowWidth="19695" windowHeight="14895" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="game_params" sheetId="1" r:id="rId1"/>
@@ -550,9 +550,6 @@
     <t>OFF</t>
   </si>
   <si>
-    <t>gparam_one</t>
-  </si>
-  <si>
     <t>mlength</t>
   </si>
   <si>
@@ -572,11 +569,6 @@
   </si>
   <si>
     <t>Capture Next</t>
-  </si>
-  <si>
-    <t>Blocks remove holes from play and are shown on the UI with an X.
-When used with ROUNDS, the holes not filled from the player with fewer seeds are blocked and thus out of play for the round.
-When used with DEPRIVE, SOW_BLCK_DIV and GPARAM_ONE holes are closed (blocked and removed from play) when sown to GPARAM_ONE seeds.</t>
   </si>
   <si>
     <t>Prescribed Opening Move</t>
@@ -820,9 +812,6 @@
     <t xml:space="preserve">Moves maybe made from any hole, independent of the side of the board. Moves need to specify side, position and directions.  </t>
   </si>
   <si>
-    <t>General Input</t>
-  </si>
-  <si>
     <t>If an opponent has no moves at the start of your turn, you must make seeds available to them if you can. This condition is enforced by only activating holes on the UI which will make seeds available to the opponent.</t>
   </si>
   <si>
@@ -864,23 +853,6 @@
 minimaxer: an Alpha-Beta Pruning MiniMaxer
 negamaxer: minimaxer with a very minor optimization for alternating turn games (no repeat turns). Uses minimaxer depths for difficulties.
 montecarlo_ts: a Monte Carlo Tree Search player.</t>
-  </si>
-  <si>
-    <t>Special sow rules add additional behavior or restrictions to the sowing phase:
-- NONE: there is no special sowing rule.
-- SOW_BLKD_DIV: If the final seed of an individual sow lands on the opposite side of the board and brings the contents of that hole to GPARAM_ONE seeds, the hole is closed closed (blocked). In single lap games, the hole's seeds are removed from play. In multilap games, the seeds are used to continue sowing.
-  + When sowing, blocked holes on your own side of the board are skipped  and blocked holes on opponent's side are diverted out of play or captured.
-  +  Game GOAL must be DEPRIVE and all of the associated restrictions apply. NOCAPTFIRST maybe used to prevent closing holes on the first move. Capture mechanisms other than closing holes are not supported. The minimum move must be 1 and thus SOW_START is incompatible.  ALLOW_RULE may not be used to limit allowable moves.  SKIP_START and VISIT_OPP are not supported with SOW_BLKD_DIV.  MLAPS of LAPPER_NEXT is not supported with SOW_BLKD_DIV(_NR).
-- SOW_BLKD_DIV_NR: Behaves the same as SOW_BLKD_DIV except that each player's rightmost hole cannot be closed. 
-- OWN_SOW_CAPT_ALL: The hole OWNer captures all holes that are sown to meet the simple capture criteria no matter who sowed them.  The simple capture criteria are: evens, min, max and capture on. Other criteria are enforced: side of the board, unlocked, and not child.
-  + The capture is done by the hole owner, so the non-sower may capture seeds while their opponents sows. If the game GOAL is TERRITORY the capturer is the hole owner; otherwise each player captures from their own side of the board no matter who is sowing. 
-  + If MLAPS is LAPPER and the final seed sown for any lap meets the simple capture criteria for that hole, the contents of the hole are captured by the sower and not the hole owner and the turn is over. For CAPTTWOOUT, CAPT_NEXT and CROSSCAPT captures, the sower always does the final capture.
-  + GRANDSLAM rules are not applied. NOCAPTFIRST prevents these capture for the first move.
-- SOW_SOW_CAPT_ALL: Similar to OWN_SOW_CAPT_ALL but only the SOWer captures seeds from their opponent's holes. 
-  + If mlaps is LAPPER and the final seed sown for any lap meets the capture criteria, the contents of the hole are captured by the sower and not the hole owner and the turn is over.
-  + GRANDSLAM rules are not applied. NOCAPTFIRST prevents this capture for the first move.
-- NO_SOW_OPP_2S: Don't sow into opponents holes with 2 seeds.
-- CHANGE_DIR_LAP: Change the direction for each lap sown. Generally used with UDIR_HOLES so the player may choose the first direction.</t>
   </si>
   <si>
     <t>Determines if seeds from more the start hole are picked up and sown:
@@ -999,31 +971,59 @@
 - UMOVE: allow the loser to choose where seeds are placed. At least one seed must be placed in each hole and the game must be playable (at least one hole has MIN_MOVE seeds), remaining seeds are placed in the store. The winner's layout is the same layout but reflected.</t>
   </si>
   <si>
+    <t>Blocks remove holes from play and are shown on the UI with an X.
+When used with ROUNDS, the holes not filled from the player with fewer seeds are blocked and thus out of play for the round.
+When used with DEPRIVE, SOW_BLCK_DIV and goal_param holes are closed (blocked and removed from play) when sown to goal_param seeds.</t>
+  </si>
+  <si>
     <t>The overall goal of the game. Defines how a player wins.
 - MAX_SEEDS: The goal is to collect the maximum number of seeds.
   + If the game is not played in rounds, the game will end when one player has more than half of the total seeds.
-  + If the game is played in rounds, the round end condition is determined by ROUNDS. These games end when one player has collected sufficient seeds to prevent the opponent from filling the required number of holes. Generally, the required number of holes is one but this may be increased by setting GPARAM_ONE. 
+  + If the game is played in rounds, the round end condition is determined by ROUNDS. These games end when one player has collected sufficient seeds to prevent the opponent from filling the required number of holes. Generally, the required number of holes is one but this may be increased by setting goal_param. 
   + In MAX_SEEDS/ROUNDS games the player only controls the holes on their side of the board, where as, in TERRITORY games a player may control holes on either side of the board.
 - DEPRIVE: eliminate all of your opponents seeds.
   + If a player has no seeds at the start of their turn, they loose. If a player has no moves at the start of their turn, then the game outcome is determined by who has seeds: If both players have seeds, the game ends in a tie. If the current player has seeds, but the previous player does not, then the current player wins because they forced the previous player to give away all their seeds.
   + GRANDSLAM must be legal for DEPRIVE games.
   + Deprive games cannot be played in ROUNDS or use children. Additionally, the following options are incompatible with DEPRIVE games: MOVEUNLOCK, MUSTPASS and MUSTSHARE.
 - TERRITORY: claim ownership of holes. Each round the ownership of holes is determined by the number of seeds captured in the previous round. In a TERRITORY game without rounds, the winner is the player that gained the most territory during play. 
-  + TERRITORY games require STORES and that GPARAM_ONE be set to a value between the number of holes and two times the number of holes.
+  + TERRITORY games require STORES and that goal_param be set to a value between the number of holes and two times the number of holes.
   + TERRITORY games are incompatible with NO_SIDES, START_PATTERN, GRANDSLAM of NOT_LEGAL, ALLOW_RULE of OPP_OR_EMPTY.
 - CLEAR: clear seeds from your own holes.
   + Moves must always be possible so MIN_MOVE must be 1 and ALLOW_RULE single_all_to_zero may not be used.
   + GRANDSLAM must be legal for DEPRIVE games.  Deprive games cannot be played in ROUNDS or use children. Additionally, the following options are incompatible with DEPRIVE games: MOVEUNLOCK, MUSTPASS and MUSTSHARE.
-- RND_WIN_COUNT:  win gparam_one rounds. ROUND_FILL is not used; each round is setup as the start of the game.
-- RND_SEED_COUNT: collect gparam_one seeds across several rounds. ROUND_FILL is not used; each round is setup as the start of the game.
-- RND_EXTRA_SEEDS: collect gparam_one extra seeds (winner - loser seeds).  ROUND_FILL is not used; each round is setup as the start of the game.
-- RND_POINTS:  score gparam_one points. WIN is 1 point. WIN and skunk (&gt; 3/4 of total seeds) is 2 points.  ROUND_FILL is not used; each round is setup as the start of the game.</t>
+- RND_WIN_COUNT:  win goal_param rounds. ROUND_FILL is not used; each round is setup as the start of the game.
+- RND_SEED_COUNT: collect goal_param seeds across several rounds. ROUND_FILL is not used; each round is setup as the start of the game.
+- RND_EXTRA_SEEDS: collect goal_param extra seeds (winner - loser seeds).  ROUND_FILL is not used; each round is setup as the start of the game.
+- RND_POINTS:  score goal_param points. WIN is 1 point. WIN and skunk (&gt; 3/4 of total seeds) is 2 points.  ROUND_FILL is not used; each round is setup as the start of the game.</t>
+  </si>
+  <si>
+    <t>goal_param</t>
   </si>
   <si>
     <t>GOAL of Territory: defines the number of holes needed for a win. The number of holes for each player are computed by rounding the number of seeds collected divided by the number of start seeds per hole.
 Goal of Deprive and Blocked Divert Sower: defines the number of seeds needed to close/block holes (sow_blkd_div).
-Goal of Max Seeds and ROUNDS: defines the minimum number of holes each player must have to continue the game. The player with fewer seeds must have enough seeds to fill gparam_one holes each with start_seeds in order to continue playing.  There is no rounding of seed counts as in territory games.
+Goal of Max Seeds and ROUNDS: defines the minimum number of holes each player must have to continue the game. The player with fewer seeds must have enough seeds to fill goal_param holes each with start_seeds in order to continue playing.  There is no rounding of seed counts as in territory games.
 RND_* Goals: number of specified parameter for win.</t>
+  </si>
+  <si>
+    <t>Special sow rules add additional behavior or restrictions to the sowing phase:
+- NONE: there is no special sowing rule.
+- SOW_BLKD_DIV: If the final seed of an individual sow lands on the opposite side of the board and brings the contents of that hole to goal_param seeds, the hole is closed closed (blocked). In single lap games, the hole's seeds are removed from play. In multilap games, the seeds are used to continue sowing.
+  + When sowing, blocked holes on your own side of the board are skipped  and blocked holes on opponent's side are diverted out of play or captured.
+  +  Game GOAL must be DEPRIVE and all of the associated restrictions apply. NOCAPTFIRST maybe used to prevent closing holes on the first move. Capture mechanisms other than closing holes are not supported. The minimum move must be 1 and thus SOW_START is incompatible.  ALLOW_RULE may not be used to limit allowable moves.  SKIP_START and VISIT_OPP are not supported with SOW_BLKD_DIV.  MLAPS of LAPPER_NEXT is not supported with SOW_BLKD_DIV(_NR).
+- SOW_BLKD_DIV_NR: Behaves the same as SOW_BLKD_DIV except that each player's rightmost hole cannot be closed. 
+- OWN_SOW_CAPT_ALL: The hole OWNer captures all holes that are sown to meet the simple capture criteria no matter who sowed them.  The simple capture criteria are: evens, min, max and capture on. Other criteria are enforced: side of the board, unlocked, and not child.
+  + The capture is done by the hole owner, so the non-sower may capture seeds while their opponents sows. If the game GOAL is TERRITORY the capturer is the hole owner; otherwise each player captures from their own side of the board no matter who is sowing. 
+  + If MLAPS is LAPPER and the final seed sown for any lap meets the simple capture criteria for that hole, the contents of the hole are captured by the sower and not the hole owner and the turn is over. For CAPTTWOOUT, CAPT_NEXT and CROSSCAPT captures, the sower always does the final capture.
+  + GRANDSLAM rules are not applied. NOCAPTFIRST prevents these capture for the first move.
+- SOW_SOW_CAPT_ALL: Similar to OWN_SOW_CAPT_ALL but only the SOWer captures seeds from their opponent's holes. 
+  + If mlaps is LAPPER and the final seed sown for any lap meets the capture criteria, the contents of the hole are captured by the sower and not the hole owner and the turn is over.
+  + GRANDSLAM rules are not applied. NOCAPTFIRST prevents this capture for the first move.
+- NO_SOW_OPP_2S: Don't sow into opponents holes with 2 seeds.
+- CHANGE_DIR_LAP: Change the direction for each lap sown. Generally used with UDIR_HOLES so the player may choose the first direction.</t>
+  </si>
+  <si>
+    <t>Goal Parameter</t>
   </si>
 </sst>
 </file>
@@ -1908,8 +1908,8 @@
   <dimension ref="A1:J70"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J33" sqref="J33"/>
+      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1941,7 +1941,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>4</v>
@@ -2020,10 +2020,10 @@
         <v>0</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="195" x14ac:dyDescent="0.25">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="180" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>60</v>
       </c>
@@ -2052,7 +2052,7 @@
         <v>0</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2084,7 +2084,7 @@
         <v>0</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -2148,10 +2148,10 @@
         <v>0</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>93</v>
       </c>
@@ -2180,10 +2180,10 @@
         <v>0</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="105" x14ac:dyDescent="0.25">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>93</v>
       </c>
@@ -2212,10 +2212,10 @@
         <v>0</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="105" x14ac:dyDescent="0.25">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>93</v>
       </c>
@@ -2244,7 +2244,7 @@
         <v>0</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2252,10 +2252,10 @@
         <v>93</v>
       </c>
       <c r="B11" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>176</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>177</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>22</v>
@@ -2276,10 +2276,10 @@
         <v>0</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="120" x14ac:dyDescent="0.25">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>93</v>
       </c>
@@ -2308,7 +2308,7 @@
         <v>0</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -2340,7 +2340,7 @@
         <v>2</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2348,10 +2348,10 @@
         <v>93</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>22</v>
@@ -2372,7 +2372,7 @@
         <v>2</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -2404,10 +2404,10 @@
         <v>2</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="180" x14ac:dyDescent="0.25">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="150" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>93</v>
       </c>
@@ -2436,7 +2436,7 @@
         <v>2</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2468,7 +2468,7 @@
         <v>2</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
@@ -2508,10 +2508,10 @@
         <v>93</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>22</v>
@@ -2532,10 +2532,10 @@
         <v>2</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="120" x14ac:dyDescent="0.25">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>93</v>
       </c>
@@ -2564,7 +2564,7 @@
         <v>2</v>
       </c>
       <c r="J20" s="4" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -2572,10 +2572,10 @@
         <v>93</v>
       </c>
       <c r="B21" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="C21" s="3" t="s">
         <v>174</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>175</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>22</v>
@@ -2596,18 +2596,18 @@
         <v>2</v>
       </c>
       <c r="J21" s="4" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" ht="150" x14ac:dyDescent="0.25">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="135" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>93</v>
       </c>
       <c r="B22" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="C22" s="3" t="s">
         <v>185</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>187</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>22</v>
@@ -2616,7 +2616,7 @@
         <v>131</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="G22" s="5" t="s">
         <v>167</v>
@@ -2628,7 +2628,7 @@
         <v>2</v>
       </c>
       <c r="J22" s="4" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2660,10 +2660,10 @@
         <v>0</v>
       </c>
       <c r="J23" s="4" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>36</v>
       </c>
@@ -2692,10 +2692,10 @@
         <v>0</v>
       </c>
       <c r="J24" s="4" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" ht="225" x14ac:dyDescent="0.25">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="210" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>36</v>
       </c>
@@ -2715,7 +2715,7 @@
         <v>42</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="H25" s="3">
         <v>4</v>
@@ -2724,7 +2724,7 @@
         <v>0</v>
       </c>
       <c r="J25" s="4" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -2756,7 +2756,7 @@
         <v>0</v>
       </c>
       <c r="J26" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="330" x14ac:dyDescent="0.25">
@@ -2764,10 +2764,10 @@
         <v>36</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>22</v>
@@ -2776,10 +2776,10 @@
         <v>133</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="H27" s="3">
         <v>6</v>
@@ -2788,10 +2788,10 @@
         <v>0</v>
       </c>
       <c r="J27" s="4" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>36</v>
       </c>
@@ -2820,7 +2820,7 @@
         <v>0</v>
       </c>
       <c r="J28" s="4" t="s">
-        <v>178</v>
+        <v>267</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="409.5" x14ac:dyDescent="0.25">
@@ -2852,30 +2852,30 @@
         <v>2</v>
       </c>
       <c r="J29" s="4" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>36</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>47</v>
+        <v>269</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>48</v>
+        <v>272</v>
       </c>
       <c r="D30" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E30" s="3">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>39</v>
+        <v>11</v>
       </c>
       <c r="G30" s="5" t="s">
-        <v>40</v>
+        <v>87</v>
       </c>
       <c r="H30" s="3">
         <v>1</v>
@@ -2884,30 +2884,30 @@
         <v>2</v>
       </c>
       <c r="J30" s="4" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" ht="165" x14ac:dyDescent="0.25">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>36</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="D31" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E31" s="3">
-        <v>141</v>
+        <v>127</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>58</v>
+        <v>39</v>
       </c>
       <c r="G31" s="5" t="s">
-        <v>59</v>
+        <v>40</v>
       </c>
       <c r="H31" s="3">
         <v>2</v>
@@ -2916,30 +2916,30 @@
         <v>2</v>
       </c>
       <c r="J31" s="4" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" ht="240" x14ac:dyDescent="0.25">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" ht="150" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>36</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>180</v>
+        <v>56</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>179</v>
+        <v>57</v>
       </c>
       <c r="D32" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E32" s="3">
-        <v>132</v>
+        <v>141</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>181</v>
+        <v>58</v>
       </c>
       <c r="G32" s="5" t="s">
-        <v>167</v>
+        <v>59</v>
       </c>
       <c r="H32" s="3">
         <v>3</v>
@@ -2948,39 +2948,39 @@
         <v>2</v>
       </c>
       <c r="J32" s="4" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" ht="105" x14ac:dyDescent="0.25">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" ht="180" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>36</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>170</v>
+        <v>178</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>241</v>
+        <v>177</v>
       </c>
       <c r="D33" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E33" s="3">
-        <v>116</v>
+        <v>132</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>11</v>
+        <v>179</v>
       </c>
       <c r="G33" s="5" t="s">
-        <v>87</v>
+        <v>167</v>
       </c>
       <c r="H33" s="3">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I33" s="3">
         <v>2</v>
       </c>
       <c r="J33" s="4" t="s">
-        <v>272</v>
+        <v>233</v>
       </c>
     </row>
     <row r="34" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -3012,7 +3012,7 @@
         <v>0</v>
       </c>
       <c r="J34" s="4" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
@@ -3044,7 +3044,7 @@
         <v>0</v>
       </c>
       <c r="J35" s="4" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
@@ -3076,10 +3076,10 @@
         <v>0</v>
       </c>
       <c r="J36" s="4" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>15</v>
       </c>
@@ -3108,7 +3108,7 @@
         <v>0</v>
       </c>
       <c r="J37" s="4" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
@@ -3140,7 +3140,7 @@
         <v>2</v>
       </c>
       <c r="J38" s="4" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="39" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3172,10 +3172,10 @@
         <v>2</v>
       </c>
       <c r="J39" s="4" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>126</v>
       </c>
@@ -3204,7 +3204,7 @@
         <v>0</v>
       </c>
       <c r="J40" s="4" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
@@ -3236,18 +3236,18 @@
         <v>0</v>
       </c>
       <c r="J41" s="4" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>126</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D42" s="3" t="s">
         <v>139</v>
@@ -3268,7 +3268,7 @@
         <v>0</v>
       </c>
       <c r="J42" s="4" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
@@ -3291,7 +3291,7 @@
         <v>90</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="H43" s="3">
         <v>4</v>
@@ -3300,10 +3300,10 @@
         <v>0</v>
       </c>
       <c r="J43" s="4" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>126</v>
       </c>
@@ -3323,7 +3323,7 @@
         <v>90</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="H44" s="3">
         <v>6</v>
@@ -3332,7 +3332,7 @@
         <v>0</v>
       </c>
       <c r="J44" s="4" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
@@ -3355,7 +3355,7 @@
         <v>90</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="H45" s="3">
         <v>7</v>
@@ -3364,7 +3364,7 @@
         <v>0</v>
       </c>
       <c r="J45" s="4" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
@@ -3396,7 +3396,7 @@
         <v>0</v>
       </c>
       <c r="J46" s="4" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="47" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -3407,7 +3407,7 @@
         <v>127</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="D47" s="3" t="s">
         <v>128</v>
@@ -3428,10 +3428,10 @@
         <v>2</v>
       </c>
       <c r="J47" s="4" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
         <v>126</v>
       </c>
@@ -3439,7 +3439,7 @@
         <v>129</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="D48" s="3" t="s">
         <v>128</v>
@@ -3460,10 +3460,10 @@
         <v>2</v>
       </c>
       <c r="J48" s="4" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
         <v>126</v>
       </c>
@@ -3471,7 +3471,7 @@
         <v>130</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="D49" s="3" t="s">
         <v>128</v>
@@ -3492,7 +3492,7 @@
         <v>2</v>
       </c>
       <c r="J49" s="4" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="50" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3503,7 +3503,7 @@
         <v>131</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="D50" s="3" t="s">
         <v>128</v>
@@ -3524,7 +3524,7 @@
         <v>2</v>
       </c>
       <c r="J50" s="4" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="51" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -3535,7 +3535,7 @@
         <v>132</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="D51" s="3" t="s">
         <v>128</v>
@@ -3556,7 +3556,7 @@
         <v>2</v>
       </c>
       <c r="J51" s="4" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="52" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -3567,7 +3567,7 @@
         <v>133</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="D52" s="3" t="s">
         <v>128</v>
@@ -3588,10 +3588,10 @@
         <v>2</v>
       </c>
       <c r="J52" s="4" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="53" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
         <v>126</v>
       </c>
@@ -3599,7 +3599,7 @@
         <v>136</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="D53" s="3" t="s">
         <v>128</v>
@@ -3620,10 +3620,10 @@
         <v>2</v>
       </c>
       <c r="J53" s="4" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="54" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
         <v>126</v>
       </c>
@@ -3652,7 +3652,7 @@
         <v>2</v>
       </c>
       <c r="J54" s="4" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
@@ -3660,7 +3660,7 @@
         <v>9</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D55" s="3" t="s">
         <v>22</v>
@@ -3678,7 +3678,7 @@
         <v>0</v>
       </c>
       <c r="J55" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
@@ -3705,10 +3705,10 @@
         <v>0</v>
       </c>
       <c r="J56" s="4" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="57" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
         <v>9</v>
       </c>
@@ -3754,7 +3754,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="59" spans="1:10" ht="210" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" ht="165" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
         <v>67</v>
       </c>
@@ -3783,7 +3783,7 @@
         <v>0</v>
       </c>
       <c r="J59" s="4" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
@@ -3818,7 +3818,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="61" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
         <v>67</v>
       </c>
@@ -3847,7 +3847,7 @@
         <v>0</v>
       </c>
       <c r="J61" s="4" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="62" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3879,7 +3879,7 @@
         <v>0</v>
       </c>
       <c r="J62" s="4" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="63" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3911,18 +3911,18 @@
         <v>0</v>
       </c>
       <c r="J63" s="4" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="64" spans="1:10" ht="409.5" x14ac:dyDescent="0.25">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" ht="375" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
         <v>67</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D64" s="3" t="s">
         <v>22</v>
@@ -3931,7 +3931,7 @@
         <v>139</v>
       </c>
       <c r="F64" s="3" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="G64" s="5" t="s">
         <v>167</v>
@@ -3943,10 +3943,10 @@
         <v>0</v>
       </c>
       <c r="J64" s="4" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="65" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
         <v>67</v>
       </c>
@@ -3975,10 +3975,10 @@
         <v>0</v>
       </c>
       <c r="J65" s="4" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="66" spans="1:10" ht="210" x14ac:dyDescent="0.25">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" ht="165" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
         <v>67</v>
       </c>
@@ -4007,7 +4007,7 @@
         <v>2</v>
       </c>
       <c r="J66" s="8" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.25">
@@ -4039,10 +4039,10 @@
         <v>2</v>
       </c>
       <c r="J67" s="4" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="68" spans="1:10" ht="405" x14ac:dyDescent="0.25">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" ht="360" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
         <v>67</v>
       </c>
@@ -4071,7 +4071,7 @@
         <v>2</v>
       </c>
       <c r="J68" s="4" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
     </row>
     <row r="69" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -4111,10 +4111,10 @@
         <v>67</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D70" s="3" t="s">
         <v>22</v>
@@ -4123,7 +4123,7 @@
         <v>111</v>
       </c>
       <c r="F70" s="3" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="G70" s="3" t="s">
         <v>167</v>
@@ -4135,7 +4135,7 @@
         <v>2</v>
       </c>
       <c r="J70" s="4" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Renamed nocaptfirst to nocaptmoves, changed to represent the number of opening moves during which captures are inhibited. Fixed an error in MLap Sowing where mlaps were ended for a capture when captures should have been inhibited.
</commit_message>
<xml_diff>
--- a/src/game_params.xlsx
+++ b/src/game_params.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Activity_Data\Mancala_github\MancalaGames\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24C3AD39-BCA4-408B-BD4B-1C9D341332B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C345DCE-62E4-4DB3-9C99-F7359F7410FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33225" yWindow="585" windowWidth="19695" windowHeight="14895" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="game_params" sheetId="1" r:id="rId1"/>
@@ -631,12 +631,6 @@
     <t>ChildRule</t>
   </si>
   <si>
-    <t>nocaptfirst</t>
-  </si>
-  <si>
-    <t>No Capture First Move</t>
-  </si>
-  <si>
     <t>NOT_APPLICABLE</t>
   </si>
   <si>
@@ -686,9 +680,6 @@
   <si>
     <t>Only allow cross capture if the player has sown onto the opposite side of board. 
 If a player ends on their own side of the board in an empty hole, but did not sow any opposite hole, they get a repeat turn.</t>
-  </si>
-  <si>
-    <t>Don't allow captures or closing of holes (SOW_RULE of SOW_BLKD_DIV) on the first move of the game or round.</t>
   </si>
   <si>
     <t>Number of end games played out from each expanded node. One value for each difficulty level (0-3).</t>
@@ -1006,24 +997,33 @@
 RND_* Goals: number of specified parameter for win.</t>
   </si>
   <si>
+    <t>Goal Parameter</t>
+  </si>
+  <si>
+    <t>nocaptmoves</t>
+  </si>
+  <si>
+    <t>Start Moves w/o Capture</t>
+  </si>
+  <si>
     <t>Special sow rules add additional behavior or restrictions to the sowing phase:
 - NONE: there is no special sowing rule.
 - SOW_BLKD_DIV: If the final seed of an individual sow lands on the opposite side of the board and brings the contents of that hole to goal_param seeds, the hole is closed closed (blocked). In single lap games, the hole's seeds are removed from play. In multilap games, the seeds are used to continue sowing.
   + When sowing, blocked holes on your own side of the board are skipped  and blocked holes on opponent's side are diverted out of play or captured.
-  +  Game GOAL must be DEPRIVE and all of the associated restrictions apply. NOCAPTFIRST maybe used to prevent closing holes on the first move. Capture mechanisms other than closing holes are not supported. The minimum move must be 1 and thus SOW_START is incompatible.  ALLOW_RULE may not be used to limit allowable moves.  SKIP_START and VISIT_OPP are not supported with SOW_BLKD_DIV.  MLAPS of LAPPER_NEXT is not supported with SOW_BLKD_DIV(_NR).
+  +  Game GOAL must be DEPRIVE and all of the associated restrictions apply. NOCAPTMOVES maybe used to prevent closing holes on the initial games moves. Capture mechanisms other than closing holes are not supported. The minimum move must be 1 and thus SOW_START is incompatible.  ALLOW_RULE may not be used to limit allowable moves.  SKIP_START and VISIT_OPP are not supported with SOW_BLKD_DIV.  MLAPS of LAPPER_NEXT is not supported with SOW_BLKD_DIV(_NR).
 - SOW_BLKD_DIV_NR: Behaves the same as SOW_BLKD_DIV except that each player's rightmost hole cannot be closed. 
 - OWN_SOW_CAPT_ALL: The hole OWNer captures all holes that are sown to meet the simple capture criteria no matter who sowed them.  The simple capture criteria are: evens, min, max and capture on. Other criteria are enforced: side of the board, unlocked, and not child.
   + The capture is done by the hole owner, so the non-sower may capture seeds while their opponents sows. If the game GOAL is TERRITORY the capturer is the hole owner; otherwise each player captures from their own side of the board no matter who is sowing. 
   + If MLAPS is LAPPER and the final seed sown for any lap meets the simple capture criteria for that hole, the contents of the hole are captured by the sower and not the hole owner and the turn is over. For CAPTTWOOUT, CAPT_NEXT and CROSSCAPT captures, the sower always does the final capture.
-  + GRANDSLAM rules are not applied. NOCAPTFIRST prevents these capture for the first move.
+  + GRANDSLAM rules are not applied. NOCAPTMOVES prevents these capture for the first moves.
 - SOW_SOW_CAPT_ALL: Similar to OWN_SOW_CAPT_ALL but only the SOWer captures seeds from their opponent's holes. 
   + If mlaps is LAPPER and the final seed sown for any lap meets the capture criteria, the contents of the hole are captured by the sower and not the hole owner and the turn is over.
-  + GRANDSLAM rules are not applied. NOCAPTFIRST prevents this capture for the first move.
+  + GRANDSLAM rules are not applied. NOCAPTMOVES prevents this capture for the first number of specified moves.
 - NO_SOW_OPP_2S: Don't sow into opponents holes with 2 seeds.
 - CHANGE_DIR_LAP: Change the direction for each lap sown. Generally used with UDIR_HOLES so the player may choose the first direction.</t>
   </si>
   <si>
-    <t>Goal Parameter</t>
+    <t>Don't allow captures or closing of holes (SOW_RULE of SOW_BLKD_DIV) for the first specified number of moves of the game or round.</t>
   </si>
 </sst>
 </file>
@@ -1908,8 +1908,8 @@
   <dimension ref="A1:J70"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D32" sqref="D32"/>
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2020,7 +2020,7 @@
         <v>0</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="180" x14ac:dyDescent="0.25">
@@ -2052,7 +2052,7 @@
         <v>0</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2084,7 +2084,7 @@
         <v>0</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -2148,7 +2148,7 @@
         <v>0</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -2180,7 +2180,7 @@
         <v>0</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -2212,7 +2212,7 @@
         <v>0</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -2244,7 +2244,7 @@
         <v>0</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2276,7 +2276,7 @@
         <v>0</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -2308,7 +2308,7 @@
         <v>0</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -2340,7 +2340,7 @@
         <v>2</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2372,7 +2372,7 @@
         <v>2</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -2404,7 +2404,7 @@
         <v>2</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="150" x14ac:dyDescent="0.25">
@@ -2436,7 +2436,7 @@
         <v>2</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2468,7 +2468,7 @@
         <v>2</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
@@ -2508,10 +2508,10 @@
         <v>93</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>197</v>
+        <v>269</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>198</v>
+        <v>270</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>22</v>
@@ -2520,10 +2520,10 @@
         <v>128</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>39</v>
+        <v>11</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>40</v>
+        <v>87</v>
       </c>
       <c r="H19" s="3">
         <v>6</v>
@@ -2532,7 +2532,7 @@
         <v>2</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>211</v>
+        <v>272</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -2564,7 +2564,7 @@
         <v>2</v>
       </c>
       <c r="J20" s="4" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -2596,7 +2596,7 @@
         <v>2</v>
       </c>
       <c r="J21" s="4" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="135" x14ac:dyDescent="0.25">
@@ -2628,7 +2628,7 @@
         <v>2</v>
       </c>
       <c r="J22" s="4" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2660,7 +2660,7 @@
         <v>0</v>
       </c>
       <c r="J23" s="4" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2692,7 +2692,7 @@
         <v>0</v>
       </c>
       <c r="J24" s="4" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="210" x14ac:dyDescent="0.25">
@@ -2715,7 +2715,7 @@
         <v>42</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="H25" s="3">
         <v>4</v>
@@ -2724,7 +2724,7 @@
         <v>0</v>
       </c>
       <c r="J25" s="4" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -2756,7 +2756,7 @@
         <v>0</v>
       </c>
       <c r="J26" s="4" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="330" x14ac:dyDescent="0.25">
@@ -2779,7 +2779,7 @@
         <v>190</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="H27" s="3">
         <v>6</v>
@@ -2788,7 +2788,7 @@
         <v>0</v>
       </c>
       <c r="J27" s="4" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -2820,7 +2820,7 @@
         <v>0</v>
       </c>
       <c r="J28" s="4" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="409.5" x14ac:dyDescent="0.25">
@@ -2852,7 +2852,7 @@
         <v>2</v>
       </c>
       <c r="J29" s="4" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="105" x14ac:dyDescent="0.25">
@@ -2860,10 +2860,10 @@
         <v>36</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="D30" s="3" t="s">
         <v>22</v>
@@ -2884,7 +2884,7 @@
         <v>2</v>
       </c>
       <c r="J30" s="4" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
@@ -2916,7 +2916,7 @@
         <v>2</v>
       </c>
       <c r="J31" s="4" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="150" x14ac:dyDescent="0.25">
@@ -2948,7 +2948,7 @@
         <v>2</v>
       </c>
       <c r="J32" s="4" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="180" x14ac:dyDescent="0.25">
@@ -2980,7 +2980,7 @@
         <v>2</v>
       </c>
       <c r="J33" s="4" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
     </row>
     <row r="34" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -3012,7 +3012,7 @@
         <v>0</v>
       </c>
       <c r="J34" s="4" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
@@ -3044,7 +3044,7 @@
         <v>0</v>
       </c>
       <c r="J35" s="4" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
@@ -3076,7 +3076,7 @@
         <v>0</v>
       </c>
       <c r="J36" s="4" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="37" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -3108,7 +3108,7 @@
         <v>0</v>
       </c>
       <c r="J37" s="4" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
@@ -3140,7 +3140,7 @@
         <v>2</v>
       </c>
       <c r="J38" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="39" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3172,7 +3172,7 @@
         <v>2</v>
       </c>
       <c r="J39" s="4" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="40" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -3204,7 +3204,7 @@
         <v>0</v>
       </c>
       <c r="J40" s="4" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
@@ -3236,7 +3236,7 @@
         <v>0</v>
       </c>
       <c r="J41" s="4" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
@@ -3268,7 +3268,7 @@
         <v>0</v>
       </c>
       <c r="J42" s="4" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
@@ -3291,7 +3291,7 @@
         <v>90</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="H43" s="3">
         <v>4</v>
@@ -3300,7 +3300,7 @@
         <v>0</v>
       </c>
       <c r="J43" s="4" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -3323,7 +3323,7 @@
         <v>90</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="H44" s="3">
         <v>6</v>
@@ -3332,7 +3332,7 @@
         <v>0</v>
       </c>
       <c r="J44" s="4" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
@@ -3355,7 +3355,7 @@
         <v>90</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="H45" s="3">
         <v>7</v>
@@ -3364,7 +3364,7 @@
         <v>0</v>
       </c>
       <c r="J45" s="4" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
@@ -3396,7 +3396,7 @@
         <v>0</v>
       </c>
       <c r="J46" s="4" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
     <row r="47" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -3407,7 +3407,7 @@
         <v>127</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="D47" s="3" t="s">
         <v>128</v>
@@ -3428,7 +3428,7 @@
         <v>2</v>
       </c>
       <c r="J47" s="4" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="48" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -3439,7 +3439,7 @@
         <v>129</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="D48" s="3" t="s">
         <v>128</v>
@@ -3460,7 +3460,7 @@
         <v>2</v>
       </c>
       <c r="J48" s="4" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
     <row r="49" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3471,7 +3471,7 @@
         <v>130</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="D49" s="3" t="s">
         <v>128</v>
@@ -3492,7 +3492,7 @@
         <v>2</v>
       </c>
       <c r="J49" s="4" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
     </row>
     <row r="50" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3503,7 +3503,7 @@
         <v>131</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="D50" s="3" t="s">
         <v>128</v>
@@ -3524,7 +3524,7 @@
         <v>2</v>
       </c>
       <c r="J50" s="4" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
     </row>
     <row r="51" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -3535,7 +3535,7 @@
         <v>132</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="D51" s="3" t="s">
         <v>128</v>
@@ -3556,7 +3556,7 @@
         <v>2</v>
       </c>
       <c r="J51" s="4" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
     </row>
     <row r="52" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -3567,7 +3567,7 @@
         <v>133</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="D52" s="3" t="s">
         <v>128</v>
@@ -3588,7 +3588,7 @@
         <v>2</v>
       </c>
       <c r="J52" s="4" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
     </row>
     <row r="53" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -3599,7 +3599,7 @@
         <v>136</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="D53" s="3" t="s">
         <v>128</v>
@@ -3620,7 +3620,7 @@
         <v>2</v>
       </c>
       <c r="J53" s="4" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
     </row>
     <row r="54" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -3652,7 +3652,7 @@
         <v>2</v>
       </c>
       <c r="J54" s="4" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
@@ -3783,7 +3783,7 @@
         <v>0</v>
       </c>
       <c r="J59" s="4" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
@@ -3847,7 +3847,7 @@
         <v>0</v>
       </c>
       <c r="J61" s="4" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="62" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3879,7 +3879,7 @@
         <v>0</v>
       </c>
       <c r="J62" s="4" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
     </row>
     <row r="63" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3911,7 +3911,7 @@
         <v>0</v>
       </c>
       <c r="J63" s="4" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="64" spans="1:10" ht="375" x14ac:dyDescent="0.25">
@@ -3975,7 +3975,7 @@
         <v>0</v>
       </c>
       <c r="J65" s="4" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
     </row>
     <row r="66" spans="1:10" ht="165" x14ac:dyDescent="0.25">
@@ -4007,7 +4007,7 @@
         <v>2</v>
       </c>
       <c r="J66" s="8" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.25">
@@ -4039,7 +4039,7 @@
         <v>2</v>
       </c>
       <c r="J67" s="4" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
     </row>
     <row r="68" spans="1:10" ht="360" x14ac:dyDescent="0.25">
@@ -4071,7 +4071,7 @@
         <v>2</v>
       </c>
       <c r="J68" s="4" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
     </row>
     <row r="69" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -4135,7 +4135,7 @@
         <v>2</v>
       </c>
       <c r="J70" s="4" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Increased capt_on to 6 checkboxes on MancalaGames. Added sow_param to parameterize sow rules. Added SowMaxN which uses sow_param. Added a UI command to end a round without ending the game (unless it would end anyway). Updated the round-end-move decorators to end the round. Added Mangala_II and Urim.
</commit_message>
<xml_diff>
--- a/src/game_params.xlsx
+++ b/src/game_params.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Activity_Data\Mancala_github\MancalaGames\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C345DCE-62E4-4DB3-9C99-F7359F7410FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF223F98-8DB8-41B6-B525-67387AB714D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="game_params" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">game_params!$A$1:$J$70</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">game_params!$A$1:$J$71</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="276">
   <si>
     <t>tab</t>
   </si>
@@ -916,25 +916,6 @@
 For example: In Weg each round ends when neither player has a valid move. The board is then set up again after determining who owns what territory (holes). Rounds continue until one player has claimed sufficient territory to be declared the game winner (e.g. ownership of 10 or more holes).
 In the case of a round win or tie  a new starter is determined via ROUND_STARTER and  the board is reset according to ROUND_FILL.
 BLOCKS are used in many games and set between rounds based on the seed placement. TERRITORY GOAL games adjust hole ownership between rounds.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Games with children allow players to claim holes. These child holes are an extension of the stores and seeds in them count towards a win. Making a child stops any multiple lap sowing, moves cannot start from children, and they cannot be captured (except for special rules associated with WEGs).
-- NOCHILD: children are not used.
-- NORMAL: children are made when a final seeds sows a hole to CHILD_CVT.
-- WALDA: STORES are not supported. Captures are instead moved into waldas, thus a player may not capture until they have created a walda. 
-  + Walda locations are limited.  Each player may create up to 6 waldas: on either end of each side of the board and the next two outer holes on their own side of the board. Note that there are only 8 total places that waldas maybe created.
-- ONE_CHILD: only one child allowed per player.
-  + Children must not be symmetrically opposite eachother. For example,  in a 9 hole per side game with holes numbered as follows, tuzdeks may not be in the same numbered holes:
-  + 9 8 7 6 5 4 3 2 1
-  + 1 2 3 4 5 6 7 8 9 
-  + Depending on sow direction some holes are prohibited from being made children: 
-  + CW &amp; CCW:  the last of your opponents holes that you would sow into may not be made a child. CW holes numbered 1 above and CCW holes numberd 9 above.
-  + SPLIT: no end holes may be made children.
-  + Used to create tuzdek style children along with CHILD_RULE of OPP_ONLY.
-- WEG: children maybe created in holes owned by the opponent. Ending a sow in an opponent's weg captures the seed just sown and one more (if there is one); generally, the player gets to play again (per CAPT_RTURN). WEGs are supported for TERRITORY games only (hole ownership required).
-- BULL: create one bull if final seed sows to CHILD_CVT, create two bulls if the final two seeds are sown to CHILD_CVT-1 and CHILD_CVT (in either order).
-- QUR: when a seed is sown into an empty hole on the player's side of the board and the opposite hole contains CHILD_CVT, create children in both holes: final seed location and opposite.
-</t>
   </si>
   <si>
     <t>The name of the Game Class. One of:
@@ -1006,6 +987,15 @@
     <t>Start Moves w/o Capture</t>
   </si>
   <si>
+    <t>Don't allow captures or closing of holes (SOW_RULE of SOW_BLKD_DIV) for the first specified number of moves of the game or round.</t>
+  </si>
+  <si>
+    <t>sow_param</t>
+  </si>
+  <si>
+    <t>Sow Parameter</t>
+  </si>
+  <si>
     <t>Special sow rules add additional behavior or restrictions to the sowing phase:
 - NONE: there is no special sowing rule.
 - SOW_BLKD_DIV: If the final seed of an individual sow lands on the opposite side of the board and brings the contents of that hole to goal_param seeds, the hole is closed closed (blocked). In single lap games, the hole's seeds are removed from play. In multilap games, the seeds are used to continue sowing.
@@ -1020,10 +1010,31 @@
   + If mlaps is LAPPER and the final seed sown for any lap meets the capture criteria, the contents of the hole are captured by the sower and not the hole owner and the turn is over.
   + GRANDSLAM rules are not applied. NOCAPTMOVES prevents this capture for the first number of specified moves.
 - NO_SOW_OPP_2S: Don't sow into opponents holes with 2 seeds.
-- CHANGE_DIR_LAP: Change the direction for each lap sown. Generally used with UDIR_HOLES so the player may choose the first direction.</t>
-  </si>
-  <si>
-    <t>Don't allow captures or closing of holes (SOW_RULE of SOW_BLKD_DIV) for the first specified number of moves of the game or round.</t>
+- CHANGE_DIR_LAP: Change the direction for each lap sown. Generally used with UDIR_HOLES so the player may choose the first direction.
+- MAX_SOW: holes sow_param seeds are skipped when sowing. That is, holes will never contain more seeds than sow_param.</t>
+  </si>
+  <si>
+    <t>A general parameter for sowing. Usage is based on other sow options:
+- Sow rule of MAX_SOW: maximum number of seeds a hole may contain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Games with children allow players to claim holes. These child holes are an extension of the stores and seeds in them count towards a win. Making a child stops any multiple lap sowing, moves cannot start from children, and they cannot be captured (except for special rules associated with WEGs).
+- NOCHILD: children are not used.
+- NORMAL: children are made when a final seeds sows a hole to CHILD_CVT.
+- WALDA: STORES are not supported. Captures are instead moved into waldas, thus a player may not capture until they have created a walda. 
+  + Walda locations are limited.  Each player may create up to 6 waldas: on either end of each side of the board and the next two outer holes on their own side of the board. Note that there are only 8 total places that waldas maybe created.
+- ONE_CHILD: only one child allowed per player.
+  + Children must not be symmetrically opposite eachother. For example,  in a 9 hole per side game with holes numbered as follows, children may not be in the same numbered holes:
+  + 9 8 7 6 5 4 3 2 1
+  + 1 2 3 4 5 6 7 8 9 
+  + Depending on sow direction some holes are prohibited from being made children: 
+  + CW &amp; CCW:  the last of your opponents holes that you would sow into may not be made a child. CW holes numbered 1 above and CCW holes numberd 9 above.
+  + SPLIT: no end holes may be made children.
+  + Used to create tuzdek style children along with CHILD_RULE of OPP_ONLY.
+- WEG: children maybe created in holes owned by the opponent. Ending a sow in an opponent's weg captures the seed just sown and one more (if there is one); generally, the player gets to play again (per CAPT_RTURN). WEGs are supported for TERRITORY games only (hole ownership required).
+- BULL: create one bull if final seed sows to CHILD_CVT, create two bulls if the final two seeds are sown to CHILD_CVT-1 and CHILD_CVT (in either order).
+- QUR: when a seed is sown into an empty hole on the player's side of the board and the opposite hole contains CHILD_CVT, create children in both holes: final seed location and opposite.
+</t>
   </si>
 </sst>
 </file>
@@ -1905,11 +1916,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:J70"/>
+  <dimension ref="A1:J71"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J19" sqref="J19"/>
+      <pane ySplit="1" topLeftCell="A67" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J69" sqref="J69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2357,7 +2368,7 @@
         <v>22</v>
       </c>
       <c r="E14" s="3">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="F14" s="3" t="s">
         <v>39</v>
@@ -2389,7 +2400,7 @@
         <v>22</v>
       </c>
       <c r="E15" s="3">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="F15" s="3" t="s">
         <v>114</v>
@@ -2508,10 +2519,10 @@
         <v>93</v>
       </c>
       <c r="B19" s="3" t="s">
+        <v>268</v>
+      </c>
+      <c r="C19" s="3" t="s">
         <v>269</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>270</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>22</v>
@@ -2532,7 +2543,7 @@
         <v>2</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -2645,7 +2656,7 @@
         <v>22</v>
       </c>
       <c r="E23" s="3">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="F23" s="3" t="s">
         <v>39</v>
@@ -2660,7 +2671,7 @@
         <v>0</v>
       </c>
       <c r="J23" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2788,7 +2799,7 @@
         <v>0</v>
       </c>
       <c r="J27" s="4" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -2820,7 +2831,7 @@
         <v>0</v>
       </c>
       <c r="J28" s="4" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="409.5" x14ac:dyDescent="0.25">
@@ -2852,7 +2863,7 @@
         <v>2</v>
       </c>
       <c r="J29" s="4" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="105" x14ac:dyDescent="0.25">
@@ -2860,10 +2871,10 @@
         <v>36</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D30" s="3" t="s">
         <v>22</v>
@@ -2884,7 +2895,7 @@
         <v>2</v>
       </c>
       <c r="J30" s="4" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
@@ -2933,7 +2944,7 @@
         <v>22</v>
       </c>
       <c r="E32" s="3">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="F32" s="3" t="s">
         <v>58</v>
@@ -3012,7 +3023,7 @@
         <v>0</v>
       </c>
       <c r="J34" s="4" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
@@ -3599,7 +3610,7 @@
         <v>136</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D53" s="3" t="s">
         <v>128</v>
@@ -3692,7 +3703,7 @@
         <v>22</v>
       </c>
       <c r="E56" s="3">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="F56" s="3" t="s">
         <v>39</v>
@@ -3914,7 +3925,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="64" spans="1:10" ht="375" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" ht="390" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
         <v>67</v>
       </c>
@@ -3943,213 +3954,245 @@
         <v>0</v>
       </c>
       <c r="J64" s="4" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="65" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
         <v>67</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>88</v>
+        <v>271</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>89</v>
+        <v>272</v>
       </c>
       <c r="D65" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E65" s="3">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F65" s="3" t="s">
-        <v>146</v>
+        <v>11</v>
       </c>
       <c r="G65" s="5" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="H65" s="3">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I65" s="3">
         <v>0</v>
       </c>
       <c r="J65" s="4" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="66" spans="1:10" ht="165" x14ac:dyDescent="0.25">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
         <v>67</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="D66" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E66" s="3">
-        <v>120</v>
+        <v>144</v>
       </c>
       <c r="F66" s="3" t="s">
-        <v>168</v>
+        <v>146</v>
       </c>
       <c r="G66" s="5" t="s">
-        <v>169</v>
+        <v>91</v>
       </c>
       <c r="H66" s="3">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="I66" s="3">
-        <v>2</v>
-      </c>
-      <c r="J66" s="8" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="J66" s="4" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" ht="165" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
         <v>67</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D67" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E67" s="3">
-        <v>145</v>
+        <v>120</v>
       </c>
       <c r="F67" s="3" t="s">
-        <v>39</v>
+        <v>168</v>
       </c>
       <c r="G67" s="5" t="s">
-        <v>40</v>
+        <v>169</v>
       </c>
       <c r="H67" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I67" s="3">
         <v>2</v>
       </c>
-      <c r="J67" s="4" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="68" spans="1:10" ht="360" x14ac:dyDescent="0.25">
+      <c r="J67" s="8" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
         <v>67</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>159</v>
+        <v>85</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>160</v>
+        <v>86</v>
       </c>
       <c r="D68" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E68" s="3">
-        <v>112</v>
+        <v>146</v>
       </c>
       <c r="F68" s="3" t="s">
-        <v>162</v>
+        <v>39</v>
       </c>
       <c r="G68" s="5" t="s">
-        <v>161</v>
+        <v>40</v>
       </c>
       <c r="H68" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I68" s="3">
         <v>2</v>
       </c>
       <c r="J68" s="4" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="69" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" ht="360" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
         <v>67</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="D69" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E69" s="3">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="F69" s="3" t="s">
-        <v>11</v>
+        <v>162</v>
       </c>
       <c r="G69" s="5" t="s">
-        <v>87</v>
+        <v>161</v>
       </c>
       <c r="H69" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I69" s="3">
         <v>2</v>
       </c>
       <c r="J69" s="4" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="70" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
         <v>67</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>194</v>
+        <v>157</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>195</v>
+        <v>158</v>
       </c>
       <c r="D70" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E70" s="3">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F70" s="3" t="s">
-        <v>196</v>
-      </c>
-      <c r="G70" s="3" t="s">
-        <v>167</v>
+        <v>11</v>
+      </c>
+      <c r="G70" s="5" t="s">
+        <v>87</v>
       </c>
       <c r="H70" s="3">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I70" s="3">
         <v>2</v>
       </c>
       <c r="J70" s="4" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A71" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B71" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="C71" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="D71" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E71" s="3">
+        <v>111</v>
+      </c>
+      <c r="F71" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="G71" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="H71" s="3">
+        <v>5</v>
+      </c>
+      <c r="I71" s="3">
+        <v>2</v>
+      </c>
+      <c r="J71" s="4" t="s">
         <v>238</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J70" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J70">
-      <sortCondition ref="A2:A70"/>
-      <sortCondition ref="I2:I70"/>
-      <sortCondition ref="H2:H70"/>
+  <autoFilter ref="A1:J71" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J71">
+      <sortCondition ref="A2:A71"/>
+      <sortCondition ref="I2:I71"/>
+      <sortCondition ref="H2:H71"/>
     </sortState>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J71">
-    <sortCondition ref="A2:A71"/>
-    <sortCondition ref="I2:I71"/>
-    <sortCondition ref="H2:H71"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J72">
+    <sortCondition ref="A2:A72"/>
+    <sortCondition ref="I2:I72"/>
+    <sortCondition ref="H2:H72"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
MancalaGames UI updates: added labels to the game_params file, to group params on the UI, allow the param section of the UI to resize, removed the Allow tab (still questioning), organized the param placement on the UI.
</commit_message>
<xml_diff>
--- a/src/game_params.xlsx
+++ b/src/game_params.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Activity_Data\Mancala_github\MancalaGames\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF223F98-8DB8-41B6-B525-67387AB714D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C97E103E-4E5C-44EA-BBA4-D0410976F149}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="game_params" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">game_params!$A$1:$J$71</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">game_params!$A$1:$J$85</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="554" uniqueCount="305">
   <si>
     <t>tab</t>
   </si>
@@ -218,9 +218,6 @@
     <t>ALL_EQUAL</t>
   </si>
   <si>
-    <t>Allow</t>
-  </si>
-  <si>
     <t>min_move</t>
   </si>
   <si>
@@ -272,9 +269,6 @@
     <t>skip_start</t>
   </si>
   <si>
-    <t>Skip Start on Lap</t>
-  </si>
-  <si>
     <t>sow_own_store</t>
   </si>
   <si>
@@ -288,9 +282,6 @@
   </si>
   <si>
     <t>mlaps</t>
-  </si>
-  <si>
-    <t>Multilap Sow</t>
   </si>
   <si>
     <t>visit_opp</t>
@@ -984,9 +975,6 @@
     <t>nocaptmoves</t>
   </si>
   <si>
-    <t>Start Moves w/o Capture</t>
-  </si>
-  <si>
     <t>Don't allow captures or closing of holes (SOW_RULE of SOW_BLKD_DIV) for the first specified number of moves of the game or round.</t>
   </si>
   <si>
@@ -1035,6 +1023,105 @@
 - BULL: create one bull if final seed sows to CHILD_CVT, create two bulls if the final two seeds are sown to CHILD_CVT-1 and CHILD_CVT (in either order).
 - QUR: when a seed is sown into an empty hole on the player's side of the board and the opposite hole contains CHILD_CVT, create children in both holes: final seed location and opposite.
 </t>
+  </si>
+  <si>
+    <t>label</t>
+  </si>
+  <si>
+    <t>Initial Setup</t>
+  </si>
+  <si>
+    <t>Parameters that control the initial game setup.</t>
+  </si>
+  <si>
+    <t>rnd_lbl</t>
+  </si>
+  <si>
+    <t>mm_params</t>
+  </si>
+  <si>
+    <t>Monte Carlo Tree Search Params</t>
+  </si>
+  <si>
+    <t>mcts_params</t>
+  </si>
+  <si>
+    <t>Mini/Nega Maxer Params</t>
+  </si>
+  <si>
+    <t>scapt_lbl</t>
+  </si>
+  <si>
+    <t>Basic Capture</t>
+  </si>
+  <si>
+    <t>ocapt_lbl</t>
+  </si>
+  <si>
+    <t>Other Captures</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0 </t>
+  </si>
+  <si>
+    <t>xc_lbl</t>
+  </si>
+  <si>
+    <t>Cross Capture</t>
+  </si>
+  <si>
+    <t>clim_lbl</t>
+  </si>
+  <si>
+    <t>Nbr Start Moves w/o Capture</t>
+  </si>
+  <si>
+    <t>cdyno_lbl</t>
+  </si>
+  <si>
+    <t>Capture Dynamics</t>
+  </si>
+  <si>
+    <t>mcapt_lbl</t>
+  </si>
+  <si>
+    <t>Skip Start on Cycle</t>
+  </si>
+  <si>
+    <t>Sow Type</t>
+  </si>
+  <si>
+    <t>schld_lbl</t>
+  </si>
+  <si>
+    <t>Children</t>
+  </si>
+  <si>
+    <t>sdyno_lbl</t>
+  </si>
+  <si>
+    <t>Sow Dynamics</t>
+  </si>
+  <si>
+    <t>Capture Restrictions</t>
+  </si>
+  <si>
+    <t>Rounds Parameters</t>
+  </si>
+  <si>
+    <t>setup_lbl</t>
+  </si>
+  <si>
+    <t>draw_lbl</t>
+  </si>
+  <si>
+    <t>Draw Parameters</t>
+  </si>
+  <si>
+    <t>Move Dynamics</t>
+  </si>
+  <si>
+    <t>mdyno_lbl</t>
   </si>
 </sst>
 </file>
@@ -1916,11 +2003,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:J71"/>
+  <dimension ref="A1:J85"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A67" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J69" sqref="J69"/>
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J30" sqref="J30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1952,7 +2039,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>4</v>
@@ -1970,27 +2057,25 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>61</v>
+        <v>280</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>22</v>
-      </c>
+        <v>281</v>
+      </c>
+      <c r="D2" s="3"/>
       <c r="E2" s="3">
-        <v>119</v>
+        <v>0</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>11</v>
+        <v>272</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>63</v>
+        <v>84</v>
       </c>
       <c r="H2" s="3">
         <v>0</v>
@@ -1998,31 +2083,29 @@
       <c r="I2" s="3">
         <v>0</v>
       </c>
-      <c r="J2" s="4" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="J2" s="4"/>
+    </row>
+    <row r="3" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>65</v>
+        <v>98</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>66</v>
+        <v>99</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E3" s="3">
-        <v>126</v>
+        <v>114</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>39</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="H3" s="3">
         <v>1</v>
@@ -2031,280 +2114,268 @@
         <v>0</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="180" x14ac:dyDescent="0.25">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>164</v>
+        <v>100</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>165</v>
+        <v>101</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E4" s="3">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>166</v>
+        <v>11</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>167</v>
+        <v>84</v>
       </c>
       <c r="H4" s="3">
+        <v>2</v>
+      </c>
+      <c r="I4" s="3">
+        <v>0</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="3">
+        <v>105</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="H5" s="3">
         <v>3</v>
       </c>
-      <c r="I4" s="3">
-        <v>0</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E5" s="3">
-        <v>103</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="H5" s="3">
-        <v>0</v>
-      </c>
       <c r="I5" s="3">
         <v>0</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>96</v>
+        <v>119</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>97</v>
+        <v>120</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E6" s="3">
-        <v>130</v>
+        <v>107</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>39</v>
+        <v>143</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>40</v>
+        <v>88</v>
       </c>
       <c r="H6" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I6" s="3">
         <v>0</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>116</v>
+        <v>285</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>22</v>
+        <v>286</v>
       </c>
       <c r="E7" s="3">
-        <v>124</v>
+        <v>0</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>39</v>
+        <v>272</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>40</v>
+        <v>84</v>
       </c>
       <c r="H7" s="3">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="I7" s="3">
         <v>0</v>
       </c>
-      <c r="J7" s="4" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E8" s="3">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>39</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="H8" s="3">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I8" s="3">
         <v>0</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E9" s="3">
-        <v>104</v>
+        <v>148</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>11</v>
+        <v>111</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>87</v>
+        <v>112</v>
       </c>
       <c r="H9" s="3">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="I9" s="3">
         <v>0</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>105</v>
+        <v>183</v>
       </c>
       <c r="C10" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" s="3">
+        <v>147</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="H10" s="3">
+        <v>8</v>
+      </c>
+      <c r="I10" s="3">
+        <v>0</v>
+      </c>
+      <c r="J10" s="4" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="E11" s="3">
+        <v>0</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="H11" s="3">
+        <v>9</v>
+      </c>
+      <c r="I11" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12" s="3">
         <v>106</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E10" s="3">
-        <v>105</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G10" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="H10" s="3">
-        <v>5</v>
-      </c>
-      <c r="I10" s="3">
-        <v>0</v>
-      </c>
-      <c r="J10" s="4" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E11" s="3">
-        <v>106</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="H11" s="3">
-        <v>6</v>
-      </c>
-      <c r="I11" s="3">
-        <v>0</v>
-      </c>
-      <c r="J11" s="4" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="90" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E12" s="3">
-        <v>109</v>
       </c>
       <c r="F12" s="3" t="s">
         <v>39</v>
@@ -2313,30 +2384,30 @@
         <v>40</v>
       </c>
       <c r="H12" s="3">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="I12" s="3">
         <v>0</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>110</v>
+        <v>121</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>111</v>
+        <v>122</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E13" s="3">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="F13" s="3" t="s">
         <v>39</v>
@@ -2345,254 +2416,242 @@
         <v>40</v>
       </c>
       <c r="H13" s="3">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="I13" s="3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>186</v>
+        <v>291</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>22</v>
+        <v>114</v>
       </c>
       <c r="E14" s="3">
-        <v>147</v>
+        <v>0</v>
       </c>
       <c r="F14" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="H14" s="3">
+        <v>0</v>
+      </c>
+      <c r="I14" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E15" s="3">
+        <v>124</v>
+      </c>
+      <c r="F15" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="G14" s="5" t="s">
+      <c r="G15" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="H14" s="3">
+      <c r="H15" s="3">
         <v>1</v>
       </c>
-      <c r="I14" s="3">
-        <v>2</v>
-      </c>
-      <c r="J14" s="4" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E15" s="3">
-        <v>148</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="G15" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="H15" s="3">
-        <v>2</v>
-      </c>
       <c r="I15" s="3">
         <v>2</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="150" x14ac:dyDescent="0.25">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>118</v>
+        <v>91</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>119</v>
+        <v>92</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E16" s="3">
-        <v>117</v>
+        <v>103</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>120</v>
+        <v>39</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>121</v>
+        <v>40</v>
       </c>
       <c r="H16" s="3">
+        <v>2</v>
+      </c>
+      <c r="I16" s="3">
+        <v>2</v>
+      </c>
+      <c r="J16" s="4" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>287</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="E17" s="3">
+        <v>0</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="H17" s="3">
         <v>3</v>
       </c>
-      <c r="I16" s="3">
-        <v>2</v>
-      </c>
-      <c r="J16" s="4" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E17" s="3">
-        <v>123</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="G17" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="H17" s="3">
-        <v>4</v>
-      </c>
       <c r="I17" s="3">
         <v>2</v>
-      </c>
-      <c r="J17" s="4" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>107</v>
+        <v>265</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>108</v>
+        <v>288</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E18" s="3">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>39</v>
+        <v>11</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>40</v>
+        <v>84</v>
       </c>
       <c r="H18" s="3">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I18" s="3">
         <v>2</v>
       </c>
       <c r="J18" s="4" t="s">
-        <v>109</v>
+        <v>266</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B19" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="B19" s="3" t="s">
-        <v>268</v>
-      </c>
       <c r="C19" s="3" t="s">
-        <v>269</v>
+        <v>94</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E19" s="3">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>87</v>
+        <v>40</v>
       </c>
       <c r="H19" s="3">
+        <v>5</v>
+      </c>
+      <c r="I19" s="3">
+        <v>2</v>
+      </c>
+      <c r="J19" s="4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E20" s="3">
+        <v>129</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="H20" s="3">
         <v>6</v>
       </c>
-      <c r="I19" s="3">
-        <v>2</v>
-      </c>
-      <c r="J19" s="4" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="90" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="C20" s="3" t="s">
+      <c r="I20" s="3">
+        <v>2</v>
+      </c>
+      <c r="J20" s="4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E21" s="3">
         <v>123</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E20" s="3">
-        <v>107</v>
-      </c>
-      <c r="F20" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="G20" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="H20" s="3">
-        <v>8</v>
-      </c>
-      <c r="I20" s="3">
-        <v>2</v>
-      </c>
-      <c r="J20" s="4" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E21" s="3">
-        <v>108</v>
       </c>
       <c r="F21" s="3" t="s">
         <v>39</v>
@@ -2601,301 +2660,286 @@
         <v>40</v>
       </c>
       <c r="H21" s="3">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="I21" s="3">
         <v>2</v>
       </c>
       <c r="J21" s="4" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" ht="135" x14ac:dyDescent="0.25">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>183</v>
+        <v>289</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>185</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>22</v>
+        <v>290</v>
       </c>
       <c r="E22" s="3">
-        <v>131</v>
+        <v>0</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>184</v>
+        <v>272</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>167</v>
+        <v>84</v>
       </c>
       <c r="H22" s="3">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="I22" s="3">
         <v>2</v>
       </c>
-      <c r="J22" s="4" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>36</v>
+        <v>90</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>49</v>
+        <v>170</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>50</v>
+        <v>171</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E23" s="3">
-        <v>143</v>
+        <v>108</v>
       </c>
       <c r="F23" s="3" t="s">
         <v>39</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="H23" s="3">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="I23" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J23" s="4" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="135" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>36</v>
+        <v>90</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>37</v>
+        <v>180</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>38</v>
+        <v>182</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E24" s="3">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>39</v>
+        <v>181</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>40</v>
+        <v>164</v>
       </c>
       <c r="H24" s="3">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="I24" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J24" s="4" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" ht="210" x14ac:dyDescent="0.25">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>36</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E25" s="3">
-        <v>135</v>
+        <v>115</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>257</v>
+        <v>55</v>
       </c>
       <c r="H25" s="3">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I25" s="3">
         <v>0</v>
       </c>
       <c r="J25" s="4" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>36</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>43</v>
+        <v>262</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>44</v>
+        <v>264</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E26" s="3">
-        <v>134</v>
+        <v>116</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>45</v>
+        <v>11</v>
       </c>
       <c r="G26" s="5" t="s">
-        <v>46</v>
+        <v>84</v>
       </c>
       <c r="H26" s="3">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I26" s="3">
         <v>0</v>
       </c>
       <c r="J26" s="4" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" ht="330" x14ac:dyDescent="0.25">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>36</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>188</v>
+        <v>300</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>189</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>22</v>
+        <v>273</v>
       </c>
       <c r="E27" s="3">
-        <v>133</v>
+        <v>0</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>190</v>
+        <v>272</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>197</v>
+        <v>84</v>
       </c>
       <c r="H27" s="3">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="I27" s="3">
         <v>0</v>
       </c>
       <c r="J27" s="4" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="150" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>36</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>81</v>
+        <v>56</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>82</v>
+        <v>57</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E28" s="3">
-        <v>102</v>
+        <v>142</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>39</v>
+        <v>58</v>
       </c>
       <c r="G28" s="5" t="s">
-        <v>40</v>
+        <v>59</v>
       </c>
       <c r="H28" s="3">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="I28" s="3">
         <v>0</v>
       </c>
       <c r="J28" s="4" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" ht="409.5" x14ac:dyDescent="0.25">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="180" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>36</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>52</v>
+        <v>175</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>53</v>
+        <v>174</v>
       </c>
       <c r="D29" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E29" s="3">
-        <v>115</v>
+        <v>132</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>54</v>
+        <v>176</v>
       </c>
       <c r="G29" s="5" t="s">
-        <v>55</v>
+        <v>164</v>
       </c>
       <c r="H29" s="3">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I29" s="3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J29" s="4" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" ht="105" x14ac:dyDescent="0.25">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>36</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>265</v>
+        <v>301</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>267</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>22</v>
+        <v>302</v>
       </c>
       <c r="E30" s="3">
-        <v>116</v>
+        <v>0</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G30" s="5" t="s">
-        <v>87</v>
+        <v>272</v>
+      </c>
+      <c r="G30" s="3">
+        <v>0</v>
       </c>
       <c r="H30" s="3">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="I30" s="3">
-        <v>2</v>
-      </c>
-      <c r="J30" s="4" t="s">
-        <v>266</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
@@ -2903,598 +2947,586 @@
         <v>36</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>47</v>
+        <v>60</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="D31" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E31" s="3">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>39</v>
+        <v>11</v>
       </c>
       <c r="G31" s="5" t="s">
-        <v>40</v>
+        <v>62</v>
       </c>
       <c r="H31" s="3">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="I31" s="3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J31" s="4" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" ht="150" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" ht="180" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>36</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>56</v>
+        <v>161</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>57</v>
+        <v>162</v>
       </c>
       <c r="D32" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E32" s="3">
-        <v>142</v>
+        <v>101</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>58</v>
+        <v>163</v>
       </c>
       <c r="G32" s="5" t="s">
-        <v>59</v>
+        <v>164</v>
       </c>
       <c r="H32" s="3">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="I32" s="3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J32" s="4" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" ht="180" x14ac:dyDescent="0.25">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>36</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>178</v>
+        <v>49</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>177</v>
+        <v>50</v>
       </c>
       <c r="D33" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E33" s="3">
-        <v>132</v>
+        <v>143</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>179</v>
+        <v>39</v>
       </c>
       <c r="G33" s="5" t="s">
-        <v>167</v>
+        <v>51</v>
       </c>
       <c r="H33" s="3">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I33" s="3">
         <v>2</v>
       </c>
       <c r="J33" s="4" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>15</v>
+        <v>36</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>17</v>
+        <v>47</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>16</v>
+        <v>48</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="E34" s="3">
+        <v>127</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G34" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="H34" s="3">
         <v>1</v>
       </c>
-      <c r="F34" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="G34" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="H34" s="3">
-        <v>0</v>
-      </c>
       <c r="I34" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J34" s="4" t="s">
-        <v>259</v>
+        <v>232</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>15</v>
+        <v>36</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>29</v>
+        <v>304</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D35" s="3" t="s">
-        <v>31</v>
+        <v>303</v>
       </c>
       <c r="E35" s="3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G35" s="5" t="s">
-        <v>32</v>
+        <v>272</v>
+      </c>
+      <c r="G35" s="3">
+        <v>0</v>
       </c>
       <c r="H35" s="3">
         <v>2</v>
       </c>
       <c r="I35" s="3">
-        <v>0</v>
-      </c>
-      <c r="J35" s="4" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>15</v>
+        <v>36</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="D36" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E36" s="3">
-        <v>118</v>
+        <v>125</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>18</v>
+        <v>39</v>
       </c>
       <c r="G36" s="5" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="H36" s="3">
         <v>3</v>
       </c>
       <c r="I36" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J36" s="4" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>15</v>
+        <v>36</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>26</v>
+        <v>64</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>27</v>
+        <v>65</v>
       </c>
       <c r="D37" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E37" s="3">
-        <v>5</v>
+        <v>126</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="G37" s="6" t="s">
-        <v>140</v>
+        <v>39</v>
+      </c>
+      <c r="G37" s="5" t="s">
+        <v>40</v>
       </c>
       <c r="H37" s="3">
         <v>4</v>
       </c>
       <c r="I37" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J37" s="4" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" ht="150" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>15</v>
+        <v>36</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>20</v>
+        <v>115</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>21</v>
+        <v>116</v>
       </c>
       <c r="D38" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E38" s="3">
-        <v>4</v>
+        <v>117</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>18</v>
+        <v>117</v>
       </c>
       <c r="G38" s="5" t="s">
-        <v>19</v>
+        <v>118</v>
       </c>
       <c r="H38" s="3">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I38" s="3">
         <v>2</v>
       </c>
       <c r="J38" s="4" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>15</v>
+        <v>36</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>33</v>
+        <v>275</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D39" s="3" t="s">
-        <v>31</v>
+        <v>299</v>
       </c>
       <c r="E39" s="3">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G39" s="5" t="s">
-        <v>35</v>
+        <v>272</v>
+      </c>
+      <c r="G39" s="3">
+        <v>0</v>
       </c>
       <c r="H39" s="3">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="I39" s="3">
         <v>2</v>
       </c>
-      <c r="J39" s="4" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:10" ht="210" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
-        <v>126</v>
+        <v>36</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>143</v>
+        <v>41</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>144</v>
+        <v>42</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>139</v>
+        <v>22</v>
       </c>
       <c r="E40" s="3">
-        <v>201</v>
+        <v>135</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="G40" s="3" t="s">
-        <v>145</v>
+        <v>42</v>
+      </c>
+      <c r="G40" s="5" t="s">
+        <v>254</v>
       </c>
       <c r="H40" s="3">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="I40" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J40" s="4" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>126</v>
+        <v>36</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>137</v>
+        <v>43</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>138</v>
+        <v>44</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>139</v>
+        <v>22</v>
       </c>
       <c r="E41" s="3">
-        <v>203</v>
+        <v>134</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>11</v>
+        <v>45</v>
       </c>
       <c r="G41" s="5" t="s">
-        <v>63</v>
+        <v>46</v>
       </c>
       <c r="H41" s="3">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="I41" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J41" s="4" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" ht="330" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
-        <v>126</v>
+        <v>36</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>139</v>
+        <v>22</v>
       </c>
       <c r="E42" s="3">
-        <v>202</v>
+        <v>133</v>
       </c>
       <c r="F42" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="G42" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="H42" s="3">
+        <v>9</v>
+      </c>
+      <c r="I42" s="3">
+        <v>2</v>
+      </c>
+      <c r="J42" s="4" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A43" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E43" s="3">
+        <v>102</v>
+      </c>
+      <c r="F43" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="G42" s="5" t="s">
+      <c r="G43" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="H42" s="3">
-        <v>2</v>
-      </c>
-      <c r="I42" s="3">
-        <v>0</v>
-      </c>
-      <c r="J42" s="4" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A43" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="B43" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="C43" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="D43" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="E43" s="3">
-        <v>213</v>
-      </c>
-      <c r="F43" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="G43" s="3" t="s">
-        <v>250</v>
-      </c>
       <c r="H43" s="3">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="I43" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J43" s="4" t="s">
-        <v>221</v>
+        <v>260</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
-        <v>126</v>
+        <v>15</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>150</v>
+        <v>17</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>154</v>
+        <v>16</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>149</v>
+        <v>17</v>
       </c>
       <c r="E44" s="3">
-        <v>210</v>
+        <v>1</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="G44" s="3" t="s">
-        <v>251</v>
+        <v>139</v>
+      </c>
+      <c r="G44" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="H44" s="3">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="I44" s="3">
         <v>0</v>
       </c>
       <c r="J44" s="4" t="s">
-        <v>211</v>
+        <v>256</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
-        <v>126</v>
+        <v>15</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>151</v>
+        <v>29</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>153</v>
+        <v>30</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>149</v>
+        <v>31</v>
       </c>
       <c r="E45" s="3">
-        <v>211</v>
+        <v>2</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="G45" s="3" t="s">
-        <v>249</v>
+        <v>11</v>
+      </c>
+      <c r="G45" s="5" t="s">
+        <v>32</v>
       </c>
       <c r="H45" s="3">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="I45" s="3">
         <v>0</v>
       </c>
       <c r="J45" s="4" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
-        <v>126</v>
+        <v>15</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>152</v>
+        <v>23</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>155</v>
+        <v>24</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>149</v>
+        <v>22</v>
       </c>
       <c r="E46" s="3">
-        <v>212</v>
+        <v>118</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="G46" s="3" t="s">
-        <v>156</v>
+        <v>18</v>
+      </c>
+      <c r="G46" s="5" t="s">
+        <v>25</v>
       </c>
       <c r="H46" s="3">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="I46" s="3">
         <v>0</v>
       </c>
       <c r="J46" s="4" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
-        <v>126</v>
+        <v>15</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>127</v>
+        <v>26</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>244</v>
+        <v>27</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>128</v>
+        <v>22</v>
       </c>
       <c r="E47" s="3">
-        <v>220</v>
+        <v>5</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G47" s="5" t="s">
-        <v>35</v>
+        <v>28</v>
+      </c>
+      <c r="G47" s="6" t="s">
+        <v>137</v>
       </c>
       <c r="H47" s="3">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I47" s="3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J47" s="4" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
-        <v>126</v>
+        <v>15</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>129</v>
+        <v>20</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>243</v>
+        <v>21</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>128</v>
+        <v>22</v>
       </c>
       <c r="E48" s="3">
-        <v>221</v>
+        <v>4</v>
       </c>
       <c r="F48" s="3" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="G48" s="5" t="s">
-        <v>87</v>
+        <v>19</v>
       </c>
       <c r="H48" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I48" s="3">
         <v>2</v>
       </c>
       <c r="J48" s="4" t="s">
-        <v>218</v>
+        <v>197</v>
       </c>
     </row>
     <row r="49" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
-        <v>126</v>
+        <v>15</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>130</v>
+        <v>33</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>242</v>
+        <v>34</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>128</v>
+        <v>31</v>
       </c>
       <c r="E49" s="3">
-        <v>222</v>
+        <v>3</v>
       </c>
       <c r="F49" s="3" t="s">
         <v>11</v>
       </c>
       <c r="G49" s="5" t="s">
-        <v>87</v>
+        <v>35</v>
       </c>
       <c r="H49" s="3">
         <v>2</v>
@@ -3503,696 +3535,1120 @@
         <v>2</v>
       </c>
       <c r="J49" s="4" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>131</v>
+        <v>140</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>241</v>
+        <v>141</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="E50" s="3">
-        <v>223</v>
+        <v>201</v>
       </c>
       <c r="F50" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G50" s="5" t="s">
-        <v>87</v>
+        <v>141</v>
+      </c>
+      <c r="G50" s="3" t="s">
+        <v>142</v>
       </c>
       <c r="H50" s="3">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I50" s="3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J50" s="4" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>240</v>
+        <v>135</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="E51" s="3">
-        <v>224</v>
+        <v>203</v>
       </c>
       <c r="F51" s="3" t="s">
         <v>11</v>
       </c>
       <c r="G51" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="H51" s="3">
+        <v>1</v>
+      </c>
+      <c r="I51" s="3">
+        <v>0</v>
+      </c>
+      <c r="J51" s="4" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A52" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="E52" s="3">
+        <v>202</v>
+      </c>
+      <c r="F52" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G52" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="H52" s="3">
+        <v>2</v>
+      </c>
+      <c r="I52" s="3">
+        <v>0</v>
+      </c>
+      <c r="J52" s="4" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A53" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="E53" s="3">
+        <v>0</v>
+      </c>
+      <c r="F53" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="G53" s="3">
+        <v>0</v>
+      </c>
+      <c r="H53" s="3">
+        <v>5</v>
+      </c>
+      <c r="I53" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A54" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="E54" s="3">
+        <v>210</v>
+      </c>
+      <c r="F54" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="H51" s="3">
-        <v>4</v>
-      </c>
-      <c r="I51" s="3">
-        <v>2</v>
-      </c>
-      <c r="J51" s="4" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="52" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A52" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="B52" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="C52" s="3" t="s">
-        <v>239</v>
-      </c>
-      <c r="D52" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="E52" s="3">
-        <v>225</v>
-      </c>
-      <c r="F52" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G52" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="H52" s="3">
-        <v>5</v>
-      </c>
-      <c r="I52" s="3">
-        <v>2</v>
-      </c>
-      <c r="J52" s="4" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="53" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A53" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="B53" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="C53" s="3" t="s">
-        <v>261</v>
-      </c>
-      <c r="D53" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="E53" s="3">
-        <v>226</v>
-      </c>
-      <c r="F53" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G53" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="H53" s="3">
+      <c r="G54" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="H54" s="3">
         <v>6</v>
       </c>
-      <c r="I53" s="3">
-        <v>2</v>
-      </c>
-      <c r="J53" s="4" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="54" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A54" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="B54" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="C54" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="D54" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="E54" s="3">
-        <v>227</v>
-      </c>
-      <c r="F54" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G54" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="H54" s="3">
-        <v>7</v>
-      </c>
       <c r="I54" s="3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J54" s="4" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
-        <v>9</v>
+        <v>123</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>170</v>
+        <v>148</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>150</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>22</v>
+        <v>146</v>
       </c>
       <c r="E55" s="3">
-        <v>121</v>
+        <v>211</v>
       </c>
       <c r="F55" s="3" t="s">
-        <v>11</v>
+        <v>87</v>
+      </c>
+      <c r="G55" s="3" t="s">
+        <v>246</v>
       </c>
       <c r="H55" s="3">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="I55" s="3">
         <v>0</v>
       </c>
       <c r="J55" s="4" t="s">
-        <v>172</v>
+        <v>207</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
-        <v>9</v>
+        <v>123</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>92</v>
+        <v>149</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>152</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>22</v>
+        <v>146</v>
       </c>
       <c r="E56" s="3">
-        <v>145</v>
+        <v>212</v>
       </c>
       <c r="F56" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="G56" s="5"/>
+        <v>87</v>
+      </c>
+      <c r="G56" s="3" t="s">
+        <v>153</v>
+      </c>
       <c r="H56" s="3">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="I56" s="3">
         <v>0</v>
       </c>
       <c r="J56" s="4" t="s">
-        <v>171</v>
+        <v>206</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
-        <v>9</v>
+        <v>123</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>13</v>
+        <v>276</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>279</v>
       </c>
       <c r="E57" s="3">
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="F57" s="3" t="s">
-        <v>14</v>
+        <v>272</v>
+      </c>
+      <c r="G57" s="3">
+        <v>0</v>
       </c>
       <c r="H57" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I57" s="3">
-        <v>0</v>
-      </c>
-      <c r="J57" s="4" t="s">
-        <v>141</v>
+        <v>2</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
-        <v>9</v>
+        <v>123</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>10</v>
+        <v>144</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="D58" s="3" t="s">
+        <v>146</v>
       </c>
       <c r="E58" s="3">
-        <v>501</v>
+        <v>213</v>
       </c>
       <c r="F58" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="G58" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="H58" s="3">
+        <v>2</v>
+      </c>
+      <c r="I58" s="3">
+        <v>2</v>
+      </c>
+      <c r="J58" s="4" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A59" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="D59" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="E59" s="3">
+        <v>220</v>
+      </c>
+      <c r="F59" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H58" s="3">
-        <v>0</v>
-      </c>
-      <c r="I58" s="3">
-        <v>0</v>
-      </c>
-      <c r="J58" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="59" spans="1:10" ht="165" x14ac:dyDescent="0.25">
-      <c r="A59" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="B59" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="C59" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="D59" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E59" s="3">
-        <v>137</v>
-      </c>
-      <c r="F59" s="3" t="s">
-        <v>70</v>
-      </c>
       <c r="G59" s="5" t="s">
-        <v>71</v>
+        <v>35</v>
       </c>
       <c r="H59" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I59" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J59" s="4" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
-        <v>67</v>
+        <v>123</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>72</v>
+        <v>126</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>73</v>
+        <v>240</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>22</v>
+        <v>125</v>
       </c>
       <c r="E60" s="3">
-        <v>140</v>
+        <v>221</v>
       </c>
       <c r="F60" s="3" t="s">
-        <v>39</v>
+        <v>11</v>
       </c>
       <c r="G60" s="5" t="s">
-        <v>40</v>
+        <v>84</v>
       </c>
       <c r="H60" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I60" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J60" s="4" t="s">
-        <v>74</v>
+        <v>215</v>
       </c>
     </row>
     <row r="61" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
-        <v>67</v>
+        <v>123</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>77</v>
+        <v>127</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>78</v>
+        <v>239</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>22</v>
+        <v>125</v>
       </c>
       <c r="E61" s="3">
-        <v>136</v>
+        <v>222</v>
       </c>
       <c r="F61" s="3" t="s">
-        <v>39</v>
+        <v>11</v>
       </c>
       <c r="G61" s="5" t="s">
-        <v>40</v>
+        <v>84</v>
       </c>
       <c r="H61" s="3">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="I61" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J61" s="4" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="62" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
-        <v>67</v>
+        <v>123</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>79</v>
+        <v>128</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>80</v>
+        <v>238</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>22</v>
+        <v>125</v>
       </c>
       <c r="E62" s="3">
-        <v>138</v>
+        <v>223</v>
       </c>
       <c r="F62" s="3" t="s">
-        <v>39</v>
+        <v>11</v>
       </c>
       <c r="G62" s="5" t="s">
-        <v>40</v>
+        <v>84</v>
       </c>
       <c r="H62" s="3">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I62" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J62" s="4" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A63" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="C63" s="3" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="63" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A63" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="B63" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="C63" s="3" t="s">
-        <v>76</v>
-      </c>
       <c r="D63" s="3" t="s">
-        <v>22</v>
+        <v>125</v>
       </c>
       <c r="E63" s="3">
-        <v>122</v>
+        <v>224</v>
       </c>
       <c r="F63" s="3" t="s">
-        <v>39</v>
+        <v>11</v>
       </c>
       <c r="G63" s="5" t="s">
-        <v>40</v>
+        <v>84</v>
       </c>
       <c r="H63" s="3">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="I63" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J63" s="4" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="64" spans="1:10" ht="390" x14ac:dyDescent="0.25">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
-        <v>67</v>
+        <v>123</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>180</v>
+        <v>130</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>181</v>
+        <v>236</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>22</v>
+        <v>125</v>
       </c>
       <c r="E64" s="3">
-        <v>139</v>
+        <v>225</v>
       </c>
       <c r="F64" s="3" t="s">
-        <v>182</v>
+        <v>11</v>
       </c>
       <c r="G64" s="5" t="s">
-        <v>167</v>
+        <v>84</v>
       </c>
       <c r="H64" s="3">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="I64" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J64" s="4" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="65" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
-        <v>67</v>
+        <v>123</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>271</v>
+        <v>133</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>272</v>
+        <v>258</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>22</v>
+        <v>125</v>
       </c>
       <c r="E65" s="3">
-        <v>141</v>
+        <v>226</v>
       </c>
       <c r="F65" s="3" t="s">
         <v>11</v>
       </c>
       <c r="G65" s="5" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="H65" s="3">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="I65" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J65" s="4" t="s">
-        <v>274</v>
+        <v>216</v>
       </c>
     </row>
     <row r="66" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
-        <v>67</v>
+        <v>123</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>88</v>
+        <v>131</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>89</v>
+        <v>132</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>22</v>
+        <v>125</v>
       </c>
       <c r="E66" s="3">
-        <v>144</v>
+        <v>227</v>
       </c>
       <c r="F66" s="3" t="s">
-        <v>146</v>
+        <v>11</v>
       </c>
       <c r="G66" s="5" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="H66" s="3">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="I66" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J66" s="4" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="67" spans="1:10" ht="165" x14ac:dyDescent="0.25">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
-        <v>67</v>
+        <v>9</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C67" s="3" t="s">
-        <v>84</v>
+        <v>167</v>
       </c>
       <c r="D67" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E67" s="3">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="F67" s="3" t="s">
-        <v>168</v>
-      </c>
-      <c r="G67" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H67" s="3">
+        <v>0</v>
+      </c>
+      <c r="I67" s="3">
+        <v>0</v>
+      </c>
+      <c r="J67" s="4" t="s">
         <v>169</v>
-      </c>
-      <c r="H67" s="3">
-        <v>0</v>
-      </c>
-      <c r="I67" s="3">
-        <v>2</v>
-      </c>
-      <c r="J67" s="8" t="s">
-        <v>247</v>
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
-        <v>67</v>
+        <v>9</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="C68" s="3" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="D68" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E68" s="3">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F68" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="G68" s="5" t="s">
-        <v>40</v>
-      </c>
+      <c r="G68" s="5"/>
       <c r="H68" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I68" s="3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J68" s="4" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="69" spans="1:10" ht="360" x14ac:dyDescent="0.25">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
-        <v>67</v>
+        <v>9</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="C69" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="D69" s="3" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="E69" s="3">
-        <v>112</v>
+        <v>500</v>
       </c>
       <c r="F69" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="G69" s="5" t="s">
-        <v>161</v>
+        <v>14</v>
       </c>
       <c r="H69" s="3">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I69" s="3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J69" s="4" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="70" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
-        <v>67</v>
+        <v>9</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="C70" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="D70" s="3" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="E70" s="3">
-        <v>110</v>
+        <v>501</v>
       </c>
       <c r="F70" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G70" s="5" t="s">
-        <v>87</v>
-      </c>
       <c r="H70" s="3">
+        <v>0</v>
+      </c>
+      <c r="I70" s="3">
+        <v>0</v>
+      </c>
+      <c r="J70" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" ht="165" x14ac:dyDescent="0.25">
+      <c r="A71" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B71" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C71" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="D71" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E71" s="3">
+        <v>120</v>
+      </c>
+      <c r="F71" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="G71" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="H71" s="3">
+        <v>0</v>
+      </c>
+      <c r="I71" s="3">
+        <v>0</v>
+      </c>
+      <c r="J71" s="8" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" ht="165" x14ac:dyDescent="0.25">
+      <c r="A72" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B72" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C72" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D72" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E72" s="3">
+        <v>137</v>
+      </c>
+      <c r="F72" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="G72" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="H72" s="3">
+        <v>1</v>
+      </c>
+      <c r="I72" s="3">
+        <v>0</v>
+      </c>
+      <c r="J72" s="4" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A73" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B73" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C73" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D73" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E73" s="3">
+        <v>144</v>
+      </c>
+      <c r="F73" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="G73" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="H73" s="3">
+        <v>2</v>
+      </c>
+      <c r="I73" s="3">
+        <v>0</v>
+      </c>
+      <c r="J73" s="4" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A74" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B74" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="C74" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="E74" s="3">
+        <v>0</v>
+      </c>
+      <c r="F74" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="G74" s="3">
+        <v>0</v>
+      </c>
+      <c r="H74" s="3">
+        <v>3</v>
+      </c>
+      <c r="I74" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A75" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B75" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C75" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D75" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E75" s="3">
+        <v>140</v>
+      </c>
+      <c r="F75" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G75" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="H75" s="3">
         <v>4</v>
       </c>
-      <c r="I70" s="3">
-        <v>2</v>
-      </c>
-      <c r="J70" s="4" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="71" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A71" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="B71" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="C71" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="D71" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E71" s="3">
+      <c r="I75" s="3">
+        <v>0</v>
+      </c>
+      <c r="J75" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A76" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B76" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C76" s="3" t="s">
+        <v>292</v>
+      </c>
+      <c r="D76" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E76" s="3">
+        <v>136</v>
+      </c>
+      <c r="F76" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G76" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="H76" s="3">
+        <v>5</v>
+      </c>
+      <c r="I76" s="3">
+        <v>0</v>
+      </c>
+      <c r="J76" s="4" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A77" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B77" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C77" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D77" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E77" s="3">
+        <v>138</v>
+      </c>
+      <c r="F77" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G77" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="H77" s="3">
+        <v>6</v>
+      </c>
+      <c r="I77" s="3">
+        <v>0</v>
+      </c>
+      <c r="J77" s="4" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A78" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B78" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C78" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D78" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E78" s="3">
+        <v>122</v>
+      </c>
+      <c r="F78" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G78" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="H78" s="3">
+        <v>7</v>
+      </c>
+      <c r="I78" s="3">
+        <v>0</v>
+      </c>
+      <c r="J78" s="4" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A79" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B79" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C79" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="D79" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E79" s="3">
+        <v>146</v>
+      </c>
+      <c r="F79" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G79" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="H79" s="3">
+        <v>8</v>
+      </c>
+      <c r="I79" s="3">
+        <v>0</v>
+      </c>
+      <c r="J79" s="4" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" ht="390" x14ac:dyDescent="0.25">
+      <c r="A80" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B80" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="C80" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="D80" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E80" s="3">
+        <v>139</v>
+      </c>
+      <c r="F80" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="G80" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="H80" s="3">
+        <v>9</v>
+      </c>
+      <c r="I80" s="3">
+        <v>0</v>
+      </c>
+      <c r="J80" s="4" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A81" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B81" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="C81" s="3" t="s">
+        <v>268</v>
+      </c>
+      <c r="D81" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E81" s="3">
+        <v>141</v>
+      </c>
+      <c r="F81" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G81" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="H81" s="3">
+        <v>10</v>
+      </c>
+      <c r="I81" s="3">
+        <v>0</v>
+      </c>
+      <c r="J81" s="4" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A82" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B82" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="C82" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="E82" s="3">
+        <v>0</v>
+      </c>
+      <c r="F82" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="G82" s="3">
+        <v>0</v>
+      </c>
+      <c r="H82" s="3">
+        <v>3</v>
+      </c>
+      <c r="I82" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" ht="360" x14ac:dyDescent="0.25">
+      <c r="A83" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B83" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="C83" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="D83" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E83" s="3">
+        <v>112</v>
+      </c>
+      <c r="F83" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="G83" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="H83" s="3">
+        <v>4</v>
+      </c>
+      <c r="I83" s="3">
+        <v>2</v>
+      </c>
+      <c r="J83" s="4" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A84" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B84" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="C84" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="D84" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E84" s="3">
+        <v>110</v>
+      </c>
+      <c r="F84" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G84" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="H84" s="3">
+        <v>5</v>
+      </c>
+      <c r="I84" s="3">
+        <v>2</v>
+      </c>
+      <c r="J84" s="4" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A85" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B85" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="C85" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="D85" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E85" s="3">
         <v>111</v>
       </c>
-      <c r="F71" s="3" t="s">
-        <v>196</v>
-      </c>
-      <c r="G71" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="H71" s="3">
-        <v>5</v>
-      </c>
-      <c r="I71" s="3">
-        <v>2</v>
-      </c>
-      <c r="J71" s="4" t="s">
-        <v>238</v>
+      <c r="F85" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="G85" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="H85" s="3">
+        <v>6</v>
+      </c>
+      <c r="I85" s="3">
+        <v>2</v>
+      </c>
+      <c r="J85" s="4" t="s">
+        <v>235</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J71" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J71">
-      <sortCondition ref="A2:A71"/>
-      <sortCondition ref="I2:I71"/>
-      <sortCondition ref="H2:H71"/>
+  <autoFilter ref="A1:J85" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J85">
+      <sortCondition ref="A2:A85"/>
+      <sortCondition ref="I2:I85"/>
+      <sortCondition ref="H2:H85"/>
     </sortState>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J72">
-    <sortCondition ref="A2:A72"/>
-    <sortCondition ref="I2:I72"/>
-    <sortCondition ref="H2:H72"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:J86">
+    <sortCondition ref="A3:A86"/>
+    <sortCondition ref="I3:I86"/>
+    <sortCondition ref="H3:H86"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added multicapture for CaptureNext.
</commit_message>
<xml_diff>
--- a/src/game_params.xlsx
+++ b/src/game_params.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Activity_Data\Mancala_github\MancalaGames\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C97E103E-4E5C-44EA-BBA4-D0410976F149}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53B61B89-5AFF-4CDB-A00A-E3E05A3CD010}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="game_params" sheetId="1" r:id="rId1"/>
@@ -2007,7 +2007,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J30" sqref="J30"/>
+      <selection pane="bottomLeft" activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
CaptNext corrected/improved now works differently for mlaps versus single sow; can be decorated with both multiple capture and capt same dir; and capture log makes more sense. Allow children for both CaptNext and CaptTwoOut--added test cases to prove they work. Implemented MoveAllFirst for Adji-boto; added appropriate rules and integrated with the rest of the software.
</commit_message>
<xml_diff>
--- a/src/game_params.xlsx
+++ b/src/game_params.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Activity_Data\Mancala_github\MancalaGames\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53B61B89-5AFF-4CDB-A00A-E3E05A3CD010}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BF253A2-624D-4226-9989-84B8424FCADB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="game_params" sheetId="1" r:id="rId1"/>
@@ -651,18 +651,6 @@
     <t>When a player has no allowable moves on their turn, they must pass, and continue to do so until they have allowable moves or the game is over. The game is over when there is a clear winner or tie condition, or when neither player has an allowable move.</t>
   </si>
   <si>
-    <t>Allow rules limit the holes from which moves may start.  Disallowed holes are not selectable.
-- NONE: no special rule
-- OPP_OR_EMPTY:  Limit the allowable holes to those that end in an empty hole or reach the opponents side of the board.
-- SINGLE_TO_ZERO: Holes with single seeds may only be played if the next hole is empty.
-- SINGLE_ONLY_ALL: Holes with single seeds may only be played if all holes contain single seeds.
-- SINGLE_ALL_TO_ZERO: Holes with single seeds may only be played if all holes contain single seeds and then only if the next hole is empty.
-- TWO_ONLY_ALL: Holes with two seeds may only be played if all holes contain two seeds.
-- TWO_ONLY_ALL_RIGHT: Holes with two seeds may not be played, unless all holes contains two seeds, in which case the rightmost hole must be played.
-- FIRST_TURN_ONLY_RIGHT_TWO: The first turn must start from one of the two rightmost holes.
-- RIGHT_2_1ST_THEN_ALL_TWO:  The first turn must start from one of the two rightmost holes. Subsequent moves may only start from holes without 2 seeds, unless all holes contain zero or 2 seeds.</t>
-  </si>
-  <si>
     <t>Only valid when SOW_START is set. Changes the SOW_START behavior so that if there is only one seed in the hole, it is moved in the sow direction by one hole.</t>
   </si>
   <si>
@@ -723,10 +711,6 @@
   </si>
   <si>
     <t>The depth that the minimaxer or negamaxer will search the game tree from the current node. One value for each difficulty.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Capture from the hole after the final seed sown into an empty hole. 
-</t>
   </si>
   <si>
     <t>After the initial capture, continue capturing as long as the capture conditions are met. This multiple capture may happen in the sow direction (unsown holes) or in the opposite direction (sown holes) as determined by CAPSAMEDIR.
@@ -1122,6 +1106,23 @@
   </si>
   <si>
     <t>mdyno_lbl</t>
+  </si>
+  <si>
+    <t>Capture from the hole after the final seed sown. 
+When multiple lap sowing, the sowing does not stop for captures. Instead, sowing continues until the final seed is sown into an empty hole. Then the capture test is made on the next hole.</t>
+  </si>
+  <si>
+    <t>Allow rules limit the holes from which moves may start.  Disallowed holes are not selectable.
+- NONE: no special rule
+- OPP_OR_EMPTY:  Limit the allowable holes to those that end in an empty hole or reach the opponents side of the board.
+- SINGLE_TO_ZERO: Holes with single seeds may only be played if the next hole is empty.
+- SINGLE_ONLY_ALL: Holes with single seeds may only be played if all holes contain single seeds.
+- SINGLE_ALL_TO_ZERO: Holes with single seeds may only be played if all holes contain single seeds and then only if the next hole is empty.
+- TWO_ONLY_ALL: Holes with two seeds may only be played if all holes contain two seeds.
+- TWO_ONLY_ALL_RIGHT: Holes with two seeds may not be played, unless all holes contains two seeds, in which case the rightmost hole must be played.
+- FIRST_TURN_ONLY_RIGHT_TWO: The first turn must start from one of the two rightmost holes.
+- RIGHT_2_1ST_THEN_ALL_TWO:  The first turn must start from one of the two rightmost holes. Subsequent moves may only start from holes without 2 seeds, unless all holes contain zero or 2 seeds.
+- MOVE_ALL_HOLES_FIRST: a move must initiated from each hole once before a second move may be made from any hole.  MOVE_ALL is incompatible with all pickers and capttwoout.</t>
   </si>
 </sst>
 </file>
@@ -2006,8 +2007,8 @@
   <dimension ref="A1:J85"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F1" sqref="F1"/>
+      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2062,17 +2063,17 @@
         <v>90</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3">
         <v>0</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="G2" s="5" t="s">
         <v>84</v>
@@ -2114,7 +2115,7 @@
         <v>0</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -2146,7 +2147,7 @@
         <v>0</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -2178,7 +2179,7 @@
         <v>0</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -2210,7 +2211,7 @@
         <v>0</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -2218,16 +2219,16 @@
         <v>90</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="E7" s="3">
         <v>0</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="G7" s="5" t="s">
         <v>84</v>
@@ -2268,7 +2269,7 @@
         <v>0</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -2300,7 +2301,7 @@
         <v>0</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2332,7 +2333,7 @@
         <v>0</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -2340,19 +2341,19 @@
         <v>90</v>
       </c>
       <c r="B11" s="3" t="s">
+        <v>280</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="E11" s="3">
+        <v>0</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>270</v>
+      </c>
+      <c r="G11" s="5" t="s">
         <v>282</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="E11" s="3">
-        <v>0</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>272</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>284</v>
       </c>
       <c r="H11" s="3">
         <v>9</v>
@@ -2361,7 +2362,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>90</v>
       </c>
@@ -2390,7 +2391,7 @@
         <v>0</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>219</v>
+        <v>303</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -2422,7 +2423,7 @@
         <v>0</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -2430,7 +2431,7 @@
         <v>90</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>114</v>
@@ -2439,7 +2440,7 @@
         <v>0</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="G14" s="5" t="s">
         <v>84</v>
@@ -2480,7 +2481,7 @@
         <v>2</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2512,7 +2513,7 @@
         <v>2</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
@@ -2520,16 +2521,16 @@
         <v>90</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="E17" s="3">
         <v>0</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="G17" s="5" t="s">
         <v>84</v>
@@ -2546,10 +2547,10 @@
         <v>90</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>22</v>
@@ -2570,7 +2571,7 @@
         <v>2</v>
       </c>
       <c r="J18" s="4" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
@@ -2666,7 +2667,7 @@
         <v>2</v>
       </c>
       <c r="J21" s="4" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
@@ -2674,16 +2675,16 @@
         <v>90</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="E22" s="3">
         <v>0</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="G22" s="5" t="s">
         <v>84</v>
@@ -2724,7 +2725,7 @@
         <v>2</v>
       </c>
       <c r="J23" s="4" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="135" x14ac:dyDescent="0.25">
@@ -2756,7 +2757,7 @@
         <v>2</v>
       </c>
       <c r="J24" s="4" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="409.5" x14ac:dyDescent="0.25">
@@ -2788,7 +2789,7 @@
         <v>0</v>
       </c>
       <c r="J25" s="4" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="105" x14ac:dyDescent="0.25">
@@ -2796,10 +2797,10 @@
         <v>36</v>
       </c>
       <c r="B26" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="C26" s="3" t="s">
         <v>262</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>264</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>22</v>
@@ -2820,7 +2821,7 @@
         <v>0</v>
       </c>
       <c r="J26" s="4" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
@@ -2828,16 +2829,16 @@
         <v>36</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="E27" s="3">
         <v>0</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="G27" s="5" t="s">
         <v>84</v>
@@ -2849,7 +2850,7 @@
         <v>0</v>
       </c>
       <c r="J27" s="4" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="150" x14ac:dyDescent="0.25">
@@ -2881,7 +2882,7 @@
         <v>0</v>
       </c>
       <c r="J28" s="4" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="180" x14ac:dyDescent="0.25">
@@ -2913,7 +2914,7 @@
         <v>0</v>
       </c>
       <c r="J29" s="4" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
@@ -2921,16 +2922,16 @@
         <v>36</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="E30" s="3">
         <v>0</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="G30" s="3">
         <v>0</v>
@@ -2974,7 +2975,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="180" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" ht="210" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>36</v>
       </c>
@@ -3003,7 +3004,7 @@
         <v>0</v>
       </c>
       <c r="J32" s="4" t="s">
-        <v>202</v>
+        <v>304</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3035,7 +3036,7 @@
         <v>2</v>
       </c>
       <c r="J33" s="4" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
@@ -3067,7 +3068,7 @@
         <v>2</v>
       </c>
       <c r="J34" s="4" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
@@ -3075,16 +3076,16 @@
         <v>36</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="E35" s="3">
         <v>0</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="G35" s="3">
         <v>0</v>
@@ -3157,7 +3158,7 @@
         <v>2</v>
       </c>
       <c r="J37" s="4" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="38" spans="1:10" ht="150" x14ac:dyDescent="0.25">
@@ -3189,7 +3190,7 @@
         <v>2</v>
       </c>
       <c r="J38" s="4" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
@@ -3197,16 +3198,16 @@
         <v>36</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="E39" s="3">
         <v>0</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="G39" s="3">
         <v>0</v>
@@ -3238,7 +3239,7 @@
         <v>42</v>
       </c>
       <c r="G40" s="5" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="H40" s="3">
         <v>7</v>
@@ -3247,7 +3248,7 @@
         <v>2</v>
       </c>
       <c r="J40" s="4" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="41" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -3311,7 +3312,7 @@
         <v>2</v>
       </c>
       <c r="J42" s="4" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="43" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -3343,7 +3344,7 @@
         <v>2</v>
       </c>
       <c r="J43" s="4" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -3375,7 +3376,7 @@
         <v>0</v>
       </c>
       <c r="J44" s="4" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
@@ -3567,7 +3568,7 @@
         <v>0</v>
       </c>
       <c r="J50" s="4" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
@@ -3599,7 +3600,7 @@
         <v>0</v>
       </c>
       <c r="J51" s="4" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
@@ -3631,7 +3632,7 @@
         <v>0</v>
       </c>
       <c r="J52" s="4" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
@@ -3639,16 +3640,16 @@
         <v>123</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E53" s="3">
         <v>0</v>
       </c>
       <c r="F53" s="3" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="G53" s="3">
         <v>0</v>
@@ -3680,7 +3681,7 @@
         <v>87</v>
       </c>
       <c r="G54" s="3" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="H54" s="3">
         <v>6</v>
@@ -3689,7 +3690,7 @@
         <v>0</v>
       </c>
       <c r="J54" s="4" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
@@ -3712,7 +3713,7 @@
         <v>87</v>
       </c>
       <c r="G55" s="3" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="H55" s="3">
         <v>7</v>
@@ -3721,7 +3722,7 @@
         <v>0</v>
       </c>
       <c r="J55" s="4" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
@@ -3753,7 +3754,7 @@
         <v>0</v>
       </c>
       <c r="J56" s="4" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
@@ -3761,16 +3762,16 @@
         <v>123</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="E57" s="3">
         <v>0</v>
       </c>
       <c r="F57" s="3" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="G57" s="3">
         <v>0</v>
@@ -3802,7 +3803,7 @@
         <v>87</v>
       </c>
       <c r="G58" s="3" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="H58" s="3">
         <v>2</v>
@@ -3811,7 +3812,7 @@
         <v>2</v>
       </c>
       <c r="J58" s="4" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="59" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -3822,7 +3823,7 @@
         <v>124</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="D59" s="3" t="s">
         <v>125</v>
@@ -3843,7 +3844,7 @@
         <v>2</v>
       </c>
       <c r="J59" s="4" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="60" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -3854,7 +3855,7 @@
         <v>126</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D60" s="3" t="s">
         <v>125</v>
@@ -3875,7 +3876,7 @@
         <v>2</v>
       </c>
       <c r="J60" s="4" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="61" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3886,7 +3887,7 @@
         <v>127</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="D61" s="3" t="s">
         <v>125</v>
@@ -3907,7 +3908,7 @@
         <v>2</v>
       </c>
       <c r="J61" s="4" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="62" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3918,7 +3919,7 @@
         <v>128</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D62" s="3" t="s">
         <v>125</v>
@@ -3939,7 +3940,7 @@
         <v>2</v>
       </c>
       <c r="J62" s="4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="63" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -3950,7 +3951,7 @@
         <v>129</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="D63" s="3" t="s">
         <v>125</v>
@@ -3971,7 +3972,7 @@
         <v>2</v>
       </c>
       <c r="J63" s="4" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="64" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -3982,7 +3983,7 @@
         <v>130</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D64" s="3" t="s">
         <v>125</v>
@@ -4003,7 +4004,7 @@
         <v>2</v>
       </c>
       <c r="J64" s="4" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="65" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -4014,7 +4015,7 @@
         <v>133</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="D65" s="3" t="s">
         <v>125</v>
@@ -4035,7 +4036,7 @@
         <v>2</v>
       </c>
       <c r="J65" s="4" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="66" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -4067,7 +4068,7 @@
         <v>2</v>
       </c>
       <c r="J66" s="4" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.25">
@@ -4177,7 +4178,7 @@
         <v>81</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="D71" s="3" t="s">
         <v>22</v>
@@ -4198,7 +4199,7 @@
         <v>0</v>
       </c>
       <c r="J71" s="8" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="72" spans="1:10" ht="165" x14ac:dyDescent="0.25">
@@ -4230,7 +4231,7 @@
         <v>0</v>
       </c>
       <c r="J72" s="4" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="73" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -4262,7 +4263,7 @@
         <v>0</v>
       </c>
       <c r="J73" s="4" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.25">
@@ -4270,16 +4271,16 @@
         <v>66</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="E74" s="3">
         <v>0</v>
       </c>
       <c r="F74" s="3" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="G74" s="3">
         <v>0</v>
@@ -4331,7 +4332,7 @@
         <v>76</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="D76" s="3" t="s">
         <v>22</v>
@@ -4352,7 +4353,7 @@
         <v>0</v>
       </c>
       <c r="J76" s="4" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="77" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -4384,7 +4385,7 @@
         <v>0</v>
       </c>
       <c r="J77" s="4" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="78" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -4416,7 +4417,7 @@
         <v>0</v>
       </c>
       <c r="J78" s="4" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.25">
@@ -4448,7 +4449,7 @@
         <v>0</v>
       </c>
       <c r="J79" s="4" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="80" spans="1:10" ht="390" x14ac:dyDescent="0.25">
@@ -4480,7 +4481,7 @@
         <v>0</v>
       </c>
       <c r="J80" s="4" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="81" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -4488,10 +4489,10 @@
         <v>66</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D81" s="3" t="s">
         <v>22</v>
@@ -4512,7 +4513,7 @@
         <v>0</v>
       </c>
       <c r="J81" s="4" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.25">
@@ -4520,16 +4521,16 @@
         <v>66</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="E82" s="3">
         <v>0</v>
       </c>
       <c r="F82" s="3" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="G82" s="3">
         <v>0</v>
@@ -4570,7 +4571,7 @@
         <v>2</v>
       </c>
       <c r="J83" s="4" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="84" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -4634,7 +4635,7 @@
         <v>2</v>
       </c>
       <c r="J85" s="4" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed the type of multicapt to int and made it so that the number of multi-captured holes can be limited. Limiting holes is only supported by CaptMultiple, the specialty capturers have not been updated. Updated all game files.
</commit_message>
<xml_diff>
--- a/src/game_params.xlsx
+++ b/src/game_params.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Activity_Data\Mancala_github\MancalaGames\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BF253A2-624D-4226-9989-84B8424FCADB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{773909ED-950A-48D6-AC1D-9E1AC16526B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -713,10 +713,6 @@
     <t>The depth that the minimaxer or negamaxer will search the game tree from the current node. One value for each difficulty.</t>
   </si>
   <si>
-    <t>After the initial capture, continue capturing as long as the capture conditions are met. This multiple capture may happen in the sow direction (unsown holes) or in the opposite direction (sown holes) as determined by CAPSAMEDIR.
-See individual capture mechanism for any special requirements.</t>
-  </si>
-  <si>
     <t>Only meaninful with MULTICAPT. Captures are done in the same direction as the sowing, i.e. following the final hole sown. If not set, captures are done from the holes just sown.</t>
   </si>
   <si>
@@ -1123,6 +1119,13 @@
 - FIRST_TURN_ONLY_RIGHT_TWO: The first turn must start from one of the two rightmost holes.
 - RIGHT_2_1ST_THEN_ALL_TWO:  The first turn must start from one of the two rightmost holes. Subsequent moves may only start from holes without 2 seeds, unless all holes contain zero or 2 seeds.
 - MOVE_ALL_HOLES_FIRST: a move must initiated from each hole once before a second move may be made from any hole.  MOVE_ALL is incompatible with all pickers and capttwoout.</t>
+  </si>
+  <si>
+    <t>An int to describe possible multicaptures:
+ 0 no multiple captures.
+ -1: After the initial capture, continue capturing as long as the capture conditions are met. This multiple capture may happen in the sow direction (unsown holes) or in the opposite direction (sown holes) as determined by CAPSAMEDIR.
+ 1 .. holes: capture at most n holes that meet the capture conditions.
+See individual capture mechanism for any special requirements.</t>
   </si>
 </sst>
 </file>
@@ -2007,8 +2010,8 @@
   <dimension ref="A1:J85"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J32" sqref="J32"/>
+      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2063,17 +2066,17 @@
         <v>90</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>278</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>279</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3">
         <v>0</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="G2" s="5" t="s">
         <v>84</v>
@@ -2115,7 +2118,7 @@
         <v>0</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -2147,7 +2150,7 @@
         <v>0</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -2179,7 +2182,7 @@
         <v>0</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -2211,7 +2214,7 @@
         <v>0</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -2219,16 +2222,16 @@
         <v>90</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>283</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>284</v>
-      </c>
       <c r="E7" s="3">
         <v>0</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="G7" s="5" t="s">
         <v>84</v>
@@ -2269,7 +2272,7 @@
         <v>0</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -2301,7 +2304,7 @@
         <v>0</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2341,19 +2344,19 @@
         <v>90</v>
       </c>
       <c r="B11" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>280</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="E11" s="3">
+        <v>0</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>269</v>
+      </c>
+      <c r="G11" s="5" t="s">
         <v>281</v>
-      </c>
-      <c r="E11" s="3">
-        <v>0</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>270</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>282</v>
       </c>
       <c r="H11" s="3">
         <v>9</v>
@@ -2391,7 +2394,7 @@
         <v>0</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -2423,7 +2426,7 @@
         <v>0</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -2431,7 +2434,7 @@
         <v>90</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>114</v>
@@ -2440,7 +2443,7 @@
         <v>0</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="G14" s="5" t="s">
         <v>84</v>
@@ -2452,7 +2455,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>90</v>
       </c>
@@ -2469,10 +2472,10 @@
         <v>124</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>39</v>
+        <v>11</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>40</v>
+        <v>84</v>
       </c>
       <c r="H15" s="3">
         <v>1</v>
@@ -2481,7 +2484,7 @@
         <v>2</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>218</v>
+        <v>304</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2513,7 +2516,7 @@
         <v>2</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
@@ -2521,16 +2524,16 @@
         <v>90</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E17" s="3">
         <v>0</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="G17" s="5" t="s">
         <v>84</v>
@@ -2547,10 +2550,10 @@
         <v>90</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>22</v>
@@ -2571,7 +2574,7 @@
         <v>2</v>
       </c>
       <c r="J18" s="4" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
@@ -2667,7 +2670,7 @@
         <v>2</v>
       </c>
       <c r="J21" s="4" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
@@ -2675,16 +2678,16 @@
         <v>90</v>
       </c>
       <c r="B22" s="3" t="s">
+        <v>286</v>
+      </c>
+      <c r="C22" s="3" t="s">
         <v>287</v>
       </c>
-      <c r="C22" s="3" t="s">
-        <v>288</v>
-      </c>
       <c r="E22" s="3">
         <v>0</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="G22" s="5" t="s">
         <v>84</v>
@@ -2757,7 +2760,7 @@
         <v>2</v>
       </c>
       <c r="J24" s="4" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="409.5" x14ac:dyDescent="0.25">
@@ -2789,7 +2792,7 @@
         <v>0</v>
       </c>
       <c r="J25" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="105" x14ac:dyDescent="0.25">
@@ -2797,10 +2800,10 @@
         <v>36</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>22</v>
@@ -2821,7 +2824,7 @@
         <v>0</v>
       </c>
       <c r="J26" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
@@ -2829,16 +2832,16 @@
         <v>36</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="E27" s="3">
         <v>0</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="G27" s="5" t="s">
         <v>84</v>
@@ -2850,7 +2853,7 @@
         <v>0</v>
       </c>
       <c r="J27" s="4" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="150" x14ac:dyDescent="0.25">
@@ -2882,7 +2885,7 @@
         <v>0</v>
       </c>
       <c r="J28" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="180" x14ac:dyDescent="0.25">
@@ -2914,7 +2917,7 @@
         <v>0</v>
       </c>
       <c r="J29" s="4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
@@ -2922,16 +2925,16 @@
         <v>36</v>
       </c>
       <c r="B30" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="C30" s="3" t="s">
         <v>299</v>
       </c>
-      <c r="C30" s="3" t="s">
-        <v>300</v>
-      </c>
       <c r="E30" s="3">
         <v>0</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="G30" s="3">
         <v>0</v>
@@ -3004,7 +3007,7 @@
         <v>0</v>
       </c>
       <c r="J32" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3036,7 +3039,7 @@
         <v>2</v>
       </c>
       <c r="J33" s="4" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
@@ -3068,7 +3071,7 @@
         <v>2</v>
       </c>
       <c r="J34" s="4" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
@@ -3076,16 +3079,16 @@
         <v>36</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="E35" s="3">
         <v>0</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="G35" s="3">
         <v>0</v>
@@ -3158,7 +3161,7 @@
         <v>2</v>
       </c>
       <c r="J37" s="4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="38" spans="1:10" ht="150" x14ac:dyDescent="0.25">
@@ -3190,7 +3193,7 @@
         <v>2</v>
       </c>
       <c r="J38" s="4" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
@@ -3198,16 +3201,16 @@
         <v>36</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="E39" s="3">
         <v>0</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="G39" s="3">
         <v>0</v>
@@ -3239,7 +3242,7 @@
         <v>42</v>
       </c>
       <c r="G40" s="5" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="H40" s="3">
         <v>7</v>
@@ -3248,7 +3251,7 @@
         <v>2</v>
       </c>
       <c r="J40" s="4" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="41" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -3312,7 +3315,7 @@
         <v>2</v>
       </c>
       <c r="J42" s="4" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="43" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -3344,7 +3347,7 @@
         <v>2</v>
       </c>
       <c r="J43" s="4" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -3376,7 +3379,7 @@
         <v>0</v>
       </c>
       <c r="J44" s="4" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
@@ -3568,7 +3571,7 @@
         <v>0</v>
       </c>
       <c r="J50" s="4" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
@@ -3640,16 +3643,16 @@
         <v>123</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="E53" s="3">
         <v>0</v>
       </c>
       <c r="F53" s="3" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="G53" s="3">
         <v>0</v>
@@ -3681,7 +3684,7 @@
         <v>87</v>
       </c>
       <c r="G54" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="H54" s="3">
         <v>6</v>
@@ -3713,7 +3716,7 @@
         <v>87</v>
       </c>
       <c r="G55" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="H55" s="3">
         <v>7</v>
@@ -3762,16 +3765,16 @@
         <v>123</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E57" s="3">
         <v>0</v>
       </c>
       <c r="F57" s="3" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="G57" s="3">
         <v>0</v>
@@ -3803,7 +3806,7 @@
         <v>87</v>
       </c>
       <c r="G58" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="H58" s="3">
         <v>2</v>
@@ -3823,7 +3826,7 @@
         <v>124</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D59" s="3" t="s">
         <v>125</v>
@@ -3855,7 +3858,7 @@
         <v>126</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D60" s="3" t="s">
         <v>125</v>
@@ -3887,7 +3890,7 @@
         <v>127</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D61" s="3" t="s">
         <v>125</v>
@@ -3908,7 +3911,7 @@
         <v>2</v>
       </c>
       <c r="J61" s="4" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="62" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3919,7 +3922,7 @@
         <v>128</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D62" s="3" t="s">
         <v>125</v>
@@ -3951,7 +3954,7 @@
         <v>129</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D63" s="3" t="s">
         <v>125</v>
@@ -3983,7 +3986,7 @@
         <v>130</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D64" s="3" t="s">
         <v>125</v>
@@ -4015,7 +4018,7 @@
         <v>133</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D65" s="3" t="s">
         <v>125</v>
@@ -4178,7 +4181,7 @@
         <v>81</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D71" s="3" t="s">
         <v>22</v>
@@ -4199,7 +4202,7 @@
         <v>0</v>
       </c>
       <c r="J71" s="8" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="72" spans="1:10" ht="165" x14ac:dyDescent="0.25">
@@ -4231,7 +4234,7 @@
         <v>0</v>
       </c>
       <c r="J72" s="4" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="73" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -4263,7 +4266,7 @@
         <v>0</v>
       </c>
       <c r="J73" s="4" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.25">
@@ -4271,16 +4274,16 @@
         <v>66</v>
       </c>
       <c r="B74" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="C74" s="3" t="s">
         <v>294</v>
       </c>
-      <c r="C74" s="3" t="s">
-        <v>295</v>
-      </c>
       <c r="E74" s="3">
         <v>0</v>
       </c>
       <c r="F74" s="3" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="G74" s="3">
         <v>0</v>
@@ -4332,7 +4335,7 @@
         <v>76</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D76" s="3" t="s">
         <v>22</v>
@@ -4353,7 +4356,7 @@
         <v>0</v>
       </c>
       <c r="J76" s="4" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="77" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -4385,7 +4388,7 @@
         <v>0</v>
       </c>
       <c r="J77" s="4" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="78" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -4449,7 +4452,7 @@
         <v>0</v>
       </c>
       <c r="J79" s="4" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="80" spans="1:10" ht="390" x14ac:dyDescent="0.25">
@@ -4481,7 +4484,7 @@
         <v>0</v>
       </c>
       <c r="J80" s="4" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="81" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -4489,10 +4492,10 @@
         <v>66</v>
       </c>
       <c r="B81" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="C81" s="3" t="s">
         <v>265</v>
-      </c>
-      <c r="C81" s="3" t="s">
-        <v>266</v>
       </c>
       <c r="D81" s="3" t="s">
         <v>22</v>
@@ -4513,7 +4516,7 @@
         <v>0</v>
       </c>
       <c r="J81" s="4" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.25">
@@ -4521,16 +4524,16 @@
         <v>66</v>
       </c>
       <c r="B82" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="C82" s="3" t="s">
         <v>292</v>
       </c>
-      <c r="C82" s="3" t="s">
-        <v>293</v>
-      </c>
       <c r="E82" s="3">
         <v>0</v>
       </c>
       <c r="F82" s="3" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="G82" s="3">
         <v>0</v>
@@ -4571,7 +4574,7 @@
         <v>2</v>
       </c>
       <c r="J83" s="4" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="84" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -4635,7 +4638,7 @@
         <v>2</v>
       </c>
       <c r="J85" s="4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added an option to control how unclaimed seeds are allocated/scored. Corrected an option in Vai_Lun_Thlan.txt. Added Adji_Kui_I, Mandoli and Obridjie.
</commit_message>
<xml_diff>
--- a/src/game_params.xlsx
+++ b/src/game_params.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Activity_Data\Mancala_github\MancalaGames\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{773909ED-950A-48D6-AC1D-9E1AC16526B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89F2684E-046A-44D6-833A-D6B0DFF96B5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="game_params" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">game_params!$A$1:$J$85</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">game_params!$A$1:$J$86</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="554" uniqueCount="305">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="560" uniqueCount="309">
   <si>
     <t>tab</t>
   </si>
@@ -1011,9 +1011,6 @@
     <t>Initial Setup</t>
   </si>
   <si>
-    <t>Parameters that control the initial game setup.</t>
-  </si>
-  <si>
     <t>rnd_lbl</t>
   </si>
   <si>
@@ -1126,6 +1123,26 @@
  -1: After the initial capture, continue capturing as long as the capture conditions are met. This multiple capture may happen in the sow direction (unsown holes) or in the opposite direction (sown holes) as determined by CAPSAMEDIR.
  1 .. holes: capture at most n holes that meet the capture conditions.
 See individual capture mechanism for any special requirements.</t>
+  </si>
+  <si>
+    <t>unclaimed</t>
+  </si>
+  <si>
+    <t>End Game Seeds</t>
+  </si>
+  <si>
+    <t>EndGameSeeds</t>
+  </si>
+  <si>
+    <t>HOLE_OWNER</t>
+  </si>
+  <si>
+    <t>Defines how to score any unclaimed seeds when a game has ended. This is not used if the game has a clear winner, e.g. one player has collected more than half the seeds for a MAX_SEEDS game.
+- HOLE_OWNER: unclaimed seeds go to the hole owner.
+- DONT_SCORE: unclaimed seeds do not score (they are ignored).
+- LAST_MOVER: unclaimed seeds go the player that moved last.
+- UNFED_PLAYER: only valid for MUSTSHARE games. If the game ended without one player being able share seeds, the seeds go to the player without seeds (the unfed player).
+- DIVVIED: the seeds are divided between the two players (an extra seed goes to the player with fewer seeds).</t>
   </si>
 </sst>
 </file>
@@ -2007,11 +2024,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:J85"/>
+  <dimension ref="A1:J86"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J15" sqref="J15"/>
+      <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A86" sqref="A86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2066,10 +2083,10 @@
         <v>90</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>277</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>278</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3">
@@ -2222,10 +2239,10 @@
         <v>90</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>282</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>283</v>
       </c>
       <c r="E7" s="3">
         <v>0</v>
@@ -2289,7 +2306,7 @@
         <v>22</v>
       </c>
       <c r="E9" s="3">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>111</v>
@@ -2321,7 +2338,7 @@
         <v>22</v>
       </c>
       <c r="E10" s="3">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>39</v>
@@ -2344,10 +2361,10 @@
         <v>90</v>
       </c>
       <c r="B11" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>279</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>280</v>
       </c>
       <c r="E11" s="3">
         <v>0</v>
@@ -2356,7 +2373,7 @@
         <v>269</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="H11" s="3">
         <v>9</v>
@@ -2394,7 +2411,7 @@
         <v>0</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -2434,7 +2451,7 @@
         <v>90</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>114</v>
@@ -2484,7 +2501,7 @@
         <v>2</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2524,10 +2541,10 @@
         <v>90</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E17" s="3">
         <v>0</v>
@@ -2553,7 +2570,7 @@
         <v>262</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>22</v>
@@ -2678,10 +2695,10 @@
         <v>90</v>
       </c>
       <c r="B22" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="C22" s="3" t="s">
         <v>286</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>287</v>
       </c>
       <c r="E22" s="3">
         <v>0</v>
@@ -2827,24 +2844,27 @@
         <v>260</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>36</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>297</v>
+        <v>304</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>270</v>
+        <v>305</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="E27" s="3">
-        <v>0</v>
+        <v>146</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>269</v>
+        <v>306</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>84</v>
+        <v>307</v>
       </c>
       <c r="H27" s="3">
         <v>2</v>
@@ -2853,30 +2873,27 @@
         <v>0</v>
       </c>
       <c r="J27" s="4" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" ht="150" x14ac:dyDescent="0.25">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>36</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>56</v>
+        <v>296</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>22</v>
+        <v>270</v>
       </c>
       <c r="E28" s="3">
-        <v>142</v>
+        <v>0</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>58</v>
+        <v>269</v>
       </c>
       <c r="G28" s="5" t="s">
-        <v>59</v>
+        <v>84</v>
       </c>
       <c r="H28" s="3">
         <v>3</v>
@@ -2884,31 +2901,28 @@
       <c r="I28" s="3">
         <v>0</v>
       </c>
-      <c r="J28" s="4" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" ht="180" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:10" ht="150" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>36</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>175</v>
+        <v>56</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>174</v>
+        <v>57</v>
       </c>
       <c r="D29" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E29" s="3">
-        <v>132</v>
+        <v>142</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>176</v>
+        <v>58</v>
       </c>
       <c r="G29" s="5" t="s">
-        <v>164</v>
+        <v>59</v>
       </c>
       <c r="H29" s="3">
         <v>4</v>
@@ -2917,33 +2931,39 @@
         <v>0</v>
       </c>
       <c r="J29" s="4" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" ht="180" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>36</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>298</v>
+        <v>175</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>299</v>
+        <v>174</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="E30" s="3">
-        <v>0</v>
+        <v>132</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>269</v>
-      </c>
-      <c r="G30" s="3">
-        <v>0</v>
+        <v>176</v>
+      </c>
+      <c r="G30" s="5" t="s">
+        <v>164</v>
       </c>
       <c r="H30" s="3">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I30" s="3">
         <v>0</v>
+      </c>
+      <c r="J30" s="4" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
@@ -2951,22 +2971,19 @@
         <v>36</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>60</v>
+        <v>297</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="D31" s="3" t="s">
-        <v>22</v>
+        <v>298</v>
       </c>
       <c r="E31" s="3">
-        <v>119</v>
+        <v>0</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G31" s="5" t="s">
-        <v>62</v>
+        <v>269</v>
+      </c>
+      <c r="G31" s="3">
+        <v>0</v>
       </c>
       <c r="H31" s="3">
         <v>7</v>
@@ -2974,31 +2991,28 @@
       <c r="I31" s="3">
         <v>0</v>
       </c>
-      <c r="J31" s="4" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" ht="210" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>36</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>161</v>
+        <v>60</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>162</v>
+        <v>61</v>
       </c>
       <c r="D32" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E32" s="3">
-        <v>101</v>
+        <v>119</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>163</v>
+        <v>11</v>
       </c>
       <c r="G32" s="5" t="s">
-        <v>164</v>
+        <v>62</v>
       </c>
       <c r="H32" s="3">
         <v>8</v>
@@ -3007,71 +3021,71 @@
         <v>0</v>
       </c>
       <c r="J32" s="4" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" ht="210" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>36</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>49</v>
+        <v>161</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>50</v>
+        <v>162</v>
       </c>
       <c r="D33" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E33" s="3">
-        <v>143</v>
+        <v>101</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>39</v>
+        <v>163</v>
       </c>
       <c r="G33" s="5" t="s">
-        <v>51</v>
+        <v>164</v>
       </c>
       <c r="H33" s="3">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="I33" s="3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J33" s="4" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>36</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D34" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E34" s="3">
-        <v>127</v>
+        <v>143</v>
       </c>
       <c r="F34" s="3" t="s">
         <v>39</v>
       </c>
       <c r="G34" s="5" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="H34" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I34" s="3">
         <v>2</v>
       </c>
       <c r="J34" s="4" t="s">
-        <v>229</v>
+        <v>254</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
@@ -3079,57 +3093,57 @@
         <v>36</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>301</v>
+        <v>47</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>300</v>
+        <v>48</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="E35" s="3">
-        <v>0</v>
+        <v>127</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>269</v>
-      </c>
-      <c r="G35" s="3">
-        <v>0</v>
+        <v>39</v>
+      </c>
+      <c r="G35" s="5" t="s">
+        <v>40</v>
       </c>
       <c r="H35" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I35" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="36" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="J35" s="4" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>36</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>37</v>
+        <v>300</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D36" s="3" t="s">
-        <v>22</v>
+        <v>299</v>
       </c>
       <c r="E36" s="3">
-        <v>125</v>
+        <v>0</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="G36" s="5" t="s">
-        <v>40</v>
+        <v>269</v>
+      </c>
+      <c r="G36" s="3">
+        <v>0</v>
       </c>
       <c r="H36" s="3">
         <v>3</v>
       </c>
       <c r="I36" s="3">
         <v>2</v>
-      </c>
-      <c r="J36" s="4" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="37" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3137,16 +3151,16 @@
         <v>36</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>64</v>
+        <v>37</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>65</v>
+        <v>38</v>
       </c>
       <c r="D37" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E37" s="3">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F37" s="3" t="s">
         <v>39</v>
@@ -3161,30 +3175,30 @@
         <v>2</v>
       </c>
       <c r="J37" s="4" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" ht="150" x14ac:dyDescent="0.25">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>36</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>115</v>
+        <v>64</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>116</v>
+        <v>65</v>
       </c>
       <c r="D38" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E38" s="3">
-        <v>117</v>
+        <v>126</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>117</v>
+        <v>39</v>
       </c>
       <c r="G38" s="5" t="s">
-        <v>118</v>
+        <v>40</v>
       </c>
       <c r="H38" s="3">
         <v>5</v>
@@ -3193,27 +3207,30 @@
         <v>2</v>
       </c>
       <c r="J38" s="4" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" ht="150" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>36</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>272</v>
+        <v>115</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>296</v>
+        <v>116</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="E39" s="3">
-        <v>0</v>
+        <v>117</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>269</v>
-      </c>
-      <c r="G39" s="3">
-        <v>0</v>
+        <v>117</v>
+      </c>
+      <c r="G39" s="5" t="s">
+        <v>118</v>
       </c>
       <c r="H39" s="3">
         <v>6</v>
@@ -3221,28 +3238,28 @@
       <c r="I39" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="40" spans="1:10" ht="210" x14ac:dyDescent="0.25">
+      <c r="J39" s="4" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>36</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>41</v>
+        <v>271</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D40" s="3" t="s">
-        <v>22</v>
+        <v>295</v>
       </c>
       <c r="E40" s="3">
-        <v>135</v>
+        <v>0</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="G40" s="5" t="s">
-        <v>251</v>
+        <v>269</v>
+      </c>
+      <c r="G40" s="3">
+        <v>0</v>
       </c>
       <c r="H40" s="3">
         <v>7</v>
@@ -3250,31 +3267,28 @@
       <c r="I40" s="3">
         <v>2</v>
       </c>
-      <c r="J40" s="4" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:10" ht="210" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>36</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D41" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E41" s="3">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="G41" s="5" t="s">
-        <v>46</v>
+        <v>251</v>
       </c>
       <c r="H41" s="3">
         <v>8</v>
@@ -3283,30 +3297,30 @@
         <v>2</v>
       </c>
       <c r="J41" s="4" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" ht="330" x14ac:dyDescent="0.25">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>36</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>185</v>
+        <v>43</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>186</v>
+        <v>44</v>
       </c>
       <c r="D42" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E42" s="3">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>187</v>
+        <v>45</v>
       </c>
       <c r="G42" s="5" t="s">
-        <v>194</v>
+        <v>46</v>
       </c>
       <c r="H42" s="3">
         <v>9</v>
@@ -3315,30 +3329,30 @@
         <v>2</v>
       </c>
       <c r="J42" s="4" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" ht="330" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>36</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>79</v>
+        <v>185</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>80</v>
+        <v>186</v>
       </c>
       <c r="D43" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E43" s="3">
-        <v>102</v>
+        <v>133</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>39</v>
+        <v>187</v>
       </c>
       <c r="G43" s="5" t="s">
-        <v>40</v>
+        <v>194</v>
       </c>
       <c r="H43" s="3">
         <v>10</v>
@@ -3347,71 +3361,71 @@
         <v>2</v>
       </c>
       <c r="J43" s="4" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
-        <v>15</v>
+        <v>36</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>17</v>
+        <v>79</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>16</v>
+        <v>80</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="E44" s="3">
-        <v>1</v>
+        <v>102</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>139</v>
+        <v>39</v>
       </c>
       <c r="G44" s="5" t="s">
-        <v>19</v>
+        <v>40</v>
       </c>
       <c r="H44" s="3">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="I44" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J44" s="4" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="E45" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>11</v>
+        <v>139</v>
       </c>
       <c r="G45" s="5" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="H45" s="3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I45" s="3">
         <v>0</v>
       </c>
       <c r="J45" s="4" t="s">
-        <v>200</v>
+        <v>253</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
@@ -3419,191 +3433,191 @@
         <v>15</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="E46" s="3">
-        <v>118</v>
+        <v>2</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="G46" s="5" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="H46" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I46" s="3">
         <v>0</v>
       </c>
       <c r="J46" s="4" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D47" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E47" s="3">
-        <v>5</v>
+        <v>118</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="G47" s="6" t="s">
-        <v>137</v>
+        <v>18</v>
+      </c>
+      <c r="G47" s="5" t="s">
+        <v>25</v>
       </c>
       <c r="H47" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I47" s="3">
         <v>0</v>
       </c>
       <c r="J47" s="4" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="D48" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E48" s="3">
+        <v>5</v>
+      </c>
+      <c r="F48" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G48" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="H48" s="3">
         <v>4</v>
       </c>
-      <c r="F48" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G48" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="H48" s="3">
-        <v>0</v>
-      </c>
       <c r="I48" s="3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J48" s="4" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="E49" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="G49" s="5" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="H49" s="3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I49" s="3">
         <v>2</v>
       </c>
       <c r="J49" s="4" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A50" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E50" s="3">
+        <v>3</v>
+      </c>
+      <c r="F50" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G50" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="H50" s="3">
+        <v>2</v>
+      </c>
+      <c r="I50" s="3">
+        <v>2</v>
+      </c>
+      <c r="J50" s="4" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="50" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A50" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="B50" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="C50" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="D50" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="E50" s="3">
-        <v>201</v>
-      </c>
-      <c r="F50" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="G50" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="H50" s="3">
-        <v>0</v>
-      </c>
-      <c r="I50" s="3">
-        <v>0</v>
-      </c>
-      <c r="J50" s="4" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
         <v>123</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="D51" s="3" t="s">
         <v>136</v>
       </c>
       <c r="E51" s="3">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="F51" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G51" s="5" t="s">
-        <v>62</v>
+        <v>141</v>
+      </c>
+      <c r="G51" s="3" t="s">
+        <v>142</v>
       </c>
       <c r="H51" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I51" s="3">
         <v>0</v>
       </c>
       <c r="J51" s="4" t="s">
-        <v>208</v>
+        <v>240</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
@@ -3611,31 +3625,31 @@
         <v>123</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>190</v>
+        <v>134</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>188</v>
+        <v>135</v>
       </c>
       <c r="D52" s="3" t="s">
         <v>136</v>
       </c>
       <c r="E52" s="3">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="F52" s="3" t="s">
-        <v>39</v>
+        <v>11</v>
       </c>
       <c r="G52" s="5" t="s">
-        <v>40</v>
+        <v>62</v>
       </c>
       <c r="H52" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I52" s="3">
         <v>0</v>
       </c>
       <c r="J52" s="4" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
@@ -3643,89 +3657,89 @@
         <v>123</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>275</v>
+        <v>190</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>274</v>
+        <v>188</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>136</v>
       </c>
       <c r="E53" s="3">
-        <v>0</v>
+        <v>202</v>
       </c>
       <c r="F53" s="3" t="s">
-        <v>269</v>
-      </c>
-      <c r="G53" s="3">
-        <v>0</v>
+        <v>39</v>
+      </c>
+      <c r="G53" s="5" t="s">
+        <v>40</v>
       </c>
       <c r="H53" s="3">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="I53" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="54" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="J53" s="4" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
         <v>123</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>147</v>
+        <v>274</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="D54" s="3" t="s">
-        <v>146</v>
+        <v>273</v>
       </c>
       <c r="E54" s="3">
-        <v>210</v>
+        <v>0</v>
       </c>
       <c r="F54" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="G54" s="3" t="s">
-        <v>245</v>
+        <v>269</v>
+      </c>
+      <c r="G54" s="3">
+        <v>0</v>
       </c>
       <c r="H54" s="3">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I54" s="3">
         <v>0</v>
       </c>
-      <c r="J54" s="4" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="55" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
         <v>123</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D55" s="3" t="s">
         <v>146</v>
       </c>
       <c r="E55" s="3">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F55" s="3" t="s">
         <v>87</v>
       </c>
       <c r="G55" s="3" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="H55" s="3">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I55" s="3">
         <v>0</v>
       </c>
       <c r="J55" s="4" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
@@ -3733,31 +3747,31 @@
         <v>123</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D56" s="3" t="s">
         <v>146</v>
       </c>
       <c r="E56" s="3">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F56" s="3" t="s">
         <v>87</v>
       </c>
       <c r="G56" s="3" t="s">
-        <v>153</v>
+        <v>243</v>
       </c>
       <c r="H56" s="3">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I56" s="3">
         <v>0</v>
       </c>
       <c r="J56" s="4" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
@@ -3765,25 +3779,31 @@
         <v>123</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>273</v>
+        <v>149</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>276</v>
+        <v>152</v>
+      </c>
+      <c r="D57" s="3" t="s">
+        <v>146</v>
       </c>
       <c r="E57" s="3">
-        <v>0</v>
+        <v>212</v>
       </c>
       <c r="F57" s="3" t="s">
-        <v>269</v>
-      </c>
-      <c r="G57" s="3">
-        <v>0</v>
+        <v>87</v>
+      </c>
+      <c r="G57" s="3" t="s">
+        <v>153</v>
       </c>
       <c r="H57" s="3">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="I57" s="3">
-        <v>2</v>
+        <v>0</v>
+      </c>
+      <c r="J57" s="4" t="s">
+        <v>205</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
@@ -3791,112 +3811,106 @@
         <v>123</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>144</v>
+        <v>272</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="D58" s="3" t="s">
-        <v>146</v>
+        <v>275</v>
       </c>
       <c r="E58" s="3">
-        <v>213</v>
+        <v>0</v>
       </c>
       <c r="F58" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="G58" s="3" t="s">
-        <v>244</v>
+        <v>269</v>
+      </c>
+      <c r="G58" s="3">
+        <v>0</v>
       </c>
       <c r="H58" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I58" s="3">
         <v>2</v>
       </c>
-      <c r="J58" s="4" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="59" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
         <v>123</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>124</v>
+        <v>144</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>238</v>
+        <v>145</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>125</v>
+        <v>146</v>
       </c>
       <c r="E59" s="3">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="F59" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G59" s="5" t="s">
-        <v>35</v>
+        <v>87</v>
+      </c>
+      <c r="G59" s="3" t="s">
+        <v>244</v>
       </c>
       <c r="H59" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I59" s="3">
         <v>2</v>
       </c>
       <c r="J59" s="4" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="60" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
         <v>123</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="D60" s="3" t="s">
         <v>125</v>
       </c>
       <c r="E60" s="3">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F60" s="3" t="s">
         <v>11</v>
       </c>
       <c r="G60" s="5" t="s">
-        <v>84</v>
+        <v>35</v>
       </c>
       <c r="H60" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I60" s="3">
         <v>2</v>
       </c>
       <c r="J60" s="4" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="61" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
         <v>123</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="D61" s="3" t="s">
         <v>125</v>
       </c>
       <c r="E61" s="3">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F61" s="3" t="s">
         <v>11</v>
@@ -3905,13 +3919,13 @@
         <v>84</v>
       </c>
       <c r="H61" s="3">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I61" s="3">
         <v>2</v>
       </c>
       <c r="J61" s="4" t="s">
-        <v>226</v>
+        <v>214</v>
       </c>
     </row>
     <row r="62" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3919,16 +3933,16 @@
         <v>123</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="D62" s="3" t="s">
         <v>125</v>
       </c>
       <c r="E62" s="3">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F62" s="3" t="s">
         <v>11</v>
@@ -3937,30 +3951,30 @@
         <v>84</v>
       </c>
       <c r="H62" s="3">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I62" s="3">
         <v>2</v>
       </c>
       <c r="J62" s="4" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="63" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
         <v>123</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="D63" s="3" t="s">
         <v>125</v>
       </c>
       <c r="E63" s="3">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F63" s="3" t="s">
         <v>11</v>
@@ -3969,13 +3983,13 @@
         <v>84</v>
       </c>
       <c r="H63" s="3">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I63" s="3">
         <v>2</v>
       </c>
       <c r="J63" s="4" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row r="64" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -3983,16 +3997,16 @@
         <v>123</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="D64" s="3" t="s">
         <v>125</v>
       </c>
       <c r="E64" s="3">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F64" s="3" t="s">
         <v>11</v>
@@ -4001,30 +4015,30 @@
         <v>84</v>
       </c>
       <c r="H64" s="3">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I64" s="3">
         <v>2</v>
       </c>
       <c r="J64" s="4" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="65" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
         <v>123</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>255</v>
+        <v>233</v>
       </c>
       <c r="D65" s="3" t="s">
         <v>125</v>
       </c>
       <c r="E65" s="3">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F65" s="3" t="s">
         <v>11</v>
@@ -4033,13 +4047,13 @@
         <v>84</v>
       </c>
       <c r="H65" s="3">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I65" s="3">
         <v>2</v>
       </c>
       <c r="J65" s="4" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
     </row>
     <row r="66" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -4047,16 +4061,16 @@
         <v>123</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>132</v>
+        <v>255</v>
       </c>
       <c r="D66" s="3" t="s">
         <v>125</v>
       </c>
       <c r="E66" s="3">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F66" s="3" t="s">
         <v>11</v>
@@ -4065,39 +4079,45 @@
         <v>84</v>
       </c>
       <c r="H66" s="3">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I66" s="3">
         <v>2</v>
       </c>
       <c r="J66" s="4" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
-        <v>9</v>
+        <v>123</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>167</v>
+        <v>131</v>
+      </c>
+      <c r="C67" s="3" t="s">
+        <v>132</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>22</v>
+        <v>125</v>
       </c>
       <c r="E67" s="3">
-        <v>121</v>
+        <v>227</v>
       </c>
       <c r="F67" s="3" t="s">
         <v>11</v>
       </c>
+      <c r="G67" s="5" t="s">
+        <v>84</v>
+      </c>
       <c r="H67" s="3">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="I67" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J67" s="4" t="s">
-        <v>169</v>
+        <v>210</v>
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.25">
@@ -4105,18 +4125,17 @@
         <v>9</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>89</v>
+        <v>167</v>
       </c>
       <c r="D68" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E68" s="3">
-        <v>145</v>
+        <v>121</v>
       </c>
       <c r="F68" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="G68" s="5"/>
+        <v>11</v>
+      </c>
       <c r="H68" s="3">
         <v>0</v>
       </c>
@@ -4124,7 +4143,7 @@
         <v>0</v>
       </c>
       <c r="J68" s="4" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.25">
@@ -4132,13 +4151,13 @@
         <v>9</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E69" s="3">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="F69" s="3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="H69" s="3">
         <v>0</v>
@@ -4147,7 +4166,7 @@
         <v>0</v>
       </c>
       <c r="J69" s="4" t="s">
-        <v>138</v>
+        <v>12</v>
       </c>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.25">
@@ -4155,13 +4174,13 @@
         <v>9</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="E70" s="3">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="F70" s="3" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="H70" s="3">
         <v>0</v>
@@ -4170,39 +4189,34 @@
         <v>0</v>
       </c>
       <c r="J70" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="71" spans="1:10" ht="165" x14ac:dyDescent="0.25">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
-        <v>66</v>
+        <v>9</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="C71" s="3" t="s">
-        <v>290</v>
+        <v>89</v>
       </c>
       <c r="D71" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E71" s="3">
-        <v>120</v>
+        <v>145</v>
       </c>
       <c r="F71" s="3" t="s">
-        <v>165</v>
-      </c>
-      <c r="G71" s="5" t="s">
-        <v>166</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="G71" s="5"/>
       <c r="H71" s="3">
         <v>0</v>
       </c>
       <c r="I71" s="3">
         <v>0</v>
       </c>
-      <c r="J71" s="8" t="s">
-        <v>241</v>
+      <c r="J71" s="4" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="72" spans="1:10" ht="165" x14ac:dyDescent="0.25">
@@ -4210,89 +4224,95 @@
         <v>66</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>67</v>
+        <v>81</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>68</v>
+        <v>289</v>
       </c>
       <c r="D72" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E72" s="3">
-        <v>137</v>
+        <v>120</v>
       </c>
       <c r="F72" s="3" t="s">
-        <v>69</v>
+        <v>165</v>
       </c>
       <c r="G72" s="5" t="s">
-        <v>70</v>
+        <v>166</v>
       </c>
       <c r="H72" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I72" s="3">
         <v>0</v>
       </c>
-      <c r="J72" s="4" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="73" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="J72" s="8" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" ht="165" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
         <v>66</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>85</v>
+        <v>67</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>86</v>
+        <v>68</v>
       </c>
       <c r="D73" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E73" s="3">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="F73" s="3" t="s">
-        <v>143</v>
+        <v>69</v>
       </c>
       <c r="G73" s="5" t="s">
-        <v>88</v>
+        <v>70</v>
       </c>
       <c r="H73" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I73" s="3">
         <v>0</v>
       </c>
       <c r="J73" s="4" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
         <v>66</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>293</v>
+        <v>85</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>294</v>
+        <v>86</v>
+      </c>
+      <c r="D74" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="E74" s="3">
-        <v>0</v>
+        <v>144</v>
       </c>
       <c r="F74" s="3" t="s">
-        <v>269</v>
-      </c>
-      <c r="G74" s="3">
-        <v>0</v>
+        <v>143</v>
+      </c>
+      <c r="G74" s="5" t="s">
+        <v>88</v>
       </c>
       <c r="H74" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I74" s="3">
         <v>0</v>
+      </c>
+      <c r="J74" s="4" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.25">
@@ -4300,48 +4320,42 @@
         <v>66</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>71</v>
+        <v>292</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="D75" s="3" t="s">
-        <v>22</v>
+        <v>293</v>
       </c>
       <c r="E75" s="3">
-        <v>140</v>
+        <v>0</v>
       </c>
       <c r="F75" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="G75" s="5" t="s">
-        <v>40</v>
+        <v>269</v>
+      </c>
+      <c r="G75" s="3">
+        <v>0</v>
       </c>
       <c r="H75" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I75" s="3">
         <v>0</v>
       </c>
-      <c r="J75" s="4" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="76" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
         <v>66</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>289</v>
+        <v>72</v>
       </c>
       <c r="D76" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E76" s="3">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="F76" s="3" t="s">
         <v>39</v>
@@ -4350,13 +4364,13 @@
         <v>40</v>
       </c>
       <c r="H76" s="3">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I76" s="3">
         <v>0</v>
       </c>
       <c r="J76" s="4" t="s">
-        <v>225</v>
+        <v>73</v>
       </c>
     </row>
     <row r="77" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -4364,16 +4378,16 @@
         <v>66</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>78</v>
+        <v>288</v>
       </c>
       <c r="D77" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E77" s="3">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F77" s="3" t="s">
         <v>39</v>
@@ -4382,13 +4396,13 @@
         <v>40</v>
       </c>
       <c r="H77" s="3">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I77" s="3">
         <v>0</v>
       </c>
       <c r="J77" s="4" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
     </row>
     <row r="78" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -4396,16 +4410,16 @@
         <v>66</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="D78" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E78" s="3">
-        <v>122</v>
+        <v>138</v>
       </c>
       <c r="F78" s="3" t="s">
         <v>39</v>
@@ -4414,30 +4428,30 @@
         <v>40</v>
       </c>
       <c r="H78" s="3">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I78" s="3">
         <v>0</v>
       </c>
       <c r="J78" s="4" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="s">
         <v>66</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="D79" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E79" s="3">
-        <v>146</v>
+        <v>122</v>
       </c>
       <c r="F79" s="3" t="s">
         <v>39</v>
@@ -4446,213 +4460,245 @@
         <v>40</v>
       </c>
       <c r="H79" s="3">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I79" s="3">
         <v>0</v>
       </c>
       <c r="J79" s="4" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="80" spans="1:10" ht="390" x14ac:dyDescent="0.25">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="s">
         <v>66</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>177</v>
+        <v>82</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>178</v>
+        <v>83</v>
       </c>
       <c r="D80" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E80" s="3">
-        <v>139</v>
+        <v>147</v>
       </c>
       <c r="F80" s="3" t="s">
-        <v>179</v>
+        <v>39</v>
       </c>
       <c r="G80" s="5" t="s">
-        <v>164</v>
+        <v>40</v>
       </c>
       <c r="H80" s="3">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I80" s="3">
         <v>0</v>
       </c>
       <c r="J80" s="4" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="81" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" ht="390" x14ac:dyDescent="0.25">
       <c r="A81" s="3" t="s">
         <v>66</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>264</v>
+        <v>177</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>265</v>
+        <v>178</v>
       </c>
       <c r="D81" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E81" s="3">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F81" s="3" t="s">
-        <v>11</v>
+        <v>179</v>
       </c>
       <c r="G81" s="5" t="s">
-        <v>84</v>
+        <v>164</v>
       </c>
       <c r="H81" s="3">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I81" s="3">
         <v>0</v>
       </c>
       <c r="J81" s="4" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A82" s="3" t="s">
         <v>66</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>291</v>
+        <v>264</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>292</v>
+        <v>265</v>
+      </c>
+      <c r="D82" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="E82" s="3">
-        <v>0</v>
+        <v>141</v>
       </c>
       <c r="F82" s="3" t="s">
-        <v>269</v>
-      </c>
-      <c r="G82" s="3">
-        <v>0</v>
+        <v>11</v>
+      </c>
+      <c r="G82" s="5" t="s">
+        <v>84</v>
       </c>
       <c r="H82" s="3">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="I82" s="3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="83" spans="1:10" ht="360" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="J82" s="4" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" s="3" t="s">
         <v>66</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>156</v>
+        <v>290</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="D83" s="3" t="s">
-        <v>22</v>
+        <v>291</v>
       </c>
       <c r="E83" s="3">
-        <v>112</v>
+        <v>0</v>
       </c>
       <c r="F83" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="G83" s="5" t="s">
-        <v>158</v>
+        <v>269</v>
+      </c>
+      <c r="G83" s="3">
+        <v>0</v>
       </c>
       <c r="H83" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I83" s="3">
         <v>2</v>
       </c>
-      <c r="J83" s="4" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="84" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="84" spans="1:10" ht="360" x14ac:dyDescent="0.25">
       <c r="A84" s="3" t="s">
         <v>66</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="D84" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E84" s="3">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="F84" s="3" t="s">
-        <v>11</v>
+        <v>159</v>
       </c>
       <c r="G84" s="5" t="s">
-        <v>84</v>
+        <v>158</v>
       </c>
       <c r="H84" s="3">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I84" s="3">
         <v>2</v>
       </c>
       <c r="J84" s="4" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="85" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A85" s="3" t="s">
         <v>66</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>191</v>
+        <v>154</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>192</v>
+        <v>155</v>
       </c>
       <c r="D85" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E85" s="3">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F85" s="3" t="s">
-        <v>193</v>
-      </c>
-      <c r="G85" s="3" t="s">
-        <v>164</v>
+        <v>11</v>
+      </c>
+      <c r="G85" s="5" t="s">
+        <v>84</v>
       </c>
       <c r="H85" s="3">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I85" s="3">
         <v>2</v>
       </c>
       <c r="J85" s="4" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A86" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B86" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="C86" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="D86" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E86" s="3">
+        <v>111</v>
+      </c>
+      <c r="F86" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="G86" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="H86" s="3">
+        <v>6</v>
+      </c>
+      <c r="I86" s="3">
+        <v>2</v>
+      </c>
+      <c r="J86" s="4" t="s">
         <v>232</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J85" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J85">
-      <sortCondition ref="A2:A85"/>
-      <sortCondition ref="I2:I85"/>
-      <sortCondition ref="H2:H85"/>
+  <autoFilter ref="A1:J86" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J86">
+      <sortCondition ref="A2:A86"/>
+      <sortCondition ref="I2:I86"/>
+      <sortCondition ref="H2:H86"/>
     </sortState>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:J86">
-    <sortCondition ref="A3:A86"/>
-    <sortCondition ref="I3:I86"/>
-    <sortCondition ref="H3:H86"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:J87">
+    <sortCondition ref="A3:A87"/>
+    <sortCondition ref="I3:I87"/>
+    <sortCondition ref="H3:H87"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Checkpoint for changing oppsidecapt to capt_side with enum type. All existing tests pass and no pylint warnings. All game prop files that used oppsidecapt where changed.
</commit_message>
<xml_diff>
--- a/src/game_params.xlsx
+++ b/src/game_params.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Activity_Data\Mancala_github\MancalaGames\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89F2684E-046A-44D6-833A-D6B0DFF96B5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7100E004-7DCC-467A-90AA-F23DC28E5E43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-25155" yWindow="780" windowWidth="22185" windowHeight="14895" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="game_params" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="560" uniqueCount="309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="560" uniqueCount="311">
   <si>
     <t>tab</t>
   </si>
@@ -315,15 +315,6 @@
   </si>
   <si>
     <t>Capture in Sow Direction</t>
-  </si>
-  <si>
-    <t>oppsidecapt</t>
-  </si>
-  <si>
-    <t>Opp Side Capt Only</t>
-  </si>
-  <si>
-    <t>Captures may only be made from your oppents side of the board.</t>
   </si>
   <si>
     <t>moveunlock</t>
@@ -1143,6 +1134,26 @@
 - LAST_MOVER: unclaimed seeds go the player that moved last.
 - UNFED_PLAYER: only valid for MUSTSHARE games. If the game ended without one player being able share seeds, the seeds go to the player without seeds (the unfed player).
 - DIVVIED: the seeds are divided between the two players (an extra seed goes to the player with fewer seeds).</t>
+  </si>
+  <si>
+    <t>capt_side</t>
+  </si>
+  <si>
+    <t>Capture side</t>
+  </si>
+  <si>
+    <t>CaptSide</t>
+  </si>
+  <si>
+    <t>BOTH</t>
+  </si>
+  <si>
+    <t>Limits which side of the board captures maybe done on:
+- BOTH: no limitations
+- OPP_SIDE: opposite side capture only.
+- OWN_SIDE: captures on own side of board only.
+- OPP_CONT: a multi-capture must begin on the opposite side of the board, but may continue onto your own side.  Requires MULTICAPT.
+- OWN_CONT: a multi-capture must being on your own side of the board and may continue onto your opponent's side. Requires multicapt.</t>
   </si>
 </sst>
 </file>
@@ -2027,8 +2038,8 @@
   <dimension ref="A1:J86"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A86" sqref="A86"/>
+      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2060,7 +2071,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>4</v>
@@ -2083,17 +2094,17 @@
         <v>90</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3">
         <v>0</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="G2" s="5" t="s">
         <v>84</v>
@@ -2111,10 +2122,10 @@
         <v>90</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>22</v>
@@ -2135,7 +2146,7 @@
         <v>0</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -2143,10 +2154,10 @@
         <v>90</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>22</v>
@@ -2167,7 +2178,7 @@
         <v>0</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -2175,10 +2186,10 @@
         <v>90</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>22</v>
@@ -2199,7 +2210,7 @@
         <v>0</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -2207,10 +2218,10 @@
         <v>90</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>22</v>
@@ -2219,7 +2230,7 @@
         <v>107</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="G6" s="5" t="s">
         <v>88</v>
@@ -2231,7 +2242,7 @@
         <v>0</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -2239,16 +2250,16 @@
         <v>90</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="E7" s="3">
         <v>0</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="G7" s="5" t="s">
         <v>84</v>
@@ -2265,10 +2276,10 @@
         <v>90</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>22</v>
@@ -2289,7 +2300,7 @@
         <v>0</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -2297,10 +2308,10 @@
         <v>90</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>22</v>
@@ -2309,10 +2320,10 @@
         <v>149</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="H9" s="3">
         <v>7</v>
@@ -2321,7 +2332,7 @@
         <v>0</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2329,10 +2340,10 @@
         <v>90</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>22</v>
@@ -2353,7 +2364,7 @@
         <v>0</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -2361,19 +2372,19 @@
         <v>90</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="E11" s="3">
         <v>0</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="H11" s="3">
         <v>9</v>
@@ -2387,10 +2398,10 @@
         <v>90</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>22</v>
@@ -2411,7 +2422,7 @@
         <v>0</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -2419,10 +2430,10 @@
         <v>90</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>22</v>
@@ -2443,7 +2454,7 @@
         <v>0</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -2451,16 +2462,16 @@
         <v>90</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E14" s="3">
         <v>0</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="G14" s="5" t="s">
         <v>84</v>
@@ -2477,10 +2488,10 @@
         <v>90</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>22</v>
@@ -2501,7 +2512,7 @@
         <v>2</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2533,7 +2544,7 @@
         <v>2</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
@@ -2541,16 +2552,16 @@
         <v>90</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="E17" s="3">
         <v>0</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="G17" s="5" t="s">
         <v>84</v>
@@ -2567,10 +2578,10 @@
         <v>90</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>22</v>
@@ -2591,18 +2602,18 @@
         <v>2</v>
       </c>
       <c r="J18" s="4" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>90</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>93</v>
+        <v>306</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>94</v>
+        <v>307</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>22</v>
@@ -2611,10 +2622,10 @@
         <v>130</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>39</v>
+        <v>308</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>40</v>
+        <v>309</v>
       </c>
       <c r="H19" s="3">
         <v>5</v>
@@ -2623,7 +2634,7 @@
         <v>2</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>95</v>
+        <v>310</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
@@ -2631,10 +2642,10 @@
         <v>90</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>22</v>
@@ -2655,7 +2666,7 @@
         <v>2</v>
       </c>
       <c r="J20" s="4" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2663,10 +2674,10 @@
         <v>90</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>22</v>
@@ -2687,7 +2698,7 @@
         <v>2</v>
       </c>
       <c r="J21" s="4" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
@@ -2695,16 +2706,16 @@
         <v>90</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="E22" s="3">
         <v>0</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="G22" s="5" t="s">
         <v>84</v>
@@ -2721,10 +2732,10 @@
         <v>90</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>22</v>
@@ -2745,7 +2756,7 @@
         <v>2</v>
       </c>
       <c r="J23" s="4" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="135" x14ac:dyDescent="0.25">
@@ -2753,10 +2764,10 @@
         <v>90</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>22</v>
@@ -2765,10 +2776,10 @@
         <v>131</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="H24" s="3">
         <v>10</v>
@@ -2777,7 +2788,7 @@
         <v>2</v>
       </c>
       <c r="J24" s="4" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="409.5" x14ac:dyDescent="0.25">
@@ -2809,7 +2820,7 @@
         <v>0</v>
       </c>
       <c r="J25" s="4" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="105" x14ac:dyDescent="0.25">
@@ -2817,10 +2828,10 @@
         <v>36</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>22</v>
@@ -2841,7 +2852,7 @@
         <v>0</v>
       </c>
       <c r="J26" s="4" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="120" x14ac:dyDescent="0.25">
@@ -2849,10 +2860,10 @@
         <v>36</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>22</v>
@@ -2861,10 +2872,10 @@
         <v>146</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="H27" s="3">
         <v>2</v>
@@ -2873,7 +2884,7 @@
         <v>0</v>
       </c>
       <c r="J27" s="4" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
@@ -2881,16 +2892,16 @@
         <v>36</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="E28" s="3">
         <v>0</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="G28" s="5" t="s">
         <v>84</v>
@@ -2931,7 +2942,7 @@
         <v>0</v>
       </c>
       <c r="J29" s="4" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="180" x14ac:dyDescent="0.25">
@@ -2939,10 +2950,10 @@
         <v>36</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="D30" s="3" t="s">
         <v>22</v>
@@ -2951,10 +2962,10 @@
         <v>132</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="G30" s="5" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="H30" s="3">
         <v>5</v>
@@ -2963,7 +2974,7 @@
         <v>0</v>
       </c>
       <c r="J30" s="4" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
@@ -2971,16 +2982,16 @@
         <v>36</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="E31" s="3">
         <v>0</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="G31" s="3">
         <v>0</v>
@@ -3029,10 +3040,10 @@
         <v>36</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="D33" s="3" t="s">
         <v>22</v>
@@ -3041,10 +3052,10 @@
         <v>101</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="G33" s="5" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="H33" s="3">
         <v>9</v>
@@ -3053,7 +3064,7 @@
         <v>0</v>
       </c>
       <c r="J33" s="4" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
     </row>
     <row r="34" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3085,7 +3096,7 @@
         <v>2</v>
       </c>
       <c r="J34" s="4" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
@@ -3117,7 +3128,7 @@
         <v>2</v>
       </c>
       <c r="J35" s="4" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
@@ -3125,16 +3136,16 @@
         <v>36</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="E36" s="3">
         <v>0</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="G36" s="3">
         <v>0</v>
@@ -3175,7 +3186,7 @@
         <v>2</v>
       </c>
       <c r="J37" s="4" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="38" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3207,7 +3218,7 @@
         <v>2</v>
       </c>
       <c r="J38" s="4" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="39" spans="1:10" ht="150" x14ac:dyDescent="0.25">
@@ -3215,10 +3226,10 @@
         <v>36</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D39" s="3" t="s">
         <v>22</v>
@@ -3227,10 +3238,10 @@
         <v>117</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="G39" s="5" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="H39" s="3">
         <v>6</v>
@@ -3239,7 +3250,7 @@
         <v>2</v>
       </c>
       <c r="J39" s="4" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
@@ -3247,16 +3258,16 @@
         <v>36</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="E40" s="3">
         <v>0</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="G40" s="3">
         <v>0</v>
@@ -3288,7 +3299,7 @@
         <v>42</v>
       </c>
       <c r="G41" s="5" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="H41" s="3">
         <v>8</v>
@@ -3297,7 +3308,7 @@
         <v>2</v>
       </c>
       <c r="J41" s="4" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
     </row>
     <row r="42" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -3329,7 +3340,7 @@
         <v>2</v>
       </c>
       <c r="J42" s="4" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="43" spans="1:10" ht="330" x14ac:dyDescent="0.25">
@@ -3337,10 +3348,10 @@
         <v>36</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="D43" s="3" t="s">
         <v>22</v>
@@ -3349,10 +3360,10 @@
         <v>133</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="G43" s="5" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H43" s="3">
         <v>10</v>
@@ -3361,7 +3372,7 @@
         <v>2</v>
       </c>
       <c r="J43" s="4" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -3393,7 +3404,7 @@
         <v>2</v>
       </c>
       <c r="J44" s="4" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
     </row>
     <row r="45" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -3413,7 +3424,7 @@
         <v>1</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="G45" s="5" t="s">
         <v>19</v>
@@ -3425,7 +3436,7 @@
         <v>0</v>
       </c>
       <c r="J45" s="4" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
@@ -3457,7 +3468,7 @@
         <v>0</v>
       </c>
       <c r="J46" s="4" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
@@ -3489,7 +3500,7 @@
         <v>0</v>
       </c>
       <c r="J47" s="4" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="48" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -3512,7 +3523,7 @@
         <v>28</v>
       </c>
       <c r="G48" s="6" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="H48" s="3">
         <v>4</v>
@@ -3521,7 +3532,7 @@
         <v>0</v>
       </c>
       <c r="J48" s="4" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
@@ -3553,7 +3564,7 @@
         <v>2</v>
       </c>
       <c r="J49" s="4" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
     </row>
     <row r="50" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3585,30 +3596,30 @@
         <v>2</v>
       </c>
       <c r="J50" s="4" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
     </row>
     <row r="51" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="E51" s="3">
         <v>201</v>
       </c>
       <c r="F51" s="3" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="G51" s="3" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="H51" s="3">
         <v>0</v>
@@ -3617,21 +3628,21 @@
         <v>0</v>
       </c>
       <c r="J51" s="4" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="E52" s="3">
         <v>203</v>
@@ -3649,21 +3660,21 @@
         <v>0</v>
       </c>
       <c r="J52" s="4" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="E53" s="3">
         <v>202</v>
@@ -3681,24 +3692,24 @@
         <v>0</v>
       </c>
       <c r="J53" s="4" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="E54" s="3">
         <v>0</v>
       </c>
       <c r="F54" s="3" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="G54" s="3">
         <v>0</v>
@@ -3712,16 +3723,16 @@
     </row>
     <row r="55" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E55" s="3">
         <v>210</v>
@@ -3730,7 +3741,7 @@
         <v>87</v>
       </c>
       <c r="G55" s="3" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="H55" s="3">
         <v>6</v>
@@ -3739,21 +3750,21 @@
         <v>0</v>
       </c>
       <c r="J55" s="4" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E56" s="3">
         <v>211</v>
@@ -3762,7 +3773,7 @@
         <v>87</v>
       </c>
       <c r="G56" s="3" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="H56" s="3">
         <v>7</v>
@@ -3771,21 +3782,21 @@
         <v>0</v>
       </c>
       <c r="J56" s="4" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B57" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="C57" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="C57" s="3" t="s">
-        <v>152</v>
-      </c>
       <c r="D57" s="3" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E57" s="3">
         <v>212</v>
@@ -3794,7 +3805,7 @@
         <v>87</v>
       </c>
       <c r="G57" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="H57" s="3">
         <v>8</v>
@@ -3803,24 +3814,24 @@
         <v>0</v>
       </c>
       <c r="J57" s="4" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B58" s="3" t="s">
+        <v>269</v>
+      </c>
+      <c r="C58" s="3" t="s">
         <v>272</v>
       </c>
-      <c r="C58" s="3" t="s">
-        <v>275</v>
-      </c>
       <c r="E58" s="3">
         <v>0</v>
       </c>
       <c r="F58" s="3" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="G58" s="3">
         <v>0</v>
@@ -3834,16 +3845,16 @@
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E59" s="3">
         <v>213</v>
@@ -3852,7 +3863,7 @@
         <v>87</v>
       </c>
       <c r="G59" s="3" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="H59" s="3">
         <v>2</v>
@@ -3861,21 +3872,21 @@
         <v>2</v>
       </c>
       <c r="J59" s="4" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
     </row>
     <row r="60" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="E60" s="3">
         <v>220</v>
@@ -3893,21 +3904,21 @@
         <v>2</v>
       </c>
       <c r="J60" s="4" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="61" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="B61" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="B61" s="3" t="s">
-        <v>126</v>
-      </c>
       <c r="C61" s="3" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="E61" s="3">
         <v>221</v>
@@ -3925,21 +3936,21 @@
         <v>2</v>
       </c>
       <c r="J61" s="4" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
     </row>
     <row r="62" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="E62" s="3">
         <v>222</v>
@@ -3957,21 +3968,21 @@
         <v>2</v>
       </c>
       <c r="J62" s="4" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
     </row>
     <row r="63" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="E63" s="3">
         <v>223</v>
@@ -3989,21 +4000,21 @@
         <v>2</v>
       </c>
       <c r="J63" s="4" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="64" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="E64" s="3">
         <v>224</v>
@@ -4021,21 +4032,21 @@
         <v>2</v>
       </c>
       <c r="J64" s="4" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
     <row r="65" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="E65" s="3">
         <v>225</v>
@@ -4053,21 +4064,21 @@
         <v>2</v>
       </c>
       <c r="J65" s="4" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="66" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="E66" s="3">
         <v>226</v>
@@ -4085,21 +4096,21 @@
         <v>2</v>
       </c>
       <c r="J66" s="4" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="67" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="E67" s="3">
         <v>227</v>
@@ -4117,7 +4128,7 @@
         <v>2</v>
       </c>
       <c r="J67" s="4" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.25">
@@ -4125,7 +4136,7 @@
         <v>9</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D68" s="3" t="s">
         <v>22</v>
@@ -4143,7 +4154,7 @@
         <v>0</v>
       </c>
       <c r="J68" s="4" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.25">
@@ -4189,7 +4200,7 @@
         <v>0</v>
       </c>
       <c r="J70" s="4" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.25">
@@ -4216,7 +4227,7 @@
         <v>0</v>
       </c>
       <c r="J71" s="4" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="72" spans="1:10" ht="165" x14ac:dyDescent="0.25">
@@ -4227,7 +4238,7 @@
         <v>81</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="D72" s="3" t="s">
         <v>22</v>
@@ -4236,10 +4247,10 @@
         <v>120</v>
       </c>
       <c r="F72" s="3" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="G72" s="5" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="H72" s="3">
         <v>0</v>
@@ -4248,7 +4259,7 @@
         <v>0</v>
       </c>
       <c r="J72" s="8" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="73" spans="1:10" ht="165" x14ac:dyDescent="0.25">
@@ -4280,7 +4291,7 @@
         <v>0</v>
       </c>
       <c r="J73" s="4" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="74" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -4300,7 +4311,7 @@
         <v>144</v>
       </c>
       <c r="F74" s="3" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="G74" s="5" t="s">
         <v>88</v>
@@ -4312,7 +4323,7 @@
         <v>0</v>
       </c>
       <c r="J74" s="4" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.25">
@@ -4320,16 +4331,16 @@
         <v>66</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="E75" s="3">
         <v>0</v>
       </c>
       <c r="F75" s="3" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="G75" s="3">
         <v>0</v>
@@ -4381,7 +4392,7 @@
         <v>76</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="D77" s="3" t="s">
         <v>22</v>
@@ -4402,7 +4413,7 @@
         <v>0</v>
       </c>
       <c r="J77" s="4" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
     </row>
     <row r="78" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -4434,7 +4445,7 @@
         <v>0</v>
       </c>
       <c r="J78" s="4" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
     </row>
     <row r="79" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -4466,7 +4477,7 @@
         <v>0</v>
       </c>
       <c r="J79" s="4" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.25">
@@ -4498,7 +4509,7 @@
         <v>0</v>
       </c>
       <c r="J80" s="4" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
     </row>
     <row r="81" spans="1:10" ht="390" x14ac:dyDescent="0.25">
@@ -4506,10 +4517,10 @@
         <v>66</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="D81" s="3" t="s">
         <v>22</v>
@@ -4518,10 +4529,10 @@
         <v>139</v>
       </c>
       <c r="F81" s="3" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="G81" s="5" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="H81" s="3">
         <v>9</v>
@@ -4530,7 +4541,7 @@
         <v>0</v>
       </c>
       <c r="J81" s="4" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
     </row>
     <row r="82" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -4538,10 +4549,10 @@
         <v>66</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="D82" s="3" t="s">
         <v>22</v>
@@ -4562,7 +4573,7 @@
         <v>0</v>
       </c>
       <c r="J82" s="4" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.25">
@@ -4570,16 +4581,16 @@
         <v>66</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="E83" s="3">
         <v>0</v>
       </c>
       <c r="F83" s="3" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="G83" s="3">
         <v>0</v>
@@ -4596,10 +4607,10 @@
         <v>66</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="D84" s="3" t="s">
         <v>22</v>
@@ -4608,10 +4619,10 @@
         <v>112</v>
       </c>
       <c r="F84" s="3" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G84" s="5" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="H84" s="3">
         <v>4</v>
@@ -4620,7 +4631,7 @@
         <v>2</v>
       </c>
       <c r="J84" s="4" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
     </row>
     <row r="85" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -4628,10 +4639,10 @@
         <v>66</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="D85" s="3" t="s">
         <v>22</v>
@@ -4652,7 +4663,7 @@
         <v>2</v>
       </c>
       <c r="J85" s="4" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="86" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -4660,10 +4671,10 @@
         <v>66</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="C86" s="3" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="D86" s="3" t="s">
         <v>22</v>
@@ -4672,10 +4683,10 @@
         <v>111</v>
       </c>
       <c r="F86" s="3" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G86" s="3" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="H86" s="3">
         <v>6</v>
@@ -4684,7 +4695,7 @@
         <v>2</v>
       </c>
       <c r="J86" s="4" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated CaptCrossPickOwn to the new capt_side. Test coverage for CaptSideOk. Updated capture test data to use new side enum (in spreadsheet), added tests. MoveAllFirst updated to work with both mlength 1 and 3 moves; wrote test code for it. New game Halusa (capt on own side).
</commit_message>
<xml_diff>
--- a/src/game_params.xlsx
+++ b/src/game_params.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Activity_Data\Mancala_github\MancalaGames\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7100E004-7DCC-467A-90AA-F23DC28E5E43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53AE01C4-811E-46A8-B6C3-56BA8A10B8A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-25155" yWindow="780" windowWidth="22185" windowHeight="14895" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2039,7 +2039,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A19" sqref="A19"/>
+      <selection pane="bottomLeft" activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
First cut of sow_rule LAP_CAPT implemented for cross captures. No test code. Added game Tegre.
</commit_message>
<xml_diff>
--- a/src/game_params.xlsx
+++ b/src/game_params.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Activity_Data\Mancala_github\MancalaGames\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53AE01C4-811E-46A8-B6C3-56BA8A10B8A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34E0DEF2-E6FB-4C59-B8A6-A3B163916CA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25155" yWindow="780" windowWidth="22185" windowHeight="14895" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="game_params" sheetId="1" r:id="rId1"/>
@@ -955,24 +955,6 @@
     <t>Sow Parameter</t>
   </si>
   <si>
-    <t>Special sow rules add additional behavior or restrictions to the sowing phase:
-- NONE: there is no special sowing rule.
-- SOW_BLKD_DIV: If the final seed of an individual sow lands on the opposite side of the board and brings the contents of that hole to goal_param seeds, the hole is closed closed (blocked). In single lap games, the hole's seeds are removed from play. In multilap games, the seeds are used to continue sowing.
-  + When sowing, blocked holes on your own side of the board are skipped  and blocked holes on opponent's side are diverted out of play or captured.
-  +  Game GOAL must be DEPRIVE and all of the associated restrictions apply. NOCAPTMOVES maybe used to prevent closing holes on the initial games moves. Capture mechanisms other than closing holes are not supported. The minimum move must be 1 and thus SOW_START is incompatible.  ALLOW_RULE may not be used to limit allowable moves.  SKIP_START and VISIT_OPP are not supported with SOW_BLKD_DIV.  MLAPS of LAPPER_NEXT is not supported with SOW_BLKD_DIV(_NR).
-- SOW_BLKD_DIV_NR: Behaves the same as SOW_BLKD_DIV except that each player's rightmost hole cannot be closed. 
-- OWN_SOW_CAPT_ALL: The hole OWNer captures all holes that are sown to meet the simple capture criteria no matter who sowed them.  The simple capture criteria are: evens, min, max and capture on. Other criteria are enforced: side of the board, unlocked, and not child.
-  + The capture is done by the hole owner, so the non-sower may capture seeds while their opponents sows. If the game GOAL is TERRITORY the capturer is the hole owner; otherwise each player captures from their own side of the board no matter who is sowing. 
-  + If MLAPS is LAPPER and the final seed sown for any lap meets the simple capture criteria for that hole, the contents of the hole are captured by the sower and not the hole owner and the turn is over. For CAPTTWOOUT, CAPT_NEXT and CROSSCAPT captures, the sower always does the final capture.
-  + GRANDSLAM rules are not applied. NOCAPTMOVES prevents these capture for the first moves.
-- SOW_SOW_CAPT_ALL: Similar to OWN_SOW_CAPT_ALL but only the SOWer captures seeds from their opponent's holes. 
-  + If mlaps is LAPPER and the final seed sown for any lap meets the capture criteria, the contents of the hole are captured by the sower and not the hole owner and the turn is over.
-  + GRANDSLAM rules are not applied. NOCAPTMOVES prevents this capture for the first number of specified moves.
-- NO_SOW_OPP_2S: Don't sow into opponents holes with 2 seeds.
-- CHANGE_DIR_LAP: Change the direction for each lap sown. Generally used with UDIR_HOLES so the player may choose the first direction.
-- MAX_SOW: holes sow_param seeds are skipped when sowing. That is, holes will never contain more seeds than sow_param.</t>
-  </si>
-  <si>
     <t>A general parameter for sowing. Usage is based on other sow options:
 - Sow rule of MAX_SOW: maximum number of seeds a hole may contain</t>
   </si>
@@ -1154,6 +1136,25 @@
 - OWN_SIDE: captures on own side of board only.
 - OPP_CONT: a multi-capture must begin on the opposite side of the board, but may continue onto your own side.  Requires MULTICAPT.
 - OWN_CONT: a multi-capture must being on your own side of the board and may continue onto your opponent's side. Requires multicapt.</t>
+  </si>
+  <si>
+    <t>Special sow rules add additional behavior or restrictions to the sowing phase:
+- NONE: there is no special sowing rule.
+- SOW_BLKD_DIV: If the final seed of an individual sow lands on the opposite side of the board and brings the contents of that hole to goal_param seeds, the hole is closed closed (blocked). In single lap games, the hole's seeds are removed from play. In multilap games, the seeds are used to continue sowing.
+  + When sowing, blocked holes on your own side of the board are skipped  and blocked holes on opponent's side are diverted out of play or captured.
+  +  Game GOAL must be DEPRIVE and all of the associated restrictions apply. NOCAPTMOVES maybe used to prevent closing holes on the initial games moves. Capture mechanisms other than closing holes are not supported. The minimum move must be 1 and thus SOW_START is incompatible.  ALLOW_RULE may not be used to limit allowable moves.  SKIP_START and VISIT_OPP are not supported with SOW_BLKD_DIV.  MLAPS of LAPPER_NEXT is not supported with SOW_BLKD_DIV(_NR).
+- SOW_BLKD_DIV_NR: Behaves the same as SOW_BLKD_DIV except that each player's rightmost hole cannot be closed. 
+- OWN_SOW_CAPT_ALL: The hole OWNer captures all holes that are sown to meet the simple capture criteria no matter who sowed them.  The simple capture criteria are: evens, min, max and capture on. Other criteria are enforced: side of the board, unlocked, and not child.
+  + The capture is done by the hole owner, so the non-sower may capture seeds while their opponents sows. If the game GOAL is TERRITORY the capturer is the hole owner; otherwise each player captures from their own side of the board no matter who is sowing. 
+  + If MLAPS is LAPPER and the final seed sown for any lap meets the simple capture criteria for that hole, the contents of the hole are captured by the sower and not the hole owner and the turn is over. For CAPTTWOOUT, CAPT_NEXT and CROSSCAPT captures, the sower always does the final capture.
+  + GRANDSLAM rules are not applied. NOCAPTMOVES prevents these capture for the first moves.
+- SOW_SOW_CAPT_ALL: Similar to OWN_SOW_CAPT_ALL but only the SOWer captures seeds from their opponent's holes. 
+  + If mlaps is LAPPER and the final seed sown for any lap meets the capture criteria, the contents of the hole are captured by the sower and not the hole owner and the turn is over.
+  + GRANDSLAM rules are not applied. NOCAPTMOVES prevents this capture for the first number of specified moves.
+- NO_SOW_OPP_2S: Don't sow into opponents holes with 2 seeds.
+- CHANGE_DIR_LAP: Change the direction for each lap sown. Generally used with UDIR_HOLES so the player may choose the first direction.
+- MAX_SOW: holes sow_param seeds are skipped when sowing. That is, holes will never contain more seeds than sow_param.
+- LAP_CAPT: after each lapt check for a capture, if there is a capture continue sowing with another lap.</t>
   </si>
 </sst>
 </file>
@@ -2038,8 +2039,8 @@
   <dimension ref="A1:J86"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C19" sqref="C19"/>
+      <pane ySplit="1" topLeftCell="A78" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J82" sqref="J82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2094,17 +2095,17 @@
         <v>90</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>273</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>274</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3">
         <v>0</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="G2" s="5" t="s">
         <v>84</v>
@@ -2250,16 +2251,16 @@
         <v>90</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>278</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>279</v>
-      </c>
       <c r="E7" s="3">
         <v>0</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="G7" s="5" t="s">
         <v>84</v>
@@ -2372,19 +2373,19 @@
         <v>90</v>
       </c>
       <c r="B11" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>275</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="E11" s="3">
+        <v>0</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="G11" s="5" t="s">
         <v>276</v>
-      </c>
-      <c r="E11" s="3">
-        <v>0</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>266</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>277</v>
       </c>
       <c r="H11" s="3">
         <v>9</v>
@@ -2422,7 +2423,7 @@
         <v>0</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -2462,7 +2463,7 @@
         <v>90</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>111</v>
@@ -2471,7 +2472,7 @@
         <v>0</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="G14" s="5" t="s">
         <v>84</v>
@@ -2512,7 +2513,7 @@
         <v>2</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2552,16 +2553,16 @@
         <v>90</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="E17" s="3">
         <v>0</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="G17" s="5" t="s">
         <v>84</v>
@@ -2581,7 +2582,7 @@
         <v>259</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>22</v>
@@ -2610,10 +2611,10 @@
         <v>90</v>
       </c>
       <c r="B19" s="3" t="s">
+        <v>305</v>
+      </c>
+      <c r="C19" s="3" t="s">
         <v>306</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>307</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>22</v>
@@ -2622,10 +2623,10 @@
         <v>130</v>
       </c>
       <c r="F19" s="3" t="s">
+        <v>307</v>
+      </c>
+      <c r="G19" s="5" t="s">
         <v>308</v>
-      </c>
-      <c r="G19" s="5" t="s">
-        <v>309</v>
       </c>
       <c r="H19" s="3">
         <v>5</v>
@@ -2634,7 +2635,7 @@
         <v>2</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
@@ -2706,16 +2707,16 @@
         <v>90</v>
       </c>
       <c r="B22" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="C22" s="3" t="s">
         <v>282</v>
       </c>
-      <c r="C22" s="3" t="s">
-        <v>283</v>
-      </c>
       <c r="E22" s="3">
         <v>0</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="G22" s="5" t="s">
         <v>84</v>
@@ -2860,10 +2861,10 @@
         <v>36</v>
       </c>
       <c r="B27" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="C27" s="3" t="s">
         <v>301</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>302</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>22</v>
@@ -2872,10 +2873,10 @@
         <v>146</v>
       </c>
       <c r="F27" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="G27" s="5" t="s">
         <v>303</v>
-      </c>
-      <c r="G27" s="5" t="s">
-        <v>304</v>
       </c>
       <c r="H27" s="3">
         <v>2</v>
@@ -2884,7 +2885,7 @@
         <v>0</v>
       </c>
       <c r="J27" s="4" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
@@ -2892,16 +2893,16 @@
         <v>36</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E28" s="3">
         <v>0</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="G28" s="5" t="s">
         <v>84</v>
@@ -2982,16 +2983,16 @@
         <v>36</v>
       </c>
       <c r="B31" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="C31" s="3" t="s">
         <v>294</v>
       </c>
-      <c r="C31" s="3" t="s">
-        <v>295</v>
-      </c>
       <c r="E31" s="3">
         <v>0</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="G31" s="3">
         <v>0</v>
@@ -3064,7 +3065,7 @@
         <v>0</v>
       </c>
       <c r="J33" s="4" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="34" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3136,16 +3137,16 @@
         <v>36</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E36" s="3">
         <v>0</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="G36" s="3">
         <v>0</v>
@@ -3258,16 +3259,16 @@
         <v>36</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="E40" s="3">
         <v>0</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="G40" s="3">
         <v>0</v>
@@ -3700,16 +3701,16 @@
         <v>120</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E54" s="3">
         <v>0</v>
       </c>
       <c r="F54" s="3" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="G54" s="3">
         <v>0</v>
@@ -3822,16 +3823,16 @@
         <v>120</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="E58" s="3">
         <v>0</v>
       </c>
       <c r="F58" s="3" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="G58" s="3">
         <v>0</v>
@@ -4238,7 +4239,7 @@
         <v>81</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D72" s="3" t="s">
         <v>22</v>
@@ -4331,16 +4332,16 @@
         <v>66</v>
       </c>
       <c r="B75" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="C75" s="3" t="s">
         <v>289</v>
       </c>
-      <c r="C75" s="3" t="s">
-        <v>290</v>
-      </c>
       <c r="E75" s="3">
         <v>0</v>
       </c>
       <c r="F75" s="3" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="G75" s="3">
         <v>0</v>
@@ -4392,7 +4393,7 @@
         <v>76</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D77" s="3" t="s">
         <v>22</v>
@@ -4512,7 +4513,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="81" spans="1:10" ht="390" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10" ht="405" x14ac:dyDescent="0.25">
       <c r="A81" s="3" t="s">
         <v>66</v>
       </c>
@@ -4541,7 +4542,7 @@
         <v>0</v>
       </c>
       <c r="J81" s="4" t="s">
-        <v>263</v>
+        <v>310</v>
       </c>
     </row>
     <row r="82" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -4573,7 +4574,7 @@
         <v>0</v>
       </c>
       <c r="J82" s="4" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.25">
@@ -4581,16 +4582,16 @@
         <v>66</v>
       </c>
       <c r="B83" s="3" t="s">
+        <v>286</v>
+      </c>
+      <c r="C83" s="3" t="s">
         <v>287</v>
       </c>
-      <c r="C83" s="3" t="s">
-        <v>288</v>
-      </c>
       <c r="E83" s="3">
         <v>0</v>
       </c>
       <c r="F83" s="3" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="G83" s="3">
         <v>0</v>
@@ -4631,7 +4632,7 @@
         <v>2</v>
       </c>
       <c r="J84" s="4" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="85" spans="1:10" ht="30" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added ContIfBasicCapt. Wrote tests for ContIfBasicCapt and ContIfXCapt. Moved the StopOnChild addition to the deco chain so that it is never added to NextLapCont--LAPPER_NEXT does not support children. Changed the size of the Mancala window (bigger). Updated helps. Added the game Motiq.
</commit_message>
<xml_diff>
--- a/src/game_params.xlsx
+++ b/src/game_params.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Activity_Data\Mancala_github\MancalaGames\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34E0DEF2-E6FB-4C59-B8A6-A3B163916CA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85832EC5-5730-4AA6-9F7A-CF215540E2DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1154,7 +1154,7 @@
 - NO_SOW_OPP_2S: Don't sow into opponents holes with 2 seeds.
 - CHANGE_DIR_LAP: Change the direction for each lap sown. Generally used with UDIR_HOLES so the player may choose the first direction.
 - MAX_SOW: holes sow_param seeds are skipped when sowing. That is, holes will never contain more seeds than sow_param.
-- LAP_CAPT: after each lapt check for a capture, if there is a capture continue sowing with another lap.</t>
+- LAP_CAPT: after each lapt check for a capture, if there is a capture continue sowing with another lap. If a basic capture is configured (evens, capt on, max or min), the hole after the captured seeds is drawn to continue lapping.</t>
   </si>
 </sst>
 </file>
@@ -2039,8 +2039,8 @@
   <dimension ref="A1:J86"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A78" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J82" sqref="J82"/>
+      <pane ySplit="1" topLeftCell="A79" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J81" sqref="J81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4513,7 +4513,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="81" spans="1:10" ht="405" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A81" s="3" t="s">
         <v>66</v>
       </c>

</xml_diff>

<commit_message>
Add pre-sow captures: SCaptOne, SCaptCrossOnOne and SCaptCrossSingles; and parameter to select (presowcapt) Added NotXfromOnes allowable. Fixed some problems with play_mancala (wasn't using man_path correctly). Added new games: Achochodi, Gelech, Kale, Lahemay_Waladat, Rio_Kadalis and Sukosowo.
</commit_message>
<xml_diff>
--- a/src/game_params.xlsx
+++ b/src/game_params.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Activity_Data\Mancala_github\MancalaGames\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85832EC5-5730-4AA6-9F7A-CF215540E2DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2482765-6594-4500-8CB7-AC35DA508C00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-27855" yWindow="915" windowWidth="22185" windowHeight="14895" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="game_params" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">game_params!$A$1:$J$86</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">game_params!$A$1:$J$87</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="560" uniqueCount="311">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="315">
   <si>
     <t>tab</t>
   </si>
@@ -1155,6 +1155,22 @@
 - CHANGE_DIR_LAP: Change the direction for each lap sown. Generally used with UDIR_HOLES so the player may choose the first direction.
 - MAX_SOW: holes sow_param seeds are skipped when sowing. That is, holes will never contain more seeds than sow_param.
 - LAP_CAPT: after each lapt check for a capture, if there is a capture continue sowing with another lap. If a basic capture is configured (evens, capt on, max or min), the hole after the captured seeds is drawn to continue lapping.</t>
+  </si>
+  <si>
+    <t>presowcapt</t>
+  </si>
+  <si>
+    <t>Pre Sow Capture</t>
+  </si>
+  <si>
+    <t>PreSowCapt</t>
+  </si>
+  <si>
+    <t>Capture type that occurs before sowing:
+- NONE: No capture before sowing.
+- CAPT_ONE: Capture 1 seed from the draw. If MLAPS, capture 1 seeds per lap.
+- ALL_SINGLE_XCAPT: Capture the seeds across from all singles.
+- DRAW_1_XCAPT: When draw 1 seed, capture any seeds on the other side of the board.</t>
   </si>
 </sst>
 </file>
@@ -2036,10 +2052,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:J86"/>
+  <dimension ref="A1:J87"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A79" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A78" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="J81" sqref="J81"/>
     </sheetView>
   </sheetViews>
@@ -2318,7 +2334,7 @@
         <v>22</v>
       </c>
       <c r="E9" s="3">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>108</v>
@@ -2350,7 +2366,7 @@
         <v>22</v>
       </c>
       <c r="E10" s="3">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>39</v>
@@ -2870,7 +2886,7 @@
         <v>22</v>
       </c>
       <c r="E27" s="3">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="F27" s="3" t="s">
         <v>302</v>
@@ -2928,7 +2944,7 @@
         <v>22</v>
       </c>
       <c r="E29" s="3">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="F29" s="3" t="s">
         <v>58</v>
@@ -3082,7 +3098,7 @@
         <v>22</v>
       </c>
       <c r="E34" s="3">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="F34" s="3" t="s">
         <v>39</v>
@@ -3294,7 +3310,7 @@
         <v>22</v>
       </c>
       <c r="E41" s="3">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="F41" s="3" t="s">
         <v>42</v>
@@ -3326,7 +3342,7 @@
         <v>22</v>
       </c>
       <c r="E42" s="3">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="F42" s="3" t="s">
         <v>45</v>
@@ -3358,7 +3374,7 @@
         <v>22</v>
       </c>
       <c r="E43" s="3">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="F43" s="3" t="s">
         <v>184</v>
@@ -4163,14 +4179,18 @@
         <v>9</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>10</v>
+        <v>89</v>
+      </c>
+      <c r="D69" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="E69" s="3">
-        <v>501</v>
+        <v>146</v>
       </c>
       <c r="F69" s="3" t="s">
-        <v>11</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="G69" s="5"/>
       <c r="H69" s="3">
         <v>0</v>
       </c>
@@ -4178,7 +4198,7 @@
         <v>0</v>
       </c>
       <c r="J69" s="4" t="s">
-        <v>12</v>
+        <v>165</v>
       </c>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.25">
@@ -4209,18 +4229,14 @@
         <v>9</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="D71" s="3" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="E71" s="3">
-        <v>145</v>
+        <v>501</v>
       </c>
       <c r="F71" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="G71" s="5"/>
+        <v>11</v>
+      </c>
       <c r="H71" s="3">
         <v>0</v>
       </c>
@@ -4228,7 +4244,7 @@
         <v>0</v>
       </c>
       <c r="J71" s="4" t="s">
-        <v>165</v>
+        <v>12</v>
       </c>
     </row>
     <row r="72" spans="1:10" ht="165" x14ac:dyDescent="0.25">
@@ -4277,7 +4293,7 @@
         <v>22</v>
       </c>
       <c r="E73" s="3">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="F73" s="3" t="s">
         <v>69</v>
@@ -4309,7 +4325,7 @@
         <v>22</v>
       </c>
       <c r="E74" s="3">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="F74" s="3" t="s">
         <v>140</v>
@@ -4367,7 +4383,7 @@
         <v>22</v>
       </c>
       <c r="E76" s="3">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="F76" s="3" t="s">
         <v>39</v>
@@ -4399,7 +4415,7 @@
         <v>22</v>
       </c>
       <c r="E77" s="3">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="F77" s="3" t="s">
         <v>39</v>
@@ -4431,7 +4447,7 @@
         <v>22</v>
       </c>
       <c r="E78" s="3">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="F78" s="3" t="s">
         <v>39</v>
@@ -4495,7 +4511,7 @@
         <v>22</v>
       </c>
       <c r="E80" s="3">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="F80" s="3" t="s">
         <v>39</v>
@@ -4513,24 +4529,24 @@
         <v>219</v>
       </c>
     </row>
-    <row r="81" spans="1:10" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A81" s="3" t="s">
         <v>66</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>174</v>
+        <v>311</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>175</v>
+        <v>312</v>
       </c>
       <c r="D81" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E81" s="3">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="F81" s="3" t="s">
-        <v>176</v>
+        <v>313</v>
       </c>
       <c r="G81" s="5" t="s">
         <v>161</v>
@@ -4542,30 +4558,30 @@
         <v>0</v>
       </c>
       <c r="J81" s="4" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="82" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A82" s="3" t="s">
         <v>66</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>261</v>
+        <v>174</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>262</v>
+        <v>175</v>
       </c>
       <c r="D82" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E82" s="3">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F82" s="3" t="s">
-        <v>11</v>
+        <v>176</v>
       </c>
       <c r="G82" s="5" t="s">
-        <v>84</v>
+        <v>161</v>
       </c>
       <c r="H82" s="3">
         <v>10</v>
@@ -4574,143 +4590,175 @@
         <v>0</v>
       </c>
       <c r="J82" s="4" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A83" s="3" t="s">
         <v>66</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>286</v>
+        <v>261</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>287</v>
+        <v>262</v>
+      </c>
+      <c r="D83" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="E83" s="3">
-        <v>0</v>
+        <v>142</v>
       </c>
       <c r="F83" s="3" t="s">
-        <v>265</v>
-      </c>
-      <c r="G83" s="3">
-        <v>0</v>
+        <v>11</v>
+      </c>
+      <c r="G83" s="5" t="s">
+        <v>84</v>
       </c>
       <c r="H83" s="3">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="I83" s="3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="84" spans="1:10" ht="360" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="J83" s="4" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" s="3" t="s">
         <v>66</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>153</v>
+        <v>286</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="D84" s="3" t="s">
-        <v>22</v>
+        <v>287</v>
       </c>
       <c r="E84" s="3">
-        <v>112</v>
+        <v>0</v>
       </c>
       <c r="F84" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="G84" s="5" t="s">
-        <v>155</v>
+        <v>265</v>
+      </c>
+      <c r="G84" s="3">
+        <v>0</v>
       </c>
       <c r="H84" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I84" s="3">
         <v>2</v>
       </c>
-      <c r="J84" s="4" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="85" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="85" spans="1:10" ht="360" x14ac:dyDescent="0.25">
       <c r="A85" s="3" t="s">
         <v>66</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="D85" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E85" s="3">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="F85" s="3" t="s">
-        <v>11</v>
+        <v>156</v>
       </c>
       <c r="G85" s="5" t="s">
-        <v>84</v>
+        <v>155</v>
       </c>
       <c r="H85" s="3">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I85" s="3">
         <v>2</v>
       </c>
       <c r="J85" s="4" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="86" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A86" s="3" t="s">
         <v>66</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>188</v>
+        <v>151</v>
       </c>
       <c r="C86" s="3" t="s">
-        <v>189</v>
+        <v>152</v>
       </c>
       <c r="D86" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E86" s="3">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F86" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="G86" s="3" t="s">
-        <v>161</v>
+        <v>11</v>
+      </c>
+      <c r="G86" s="5" t="s">
+        <v>84</v>
       </c>
       <c r="H86" s="3">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I86" s="3">
         <v>2</v>
       </c>
       <c r="J86" s="4" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A87" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B87" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="C87" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="D87" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E87" s="3">
+        <v>111</v>
+      </c>
+      <c r="F87" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="G87" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="H87" s="3">
+        <v>6</v>
+      </c>
+      <c r="I87" s="3">
+        <v>2</v>
+      </c>
+      <c r="J87" s="4" t="s">
         <v>229</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J86" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J86">
-      <sortCondition ref="A2:A86"/>
-      <sortCondition ref="I2:I86"/>
-      <sortCondition ref="H2:H86"/>
+  <autoFilter ref="A1:J87" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J87">
+      <sortCondition ref="A2:A87"/>
+      <sortCondition ref="I2:I87"/>
+      <sortCondition ref="H2:H87"/>
     </sortState>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:J87">
-    <sortCondition ref="A3:A87"/>
-    <sortCondition ref="I3:I87"/>
-    <sortCondition ref="H3:H87"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:J88">
+    <sortCondition ref="A3:A88"/>
+    <sortCondition ref="I3:I88"/>
+    <sortCondition ref="H3:H88"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Change SOW_SOW_CAPT_ALL to SOW_CAPT_ALL, side of capture is now controlled by CAPT_SIDE. Updated variation in games that mentioned SOW_SOW_CAPT_ALL. Added games Hoyito_I and Hoyito_II
</commit_message>
<xml_diff>
--- a/src/game_params.xlsx
+++ b/src/game_params.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Activity_Data\Mancala_github\MancalaGames\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2482765-6594-4500-8CB7-AC35DA508C00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B732EB63-3A40-47D4-9107-9746A6E8DE09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27855" yWindow="915" windowWidth="22185" windowHeight="14895" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="game_params" sheetId="1" r:id="rId1"/>
@@ -1078,6 +1078,88 @@
 When multiple lap sowing, the sowing does not stop for captures. Instead, sowing continues until the final seed is sown into an empty hole. Then the capture test is made on the next hole.</t>
   </si>
   <si>
+    <t>An int to describe possible multicaptures:
+ 0 no multiple captures.
+ -1: After the initial capture, continue capturing as long as the capture conditions are met. This multiple capture may happen in the sow direction (unsown holes) or in the opposite direction (sown holes) as determined by CAPSAMEDIR.
+ 1 .. holes: capture at most n holes that meet the capture conditions.
+See individual capture mechanism for any special requirements.</t>
+  </si>
+  <si>
+    <t>unclaimed</t>
+  </si>
+  <si>
+    <t>End Game Seeds</t>
+  </si>
+  <si>
+    <t>EndGameSeeds</t>
+  </si>
+  <si>
+    <t>HOLE_OWNER</t>
+  </si>
+  <si>
+    <t>Defines how to score any unclaimed seeds when a game has ended. This is not used if the game has a clear winner, e.g. one player has collected more than half the seeds for a MAX_SEEDS game.
+- HOLE_OWNER: unclaimed seeds go to the hole owner.
+- DONT_SCORE: unclaimed seeds do not score (they are ignored).
+- LAST_MOVER: unclaimed seeds go the player that moved last.
+- UNFED_PLAYER: only valid for MUSTSHARE games. If the game ended without one player being able share seeds, the seeds go to the player without seeds (the unfed player).
+- DIVVIED: the seeds are divided between the two players (an extra seed goes to the player with fewer seeds).</t>
+  </si>
+  <si>
+    <t>capt_side</t>
+  </si>
+  <si>
+    <t>Capture side</t>
+  </si>
+  <si>
+    <t>CaptSide</t>
+  </si>
+  <si>
+    <t>BOTH</t>
+  </si>
+  <si>
+    <t>Limits which side of the board captures maybe done on:
+- BOTH: no limitations
+- OPP_SIDE: opposite side capture only.
+- OWN_SIDE: captures on own side of board only.
+- OPP_CONT: a multi-capture must begin on the opposite side of the board, but may continue onto your own side.  Requires MULTICAPT.
+- OWN_CONT: a multi-capture must being on your own side of the board and may continue onto your opponent's side. Requires multicapt.</t>
+  </si>
+  <si>
+    <t>presowcapt</t>
+  </si>
+  <si>
+    <t>Pre Sow Capture</t>
+  </si>
+  <si>
+    <t>PreSowCapt</t>
+  </si>
+  <si>
+    <t>Capture type that occurs before sowing:
+- NONE: No capture before sowing.
+- CAPT_ONE: Capture 1 seed from the draw. If MLAPS, capture 1 seeds per lap.
+- ALL_SINGLE_XCAPT: Capture the seeds across from all singles.
+- DRAW_1_XCAPT: When draw 1 seed, capture any seeds on the other side of the board.</t>
+  </si>
+  <si>
+    <t>Special sow rules add additional behavior or restrictions to the sowing phase:
+- NONE: there is no special sowing rule.
+- SOW_BLKD_DIV: If the final seed of an individual sow lands on the opposite side of the board and brings the contents of that hole to goal_param seeds, the hole is closed closed (blocked). In single lap games, the hole's seeds are removed from play. In multilap games, the seeds are used to continue sowing.
+  + When sowing, blocked holes on your own side of the board are skipped  and blocked holes on opponent's side are diverted out of play or captured.
+  +  Game GOAL must be DEPRIVE and all of the associated restrictions apply. NOCAPTMOVES maybe used to prevent closing holes on the initial games moves. Capture mechanisms other than closing holes are not supported. The minimum move must be 1 and thus SOW_START is incompatible.  ALLOW_RULE may not be used to limit allowable moves.  SKIP_START and VISIT_OPP are not supported with SOW_BLKD_DIV.  MLAPS of LAPPER_NEXT is not supported with SOW_BLKD_DIV(_NR).
+- SOW_BLKD_DIV_NR: Behaves the same as SOW_BLKD_DIV except that each player's rightmost hole cannot be closed. 
+- OWN_SOW_CAPT_ALL: The hole OWNer captures all holes that are sown to meet the simple capture criteria no matter who sowed them.  The simple capture criteria are: evens, min, max and capture on. Other criteria are enforced: side of the board, unlocked, and not child.
+  + The capture is done by the hole owner, so the non-sower may capture seeds while their opponents sows. If the game GOAL is TERRITORY the capturer is the hole owner; otherwise each player captures from their own side of the board no matter who is sowing. 
+  + If MLAPS is LAPPER and the final seed sown for any lap meets the simple capture criteria for that hole, the contents of the hole are captured by the sower and not the hole owner and the turn is over. For CAPTTWOOUT, CAPT_NEXT and CROSSCAPT captures, the sower always does the final capture.
+  + GRANDSLAM rules are not applied. NOCAPTMOVES prevents these capture for the first moves.
+- SOW_CAPT_ALL: Similar to OWN_SOW_CAPT_ALL but only the SOWer captures seeds from the side specified by CAPT_SIDE. BOTH sower capturers from any hole. OPP sower capturer only from opponents holes.  OWN sower captures only from their own holes. 
+  + If mlaps is LAPPER and the final seed sown for any lap meets the capture criteria, the contents of the hole are captured by the sower and not the hole owner and the turn is over.
+  + GRANDSLAM rules are not applied. NOCAPTMOVES prevents this capture for the first number of specified moves.
+- NO_SOW_OPP_2S: Don't sow into opponents holes with 2 seeds.
+- CHANGE_DIR_LAP: Change the direction for each lap sown. Generally used with UDIR_HOLES so the player may choose the first direction.
+- MAX_SOW: holes sow_param seeds are skipped when sowing. That is, holes will never contain more seeds than sow_param.
+- LAP_CAPT: after each lapt check for a capture, if there is a capture continue sowing with another lap. If a basic capture is configured (evens, capt on, max or min), the hole after the captured seeds is drawn to continue lapping.</t>
+  </si>
+  <si>
     <t>Allow rules limit the holes from which moves may start.  Disallowed holes are not selectable.
 - NONE: no special rule
 - OPP_OR_EMPTY:  Limit the allowable holes to those that end in an empty hole or reach the opponents side of the board.
@@ -1088,89 +1170,8 @@
 - TWO_ONLY_ALL_RIGHT: Holes with two seeds may not be played, unless all holes contains two seeds, in which case the rightmost hole must be played.
 - FIRST_TURN_ONLY_RIGHT_TWO: The first turn must start from one of the two rightmost holes.
 - RIGHT_2_1ST_THEN_ALL_TWO:  The first turn must start from one of the two rightmost holes. Subsequent moves may only start from holes without 2 seeds, unless all holes contain zero or 2 seeds.
-- MOVE_ALL_HOLES_FIRST: a move must initiated from each hole once before a second move may be made from any hole.  MOVE_ALL is incompatible with all pickers and capttwoout.</t>
-  </si>
-  <si>
-    <t>An int to describe possible multicaptures:
- 0 no multiple captures.
- -1: After the initial capture, continue capturing as long as the capture conditions are met. This multiple capture may happen in the sow direction (unsown holes) or in the opposite direction (sown holes) as determined by CAPSAMEDIR.
- 1 .. holes: capture at most n holes that meet the capture conditions.
-See individual capture mechanism for any special requirements.</t>
-  </si>
-  <si>
-    <t>unclaimed</t>
-  </si>
-  <si>
-    <t>End Game Seeds</t>
-  </si>
-  <si>
-    <t>EndGameSeeds</t>
-  </si>
-  <si>
-    <t>HOLE_OWNER</t>
-  </si>
-  <si>
-    <t>Defines how to score any unclaimed seeds when a game has ended. This is not used if the game has a clear winner, e.g. one player has collected more than half the seeds for a MAX_SEEDS game.
-- HOLE_OWNER: unclaimed seeds go to the hole owner.
-- DONT_SCORE: unclaimed seeds do not score (they are ignored).
-- LAST_MOVER: unclaimed seeds go the player that moved last.
-- UNFED_PLAYER: only valid for MUSTSHARE games. If the game ended without one player being able share seeds, the seeds go to the player without seeds (the unfed player).
-- DIVVIED: the seeds are divided between the two players (an extra seed goes to the player with fewer seeds).</t>
-  </si>
-  <si>
-    <t>capt_side</t>
-  </si>
-  <si>
-    <t>Capture side</t>
-  </si>
-  <si>
-    <t>CaptSide</t>
-  </si>
-  <si>
-    <t>BOTH</t>
-  </si>
-  <si>
-    <t>Limits which side of the board captures maybe done on:
-- BOTH: no limitations
-- OPP_SIDE: opposite side capture only.
-- OWN_SIDE: captures on own side of board only.
-- OPP_CONT: a multi-capture must begin on the opposite side of the board, but may continue onto your own side.  Requires MULTICAPT.
-- OWN_CONT: a multi-capture must being on your own side of the board and may continue onto your opponent's side. Requires multicapt.</t>
-  </si>
-  <si>
-    <t>Special sow rules add additional behavior or restrictions to the sowing phase:
-- NONE: there is no special sowing rule.
-- SOW_BLKD_DIV: If the final seed of an individual sow lands on the opposite side of the board and brings the contents of that hole to goal_param seeds, the hole is closed closed (blocked). In single lap games, the hole's seeds are removed from play. In multilap games, the seeds are used to continue sowing.
-  + When sowing, blocked holes on your own side of the board are skipped  and blocked holes on opponent's side are diverted out of play or captured.
-  +  Game GOAL must be DEPRIVE and all of the associated restrictions apply. NOCAPTMOVES maybe used to prevent closing holes on the initial games moves. Capture mechanisms other than closing holes are not supported. The minimum move must be 1 and thus SOW_START is incompatible.  ALLOW_RULE may not be used to limit allowable moves.  SKIP_START and VISIT_OPP are not supported with SOW_BLKD_DIV.  MLAPS of LAPPER_NEXT is not supported with SOW_BLKD_DIV(_NR).
-- SOW_BLKD_DIV_NR: Behaves the same as SOW_BLKD_DIV except that each player's rightmost hole cannot be closed. 
-- OWN_SOW_CAPT_ALL: The hole OWNer captures all holes that are sown to meet the simple capture criteria no matter who sowed them.  The simple capture criteria are: evens, min, max and capture on. Other criteria are enforced: side of the board, unlocked, and not child.
-  + The capture is done by the hole owner, so the non-sower may capture seeds while their opponents sows. If the game GOAL is TERRITORY the capturer is the hole owner; otherwise each player captures from their own side of the board no matter who is sowing. 
-  + If MLAPS is LAPPER and the final seed sown for any lap meets the simple capture criteria for that hole, the contents of the hole are captured by the sower and not the hole owner and the turn is over. For CAPTTWOOUT, CAPT_NEXT and CROSSCAPT captures, the sower always does the final capture.
-  + GRANDSLAM rules are not applied. NOCAPTMOVES prevents these capture for the first moves.
-- SOW_SOW_CAPT_ALL: Similar to OWN_SOW_CAPT_ALL but only the SOWer captures seeds from their opponent's holes. 
-  + If mlaps is LAPPER and the final seed sown for any lap meets the capture criteria, the contents of the hole are captured by the sower and not the hole owner and the turn is over.
-  + GRANDSLAM rules are not applied. NOCAPTMOVES prevents this capture for the first number of specified moves.
-- NO_SOW_OPP_2S: Don't sow into opponents holes with 2 seeds.
-- CHANGE_DIR_LAP: Change the direction for each lap sown. Generally used with UDIR_HOLES so the player may choose the first direction.
-- MAX_SOW: holes sow_param seeds are skipped when sowing. That is, holes will never contain more seeds than sow_param.
-- LAP_CAPT: after each lapt check for a capture, if there is a capture continue sowing with another lap. If a basic capture is configured (evens, capt on, max or min), the hole after the captured seeds is drawn to continue lapping.</t>
-  </si>
-  <si>
-    <t>presowcapt</t>
-  </si>
-  <si>
-    <t>Pre Sow Capture</t>
-  </si>
-  <si>
-    <t>PreSowCapt</t>
-  </si>
-  <si>
-    <t>Capture type that occurs before sowing:
-- NONE: No capture before sowing.
-- CAPT_ONE: Capture 1 seed from the draw. If MLAPS, capture 1 seeds per lap.
-- ALL_SINGLE_XCAPT: Capture the seeds across from all singles.
-- DRAW_1_XCAPT: When draw 1 seed, capture any seeds on the other side of the board.</t>
+- MOVE_ALL_HOLES_FIRST: a move must initiated from each hole once before a second move may be made from any hole.  MOVE_ALL is incompatible with all pickers and capttwoout.
+- NOT_XFROM_1S: moves may not start from holes with a singleton opposite it.</t>
   </si>
 </sst>
 </file>
@@ -2054,9 +2055,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:J87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A78" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J81" sqref="J81"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J33" sqref="J33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2529,7 +2530,7 @@
         <v>2</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2627,10 +2628,10 @@
         <v>90</v>
       </c>
       <c r="B19" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="C19" s="3" t="s">
         <v>305</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>306</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>22</v>
@@ -2639,10 +2640,10 @@
         <v>130</v>
       </c>
       <c r="F19" s="3" t="s">
+        <v>306</v>
+      </c>
+      <c r="G19" s="5" t="s">
         <v>307</v>
-      </c>
-      <c r="G19" s="5" t="s">
-        <v>308</v>
       </c>
       <c r="H19" s="3">
         <v>5</v>
@@ -2651,7 +2652,7 @@
         <v>2</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
@@ -2877,10 +2878,10 @@
         <v>36</v>
       </c>
       <c r="B27" s="3" t="s">
+        <v>299</v>
+      </c>
+      <c r="C27" s="3" t="s">
         <v>300</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>301</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>22</v>
@@ -2889,10 +2890,10 @@
         <v>147</v>
       </c>
       <c r="F27" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="G27" s="5" t="s">
         <v>302</v>
-      </c>
-      <c r="G27" s="5" t="s">
-        <v>303</v>
       </c>
       <c r="H27" s="3">
         <v>2</v>
@@ -2901,7 +2902,7 @@
         <v>0</v>
       </c>
       <c r="J27" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
@@ -3052,7 +3053,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="210" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" ht="225" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>36</v>
       </c>
@@ -3081,7 +3082,7 @@
         <v>0</v>
       </c>
       <c r="J33" s="4" t="s">
-        <v>298</v>
+        <v>314</v>
       </c>
     </row>
     <row r="34" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -4534,10 +4535,10 @@
         <v>66</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="D81" s="3" t="s">
         <v>22</v>
@@ -4546,7 +4547,7 @@
         <v>133</v>
       </c>
       <c r="F81" s="3" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="G81" s="5" t="s">
         <v>161</v>
@@ -4558,7 +4559,7 @@
         <v>0</v>
       </c>
       <c r="J81" s="4" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
     <row r="82" spans="1:10" ht="409.5" x14ac:dyDescent="0.25">
@@ -4590,7 +4591,7 @@
         <v>0</v>
       </c>
       <c r="J82" s="4" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
     </row>
     <row r="83" spans="1:10" ht="30" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added a btn_behavior to allow selection of owned holes in territory games. It is selected via a round_fill that is allowed for territory games. Added two new round end mechanism: end when seeds on the board are fewer than either nbr_start or 2 times nbr_start. Added Adji_Kui_II. Updated Layemay_Waladat with the new round fill. Added note about Valdez description of Layli Goobalay (to Leyla-Gobale.txt).
</commit_message>
<xml_diff>
--- a/src/game_params.xlsx
+++ b/src/game_params.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Activity_Data\Mancala_github\MancalaGames\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B732EB63-3A40-47D4-9107-9746A6E8DE09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6949E52-56F7-411E-A297-29DAC4335B51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -870,16 +870,6 @@
     <t>NO_ROUNDS</t>
   </si>
   <si>
-    <t>When rounds are employed, each round may end under conditions that do not win the overall game. The board is then setup again per the game rules, generally with some feature changed based on the previous round: hole ownership, holes out of play, a shortened board. Play continues in rounds until either player meets the overall game winning condition.
-If the game is played in round, defines how each round ends: 
-- NO_ROUNDS: the game is not played in rounds
-- HALF_SEEDS: each round ends when one player has more that half the seeds
-- NO_MOVES: When MUSTSHARE is set, each round ends when neither player has a valid move.  When MUSTSHARE is not set, each round ends when a  player does have not a valid move at the start of their turn.
-For example: In Weg each round ends when neither player has a valid move. The board is then set up again after determining who owns what territory (holes). Rounds continue until one player has claimed sufficient territory to be declared the game winner (e.g. ownership of 10 or more holes).
-In the case of a round win or tie  a new starter is determined via ROUND_STARTER and  the board is reset according to ROUND_FILL.
-BLOCKS are used in many games and set between rounds based on the seed placement. TERRITORY GOAL games adjust hole ownership between rounds.</t>
-  </si>
-  <si>
     <t>The name of the Game Class. One of:
 Mancala: allows setting all parameters though there are limited combinations.
 Diffusion: has unique sow method and win conditions. Only very limited parameters may be changed from defaults.</t>
@@ -891,44 +881,9 @@
     <t>Repeat Turn Addin</t>
   </si>
   <si>
-    <t>The round fill method determines which holes are filled and how many seeds they are filled with when setting up for a new round.
-Several round fill mechanisms use the same general approach called the Empty Hole Method. The loser of the previous round will end up with empty holes. These holes are not playable if BLOCKS are used; otherwise they are playable. This method is not used for RND_ GOAL games.
-The seeds each player accummulated in the previous round are distributed into holes with exactly the same number in each. That number of seeds is NBR_START. The winner will fill all of their holes and put any remaining seeds into their own store. The loser will fill as many holes as they can with nbr_start seeds and put any remaining seeds (fewer than nbr_start) into their own store.
-LEFT_FILE, RIGHT_FILL and OUTSIDE_FILL define which holes that the loser must fill. UCHOOSE allows the loser to choose which holes have seeds.
-- NOT_APPLICABLE: round fill doesn't need to be specified: either the game not played in rounds (DEPRIVE game included) or game goal is TERRITORY (all holes filled).
-- LEFT_FILL: fill the round loser's holes from the player's left with nbr_start seeds each.  
-- RIGHT_FILL: fill the round loser's holes from the player's right with nbr_start seeds each. 
-- OUTSIDE_FILL: fill the round loser's holes from the outside ends toward the middle with nbr_start seeds each. Leftmost, rightmost, 2nd leftmost, 2nd rightmost, etc. until the seeds are used up.
-- EVEN_FILL: fill all holes (both sides) with the same number of seeds; determined by dividing the losers seeds by the number of holes per side. If that is not playable based on the minimum number of seeds required for a move (MIN_MOVE); extra seeds are put in each players leftmost hole. Any extra seeds are put in each player's store.
-- SHORTEN: the number of holes that the round loser can fill with NBR_START seeds are fill on both sides, other holes are left empty. Holes are filled opposite eachother. If BLOCKS is selected, the board is shortened to the number of holes filled (empty holes are blocked and out of play). If the game uses children, they will not be created if the board size is reduced to 3 or less.
-- UCHOOSE: allow user to choose which holes have seeds (are not blocked) when ROUNDS and BLOCKS are used.
-- UMOVE: allow the loser to choose where seeds are placed. At least one seed must be placed in each hole and the game must be playable (at least one hole has MIN_MOVE seeds), remaining seeds are placed in the store. The winner's layout is the same layout but reflected.</t>
-  </si>
-  <si>
     <t>Blocks remove holes from play and are shown on the UI with an X.
 When used with ROUNDS, the holes not filled from the player with fewer seeds are blocked and thus out of play for the round.
 When used with DEPRIVE, SOW_BLCK_DIV and goal_param holes are closed (blocked and removed from play) when sown to goal_param seeds.</t>
-  </si>
-  <si>
-    <t>The overall goal of the game. Defines how a player wins.
-- MAX_SEEDS: The goal is to collect the maximum number of seeds.
-  + If the game is not played in rounds, the game will end when one player has more than half of the total seeds.
-  + If the game is played in rounds, the round end condition is determined by ROUNDS. These games end when one player has collected sufficient seeds to prevent the opponent from filling the required number of holes. Generally, the required number of holes is one but this may be increased by setting goal_param. 
-  + In MAX_SEEDS/ROUNDS games the player only controls the holes on their side of the board, where as, in TERRITORY games a player may control holes on either side of the board.
-- DEPRIVE: eliminate all of your opponents seeds.
-  + If a player has no seeds at the start of their turn, they loose. If a player has no moves at the start of their turn, then the game outcome is determined by who has seeds: If both players have seeds, the game ends in a tie. If the current player has seeds, but the previous player does not, then the current player wins because they forced the previous player to give away all their seeds.
-  + GRANDSLAM must be legal for DEPRIVE games.
-  + Deprive games cannot be played in ROUNDS or use children. Additionally, the following options are incompatible with DEPRIVE games: MOVEUNLOCK, MUSTPASS and MUSTSHARE.
-- TERRITORY: claim ownership of holes. Each round the ownership of holes is determined by the number of seeds captured in the previous round. In a TERRITORY game without rounds, the winner is the player that gained the most territory during play. 
-  + TERRITORY games require STORES and that goal_param be set to a value between the number of holes and two times the number of holes.
-  + TERRITORY games are incompatible with NO_SIDES, START_PATTERN, GRANDSLAM of NOT_LEGAL, ALLOW_RULE of OPP_OR_EMPTY.
-- CLEAR: clear seeds from your own holes.
-  + Moves must always be possible so MIN_MOVE must be 1 and ALLOW_RULE single_all_to_zero may not be used.
-  + GRANDSLAM must be legal for DEPRIVE games.  Deprive games cannot be played in ROUNDS or use children. Additionally, the following options are incompatible with DEPRIVE games: MOVEUNLOCK, MUSTPASS and MUSTSHARE.
-- RND_WIN_COUNT:  win goal_param rounds. ROUND_FILL is not used; each round is setup as the start of the game.
-- RND_SEED_COUNT: collect goal_param seeds across several rounds. ROUND_FILL is not used; each round is setup as the start of the game.
-- RND_EXTRA_SEEDS: collect goal_param extra seeds (winner - loser seeds).  ROUND_FILL is not used; each round is setup as the start of the game.
-- RND_POINTS:  score goal_param points. WIN is 1 point. WIN and skunk (&gt; 3/4 of total seeds) is 2 points.  ROUND_FILL is not used; each round is setup as the start of the game.</t>
   </si>
   <si>
     <t>goal_param</t>
@@ -1172,6 +1127,54 @@
 - RIGHT_2_1ST_THEN_ALL_TWO:  The first turn must start from one of the two rightmost holes. Subsequent moves may only start from holes without 2 seeds, unless all holes contain zero or 2 seeds.
 - MOVE_ALL_HOLES_FIRST: a move must initiated from each hole once before a second move may be made from any hole.  MOVE_ALL is incompatible with all pickers and capttwoout.
 - NOT_XFROM_1S: moves may not start from holes with a singleton opposite it.</t>
+  </si>
+  <si>
+    <t>When rounds are employed, each round may end under conditions that do not win the overall game. The board is then setup again per the game rules, generally with some feature changed based on the previous round: hole ownership, holes out of play, a shortened board. Play continues in rounds until either player meets the overall game winning condition.
+If the game is played in round, defines how each round ends: 
+- NO_ROUNDS: the game is not played in rounds
+- HALF_SEEDS: each round ends when one player has more that half the seeds
+- NO_MOVES: When MUSTSHARE is set, each round ends when neither player has a valid move.  When MUSTSHARE is not set, each round ends when a  player does have not a valid move at the start of their turn.
+- END_S_SEEDS: End the round when there are number of start seeds or fewer in play.
+- END_2S_SEEDS: End the round when there are two times the number of start seeds or fewer in play.
+For example: In Weg each round ends when neither player has a valid move. The board is then set up again after determining who owns what territory (holes). Rounds continue until one player has claimed sufficient territory to be declared the game winner (e.g. ownership of 10 or more holes).
+In the case of a round win or tie  a new starter is determined via ROUND_STARTER and  the board is reset according to ROUND_FILL.
+BLOCKS are used in many games and set between rounds based on the seed placement. TERRITORY GOAL games adjust hole ownership between rounds.</t>
+  </si>
+  <si>
+    <t>The overall goal of the game. Defines how a player wins.
+- MAX_SEEDS: The goal is to collect the maximum number of seeds.
+  + If the game is not played in rounds, the game will end when one player has more than half of the total seeds.
+  + If the game is played in rounds, the round end condition is determined by ROUNDS. These games end when one player has collected sufficient seeds to prevent the opponent from filling the required number of holes. Generally, the required number of holes is one but this may be increased by setting goal_param. 
+  + In MAX_SEEDS/ROUNDS games the player only controls the holes on their side of the board, where as, in TERRITORY games a player may control holes on either side of the board.
+- DEPRIVE: eliminate all of your opponents seeds.
+  + If a player has no seeds at the start of their turn, they loose. If a player has no moves at the start of their turn, then the game outcome is determined by who has seeds: If both players have seeds, the game ends in a tie. If the current player has seeds, but the previous player does not, then the current player wins because they forced the previous player to give away all their seeds.
+  + GRANDSLAM must be legal for DEPRIVE games.
+  + DEPRIVE games cannot be played in ROUNDS or use children. Additionally, the following options are incompatible with DEPRIVE games: MOVEUNLOCK, MUSTPASS and MUSTSHARE.
+- TERRITORY: claim ownership of holes. Each round the ownership of holes is determined by the number of seeds captured in the previous round. In a TERRITORY game without rounds, the winner is the player that gained the most territory during play. 
+  + TERRITORY games require STORES and that goal_param be set to a value between the number of holes and two times the number of holes.
+  + TERRITORY games are incompatible with NO_SIDES, START_PATTERN, GRANDSLAM of NOT_LEGAL, ALLOW_RULE of OPP_OR_EMPTY.
+- CLEAR: clear seeds from your own holes.
+  + Moves must always be possible so MIN_MOVE must be 1 and ALLOW_RULE single_all_to_zero may not be used.
+  + GRANDSLAM must be legal for CLEAR games.  CLEAR games cannot be played in ROUNDS or use children. Additionally, the following options are incompatible with CLEAR games: MOVEUNLOCK, MUSTPASS and MUSTSHARE.
+- RND_WIN_COUNT:  win goal_param rounds. ROUND_FILL is not used; each round is setup as the start of the game.
+- RND_SEED_COUNT: collect goal_param seeds across several rounds. ROUND_FILL is not used; each round is setup as the start of the game.
+- RND_EXTRA_SEEDS: collect goal_param extra seeds (winner - loser seeds).  ROUND_FILL is not used; each round is setup as the start of the game.
+- RND_POINTS:  score goal_param points. WIN is 1 point. WIN and skunk (&gt; 3/4 of total seeds) is 2 points.  ROUND_FILL is not used; each round is setup as the start of the game.</t>
+  </si>
+  <si>
+    <t>The round fill method determines which holes are filled and how many seeds they are filled with when setting up for a new round.
+Several round fill mechanisms use the same general approach called the Empty Hole Method. The loser of the previous round will end up with empty holes. These holes are not playable if BLOCKS are used; otherwise they are playable. This method is not used for RND_* GOAL games.
+The seeds each player accummulated in the previous round are distributed into holes with exactly the same number in each. That number of seeds is NBR_START. The winner will fill all of their holes and put any remaining seeds into their own store. The loser will fill as many holes as they can with nbr_start seeds and put any remaining seeds (fewer than nbr_start) into their own store.
+LEFT_FILE, RIGHT_FILL and OUTSIDE_FILL define which holes that the loser must fill. UCHOOSE allows the loser to choose which holes have seeds.
+- NOT_APPLICABLE: round fill doesn't need to be specified: either the game not played in rounds (CLEAR &amp; DEPRIVE games included) or game goal is TERRITORY  without UCHOWN (see below, all holes filled).
+- LEFT_FILL: fill the round loser's holes from the player's left with nbr_start seeds each.  
+- RIGHT_FILL: fill the round loser's holes from the player's right with nbr_start seeds each. 
+- OUTSIDE_FILL: fill the round loser's holes from the outside ends toward the middle with nbr_start seeds each. Leftmost, rightmost, 2nd leftmost, 2nd rightmost, etc. until the seeds are used up.
+- EVEN_FILL: fill all holes (both sides) with the same number of seeds; determined by dividing the losers seeds by the number of holes per side. If that is not playable based on the minimum number of seeds required for a move (MIN_MOVE); extra seeds are put in each players leftmost hole. Any extra seeds are put in each player's store.
+- SHORTEN: the number of holes that the round loser can fill with NBR_START seeds are fill on both sides, other holes are left empty. Holes are filled opposite eachother. If BLOCKS is selected, the board is shortened to the number of holes filled (empty holes are blocked and out of play). If the game uses children, they will not be created if the board size is reduced to 3 or less.
+- UCHOOSE: allow user to choose which holes have seeds (are not blocked) when ROUNDS and BLOCKS are used.
+- UMOVE: allow the loser to choose where seeds are placed. At least one seed must be placed in each hole and the game must be playable (at least one hole has MIN_MOVE seeds), remaining seeds are placed in the store. The winner's layout is the same layout but reflected.
+- UCHOWN: The only round fill supported for territory games. The winner may choose which holes they control.</t>
   </si>
 </sst>
 </file>
@@ -2056,8 +2059,8 @@
   <dimension ref="A1:J87"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J33" sqref="J33"/>
+      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J43" sqref="J43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2112,17 +2115,17 @@
         <v>90</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3">
         <v>0</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="G2" s="5" t="s">
         <v>84</v>
@@ -2268,16 +2271,16 @@
         <v>90</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="E7" s="3">
         <v>0</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="G7" s="5" t="s">
         <v>84</v>
@@ -2390,19 +2393,19 @@
         <v>90</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="E11" s="3">
         <v>0</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="H11" s="3">
         <v>9</v>
@@ -2440,7 +2443,7 @@
         <v>0</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -2480,7 +2483,7 @@
         <v>90</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>111</v>
@@ -2489,7 +2492,7 @@
         <v>0</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="G14" s="5" t="s">
         <v>84</v>
@@ -2530,7 +2533,7 @@
         <v>2</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2570,16 +2573,16 @@
         <v>90</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="E17" s="3">
         <v>0</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="G17" s="5" t="s">
         <v>84</v>
@@ -2596,10 +2599,10 @@
         <v>90</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>22</v>
@@ -2620,7 +2623,7 @@
         <v>2</v>
       </c>
       <c r="J18" s="4" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -2628,10 +2631,10 @@
         <v>90</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>22</v>
@@ -2640,10 +2643,10 @@
         <v>130</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="H19" s="3">
         <v>5</v>
@@ -2652,7 +2655,7 @@
         <v>2</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
@@ -2724,16 +2727,16 @@
         <v>90</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="E22" s="3">
         <v>0</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="G22" s="5" t="s">
         <v>84</v>
@@ -2838,7 +2841,7 @@
         <v>0</v>
       </c>
       <c r="J25" s="4" t="s">
-        <v>255</v>
+        <v>313</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="105" x14ac:dyDescent="0.25">
@@ -2846,10 +2849,10 @@
         <v>36</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>22</v>
@@ -2870,7 +2873,7 @@
         <v>0</v>
       </c>
       <c r="J26" s="4" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="120" x14ac:dyDescent="0.25">
@@ -2878,10 +2881,10 @@
         <v>36</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>22</v>
@@ -2890,10 +2893,10 @@
         <v>147</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="H27" s="3">
         <v>2</v>
@@ -2902,7 +2905,7 @@
         <v>0</v>
       </c>
       <c r="J27" s="4" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
@@ -2910,16 +2913,16 @@
         <v>36</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="E28" s="3">
         <v>0</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="G28" s="5" t="s">
         <v>84</v>
@@ -3000,16 +3003,16 @@
         <v>36</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="E31" s="3">
         <v>0</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="G31" s="3">
         <v>0</v>
@@ -3082,7 +3085,7 @@
         <v>0</v>
       </c>
       <c r="J33" s="4" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
     </row>
     <row r="34" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3114,7 +3117,7 @@
         <v>2</v>
       </c>
       <c r="J34" s="4" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
@@ -3154,16 +3157,16 @@
         <v>36</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="E36" s="3">
         <v>0</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="G36" s="3">
         <v>0</v>
@@ -3276,16 +3279,16 @@
         <v>36</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="E40" s="3">
         <v>0</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="G40" s="3">
         <v>0</v>
@@ -3297,7 +3300,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:10" ht="210" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" ht="240" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>36</v>
       </c>
@@ -3326,7 +3329,7 @@
         <v>2</v>
       </c>
       <c r="J41" s="4" t="s">
-        <v>249</v>
+        <v>312</v>
       </c>
     </row>
     <row r="42" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -3361,7 +3364,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="43" spans="1:10" ht="330" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" ht="345" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>36</v>
       </c>
@@ -3390,7 +3393,7 @@
         <v>2</v>
       </c>
       <c r="J43" s="4" t="s">
-        <v>253</v>
+        <v>314</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -3422,7 +3425,7 @@
         <v>2</v>
       </c>
       <c r="J44" s="4" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="45" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -3454,7 +3457,7 @@
         <v>0</v>
       </c>
       <c r="J45" s="4" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
@@ -3718,16 +3721,16 @@
         <v>120</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="E54" s="3">
         <v>0</v>
       </c>
       <c r="F54" s="3" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="G54" s="3">
         <v>0</v>
@@ -3840,16 +3843,16 @@
         <v>120</v>
       </c>
       <c r="B58" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="C58" s="3" t="s">
         <v>268</v>
       </c>
-      <c r="C58" s="3" t="s">
-        <v>271</v>
-      </c>
       <c r="E58" s="3">
         <v>0</v>
       </c>
       <c r="F58" s="3" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="G58" s="3">
         <v>0</v>
@@ -4093,7 +4096,7 @@
         <v>130</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D66" s="3" t="s">
         <v>122</v>
@@ -4256,7 +4259,7 @@
         <v>81</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="D72" s="3" t="s">
         <v>22</v>
@@ -4349,16 +4352,16 @@
         <v>66</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="E75" s="3">
         <v>0</v>
       </c>
       <c r="F75" s="3" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="G75" s="3">
         <v>0</v>
@@ -4410,7 +4413,7 @@
         <v>76</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="D77" s="3" t="s">
         <v>22</v>
@@ -4535,10 +4538,10 @@
         <v>66</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="D81" s="3" t="s">
         <v>22</v>
@@ -4547,7 +4550,7 @@
         <v>133</v>
       </c>
       <c r="F81" s="3" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="G81" s="5" t="s">
         <v>161</v>
@@ -4559,7 +4562,7 @@
         <v>0</v>
       </c>
       <c r="J81" s="4" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
     </row>
     <row r="82" spans="1:10" ht="409.5" x14ac:dyDescent="0.25">
@@ -4591,7 +4594,7 @@
         <v>0</v>
       </c>
       <c r="J82" s="4" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
     </row>
     <row r="83" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -4599,10 +4602,10 @@
         <v>66</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="D83" s="3" t="s">
         <v>22</v>
@@ -4623,7 +4626,7 @@
         <v>0</v>
       </c>
       <c r="J83" s="4" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.25">
@@ -4631,16 +4634,16 @@
         <v>66</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="E84" s="3">
         <v>0</v>
       </c>
       <c r="F84" s="3" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="G84" s="3">
         <v>0</v>
@@ -4681,7 +4684,7 @@
         <v>2</v>
       </c>
       <c r="J85" s="4" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
     </row>
     <row r="86" spans="1:10" ht="30" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added a parameter to describe where children can be made. This removed the need for Walda as separate child type. Children without stores are now treated exactly like walda were. Child location checks were all moved from the  capturer to make_child (fixed a bug, where the mlap sower would stop even if a child couldn't actually be made). ChildLocOk decorator/wrapper was added to implement the hole checking. Minor effort made to improve handling of ints in game_params file. order, row & col now read in as strs. Game Andot was added.
</commit_message>
<xml_diff>
--- a/src/game_params.xlsx
+++ b/src/game_params.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Activity_Data\Mancala_github\MancalaGames\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6949E52-56F7-411E-A297-29DAC4335B51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCE053FA-B936-4CB3-90A3-4C5863791E57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="34335" yWindow="1260" windowWidth="22185" windowHeight="14895" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="game_params" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">game_params!$A$1:$J$87</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">game_params!$A$1:$J$88</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="315">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="320">
   <si>
     <t>tab</t>
   </si>
@@ -771,12 +771,6 @@
     <t>Sow seeds into your own store when passing it. Do not sow into your opponents store. When the final seed is sown into the store, the sower gets another turn.</t>
   </si>
   <si>
-    <t>Additional child creation requirements may be set:
-- NONE: no additional restrictions.
-- OPP_ONLY:  Only make children on the opposite side of the board. Incompatible with BULL, QUR, and WEG child types.
-- NOT_1ST_OPP: Don't make a child in the first hole on the opponents side/territory with one seed.</t>
-  </si>
-  <si>
     <t>Evens Multiplier</t>
   </si>
   <si>
@@ -912,25 +906,6 @@
   <si>
     <t>A general parameter for sowing. Usage is based on other sow options:
 - Sow rule of MAX_SOW: maximum number of seeds a hole may contain</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Games with children allow players to claim holes. These child holes are an extension of the stores and seeds in them count towards a win. Making a child stops any multiple lap sowing, moves cannot start from children, and they cannot be captured (except for special rules associated with WEGs).
-- NOCHILD: children are not used.
-- NORMAL: children are made when a final seeds sows a hole to CHILD_CVT.
-- WALDA: STORES are not supported. Captures are instead moved into waldas, thus a player may not capture until they have created a walda. 
-  + Walda locations are limited.  Each player may create up to 6 waldas: on either end of each side of the board and the next two outer holes on their own side of the board. Note that there are only 8 total places that waldas maybe created.
-- ONE_CHILD: only one child allowed per player.
-  + Children must not be symmetrically opposite eachother. For example,  in a 9 hole per side game with holes numbered as follows, children may not be in the same numbered holes:
-  + 9 8 7 6 5 4 3 2 1
-  + 1 2 3 4 5 6 7 8 9 
-  + Depending on sow direction some holes are prohibited from being made children: 
-  + CW &amp; CCW:  the last of your opponents holes that you would sow into may not be made a child. CW holes numbered 1 above and CCW holes numberd 9 above.
-  + SPLIT: no end holes may be made children.
-  + Used to create tuzdek style children along with CHILD_RULE of OPP_ONLY.
-- WEG: children maybe created in holes owned by the opponent. Ending a sow in an opponent's weg captures the seed just sown and one more (if there is one); generally, the player gets to play again (per CAPT_RTURN). WEGs are supported for TERRITORY games only (hole ownership required).
-- BULL: create one bull if final seed sows to CHILD_CVT, create two bulls if the final two seeds are sown to CHILD_CVT-1 and CHILD_CVT (in either order).
-- QUR: when a seed is sown into an empty hole on the player's side of the board and the opposite hole contains CHILD_CVT, create children in both holes: final seed location and opposite.
-</t>
   </si>
   <si>
     <t>label</t>
@@ -1175,6 +1150,68 @@
 - UCHOOSE: allow user to choose which holes have seeds (are not blocked) when ROUNDS and BLOCKS are used.
 - UMOVE: allow the loser to choose where seeds are placed. At least one seed must be placed in each hole and the game must be playable (at least one hole has MIN_MOVE seeds), remaining seeds are placed in the store. The winner's layout is the same layout but reflected.
 - UCHOWN: The only round fill supported for territory games. The winner may choose which holes they control.</t>
+  </si>
+  <si>
+    <t>child_locs</t>
+  </si>
+  <si>
+    <t>Child Locations</t>
+  </si>
+  <si>
+    <t>ChildLocs</t>
+  </si>
+  <si>
+    <t>ANYWHERE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Games with children allow players to claim holes. These child holes are an extension of the stores and seeds in them count towards a win. Making a child stops any multiple lap sowing, moves cannot start from children, and they cannot be captured (except for special rules associated with WEGs).
+- NOCHILD: children are not used.
+- NORMAL: children are made when a final seeds sows a hole to CHILD_CVT. If stores are not included captures are instead moved into children, thus a player may not capture until they have created a child. 
+- ONE_CHILD: only one child allowed per player.
+  + Children must not be symmetrically opposite eachother. For example,  in a 9 hole per side game with holes numbered as follows, children may not be in the same numbered holes:
+  + 9 8 7 6 5 4 3 2 1
+  + 1 2 3 4 5 6 7 8 9 
+  + Depending on sow direction some holes are prohibited from being made children: 
+  + CW &amp; CCW:  the last of your opponents holes that you would sow into may not be made a child. CW holes numbered 1 above and CCW holes numberd 9 above.
+  + SPLIT: no end holes may be made children.
+  + Used to create tuzdek style children along with CHILD_RULE of OPP_ONLY.
+- WEG: children maybe created in holes owned by the opponent. Ending a sow in an opponent's weg captures the seed just sown and one more (if there is one); generally, the player gets to play again (per CAPT_RTURN). WEGs are supported for TERRITORY games only (hole ownership required).
+- BULL: create one bull if final seed sows to CHILD_CVT, create two bulls if the final two seeds are sown to CHILD_CVT-1 and CHILD_CVT (in either order).
+- QUR: when a seed is sown into an empty hole on the player's side of the board and the opposite hole contains CHILD_CVT, create children in both holes: final seed location and opposite.
+</t>
+  </si>
+  <si>
+    <t>Additional child creation requirements may be set. These are in addition to location restrictions specified by CHILD_LOCS.
+- NONE: no additional restrictions.
+- OPP_ONLY:  Only make children on the opposite side of the board. Incompatible with BULL, QUR, and WEG child types.
+- NOT_1ST_OPP: Don't make a child in the first hole on the opponents side/territory with one seed.</t>
+  </si>
+  <si>
+    <t>Locations where children can be made by each player. The notes designate players as: T - top player, B - bottom player. N - neither player. For shorter boards, the pattern is generated using assignments (a b c d e) as:
+board length 2: a e
+board length 3: a c e
+board length 4: a b d e
+The center hole  (c) is replicated for larger boards. 
+- ANYWHERE: children may be made anywhere.
+- ENDS_ONLY: children may be made in the end holes only.
+  + TB N N N TB
+  + TB N N N TB
+- NO_ENDS: children may only be made on internal holes, no end holes.
+  + N TB TB TB N
+  + N TB TB TB N
+- INV_ENDS_PLUS_MID: children may be made by each player on the opposite side ends and all own side middle holes.
+  + B T T T B
+  + T B B B T
+- ENDS_PLUS_ONE_OPP: Either player may make children in any end hole, but the next inner hole can only be made on the opposite side. 
+  +  Used for Walda type children: Each player may create up to 6 walda: on either end of each side of the board and the next two outer holes on their own side of the board. Note that there are only 8 total places that walda maybe created.
+  + TB B N B TB
+  + TB T N T TB
+- NO_OWN_RIGHT: children may not be made on the your own rightmost hole. 
+  + B TB TB TB TB
+  + TB TB TB TB T
+- NO_OPP_RIGHT: children may not be made on the opposite rightmost hole.
+  + TB TB TB TB T
+  + B TB TB TB TB</t>
   </si>
 </sst>
 </file>
@@ -2056,11 +2093,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:J87"/>
+  <dimension ref="A1:J88"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J43" sqref="J43"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A86" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J88" sqref="J88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2115,17 +2152,17 @@
         <v>90</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3">
         <v>0</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="G2" s="5" t="s">
         <v>84</v>
@@ -2199,7 +2236,7 @@
         <v>0</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -2231,7 +2268,7 @@
         <v>0</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -2263,7 +2300,7 @@
         <v>0</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -2271,16 +2308,16 @@
         <v>90</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="E7" s="3">
         <v>0</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="G7" s="5" t="s">
         <v>84</v>
@@ -2353,7 +2390,7 @@
         <v>0</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2393,19 +2430,19 @@
         <v>90</v>
       </c>
       <c r="B11" s="3" t="s">
+        <v>269</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>270</v>
+      </c>
+      <c r="E11" s="3">
+        <v>0</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="G11" s="5" t="s">
         <v>271</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>272</v>
-      </c>
-      <c r="E11" s="3">
-        <v>0</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>262</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>273</v>
       </c>
       <c r="H11" s="3">
         <v>9</v>
@@ -2443,7 +2480,7 @@
         <v>0</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -2475,7 +2512,7 @@
         <v>0</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -2483,7 +2520,7 @@
         <v>90</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>111</v>
@@ -2492,7 +2529,7 @@
         <v>0</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="G14" s="5" t="s">
         <v>84</v>
@@ -2533,7 +2570,7 @@
         <v>2</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2573,16 +2610,16 @@
         <v>90</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="E17" s="3">
         <v>0</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="G17" s="5" t="s">
         <v>84</v>
@@ -2599,10 +2636,10 @@
         <v>90</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>22</v>
@@ -2623,7 +2660,7 @@
         <v>2</v>
       </c>
       <c r="J18" s="4" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -2631,10 +2668,10 @@
         <v>90</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>22</v>
@@ -2643,10 +2680,10 @@
         <v>130</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="H19" s="3">
         <v>5</v>
@@ -2655,7 +2692,7 @@
         <v>2</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
@@ -2727,16 +2764,16 @@
         <v>90</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="E22" s="3">
         <v>0</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="G22" s="5" t="s">
         <v>84</v>
@@ -2809,7 +2846,7 @@
         <v>2</v>
       </c>
       <c r="J24" s="4" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="409.5" x14ac:dyDescent="0.25">
@@ -2841,7 +2878,7 @@
         <v>0</v>
       </c>
       <c r="J25" s="4" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="105" x14ac:dyDescent="0.25">
@@ -2849,10 +2886,10 @@
         <v>36</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>22</v>
@@ -2873,7 +2910,7 @@
         <v>0</v>
       </c>
       <c r="J26" s="4" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="120" x14ac:dyDescent="0.25">
@@ -2881,10 +2918,10 @@
         <v>36</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>22</v>
@@ -2893,10 +2930,10 @@
         <v>147</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="H27" s="3">
         <v>2</v>
@@ -2905,7 +2942,7 @@
         <v>0</v>
       </c>
       <c r="J27" s="4" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
@@ -2913,16 +2950,16 @@
         <v>36</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="E28" s="3">
         <v>0</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="G28" s="5" t="s">
         <v>84</v>
@@ -3003,19 +3040,19 @@
         <v>36</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="E31" s="3">
         <v>0</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>262</v>
-      </c>
-      <c r="G31" s="3">
-        <v>0</v>
+        <v>260</v>
+      </c>
+      <c r="G31" s="5" t="s">
+        <v>84</v>
       </c>
       <c r="H31" s="3">
         <v>7</v>
@@ -3085,7 +3122,7 @@
         <v>0</v>
       </c>
       <c r="J33" s="4" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
     </row>
     <row r="34" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3117,7 +3154,7 @@
         <v>2</v>
       </c>
       <c r="J34" s="4" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
@@ -3157,19 +3194,19 @@
         <v>36</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="E36" s="3">
         <v>0</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>262</v>
-      </c>
-      <c r="G36" s="3">
-        <v>0</v>
+        <v>260</v>
+      </c>
+      <c r="G36" s="5" t="s">
+        <v>84</v>
       </c>
       <c r="H36" s="3">
         <v>3</v>
@@ -3271,7 +3308,7 @@
         <v>2</v>
       </c>
       <c r="J39" s="4" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
@@ -3279,19 +3316,19 @@
         <v>36</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="E40" s="3">
         <v>0</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>262</v>
-      </c>
-      <c r="G40" s="3">
-        <v>0</v>
+        <v>260</v>
+      </c>
+      <c r="G40" s="5" t="s">
+        <v>84</v>
       </c>
       <c r="H40" s="3">
         <v>7</v>
@@ -3320,7 +3357,7 @@
         <v>42</v>
       </c>
       <c r="G41" s="5" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="H41" s="3">
         <v>8</v>
@@ -3329,7 +3366,7 @@
         <v>2</v>
       </c>
       <c r="J41" s="4" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="42" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -3393,7 +3430,7 @@
         <v>2</v>
       </c>
       <c r="J43" s="4" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -3425,7 +3462,7 @@
         <v>2</v>
       </c>
       <c r="J44" s="4" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="45" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -3457,7 +3494,7 @@
         <v>0</v>
       </c>
       <c r="J45" s="4" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
@@ -3649,7 +3686,7 @@
         <v>0</v>
       </c>
       <c r="J51" s="4" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
@@ -3721,19 +3758,19 @@
         <v>120</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="E54" s="3">
         <v>0</v>
       </c>
       <c r="F54" s="3" t="s">
-        <v>262</v>
-      </c>
-      <c r="G54" s="3">
-        <v>0</v>
+        <v>260</v>
+      </c>
+      <c r="G54" s="5" t="s">
+        <v>84</v>
       </c>
       <c r="H54" s="3">
         <v>5</v>
@@ -3762,7 +3799,7 @@
         <v>87</v>
       </c>
       <c r="G55" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="H55" s="3">
         <v>6</v>
@@ -3794,7 +3831,7 @@
         <v>87</v>
       </c>
       <c r="G56" s="3" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="H56" s="3">
         <v>7</v>
@@ -3843,19 +3880,19 @@
         <v>120</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="E58" s="3">
         <v>0</v>
       </c>
       <c r="F58" s="3" t="s">
-        <v>262</v>
-      </c>
-      <c r="G58" s="3">
-        <v>0</v>
+        <v>260</v>
+      </c>
+      <c r="G58" s="5" t="s">
+        <v>84</v>
       </c>
       <c r="H58" s="3">
         <v>1</v>
@@ -3884,7 +3921,7 @@
         <v>87</v>
       </c>
       <c r="G59" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="H59" s="3">
         <v>2</v>
@@ -3904,7 +3941,7 @@
         <v>121</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D60" s="3" t="s">
         <v>122</v>
@@ -3936,7 +3973,7 @@
         <v>123</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D61" s="3" t="s">
         <v>122</v>
@@ -3968,7 +4005,7 @@
         <v>124</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D62" s="3" t="s">
         <v>122</v>
@@ -4000,7 +4037,7 @@
         <v>125</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D63" s="3" t="s">
         <v>122</v>
@@ -4032,7 +4069,7 @@
         <v>126</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D64" s="3" t="s">
         <v>122</v>
@@ -4064,7 +4101,7 @@
         <v>127</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D65" s="3" t="s">
         <v>122</v>
@@ -4096,7 +4133,7 @@
         <v>130</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D66" s="3" t="s">
         <v>122</v>
@@ -4259,7 +4296,7 @@
         <v>81</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="D72" s="3" t="s">
         <v>22</v>
@@ -4280,7 +4317,7 @@
         <v>0</v>
       </c>
       <c r="J72" s="8" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="73" spans="1:10" ht="165" x14ac:dyDescent="0.25">
@@ -4352,19 +4389,19 @@
         <v>66</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="E75" s="3">
         <v>0</v>
       </c>
       <c r="F75" s="3" t="s">
-        <v>262</v>
-      </c>
-      <c r="G75" s="3">
-        <v>0</v>
+        <v>260</v>
+      </c>
+      <c r="G75" s="5" t="s">
+        <v>84</v>
       </c>
       <c r="H75" s="3">
         <v>3</v>
@@ -4413,7 +4450,7 @@
         <v>76</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="D77" s="3" t="s">
         <v>22</v>
@@ -4538,10 +4575,10 @@
         <v>66</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="D81" s="3" t="s">
         <v>22</v>
@@ -4550,7 +4587,7 @@
         <v>133</v>
       </c>
       <c r="F81" s="3" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="G81" s="5" t="s">
         <v>161</v>
@@ -4562,7 +4599,7 @@
         <v>0</v>
       </c>
       <c r="J81" s="4" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
     </row>
     <row r="82" spans="1:10" ht="409.5" x14ac:dyDescent="0.25">
@@ -4594,7 +4631,7 @@
         <v>0</v>
       </c>
       <c r="J82" s="4" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="83" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -4602,10 +4639,10 @@
         <v>66</v>
       </c>
       <c r="B83" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="C83" s="3" t="s">
         <v>258</v>
-      </c>
-      <c r="C83" s="3" t="s">
-        <v>259</v>
       </c>
       <c r="D83" s="3" t="s">
         <v>22</v>
@@ -4626,7 +4663,7 @@
         <v>0</v>
       </c>
       <c r="J83" s="4" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.25">
@@ -4634,19 +4671,19 @@
         <v>66</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="E84" s="3">
         <v>0</v>
       </c>
       <c r="F84" s="3" t="s">
-        <v>262</v>
-      </c>
-      <c r="G84" s="3">
-        <v>0</v>
+        <v>260</v>
+      </c>
+      <c r="G84" s="5" t="s">
+        <v>84</v>
       </c>
       <c r="H84" s="3">
         <v>3</v>
@@ -4655,7 +4692,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="85" spans="1:10" ht="360" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:10" ht="330" x14ac:dyDescent="0.25">
       <c r="A85" s="3" t="s">
         <v>66</v>
       </c>
@@ -4684,7 +4721,7 @@
         <v>2</v>
       </c>
       <c r="J85" s="4" t="s">
-        <v>261</v>
+        <v>317</v>
       </c>
     </row>
     <row r="86" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -4748,11 +4785,43 @@
         <v>2</v>
       </c>
       <c r="J87" s="4" t="s">
-        <v>229</v>
+        <v>318</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" ht="405" x14ac:dyDescent="0.25">
+      <c r="A88" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B88" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="C88" s="3" t="s">
+        <v>314</v>
+      </c>
+      <c r="D88" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E88" s="3">
+        <v>112</v>
+      </c>
+      <c r="F88" s="3" t="s">
+        <v>315</v>
+      </c>
+      <c r="G88" s="3" t="s">
+        <v>316</v>
+      </c>
+      <c r="H88" s="3">
+        <v>7</v>
+      </c>
+      <c r="I88" s="3">
+        <v>2</v>
+      </c>
+      <c r="J88" s="4" t="s">
+        <v>319</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J87" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <autoFilter ref="A1:J88" xr:uid="{00000000-0001-0000-0000-000000000000}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J87">
       <sortCondition ref="A2:A87"/>
       <sortCondition ref="I2:I87"/>

</xml_diff>

<commit_message>
Game text improvements. Added allow_rule don't sow opponents children. Corrected _all_games in analysis files.
</commit_message>
<xml_diff>
--- a/src/game_params.xlsx
+++ b/src/game_params.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Activity_Data\Mancala_github\MancalaGames\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCE053FA-B936-4CB3-90A3-4C5863791E57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EA7CD5D-A9A8-4C4F-B266-32A2AB7AB8CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34335" yWindow="1260" windowWidth="22185" windowHeight="14895" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="game_params" sheetId="1" r:id="rId1"/>
@@ -1071,25 +1071,6 @@
 - DRAW_1_XCAPT: When draw 1 seed, capture any seeds on the other side of the board.</t>
   </si>
   <si>
-    <t>Special sow rules add additional behavior or restrictions to the sowing phase:
-- NONE: there is no special sowing rule.
-- SOW_BLKD_DIV: If the final seed of an individual sow lands on the opposite side of the board and brings the contents of that hole to goal_param seeds, the hole is closed closed (blocked). In single lap games, the hole's seeds are removed from play. In multilap games, the seeds are used to continue sowing.
-  + When sowing, blocked holes on your own side of the board are skipped  and blocked holes on opponent's side are diverted out of play or captured.
-  +  Game GOAL must be DEPRIVE and all of the associated restrictions apply. NOCAPTMOVES maybe used to prevent closing holes on the initial games moves. Capture mechanisms other than closing holes are not supported. The minimum move must be 1 and thus SOW_START is incompatible.  ALLOW_RULE may not be used to limit allowable moves.  SKIP_START and VISIT_OPP are not supported with SOW_BLKD_DIV.  MLAPS of LAPPER_NEXT is not supported with SOW_BLKD_DIV(_NR).
-- SOW_BLKD_DIV_NR: Behaves the same as SOW_BLKD_DIV except that each player's rightmost hole cannot be closed. 
-- OWN_SOW_CAPT_ALL: The hole OWNer captures all holes that are sown to meet the simple capture criteria no matter who sowed them.  The simple capture criteria are: evens, min, max and capture on. Other criteria are enforced: side of the board, unlocked, and not child.
-  + The capture is done by the hole owner, so the non-sower may capture seeds while their opponents sows. If the game GOAL is TERRITORY the capturer is the hole owner; otherwise each player captures from their own side of the board no matter who is sowing. 
-  + If MLAPS is LAPPER and the final seed sown for any lap meets the simple capture criteria for that hole, the contents of the hole are captured by the sower and not the hole owner and the turn is over. For CAPTTWOOUT, CAPT_NEXT and CROSSCAPT captures, the sower always does the final capture.
-  + GRANDSLAM rules are not applied. NOCAPTMOVES prevents these capture for the first moves.
-- SOW_CAPT_ALL: Similar to OWN_SOW_CAPT_ALL but only the SOWer captures seeds from the side specified by CAPT_SIDE. BOTH sower capturers from any hole. OPP sower capturer only from opponents holes.  OWN sower captures only from their own holes. 
-  + If mlaps is LAPPER and the final seed sown for any lap meets the capture criteria, the contents of the hole are captured by the sower and not the hole owner and the turn is over.
-  + GRANDSLAM rules are not applied. NOCAPTMOVES prevents this capture for the first number of specified moves.
-- NO_SOW_OPP_2S: Don't sow into opponents holes with 2 seeds.
-- CHANGE_DIR_LAP: Change the direction for each lap sown. Generally used with UDIR_HOLES so the player may choose the first direction.
-- MAX_SOW: holes sow_param seeds are skipped when sowing. That is, holes will never contain more seeds than sow_param.
-- LAP_CAPT: after each lapt check for a capture, if there is a capture continue sowing with another lap. If a basic capture is configured (evens, capt on, max or min), the hole after the captured seeds is drawn to continue lapping.</t>
-  </si>
-  <si>
     <t>Allow rules limit the holes from which moves may start.  Disallowed holes are not selectable.
 - NONE: no special rule
 - OPP_OR_EMPTY:  Limit the allowable holes to those that end in an empty hole or reach the opponents side of the board.
@@ -1212,6 +1193,26 @@
 - NO_OPP_RIGHT: children may not be made on the opposite rightmost hole.
   + TB TB TB TB T
   + B TB TB TB TB</t>
+  </si>
+  <si>
+    <t>Special sow rules add additional behavior or restrictions to the sowing phase:
+- NONE: there is no special sowing rule.
+- SOW_BLKD_DIV: If the final seed of an individual sow lands on the opposite side of the board and brings the contents of that hole to goal_param seeds, the hole is closed closed (blocked). In single lap games, the hole's seeds are removed from play. In multilap games, the seeds are used to continue sowing.
+  + When sowing, blocked holes on your own side of the board are skipped  and blocked holes on opponent's side are diverted out of play or captured.
+  +  Game GOAL must be DEPRIVE and all of the associated restrictions apply. NOCAPTMOVES maybe used to prevent closing holes on the initial games moves. Capture mechanisms other than closing holes are not supported. The minimum move must be 1 and thus SOW_START is incompatible.  ALLOW_RULE may not be used to limit allowable moves.  SKIP_START and VISIT_OPP are not supported with SOW_BLKD_DIV.  MLAPS of LAPPER_NEXT is not supported with SOW_BLKD_DIV(_NR).
+- SOW_BLKD_DIV_NR: Behaves the same as SOW_BLKD_DIV except that each player's rightmost hole cannot be closed. 
+- OWN_SOW_CAPT_ALL: The hole OWNer captures all holes that are sown to meet the simple capture criteria no matter who sowed them.  The simple capture criteria are: evens, min, max and capture on. Other criteria are enforced: side of the board, unlocked, and not child.
+  + The capture is done by the hole owner, so the non-sower may capture seeds while their opponents sows. If the game GOAL is TERRITORY the capturer is the hole owner; otherwise each player captures from their own side of the board no matter who is sowing. 
+  + If MLAPS is LAPPER and the final seed sown for any lap meets the simple capture criteria for that hole, the contents of the hole are captured by the sower and not the hole owner and the turn is over. For CAPTTWOOUT, CAPT_NEXT and CROSSCAPT captures, the sower always does the final capture.
+  + GRANDSLAM rules are not applied. NOCAPTMOVES prevents these capture for the first moves.
+- SOW_CAPT_ALL: Similar to OWN_SOW_CAPT_ALL but only the SOWer captures seeds from the side specified by CAPT_SIDE. BOTH sower capturers from any hole. OPP sower capturer only from opponents holes.  OWN sower captures only from their own holes. 
+  + If mlaps is LAPPER and the final seed sown for any lap meets the capture criteria, the contents of the hole are captured by the sower and not the hole owner and the turn is over.
+  + GRANDSLAM rules are not applied. NOCAPTMOVES prevents this capture for the first number of specified moves.
+- NO_SOW_OPP_2S: Don't sow into opponents holes with 2 seeds.
+- CHANGE_DIR_LAP: Change the direction for each lap sown. Generally used with UDIR_HOLES so the player may choose the first direction.
+- MAX_SOW: holes sow_param seeds are skipped when sowing. That is, holes will never contain more seeds than sow_param.
+- LAP_CAPT: after each lapt check for a capture, if there is a capture continue sowing with another lap. If a basic capture is configured (evens, capt on, max or min), the hole after the captured seeds is drawn to continue lapping.
+- NO_OPP_CHILD: do not sow into your opponents children.</t>
   </si>
 </sst>
 </file>
@@ -2095,9 +2096,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:J88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A86" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J88" sqref="J88"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J82" sqref="J82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2878,7 +2879,7 @@
         <v>0</v>
       </c>
       <c r="J25" s="4" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="105" x14ac:dyDescent="0.25">
@@ -3122,7 +3123,7 @@
         <v>0</v>
       </c>
       <c r="J33" s="4" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="34" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3366,7 +3367,7 @@
         <v>2</v>
       </c>
       <c r="J41" s="4" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="42" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -3430,7 +3431,7 @@
         <v>2</v>
       </c>
       <c r="J43" s="4" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -4631,7 +4632,7 @@
         <v>0</v>
       </c>
       <c r="J82" s="4" t="s">
-        <v>308</v>
+        <v>319</v>
       </c>
     </row>
     <row r="83" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -4721,7 +4722,7 @@
         <v>2</v>
       </c>
       <c r="J85" s="4" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="86" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -4785,7 +4786,7 @@
         <v>2</v>
       </c>
       <c r="J87" s="4" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="88" spans="1:10" ht="405" x14ac:dyDescent="0.25">
@@ -4793,10 +4794,10 @@
         <v>66</v>
       </c>
       <c r="B88" s="3" t="s">
+        <v>312</v>
+      </c>
+      <c r="C88" s="3" t="s">
         <v>313</v>
-      </c>
-      <c r="C88" s="3" t="s">
-        <v>314</v>
       </c>
       <c r="D88" s="3" t="s">
         <v>22</v>
@@ -4805,10 +4806,10 @@
         <v>112</v>
       </c>
       <c r="F88" s="3" t="s">
+        <v>314</v>
+      </c>
+      <c r="G88" s="3" t="s">
         <v>315</v>
-      </c>
-      <c r="G88" s="3" t="s">
-        <v>316</v>
       </c>
       <c r="H88" s="3">
         <v>7</v>
@@ -4817,7 +4818,7 @@
         <v>2</v>
       </c>
       <c r="J88" s="4" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Game text improvements. Change DontUndoMoveOne to work with mlength 3 games. Corrected _all_games in analysis files.
</commit_message>
<xml_diff>
--- a/src/game_params.xlsx
+++ b/src/game_params.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Activity_Data\Mancala_github\MancalaGames\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCE053FA-B936-4CB3-90A3-4C5863791E57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EA7CD5D-A9A8-4C4F-B266-32A2AB7AB8CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34335" yWindow="1260" windowWidth="22185" windowHeight="14895" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="game_params" sheetId="1" r:id="rId1"/>
@@ -1071,25 +1071,6 @@
 - DRAW_1_XCAPT: When draw 1 seed, capture any seeds on the other side of the board.</t>
   </si>
   <si>
-    <t>Special sow rules add additional behavior or restrictions to the sowing phase:
-- NONE: there is no special sowing rule.
-- SOW_BLKD_DIV: If the final seed of an individual sow lands on the opposite side of the board and brings the contents of that hole to goal_param seeds, the hole is closed closed (blocked). In single lap games, the hole's seeds are removed from play. In multilap games, the seeds are used to continue sowing.
-  + When sowing, blocked holes on your own side of the board are skipped  and blocked holes on opponent's side are diverted out of play or captured.
-  +  Game GOAL must be DEPRIVE and all of the associated restrictions apply. NOCAPTMOVES maybe used to prevent closing holes on the initial games moves. Capture mechanisms other than closing holes are not supported. The minimum move must be 1 and thus SOW_START is incompatible.  ALLOW_RULE may not be used to limit allowable moves.  SKIP_START and VISIT_OPP are not supported with SOW_BLKD_DIV.  MLAPS of LAPPER_NEXT is not supported with SOW_BLKD_DIV(_NR).
-- SOW_BLKD_DIV_NR: Behaves the same as SOW_BLKD_DIV except that each player's rightmost hole cannot be closed. 
-- OWN_SOW_CAPT_ALL: The hole OWNer captures all holes that are sown to meet the simple capture criteria no matter who sowed them.  The simple capture criteria are: evens, min, max and capture on. Other criteria are enforced: side of the board, unlocked, and not child.
-  + The capture is done by the hole owner, so the non-sower may capture seeds while their opponents sows. If the game GOAL is TERRITORY the capturer is the hole owner; otherwise each player captures from their own side of the board no matter who is sowing. 
-  + If MLAPS is LAPPER and the final seed sown for any lap meets the simple capture criteria for that hole, the contents of the hole are captured by the sower and not the hole owner and the turn is over. For CAPTTWOOUT, CAPT_NEXT and CROSSCAPT captures, the sower always does the final capture.
-  + GRANDSLAM rules are not applied. NOCAPTMOVES prevents these capture for the first moves.
-- SOW_CAPT_ALL: Similar to OWN_SOW_CAPT_ALL but only the SOWer captures seeds from the side specified by CAPT_SIDE. BOTH sower capturers from any hole. OPP sower capturer only from opponents holes.  OWN sower captures only from their own holes. 
-  + If mlaps is LAPPER and the final seed sown for any lap meets the capture criteria, the contents of the hole are captured by the sower and not the hole owner and the turn is over.
-  + GRANDSLAM rules are not applied. NOCAPTMOVES prevents this capture for the first number of specified moves.
-- NO_SOW_OPP_2S: Don't sow into opponents holes with 2 seeds.
-- CHANGE_DIR_LAP: Change the direction for each lap sown. Generally used with UDIR_HOLES so the player may choose the first direction.
-- MAX_SOW: holes sow_param seeds are skipped when sowing. That is, holes will never contain more seeds than sow_param.
-- LAP_CAPT: after each lapt check for a capture, if there is a capture continue sowing with another lap. If a basic capture is configured (evens, capt on, max or min), the hole after the captured seeds is drawn to continue lapping.</t>
-  </si>
-  <si>
     <t>Allow rules limit the holes from which moves may start.  Disallowed holes are not selectable.
 - NONE: no special rule
 - OPP_OR_EMPTY:  Limit the allowable holes to those that end in an empty hole or reach the opponents side of the board.
@@ -1212,6 +1193,26 @@
 - NO_OPP_RIGHT: children may not be made on the opposite rightmost hole.
   + TB TB TB TB T
   + B TB TB TB TB</t>
+  </si>
+  <si>
+    <t>Special sow rules add additional behavior or restrictions to the sowing phase:
+- NONE: there is no special sowing rule.
+- SOW_BLKD_DIV: If the final seed of an individual sow lands on the opposite side of the board and brings the contents of that hole to goal_param seeds, the hole is closed closed (blocked). In single lap games, the hole's seeds are removed from play. In multilap games, the seeds are used to continue sowing.
+  + When sowing, blocked holes on your own side of the board are skipped  and blocked holes on opponent's side are diverted out of play or captured.
+  +  Game GOAL must be DEPRIVE and all of the associated restrictions apply. NOCAPTMOVES maybe used to prevent closing holes on the initial games moves. Capture mechanisms other than closing holes are not supported. The minimum move must be 1 and thus SOW_START is incompatible.  ALLOW_RULE may not be used to limit allowable moves.  SKIP_START and VISIT_OPP are not supported with SOW_BLKD_DIV.  MLAPS of LAPPER_NEXT is not supported with SOW_BLKD_DIV(_NR).
+- SOW_BLKD_DIV_NR: Behaves the same as SOW_BLKD_DIV except that each player's rightmost hole cannot be closed. 
+- OWN_SOW_CAPT_ALL: The hole OWNer captures all holes that are sown to meet the simple capture criteria no matter who sowed them.  The simple capture criteria are: evens, min, max and capture on. Other criteria are enforced: side of the board, unlocked, and not child.
+  + The capture is done by the hole owner, so the non-sower may capture seeds while their opponents sows. If the game GOAL is TERRITORY the capturer is the hole owner; otherwise each player captures from their own side of the board no matter who is sowing. 
+  + If MLAPS is LAPPER and the final seed sown for any lap meets the simple capture criteria for that hole, the contents of the hole are captured by the sower and not the hole owner and the turn is over. For CAPTTWOOUT, CAPT_NEXT and CROSSCAPT captures, the sower always does the final capture.
+  + GRANDSLAM rules are not applied. NOCAPTMOVES prevents these capture for the first moves.
+- SOW_CAPT_ALL: Similar to OWN_SOW_CAPT_ALL but only the SOWer captures seeds from the side specified by CAPT_SIDE. BOTH sower capturers from any hole. OPP sower capturer only from opponents holes.  OWN sower captures only from their own holes. 
+  + If mlaps is LAPPER and the final seed sown for any lap meets the capture criteria, the contents of the hole are captured by the sower and not the hole owner and the turn is over.
+  + GRANDSLAM rules are not applied. NOCAPTMOVES prevents this capture for the first number of specified moves.
+- NO_SOW_OPP_2S: Don't sow into opponents holes with 2 seeds.
+- CHANGE_DIR_LAP: Change the direction for each lap sown. Generally used with UDIR_HOLES so the player may choose the first direction.
+- MAX_SOW: holes sow_param seeds are skipped when sowing. That is, holes will never contain more seeds than sow_param.
+- LAP_CAPT: after each lapt check for a capture, if there is a capture continue sowing with another lap. If a basic capture is configured (evens, capt on, max or min), the hole after the captured seeds is drawn to continue lapping.
+- NO_OPP_CHILD: do not sow into your opponents children.</t>
   </si>
 </sst>
 </file>
@@ -2095,9 +2096,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:J88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A86" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J88" sqref="J88"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J82" sqref="J82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2878,7 +2879,7 @@
         <v>0</v>
       </c>
       <c r="J25" s="4" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="105" x14ac:dyDescent="0.25">
@@ -3122,7 +3123,7 @@
         <v>0</v>
       </c>
       <c r="J33" s="4" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="34" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3366,7 +3367,7 @@
         <v>2</v>
       </c>
       <c r="J41" s="4" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="42" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -3430,7 +3431,7 @@
         <v>2</v>
       </c>
       <c r="J43" s="4" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -4631,7 +4632,7 @@
         <v>0</v>
       </c>
       <c r="J82" s="4" t="s">
-        <v>308</v>
+        <v>319</v>
       </c>
     </row>
     <row r="83" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -4721,7 +4722,7 @@
         <v>2</v>
       </c>
       <c r="J85" s="4" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="86" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -4785,7 +4786,7 @@
         <v>2</v>
       </c>
       <c r="J87" s="4" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="88" spans="1:10" ht="405" x14ac:dyDescent="0.25">
@@ -4793,10 +4794,10 @@
         <v>66</v>
       </c>
       <c r="B88" s="3" t="s">
+        <v>312</v>
+      </c>
+      <c r="C88" s="3" t="s">
         <v>313</v>
-      </c>
-      <c r="C88" s="3" t="s">
-        <v>314</v>
       </c>
       <c r="D88" s="3" t="s">
         <v>22</v>
@@ -4805,10 +4806,10 @@
         <v>112</v>
       </c>
       <c r="F88" s="3" t="s">
+        <v>314</v>
+      </c>
+      <c r="G88" s="3" t="s">
         <v>315</v>
-      </c>
-      <c r="G88" s="3" t="s">
-        <v>316</v>
       </c>
       <c r="H88" s="3">
         <v>7</v>
@@ -4817,7 +4818,7 @@
         <v>2</v>
       </c>
       <c r="J88" s="4" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Checkpoint before testing new features: Collected capttwoout, capt_next into capt_type enum. Added MATCH_OPP to that enum. Added a random fill start pattern. Added a StopCaptureSimul lap continuer for when the capture mechanism is rather complicated and needs to be simulated (not replicated from the capturer), only used MATCH_OPP captures now. Wrote an adapted version of Mangala_I.
</commit_message>
<xml_diff>
--- a/src/game_params.xlsx
+++ b/src/game_params.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Activity_Data\Mancala_github\MancalaGames\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EA7CD5D-A9A8-4C4F-B266-32A2AB7AB8CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05DBE1F7-D283-4F68-80A9-619D1DECAB01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="game_params" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">game_params!$A$1:$J$88</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">game_params!$A$1:$J$87</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="320">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="318">
   <si>
     <t>tab</t>
   </si>
@@ -390,12 +390,6 @@
   </si>
   <si>
     <t>Capture On Values</t>
-  </si>
-  <si>
-    <t>capttwoout</t>
-  </si>
-  <si>
-    <t>Capture Two Out</t>
   </si>
   <si>
     <t>Player</t>
@@ -545,12 +539,6 @@
   </si>
   <si>
     <t>Repeat Turn on Capture</t>
-  </si>
-  <si>
-    <t>capt_next</t>
-  </si>
-  <si>
-    <t>Capture Next</t>
   </si>
   <si>
     <t>Prescribed Opening Move</t>
@@ -789,13 +777,6 @@
     <t>Stores (captured) Multiplier</t>
   </si>
   <si>
-    <t xml:space="preserve">There are three flavors of capture two out:
-Single lap game: capture if sow ends in occupied hole, then an empty hole, followed by an occupied hole the contents of this are hole captured.
-Multi lap game but single capture: capture when last hole sown is followed by an empty hole which is then followed by an occupied hole.
-Multi lap game with multiple captures: capture when last hole sown is followed by an empty hole which is then followed by an occupied hole. Continue captures as long as the pattern of empty hole followed by an occupied hole continues.
-</t>
-  </si>
-  <si>
     <t>The algorithm value is the name of the AI player algorithm (a string):
 minimaxer: an Alpha-Beta Pruning MiniMaxer
 negamaxer: minimaxer with a very minor optimization for alternating turn games (no repeat turns). Uses minimaxer depths for difficulties.
@@ -1002,10 +983,6 @@
   </si>
   <si>
     <t>mdyno_lbl</t>
-  </si>
-  <si>
-    <t>Capture from the hole after the final seed sown. 
-When multiple lap sowing, the sowing does not stop for captures. Instead, sowing continues until the final seed is sown into an empty hole. Then the capture test is made on the next hole.</t>
   </si>
   <si>
     <t>An int to describe possible multicaptures:
@@ -1213,6 +1190,25 @@
 - MAX_SOW: holes sow_param seeds are skipped when sowing. That is, holes will never contain more seeds than sow_param.
 - LAP_CAPT: after each lapt check for a capture, if there is a capture continue sowing with another lap. If a basic capture is configured (evens, capt on, max or min), the hole after the captured seeds is drawn to continue lapping.
 - NO_OPP_CHILD: do not sow into your opponents children.</t>
+  </si>
+  <si>
+    <t>capt_type</t>
+  </si>
+  <si>
+    <t>Capture Type</t>
+  </si>
+  <si>
+    <t>CaptType</t>
+  </si>
+  <si>
+    <t>Capture type.  Basic capture rules are not applied and are incompatible with cross capture.
+- NEXT: Capture from the hole after the final seed sown. 
+  + When multiple lap sowing, the sowing does not stop for captures. Instead, sowing continues until the final seed is sown into an empty hole. Then the capture test is made on the next hole.
+- TWO_OUT: There are three flavors of capture two out:
+  + Single lap game: capture if sow ends in occupied hole, then an empty hole, followed by an occupied hole the contents of this are hole captured.
+  + Multi lap game but single capture: capture when last hole sown is followed by an empty hole which is then followed by an occupied hole.
+  + Multi lap game with multiple captures: capture when last hole sown is followed by an empty hole which is then followed by an occupied hole. Continue captures as long as the pattern of empty hole followed by an occupied hole continues.
+- MATCH_OPP: capture when the number of seeds in the final hole sown match the oppocite hole.</t>
   </si>
 </sst>
 </file>
@@ -2094,11 +2090,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:J88"/>
+  <dimension ref="A1:J87"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J82" sqref="J82"/>
+      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2130,7 +2126,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>4</v>
@@ -2153,17 +2149,17 @@
         <v>90</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3">
         <v>0</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="G2" s="5" t="s">
         <v>84</v>
@@ -2205,7 +2201,7 @@
         <v>0</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -2237,7 +2233,7 @@
         <v>0</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -2269,7 +2265,7 @@
         <v>0</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -2289,7 +2285,7 @@
         <v>107</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="G6" s="5" t="s">
         <v>88</v>
@@ -2301,7 +2297,7 @@
         <v>0</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -2309,16 +2305,16 @@
         <v>90</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="E7" s="3">
         <v>0</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="G7" s="5" t="s">
         <v>84</v>
@@ -2359,7 +2355,7 @@
         <v>0</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -2391,7 +2387,7 @@
         <v>0</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2399,10 +2395,10 @@
         <v>90</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>22</v>
@@ -2423,7 +2419,7 @@
         <v>0</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -2431,19 +2427,19 @@
         <v>90</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="E11" s="3">
         <v>0</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="H11" s="3">
         <v>9</v>
@@ -2452,15 +2448,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="150" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>90</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>169</v>
+        <v>314</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>170</v>
+        <v>315</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>22</v>
@@ -2469,10 +2465,10 @@
         <v>106</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>39</v>
+        <v>316</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>40</v>
+        <v>159</v>
       </c>
       <c r="H12" s="3">
         <v>10</v>
@@ -2481,129 +2477,123 @@
         <v>0</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>90</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>118</v>
+        <v>273</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>22</v>
+        <v>111</v>
       </c>
       <c r="E13" s="3">
-        <v>109</v>
+        <v>0</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>39</v>
+        <v>255</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>40</v>
+        <v>84</v>
       </c>
       <c r="H13" s="3">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="I13" s="3">
-        <v>0</v>
-      </c>
-      <c r="J13" s="4" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>90</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>278</v>
+        <v>110</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>111</v>
       </c>
+      <c r="D14" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="E14" s="3">
-        <v>0</v>
+        <v>124</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>260</v>
+        <v>11</v>
       </c>
       <c r="G14" s="5" t="s">
         <v>84</v>
       </c>
       <c r="H14" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I14" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+      <c r="J14" s="4" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>90</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>110</v>
+        <v>91</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>111</v>
+        <v>92</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E15" s="3">
-        <v>124</v>
+        <v>103</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>84</v>
+        <v>40</v>
       </c>
       <c r="H15" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I15" s="3">
         <v>2</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>90</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>91</v>
+        <v>269</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>22</v>
+        <v>280</v>
       </c>
       <c r="E16" s="3">
-        <v>103</v>
+        <v>0</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>39</v>
+        <v>255</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>40</v>
+        <v>84</v>
       </c>
       <c r="H16" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I16" s="3">
         <v>2</v>
-      </c>
-      <c r="J16" s="4" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
@@ -2611,106 +2601,112 @@
         <v>90</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>274</v>
+        <v>250</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>285</v>
+        <v>270</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="E17" s="3">
-        <v>0</v>
+        <v>128</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>260</v>
+        <v>11</v>
       </c>
       <c r="G17" s="5" t="s">
         <v>84</v>
       </c>
       <c r="H17" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I17" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J17" s="4" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>90</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>255</v>
+        <v>293</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>275</v>
+        <v>294</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E18" s="3">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>11</v>
+        <v>295</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>84</v>
+        <v>296</v>
       </c>
       <c r="H18" s="3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I18" s="3">
         <v>2</v>
       </c>
       <c r="J18" s="4" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>90</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>299</v>
+        <v>101</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>300</v>
+        <v>102</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E19" s="3">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>301</v>
+        <v>39</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>302</v>
+        <v>40</v>
       </c>
       <c r="H19" s="3">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I19" s="3">
         <v>2</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>90</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E20" s="3">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="F20" s="3" t="s">
         <v>39</v>
@@ -2719,45 +2715,39 @@
         <v>40</v>
       </c>
       <c r="H20" s="3">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I20" s="3">
         <v>2</v>
       </c>
       <c r="J20" s="4" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>90</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>93</v>
+        <v>271</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>22</v>
+        <v>272</v>
       </c>
       <c r="E21" s="3">
-        <v>123</v>
+        <v>0</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>39</v>
+        <v>255</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>40</v>
+        <v>84</v>
       </c>
       <c r="H21" s="3">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I21" s="3">
         <v>2</v>
-      </c>
-      <c r="J21" s="4" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
@@ -2765,275 +2755,275 @@
         <v>90</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>276</v>
+        <v>165</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>277</v>
+        <v>166</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="E22" s="3">
-        <v>0</v>
+        <v>108</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>260</v>
+        <v>39</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>84</v>
+        <v>40</v>
       </c>
       <c r="H22" s="3">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="I22" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J22" s="4" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="135" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>90</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>167</v>
+        <v>173</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>168</v>
+        <v>175</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E23" s="3">
-        <v>108</v>
+        <v>131</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>39</v>
+        <v>174</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>40</v>
+        <v>159</v>
       </c>
       <c r="H23" s="3">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I23" s="3">
         <v>2</v>
       </c>
       <c r="J23" s="4" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" ht="135" x14ac:dyDescent="0.25">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>90</v>
+        <v>36</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>177</v>
+        <v>52</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>179</v>
+        <v>53</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E24" s="3">
-        <v>131</v>
+        <v>115</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>178</v>
+        <v>54</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>161</v>
+        <v>55</v>
       </c>
       <c r="H24" s="3">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="I24" s="3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J24" s="4" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" ht="409.5" x14ac:dyDescent="0.25">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>36</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>52</v>
+        <v>247</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>53</v>
+        <v>249</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E25" s="3">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>54</v>
+        <v>11</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>55</v>
+        <v>84</v>
       </c>
       <c r="H25" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I25" s="3">
         <v>0</v>
       </c>
       <c r="J25" s="4" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" ht="105" x14ac:dyDescent="0.25">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>36</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>252</v>
+        <v>288</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>254</v>
+        <v>289</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E26" s="3">
-        <v>116</v>
+        <v>147</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>11</v>
+        <v>290</v>
       </c>
       <c r="G26" s="5" t="s">
-        <v>84</v>
+        <v>291</v>
       </c>
       <c r="H26" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I26" s="3">
         <v>0</v>
       </c>
       <c r="J26" s="4" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" ht="120" x14ac:dyDescent="0.25">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>36</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>294</v>
+        <v>282</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>295</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>22</v>
+        <v>256</v>
       </c>
       <c r="E27" s="3">
-        <v>147</v>
+        <v>0</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>296</v>
+        <v>255</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>297</v>
+        <v>84</v>
       </c>
       <c r="H27" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I27" s="3">
         <v>0</v>
       </c>
-      <c r="J27" s="4" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:10" ht="150" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>36</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>287</v>
+        <v>56</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>261</v>
+        <v>57</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="E28" s="3">
-        <v>0</v>
+        <v>143</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>260</v>
+        <v>58</v>
       </c>
       <c r="G28" s="5" t="s">
-        <v>84</v>
+        <v>59</v>
       </c>
       <c r="H28" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I28" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:10" ht="150" x14ac:dyDescent="0.25">
+      <c r="J28" s="4" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="180" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>36</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>56</v>
+        <v>168</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>57</v>
+        <v>167</v>
       </c>
       <c r="D29" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E29" s="3">
-        <v>143</v>
+        <v>132</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>58</v>
+        <v>169</v>
       </c>
       <c r="G29" s="5" t="s">
-        <v>59</v>
+        <v>159</v>
       </c>
       <c r="H29" s="3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I29" s="3">
         <v>0</v>
       </c>
       <c r="J29" s="4" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" ht="180" x14ac:dyDescent="0.25">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>36</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>172</v>
+        <v>283</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>22</v>
+        <v>284</v>
       </c>
       <c r="E30" s="3">
-        <v>132</v>
+        <v>0</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>173</v>
+        <v>255</v>
       </c>
       <c r="G30" s="5" t="s">
-        <v>161</v>
+        <v>84</v>
       </c>
       <c r="H30" s="3">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="I30" s="3">
         <v>0</v>
-      </c>
-      <c r="J30" s="4" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
@@ -3041,121 +3031,127 @@
         <v>36</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>288</v>
+        <v>60</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>289</v>
+        <v>61</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="E31" s="3">
-        <v>0</v>
+        <v>119</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>260</v>
+        <v>11</v>
       </c>
       <c r="G31" s="5" t="s">
-        <v>84</v>
+        <v>62</v>
       </c>
       <c r="H31" s="3">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I31" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J31" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" ht="225" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>36</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>60</v>
+        <v>156</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>61</v>
+        <v>157</v>
       </c>
       <c r="D32" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E32" s="3">
-        <v>119</v>
+        <v>101</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>11</v>
+        <v>158</v>
       </c>
       <c r="G32" s="5" t="s">
-        <v>62</v>
+        <v>159</v>
       </c>
       <c r="H32" s="3">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="I32" s="3">
         <v>0</v>
       </c>
       <c r="J32" s="4" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" ht="225" x14ac:dyDescent="0.25">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>36</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>158</v>
+        <v>49</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>159</v>
+        <v>50</v>
       </c>
       <c r="D33" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E33" s="3">
-        <v>101</v>
+        <v>144</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>160</v>
+        <v>39</v>
       </c>
       <c r="G33" s="5" t="s">
-        <v>161</v>
+        <v>51</v>
       </c>
       <c r="H33" s="3">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="I33" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J33" s="4" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>36</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D34" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E34" s="3">
-        <v>144</v>
+        <v>127</v>
       </c>
       <c r="F34" s="3" t="s">
         <v>39</v>
       </c>
       <c r="G34" s="5" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="H34" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I34" s="3">
         <v>2</v>
       </c>
       <c r="J34" s="4" t="s">
-        <v>249</v>
+        <v>222</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
@@ -3163,57 +3159,57 @@
         <v>36</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>47</v>
+        <v>286</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="D35" s="3" t="s">
-        <v>22</v>
+        <v>285</v>
       </c>
       <c r="E35" s="3">
-        <v>127</v>
+        <v>0</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>39</v>
+        <v>255</v>
       </c>
       <c r="G35" s="5" t="s">
-        <v>40</v>
+        <v>84</v>
       </c>
       <c r="H35" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I35" s="3">
         <v>2</v>
       </c>
-      <c r="J35" s="4" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>36</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>291</v>
+        <v>37</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>290</v>
+        <v>38</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="E36" s="3">
-        <v>0</v>
+        <v>125</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>260</v>
+        <v>39</v>
       </c>
       <c r="G36" s="5" t="s">
-        <v>84</v>
+        <v>40</v>
       </c>
       <c r="H36" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I36" s="3">
         <v>2</v>
+      </c>
+      <c r="J36" s="4" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="37" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3221,16 +3217,16 @@
         <v>36</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>37</v>
+        <v>64</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>38</v>
+        <v>65</v>
       </c>
       <c r="D37" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E37" s="3">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="F37" s="3" t="s">
         <v>39</v>
@@ -3239,263 +3235,263 @@
         <v>40</v>
       </c>
       <c r="H37" s="3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I37" s="3">
         <v>2</v>
       </c>
       <c r="J37" s="4" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" ht="150" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>36</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>64</v>
+        <v>112</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>65</v>
+        <v>113</v>
       </c>
       <c r="D38" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E38" s="3">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>39</v>
+        <v>114</v>
       </c>
       <c r="G38" s="5" t="s">
-        <v>40</v>
+        <v>115</v>
       </c>
       <c r="H38" s="3">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I38" s="3">
         <v>2</v>
       </c>
       <c r="J38" s="4" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" ht="150" x14ac:dyDescent="0.25">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>36</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>112</v>
+        <v>257</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="D39" s="3" t="s">
-        <v>22</v>
+        <v>281</v>
       </c>
       <c r="E39" s="3">
-        <v>117</v>
+        <v>0</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>114</v>
+        <v>255</v>
       </c>
       <c r="G39" s="5" t="s">
-        <v>115</v>
+        <v>84</v>
       </c>
       <c r="H39" s="3">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I39" s="3">
         <v>2</v>
       </c>
-      <c r="J39" s="4" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:10" ht="240" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>36</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>262</v>
+        <v>41</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>286</v>
+        <v>42</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="E40" s="3">
-        <v>0</v>
+        <v>136</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>260</v>
+        <v>42</v>
       </c>
       <c r="G40" s="5" t="s">
-        <v>84</v>
+        <v>242</v>
       </c>
       <c r="H40" s="3">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I40" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="41" spans="1:10" ht="240" x14ac:dyDescent="0.25">
+      <c r="J40" s="4" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>36</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D41" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E41" s="3">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="G41" s="5" t="s">
-        <v>247</v>
+        <v>46</v>
       </c>
       <c r="H41" s="3">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="I41" s="3">
         <v>2</v>
       </c>
       <c r="J41" s="4" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" ht="345" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>36</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>43</v>
+        <v>178</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>44</v>
+        <v>179</v>
       </c>
       <c r="D42" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E42" s="3">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>45</v>
+        <v>180</v>
       </c>
       <c r="G42" s="5" t="s">
-        <v>46</v>
+        <v>187</v>
       </c>
       <c r="H42" s="3">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I42" s="3">
         <v>2</v>
       </c>
       <c r="J42" s="4" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" ht="345" x14ac:dyDescent="0.25">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>36</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>182</v>
+        <v>79</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>183</v>
+        <v>80</v>
       </c>
       <c r="D43" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E43" s="3">
-        <v>134</v>
+        <v>102</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>184</v>
+        <v>39</v>
       </c>
       <c r="G43" s="5" t="s">
-        <v>191</v>
+        <v>40</v>
       </c>
       <c r="H43" s="3">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I43" s="3">
         <v>2</v>
       </c>
       <c r="J43" s="4" t="s">
-        <v>311</v>
+        <v>246</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
-        <v>36</v>
+        <v>15</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>79</v>
+        <v>17</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>80</v>
+        <v>16</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="E44" s="3">
-        <v>102</v>
+        <v>1</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>39</v>
+        <v>134</v>
       </c>
       <c r="G44" s="5" t="s">
-        <v>40</v>
+        <v>19</v>
       </c>
       <c r="H44" s="3">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="I44" s="3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J44" s="4" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="E45" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>136</v>
+        <v>11</v>
       </c>
       <c r="G45" s="5" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="H45" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I45" s="3">
         <v>0</v>
       </c>
       <c r="J45" s="4" t="s">
-        <v>248</v>
+        <v>193</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
@@ -3503,484 +3499,484 @@
         <v>15</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="E46" s="3">
-        <v>2</v>
+        <v>118</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="G46" s="5" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="H46" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I46" s="3">
         <v>0</v>
       </c>
       <c r="J46" s="4" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D47" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E47" s="3">
-        <v>118</v>
+        <v>5</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G47" s="5" t="s">
-        <v>25</v>
+        <v>28</v>
+      </c>
+      <c r="G47" s="6" t="s">
+        <v>132</v>
       </c>
       <c r="H47" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I47" s="3">
         <v>0</v>
       </c>
       <c r="J47" s="4" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D48" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E48" s="3">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F48" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="G48" s="6" t="s">
-        <v>134</v>
+        <v>18</v>
+      </c>
+      <c r="G48" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="H48" s="3">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I48" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J48" s="4" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="E49" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="G49" s="5" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="H49" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I49" s="3">
         <v>2</v>
       </c>
       <c r="J49" s="4" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
-        <v>15</v>
+        <v>118</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>33</v>
+        <v>135</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>34</v>
+        <v>136</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>31</v>
+        <v>131</v>
       </c>
       <c r="E50" s="3">
-        <v>3</v>
+        <v>201</v>
       </c>
       <c r="F50" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="G50" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="H50" s="3">
+        <v>0</v>
+      </c>
+      <c r="I50" s="3">
+        <v>0</v>
+      </c>
+      <c r="J50" s="4" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A51" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="E51" s="3">
+        <v>203</v>
+      </c>
+      <c r="F51" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G50" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="H50" s="3">
-        <v>2</v>
-      </c>
-      <c r="I50" s="3">
-        <v>2</v>
-      </c>
-      <c r="J50" s="4" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A51" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="B51" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="C51" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="D51" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="E51" s="3">
+      <c r="G51" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="H51" s="3">
+        <v>1</v>
+      </c>
+      <c r="I51" s="3">
+        <v>0</v>
+      </c>
+      <c r="J51" s="4" t="s">
         <v>201</v>
-      </c>
-      <c r="F51" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="G51" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="H51" s="3">
-        <v>0</v>
-      </c>
-      <c r="I51" s="3">
-        <v>0</v>
-      </c>
-      <c r="J51" s="4" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B52" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="D52" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="C52" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="D52" s="3" t="s">
-        <v>133</v>
-      </c>
       <c r="E52" s="3">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F52" s="3" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
       <c r="G52" s="5" t="s">
-        <v>62</v>
+        <v>40</v>
       </c>
       <c r="H52" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I52" s="3">
         <v>0</v>
       </c>
       <c r="J52" s="4" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>187</v>
+        <v>260</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>185</v>
-      </c>
-      <c r="D53" s="3" t="s">
-        <v>133</v>
+        <v>259</v>
       </c>
       <c r="E53" s="3">
-        <v>202</v>
+        <v>0</v>
       </c>
       <c r="F53" s="3" t="s">
-        <v>39</v>
+        <v>255</v>
       </c>
       <c r="G53" s="5" t="s">
-        <v>40</v>
+        <v>84</v>
       </c>
       <c r="H53" s="3">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="I53" s="3">
         <v>0</v>
       </c>
-      <c r="J53" s="4" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="54" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>265</v>
+        <v>142</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>264</v>
+        <v>146</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>141</v>
       </c>
       <c r="E54" s="3">
-        <v>0</v>
+        <v>210</v>
       </c>
       <c r="F54" s="3" t="s">
-        <v>260</v>
-      </c>
-      <c r="G54" s="5" t="s">
-        <v>84</v>
+        <v>87</v>
+      </c>
+      <c r="G54" s="3" t="s">
+        <v>236</v>
       </c>
       <c r="H54" s="3">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I54" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="55" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="J54" s="4" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E55" s="3">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="F55" s="3" t="s">
         <v>87</v>
       </c>
       <c r="G55" s="3" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="H55" s="3">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I55" s="3">
         <v>0</v>
       </c>
       <c r="J55" s="4" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C56" s="3" t="s">
         <v>147</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E56" s="3">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="F56" s="3" t="s">
         <v>87</v>
       </c>
       <c r="G56" s="3" t="s">
-        <v>239</v>
+        <v>148</v>
       </c>
       <c r="H56" s="3">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I56" s="3">
         <v>0</v>
       </c>
       <c r="J56" s="4" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>146</v>
+        <v>258</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="D57" s="3" t="s">
-        <v>143</v>
+        <v>261</v>
       </c>
       <c r="E57" s="3">
-        <v>212</v>
+        <v>0</v>
       </c>
       <c r="F57" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="G57" s="3" t="s">
-        <v>150</v>
+        <v>255</v>
+      </c>
+      <c r="G57" s="5" t="s">
+        <v>84</v>
       </c>
       <c r="H57" s="3">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="I57" s="3">
-        <v>0</v>
-      </c>
-      <c r="J57" s="4" t="s">
-        <v>202</v>
+        <v>2</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>263</v>
+        <v>139</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>266</v>
+        <v>140</v>
+      </c>
+      <c r="D58" s="3" t="s">
+        <v>141</v>
       </c>
       <c r="E58" s="3">
-        <v>0</v>
+        <v>213</v>
       </c>
       <c r="F58" s="3" t="s">
-        <v>260</v>
-      </c>
-      <c r="G58" s="5" t="s">
-        <v>84</v>
+        <v>87</v>
+      </c>
+      <c r="G58" s="3" t="s">
+        <v>235</v>
       </c>
       <c r="H58" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I58" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J58" s="4" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="D59" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="B59" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="C59" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="D59" s="3" t="s">
-        <v>143</v>
-      </c>
       <c r="E59" s="3">
-        <v>213</v>
+        <v>220</v>
       </c>
       <c r="F59" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="G59" s="3" t="s">
-        <v>240</v>
+        <v>11</v>
+      </c>
+      <c r="G59" s="5" t="s">
+        <v>35</v>
       </c>
       <c r="H59" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I59" s="3">
         <v>2</v>
       </c>
       <c r="J59" s="4" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="60" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B60" s="3" t="s">
         <v>121</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E60" s="3">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="F60" s="3" t="s">
         <v>11</v>
       </c>
       <c r="G60" s="5" t="s">
-        <v>35</v>
+        <v>84</v>
       </c>
       <c r="H60" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I60" s="3">
         <v>2</v>
       </c>
       <c r="J60" s="4" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="61" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="C61" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="D61" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="B61" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="C61" s="3" t="s">
-        <v>233</v>
-      </c>
-      <c r="D61" s="3" t="s">
-        <v>122</v>
-      </c>
       <c r="E61" s="3">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="F61" s="3" t="s">
         <v>11</v>
@@ -3989,30 +3985,30 @@
         <v>84</v>
       </c>
       <c r="H61" s="3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I61" s="3">
         <v>2</v>
       </c>
       <c r="J61" s="4" t="s">
-        <v>211</v>
+        <v>219</v>
       </c>
     </row>
     <row r="62" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="C62" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="D62" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="B62" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="C62" s="3" t="s">
-        <v>232</v>
-      </c>
-      <c r="D62" s="3" t="s">
-        <v>122</v>
-      </c>
       <c r="E62" s="3">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="F62" s="3" t="s">
         <v>11</v>
@@ -4021,30 +4017,30 @@
         <v>84</v>
       </c>
       <c r="H62" s="3">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I62" s="3">
         <v>2</v>
       </c>
       <c r="J62" s="4" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="63" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="C63" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="D63" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="B63" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="C63" s="3" t="s">
-        <v>231</v>
-      </c>
-      <c r="D63" s="3" t="s">
-        <v>122</v>
-      </c>
       <c r="E63" s="3">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="F63" s="3" t="s">
         <v>11</v>
@@ -4053,30 +4049,30 @@
         <v>84</v>
       </c>
       <c r="H63" s="3">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I63" s="3">
         <v>2</v>
       </c>
       <c r="J63" s="4" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
     </row>
     <row r="64" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="C64" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="D64" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="B64" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="C64" s="3" t="s">
-        <v>230</v>
-      </c>
-      <c r="D64" s="3" t="s">
-        <v>122</v>
-      </c>
       <c r="E64" s="3">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="F64" s="3" t="s">
         <v>11</v>
@@ -4085,30 +4081,30 @@
         <v>84</v>
       </c>
       <c r="H64" s="3">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I64" s="3">
         <v>2</v>
       </c>
       <c r="J64" s="4" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="65" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="C65" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="D65" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="B65" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="C65" s="3" t="s">
-        <v>229</v>
-      </c>
-      <c r="D65" s="3" t="s">
-        <v>122</v>
-      </c>
       <c r="E65" s="3">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="F65" s="3" t="s">
         <v>11</v>
@@ -4117,7 +4113,7 @@
         <v>84</v>
       </c>
       <c r="H65" s="3">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="I65" s="3">
         <v>2</v>
@@ -4128,19 +4124,19 @@
     </row>
     <row r="66" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="C66" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="D66" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="B66" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="C66" s="3" t="s">
-        <v>250</v>
-      </c>
-      <c r="D66" s="3" t="s">
-        <v>122</v>
-      </c>
       <c r="E66" s="3">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="F66" s="3" t="s">
         <v>11</v>
@@ -4149,45 +4145,39 @@
         <v>84</v>
       </c>
       <c r="H66" s="3">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I66" s="3">
         <v>2</v>
       </c>
       <c r="J66" s="4" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="67" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
-        <v>120</v>
+        <v>9</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="C67" s="3" t="s">
-        <v>129</v>
+        <v>162</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>122</v>
+        <v>22</v>
       </c>
       <c r="E67" s="3">
-        <v>227</v>
+        <v>121</v>
       </c>
       <c r="F67" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G67" s="5" t="s">
-        <v>84</v>
-      </c>
       <c r="H67" s="3">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="I67" s="3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J67" s="4" t="s">
-        <v>207</v>
+        <v>164</v>
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.25">
@@ -4195,17 +4185,18 @@
         <v>9</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>164</v>
+        <v>89</v>
       </c>
       <c r="D68" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E68" s="3">
-        <v>121</v>
+        <v>146</v>
       </c>
       <c r="F68" s="3" t="s">
-        <v>11</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="G68" s="5"/>
       <c r="H68" s="3">
         <v>0</v>
       </c>
@@ -4213,7 +4204,7 @@
         <v>0</v>
       </c>
       <c r="J68" s="4" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.25">
@@ -4221,18 +4212,14 @@
         <v>9</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="D69" s="3" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="E69" s="3">
-        <v>146</v>
+        <v>500</v>
       </c>
       <c r="F69" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="G69" s="5"/>
+        <v>14</v>
+      </c>
       <c r="H69" s="3">
         <v>0</v>
       </c>
@@ -4240,7 +4227,7 @@
         <v>0</v>
       </c>
       <c r="J69" s="4" t="s">
-        <v>165</v>
+        <v>133</v>
       </c>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.25">
@@ -4248,13 +4235,13 @@
         <v>9</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E70" s="3">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="F70" s="3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="H70" s="3">
         <v>0</v>
@@ -4263,21 +4250,30 @@
         <v>0</v>
       </c>
       <c r="J70" s="4" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" ht="165" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
-        <v>9</v>
+        <v>66</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>10</v>
+        <v>81</v>
+      </c>
+      <c r="C71" s="3" t="s">
+        <v>275</v>
+      </c>
+      <c r="D71" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="E71" s="3">
-        <v>501</v>
+        <v>120</v>
       </c>
       <c r="F71" s="3" t="s">
-        <v>11</v>
+        <v>160</v>
+      </c>
+      <c r="G71" s="5" t="s">
+        <v>161</v>
       </c>
       <c r="H71" s="3">
         <v>0</v>
@@ -4285,8 +4281,8 @@
       <c r="I71" s="3">
         <v>0</v>
       </c>
-      <c r="J71" s="4" t="s">
-        <v>12</v>
+      <c r="J71" s="8" t="s">
+        <v>232</v>
       </c>
     </row>
     <row r="72" spans="1:10" ht="165" x14ac:dyDescent="0.25">
@@ -4294,95 +4290,89 @@
         <v>66</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>280</v>
+        <v>68</v>
       </c>
       <c r="D72" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E72" s="3">
-        <v>120</v>
+        <v>138</v>
       </c>
       <c r="F72" s="3" t="s">
-        <v>162</v>
+        <v>69</v>
       </c>
       <c r="G72" s="5" t="s">
-        <v>163</v>
+        <v>70</v>
       </c>
       <c r="H72" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I72" s="3">
         <v>0</v>
       </c>
-      <c r="J72" s="8" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="73" spans="1:10" ht="165" x14ac:dyDescent="0.25">
+      <c r="J72" s="4" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
         <v>66</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>67</v>
+        <v>85</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>68</v>
+        <v>86</v>
       </c>
       <c r="D73" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E73" s="3">
+        <v>145</v>
+      </c>
+      <c r="F73" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="F73" s="3" t="s">
-        <v>69</v>
-      </c>
       <c r="G73" s="5" t="s">
-        <v>70</v>
+        <v>88</v>
       </c>
       <c r="H73" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I73" s="3">
         <v>0</v>
       </c>
       <c r="J73" s="4" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="74" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
         <v>66</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>85</v>
+        <v>278</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="D74" s="3" t="s">
-        <v>22</v>
+        <v>279</v>
       </c>
       <c r="E74" s="3">
-        <v>145</v>
+        <v>0</v>
       </c>
       <c r="F74" s="3" t="s">
-        <v>140</v>
+        <v>255</v>
       </c>
       <c r="G74" s="5" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="H74" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I74" s="3">
         <v>0</v>
-      </c>
-      <c r="J74" s="4" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.25">
@@ -4390,42 +4380,48 @@
         <v>66</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>283</v>
+        <v>71</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>284</v>
+        <v>72</v>
+      </c>
+      <c r="D75" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="E75" s="3">
-        <v>0</v>
+        <v>141</v>
       </c>
       <c r="F75" s="3" t="s">
-        <v>260</v>
+        <v>39</v>
       </c>
       <c r="G75" s="5" t="s">
-        <v>84</v>
+        <v>40</v>
       </c>
       <c r="H75" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I75" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J75" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
         <v>66</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>72</v>
+        <v>274</v>
       </c>
       <c r="D76" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E76" s="3">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="F76" s="3" t="s">
         <v>39</v>
@@ -4434,13 +4430,13 @@
         <v>40</v>
       </c>
       <c r="H76" s="3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I76" s="3">
         <v>0</v>
       </c>
       <c r="J76" s="4" t="s">
-        <v>73</v>
+        <v>218</v>
       </c>
     </row>
     <row r="77" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -4448,16 +4444,16 @@
         <v>66</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>279</v>
+        <v>78</v>
       </c>
       <c r="D77" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E77" s="3">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="F77" s="3" t="s">
         <v>39</v>
@@ -4466,13 +4462,13 @@
         <v>40</v>
       </c>
       <c r="H77" s="3">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I77" s="3">
         <v>0</v>
       </c>
       <c r="J77" s="4" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
     </row>
     <row r="78" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -4480,16 +4476,16 @@
         <v>66</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D78" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E78" s="3">
-        <v>139</v>
+        <v>122</v>
       </c>
       <c r="F78" s="3" t="s">
         <v>39</v>
@@ -4498,30 +4494,30 @@
         <v>40</v>
       </c>
       <c r="H78" s="3">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I78" s="3">
         <v>0</v>
       </c>
       <c r="J78" s="4" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="79" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="s">
         <v>66</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="D79" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E79" s="3">
-        <v>122</v>
+        <v>148</v>
       </c>
       <c r="F79" s="3" t="s">
         <v>39</v>
@@ -4530,309 +4526,277 @@
         <v>40</v>
       </c>
       <c r="H79" s="3">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I79" s="3">
         <v>0</v>
       </c>
       <c r="J79" s="4" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="s">
         <v>66</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>82</v>
+        <v>298</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>83</v>
+        <v>299</v>
       </c>
       <c r="D80" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E80" s="3">
-        <v>148</v>
+        <v>133</v>
       </c>
       <c r="F80" s="3" t="s">
-        <v>39</v>
+        <v>300</v>
       </c>
       <c r="G80" s="5" t="s">
-        <v>40</v>
+        <v>159</v>
       </c>
       <c r="H80" s="3">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="I80" s="3">
         <v>0</v>
       </c>
       <c r="J80" s="4" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="81" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A81" s="3" t="s">
         <v>66</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>304</v>
+        <v>170</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>305</v>
+        <v>171</v>
       </c>
       <c r="D81" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E81" s="3">
-        <v>133</v>
+        <v>140</v>
       </c>
       <c r="F81" s="3" t="s">
-        <v>306</v>
+        <v>172</v>
       </c>
       <c r="G81" s="5" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="H81" s="3">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I81" s="3">
         <v>0</v>
       </c>
       <c r="J81" s="4" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="82" spans="1:10" ht="409.5" x14ac:dyDescent="0.25">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A82" s="3" t="s">
         <v>66</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>174</v>
+        <v>252</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>175</v>
+        <v>253</v>
       </c>
       <c r="D82" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E82" s="3">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="F82" s="3" t="s">
-        <v>176</v>
+        <v>11</v>
       </c>
       <c r="G82" s="5" t="s">
-        <v>161</v>
+        <v>84</v>
       </c>
       <c r="H82" s="3">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I82" s="3">
         <v>0</v>
       </c>
       <c r="J82" s="4" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="83" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" s="3" t="s">
         <v>66</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>257</v>
+        <v>276</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>258</v>
-      </c>
-      <c r="D83" s="3" t="s">
-        <v>22</v>
+        <v>277</v>
       </c>
       <c r="E83" s="3">
-        <v>142</v>
+        <v>0</v>
       </c>
       <c r="F83" s="3" t="s">
-        <v>11</v>
+        <v>255</v>
       </c>
       <c r="G83" s="5" t="s">
         <v>84</v>
       </c>
       <c r="H83" s="3">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="I83" s="3">
-        <v>0</v>
-      </c>
-      <c r="J83" s="4" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" ht="330" x14ac:dyDescent="0.25">
       <c r="A84" s="3" t="s">
         <v>66</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>281</v>
+        <v>151</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>282</v>
+        <v>152</v>
+      </c>
+      <c r="D84" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="E84" s="3">
-        <v>0</v>
+        <v>112</v>
       </c>
       <c r="F84" s="3" t="s">
-        <v>260</v>
+        <v>154</v>
       </c>
       <c r="G84" s="5" t="s">
-        <v>84</v>
+        <v>153</v>
       </c>
       <c r="H84" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I84" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="85" spans="1:10" ht="330" x14ac:dyDescent="0.25">
+      <c r="J84" s="4" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A85" s="3" t="s">
         <v>66</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="D85" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E85" s="3">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F85" s="3" t="s">
-        <v>156</v>
+        <v>11</v>
       </c>
       <c r="G85" s="5" t="s">
-        <v>155</v>
+        <v>84</v>
       </c>
       <c r="H85" s="3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I85" s="3">
         <v>2</v>
       </c>
       <c r="J85" s="4" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="86" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A86" s="3" t="s">
         <v>66</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>151</v>
+        <v>184</v>
       </c>
       <c r="C86" s="3" t="s">
-        <v>152</v>
+        <v>185</v>
       </c>
       <c r="D86" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E86" s="3">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F86" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G86" s="5" t="s">
-        <v>84</v>
+        <v>186</v>
+      </c>
+      <c r="G86" s="3" t="s">
+        <v>159</v>
       </c>
       <c r="H86" s="3">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I86" s="3">
         <v>2</v>
       </c>
       <c r="J86" s="4" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="87" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" ht="405" x14ac:dyDescent="0.25">
       <c r="A87" s="3" t="s">
         <v>66</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>188</v>
+        <v>306</v>
       </c>
       <c r="C87" s="3" t="s">
-        <v>189</v>
+        <v>307</v>
       </c>
       <c r="D87" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E87" s="3">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F87" s="3" t="s">
-        <v>190</v>
+        <v>308</v>
       </c>
       <c r="G87" s="3" t="s">
-        <v>161</v>
+        <v>309</v>
       </c>
       <c r="H87" s="3">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I87" s="3">
         <v>2</v>
       </c>
       <c r="J87" s="4" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="88" spans="1:10" ht="405" x14ac:dyDescent="0.25">
-      <c r="A88" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="B88" s="3" t="s">
         <v>312</v>
       </c>
-      <c r="C88" s="3" t="s">
-        <v>313</v>
-      </c>
-      <c r="D88" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E88" s="3">
-        <v>112</v>
-      </c>
-      <c r="F88" s="3" t="s">
-        <v>314</v>
-      </c>
-      <c r="G88" s="3" t="s">
-        <v>315</v>
-      </c>
-      <c r="H88" s="3">
-        <v>7</v>
-      </c>
-      <c r="I88" s="3">
-        <v>2</v>
-      </c>
-      <c r="J88" s="4" t="s">
-        <v>318</v>
-      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J88" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J87">
-      <sortCondition ref="A2:A87"/>
-      <sortCondition ref="I2:I87"/>
-      <sortCondition ref="H2:H87"/>
+  <autoFilter ref="A1:J87" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J86">
+      <sortCondition ref="A2:A86"/>
+      <sortCondition ref="I2:I86"/>
+      <sortCondition ref="H2:H86"/>
     </sortState>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:J88">
-    <sortCondition ref="A3:A88"/>
-    <sortCondition ref="I3:I88"/>
-    <sortCondition ref="H3:H88"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:J87">
+    <sortCondition ref="A3:A87"/>
+    <sortCondition ref="I3:I87"/>
+    <sortCondition ref="H3:H87"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added multicapt option to MATCH_OPP. Tested fill_pattern, sower and capturer.
</commit_message>
<xml_diff>
--- a/src/game_params.xlsx
+++ b/src/game_params.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Activity_Data\Mancala_github\MancalaGames\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05DBE1F7-D283-4F68-80A9-619D1DECAB01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACD2BAF0-3628-4D62-AD00-8FE42E22B70A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -710,15 +710,6 @@
     <t xml:space="preserve">Requires MLAPS. If the first 'lap' does not reach the opponent's side of the board, the sowing ends after the first lap. </t>
   </si>
   <si>
-    <t>Allows specifing non-all-equal start patterns. The following patterns are supported:
-- ALL_EQUAL: all holes start with the same number of seeds.
-- GAMACHA: starting from the third hold (from start player's left) place nbr_seeds in every other hole, the first move is prescribed move the center hole's seeds to the other side (this is done automatically).
-- ALTERNATES: everyother hole is filled with nbr_seeds, no seeds end up opposite eachother. If a player has fewer seeds than their opponent, then they start.
-- ALTS_WITH_1: like Alternates except the starter's 2nd from right hole with nbr_seeds is replaced with one seed.
-- CLIPPEDTRIPLES: pattern of 0 S S (where S is nbr_seeds) is used to fill the holes; if a full cycle of 3 cannot be placed, the holes are left empty. The True and False sides are the same from the player's perspective, e.g. they will look reversed when viewed from one side of the game board.
-- TWOEMPTY: all but the rightmost two holes for each player are filled with is nbr_seeds.</t>
-  </si>
-  <si>
     <t>The first sow of the game maybe defined by a specific rule. Prescribed openings are different than start patterns because the player may choose the sow start point. SOW_OWN_STORE and SOW_RULE are ignored during the prescribed openings.
 - NONE: there is no prescribed opening move.
 - BASIC_SOWER: the first sow is a very basic pickup the seeds and drop them one at a time in each hole ignoring any other sow parameters. Other sow parameters will be enacted  afterward. This can be used to force the first sow of an MLAPS game to be a single sow. 
@@ -1201,14 +1192,25 @@
     <t>CaptType</t>
   </si>
   <si>
-    <t>Capture type.  Basic capture rules are not applied and are incompatible with cross capture.
-- NEXT: Capture from the hole after the final seed sown. 
+    <t>Allows specifing non-all-equal start patterns. The following patterns are supported:
+- ALL_EQUAL: all holes start with the same number of seeds.
+- GAMACHA: starting from the third hold (from start player's left) place nbr_seeds in every other hole, the first move is prescribed move the center hole's seeds to the other side (this is done automatically).
+- ALTERNATES: everyother hole is filled with nbr_seeds, no seeds end up opposite eachother. If a player has fewer seeds than their opponent, then they start.
+- ALTS_WITH_1: like Alternates except the starter's 2nd from right hole with nbr_seeds is replaced with one seed.
+- CLIPPEDTRIPLES: pattern of 0 S S (where S is nbr_seeds) is used to fill the holes; if a full cycle of 3 cannot be placed, the holes are left empty. The True and False sides are the same from the player's perspective, e.g. they will look reversed when viewed from one side of the game board.
+- TWOEMPTY: all but the rightmost two holes for each player are filled with is nbr_seeds.
+- RANDOM: the total seeds are computed as (10 * holes) + (2 * nbr_start). The seeds are randomly distributed into all holes.</t>
+  </si>
+  <si>
+    <t>Capture type.
+- NONE: No other capture type.
+- NEXT: Capture from the hole after the final seed sown. Basic capture rules are applied; capture side is checked; and multiple captures in either direction are supported.
   + When multiple lap sowing, the sowing does not stop for captures. Instead, sowing continues until the final seed is sown into an empty hole. Then the capture test is made on the next hole.
-- TWO_OUT: There are three flavors of capture two out:
+- TWO_OUT: Basic capture rules and capture side are ignored. There are three flavors of capture two out:
   + Single lap game: capture if sow ends in occupied hole, then an empty hole, followed by an occupied hole the contents of this are hole captured.
   + Multi lap game but single capture: capture when last hole sown is followed by an empty hole which is then followed by an occupied hole.
-  + Multi lap game with multiple captures: capture when last hole sown is followed by an empty hole which is then followed by an occupied hole. Continue captures as long as the pattern of empty hole followed by an occupied hole continues.
-- MATCH_OPP: capture when the number of seeds in the final hole sown match the oppocite hole.</t>
+  + Multi lap game with multiple captures: capture when last hole sown is followed by an empty hole which is then followed by an occupied hole. Continue captures as long as the pattern of empty hole followed by an occupied hole continues. CAPSAMEDIR must be true. 
+- MATCH_OPP: capture when the number of seeds in the final hole sown match the opposite-side hole. Multiple captures maybe made in either direction. Multilap sowing does stop for captures.</t>
   </si>
 </sst>
 </file>
@@ -2093,7 +2095,7 @@
   <dimension ref="A1:J87"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
@@ -2149,17 +2151,17 @@
         <v>90</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>262</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>263</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3">
         <v>0</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="G2" s="5" t="s">
         <v>84</v>
@@ -2233,7 +2235,7 @@
         <v>0</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -2265,7 +2267,7 @@
         <v>0</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -2297,7 +2299,7 @@
         <v>0</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -2305,16 +2307,16 @@
         <v>90</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>267</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>268</v>
-      </c>
       <c r="E7" s="3">
         <v>0</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="G7" s="5" t="s">
         <v>84</v>
@@ -2387,7 +2389,7 @@
         <v>0</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2427,19 +2429,19 @@
         <v>90</v>
       </c>
       <c r="B11" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>264</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="E11" s="3">
+        <v>0</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="G11" s="5" t="s">
         <v>265</v>
-      </c>
-      <c r="E11" s="3">
-        <v>0</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>255</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>266</v>
       </c>
       <c r="H11" s="3">
         <v>9</v>
@@ -2448,15 +2450,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="150" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="195" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>90</v>
       </c>
       <c r="B12" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>314</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>315</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>22</v>
@@ -2465,7 +2467,7 @@
         <v>106</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="G12" s="5" t="s">
         <v>159</v>
@@ -2485,7 +2487,7 @@
         <v>90</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>111</v>
@@ -2494,7 +2496,7 @@
         <v>0</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="G13" s="5" t="s">
         <v>84</v>
@@ -2535,7 +2537,7 @@
         <v>2</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2575,16 +2577,16 @@
         <v>90</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="E16" s="3">
         <v>0</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="G16" s="5" t="s">
         <v>84</v>
@@ -2601,10 +2603,10 @@
         <v>90</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>22</v>
@@ -2625,7 +2627,7 @@
         <v>2</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -2633,10 +2635,10 @@
         <v>90</v>
       </c>
       <c r="B18" s="3" t="s">
+        <v>292</v>
+      </c>
+      <c r="C18" s="3" t="s">
         <v>293</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>294</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>22</v>
@@ -2645,10 +2647,10 @@
         <v>130</v>
       </c>
       <c r="F18" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="G18" s="5" t="s">
         <v>295</v>
-      </c>
-      <c r="G18" s="5" t="s">
-        <v>296</v>
       </c>
       <c r="H18" s="3">
         <v>5</v>
@@ -2657,7 +2659,7 @@
         <v>2</v>
       </c>
       <c r="J18" s="4" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
@@ -2729,16 +2731,16 @@
         <v>90</v>
       </c>
       <c r="B21" s="3" t="s">
+        <v>270</v>
+      </c>
+      <c r="C21" s="3" t="s">
         <v>271</v>
       </c>
-      <c r="C21" s="3" t="s">
-        <v>272</v>
-      </c>
       <c r="E21" s="3">
         <v>0</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="G21" s="5" t="s">
         <v>84</v>
@@ -2811,7 +2813,7 @@
         <v>2</v>
       </c>
       <c r="J23" s="4" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="409.5" x14ac:dyDescent="0.25">
@@ -2843,7 +2845,7 @@
         <v>0</v>
       </c>
       <c r="J24" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="105" x14ac:dyDescent="0.25">
@@ -2851,10 +2853,10 @@
         <v>36</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>22</v>
@@ -2875,7 +2877,7 @@
         <v>0</v>
       </c>
       <c r="J25" s="4" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="120" x14ac:dyDescent="0.25">
@@ -2883,10 +2885,10 @@
         <v>36</v>
       </c>
       <c r="B26" s="3" t="s">
+        <v>287</v>
+      </c>
+      <c r="C26" s="3" t="s">
         <v>288</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>289</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>22</v>
@@ -2895,10 +2897,10 @@
         <v>147</v>
       </c>
       <c r="F26" s="3" t="s">
+        <v>289</v>
+      </c>
+      <c r="G26" s="5" t="s">
         <v>290</v>
-      </c>
-      <c r="G26" s="5" t="s">
-        <v>291</v>
       </c>
       <c r="H26" s="3">
         <v>2</v>
@@ -2907,7 +2909,7 @@
         <v>0</v>
       </c>
       <c r="J26" s="4" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
@@ -2915,16 +2917,16 @@
         <v>36</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E27" s="3">
         <v>0</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="G27" s="5" t="s">
         <v>84</v>
@@ -2936,7 +2938,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="150" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" ht="165" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>36</v>
       </c>
@@ -2965,7 +2967,7 @@
         <v>0</v>
       </c>
       <c r="J28" s="4" t="s">
-        <v>216</v>
+        <v>316</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="180" x14ac:dyDescent="0.25">
@@ -2997,7 +2999,7 @@
         <v>0</v>
       </c>
       <c r="J29" s="4" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
@@ -3005,16 +3007,16 @@
         <v>36</v>
       </c>
       <c r="B30" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="C30" s="3" t="s">
         <v>283</v>
       </c>
-      <c r="C30" s="3" t="s">
-        <v>284</v>
-      </c>
       <c r="E30" s="3">
         <v>0</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="G30" s="5" t="s">
         <v>84</v>
@@ -3087,7 +3089,7 @@
         <v>0</v>
       </c>
       <c r="J32" s="4" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3119,7 +3121,7 @@
         <v>2</v>
       </c>
       <c r="J33" s="4" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
@@ -3151,7 +3153,7 @@
         <v>2</v>
       </c>
       <c r="J34" s="4" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
@@ -3159,16 +3161,16 @@
         <v>36</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E35" s="3">
         <v>0</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="G35" s="5" t="s">
         <v>84</v>
@@ -3241,7 +3243,7 @@
         <v>2</v>
       </c>
       <c r="J37" s="4" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="38" spans="1:10" ht="150" x14ac:dyDescent="0.25">
@@ -3273,7 +3275,7 @@
         <v>2</v>
       </c>
       <c r="J38" s="4" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
@@ -3281,16 +3283,16 @@
         <v>36</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="E39" s="3">
         <v>0</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="G39" s="5" t="s">
         <v>84</v>
@@ -3322,7 +3324,7 @@
         <v>42</v>
       </c>
       <c r="G40" s="5" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="H40" s="3">
         <v>8</v>
@@ -3331,7 +3333,7 @@
         <v>2</v>
       </c>
       <c r="J40" s="4" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="41" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -3395,7 +3397,7 @@
         <v>2</v>
       </c>
       <c r="J42" s="4" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="43" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -3427,7 +3429,7 @@
         <v>2</v>
       </c>
       <c r="J43" s="4" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -3459,7 +3461,7 @@
         <v>0</v>
       </c>
       <c r="J44" s="4" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
@@ -3651,7 +3653,7 @@
         <v>0</v>
       </c>
       <c r="J50" s="4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
@@ -3723,16 +3725,16 @@
         <v>118</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E53" s="3">
         <v>0</v>
       </c>
       <c r="F53" s="3" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="G53" s="5" t="s">
         <v>84</v>
@@ -3764,7 +3766,7 @@
         <v>87</v>
       </c>
       <c r="G54" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="H54" s="3">
         <v>6</v>
@@ -3796,7 +3798,7 @@
         <v>87</v>
       </c>
       <c r="G55" s="3" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="H55" s="3">
         <v>7</v>
@@ -3845,16 +3847,16 @@
         <v>118</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E57" s="3">
         <v>0</v>
       </c>
       <c r="F57" s="3" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="G57" s="5" t="s">
         <v>84</v>
@@ -3886,7 +3888,7 @@
         <v>87</v>
       </c>
       <c r="G58" s="3" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="H58" s="3">
         <v>2</v>
@@ -3906,7 +3908,7 @@
         <v>119</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D59" s="3" t="s">
         <v>120</v>
@@ -3938,7 +3940,7 @@
         <v>121</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D60" s="3" t="s">
         <v>120</v>
@@ -3970,7 +3972,7 @@
         <v>122</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D61" s="3" t="s">
         <v>120</v>
@@ -3991,7 +3993,7 @@
         <v>2</v>
       </c>
       <c r="J61" s="4" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="62" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -4002,7 +4004,7 @@
         <v>123</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D62" s="3" t="s">
         <v>120</v>
@@ -4034,7 +4036,7 @@
         <v>124</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D63" s="3" t="s">
         <v>120</v>
@@ -4066,7 +4068,7 @@
         <v>125</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D64" s="3" t="s">
         <v>120</v>
@@ -4098,7 +4100,7 @@
         <v>128</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D65" s="3" t="s">
         <v>120</v>
@@ -4261,7 +4263,7 @@
         <v>81</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D71" s="3" t="s">
         <v>22</v>
@@ -4282,7 +4284,7 @@
         <v>0</v>
       </c>
       <c r="J71" s="8" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="72" spans="1:10" ht="165" x14ac:dyDescent="0.25">
@@ -4314,7 +4316,7 @@
         <v>0</v>
       </c>
       <c r="J72" s="4" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="73" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -4346,7 +4348,7 @@
         <v>0</v>
       </c>
       <c r="J73" s="4" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.25">
@@ -4354,16 +4356,16 @@
         <v>66</v>
       </c>
       <c r="B74" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="C74" s="3" t="s">
         <v>278</v>
       </c>
-      <c r="C74" s="3" t="s">
-        <v>279</v>
-      </c>
       <c r="E74" s="3">
         <v>0</v>
       </c>
       <c r="F74" s="3" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="G74" s="5" t="s">
         <v>84</v>
@@ -4415,7 +4417,7 @@
         <v>76</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D76" s="3" t="s">
         <v>22</v>
@@ -4436,7 +4438,7 @@
         <v>0</v>
       </c>
       <c r="J76" s="4" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="77" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -4468,7 +4470,7 @@
         <v>0</v>
       </c>
       <c r="J77" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="78" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -4540,10 +4542,10 @@
         <v>66</v>
       </c>
       <c r="B80" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="C80" s="3" t="s">
         <v>298</v>
-      </c>
-      <c r="C80" s="3" t="s">
-        <v>299</v>
       </c>
       <c r="D80" s="3" t="s">
         <v>22</v>
@@ -4552,7 +4554,7 @@
         <v>133</v>
       </c>
       <c r="F80" s="3" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="G80" s="5" t="s">
         <v>159</v>
@@ -4564,7 +4566,7 @@
         <v>0</v>
       </c>
       <c r="J80" s="4" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="81" spans="1:10" ht="409.5" x14ac:dyDescent="0.25">
@@ -4596,7 +4598,7 @@
         <v>0</v>
       </c>
       <c r="J81" s="4" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="82" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -4604,10 +4606,10 @@
         <v>66</v>
       </c>
       <c r="B82" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="C82" s="3" t="s">
         <v>252</v>
-      </c>
-      <c r="C82" s="3" t="s">
-        <v>253</v>
       </c>
       <c r="D82" s="3" t="s">
         <v>22</v>
@@ -4628,7 +4630,7 @@
         <v>0</v>
       </c>
       <c r="J82" s="4" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.25">
@@ -4636,16 +4638,16 @@
         <v>66</v>
       </c>
       <c r="B83" s="3" t="s">
+        <v>275</v>
+      </c>
+      <c r="C83" s="3" t="s">
         <v>276</v>
       </c>
-      <c r="C83" s="3" t="s">
-        <v>277</v>
-      </c>
       <c r="E83" s="3">
         <v>0</v>
       </c>
       <c r="F83" s="3" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="G83" s="5" t="s">
         <v>84</v>
@@ -4686,7 +4688,7 @@
         <v>2</v>
       </c>
       <c r="J84" s="4" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="85" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -4750,7 +4752,7 @@
         <v>2</v>
       </c>
       <c r="J86" s="4" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="87" spans="1:10" ht="405" x14ac:dyDescent="0.25">
@@ -4758,10 +4760,10 @@
         <v>66</v>
       </c>
       <c r="B87" s="3" t="s">
+        <v>305</v>
+      </c>
+      <c r="C87" s="3" t="s">
         <v>306</v>
-      </c>
-      <c r="C87" s="3" t="s">
-        <v>307</v>
       </c>
       <c r="D87" s="3" t="s">
         <v>22</v>
@@ -4770,10 +4772,10 @@
         <v>112</v>
       </c>
       <c r="F87" s="3" t="s">
+        <v>307</v>
+      </c>
+      <c r="G87" s="3" t="s">
         <v>308</v>
-      </c>
-      <c r="G87" s="3" t="s">
-        <v>309</v>
       </c>
       <c r="H87" s="3">
         <v>7</v>
@@ -4782,7 +4784,7 @@
         <v>2</v>
       </c>
       <c r="J87" s="4" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Wrote a SameSide game class inspired by Ohojichi: only sow on your own side of the board and put your captures in the hole of your choice on your opponents side. Sides are Top/Bottom not East/West as in Ohojichi. No unit test code yet.
</commit_message>
<xml_diff>
--- a/src/game_params.xlsx
+++ b/src/game_params.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Activity_Data\Mancala_github\MancalaGames\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACD2BAF0-3628-4D62-AD00-8FE42E22B70A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63270AF1-94F2-4DAC-B7EE-41399887876D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -836,11 +836,6 @@
     <t>NO_ROUNDS</t>
   </si>
   <si>
-    <t>The name of the Game Class. One of:
-Mancala: allows setting all parameters though there are limited combinations.
-Diffusion: has unique sow method and win conditions. Only very limited parameters may be changed from defaults.</t>
-  </si>
-  <si>
     <t>True when stores are present on the game board. For games with GOAL of DEPRIVE or CLEAR, stores can be used to show whose turn it is (seed counts will not be sown).</t>
   </si>
   <si>
@@ -1211,6 +1206,12 @@
   + Multi lap game but single capture: capture when last hole sown is followed by an empty hole which is then followed by an occupied hole.
   + Multi lap game with multiple captures: capture when last hole sown is followed by an empty hole which is then followed by an occupied hole. Continue captures as long as the pattern of empty hole followed by an occupied hole continues. CAPSAMEDIR must be true. 
 - MATCH_OPP: capture when the number of seeds in the final hole sown match the opposite-side hole. Multiple captures maybe made in either direction. Multilap sowing does stop for captures.</t>
+  </si>
+  <si>
+    <t>The name of the Game Class. One of:
+Mancala: allows setting all parameters though some combinations are limited.
+Diffusion: has unique sow method and win conditions.  The game is basically preconfigured, only the board size can be changed to any even size. Game goal must be clear.
+SameSide: a game class in which seeds are only sown on the player's own side of the board. If a capture is made, the capturer chooses one of their opponent's holes to put the seeds into. All seeds go into exactly one hole. Capture mechanisms must be limited to one side of the board: basic captures, next, and two out. Game goal must be clear.</t>
   </si>
 </sst>
 </file>
@@ -2095,8 +2096,8 @@
   <dimension ref="A1:J87"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J12" sqref="J12"/>
+      <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J44" sqref="J44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2151,17 +2152,17 @@
         <v>90</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>261</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>262</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3">
         <v>0</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="G2" s="5" t="s">
         <v>84</v>
@@ -2307,16 +2308,16 @@
         <v>90</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>266</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>267</v>
-      </c>
       <c r="E7" s="3">
         <v>0</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="G7" s="5" t="s">
         <v>84</v>
@@ -2429,19 +2430,19 @@
         <v>90</v>
       </c>
       <c r="B11" s="3" t="s">
+        <v>262</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>263</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="E11" s="3">
+        <v>0</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="G11" s="5" t="s">
         <v>264</v>
-      </c>
-      <c r="E11" s="3">
-        <v>0</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>254</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>265</v>
       </c>
       <c r="H11" s="3">
         <v>9</v>
@@ -2455,10 +2456,10 @@
         <v>90</v>
       </c>
       <c r="B12" s="3" t="s">
+        <v>312</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>313</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>314</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>22</v>
@@ -2467,7 +2468,7 @@
         <v>106</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="G12" s="5" t="s">
         <v>159</v>
@@ -2479,7 +2480,7 @@
         <v>0</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -2487,7 +2488,7 @@
         <v>90</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>111</v>
@@ -2496,7 +2497,7 @@
         <v>0</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="G13" s="5" t="s">
         <v>84</v>
@@ -2537,7 +2538,7 @@
         <v>2</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2577,16 +2578,16 @@
         <v>90</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E16" s="3">
         <v>0</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="G16" s="5" t="s">
         <v>84</v>
@@ -2603,10 +2604,10 @@
         <v>90</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>22</v>
@@ -2627,7 +2628,7 @@
         <v>2</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -2635,10 +2636,10 @@
         <v>90</v>
       </c>
       <c r="B18" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="C18" s="3" t="s">
         <v>292</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>293</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>22</v>
@@ -2647,10 +2648,10 @@
         <v>130</v>
       </c>
       <c r="F18" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="G18" s="5" t="s">
         <v>294</v>
-      </c>
-      <c r="G18" s="5" t="s">
-        <v>295</v>
       </c>
       <c r="H18" s="3">
         <v>5</v>
@@ -2659,7 +2660,7 @@
         <v>2</v>
       </c>
       <c r="J18" s="4" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
@@ -2731,16 +2732,16 @@
         <v>90</v>
       </c>
       <c r="B21" s="3" t="s">
+        <v>269</v>
+      </c>
+      <c r="C21" s="3" t="s">
         <v>270</v>
       </c>
-      <c r="C21" s="3" t="s">
-        <v>271</v>
-      </c>
       <c r="E21" s="3">
         <v>0</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="G21" s="5" t="s">
         <v>84</v>
@@ -2845,7 +2846,7 @@
         <v>0</v>
       </c>
       <c r="J24" s="4" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="105" x14ac:dyDescent="0.25">
@@ -2853,10 +2854,10 @@
         <v>36</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>22</v>
@@ -2877,7 +2878,7 @@
         <v>0</v>
       </c>
       <c r="J25" s="4" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="120" x14ac:dyDescent="0.25">
@@ -2885,10 +2886,10 @@
         <v>36</v>
       </c>
       <c r="B26" s="3" t="s">
+        <v>286</v>
+      </c>
+      <c r="C26" s="3" t="s">
         <v>287</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>288</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>22</v>
@@ -2897,10 +2898,10 @@
         <v>147</v>
       </c>
       <c r="F26" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="G26" s="5" t="s">
         <v>289</v>
-      </c>
-      <c r="G26" s="5" t="s">
-        <v>290</v>
       </c>
       <c r="H26" s="3">
         <v>2</v>
@@ -2909,7 +2910,7 @@
         <v>0</v>
       </c>
       <c r="J26" s="4" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
@@ -2917,16 +2918,16 @@
         <v>36</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E27" s="3">
         <v>0</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="G27" s="5" t="s">
         <v>84</v>
@@ -2967,7 +2968,7 @@
         <v>0</v>
       </c>
       <c r="J28" s="4" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="180" x14ac:dyDescent="0.25">
@@ -3007,16 +3008,16 @@
         <v>36</v>
       </c>
       <c r="B30" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="C30" s="3" t="s">
         <v>282</v>
       </c>
-      <c r="C30" s="3" t="s">
-        <v>283</v>
-      </c>
       <c r="E30" s="3">
         <v>0</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="G30" s="5" t="s">
         <v>84</v>
@@ -3089,7 +3090,7 @@
         <v>0</v>
       </c>
       <c r="J32" s="4" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3121,7 +3122,7 @@
         <v>2</v>
       </c>
       <c r="J33" s="4" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
@@ -3161,16 +3162,16 @@
         <v>36</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="E35" s="3">
         <v>0</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="G35" s="5" t="s">
         <v>84</v>
@@ -3283,16 +3284,16 @@
         <v>36</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="E39" s="3">
         <v>0</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="G39" s="5" t="s">
         <v>84</v>
@@ -3333,7 +3334,7 @@
         <v>2</v>
       </c>
       <c r="J40" s="4" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="41" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -3397,7 +3398,7 @@
         <v>2</v>
       </c>
       <c r="J42" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="43" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -3429,10 +3430,10 @@
         <v>2</v>
       </c>
       <c r="J43" s="4" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>15</v>
       </c>
@@ -3461,7 +3462,7 @@
         <v>0</v>
       </c>
       <c r="J44" s="4" t="s">
-        <v>242</v>
+        <v>317</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
@@ -3725,16 +3726,16 @@
         <v>118</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E53" s="3">
         <v>0</v>
       </c>
       <c r="F53" s="3" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="G53" s="5" t="s">
         <v>84</v>
@@ -3847,16 +3848,16 @@
         <v>118</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E57" s="3">
         <v>0</v>
       </c>
       <c r="F57" s="3" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="G57" s="5" t="s">
         <v>84</v>
@@ -4100,7 +4101,7 @@
         <v>128</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D65" s="3" t="s">
         <v>120</v>
@@ -4263,7 +4264,7 @@
         <v>81</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D71" s="3" t="s">
         <v>22</v>
@@ -4356,16 +4357,16 @@
         <v>66</v>
       </c>
       <c r="B74" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="C74" s="3" t="s">
         <v>277</v>
       </c>
-      <c r="C74" s="3" t="s">
-        <v>278</v>
-      </c>
       <c r="E74" s="3">
         <v>0</v>
       </c>
       <c r="F74" s="3" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="G74" s="5" t="s">
         <v>84</v>
@@ -4417,7 +4418,7 @@
         <v>76</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D76" s="3" t="s">
         <v>22</v>
@@ -4542,10 +4543,10 @@
         <v>66</v>
       </c>
       <c r="B80" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="C80" s="3" t="s">
         <v>297</v>
-      </c>
-      <c r="C80" s="3" t="s">
-        <v>298</v>
       </c>
       <c r="D80" s="3" t="s">
         <v>22</v>
@@ -4554,7 +4555,7 @@
         <v>133</v>
       </c>
       <c r="F80" s="3" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="G80" s="5" t="s">
         <v>159</v>
@@ -4566,7 +4567,7 @@
         <v>0</v>
       </c>
       <c r="J80" s="4" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="81" spans="1:10" ht="409.5" x14ac:dyDescent="0.25">
@@ -4598,7 +4599,7 @@
         <v>0</v>
       </c>
       <c r="J81" s="4" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="82" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -4606,10 +4607,10 @@
         <v>66</v>
       </c>
       <c r="B82" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="C82" s="3" t="s">
         <v>251</v>
-      </c>
-      <c r="C82" s="3" t="s">
-        <v>252</v>
       </c>
       <c r="D82" s="3" t="s">
         <v>22</v>
@@ -4630,7 +4631,7 @@
         <v>0</v>
       </c>
       <c r="J82" s="4" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.25">
@@ -4638,16 +4639,16 @@
         <v>66</v>
       </c>
       <c r="B83" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="C83" s="3" t="s">
         <v>275</v>
       </c>
-      <c r="C83" s="3" t="s">
-        <v>276</v>
-      </c>
       <c r="E83" s="3">
         <v>0</v>
       </c>
       <c r="F83" s="3" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="G83" s="5" t="s">
         <v>84</v>
@@ -4688,7 +4689,7 @@
         <v>2</v>
       </c>
       <c r="J84" s="4" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="85" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -4752,7 +4753,7 @@
         <v>2</v>
       </c>
       <c r="J86" s="4" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="87" spans="1:10" ht="405" x14ac:dyDescent="0.25">
@@ -4760,10 +4761,10 @@
         <v>66</v>
       </c>
       <c r="B87" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="C87" s="3" t="s">
         <v>305</v>
-      </c>
-      <c r="C87" s="3" t="s">
-        <v>306</v>
       </c>
       <c r="D87" s="3" t="s">
         <v>22</v>
@@ -4772,10 +4773,10 @@
         <v>112</v>
       </c>
       <c r="F87" s="3" t="s">
+        <v>306</v>
+      </c>
+      <c r="G87" s="3" t="s">
         <v>307</v>
-      </c>
-      <c r="G87" s="3" t="s">
-        <v>308</v>
       </c>
       <c r="H87" s="3">
         <v>7</v>
@@ -4784,7 +4785,7 @@
         <v>2</v>
       </c>
       <c r="J87" s="4" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Minimaxer scorer updated so that it will work with East/West games. Add true_holes to the game classes to support this. Button state logic consolidated to mancala_ui (behaviors just executes the decisions now). Put the diffusion rule back in to suggest the use of stores (no other way to know whose turn it is).
</commit_message>
<xml_diff>
--- a/src/game_params.xlsx
+++ b/src/game_params.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Activity_Data\Mancala_github\MancalaGames\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63270AF1-94F2-4DAC-B7EE-41399887876D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8BAD0AD-76BD-4668-B1F2-39B65D01FE9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1210,8 +1210,10 @@
   <si>
     <t>The name of the Game Class. One of:
 Mancala: allows setting all parameters though some combinations are limited.
-Diffusion: has unique sow method and win conditions.  The game is basically preconfigured, only the board size can be changed to any even size. Game goal must be clear.
-SameSide: a game class in which seeds are only sown on the player's own side of the board. If a capture is made, the capturer chooses one of their opponent's holes to put the seeds into. All seeds go into exactly one hole. Capture mechanisms must be limited to one side of the board: basic captures, next, and two out. Game goal must be clear.</t>
+Diffusion: has unique sow method and win conditions.  Players control the east/west sides of the board. The game is basically preconfigured, only the board size can be changed to any even size. Game goal must be clear.
+DiffusionV2: similar to Diffusion but players control the typical north/south sides of the board.
+SameSide: a game class in which seeds are only sown on the player's own side of the board. If a capture is made, the capturer chooses one of their opponent's holes to put the seeds into. All seeds go into exactly one hole. Sow direction is unconstrained Capture mechanisms must be limited to one side of the board: basic captures, next, and two out. Game goal must be clear.
+Ohojichi: very similar to SameSide but the board is divided east/west instead of north/south. Most parameter restrictions from SameSide apply to Ohojichi. For Ohojichi, if UDIR_HOLES is used, all holes must be UDIR; capture side must be BOTH.</t>
   </si>
 </sst>
 </file>
@@ -2096,7 +2098,7 @@
   <dimension ref="A1:J87"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A43" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="J44" sqref="J44"/>
     </sheetView>
   </sheetViews>
@@ -3433,7 +3435,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="44" spans="1:10" ht="105" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" ht="150" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>15</v>
       </c>

</xml_diff>

<commit_message>
Added child_rule OWN_ONLY. Renumbered child_rule and updated Bao_Tanzanian. Helps updated.
</commit_message>
<xml_diff>
--- a/src/game_params.xlsx
+++ b/src/game_params.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Activity_Data\Mancala_github\MancalaGames\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8BAD0AD-76BD-4668-B1F2-39B65D01FE9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26DEC2DE-392F-46A0-B312-0C6BDCFA5656}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32790" yWindow="375" windowWidth="20520" windowHeight="15510" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="game_params" sheetId="1" r:id="rId1"/>
@@ -1108,29 +1108,6 @@
     <t>ANYWHERE</t>
   </si>
   <si>
-    <t xml:space="preserve">Games with children allow players to claim holes. These child holes are an extension of the stores and seeds in them count towards a win. Making a child stops any multiple lap sowing, moves cannot start from children, and they cannot be captured (except for special rules associated with WEGs).
-- NOCHILD: children are not used.
-- NORMAL: children are made when a final seeds sows a hole to CHILD_CVT. If stores are not included captures are instead moved into children, thus a player may not capture until they have created a child. 
-- ONE_CHILD: only one child allowed per player.
-  + Children must not be symmetrically opposite eachother. For example,  in a 9 hole per side game with holes numbered as follows, children may not be in the same numbered holes:
-  + 9 8 7 6 5 4 3 2 1
-  + 1 2 3 4 5 6 7 8 9 
-  + Depending on sow direction some holes are prohibited from being made children: 
-  + CW &amp; CCW:  the last of your opponents holes that you would sow into may not be made a child. CW holes numbered 1 above and CCW holes numberd 9 above.
-  + SPLIT: no end holes may be made children.
-  + Used to create tuzdek style children along with CHILD_RULE of OPP_ONLY.
-- WEG: children maybe created in holes owned by the opponent. Ending a sow in an opponent's weg captures the seed just sown and one more (if there is one); generally, the player gets to play again (per CAPT_RTURN). WEGs are supported for TERRITORY games only (hole ownership required).
-- BULL: create one bull if final seed sows to CHILD_CVT, create two bulls if the final two seeds are sown to CHILD_CVT-1 and CHILD_CVT (in either order).
-- QUR: when a seed is sown into an empty hole on the player's side of the board and the opposite hole contains CHILD_CVT, create children in both holes: final seed location and opposite.
-</t>
-  </si>
-  <si>
-    <t>Additional child creation requirements may be set. These are in addition to location restrictions specified by CHILD_LOCS.
-- NONE: no additional restrictions.
-- OPP_ONLY:  Only make children on the opposite side of the board. Incompatible with BULL, QUR, and WEG child types.
-- NOT_1ST_OPP: Don't make a child in the first hole on the opponents side/territory with one seed.</t>
-  </si>
-  <si>
     <t>Locations where children can be made by each player. The notes designate players as: T - top player, B - bottom player. N - neither player. For shorter boards, the pattern is generated using assignments (a b c d e) as:
 board length 2: a e
 board length 3: a c e
@@ -1214,6 +1191,27 @@
 DiffusionV2: similar to Diffusion but players control the typical north/south sides of the board.
 SameSide: a game class in which seeds are only sown on the player's own side of the board. If a capture is made, the capturer chooses one of their opponent's holes to put the seeds into. All seeds go into exactly one hole. Sow direction is unconstrained Capture mechanisms must be limited to one side of the board: basic captures, next, and two out. Game goal must be clear.
 Ohojichi: very similar to SameSide but the board is divided east/west instead of north/south. Most parameter restrictions from SameSide apply to Ohojichi. For Ohojichi, if UDIR_HOLES is used, all holes must be UDIR; capture side must be BOTH.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Games with children allow players to claim holes. These child holes are an extension of the stores and seeds in them count towards a win. Making a child stops any multiple lap sowing, moves cannot start from children, and they cannot be captured (except for special rules associated with WEGs).
+- NOCHILD: children are not used.
+- NORMAL: children are made when a final seeds sows a hole to CHILD_CVT. If stores are not included captures are instead moved into children, thus a player may not capture until they have created a child. 
+- ONE_CHILD: only one child allowed per player.
+  + Children must not be symmetrically opposite eachother. For example,  in a 9 hole per side game with holes numbered as follows, children may not be in the same numbered holes:
+  + 9 8 7 6 5 4 3 2 1
+  + 1 2 3 4 5 6 7 8 9 
+  + Used to create tuzdek style children along with CHILD_RULE of OPP_ONLY.
+- WEG: children maybe created in holes owned by the opponent. Ending a sow in an opponent's weg captures the seed just sown and one more (if there is one); generally, the player gets to play again (per CAPT_RTURN). WEGs are supported for TERRITORY games only (hole ownership required).
+- BULL: create one bull if final seed sows to CHILD_CVT, create two bulls if the final two seeds are sown to CHILD_CVT-1 and CHILD_CVT (in either order).
+- QUR: when a seed is sown into an empty hole on the player's side of the board and the opposite hole contains CHILD_CVT, create children in both holes: final seed location and opposite.
+</t>
+  </si>
+  <si>
+    <t>Additional child creation requirements may be set. These are in addition to location restrictions specified by CHILD_LOCS.
+- NONE: no additional restrictions.
+- OPP_ONLY:  Only make children on the opposite side of the board. Incompatible with BULL, QUR, and WEG child types.
+- OWN_ONLY: Only make children on own side of the board.  Incompatible with BULL, QUR, and WEG child types.
+- NOT_1ST_OPP: Don't make a child in the first hole on the opponents side/territory with one seed.</t>
   </si>
 </sst>
 </file>
@@ -2099,7 +2097,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A43" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J44" sqref="J44"/>
+      <selection pane="bottomLeft" activeCell="J86" sqref="J86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2458,10 +2456,10 @@
         <v>90</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>22</v>
@@ -2470,7 +2468,7 @@
         <v>106</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="G12" s="5" t="s">
         <v>159</v>
@@ -2482,7 +2480,7 @@
         <v>0</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -2970,7 +2968,7 @@
         <v>0</v>
       </c>
       <c r="J28" s="4" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="180" x14ac:dyDescent="0.25">
@@ -3464,7 +3462,7 @@
         <v>0</v>
       </c>
       <c r="J44" s="4" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
@@ -4601,7 +4599,7 @@
         <v>0</v>
       </c>
       <c r="J81" s="4" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
     </row>
     <row r="82" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -4662,7 +4660,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="84" spans="1:10" ht="330" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10" ht="270" x14ac:dyDescent="0.25">
       <c r="A84" s="3" t="s">
         <v>66</v>
       </c>
@@ -4691,7 +4689,7 @@
         <v>2</v>
       </c>
       <c r="J84" s="4" t="s">
-        <v>308</v>
+        <v>316</v>
       </c>
     </row>
     <row r="85" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -4726,7 +4724,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="86" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A86" s="3" t="s">
         <v>66</v>
       </c>
@@ -4755,7 +4753,7 @@
         <v>2</v>
       </c>
       <c r="J86" s="4" t="s">
-        <v>309</v>
+        <v>317</v>
       </c>
     </row>
     <row r="87" spans="1:10" ht="405" x14ac:dyDescent="0.25">
@@ -4787,7 +4785,7 @@
         <v>2</v>
       </c>
       <c r="J87" s="4" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated css that might work better for narrow screens. Spell check on parameter descriptions. Updated the executables.
</commit_message>
<xml_diff>
--- a/src/game_params.xlsx
+++ b/src/game_params.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Activity_Data\Mancala_github\MancalaGames\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26DEC2DE-392F-46A0-B312-0C6BDCFA5656}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DE9A3B5-9D9F-4288-9B7A-026FB3234806}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32790" yWindow="375" windowWidth="20520" windowHeight="15510" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="game_params" sheetId="1" r:id="rId1"/>
@@ -646,19 +646,10 @@
     <t>Number of game tree expansions to perform each time we pick a new move. One value for each difficulty level (0-3).</t>
   </si>
   <si>
-    <t>Bias for the Monte Carlo Tree seach algorithm for each difficulty level (0-3).  A larger bias encourages move game tree exploration, but defocuses the exploration from the best choices. This is critical in avoiding getting stuck in sub-obtimal move choices.
-Value is divided by 1000.</t>
-  </si>
-  <si>
     <t>The default difficulty for the game. The difficulty can be changed at play time,  even during game play, in the Mancala UI.</t>
   </si>
   <si>
     <t>Automatically activate the AI player. The AI player can be manually deactivated, but it is selected for the starter it will start the game.</t>
-  </si>
-  <si>
-    <t>If the game is being played on easy mode (game difficult of easy/0), a random value may be added to the static evaluation. This can be done to induce errors into the ai player's game play. A random value is selected between -easy_rand and + easy_rand.
-The specific value for this should be selected based on the ranges of the paremeters and multiplier.
-Used only for minimax &amp; negamax players.</t>
   </si>
   <si>
     <t>The multiplier for the even scorer. The even scorer counts the number of holes with an even number of seeds. This is useful to use when the capture mechanism is evens.
@@ -692,9 +683,6 @@
     <t>The depth that the minimaxer or negamaxer will search the game tree from the current node. One value for each difficulty.</t>
   </si>
   <si>
-    <t>Only meaninful with MULTICAPT. Captures are done in the same direction as the sowing, i.e. following the final hole sown. If not set, captures are done from the holes just sown.</t>
-  </si>
-  <si>
     <t>Capture when a hole contains an even number of seeds, greater than 0. When selected with other basic capture mechanisms, the capture mechanism are ANDed (all must be true for capture). Basic capture mechanisms are: CAPT_MAX, CAPT_MIN, CAPT_ON and EVENS with restrictions from OPPSIDECAPT, MOVEUNLOCK and not child holes of any type.
 MLAPS LAPPER sowing will stop the sowing on a final seed that would capture based on the selected basic capture mechanisms.
 Either SOW_RULE of OWN_SOW_CAPT_ALL or SOW_SOW_CAPT_ALL includes the basic capture mechanisms.</t>
@@ -708,15 +696,6 @@
   </si>
   <si>
     <t xml:space="preserve">Requires MLAPS. If the first 'lap' does not reach the opponent's side of the board, the sowing ends after the first lap. </t>
-  </si>
-  <si>
-    <t>The first sow of the game maybe defined by a specific rule. Prescribed openings are different than start patterns because the player may choose the sow start point. SOW_OWN_STORE and SOW_RULE are ignored during the prescribed openings.
-- NONE: there is no prescribed opening move.
-- BASIC_SOWER: the first sow is a very basic pickup the seeds and drop them one at a time in each hole ignoring any other sow parameters. Other sow parameters will be enacted  afterward. This can be used to force the first sow of an MLAPS game to be a single sow. 
-- MLAPS_SOWER: the first sow follows basic rules of multi-lap sowing (LAPPER). Other sow parameters will be enacted  afterward. 
-- SOW1OPP: at least one seed must be sown on the opponents side of the board which is accomplished by sowing as normal until the final seed, then any remaining holes on the player's side are skipped and the last seed is sown in the oppenents first hole (based on current sow direction).
-- PLUS1MINUS1: proceed from the selected hole by moving one seed from the next hole into the following hole, next skip that hole and repeat moving seed forward. After cycling the board, capture across from the opening hole. 
-- ARNGE_LIMIT: the first move may be used to rearrange the seeds (opponent is same layout). If the first move is not used for rearrangement, captures and child creation are not allowed from the starter until the second player makes a child or captures.</t>
   </si>
   <si>
     <t>When sowing a second or subsequent circuit of the board, skip the start hole. This will leave the start hole empty for single lap games.
@@ -774,14 +753,6 @@
 montecarlo_ts: a Monte Carlo Tree Search player.</t>
   </si>
   <si>
-    <t>Determines if seeds from more the start hole are picked up and sown:
-- OFF: Single lap sowing. Seeds from the start hole are sown, typically, one per hole until expened.
-- LAPPER:  If the first sow ends in a hole with more than one seed, pickup all the seeds and continue sowing another "lap". Note that lap here does not mean a full cicuit of the board, only an individual sow operation. In general, sowing laps continues in this manner until the final seed of a lap reaches an empty hole. There are games with other conditions for ending a multilap low such as making a capture or making a child. 
-  + Several values of SOW_RULE perform an operation after each lap sown: SOW_CLKD_DIV(_NR) closes the final hole and CHANGE_DIR_LAP changes the direction of sowing after each lap.
-- LAPPER_NEXT:  For lapper_next sowing, the number of seeds in the last sown hole of lap do not matter. Instead, if the hole after the last sown hole has any seeds, those seeds are used to continue sowing the next lap. Sowing continues until the hole after the lap's final seed is empty. There are games with other conditions for ending a multilap low such as making a capture or making a child.
-  + A SOW_RULE of CHANGE_DIR_LAP changes the direction of sowing after each lap. SOW_BLKD_DIV(_NR) is not supported for LAPPER_NEXT.</t>
-  </si>
-  <si>
     <t>Capture when the contents of the hole is in the capt_on list. The Mancala Games UI only has checkboxes for 1 to 5 seeds, but any number may be put into the configuration file.
 When selected with other basic capture mechanisms, the capture mechanism are ANDed (all must be true for capture). Basic capture mechanisms are: CAPT_MAX, CAPT_MIN, CAPT_ON and EVENS   with restrictions from OPPSIDECAPT, MOVEUNLOCK and not child holes of any type.
 MLAP LAPPER sowing will stop the sowing on a final seed that would capture based on the selected basic capture mechanisms.
@@ -807,12 +778,6 @@
 When selected with other basic capture mechanisms, the capture mechanism are ANDed (all must be true for capture). Basic capture mechanisms are: CAPT_MAX, CAPT_MIN, CAPT_ON and EVENS  with restrictions from OPPSIDECAPT, MOVEUNLOCK and not child holes of any type.
 MLAPS LAPPER sowing will stop the sowing on a final seed that would capture based on the selected basic capture mechanisms.
 Either SOW_RULE of OWN_SOW_CAPT_ALL or SOW_SOW_CAPT_ALL includes the basic capture mechanisms.</t>
-  </si>
-  <si>
-    <t>When crosscapt is set, defines what to do with the single seed initiating the cross capture.
-- LEAVE: always leave the signle seed
-- PICK_ON_CAPT: only pick (capture) the seed if there was a capture
-- ALWAYS_PICK: always pick (capture) the final single seed, even if there was not a capture</t>
   </si>
   <si>
     <t>Rules to allow taking of more than otherwise captured or picked seeds:
@@ -822,15 +787,6 @@
 - PICKLASTSEEDS: If there are the number of starts seeds or fewer left,  the current player collects them and the game is over. This rule is applied at the end of each turn, even if there is not a capture because the sow phase may have reduced the seed count.
 - PICK2XLASTSEEDS: If there are 2 times the number of start seeds or fewer, the round starter picks them. This rule is applied at the end of each turn, even if there is not a capture because the sow phase may have reduced the seed count.
 In terms of GRANDSLAM, these picks are considered captures.</t>
-  </si>
-  <si>
-    <t>A grandslam is when your opponent has seeds at the start of your turn and you capture them all. This option selects what to do:
-- LEGAL: the seeds are captured
-- NOT_LEGAL: you may not capture all of your opponents seeds, a move which would do so is not allowed
-- NO_CAPT: you may sow the seeds, but the capture is not performed
-- OPP_GETS_REMAIN: if you capture all your opponents seeds, they capture all of your remaining seeds and the game is over. Winner is determined by game goal. Seeds picked because of PICKEXTRA PICK*LASTSEEDS go the current player and not the opponent.
-- LEAVE_LEFT: the capture is performed from all but the leftmost hole from the sower perspective. This might leave your oppenents without seeds or might not capture any seeds.
-- LEAVE_RIGHT: the capture is performed from all but the rightmost hole from the sower perspective. This might leave your oppenents without seeds.</t>
   </si>
   <si>
     <t>NO_ROUNDS</t>
@@ -1079,21 +1035,6 @@
 - RND_SEED_COUNT: collect goal_param seeds across several rounds. ROUND_FILL is not used; each round is setup as the start of the game.
 - RND_EXTRA_SEEDS: collect goal_param extra seeds (winner - loser seeds).  ROUND_FILL is not used; each round is setup as the start of the game.
 - RND_POINTS:  score goal_param points. WIN is 1 point. WIN and skunk (&gt; 3/4 of total seeds) is 2 points.  ROUND_FILL is not used; each round is setup as the start of the game.</t>
-  </si>
-  <si>
-    <t>The round fill method determines which holes are filled and how many seeds they are filled with when setting up for a new round.
-Several round fill mechanisms use the same general approach called the Empty Hole Method. The loser of the previous round will end up with empty holes. These holes are not playable if BLOCKS are used; otherwise they are playable. This method is not used for RND_* GOAL games.
-The seeds each player accummulated in the previous round are distributed into holes with exactly the same number in each. That number of seeds is NBR_START. The winner will fill all of their holes and put any remaining seeds into their own store. The loser will fill as many holes as they can with nbr_start seeds and put any remaining seeds (fewer than nbr_start) into their own store.
-LEFT_FILE, RIGHT_FILL and OUTSIDE_FILL define which holes that the loser must fill. UCHOOSE allows the loser to choose which holes have seeds.
-- NOT_APPLICABLE: round fill doesn't need to be specified: either the game not played in rounds (CLEAR &amp; DEPRIVE games included) or game goal is TERRITORY  without UCHOWN (see below, all holes filled).
-- LEFT_FILL: fill the round loser's holes from the player's left with nbr_start seeds each.  
-- RIGHT_FILL: fill the round loser's holes from the player's right with nbr_start seeds each. 
-- OUTSIDE_FILL: fill the round loser's holes from the outside ends toward the middle with nbr_start seeds each. Leftmost, rightmost, 2nd leftmost, 2nd rightmost, etc. until the seeds are used up.
-- EVEN_FILL: fill all holes (both sides) with the same number of seeds; determined by dividing the losers seeds by the number of holes per side. If that is not playable based on the minimum number of seeds required for a move (MIN_MOVE); extra seeds are put in each players leftmost hole. Any extra seeds are put in each player's store.
-- SHORTEN: the number of holes that the round loser can fill with NBR_START seeds are fill on both sides, other holes are left empty. Holes are filled opposite eachother. If BLOCKS is selected, the board is shortened to the number of holes filled (empty holes are blocked and out of play). If the game uses children, they will not be created if the board size is reduced to 3 or less.
-- UCHOOSE: allow user to choose which holes have seeds (are not blocked) when ROUNDS and BLOCKS are used.
-- UMOVE: allow the loser to choose where seeds are placed. At least one seed must be placed in each hole and the game must be playable (at least one hole has MIN_MOVE seeds), remaining seeds are placed in the store. The winner's layout is the same layout but reflected.
-- UCHOWN: The only round fill supported for territory games. The winner may choose which holes they control.</t>
   </si>
   <si>
     <t>child_locs</t>
@@ -1135,9 +1076,113 @@
   + B TB TB TB TB</t>
   </si>
   <si>
+    <t>capt_type</t>
+  </si>
+  <si>
+    <t>Capture Type</t>
+  </si>
+  <si>
+    <t>CaptType</t>
+  </si>
+  <si>
+    <t>Capture type.
+- NONE: No other capture type.
+- NEXT: Capture from the hole after the final seed sown. Basic capture rules are applied; capture side is checked; and multiple captures in either direction are supported.
+  + When multiple lap sowing, the sowing does not stop for captures. Instead, sowing continues until the final seed is sown into an empty hole. Then the capture test is made on the next hole.
+- TWO_OUT: Basic capture rules and capture side are ignored. There are three flavors of capture two out:
+  + Single lap game: capture if sow ends in occupied hole, then an empty hole, followed by an occupied hole the contents of this are hole captured.
+  + Multi lap game but single capture: capture when last hole sown is followed by an empty hole which is then followed by an occupied hole.
+  + Multi lap game with multiple captures: capture when last hole sown is followed by an empty hole which is then followed by an occupied hole. Continue captures as long as the pattern of empty hole followed by an occupied hole continues. CAPSAMEDIR must be true. 
+- MATCH_OPP: capture when the number of seeds in the final hole sown match the opposite-side hole. Multiple captures maybe made in either direction. Multilap sowing does stop for captures.</t>
+  </si>
+  <si>
+    <t>The name of the Game Class. One of:
+Mancala: allows setting all parameters though some combinations are limited.
+Diffusion: has unique sow method and win conditions.  Players control the east/west sides of the board. The game is basically preconfigured, only the board size can be changed to any even size. Game goal must be clear.
+DiffusionV2: similar to Diffusion but players control the typical north/south sides of the board.
+SameSide: a game class in which seeds are only sown on the player's own side of the board. If a capture is made, the capturer chooses one of their opponent's holes to put the seeds into. All seeds go into exactly one hole. Sow direction is unconstrained Capture mechanisms must be limited to one side of the board: basic captures, next, and two out. Game goal must be clear.
+Ohojichi: very similar to SameSide but the board is divided east/west instead of north/south. Most parameter restrictions from SameSide apply to Ohojichi. For Ohojichi, if UDIR_HOLES is used, all holes must be UDIR; capture side must be BOTH.</t>
+  </si>
+  <si>
+    <t>Additional child creation requirements may be set. These are in addition to location restrictions specified by CHILD_LOCS.
+- NONE: no additional restrictions.
+- OPP_ONLY:  Only make children on the opposite side of the board. Incompatible with BULL, QUR, and WEG child types.
+- OWN_ONLY: Only make children on own side of the board.  Incompatible with BULL, QUR, and WEG child types.
+- NOT_1ST_OPP: Don't make a child in the first hole on the opponents side/territory with one seed.</t>
+  </si>
+  <si>
+    <t>When crosscapt is set, defines what to do with the single seed initiating the cross capture.
+- LEAVE: always leave the single seed
+- PICK_ON_CAPT: only pick (capture) the seed if there was a capture
+- ALWAYS_PICK: always pick (capture) the final single seed, even if there was not a capture</t>
+  </si>
+  <si>
+    <t>Only meaningful with MULTICAPT. Captures are done in the same direction as the sowing, i.e. following the final hole sown. If not set, captures are done from the holes just sown.</t>
+  </si>
+  <si>
+    <t>Allows specifying non-all-equal start patterns. The following patterns are supported:
+- ALL_EQUAL: all holes start with the same number of seeds.
+- GAMACHA: starting from the third hold (from start player's left) place nbr_seeds in every other hole, the first move is prescribed move the center hole's seeds to the other side (this is done automatically).
+- ALTERNATES: every other hole is filled with nbr_seeds, no seeds end up opposite each other. If a player has fewer seeds than their opponent, then they start.
+- ALTS_WITH_1: like Alternates except the starter's 2nd from right hole with nbr_seeds is replaced with one seed.
+- CLIPPEDTRIPLES: pattern of 0 S S (where S is nbr_seeds) is used to fill the holes; if a full cycle of 3 cannot be placed, the holes are left empty. The True and False sides are the same from the player's perspective, e.g. they will look reversed when viewed from one side of the game board.
+- TWOEMPTY: all but the rightmost two holes for each player are filled with is nbr_seeds.
+- RANDOM: the total seeds are computed as (10 * holes) + (2 * nbr_start). The seeds are randomly distributed into all holes.</t>
+  </si>
+  <si>
+    <t>The first sow of the game maybe defined by a specific rule. Prescribed openings are different than start patterns because the player may choose the sow start point. SOW_OWN_STORE and SOW_RULE are ignored during the prescribed openings.
+- NONE: there is no prescribed opening move.
+- BASIC_SOWER: the first sow is a very basic pickup the seeds and drop them one at a time in each hole ignoring any other sow parameters. Other sow parameters will be enacted  afterward. This can be used to force the first sow of an MLAPS game to be a single sow. 
+- MLAPS_SOWER: the first sow follows basic rules of multi-lap sowing (LAPPER). Other sow parameters will be enacted  afterward. 
+- SOW1OPP: at least one seed must be sown on the opponents side of the board which is accomplished by sowing as normal until the final seed, then any remaining holes on the player's side are skipped and the last seed is sown in the opponents first hole (based on current sow direction).
+- PLUS1MINUS1: proceed from the selected hole by moving one seed from the next hole into the following hole, next skip that hole and repeat moving seed forward. After cycling the board, capture across from the opening hole. 
+- ARNGE_LIMIT: the first move may be used to rearrange the seeds (opponent is same layout). If the first move is not used for rearrangement, captures and child creation are not allowed from the starter until the second player makes a child or captures.</t>
+  </si>
+  <si>
+    <t>A grandslam is when your opponent has seeds at the start of your turn and you capture them all. This option selects what to do:
+- LEGAL: the seeds are captured
+- NOT_LEGAL: you may not capture all of your opponents seeds, a move which would do so is not allowed
+- NO_CAPT: you may sow the seeds, but the capture is not performed
+- OPP_GETS_REMAIN: if you capture all your opponents seeds, they capture all of your remaining seeds and the game is over. Winner is determined by game goal. Seeds picked because of PICKEXTRA PICK*LASTSEEDS go the current player and not the opponent.
+- LEAVE_LEFT: the capture is performed from all but the leftmost hole from the sower perspective. This might leave your opponents without seeds or might not capture any seeds.
+- LEAVE_RIGHT: the capture is performed from all but the rightmost hole from the sower perspective. This might leave your opponents without seeds.</t>
+  </si>
+  <si>
+    <t>The round fill method determines which holes are filled and how many seeds they are filled with when setting up for a new round.
+Several round fill mechanisms use the same general approach called the Empty Hole Method. The loser of the previous round will end up with empty holes. These holes are not playable if BLOCKS are used; otherwise they are playable. This method is not used for RND_* GOAL games.
+The seeds each player accumulated in the previous round are distributed into holes with exactly the same number in each. That number of seeds is NBR_START. The winner will fill all of their holes and put any remaining seeds into their own store. The loser will fill as many holes as they can with nbr_start seeds and put any remaining seeds (fewer than nbr_start) into their own store.
+LEFT_FILE, RIGHT_FILL and OUTSIDE_FILL define which holes that the loser must fill. UCHOOSE allows the loser to choose which holes have seeds.
+- NOT_APPLICABLE: round fill doesn't need to be specified: either the game not played in rounds (CLEAR &amp; DEPRIVE games included) or game goal is TERRITORY  without UCHOWN (see below, all holes filled).
+- LEFT_FILL: fill the round loser's holes from the player's left with nbr_start seeds each.  
+- RIGHT_FILL: fill the round loser's holes from the player's right with nbr_start seeds each. 
+- OUTSIDE_FILL: fill the round loser's holes from the outside ends toward the middle with nbr_start seeds each. Leftmost, rightmost, 2nd leftmost, 2nd rightmost, etc. until the seeds are used up.
+- EVEN_FILL: fill all holes (both sides) with the same number of seeds; determined by dividing the losers seeds by the number of holes per side. If that is not playable based on the minimum number of seeds required for a move (MIN_MOVE); extra seeds are put in each players leftmost hole. Any extra seeds are put in each player's store.
+- SHORTEN: the number of holes that the round loser can fill with NBR_START seeds are fill on both sides, other holes are left empty. Holes are filled opposite each other. If BLOCKS is selected, the board is shortened to the number of holes filled (empty holes are blocked and out of play). If the game uses children, they will not be created if the board size is reduced to 3 or less.
+- UCHOOSE: allow user to choose which holes have seeds (are not blocked) when ROUNDS and BLOCKS are used.
+- UMOVE: allow the loser to choose where seeds are placed. At least one seed must be placed in each hole and the game must be playable (at least one hole has MIN_MOVE seeds), remaining seeds are placed in the store. The winner's layout is the same layout but reflected.
+- UCHOWN: The only round fill supported for territory games. The winner may choose which holes they control.</t>
+  </si>
+  <si>
+    <t>Bias for the Monte Carlo Tree search algorithm for each difficulty level (0-3).  A larger bias encourages move game tree exploration, but defocuses the exploration from the best choices. This is critical in avoiding getting stuck in sub-optimal move choices.
+Value is divided by 1000.</t>
+  </si>
+  <si>
+    <t>If the game is being played on easy mode (game difficult of easy/0), a random value may be added to the static evaluation. This can be done to induce errors into the ai player's game play. A random value is selected between -easy_rand and + easy_rand.
+The specific value for this should be selected based on the ranges of the parameters and multiplier.
+Used only for minimax &amp; negamax players.</t>
+  </si>
+  <si>
+    <t>Determines if seeds from more the start hole are picked up and sown:
+- OFF: Single lap sowing. Seeds from the start hole are sown, typically, one per hole until expended.
+- LAPPER:  If the first sow ends in a hole with more than one seed, pickup all the seeds and continue sowing another "lap". Note that lap here does not mean a full circuit of the board, only an individual sow operation. In general, sowing laps continues in this manner until the final seed of a lap reaches an empty hole. There are games with other conditions for ending a multilap low such as making a capture or making a child. 
+  + Several values of SOW_RULE perform an operation after each lap sown: SOW_CLKD_DIV(_NR) closes the final hole and CHANGE_DIR_LAP changes the direction of sowing after each lap.
+- LAPPER_NEXT:  For lapper_next sowing, the number of seeds in the last sown hole of lap do not matter. Instead, if the hole after the last sown hole has any seeds, those seeds are used to continue sowing the next lap. Sowing continues until the hole after the lap's final seed is empty. There are games with other conditions for ending a multilap low such as making a capture or making a child.
+  + A SOW_RULE of CHANGE_DIR_LAP changes the direction of sowing after each lap. SOW_BLKD_DIV(_NR) is not supported for LAPPER_NEXT.</t>
+  </si>
+  <si>
     <t>Special sow rules add additional behavior or restrictions to the sowing phase:
 - NONE: there is no special sowing rule.
-- SOW_BLKD_DIV: If the final seed of an individual sow lands on the opposite side of the board and brings the contents of that hole to goal_param seeds, the hole is closed closed (blocked). In single lap games, the hole's seeds are removed from play. In multilap games, the seeds are used to continue sowing.
+- SOW_BLKD_DIV: If the final seed of an individual sow lands on the opposite side of the board and brings the contents of that hole to goal_param seeds, the hole is closed  (blocked). In single lap games, the hole's seeds are removed from play. In multilap games, the seeds are used to continue sowing.
   + When sowing, blocked holes on your own side of the board are skipped  and blocked holes on opponent's side are diverted out of play or captured.
   +  Game GOAL must be DEPRIVE and all of the associated restrictions apply. NOCAPTMOVES maybe used to prevent closing holes on the initial games moves. Capture mechanisms other than closing holes are not supported. The minimum move must be 1 and thus SOW_START is incompatible.  ALLOW_RULE may not be used to limit allowable moves.  SKIP_START and VISIT_OPP are not supported with SOW_BLKD_DIV.  MLAPS of LAPPER_NEXT is not supported with SOW_BLKD_DIV(_NR).
 - SOW_BLKD_DIV_NR: Behaves the same as SOW_BLKD_DIV except that each player's rightmost hole cannot be closed. 
@@ -1151,53 +1196,15 @@
 - NO_SOW_OPP_2S: Don't sow into opponents holes with 2 seeds.
 - CHANGE_DIR_LAP: Change the direction for each lap sown. Generally used with UDIR_HOLES so the player may choose the first direction.
 - MAX_SOW: holes sow_param seeds are skipped when sowing. That is, holes will never contain more seeds than sow_param.
-- LAP_CAPT: after each lapt check for a capture, if there is a capture continue sowing with another lap. If a basic capture is configured (evens, capt on, max or min), the hole after the captured seeds is drawn to continue lapping.
+- LAP_CAPT: after each lap check for a capture, if there is a capture continue sowing with another lap. If a basic capture is configured (evens, capt on, max or min), the hole after the captured seeds is drawn to continue lapping.
 - NO_OPP_CHILD: do not sow into your opponents children.</t>
-  </si>
-  <si>
-    <t>capt_type</t>
-  </si>
-  <si>
-    <t>Capture Type</t>
-  </si>
-  <si>
-    <t>CaptType</t>
-  </si>
-  <si>
-    <t>Allows specifing non-all-equal start patterns. The following patterns are supported:
-- ALL_EQUAL: all holes start with the same number of seeds.
-- GAMACHA: starting from the third hold (from start player's left) place nbr_seeds in every other hole, the first move is prescribed move the center hole's seeds to the other side (this is done automatically).
-- ALTERNATES: everyother hole is filled with nbr_seeds, no seeds end up opposite eachother. If a player has fewer seeds than their opponent, then they start.
-- ALTS_WITH_1: like Alternates except the starter's 2nd from right hole with nbr_seeds is replaced with one seed.
-- CLIPPEDTRIPLES: pattern of 0 S S (where S is nbr_seeds) is used to fill the holes; if a full cycle of 3 cannot be placed, the holes are left empty. The True and False sides are the same from the player's perspective, e.g. they will look reversed when viewed from one side of the game board.
-- TWOEMPTY: all but the rightmost two holes for each player are filled with is nbr_seeds.
-- RANDOM: the total seeds are computed as (10 * holes) + (2 * nbr_start). The seeds are randomly distributed into all holes.</t>
-  </si>
-  <si>
-    <t>Capture type.
-- NONE: No other capture type.
-- NEXT: Capture from the hole after the final seed sown. Basic capture rules are applied; capture side is checked; and multiple captures in either direction are supported.
-  + When multiple lap sowing, the sowing does not stop for captures. Instead, sowing continues until the final seed is sown into an empty hole. Then the capture test is made on the next hole.
-- TWO_OUT: Basic capture rules and capture side are ignored. There are three flavors of capture two out:
-  + Single lap game: capture if sow ends in occupied hole, then an empty hole, followed by an occupied hole the contents of this are hole captured.
-  + Multi lap game but single capture: capture when last hole sown is followed by an empty hole which is then followed by an occupied hole.
-  + Multi lap game with multiple captures: capture when last hole sown is followed by an empty hole which is then followed by an occupied hole. Continue captures as long as the pattern of empty hole followed by an occupied hole continues. CAPSAMEDIR must be true. 
-- MATCH_OPP: capture when the number of seeds in the final hole sown match the opposite-side hole. Multiple captures maybe made in either direction. Multilap sowing does stop for captures.</t>
-  </si>
-  <si>
-    <t>The name of the Game Class. One of:
-Mancala: allows setting all parameters though some combinations are limited.
-Diffusion: has unique sow method and win conditions.  Players control the east/west sides of the board. The game is basically preconfigured, only the board size can be changed to any even size. Game goal must be clear.
-DiffusionV2: similar to Diffusion but players control the typical north/south sides of the board.
-SameSide: a game class in which seeds are only sown on the player's own side of the board. If a capture is made, the capturer chooses one of their opponent's holes to put the seeds into. All seeds go into exactly one hole. Sow direction is unconstrained Capture mechanisms must be limited to one side of the board: basic captures, next, and two out. Game goal must be clear.
-Ohojichi: very similar to SameSide but the board is divided east/west instead of north/south. Most parameter restrictions from SameSide apply to Ohojichi. For Ohojichi, if UDIR_HOLES is used, all holes must be UDIR; capture side must be BOTH.</t>
   </si>
   <si>
     <t xml:space="preserve">Games with children allow players to claim holes. These child holes are an extension of the stores and seeds in them count towards a win. Making a child stops any multiple lap sowing, moves cannot start from children, and they cannot be captured (except for special rules associated with WEGs).
 - NOCHILD: children are not used.
 - NORMAL: children are made when a final seeds sows a hole to CHILD_CVT. If stores are not included captures are instead moved into children, thus a player may not capture until they have created a child. 
 - ONE_CHILD: only one child allowed per player.
-  + Children must not be symmetrically opposite eachother. For example,  in a 9 hole per side game with holes numbered as follows, children may not be in the same numbered holes:
+  + Children must not be symmetrically opposite each other. For example,  in a 9 hole per side game with holes numbered as follows, children may not be in the same numbered holes:
   + 9 8 7 6 5 4 3 2 1
   + 1 2 3 4 5 6 7 8 9 
   + Used to create tuzdek style children along with CHILD_RULE of OPP_ONLY.
@@ -1205,13 +1212,6 @@
 - BULL: create one bull if final seed sows to CHILD_CVT, create two bulls if the final two seeds are sown to CHILD_CVT-1 and CHILD_CVT (in either order).
 - QUR: when a seed is sown into an empty hole on the player's side of the board and the opposite hole contains CHILD_CVT, create children in both holes: final seed location and opposite.
 </t>
-  </si>
-  <si>
-    <t>Additional child creation requirements may be set. These are in addition to location restrictions specified by CHILD_LOCS.
-- NONE: no additional restrictions.
-- OPP_ONLY:  Only make children on the opposite side of the board. Incompatible with BULL, QUR, and WEG child types.
-- OWN_ONLY: Only make children on own side of the board.  Incompatible with BULL, QUR, and WEG child types.
-- NOT_1ST_OPP: Don't make a child in the first hole on the opponents side/territory with one seed.</t>
   </si>
 </sst>
 </file>
@@ -2096,8 +2096,8 @@
   <dimension ref="A1:J87"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A43" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J86" sqref="J86"/>
+      <pane ySplit="1" topLeftCell="A82" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F86" sqref="F86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2152,17 +2152,17 @@
         <v>90</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3">
         <v>0</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
       <c r="G2" s="5" t="s">
         <v>84</v>
@@ -2204,7 +2204,7 @@
         <v>0</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -2236,7 +2236,7 @@
         <v>0</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -2268,7 +2268,7 @@
         <v>0</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -2300,7 +2300,7 @@
         <v>0</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -2308,16 +2308,16 @@
         <v>90</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>265</v>
+        <v>258</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>266</v>
+        <v>259</v>
       </c>
       <c r="E7" s="3">
         <v>0</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
       <c r="G7" s="5" t="s">
         <v>84</v>
@@ -2358,7 +2358,7 @@
         <v>0</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -2390,7 +2390,7 @@
         <v>0</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>238</v>
+        <v>307</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2430,19 +2430,19 @@
         <v>90</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
       <c r="E11" s="3">
         <v>0</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>264</v>
+        <v>257</v>
       </c>
       <c r="H11" s="3">
         <v>9</v>
@@ -2456,10 +2456,10 @@
         <v>90</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>310</v>
+        <v>301</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>311</v>
+        <v>302</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>22</v>
@@ -2468,7 +2468,7 @@
         <v>106</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>312</v>
+        <v>303</v>
       </c>
       <c r="G12" s="5" t="s">
         <v>159</v>
@@ -2480,7 +2480,7 @@
         <v>0</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>314</v>
+        <v>304</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -2488,7 +2488,7 @@
         <v>90</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>111</v>
@@ -2497,7 +2497,7 @@
         <v>0</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
       <c r="G13" s="5" t="s">
         <v>84</v>
@@ -2538,7 +2538,7 @@
         <v>2</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>285</v>
+        <v>278</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2570,7 +2570,7 @@
         <v>2</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>211</v>
+        <v>308</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -2578,16 +2578,16 @@
         <v>90</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>267</v>
+        <v>260</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
       <c r="E16" s="3">
         <v>0</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
       <c r="G16" s="5" t="s">
         <v>84</v>
@@ -2604,10 +2604,10 @@
         <v>90</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>22</v>
@@ -2628,7 +2628,7 @@
         <v>2</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -2636,10 +2636,10 @@
         <v>90</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>291</v>
+        <v>284</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>292</v>
+        <v>285</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>22</v>
@@ -2648,10 +2648,10 @@
         <v>130</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>293</v>
+        <v>286</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>294</v>
+        <v>287</v>
       </c>
       <c r="H18" s="3">
         <v>5</v>
@@ -2660,7 +2660,7 @@
         <v>2</v>
       </c>
       <c r="J18" s="4" t="s">
-        <v>295</v>
+        <v>288</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
@@ -2724,7 +2724,7 @@
         <v>2</v>
       </c>
       <c r="J20" s="4" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -2732,16 +2732,16 @@
         <v>90</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>269</v>
+        <v>262</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>270</v>
+        <v>263</v>
       </c>
       <c r="E21" s="3">
         <v>0</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
       <c r="G21" s="5" t="s">
         <v>84</v>
@@ -2814,7 +2814,7 @@
         <v>2</v>
       </c>
       <c r="J23" s="4" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="409.5" x14ac:dyDescent="0.25">
@@ -2846,7 +2846,7 @@
         <v>0</v>
       </c>
       <c r="J24" s="4" t="s">
-        <v>302</v>
+        <v>295</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="105" x14ac:dyDescent="0.25">
@@ -2854,10 +2854,10 @@
         <v>36</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>22</v>
@@ -2878,7 +2878,7 @@
         <v>0</v>
       </c>
       <c r="J25" s="4" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="120" x14ac:dyDescent="0.25">
@@ -2886,10 +2886,10 @@
         <v>36</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>287</v>
+        <v>280</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>22</v>
@@ -2898,10 +2898,10 @@
         <v>147</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>288</v>
+        <v>281</v>
       </c>
       <c r="G26" s="5" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="H26" s="3">
         <v>2</v>
@@ -2910,7 +2910,7 @@
         <v>0</v>
       </c>
       <c r="J26" s="4" t="s">
-        <v>290</v>
+        <v>283</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
@@ -2918,16 +2918,16 @@
         <v>36</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="E27" s="3">
         <v>0</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
       <c r="G27" s="5" t="s">
         <v>84</v>
@@ -2968,7 +2968,7 @@
         <v>0</v>
       </c>
       <c r="J28" s="4" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="180" x14ac:dyDescent="0.25">
@@ -3000,7 +3000,7 @@
         <v>0</v>
       </c>
       <c r="J29" s="4" t="s">
-        <v>216</v>
+        <v>310</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
@@ -3008,16 +3008,16 @@
         <v>36</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>282</v>
+        <v>275</v>
       </c>
       <c r="E30" s="3">
         <v>0</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
       <c r="G30" s="5" t="s">
         <v>84</v>
@@ -3090,7 +3090,7 @@
         <v>0</v>
       </c>
       <c r="J32" s="4" t="s">
-        <v>300</v>
+        <v>293</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3122,7 +3122,7 @@
         <v>2</v>
       </c>
       <c r="J33" s="4" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
@@ -3154,7 +3154,7 @@
         <v>2</v>
       </c>
       <c r="J34" s="4" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
@@ -3162,16 +3162,16 @@
         <v>36</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>284</v>
+        <v>277</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>283</v>
+        <v>276</v>
       </c>
       <c r="E35" s="3">
         <v>0</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
       <c r="G35" s="5" t="s">
         <v>84</v>
@@ -3244,7 +3244,7 @@
         <v>2</v>
       </c>
       <c r="J37" s="4" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
     </row>
     <row r="38" spans="1:10" ht="150" x14ac:dyDescent="0.25">
@@ -3276,7 +3276,7 @@
         <v>2</v>
       </c>
       <c r="J38" s="4" t="s">
-        <v>240</v>
+        <v>311</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
@@ -3284,16 +3284,16 @@
         <v>36</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="E39" s="3">
         <v>0</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
       <c r="G39" s="5" t="s">
         <v>84</v>
@@ -3325,7 +3325,7 @@
         <v>42</v>
       </c>
       <c r="G40" s="5" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="H40" s="3">
         <v>8</v>
@@ -3334,7 +3334,7 @@
         <v>2</v>
       </c>
       <c r="J40" s="4" t="s">
-        <v>301</v>
+        <v>294</v>
       </c>
     </row>
     <row r="41" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -3398,7 +3398,7 @@
         <v>2</v>
       </c>
       <c r="J42" s="4" t="s">
-        <v>303</v>
+        <v>312</v>
       </c>
     </row>
     <row r="43" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -3430,7 +3430,7 @@
         <v>2</v>
       </c>
       <c r="J43" s="4" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="150" x14ac:dyDescent="0.25">
@@ -3462,7 +3462,7 @@
         <v>0</v>
       </c>
       <c r="J44" s="4" t="s">
-        <v>315</v>
+        <v>305</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
@@ -3654,7 +3654,7 @@
         <v>0</v>
       </c>
       <c r="J50" s="4" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
@@ -3686,7 +3686,7 @@
         <v>0</v>
       </c>
       <c r="J51" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
@@ -3718,7 +3718,7 @@
         <v>0</v>
       </c>
       <c r="J52" s="4" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
@@ -3726,16 +3726,16 @@
         <v>118</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="E53" s="3">
         <v>0</v>
       </c>
       <c r="F53" s="3" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
       <c r="G53" s="5" t="s">
         <v>84</v>
@@ -3767,7 +3767,7 @@
         <v>87</v>
       </c>
       <c r="G54" s="3" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="H54" s="3">
         <v>6</v>
@@ -3776,7 +3776,7 @@
         <v>0</v>
       </c>
       <c r="J54" s="4" t="s">
-        <v>200</v>
+        <v>313</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
@@ -3799,7 +3799,7 @@
         <v>87</v>
       </c>
       <c r="G55" s="3" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="H55" s="3">
         <v>7</v>
@@ -3848,16 +3848,16 @@
         <v>118</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>256</v>
+        <v>249</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
       <c r="E57" s="3">
         <v>0</v>
       </c>
       <c r="F57" s="3" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
       <c r="G57" s="5" t="s">
         <v>84</v>
@@ -3889,7 +3889,7 @@
         <v>87</v>
       </c>
       <c r="G58" s="3" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="H58" s="3">
         <v>2</v>
@@ -3898,7 +3898,7 @@
         <v>2</v>
       </c>
       <c r="J58" s="4" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="59" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -3909,7 +3909,7 @@
         <v>119</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="D59" s="3" t="s">
         <v>120</v>
@@ -3930,7 +3930,7 @@
         <v>2</v>
       </c>
       <c r="J59" s="4" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="60" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -3941,7 +3941,7 @@
         <v>121</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="D60" s="3" t="s">
         <v>120</v>
@@ -3962,7 +3962,7 @@
         <v>2</v>
       </c>
       <c r="J60" s="4" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="61" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3973,7 +3973,7 @@
         <v>122</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="D61" s="3" t="s">
         <v>120</v>
@@ -3994,7 +3994,7 @@
         <v>2</v>
       </c>
       <c r="J61" s="4" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
     </row>
     <row r="62" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -4005,7 +4005,7 @@
         <v>123</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="D62" s="3" t="s">
         <v>120</v>
@@ -4026,7 +4026,7 @@
         <v>2</v>
       </c>
       <c r="J62" s="4" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="63" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -4037,7 +4037,7 @@
         <v>124</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="D63" s="3" t="s">
         <v>120</v>
@@ -4058,7 +4058,7 @@
         <v>2</v>
       </c>
       <c r="J63" s="4" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="64" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -4069,7 +4069,7 @@
         <v>125</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="D64" s="3" t="s">
         <v>120</v>
@@ -4090,7 +4090,7 @@
         <v>2</v>
       </c>
       <c r="J64" s="4" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="65" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -4101,7 +4101,7 @@
         <v>128</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="D65" s="3" t="s">
         <v>120</v>
@@ -4122,7 +4122,7 @@
         <v>2</v>
       </c>
       <c r="J65" s="4" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="66" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -4154,7 +4154,7 @@
         <v>2</v>
       </c>
       <c r="J66" s="4" t="s">
-        <v>203</v>
+        <v>314</v>
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.25">
@@ -4264,7 +4264,7 @@
         <v>81</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
       <c r="D71" s="3" t="s">
         <v>22</v>
@@ -4285,7 +4285,7 @@
         <v>0</v>
       </c>
       <c r="J71" s="8" t="s">
-        <v>231</v>
+        <v>315</v>
       </c>
     </row>
     <row r="72" spans="1:10" ht="165" x14ac:dyDescent="0.25">
@@ -4317,7 +4317,7 @@
         <v>0</v>
       </c>
       <c r="J72" s="4" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
     </row>
     <row r="73" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -4349,7 +4349,7 @@
         <v>0</v>
       </c>
       <c r="J73" s="4" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.25">
@@ -4357,16 +4357,16 @@
         <v>66</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
       <c r="E74" s="3">
         <v>0</v>
       </c>
       <c r="F74" s="3" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
       <c r="G74" s="5" t="s">
         <v>84</v>
@@ -4418,7 +4418,7 @@
         <v>76</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
       <c r="D76" s="3" t="s">
         <v>22</v>
@@ -4439,7 +4439,7 @@
         <v>0</v>
       </c>
       <c r="J76" s="4" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
     </row>
     <row r="77" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -4471,7 +4471,7 @@
         <v>0</v>
       </c>
       <c r="J77" s="4" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
     </row>
     <row r="78" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -4535,7 +4535,7 @@
         <v>0</v>
       </c>
       <c r="J79" s="4" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="80" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -4543,10 +4543,10 @@
         <v>66</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>296</v>
+        <v>289</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>297</v>
+        <v>290</v>
       </c>
       <c r="D80" s="3" t="s">
         <v>22</v>
@@ -4555,7 +4555,7 @@
         <v>133</v>
       </c>
       <c r="F80" s="3" t="s">
-        <v>298</v>
+        <v>291</v>
       </c>
       <c r="G80" s="5" t="s">
         <v>159</v>
@@ -4567,7 +4567,7 @@
         <v>0</v>
       </c>
       <c r="J80" s="4" t="s">
-        <v>299</v>
+        <v>292</v>
       </c>
     </row>
     <row r="81" spans="1:10" ht="409.5" x14ac:dyDescent="0.25">
@@ -4599,7 +4599,7 @@
         <v>0</v>
       </c>
       <c r="J81" s="4" t="s">
-        <v>309</v>
+        <v>316</v>
       </c>
     </row>
     <row r="82" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -4607,10 +4607,10 @@
         <v>66</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="D82" s="3" t="s">
         <v>22</v>
@@ -4631,7 +4631,7 @@
         <v>0</v>
       </c>
       <c r="J82" s="4" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.25">
@@ -4639,16 +4639,16 @@
         <v>66</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="E83" s="3">
         <v>0</v>
       </c>
       <c r="F83" s="3" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
       <c r="G83" s="5" t="s">
         <v>84</v>
@@ -4689,7 +4689,7 @@
         <v>2</v>
       </c>
       <c r="J84" s="4" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
     </row>
     <row r="85" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -4753,7 +4753,7 @@
         <v>2</v>
       </c>
       <c r="J86" s="4" t="s">
-        <v>317</v>
+        <v>306</v>
       </c>
     </row>
     <row r="87" spans="1:10" ht="405" x14ac:dyDescent="0.25">
@@ -4761,10 +4761,10 @@
         <v>66</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>304</v>
+        <v>296</v>
       </c>
       <c r="C87" s="3" t="s">
-        <v>305</v>
+        <v>297</v>
       </c>
       <c r="D87" s="3" t="s">
         <v>22</v>
@@ -4773,10 +4773,10 @@
         <v>112</v>
       </c>
       <c r="F87" s="3" t="s">
-        <v>306</v>
+        <v>298</v>
       </c>
       <c r="G87" s="3" t="s">
-        <v>307</v>
+        <v>299</v>
       </c>
       <c r="H87" s="3">
         <v>7</v>
@@ -4785,7 +4785,7 @@
         <v>2</v>
       </c>
       <c r="J87" s="4" t="s">
-        <v>308</v>
+        <v>300</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Move the parameter descriptions out of the spread sheet and into a stand-alone text file <param tags used to identify parameter descriptions. Did spelling/grammar checking on the descriptions. Move the code to read the parameter files to man_config. Added additional error checking and raise exceptions instead of doing a print that could be missed. Updated makefile with new dependencies.
</commit_message>
<xml_diff>
--- a/src/game_params.xlsx
+++ b/src/game_params.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Activity_Data\Mancala_github\MancalaGames\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DE9A3B5-9D9F-4288-9B7A-026FB3234806}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C25E4685-125A-4291-9EE7-D0AA49254DAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6330" yWindow="360" windowWidth="20520" windowHeight="15510" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="game_params" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">game_params!$A$1:$J$87</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">game_params!$A$1:$I$83</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="318">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="239">
   <si>
     <t>tab</t>
   </si>
@@ -62,27 +62,9 @@
     <t>col</t>
   </si>
   <si>
-    <t>description</t>
-  </si>
-  <si>
-    <t>skip</t>
-  </si>
-  <si>
-    <t>nbr_holes</t>
-  </si>
-  <si>
     <t>int</t>
   </si>
   <si>
-    <t>An init only parameter that is used to check the other parameters in the creation of game info.</t>
-  </si>
-  <si>
-    <t>rules</t>
-  </si>
-  <si>
-    <t>RuleDict</t>
-  </si>
-  <si>
     <t>Game</t>
   </si>
   <si>
@@ -227,9 +209,6 @@
     <t>1</t>
   </si>
   <si>
-    <t>The minimum number of seeds a hole must have for it to be an allowable move start hole.</t>
-  </si>
-  <si>
     <t>mustshare</t>
   </si>
   <si>
@@ -257,9 +236,6 @@
     <t>Sow Start Hole</t>
   </si>
   <si>
-    <t>When selected, the first seed is sown into  (i.e. left in) the start hole.</t>
-  </si>
-  <si>
     <t>move_one</t>
   </si>
   <si>
@@ -305,9 +281,6 @@
     <t>[]</t>
   </si>
   <si>
-    <t>udirect</t>
-  </si>
-  <si>
     <t>Capture</t>
   </si>
   <si>
@@ -345,9 +318,6 @@
   </si>
   <si>
     <t>No Single Seed Capture</t>
-  </si>
-  <si>
-    <t>If the selected start hole contains one seed, no capture may be made with it.</t>
   </si>
   <si>
     <t>crosscapt</t>
@@ -438,9 +408,6 @@
 Capture on evens. </t>
   </si>
   <si>
-    <t>An init only parameter that used to check the consistency of the game info. Errors and warnings are raised as the rules are processed.</t>
-  </si>
-  <si>
     <t>GameClasses</t>
   </si>
   <si>
@@ -504,10 +471,6 @@
     <t>ChildType</t>
   </si>
   <si>
-    <t xml:space="preserve">Defines the number of seeds required to make a child.
-</t>
-  </si>
-  <si>
     <t>allow_rule</t>
   </si>
   <si>
@@ -526,15 +489,6 @@
     <t>OFF</t>
   </si>
   <si>
-    <t>mlength</t>
-  </si>
-  <si>
-    <t>A derived parameter. Do not include in config files. Set during game construction to True if any udir holes are set.</t>
-  </si>
-  <si>
-    <t>A derived parameter. Do not include in config files. Set during game construction length of moves: 1 (int) or 2, 3 (tuple).</t>
-  </si>
-  <si>
     <t>capt_rturn</t>
   </si>
   <si>
@@ -604,131 +558,6 @@
     <t>NOT_APPLICABLE</t>
   </si>
   <si>
-    <t>Defines which player starts 2nd and subsequent rounds:
-- ALTERNATE: the round starter alternates.
-- LOSER: the loser of the previous round starts the current round.
-- WINNER: the winner of the previous round starts the current round.
-- LAST_MOVER: the player that made the last move of the previous round, starts the new round.</t>
-  </si>
-  <si>
-    <t>An html help file describing the game (mancala_help.html is the main help file).</t>
-  </si>
-  <si>
-    <t>The game name, may have spaces. Used for the window title and the filename (with spaces replaced with underscores).</t>
-  </si>
-  <si>
-    <t>The number of seeds in each hole at the start of a game when START_PATTERN is ALL_EQUAL. Other sow patterns use this as the number of seeds for some holes in the associated patterns.</t>
-  </si>
-  <si>
-    <t>A description of the game, typically enough to remind the player what the game options are.
-New lines can be inserted with \n.</t>
-  </si>
-  <si>
-    <t>Number of holes on each side of the board.</t>
-  </si>
-  <si>
-    <t>When a player has no allowable moves on their turn, they must pass, and continue to do so until they have allowable moves or the game is over. The game is over when there is a clear winner or tie condition, or when neither player has an allowable move.</t>
-  </si>
-  <si>
-    <t>Only valid when SOW_START is set. Changes the SOW_START behavior so that if there is only one seed in the hole, it is moved in the sow direction by one hole.</t>
-  </si>
-  <si>
-    <t>Repeat turn if there was a capture. Making children is not a capture.</t>
-  </si>
-  <si>
-    <t>Only allow cross capture if the player has sown onto the opposite side of board. 
-If a player ends on their own side of the board in an empty hole, but did not sow any opposite hole, they get a repeat turn.</t>
-  </si>
-  <si>
-    <t>Number of end games played out from each expanded node. One value for each difficulty level (0-3).</t>
-  </si>
-  <si>
-    <t>Number of game tree expansions to perform each time we pick a new move. One value for each difficulty level (0-3).</t>
-  </si>
-  <si>
-    <t>The default difficulty for the game. The difficulty can be changed at play time,  even during game play, in the Mancala UI.</t>
-  </si>
-  <si>
-    <t>Automatically activate the AI player. The AI player can be manually deactivated, but it is selected for the starter it will start the game.</t>
-  </si>
-  <si>
-    <t>The multiplier for the even scorer. The even scorer counts the number of holes with an even number of seeds. This is useful to use when the capture mechanism is evens.
-Used only for minimax &amp; negamax players.</t>
-  </si>
-  <si>
-    <t>The multiplier for the child scorer. The child scorer counts the number children each player has.
-The child scorer may only be used on games with children. If the game does not include child the multiplier must be zero.
-Used only for the minimax &amp; negamax players.</t>
-  </si>
-  <si>
-    <t>The multiplier for the empties scorer. The empties scorer counts the number empty holes each player has on the board.
-Used only for minimax &amp; negamax players.</t>
-  </si>
-  <si>
-    <t>The multiplier for the access scorer. The access scorer computes how many of the opponents holes can be accessed for the given game state.
-The access scorer is slow and therefore is prohibited from being used in multilap games (MLAPS); games with user choice of move direction (UDIR_HOLES); and games where hole owners are not predefined (NO_SIDES). In these game configurations, the multiplier must be zero to disable the access scorer.
-Used only for minimax &amp; negamax players.</t>
-  </si>
-  <si>
-    <t>A value used to encourage or discourage repeat turns. The value is added in for the current player and subtracted off the score for the opposing playing. Use a positive value to encourage the AI player to repeat turns.
-This parameter may only be used for games in which repeated turns are possible (SOW_OWN_STORE, CAPT_RTURN or XC_SOWN).
-Used only for minimax &amp; negamax players.</t>
-  </si>
-  <si>
-    <t>The multiplier for the stores scorer. Seeds in stores and children are included.
-The stores scorer may not be used in games without STORES or CHILDREN. A zero multiplier disables the stores scorer.
-Used only for  minimax &amp; negamax players.</t>
-  </si>
-  <si>
-    <t>The depth that the minimaxer or negamaxer will search the game tree from the current node. One value for each difficulty.</t>
-  </si>
-  <si>
-    <t>Capture when a hole contains an even number of seeds, greater than 0. When selected with other basic capture mechanisms, the capture mechanism are ANDed (all must be true for capture). Basic capture mechanisms are: CAPT_MAX, CAPT_MIN, CAPT_ON and EVENS with restrictions from OPPSIDECAPT, MOVEUNLOCK and not child holes of any type.
-MLAPS LAPPER sowing will stop the sowing on a final seed that would capture based on the selected basic capture mechanisms.
-Either SOW_RULE of OWN_SOW_CAPT_ALL or SOW_SOW_CAPT_ALL includes the basic capture mechanisms.</t>
-  </si>
-  <si>
-    <t>If the last sown seed is put in an empty hole, seeds on the opposite side of the board are captured. The capture of those seeds can be limited by CAPT_MAX, CAPT_MIN, CAPT_ON, EVENS, MOVEUNLOCK, OPPSIDECAPT. For example, crosscapt with evens will only capture when there are an even number of seeds in the opposite hole.
-SOW_RULE of either SOW_CAPT_ALL do not do this capture.</t>
-  </si>
-  <si>
-    <t>Holes in the game start each game and round locked. Captures may not be made from locked holes. Starting a sow from a hole unlocks it allowing future captures.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Requires MLAPS. If the first 'lap' does not reach the opponent's side of the board, the sowing ends after the first lap. </t>
-  </si>
-  <si>
-    <t>When sowing a second or subsequent circuit of the board, skip the start hole. This will leave the start hole empty for single lap games.
-In multilap games, the start hole for the current lap is skipped. Second or subsequent laps may sow into the original start hole.</t>
-  </si>
-  <si>
-    <t>The multiplier for the seeds scorer. The seeds scorer computes how many seeds each player has on the game board that are not in children.
-Used only for minimax &amp; negamax players.</t>
-  </si>
-  <si>
-    <t>A list of holes from which the user can choose the sow direction. Control is via the mouse button: left is clockwise and right is counter-clockwise.
-Note: all holes respond to both mouse buttons, but if the hole is not in udir_holes, the sow direction will be that prescribed by sow_direct with either button.
-Games with any hole set to user chooses direction must not use MUSTSHARE; GRANDSLAM must be LEGAL; and no special ALLOW_RULE is supported.</t>
-  </si>
-  <si>
-    <t>Direction of sow:
-- CW: clockwise
-- SPLIT: left side holes sow counter-clockwise and right side holes sow clockwise, an odd middle hole must be set in UDIR_HOLES.
-- CCW: counter-clockwise
-- PLAYALTDIR: on the first move of the game, the first player chooses their sow direction using the UDIR_HOLES method (by mouse button). The second player will sow their moves in the opposite direction. Once the first player makes their first move, both player's sow directions are set for the duration of the game no matter which button is used.  All UDIR_HOLES will apply to the game configuration.
-Both mouse buttons will start a move no matter the sow direction. If the hole is marked as UDIR_HOLES, the button selects sow direction. On the other hand, if the hole is not marked as UDIR_HOLES, either button will sow in the prescribed direction. This can be useful, mechanism to remind yourself that on SPLIT sow, the left holes go CW by using the left button and the right holes go CCW by using the right button.
-When PLAYALTDIR is not selected, any hole can be set as UDIR_HOLES to allow the user to override the sow_direct setting.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Moves maybe made from any hole, independent of the side of the board. Moves need to specify side, position and directions.  </t>
-  </si>
-  <si>
-    <t>If an opponent has no moves at the start of your turn, you must make seeds available to them if you can. This condition is enforced by only activating holes on the UI which will make seeds available to the opponent.</t>
-  </si>
-  <si>
-    <t>Sow seeds into your own store when passing it. Do not sow into your opponents store. When the final seed is sown into the store, the sower gets another turn.</t>
-  </si>
-  <si>
     <t>Evens Multiplier</t>
   </si>
   <si>
@@ -747,18 +576,6 @@
     <t>Stores (captured) Multiplier</t>
   </si>
   <si>
-    <t>The algorithm value is the name of the AI player algorithm (a string):
-minimaxer: an Alpha-Beta Pruning MiniMaxer
-negamaxer: minimaxer with a very minor optimization for alternating turn games (no repeat turns). Uses minimaxer depths for difficulties.
-montecarlo_ts: a Monte Carlo Tree Search player.</t>
-  </si>
-  <si>
-    <t>Capture when the contents of the hole is in the capt_on list. The Mancala Games UI only has checkboxes for 1 to 5 seeds, but any number may be put into the configuration file.
-When selected with other basic capture mechanisms, the capture mechanism are ANDed (all must be true for capture). Basic capture mechanisms are: CAPT_MAX, CAPT_MIN, CAPT_ON and EVENS   with restrictions from OPPSIDECAPT, MOVEUNLOCK and not child holes of any type.
-MLAP LAPPER sowing will stop the sowing on a final seed that would capture based on the selected basic capture mechanisms.
-Either SOWRULE of OWN_SOW_CAPT_ALL or SOW_SOW_CAPT_ALL includes the basic capture mechanisms.</t>
-  </si>
-  <si>
     <t>[100, 300, 500, 800]</t>
   </si>
   <si>
@@ -768,69 +585,27 @@
     <t>[300, 200, 100, 100]</t>
   </si>
   <si>
-    <t>Capture when the contents of the hole are greater than or equal to capt_min. Disable with 0 value.
-When selected with other basic capture mechanisms, the capture mechanism are ANDed (all must be true for capture). Basic capture mechanisms are: CAPT_MAX, CAPT_MIN, CAPT_ON and EVENS  with restrictions from OPPSIDECAPT, MOVEUNLOCK and not child holes of any type.
-MLAP LAPPER sowing will stop the sowing on a final seed that would capture based on the selected basic capture mechanisms.
-Either SOW_RULE of OWN_SOW_CAPT_ALL or SOW_SOW_CAPT_ALL includes the basic capture mechanisms.</t>
-  </si>
-  <si>
-    <t>Capture when the contents of the hole are less than or equal to capt_max.  Disable with 0 value.
-When selected with other basic capture mechanisms, the capture mechanism are ANDed (all must be true for capture). Basic capture mechanisms are: CAPT_MAX, CAPT_MIN, CAPT_ON and EVENS  with restrictions from OPPSIDECAPT, MOVEUNLOCK and not child holes of any type.
-MLAPS LAPPER sowing will stop the sowing on a final seed that would capture based on the selected basic capture mechanisms.
-Either SOW_RULE of OWN_SOW_CAPT_ALL or SOW_SOW_CAPT_ALL includes the basic capture mechanisms.</t>
-  </si>
-  <si>
-    <t>Rules to allow taking of more than otherwise captured or picked seeds:
-- NONE: Nothing extra
-- PICKCROSS: Take the seeds from the opposite side of the board. 
-- PICKTWOS: Take seeds from opponents holes containing two seeds.
-- PICKLASTSEEDS: If there are the number of starts seeds or fewer left,  the current player collects them and the game is over. This rule is applied at the end of each turn, even if there is not a capture because the sow phase may have reduced the seed count.
-- PICK2XLASTSEEDS: If there are 2 times the number of start seeds or fewer, the round starter picks them. This rule is applied at the end of each turn, even if there is not a capture because the sow phase may have reduced the seed count.
-In terms of GRANDSLAM, these picks are considered captures.</t>
-  </si>
-  <si>
     <t>NO_ROUNDS</t>
   </si>
   <si>
-    <t>True when stores are present on the game board. For games with GOAL of DEPRIVE or CLEAR, stores can be used to show whose turn it is (seed counts will not be sown).</t>
-  </si>
-  <si>
     <t>Repeat Turn Addin</t>
   </si>
   <si>
-    <t>Blocks remove holes from play and are shown on the UI with an X.
-When used with ROUNDS, the holes not filled from the player with fewer seeds are blocked and thus out of play for the round.
-When used with DEPRIVE, SOW_BLCK_DIV and goal_param holes are closed (blocked and removed from play) when sown to goal_param seeds.</t>
-  </si>
-  <si>
     <t>goal_param</t>
   </si>
   <si>
-    <t>GOAL of Territory: defines the number of holes needed for a win. The number of holes for each player are computed by rounding the number of seeds collected divided by the number of start seeds per hole.
-Goal of Deprive and Blocked Divert Sower: defines the number of seeds needed to close/block holes (sow_blkd_div).
-Goal of Max Seeds and ROUNDS: defines the minimum number of holes each player must have to continue the game. The player with fewer seeds must have enough seeds to fill goal_param holes each with start_seeds in order to continue playing.  There is no rounding of seed counts as in territory games.
-RND_* Goals: number of specified parameter for win.</t>
-  </si>
-  <si>
     <t>Goal Parameter</t>
   </si>
   <si>
     <t>nocaptmoves</t>
   </si>
   <si>
-    <t>Don't allow captures or closing of holes (SOW_RULE of SOW_BLKD_DIV) for the first specified number of moves of the game or round.</t>
-  </si>
-  <si>
     <t>sow_param</t>
   </si>
   <si>
     <t>Sow Parameter</t>
   </si>
   <si>
-    <t>A general parameter for sowing. Usage is based on other sow options:
-- Sow rule of MAX_SOW: maximum number of seeds a hole may contain</t>
-  </si>
-  <si>
     <t>label</t>
   </si>
   <si>
@@ -927,13 +702,6 @@
     <t>mdyno_lbl</t>
   </si>
   <si>
-    <t>An int to describe possible multicaptures:
- 0 no multiple captures.
- -1: After the initial capture, continue capturing as long as the capture conditions are met. This multiple capture may happen in the sow direction (unsown holes) or in the opposite direction (sown holes) as determined by CAPSAMEDIR.
- 1 .. holes: capture at most n holes that meet the capture conditions.
-See individual capture mechanism for any special requirements.</t>
-  </si>
-  <si>
     <t>unclaimed</t>
   </si>
   <si>
@@ -946,14 +714,6 @@
     <t>HOLE_OWNER</t>
   </si>
   <si>
-    <t>Defines how to score any unclaimed seeds when a game has ended. This is not used if the game has a clear winner, e.g. one player has collected more than half the seeds for a MAX_SEEDS game.
-- HOLE_OWNER: unclaimed seeds go to the hole owner.
-- DONT_SCORE: unclaimed seeds do not score (they are ignored).
-- LAST_MOVER: unclaimed seeds go the player that moved last.
-- UNFED_PLAYER: only valid for MUSTSHARE games. If the game ended without one player being able share seeds, the seeds go to the player without seeds (the unfed player).
-- DIVVIED: the seeds are divided between the two players (an extra seed goes to the player with fewer seeds).</t>
-  </si>
-  <si>
     <t>capt_side</t>
   </si>
   <si>
@@ -966,14 +726,6 @@
     <t>BOTH</t>
   </si>
   <si>
-    <t>Limits which side of the board captures maybe done on:
-- BOTH: no limitations
-- OPP_SIDE: opposite side capture only.
-- OWN_SIDE: captures on own side of board only.
-- OPP_CONT: a multi-capture must begin on the opposite side of the board, but may continue onto your own side.  Requires MULTICAPT.
-- OWN_CONT: a multi-capture must being on your own side of the board and may continue onto your opponent's side. Requires multicapt.</t>
-  </si>
-  <si>
     <t>presowcapt</t>
   </si>
   <si>
@@ -983,60 +735,6 @@
     <t>PreSowCapt</t>
   </si>
   <si>
-    <t>Capture type that occurs before sowing:
-- NONE: No capture before sowing.
-- CAPT_ONE: Capture 1 seed from the draw. If MLAPS, capture 1 seeds per lap.
-- ALL_SINGLE_XCAPT: Capture the seeds across from all singles.
-- DRAW_1_XCAPT: When draw 1 seed, capture any seeds on the other side of the board.</t>
-  </si>
-  <si>
-    <t>Allow rules limit the holes from which moves may start.  Disallowed holes are not selectable.
-- NONE: no special rule
-- OPP_OR_EMPTY:  Limit the allowable holes to those that end in an empty hole or reach the opponents side of the board.
-- SINGLE_TO_ZERO: Holes with single seeds may only be played if the next hole is empty.
-- SINGLE_ONLY_ALL: Holes with single seeds may only be played if all holes contain single seeds.
-- SINGLE_ALL_TO_ZERO: Holes with single seeds may only be played if all holes contain single seeds and then only if the next hole is empty.
-- TWO_ONLY_ALL: Holes with two seeds may only be played if all holes contain two seeds.
-- TWO_ONLY_ALL_RIGHT: Holes with two seeds may not be played, unless all holes contains two seeds, in which case the rightmost hole must be played.
-- FIRST_TURN_ONLY_RIGHT_TWO: The first turn must start from one of the two rightmost holes.
-- RIGHT_2_1ST_THEN_ALL_TWO:  The first turn must start from one of the two rightmost holes. Subsequent moves may only start from holes without 2 seeds, unless all holes contain zero or 2 seeds.
-- MOVE_ALL_HOLES_FIRST: a move must initiated from each hole once before a second move may be made from any hole.  MOVE_ALL is incompatible with all pickers and capttwoout.
-- NOT_XFROM_1S: moves may not start from holes with a singleton opposite it.</t>
-  </si>
-  <si>
-    <t>When rounds are employed, each round may end under conditions that do not win the overall game. The board is then setup again per the game rules, generally with some feature changed based on the previous round: hole ownership, holes out of play, a shortened board. Play continues in rounds until either player meets the overall game winning condition.
-If the game is played in round, defines how each round ends: 
-- NO_ROUNDS: the game is not played in rounds
-- HALF_SEEDS: each round ends when one player has more that half the seeds
-- NO_MOVES: When MUSTSHARE is set, each round ends when neither player has a valid move.  When MUSTSHARE is not set, each round ends when a  player does have not a valid move at the start of their turn.
-- END_S_SEEDS: End the round when there are number of start seeds or fewer in play.
-- END_2S_SEEDS: End the round when there are two times the number of start seeds or fewer in play.
-For example: In Weg each round ends when neither player has a valid move. The board is then set up again after determining who owns what territory (holes). Rounds continue until one player has claimed sufficient territory to be declared the game winner (e.g. ownership of 10 or more holes).
-In the case of a round win or tie  a new starter is determined via ROUND_STARTER and  the board is reset according to ROUND_FILL.
-BLOCKS are used in many games and set between rounds based on the seed placement. TERRITORY GOAL games adjust hole ownership between rounds.</t>
-  </si>
-  <si>
-    <t>The overall goal of the game. Defines how a player wins.
-- MAX_SEEDS: The goal is to collect the maximum number of seeds.
-  + If the game is not played in rounds, the game will end when one player has more than half of the total seeds.
-  + If the game is played in rounds, the round end condition is determined by ROUNDS. These games end when one player has collected sufficient seeds to prevent the opponent from filling the required number of holes. Generally, the required number of holes is one but this may be increased by setting goal_param. 
-  + In MAX_SEEDS/ROUNDS games the player only controls the holes on their side of the board, where as, in TERRITORY games a player may control holes on either side of the board.
-- DEPRIVE: eliminate all of your opponents seeds.
-  + If a player has no seeds at the start of their turn, they loose. If a player has no moves at the start of their turn, then the game outcome is determined by who has seeds: If both players have seeds, the game ends in a tie. If the current player has seeds, but the previous player does not, then the current player wins because they forced the previous player to give away all their seeds.
-  + GRANDSLAM must be legal for DEPRIVE games.
-  + DEPRIVE games cannot be played in ROUNDS or use children. Additionally, the following options are incompatible with DEPRIVE games: MOVEUNLOCK, MUSTPASS and MUSTSHARE.
-- TERRITORY: claim ownership of holes. Each round the ownership of holes is determined by the number of seeds captured in the previous round. In a TERRITORY game without rounds, the winner is the player that gained the most territory during play. 
-  + TERRITORY games require STORES and that goal_param be set to a value between the number of holes and two times the number of holes.
-  + TERRITORY games are incompatible with NO_SIDES, START_PATTERN, GRANDSLAM of NOT_LEGAL, ALLOW_RULE of OPP_OR_EMPTY.
-- CLEAR: clear seeds from your own holes.
-  + Moves must always be possible so MIN_MOVE must be 1 and ALLOW_RULE single_all_to_zero may not be used.
-  + GRANDSLAM must be legal for CLEAR games.  CLEAR games cannot be played in ROUNDS or use children. Additionally, the following options are incompatible with CLEAR games: MOVEUNLOCK, MUSTPASS and MUSTSHARE.
-- RND_WIN_COUNT:  win goal_param rounds. ROUND_FILL is not used; each round is setup as the start of the game.
-- RND_SEED_COUNT: collect goal_param seeds across several rounds. ROUND_FILL is not used; each round is setup as the start of the game.
-- RND_EXTRA_SEEDS: collect goal_param extra seeds (winner - loser seeds).  ROUND_FILL is not used; each round is setup as the start of the game.
-- RND_POINTS:  score goal_param points. WIN is 1 point. WIN and skunk (&gt; 3/4 of total seeds) is 2 points.  ROUND_FILL is not used; each round is setup as the start of the game.</t>
-  </si>
-  <si>
     <t>child_locs</t>
   </si>
   <si>
@@ -1049,33 +747,6 @@
     <t>ANYWHERE</t>
   </si>
   <si>
-    <t>Locations where children can be made by each player. The notes designate players as: T - top player, B - bottom player. N - neither player. For shorter boards, the pattern is generated using assignments (a b c d e) as:
-board length 2: a e
-board length 3: a c e
-board length 4: a b d e
-The center hole  (c) is replicated for larger boards. 
-- ANYWHERE: children may be made anywhere.
-- ENDS_ONLY: children may be made in the end holes only.
-  + TB N N N TB
-  + TB N N N TB
-- NO_ENDS: children may only be made on internal holes, no end holes.
-  + N TB TB TB N
-  + N TB TB TB N
-- INV_ENDS_PLUS_MID: children may be made by each player on the opposite side ends and all own side middle holes.
-  + B T T T B
-  + T B B B T
-- ENDS_PLUS_ONE_OPP: Either player may make children in any end hole, but the next inner hole can only be made on the opposite side. 
-  +  Used for Walda type children: Each player may create up to 6 walda: on either end of each side of the board and the next two outer holes on their own side of the board. Note that there are only 8 total places that walda maybe created.
-  + TB B N B TB
-  + TB T N T TB
-- NO_OWN_RIGHT: children may not be made on the your own rightmost hole. 
-  + B TB TB TB TB
-  + TB TB TB TB T
-- NO_OPP_RIGHT: children may not be made on the opposite rightmost hole.
-  + TB TB TB TB T
-  + B TB TB TB TB</t>
-  </si>
-  <si>
     <t>capt_type</t>
   </si>
   <si>
@@ -1083,135 +754,6 @@
   </si>
   <si>
     <t>CaptType</t>
-  </si>
-  <si>
-    <t>Capture type.
-- NONE: No other capture type.
-- NEXT: Capture from the hole after the final seed sown. Basic capture rules are applied; capture side is checked; and multiple captures in either direction are supported.
-  + When multiple lap sowing, the sowing does not stop for captures. Instead, sowing continues until the final seed is sown into an empty hole. Then the capture test is made on the next hole.
-- TWO_OUT: Basic capture rules and capture side are ignored. There are three flavors of capture two out:
-  + Single lap game: capture if sow ends in occupied hole, then an empty hole, followed by an occupied hole the contents of this are hole captured.
-  + Multi lap game but single capture: capture when last hole sown is followed by an empty hole which is then followed by an occupied hole.
-  + Multi lap game with multiple captures: capture when last hole sown is followed by an empty hole which is then followed by an occupied hole. Continue captures as long as the pattern of empty hole followed by an occupied hole continues. CAPSAMEDIR must be true. 
-- MATCH_OPP: capture when the number of seeds in the final hole sown match the opposite-side hole. Multiple captures maybe made in either direction. Multilap sowing does stop for captures.</t>
-  </si>
-  <si>
-    <t>The name of the Game Class. One of:
-Mancala: allows setting all parameters though some combinations are limited.
-Diffusion: has unique sow method and win conditions.  Players control the east/west sides of the board. The game is basically preconfigured, only the board size can be changed to any even size. Game goal must be clear.
-DiffusionV2: similar to Diffusion but players control the typical north/south sides of the board.
-SameSide: a game class in which seeds are only sown on the player's own side of the board. If a capture is made, the capturer chooses one of their opponent's holes to put the seeds into. All seeds go into exactly one hole. Sow direction is unconstrained Capture mechanisms must be limited to one side of the board: basic captures, next, and two out. Game goal must be clear.
-Ohojichi: very similar to SameSide but the board is divided east/west instead of north/south. Most parameter restrictions from SameSide apply to Ohojichi. For Ohojichi, if UDIR_HOLES is used, all holes must be UDIR; capture side must be BOTH.</t>
-  </si>
-  <si>
-    <t>Additional child creation requirements may be set. These are in addition to location restrictions specified by CHILD_LOCS.
-- NONE: no additional restrictions.
-- OPP_ONLY:  Only make children on the opposite side of the board. Incompatible with BULL, QUR, and WEG child types.
-- OWN_ONLY: Only make children on own side of the board.  Incompatible with BULL, QUR, and WEG child types.
-- NOT_1ST_OPP: Don't make a child in the first hole on the opponents side/territory with one seed.</t>
-  </si>
-  <si>
-    <t>When crosscapt is set, defines what to do with the single seed initiating the cross capture.
-- LEAVE: always leave the single seed
-- PICK_ON_CAPT: only pick (capture) the seed if there was a capture
-- ALWAYS_PICK: always pick (capture) the final single seed, even if there was not a capture</t>
-  </si>
-  <si>
-    <t>Only meaningful with MULTICAPT. Captures are done in the same direction as the sowing, i.e. following the final hole sown. If not set, captures are done from the holes just sown.</t>
-  </si>
-  <si>
-    <t>Allows specifying non-all-equal start patterns. The following patterns are supported:
-- ALL_EQUAL: all holes start with the same number of seeds.
-- GAMACHA: starting from the third hold (from start player's left) place nbr_seeds in every other hole, the first move is prescribed move the center hole's seeds to the other side (this is done automatically).
-- ALTERNATES: every other hole is filled with nbr_seeds, no seeds end up opposite each other. If a player has fewer seeds than their opponent, then they start.
-- ALTS_WITH_1: like Alternates except the starter's 2nd from right hole with nbr_seeds is replaced with one seed.
-- CLIPPEDTRIPLES: pattern of 0 S S (where S is nbr_seeds) is used to fill the holes; if a full cycle of 3 cannot be placed, the holes are left empty. The True and False sides are the same from the player's perspective, e.g. they will look reversed when viewed from one side of the game board.
-- TWOEMPTY: all but the rightmost two holes for each player are filled with is nbr_seeds.
-- RANDOM: the total seeds are computed as (10 * holes) + (2 * nbr_start). The seeds are randomly distributed into all holes.</t>
-  </si>
-  <si>
-    <t>The first sow of the game maybe defined by a specific rule. Prescribed openings are different than start patterns because the player may choose the sow start point. SOW_OWN_STORE and SOW_RULE are ignored during the prescribed openings.
-- NONE: there is no prescribed opening move.
-- BASIC_SOWER: the first sow is a very basic pickup the seeds and drop them one at a time in each hole ignoring any other sow parameters. Other sow parameters will be enacted  afterward. This can be used to force the first sow of an MLAPS game to be a single sow. 
-- MLAPS_SOWER: the first sow follows basic rules of multi-lap sowing (LAPPER). Other sow parameters will be enacted  afterward. 
-- SOW1OPP: at least one seed must be sown on the opponents side of the board which is accomplished by sowing as normal until the final seed, then any remaining holes on the player's side are skipped and the last seed is sown in the opponents first hole (based on current sow direction).
-- PLUS1MINUS1: proceed from the selected hole by moving one seed from the next hole into the following hole, next skip that hole and repeat moving seed forward. After cycling the board, capture across from the opening hole. 
-- ARNGE_LIMIT: the first move may be used to rearrange the seeds (opponent is same layout). If the first move is not used for rearrangement, captures and child creation are not allowed from the starter until the second player makes a child or captures.</t>
-  </si>
-  <si>
-    <t>A grandslam is when your opponent has seeds at the start of your turn and you capture them all. This option selects what to do:
-- LEGAL: the seeds are captured
-- NOT_LEGAL: you may not capture all of your opponents seeds, a move which would do so is not allowed
-- NO_CAPT: you may sow the seeds, but the capture is not performed
-- OPP_GETS_REMAIN: if you capture all your opponents seeds, they capture all of your remaining seeds and the game is over. Winner is determined by game goal. Seeds picked because of PICKEXTRA PICK*LASTSEEDS go the current player and not the opponent.
-- LEAVE_LEFT: the capture is performed from all but the leftmost hole from the sower perspective. This might leave your opponents without seeds or might not capture any seeds.
-- LEAVE_RIGHT: the capture is performed from all but the rightmost hole from the sower perspective. This might leave your opponents without seeds.</t>
-  </si>
-  <si>
-    <t>The round fill method determines which holes are filled and how many seeds they are filled with when setting up for a new round.
-Several round fill mechanisms use the same general approach called the Empty Hole Method. The loser of the previous round will end up with empty holes. These holes are not playable if BLOCKS are used; otherwise they are playable. This method is not used for RND_* GOAL games.
-The seeds each player accumulated in the previous round are distributed into holes with exactly the same number in each. That number of seeds is NBR_START. The winner will fill all of their holes and put any remaining seeds into their own store. The loser will fill as many holes as they can with nbr_start seeds and put any remaining seeds (fewer than nbr_start) into their own store.
-LEFT_FILE, RIGHT_FILL and OUTSIDE_FILL define which holes that the loser must fill. UCHOOSE allows the loser to choose which holes have seeds.
-- NOT_APPLICABLE: round fill doesn't need to be specified: either the game not played in rounds (CLEAR &amp; DEPRIVE games included) or game goal is TERRITORY  without UCHOWN (see below, all holes filled).
-- LEFT_FILL: fill the round loser's holes from the player's left with nbr_start seeds each.  
-- RIGHT_FILL: fill the round loser's holes from the player's right with nbr_start seeds each. 
-- OUTSIDE_FILL: fill the round loser's holes from the outside ends toward the middle with nbr_start seeds each. Leftmost, rightmost, 2nd leftmost, 2nd rightmost, etc. until the seeds are used up.
-- EVEN_FILL: fill all holes (both sides) with the same number of seeds; determined by dividing the losers seeds by the number of holes per side. If that is not playable based on the minimum number of seeds required for a move (MIN_MOVE); extra seeds are put in each players leftmost hole. Any extra seeds are put in each player's store.
-- SHORTEN: the number of holes that the round loser can fill with NBR_START seeds are fill on both sides, other holes are left empty. Holes are filled opposite each other. If BLOCKS is selected, the board is shortened to the number of holes filled (empty holes are blocked and out of play). If the game uses children, they will not be created if the board size is reduced to 3 or less.
-- UCHOOSE: allow user to choose which holes have seeds (are not blocked) when ROUNDS and BLOCKS are used.
-- UMOVE: allow the loser to choose where seeds are placed. At least one seed must be placed in each hole and the game must be playable (at least one hole has MIN_MOVE seeds), remaining seeds are placed in the store. The winner's layout is the same layout but reflected.
-- UCHOWN: The only round fill supported for territory games. The winner may choose which holes they control.</t>
-  </si>
-  <si>
-    <t>Bias for the Monte Carlo Tree search algorithm for each difficulty level (0-3).  A larger bias encourages move game tree exploration, but defocuses the exploration from the best choices. This is critical in avoiding getting stuck in sub-optimal move choices.
-Value is divided by 1000.</t>
-  </si>
-  <si>
-    <t>If the game is being played on easy mode (game difficult of easy/0), a random value may be added to the static evaluation. This can be done to induce errors into the ai player's game play. A random value is selected between -easy_rand and + easy_rand.
-The specific value for this should be selected based on the ranges of the parameters and multiplier.
-Used only for minimax &amp; negamax players.</t>
-  </si>
-  <si>
-    <t>Determines if seeds from more the start hole are picked up and sown:
-- OFF: Single lap sowing. Seeds from the start hole are sown, typically, one per hole until expended.
-- LAPPER:  If the first sow ends in a hole with more than one seed, pickup all the seeds and continue sowing another "lap". Note that lap here does not mean a full circuit of the board, only an individual sow operation. In general, sowing laps continues in this manner until the final seed of a lap reaches an empty hole. There are games with other conditions for ending a multilap low such as making a capture or making a child. 
-  + Several values of SOW_RULE perform an operation after each lap sown: SOW_CLKD_DIV(_NR) closes the final hole and CHANGE_DIR_LAP changes the direction of sowing after each lap.
-- LAPPER_NEXT:  For lapper_next sowing, the number of seeds in the last sown hole of lap do not matter. Instead, if the hole after the last sown hole has any seeds, those seeds are used to continue sowing the next lap. Sowing continues until the hole after the lap's final seed is empty. There are games with other conditions for ending a multilap low such as making a capture or making a child.
-  + A SOW_RULE of CHANGE_DIR_LAP changes the direction of sowing after each lap. SOW_BLKD_DIV(_NR) is not supported for LAPPER_NEXT.</t>
-  </si>
-  <si>
-    <t>Special sow rules add additional behavior or restrictions to the sowing phase:
-- NONE: there is no special sowing rule.
-- SOW_BLKD_DIV: If the final seed of an individual sow lands on the opposite side of the board and brings the contents of that hole to goal_param seeds, the hole is closed  (blocked). In single lap games, the hole's seeds are removed from play. In multilap games, the seeds are used to continue sowing.
-  + When sowing, blocked holes on your own side of the board are skipped  and blocked holes on opponent's side are diverted out of play or captured.
-  +  Game GOAL must be DEPRIVE and all of the associated restrictions apply. NOCAPTMOVES maybe used to prevent closing holes on the initial games moves. Capture mechanisms other than closing holes are not supported. The minimum move must be 1 and thus SOW_START is incompatible.  ALLOW_RULE may not be used to limit allowable moves.  SKIP_START and VISIT_OPP are not supported with SOW_BLKD_DIV.  MLAPS of LAPPER_NEXT is not supported with SOW_BLKD_DIV(_NR).
-- SOW_BLKD_DIV_NR: Behaves the same as SOW_BLKD_DIV except that each player's rightmost hole cannot be closed. 
-- OWN_SOW_CAPT_ALL: The hole OWNer captures all holes that are sown to meet the simple capture criteria no matter who sowed them.  The simple capture criteria are: evens, min, max and capture on. Other criteria are enforced: side of the board, unlocked, and not child.
-  + The capture is done by the hole owner, so the non-sower may capture seeds while their opponents sows. If the game GOAL is TERRITORY the capturer is the hole owner; otherwise each player captures from their own side of the board no matter who is sowing. 
-  + If MLAPS is LAPPER and the final seed sown for any lap meets the simple capture criteria for that hole, the contents of the hole are captured by the sower and not the hole owner and the turn is over. For CAPTTWOOUT, CAPT_NEXT and CROSSCAPT captures, the sower always does the final capture.
-  + GRANDSLAM rules are not applied. NOCAPTMOVES prevents these capture for the first moves.
-- SOW_CAPT_ALL: Similar to OWN_SOW_CAPT_ALL but only the SOWer captures seeds from the side specified by CAPT_SIDE. BOTH sower capturers from any hole. OPP sower capturer only from opponents holes.  OWN sower captures only from their own holes. 
-  + If mlaps is LAPPER and the final seed sown for any lap meets the capture criteria, the contents of the hole are captured by the sower and not the hole owner and the turn is over.
-  + GRANDSLAM rules are not applied. NOCAPTMOVES prevents this capture for the first number of specified moves.
-- NO_SOW_OPP_2S: Don't sow into opponents holes with 2 seeds.
-- CHANGE_DIR_LAP: Change the direction for each lap sown. Generally used with UDIR_HOLES so the player may choose the first direction.
-- MAX_SOW: holes sow_param seeds are skipped when sowing. That is, holes will never contain more seeds than sow_param.
-- LAP_CAPT: after each lap check for a capture, if there is a capture continue sowing with another lap. If a basic capture is configured (evens, capt on, max or min), the hole after the captured seeds is drawn to continue lapping.
-- NO_OPP_CHILD: do not sow into your opponents children.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Games with children allow players to claim holes. These child holes are an extension of the stores and seeds in them count towards a win. Making a child stops any multiple lap sowing, moves cannot start from children, and they cannot be captured (except for special rules associated with WEGs).
-- NOCHILD: children are not used.
-- NORMAL: children are made when a final seeds sows a hole to CHILD_CVT. If stores are not included captures are instead moved into children, thus a player may not capture until they have created a child. 
-- ONE_CHILD: only one child allowed per player.
-  + Children must not be symmetrically opposite each other. For example,  in a 9 hole per side game with holes numbered as follows, children may not be in the same numbered holes:
-  + 9 8 7 6 5 4 3 2 1
-  + 1 2 3 4 5 6 7 8 9 
-  + Used to create tuzdek style children along with CHILD_RULE of OPP_ONLY.
-- WEG: children maybe created in holes owned by the opponent. Ending a sow in an opponent's weg captures the seed just sown and one more (if there is one); generally, the player gets to play again (per CAPT_RTURN). WEGs are supported for TERRITORY games only (hole ownership required).
-- BULL: create one bull if final seed sows to CHILD_CVT, create two bulls if the final two seeds are sown to CHILD_CVT-1 and CHILD_CVT (in either order).
-- QUR: when a seed is sown into an empty hole on the player's side of the board and the opposite hole contains CHILD_CVT, create children in both holes: final seed location and opposite.
-</t>
   </si>
 </sst>
 </file>
@@ -1710,7 +1252,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1721,9 +1263,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -1732,9 +1271,6 @@
     </xf>
     <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
@@ -2093,29 +1629,28 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:J87"/>
+  <dimension ref="A1:I83"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A82" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F86" sqref="F86"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G47" sqref="G47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.5703125" style="3" customWidth="1"/>
     <col min="2" max="2" width="16" style="3" customWidth="1"/>
-    <col min="3" max="3" width="24.42578125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="36.28515625" style="3" customWidth="1"/>
     <col min="4" max="4" width="16.5703125" style="3" customWidth="1"/>
     <col min="5" max="5" width="11.5703125" style="3" customWidth="1"/>
     <col min="6" max="6" width="14.7109375" style="3" customWidth="1"/>
-    <col min="7" max="7" width="16.42578125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="26.140625" style="3" customWidth="1"/>
     <col min="8" max="8" width="6.7109375" style="3" customWidth="1"/>
     <col min="9" max="9" width="7.28515625" style="3" customWidth="1"/>
-    <col min="10" max="10" width="136.42578125" style="4" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="3"/>
+    <col min="10" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2129,12 +1664,12 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>182</v>
+        <v>167</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="6" t="s">
         <v>5</v>
       </c>
       <c r="H1" s="1" t="s">
@@ -2143,29 +1678,26 @@
       <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>253</v>
+        <v>196</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>254</v>
+        <v>197</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3">
         <v>0</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>246</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>84</v>
+        <v>189</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>76</v>
       </c>
       <c r="H2" s="3">
         <v>0</v>
@@ -2173,29 +1705,28 @@
       <c r="I2" s="3">
         <v>0</v>
       </c>
-      <c r="J2" s="4"/>
-    </row>
-    <row r="3" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="E3" s="3">
         <v>114</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>51</v>
+        <v>33</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>45</v>
       </c>
       <c r="H3" s="3">
         <v>1</v>
@@ -2203,31 +1734,28 @@
       <c r="I3" s="3">
         <v>0</v>
       </c>
-      <c r="J3" s="4" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="E4" s="3">
         <v>104</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>84</v>
+        <v>8</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>76</v>
       </c>
       <c r="H4" s="3">
         <v>2</v>
@@ -2235,31 +1763,28 @@
       <c r="I4" s="3">
         <v>0</v>
       </c>
-      <c r="J4" s="4" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>99</v>
-      </c>
       <c r="C5" s="3" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="E5" s="3">
         <v>105</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>84</v>
+        <v>8</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>76</v>
       </c>
       <c r="H5" s="3">
         <v>3</v>
@@ -2267,31 +1792,28 @@
       <c r="I5" s="3">
         <v>0</v>
       </c>
-      <c r="J5" s="4" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="E6" s="3">
         <v>107</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>88</v>
+        <v>127</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>80</v>
       </c>
       <c r="H6" s="3">
         <v>4</v>
@@ -2299,28 +1821,25 @@
       <c r="I6" s="3">
         <v>0</v>
       </c>
-      <c r="J6" s="4" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>258</v>
+        <v>201</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>259</v>
+        <v>202</v>
       </c>
       <c r="E7" s="3">
         <v>0</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>246</v>
-      </c>
-      <c r="G7" s="5" t="s">
-        <v>84</v>
+        <v>189</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>76</v>
       </c>
       <c r="H7" s="3">
         <v>5</v>
@@ -2329,27 +1848,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="E8" s="3">
         <v>113</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>40</v>
+        <v>33</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>34</v>
       </c>
       <c r="H8" s="3">
         <v>6</v>
@@ -2357,31 +1876,28 @@
       <c r="I8" s="3">
         <v>0</v>
       </c>
-      <c r="J8" s="4" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="E9" s="3">
         <v>150</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="G9" s="5" t="s">
-        <v>109</v>
+        <v>98</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>99</v>
       </c>
       <c r="H9" s="3">
         <v>7</v>
@@ -2389,31 +1905,28 @@
       <c r="I9" s="3">
         <v>0</v>
       </c>
-      <c r="J9" s="4" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>176</v>
+        <v>161</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>177</v>
+        <v>162</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="E10" s="3">
         <v>149</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="G10" s="5" t="s">
-        <v>40</v>
+        <v>33</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>34</v>
       </c>
       <c r="H10" s="3">
         <v>8</v>
@@ -2421,28 +1934,25 @@
       <c r="I10" s="3">
         <v>0</v>
       </c>
-      <c r="J10" s="4" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>255</v>
+        <v>198</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>256</v>
+        <v>199</v>
       </c>
       <c r="E11" s="3">
         <v>0</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>246</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>257</v>
+        <v>189</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>200</v>
       </c>
       <c r="H11" s="3">
         <v>9</v>
@@ -2451,27 +1961,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="195" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>301</v>
+        <v>236</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>302</v>
+        <v>237</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="E12" s="3">
         <v>106</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>303</v>
-      </c>
-      <c r="G12" s="5" t="s">
-        <v>159</v>
+        <v>238</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>147</v>
       </c>
       <c r="H12" s="3">
         <v>10</v>
@@ -2479,28 +1989,25 @@
       <c r="I12" s="3">
         <v>0</v>
       </c>
-      <c r="J12" s="4" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>264</v>
+        <v>207</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="E13" s="3">
         <v>0</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>246</v>
-      </c>
-      <c r="G13" s="5" t="s">
-        <v>84</v>
+        <v>189</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>76</v>
       </c>
       <c r="H13" s="3">
         <v>0</v>
@@ -2509,27 +2016,27 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="E14" s="3">
         <v>124</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G14" s="5" t="s">
-        <v>84</v>
+        <v>8</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>76</v>
       </c>
       <c r="H14" s="3">
         <v>1</v>
@@ -2537,31 +2044,28 @@
       <c r="I14" s="3">
         <v>2</v>
       </c>
-      <c r="J14" s="4" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="E15" s="3">
         <v>103</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="G15" s="5" t="s">
-        <v>40</v>
+        <v>33</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>34</v>
       </c>
       <c r="H15" s="3">
         <v>2</v>
@@ -2569,28 +2073,25 @@
       <c r="I15" s="3">
         <v>2</v>
       </c>
-      <c r="J15" s="4" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>260</v>
+        <v>203</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>271</v>
+        <v>214</v>
       </c>
       <c r="E16" s="3">
         <v>0</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>246</v>
-      </c>
-      <c r="G16" s="5" t="s">
-        <v>84</v>
+        <v>189</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>76</v>
       </c>
       <c r="H16" s="3">
         <v>3</v>
@@ -2599,27 +2100,27 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>241</v>
+        <v>186</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>261</v>
+        <v>204</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="E17" s="3">
         <v>128</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G17" s="5" t="s">
-        <v>84</v>
+        <v>8</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>76</v>
       </c>
       <c r="H17" s="3">
         <v>4</v>
@@ -2627,31 +2128,28 @@
       <c r="I17" s="3">
         <v>2</v>
       </c>
-      <c r="J17" s="4" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>284</v>
+        <v>225</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>285</v>
+        <v>226</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="E18" s="3">
         <v>130</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="G18" s="5" t="s">
-        <v>287</v>
+        <v>227</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>228</v>
       </c>
       <c r="H18" s="3">
         <v>5</v>
@@ -2659,31 +2157,28 @@
       <c r="I18" s="3">
         <v>2</v>
       </c>
-      <c r="J18" s="4" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="E19" s="3">
         <v>129</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="G19" s="5" t="s">
-        <v>40</v>
+        <v>33</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>34</v>
       </c>
       <c r="H19" s="3">
         <v>6</v>
@@ -2691,31 +2186,28 @@
       <c r="I19" s="3">
         <v>2</v>
       </c>
-      <c r="J19" s="4" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="E20" s="3">
         <v>123</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="G20" s="5" t="s">
-        <v>40</v>
+        <v>33</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>34</v>
       </c>
       <c r="H20" s="3">
         <v>7</v>
@@ -2723,28 +2215,25 @@
       <c r="I20" s="3">
         <v>2</v>
       </c>
-      <c r="J20" s="4" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>262</v>
+        <v>205</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>263</v>
+        <v>206</v>
       </c>
       <c r="E21" s="3">
         <v>0</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>246</v>
-      </c>
-      <c r="G21" s="5" t="s">
-        <v>84</v>
+        <v>189</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>76</v>
       </c>
       <c r="H21" s="3">
         <v>8</v>
@@ -2753,27 +2242,27 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>165</v>
+        <v>150</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>166</v>
+        <v>151</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="E22" s="3">
         <v>108</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="G22" s="5" t="s">
-        <v>40</v>
+        <v>33</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>34</v>
       </c>
       <c r="H22" s="3">
         <v>9</v>
@@ -2781,31 +2270,28 @@
       <c r="I22" s="3">
         <v>2</v>
       </c>
-      <c r="J22" s="4" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" ht="135" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>173</v>
+        <v>158</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>175</v>
+        <v>160</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="E23" s="3">
         <v>131</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="G23" s="5" t="s">
         <v>159</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>147</v>
       </c>
       <c r="H23" s="3">
         <v>10</v>
@@ -2813,31 +2299,28 @@
       <c r="I23" s="3">
         <v>2</v>
       </c>
-      <c r="J23" s="4" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" ht="409.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="E24" s="3">
         <v>115</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="G24" s="5" t="s">
-        <v>55</v>
+        <v>48</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>49</v>
       </c>
       <c r="H24" s="3">
         <v>0</v>
@@ -2845,31 +2328,28 @@
       <c r="I24" s="3">
         <v>0</v>
       </c>
-      <c r="J24" s="4" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" ht="105" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>238</v>
+        <v>184</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>240</v>
+        <v>185</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="E25" s="3">
         <v>116</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G25" s="5" t="s">
-        <v>84</v>
+        <v>8</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>76</v>
       </c>
       <c r="H25" s="3">
         <v>1</v>
@@ -2877,31 +2357,28 @@
       <c r="I25" s="3">
         <v>0</v>
       </c>
-      <c r="J25" s="4" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" ht="120" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>279</v>
+        <v>221</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>280</v>
+        <v>222</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="E26" s="3">
         <v>147</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>281</v>
-      </c>
-      <c r="G26" s="5" t="s">
-        <v>282</v>
+        <v>223</v>
+      </c>
+      <c r="G26" s="4" t="s">
+        <v>224</v>
       </c>
       <c r="H26" s="3">
         <v>2</v>
@@ -2909,28 +2386,25 @@
       <c r="I26" s="3">
         <v>0</v>
       </c>
-      <c r="J26" s="4" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>273</v>
+        <v>216</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>247</v>
+        <v>190</v>
       </c>
       <c r="E27" s="3">
         <v>0</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>246</v>
-      </c>
-      <c r="G27" s="5" t="s">
-        <v>84</v>
+        <v>189</v>
+      </c>
+      <c r="G27" s="4" t="s">
+        <v>76</v>
       </c>
       <c r="H27" s="3">
         <v>3</v>
@@ -2939,27 +2413,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="165" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="E28" s="3">
         <v>143</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="G28" s="5" t="s">
-        <v>59</v>
+        <v>52</v>
+      </c>
+      <c r="G28" s="4" t="s">
+        <v>53</v>
       </c>
       <c r="H28" s="3">
         <v>4</v>
@@ -2967,31 +2441,28 @@
       <c r="I28" s="3">
         <v>0</v>
       </c>
-      <c r="J28" s="4" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" ht="180" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>168</v>
+        <v>153</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>167</v>
+        <v>152</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="E29" s="3">
         <v>132</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="G29" s="5" t="s">
-        <v>159</v>
+        <v>154</v>
+      </c>
+      <c r="G29" s="4" t="s">
+        <v>147</v>
       </c>
       <c r="H29" s="3">
         <v>5</v>
@@ -2999,28 +2470,25 @@
       <c r="I29" s="3">
         <v>0</v>
       </c>
-      <c r="J29" s="4" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>274</v>
+        <v>217</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>275</v>
+        <v>218</v>
       </c>
       <c r="E30" s="3">
         <v>0</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>246</v>
-      </c>
-      <c r="G30" s="5" t="s">
-        <v>84</v>
+        <v>189</v>
+      </c>
+      <c r="G30" s="4" t="s">
+        <v>76</v>
       </c>
       <c r="H30" s="3">
         <v>7</v>
@@ -3029,27 +2497,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="E31" s="3">
         <v>119</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G31" s="5" t="s">
-        <v>62</v>
+        <v>8</v>
+      </c>
+      <c r="G31" s="4" t="s">
+        <v>56</v>
       </c>
       <c r="H31" s="3">
         <v>8</v>
@@ -3057,31 +2525,28 @@
       <c r="I31" s="3">
         <v>0</v>
       </c>
-      <c r="J31" s="4" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" ht="225" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>156</v>
+        <v>144</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="E32" s="3">
         <v>101</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="G32" s="5" t="s">
-        <v>159</v>
+        <v>146</v>
+      </c>
+      <c r="G32" s="4" t="s">
+        <v>147</v>
       </c>
       <c r="H32" s="3">
         <v>9</v>
@@ -3089,31 +2554,28 @@
       <c r="I32" s="3">
         <v>0</v>
       </c>
-      <c r="J32" s="4" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="E33" s="3">
         <v>144</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="G33" s="5" t="s">
-        <v>51</v>
+        <v>33</v>
+      </c>
+      <c r="G33" s="4" t="s">
+        <v>45</v>
       </c>
       <c r="H33" s="3">
         <v>0</v>
@@ -3121,31 +2583,28 @@
       <c r="I33" s="3">
         <v>2</v>
       </c>
-      <c r="J33" s="4" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="E34" s="3">
         <v>127</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="G34" s="5" t="s">
-        <v>40</v>
+        <v>33</v>
+      </c>
+      <c r="G34" s="4" t="s">
+        <v>34</v>
       </c>
       <c r="H34" s="3">
         <v>1</v>
@@ -3153,28 +2612,25 @@
       <c r="I34" s="3">
         <v>2</v>
       </c>
-      <c r="J34" s="4" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>277</v>
+        <v>220</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>276</v>
+        <v>219</v>
       </c>
       <c r="E35" s="3">
         <v>0</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>246</v>
-      </c>
-      <c r="G35" s="5" t="s">
-        <v>84</v>
+        <v>189</v>
+      </c>
+      <c r="G35" s="4" t="s">
+        <v>76</v>
       </c>
       <c r="H35" s="3">
         <v>3</v>
@@ -3183,27 +2639,27 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="E36" s="3">
         <v>125</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="G36" s="5" t="s">
-        <v>40</v>
+        <v>33</v>
+      </c>
+      <c r="G36" s="4" t="s">
+        <v>34</v>
       </c>
       <c r="H36" s="3">
         <v>4</v>
@@ -3211,31 +2667,28 @@
       <c r="I36" s="3">
         <v>2</v>
       </c>
-      <c r="J36" s="4" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="E37" s="3">
         <v>126</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="G37" s="5" t="s">
-        <v>40</v>
+        <v>33</v>
+      </c>
+      <c r="G37" s="4" t="s">
+        <v>34</v>
       </c>
       <c r="H37" s="3">
         <v>5</v>
@@ -3243,31 +2696,28 @@
       <c r="I37" s="3">
         <v>2</v>
       </c>
-      <c r="J37" s="4" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" ht="150" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="E38" s="3">
         <v>117</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="G38" s="5" t="s">
-        <v>115</v>
+        <v>104</v>
+      </c>
+      <c r="G38" s="4" t="s">
+        <v>105</v>
       </c>
       <c r="H38" s="3">
         <v>6</v>
@@ -3275,28 +2725,25 @@
       <c r="I38" s="3">
         <v>2</v>
       </c>
-      <c r="J38" s="4" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>248</v>
+        <v>191</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>272</v>
+        <v>215</v>
       </c>
       <c r="E39" s="3">
         <v>0</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>246</v>
-      </c>
-      <c r="G39" s="5" t="s">
-        <v>84</v>
+        <v>189</v>
+      </c>
+      <c r="G39" s="4" t="s">
+        <v>76</v>
       </c>
       <c r="H39" s="3">
         <v>7</v>
@@ -3305,27 +2752,27 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="240" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C40" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B40" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C40" s="3" t="s">
-        <v>42</v>
-      </c>
       <c r="D40" s="3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="E40" s="3">
         <v>136</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="G40" s="5" t="s">
-        <v>234</v>
+        <v>36</v>
+      </c>
+      <c r="G40" s="4" t="s">
+        <v>182</v>
       </c>
       <c r="H40" s="3">
         <v>8</v>
@@ -3333,31 +2780,28 @@
       <c r="I40" s="3">
         <v>2</v>
       </c>
-      <c r="J40" s="4" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="E41" s="3">
         <v>135</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="G41" s="5" t="s">
-        <v>46</v>
+        <v>39</v>
+      </c>
+      <c r="G41" s="4" t="s">
+        <v>40</v>
       </c>
       <c r="H41" s="3">
         <v>9</v>
@@ -3365,31 +2809,28 @@
       <c r="I41" s="3">
         <v>2</v>
       </c>
-      <c r="J41" s="4" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" ht="345" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>178</v>
+        <v>163</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>179</v>
+        <v>164</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="E42" s="3">
         <v>134</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>180</v>
-      </c>
-      <c r="G42" s="5" t="s">
-        <v>187</v>
+        <v>165</v>
+      </c>
+      <c r="G42" s="4" t="s">
+        <v>172</v>
       </c>
       <c r="H42" s="3">
         <v>10</v>
@@ -3397,31 +2838,28 @@
       <c r="I42" s="3">
         <v>2</v>
       </c>
-      <c r="J42" s="4" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="E43" s="3">
         <v>102</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="G43" s="5" t="s">
-        <v>40</v>
+        <v>33</v>
+      </c>
+      <c r="G43" s="4" t="s">
+        <v>34</v>
       </c>
       <c r="H43" s="3">
         <v>11</v>
@@ -3429,31 +2867,28 @@
       <c r="I43" s="3">
         <v>2</v>
       </c>
-      <c r="J43" s="4" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" ht="150" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E44" s="3">
         <v>1</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="G44" s="5" t="s">
-        <v>19</v>
+        <v>123</v>
+      </c>
+      <c r="G44" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="H44" s="3">
         <v>0</v>
@@ -3461,31 +2896,28 @@
       <c r="I44" s="3">
         <v>0</v>
       </c>
-      <c r="J44" s="4" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="E45" s="3">
         <v>2</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G45" s="5" t="s">
-        <v>32</v>
+        <v>8</v>
+      </c>
+      <c r="G45" s="4" t="s">
+        <v>26</v>
       </c>
       <c r="H45" s="3">
         <v>2</v>
@@ -3493,31 +2925,28 @@
       <c r="I45" s="3">
         <v>0</v>
       </c>
-      <c r="J45" s="4" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="E46" s="3">
         <v>118</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G46" s="5" t="s">
-        <v>25</v>
+        <v>12</v>
+      </c>
+      <c r="G46" s="4" t="s">
+        <v>19</v>
       </c>
       <c r="H46" s="3">
         <v>3</v>
@@ -3525,31 +2954,28 @@
       <c r="I46" s="3">
         <v>0</v>
       </c>
-      <c r="J46" s="4" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+    </row>
+    <row r="47" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="E47" s="3">
         <v>5</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="G47" s="6" t="s">
-        <v>132</v>
+        <v>22</v>
+      </c>
+      <c r="G47" s="5" t="s">
+        <v>122</v>
       </c>
       <c r="H47" s="3">
         <v>4</v>
@@ -3557,31 +2983,28 @@
       <c r="I47" s="3">
         <v>0</v>
       </c>
-      <c r="J47" s="4" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C48" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B48" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C48" s="3" t="s">
-        <v>21</v>
-      </c>
       <c r="D48" s="3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="E48" s="3">
         <v>4</v>
       </c>
       <c r="F48" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G48" s="5" t="s">
-        <v>19</v>
+        <v>12</v>
+      </c>
+      <c r="G48" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="H48" s="3">
         <v>0</v>
@@ -3589,31 +3012,28 @@
       <c r="I48" s="3">
         <v>2</v>
       </c>
-      <c r="J48" s="4" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="E49" s="3">
         <v>3</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G49" s="5" t="s">
-        <v>35</v>
+        <v>8</v>
+      </c>
+      <c r="G49" s="4" t="s">
+        <v>29</v>
       </c>
       <c r="H49" s="3">
         <v>2</v>
@@ -3621,31 +3041,28 @@
       <c r="I49" s="3">
         <v>2</v>
       </c>
-      <c r="J49" s="4" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="E50" s="3">
         <v>201</v>
       </c>
       <c r="F50" s="3" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
       <c r="G50" s="3" t="s">
-        <v>137</v>
+        <v>126</v>
       </c>
       <c r="H50" s="3">
         <v>0</v>
@@ -3653,31 +3070,28 @@
       <c r="I50" s="3">
         <v>0</v>
       </c>
-      <c r="J50" s="4" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="E51" s="3">
         <v>203</v>
       </c>
       <c r="F51" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G51" s="5" t="s">
-        <v>62</v>
+        <v>8</v>
+      </c>
+      <c r="G51" s="4" t="s">
+        <v>56</v>
       </c>
       <c r="H51" s="3">
         <v>1</v>
@@ -3685,31 +3099,28 @@
       <c r="I51" s="3">
         <v>0</v>
       </c>
-      <c r="J51" s="4" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>183</v>
+        <v>168</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>181</v>
+        <v>166</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="E52" s="3">
         <v>202</v>
       </c>
       <c r="F52" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="G52" s="5" t="s">
-        <v>40</v>
+        <v>33</v>
+      </c>
+      <c r="G52" s="4" t="s">
+        <v>34</v>
       </c>
       <c r="H52" s="3">
         <v>2</v>
@@ -3717,28 +3128,25 @@
       <c r="I52" s="3">
         <v>0</v>
       </c>
-      <c r="J52" s="4" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>251</v>
+        <v>194</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>250</v>
+        <v>193</v>
       </c>
       <c r="E53" s="3">
         <v>0</v>
       </c>
       <c r="F53" s="3" t="s">
-        <v>246</v>
-      </c>
-      <c r="G53" s="5" t="s">
-        <v>84</v>
+        <v>189</v>
+      </c>
+      <c r="G53" s="4" t="s">
+        <v>76</v>
       </c>
       <c r="H53" s="3">
         <v>5</v>
@@ -3747,27 +3155,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>142</v>
+        <v>131</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
       <c r="E54" s="3">
         <v>210</v>
       </c>
       <c r="F54" s="3" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="G54" s="3" t="s">
-        <v>230</v>
+        <v>181</v>
       </c>
       <c r="H54" s="3">
         <v>6</v>
@@ -3775,31 +3183,28 @@
       <c r="I54" s="3">
         <v>0</v>
       </c>
-      <c r="J54" s="4" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>145</v>
+        <v>134</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
       <c r="E55" s="3">
         <v>211</v>
       </c>
       <c r="F55" s="3" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="G55" s="3" t="s">
-        <v>228</v>
+        <v>179</v>
       </c>
       <c r="H55" s="3">
         <v>7</v>
@@ -3807,31 +3212,28 @@
       <c r="I55" s="3">
         <v>0</v>
       </c>
-      <c r="J55" s="4" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>147</v>
+        <v>136</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
       <c r="E56" s="3">
         <v>212</v>
       </c>
       <c r="F56" s="3" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="G56" s="3" t="s">
-        <v>148</v>
+        <v>137</v>
       </c>
       <c r="H56" s="3">
         <v>8</v>
@@ -3839,28 +3241,25 @@
       <c r="I56" s="3">
         <v>0</v>
       </c>
-      <c r="J56" s="4" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>249</v>
+        <v>192</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>252</v>
+        <v>195</v>
       </c>
       <c r="E57" s="3">
         <v>0</v>
       </c>
       <c r="F57" s="3" t="s">
-        <v>246</v>
-      </c>
-      <c r="G57" s="5" t="s">
-        <v>84</v>
+        <v>189</v>
+      </c>
+      <c r="G57" s="4" t="s">
+        <v>76</v>
       </c>
       <c r="H57" s="3">
         <v>1</v>
@@ -3869,27 +3268,27 @@
         <v>2</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>140</v>
+        <v>129</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
       <c r="E58" s="3">
         <v>213</v>
       </c>
       <c r="F58" s="3" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="G58" s="3" t="s">
-        <v>229</v>
+        <v>180</v>
       </c>
       <c r="H58" s="3">
         <v>2</v>
@@ -3897,31 +3296,28 @@
       <c r="I58" s="3">
         <v>2</v>
       </c>
-      <c r="J58" s="4" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="59" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>225</v>
+        <v>178</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="E59" s="3">
         <v>220</v>
       </c>
       <c r="F59" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G59" s="5" t="s">
-        <v>35</v>
+        <v>8</v>
+      </c>
+      <c r="G59" s="4" t="s">
+        <v>29</v>
       </c>
       <c r="H59" s="3">
         <v>3</v>
@@ -3929,31 +3325,28 @@
       <c r="I59" s="3">
         <v>2</v>
       </c>
-      <c r="J59" s="4" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="60" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>224</v>
+        <v>177</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="E60" s="3">
         <v>221</v>
       </c>
       <c r="F60" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G60" s="5" t="s">
-        <v>84</v>
+        <v>8</v>
+      </c>
+      <c r="G60" s="4" t="s">
+        <v>76</v>
       </c>
       <c r="H60" s="3">
         <v>4</v>
@@ -3961,31 +3354,28 @@
       <c r="I60" s="3">
         <v>2</v>
       </c>
-      <c r="J60" s="4" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="61" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>223</v>
+        <v>176</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="E61" s="3">
         <v>222</v>
       </c>
       <c r="F61" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G61" s="5" t="s">
-        <v>84</v>
+        <v>8</v>
+      </c>
+      <c r="G61" s="4" t="s">
+        <v>76</v>
       </c>
       <c r="H61" s="3">
         <v>5</v>
@@ -3993,31 +3383,28 @@
       <c r="I61" s="3">
         <v>2</v>
       </c>
-      <c r="J61" s="4" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="62" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>222</v>
+        <v>175</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="E62" s="3">
         <v>223</v>
       </c>
       <c r="F62" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G62" s="5" t="s">
-        <v>84</v>
+        <v>8</v>
+      </c>
+      <c r="G62" s="4" t="s">
+        <v>76</v>
       </c>
       <c r="H62" s="3">
         <v>6</v>
@@ -4025,31 +3412,28 @@
       <c r="I62" s="3">
         <v>2</v>
       </c>
-      <c r="J62" s="4" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="63" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>221</v>
+        <v>174</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="E63" s="3">
         <v>224</v>
       </c>
       <c r="F63" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G63" s="5" t="s">
-        <v>84</v>
+        <v>8</v>
+      </c>
+      <c r="G63" s="4" t="s">
+        <v>76</v>
       </c>
       <c r="H63" s="3">
         <v>7</v>
@@ -4057,31 +3441,28 @@
       <c r="I63" s="3">
         <v>2</v>
       </c>
-      <c r="J63" s="4" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="64" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>220</v>
+        <v>173</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="E64" s="3">
         <v>225</v>
       </c>
       <c r="F64" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G64" s="5" t="s">
-        <v>84</v>
+        <v>8</v>
+      </c>
+      <c r="G64" s="4" t="s">
+        <v>76</v>
       </c>
       <c r="H64" s="3">
         <v>8</v>
@@ -4089,31 +3470,28 @@
       <c r="I64" s="3">
         <v>2</v>
       </c>
-      <c r="J64" s="4" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="65" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="B65" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="B65" s="3" t="s">
-        <v>128</v>
-      </c>
       <c r="C65" s="3" t="s">
-        <v>236</v>
+        <v>183</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="E65" s="3">
         <v>226</v>
       </c>
       <c r="F65" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G65" s="5" t="s">
-        <v>84</v>
+        <v>8</v>
+      </c>
+      <c r="G65" s="4" t="s">
+        <v>76</v>
       </c>
       <c r="H65" s="3">
         <v>9</v>
@@ -4121,31 +3499,28 @@
       <c r="I65" s="3">
         <v>2</v>
       </c>
-      <c r="J65" s="4" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="66" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="E66" s="3">
         <v>227</v>
       </c>
       <c r="F66" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G66" s="5" t="s">
-        <v>84</v>
+        <v>8</v>
+      </c>
+      <c r="G66" s="4" t="s">
+        <v>76</v>
       </c>
       <c r="H66" s="3">
         <v>10</v>
@@ -4153,653 +3528,506 @@
       <c r="I66" s="3">
         <v>2</v>
       </c>
-      <c r="J66" s="4" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B67" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C67" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="D67" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E67" s="3">
+        <v>120</v>
+      </c>
+      <c r="F67" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="G67" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="H67" s="3">
+        <v>0</v>
+      </c>
+      <c r="I67" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A68" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B68" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C68" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D68" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E68" s="3">
+        <v>138</v>
+      </c>
+      <c r="F68" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="G68" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="H68" s="3">
+        <v>1</v>
+      </c>
+      <c r="I68" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A69" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B69" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C69" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D69" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E69" s="3">
+        <v>145</v>
+      </c>
+      <c r="F69" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="G69" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="H69" s="3">
+        <v>2</v>
+      </c>
+      <c r="I69" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A70" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B70" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="C70" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="E70" s="3">
+        <v>0</v>
+      </c>
+      <c r="F70" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="G70" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="H70" s="3">
+        <v>3</v>
+      </c>
+      <c r="I70" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A71" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B71" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C71" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D71" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E71" s="3">
+        <v>141</v>
+      </c>
+      <c r="F71" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="G71" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H71" s="3">
+        <v>4</v>
+      </c>
+      <c r="I71" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A72" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B72" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C72" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="D72" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E72" s="3">
+        <v>137</v>
+      </c>
+      <c r="F72" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="G72" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H72" s="3">
+        <v>5</v>
+      </c>
+      <c r="I72" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A73" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B73" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C73" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D73" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E73" s="3">
+        <v>139</v>
+      </c>
+      <c r="F73" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="G73" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H73" s="3">
+        <v>6</v>
+      </c>
+      <c r="I73" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A74" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B74" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C74" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D74" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E74" s="3">
+        <v>122</v>
+      </c>
+      <c r="F74" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="G74" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H74" s="3">
+        <v>7</v>
+      </c>
+      <c r="I74" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A75" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B75" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C75" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D75" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E75" s="3">
+        <v>148</v>
+      </c>
+      <c r="F75" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="G75" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H75" s="3">
+        <v>8</v>
+      </c>
+      <c r="I75" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A76" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B76" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="C76" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="D76" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E76" s="3">
+        <v>133</v>
+      </c>
+      <c r="F76" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="G76" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="H76" s="3">
         <v>9</v>
       </c>
-      <c r="B67" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="D67" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E67" s="3">
-        <v>121</v>
-      </c>
-      <c r="F67" s="3" t="s">
+      <c r="I76" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A77" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B77" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="C77" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="D77" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E77" s="3">
+        <v>140</v>
+      </c>
+      <c r="F77" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="G77" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="H77" s="3">
+        <v>10</v>
+      </c>
+      <c r="I77" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A78" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B78" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="C78" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="D78" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E78" s="3">
+        <v>142</v>
+      </c>
+      <c r="F78" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G78" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="H78" s="3">
         <v>11</v>
       </c>
-      <c r="H67" s="3">
-        <v>0</v>
-      </c>
-      <c r="I67" s="3">
-        <v>0</v>
-      </c>
-      <c r="J67" s="4" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A68" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B68" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="D68" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E68" s="3">
-        <v>146</v>
-      </c>
-      <c r="F68" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="G68" s="5"/>
-      <c r="H68" s="3">
-        <v>0</v>
-      </c>
-      <c r="I68" s="3">
-        <v>0</v>
-      </c>
-      <c r="J68" s="4" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A69" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B69" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E69" s="3">
-        <v>500</v>
-      </c>
-      <c r="F69" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H69" s="3">
-        <v>0</v>
-      </c>
-      <c r="I69" s="3">
-        <v>0</v>
-      </c>
-      <c r="J69" s="4" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A70" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B70" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E70" s="3">
-        <v>501</v>
-      </c>
-      <c r="F70" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="H70" s="3">
-        <v>0</v>
-      </c>
-      <c r="I70" s="3">
-        <v>0</v>
-      </c>
-      <c r="J70" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="71" spans="1:10" ht="165" x14ac:dyDescent="0.25">
-      <c r="A71" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="B71" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="C71" s="3" t="s">
-        <v>266</v>
-      </c>
-      <c r="D71" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E71" s="3">
-        <v>120</v>
-      </c>
-      <c r="F71" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="G71" s="5" t="s">
-        <v>161</v>
-      </c>
-      <c r="H71" s="3">
-        <v>0</v>
-      </c>
-      <c r="I71" s="3">
-        <v>0</v>
-      </c>
-      <c r="J71" s="8" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="72" spans="1:10" ht="165" x14ac:dyDescent="0.25">
-      <c r="A72" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="B72" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="C72" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="D72" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E72" s="3">
+      <c r="I78" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A79" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B79" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="C79" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="E79" s="3">
+        <v>0</v>
+      </c>
+      <c r="F79" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="G79" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="H79" s="3">
+        <v>3</v>
+      </c>
+      <c r="I79" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A80" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B80" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="C80" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="D80" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E80" s="3">
+        <v>112</v>
+      </c>
+      <c r="F80" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="G80" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="H80" s="3">
+        <v>4</v>
+      </c>
+      <c r="I80" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A81" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B81" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="F72" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="G72" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="H72" s="3">
-        <v>1</v>
-      </c>
-      <c r="I72" s="3">
-        <v>0</v>
-      </c>
-      <c r="J72" s="4" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="73" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A73" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="B73" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="C73" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="D73" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E73" s="3">
-        <v>145</v>
-      </c>
-      <c r="F73" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="G73" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="H73" s="3">
-        <v>2</v>
-      </c>
-      <c r="I73" s="3">
-        <v>0</v>
-      </c>
-      <c r="J73" s="4" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A74" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="B74" s="3" t="s">
-        <v>269</v>
-      </c>
-      <c r="C74" s="3" t="s">
-        <v>270</v>
-      </c>
-      <c r="E74" s="3">
-        <v>0</v>
-      </c>
-      <c r="F74" s="3" t="s">
-        <v>246</v>
-      </c>
-      <c r="G74" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="H74" s="3">
-        <v>3</v>
-      </c>
-      <c r="I74" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A75" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="B75" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="C75" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="D75" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E75" s="3">
-        <v>141</v>
-      </c>
-      <c r="F75" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="G75" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="H75" s="3">
-        <v>4</v>
-      </c>
-      <c r="I75" s="3">
-        <v>0</v>
-      </c>
-      <c r="J75" s="4" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="76" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A76" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="B76" s="3" t="s">
+      <c r="C81" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="D81" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E81" s="3">
+        <v>110</v>
+      </c>
+      <c r="F81" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G81" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C76" s="3" t="s">
-        <v>265</v>
-      </c>
-      <c r="D76" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E76" s="3">
-        <v>137</v>
-      </c>
-      <c r="F76" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="G76" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="H76" s="3">
+      <c r="H81" s="3">
         <v>5</v>
       </c>
-      <c r="I76" s="3">
-        <v>0</v>
-      </c>
-      <c r="J76" s="4" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="77" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A77" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="B77" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="C77" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="D77" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E77" s="3">
-        <v>139</v>
-      </c>
-      <c r="F77" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="G77" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="H77" s="3">
+      <c r="I81" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A82" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B82" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="C82" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="D82" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E82" s="3">
+        <v>111</v>
+      </c>
+      <c r="F82" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="G82" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="H82" s="3">
         <v>6</v>
       </c>
-      <c r="I77" s="3">
-        <v>0</v>
-      </c>
-      <c r="J77" s="4" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="78" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A78" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="B78" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="C78" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="D78" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E78" s="3">
-        <v>122</v>
-      </c>
-      <c r="F78" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="G78" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="H78" s="3">
+      <c r="I82" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A83" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B83" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="C83" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="D83" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E83" s="3">
+        <v>112</v>
+      </c>
+      <c r="F83" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="G83" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="H83" s="3">
         <v>7</v>
       </c>
-      <c r="I78" s="3">
-        <v>0</v>
-      </c>
-      <c r="J78" s="4" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A79" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="B79" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="C79" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="D79" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E79" s="3">
-        <v>148</v>
-      </c>
-      <c r="F79" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="G79" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="H79" s="3">
-        <v>8</v>
-      </c>
-      <c r="I79" s="3">
-        <v>0</v>
-      </c>
-      <c r="J79" s="4" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="80" spans="1:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="A80" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="B80" s="3" t="s">
-        <v>289</v>
-      </c>
-      <c r="C80" s="3" t="s">
-        <v>290</v>
-      </c>
-      <c r="D80" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E80" s="3">
-        <v>133</v>
-      </c>
-      <c r="F80" s="3" t="s">
-        <v>291</v>
-      </c>
-      <c r="G80" s="5" t="s">
-        <v>159</v>
-      </c>
-      <c r="H80" s="3">
-        <v>9</v>
-      </c>
-      <c r="I80" s="3">
-        <v>0</v>
-      </c>
-      <c r="J80" s="4" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="81" spans="1:10" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A81" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="B81" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="C81" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="D81" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E81" s="3">
-        <v>140</v>
-      </c>
-      <c r="F81" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="G81" s="5" t="s">
-        <v>159</v>
-      </c>
-      <c r="H81" s="3">
-        <v>10</v>
-      </c>
-      <c r="I81" s="3">
-        <v>0</v>
-      </c>
-      <c r="J81" s="4" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="82" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A82" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="B82" s="3" t="s">
-        <v>243</v>
-      </c>
-      <c r="C82" s="3" t="s">
-        <v>244</v>
-      </c>
-      <c r="D82" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E82" s="3">
-        <v>142</v>
-      </c>
-      <c r="F82" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G82" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="H82" s="3">
-        <v>11</v>
-      </c>
-      <c r="I82" s="3">
-        <v>0</v>
-      </c>
-      <c r="J82" s="4" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A83" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="B83" s="3" t="s">
-        <v>267</v>
-      </c>
-      <c r="C83" s="3" t="s">
-        <v>268</v>
-      </c>
-      <c r="E83" s="3">
-        <v>0</v>
-      </c>
-      <c r="F83" s="3" t="s">
-        <v>246</v>
-      </c>
-      <c r="G83" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="H83" s="3">
-        <v>3</v>
-      </c>
       <c r="I83" s="3">
         <v>2</v>
       </c>
     </row>
-    <row r="84" spans="1:10" ht="270" x14ac:dyDescent="0.25">
-      <c r="A84" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="B84" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="C84" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="D84" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E84" s="3">
-        <v>112</v>
-      </c>
-      <c r="F84" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="G84" s="5" t="s">
-        <v>153</v>
-      </c>
-      <c r="H84" s="3">
-        <v>4</v>
-      </c>
-      <c r="I84" s="3">
-        <v>2</v>
-      </c>
-      <c r="J84" s="4" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="85" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A85" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="B85" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="C85" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="D85" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E85" s="3">
-        <v>110</v>
-      </c>
-      <c r="F85" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G85" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="H85" s="3">
-        <v>5</v>
-      </c>
-      <c r="I85" s="3">
-        <v>2</v>
-      </c>
-      <c r="J85" s="4" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="86" spans="1:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="A86" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="B86" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="C86" s="3" t="s">
-        <v>185</v>
-      </c>
-      <c r="D86" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E86" s="3">
-        <v>111</v>
-      </c>
-      <c r="F86" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="G86" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="H86" s="3">
-        <v>6</v>
-      </c>
-      <c r="I86" s="3">
-        <v>2</v>
-      </c>
-      <c r="J86" s="4" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="87" spans="1:10" ht="405" x14ac:dyDescent="0.25">
-      <c r="A87" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="B87" s="3" t="s">
-        <v>296</v>
-      </c>
-      <c r="C87" s="3" t="s">
-        <v>297</v>
-      </c>
-      <c r="D87" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E87" s="3">
-        <v>112</v>
-      </c>
-      <c r="F87" s="3" t="s">
-        <v>298</v>
-      </c>
-      <c r="G87" s="3" t="s">
-        <v>299</v>
-      </c>
-      <c r="H87" s="3">
-        <v>7</v>
-      </c>
-      <c r="I87" s="3">
-        <v>2</v>
-      </c>
-      <c r="J87" s="4" t="s">
-        <v>300</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:J87" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J86">
-      <sortCondition ref="A2:A86"/>
-      <sortCondition ref="I2:I86"/>
-      <sortCondition ref="H2:H86"/>
+  <autoFilter ref="A1:I83" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I82">
+      <sortCondition ref="A2:A82"/>
+      <sortCondition ref="I2:I82"/>
+      <sortCondition ref="H2:H82"/>
     </sortState>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:J87">
-    <sortCondition ref="A3:A87"/>
-    <sortCondition ref="I3:I87"/>
-    <sortCondition ref="H3:H87"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:I83">
+    <sortCondition ref="A3:A83"/>
+    <sortCondition ref="I3:I83"/>
+    <sortCondition ref="H3:H83"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Changed repeat turn to an enumeration (none, once, always). Added game Ali_Guli_Mane.
</commit_message>
<xml_diff>
--- a/src/game_params.xlsx
+++ b/src/game_params.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Activity_Data\Mancala_github\MancalaGames\src\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\annda\Desktop\software\Mancala_github\MancalaGames\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C25E4685-125A-4291-9EE7-D0AA49254DAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4384FB9B-1BE9-4B17-92C5-6ECB8E494A23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6330" yWindow="360" windowWidth="20520" windowHeight="15510" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="14595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="game_params" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="241">
   <si>
     <t>tab</t>
   </si>
@@ -754,13 +754,19 @@
   </si>
   <si>
     <t>CaptType</t>
+  </si>
+  <si>
+    <t>CaptRTurn</t>
+  </si>
+  <si>
+    <t>NO_REPEAT</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1633,24 +1639,24 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G47" sqref="G47"/>
+      <selection pane="bottomLeft" activeCell="G84" sqref="G84"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" style="3" customWidth="1"/>
+    <col min="1" max="1" width="11.59765625" style="3" customWidth="1"/>
     <col min="2" max="2" width="16" style="3" customWidth="1"/>
-    <col min="3" max="3" width="36.28515625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="16.5703125" style="3" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="14.7109375" style="3" customWidth="1"/>
-    <col min="7" max="7" width="26.140625" style="3" customWidth="1"/>
-    <col min="8" max="8" width="6.7109375" style="3" customWidth="1"/>
-    <col min="9" max="9" width="7.28515625" style="3" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="3"/>
+    <col min="3" max="3" width="36.265625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="16.59765625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="11.59765625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="14.73046875" style="3" customWidth="1"/>
+    <col min="7" max="7" width="26.1328125" style="3" customWidth="1"/>
+    <col min="8" max="8" width="6.73046875" style="3" customWidth="1"/>
+    <col min="9" max="9" width="7.265625" style="3" customWidth="1"/>
+    <col min="10" max="16384" width="9.1328125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1679,7 +1685,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" s="1" customFormat="1">
       <c r="A2" s="3" t="s">
         <v>81</v>
       </c>
@@ -1706,7 +1712,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9">
       <c r="A3" s="3" t="s">
         <v>81</v>
       </c>
@@ -1735,7 +1741,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9">
       <c r="A4" s="3" t="s">
         <v>81</v>
       </c>
@@ -1764,7 +1770,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9">
       <c r="A5" s="3" t="s">
         <v>81</v>
       </c>
@@ -1793,7 +1799,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9">
       <c r="A6" s="3" t="s">
         <v>81</v>
       </c>
@@ -1822,7 +1828,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9">
       <c r="A7" s="3" t="s">
         <v>81</v>
       </c>
@@ -1848,7 +1854,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9">
       <c r="A8" s="3" t="s">
         <v>81</v>
       </c>
@@ -1877,7 +1883,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9">
       <c r="A9" s="3" t="s">
         <v>81</v>
       </c>
@@ -1906,7 +1912,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9">
       <c r="A10" s="3" t="s">
         <v>81</v>
       </c>
@@ -1935,7 +1941,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9">
       <c r="A11" s="3" t="s">
         <v>81</v>
       </c>
@@ -1961,7 +1967,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9">
       <c r="A12" s="3" t="s">
         <v>81</v>
       </c>
@@ -1990,7 +1996,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9">
       <c r="A13" s="3" t="s">
         <v>81</v>
       </c>
@@ -2016,7 +2022,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9">
       <c r="A14" s="3" t="s">
         <v>81</v>
       </c>
@@ -2045,7 +2051,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9">
       <c r="A15" s="3" t="s">
         <v>81</v>
       </c>
@@ -2074,7 +2080,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9">
       <c r="A16" s="3" t="s">
         <v>81</v>
       </c>
@@ -2100,7 +2106,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9">
       <c r="A17" s="3" t="s">
         <v>81</v>
       </c>
@@ -2129,7 +2135,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9">
       <c r="A18" s="3" t="s">
         <v>81</v>
       </c>
@@ -2158,7 +2164,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9">
       <c r="A19" s="3" t="s">
         <v>81</v>
       </c>
@@ -2187,7 +2193,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9">
       <c r="A20" s="3" t="s">
         <v>81</v>
       </c>
@@ -2216,7 +2222,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9">
       <c r="A21" s="3" t="s">
         <v>81</v>
       </c>
@@ -2242,7 +2248,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9">
       <c r="A22" s="3" t="s">
         <v>81</v>
       </c>
@@ -2259,10 +2265,10 @@
         <v>108</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>33</v>
+        <v>239</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>34</v>
+        <v>240</v>
       </c>
       <c r="H22" s="3">
         <v>9</v>
@@ -2271,7 +2277,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9">
       <c r="A23" s="3" t="s">
         <v>81</v>
       </c>
@@ -2300,7 +2306,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9">
       <c r="A24" s="3" t="s">
         <v>30</v>
       </c>
@@ -2329,7 +2335,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9">
       <c r="A25" s="3" t="s">
         <v>30</v>
       </c>
@@ -2358,7 +2364,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9">
       <c r="A26" s="3" t="s">
         <v>30</v>
       </c>
@@ -2387,7 +2393,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9">
       <c r="A27" s="3" t="s">
         <v>30</v>
       </c>
@@ -2413,7 +2419,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9">
       <c r="A28" s="3" t="s">
         <v>30</v>
       </c>
@@ -2442,7 +2448,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9">
       <c r="A29" s="3" t="s">
         <v>30</v>
       </c>
@@ -2471,7 +2477,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9">
       <c r="A30" s="3" t="s">
         <v>30</v>
       </c>
@@ -2497,7 +2503,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9">
       <c r="A31" s="3" t="s">
         <v>30</v>
       </c>
@@ -2526,7 +2532,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9">
       <c r="A32" s="3" t="s">
         <v>30</v>
       </c>
@@ -2555,7 +2561,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9">
       <c r="A33" s="3" t="s">
         <v>30</v>
       </c>
@@ -2584,7 +2590,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9">
       <c r="A34" s="3" t="s">
         <v>30</v>
       </c>
@@ -2613,7 +2619,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9">
       <c r="A35" s="3" t="s">
         <v>30</v>
       </c>
@@ -2639,7 +2645,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9">
       <c r="A36" s="3" t="s">
         <v>30</v>
       </c>
@@ -2668,7 +2674,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9">
       <c r="A37" s="3" t="s">
         <v>30</v>
       </c>
@@ -2697,7 +2703,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9">
       <c r="A38" s="3" t="s">
         <v>30</v>
       </c>
@@ -2726,7 +2732,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9">
       <c r="A39" s="3" t="s">
         <v>30</v>
       </c>
@@ -2752,7 +2758,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9">
       <c r="A40" s="3" t="s">
         <v>30</v>
       </c>
@@ -2781,7 +2787,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9">
       <c r="A41" s="3" t="s">
         <v>30</v>
       </c>
@@ -2810,7 +2816,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9">
       <c r="A42" s="3" t="s">
         <v>30</v>
       </c>
@@ -2839,7 +2845,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9">
       <c r="A43" s="3" t="s">
         <v>30</v>
       </c>
@@ -2868,7 +2874,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9">
       <c r="A44" s="3" t="s">
         <v>9</v>
       </c>
@@ -2897,7 +2903,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9">
       <c r="A45" s="3" t="s">
         <v>9</v>
       </c>
@@ -2926,7 +2932,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9">
       <c r="A46" s="3" t="s">
         <v>9</v>
       </c>
@@ -2955,7 +2961,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" ht="28.5">
       <c r="A47" s="3" t="s">
         <v>9</v>
       </c>
@@ -2984,7 +2990,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9">
       <c r="A48" s="3" t="s">
         <v>9</v>
       </c>
@@ -3013,7 +3019,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9">
       <c r="A49" s="3" t="s">
         <v>9</v>
       </c>
@@ -3042,7 +3048,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9">
       <c r="A50" s="3" t="s">
         <v>108</v>
       </c>
@@ -3071,7 +3077,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9">
       <c r="A51" s="3" t="s">
         <v>108</v>
       </c>
@@ -3100,7 +3106,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9">
       <c r="A52" s="3" t="s">
         <v>108</v>
       </c>
@@ -3129,7 +3135,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9">
       <c r="A53" s="3" t="s">
         <v>108</v>
       </c>
@@ -3155,7 +3161,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9">
       <c r="A54" s="3" t="s">
         <v>108</v>
       </c>
@@ -3184,7 +3190,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9">
       <c r="A55" s="3" t="s">
         <v>108</v>
       </c>
@@ -3213,7 +3219,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9">
       <c r="A56" s="3" t="s">
         <v>108</v>
       </c>
@@ -3242,7 +3248,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9">
       <c r="A57" s="3" t="s">
         <v>108</v>
       </c>
@@ -3268,7 +3274,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9">
       <c r="A58" s="3" t="s">
         <v>108</v>
       </c>
@@ -3297,7 +3303,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9">
       <c r="A59" s="3" t="s">
         <v>108</v>
       </c>
@@ -3326,7 +3332,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9">
       <c r="A60" s="3" t="s">
         <v>108</v>
       </c>
@@ -3355,7 +3361,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9">
       <c r="A61" s="3" t="s">
         <v>108</v>
       </c>
@@ -3384,7 +3390,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9">
       <c r="A62" s="3" t="s">
         <v>108</v>
       </c>
@@ -3413,7 +3419,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9">
       <c r="A63" s="3" t="s">
         <v>108</v>
       </c>
@@ -3442,7 +3448,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9">
       <c r="A64" s="3" t="s">
         <v>108</v>
       </c>
@@ -3471,7 +3477,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9">
       <c r="A65" s="3" t="s">
         <v>108</v>
       </c>
@@ -3500,7 +3506,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9">
       <c r="A66" s="3" t="s">
         <v>108</v>
       </c>
@@ -3529,7 +3535,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:9">
       <c r="A67" s="3" t="s">
         <v>59</v>
       </c>
@@ -3558,7 +3564,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9">
       <c r="A68" s="3" t="s">
         <v>59</v>
       </c>
@@ -3587,7 +3593,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:9">
       <c r="A69" s="3" t="s">
         <v>59</v>
       </c>
@@ -3616,7 +3622,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:9">
       <c r="A70" s="3" t="s">
         <v>59</v>
       </c>
@@ -3642,7 +3648,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:9">
       <c r="A71" s="3" t="s">
         <v>59</v>
       </c>
@@ -3671,7 +3677,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:9">
       <c r="A72" s="3" t="s">
         <v>59</v>
       </c>
@@ -3700,7 +3706,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:9">
       <c r="A73" s="3" t="s">
         <v>59</v>
       </c>
@@ -3729,7 +3735,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:9">
       <c r="A74" s="3" t="s">
         <v>59</v>
       </c>
@@ -3758,7 +3764,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:9">
       <c r="A75" s="3" t="s">
         <v>59</v>
       </c>
@@ -3787,7 +3793,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:9">
       <c r="A76" s="3" t="s">
         <v>59</v>
       </c>
@@ -3816,7 +3822,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:9">
       <c r="A77" s="3" t="s">
         <v>59</v>
       </c>
@@ -3845,7 +3851,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:9">
       <c r="A78" s="3" t="s">
         <v>59</v>
       </c>
@@ -3874,7 +3880,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:9">
       <c r="A79" s="3" t="s">
         <v>59</v>
       </c>
@@ -3900,7 +3906,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:9">
       <c r="A80" s="3" t="s">
         <v>59</v>
       </c>
@@ -3929,7 +3935,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:9">
       <c r="A81" s="3" t="s">
         <v>59</v>
       </c>
@@ -3958,7 +3964,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:9">
       <c r="A82" s="3" t="s">
         <v>59</v>
       </c>
@@ -3987,7 +3993,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:9">
       <c r="A83" s="3" t="s">
         <v>59</v>
       </c>

</xml_diff>

<commit_message>
Corrected clear and deprive enders to actually end a game when requested. Added a parameter so that behavior of the quitter can be controlled. Allow both the ender and quitter to be accessed from the menu, menu items are greyed if they do the same as another menu item. Combined end_round into end_game and paramterized it. Added a means to omit missing enum errors, used for quitter because we only need to describe EndGameSeeds once. Updated the csv to xlsx formatter for the new parameter. Corrected enders for En Dodoi, Qelat and Urim. Chose quitters for all games that should not be the default DIVVY.
</commit_message>
<xml_diff>
--- a/src/game_params.xlsx
+++ b/src/game_params.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\annda\Desktop\software\Mancala_github\MancalaGames\src\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Activity_Data\Mancala_github\MancalaGames\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4384FB9B-1BE9-4B17-92C5-6ECB8E494A23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE20A46C-BACF-4957-BC8F-DFD822755C8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="14595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="game_params" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">game_params!$A$1:$I$83</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">game_params!$A$1:$I$84</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="244">
   <si>
     <t>tab</t>
   </si>
@@ -705,9 +705,6 @@
     <t>unclaimed</t>
   </si>
   <si>
-    <t>End Game Seeds</t>
-  </si>
-  <si>
     <t>EndGameSeeds</t>
   </si>
   <si>
@@ -760,13 +757,25 @@
   </si>
   <si>
     <t>NO_REPEAT</t>
+  </si>
+  <si>
+    <t>DIVVIED</t>
+  </si>
+  <si>
+    <t>Quit Game Seeds</t>
+  </si>
+  <si>
+    <t>quitter</t>
+  </si>
+  <si>
+    <t>Unclaimed Seeds at End</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1635,28 +1644,28 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:I83"/>
+  <dimension ref="A1:I84"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G84" sqref="G84"/>
+      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.59765625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="11.5703125" style="3" customWidth="1"/>
     <col min="2" max="2" width="16" style="3" customWidth="1"/>
-    <col min="3" max="3" width="36.265625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="16.59765625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="11.59765625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="14.73046875" style="3" customWidth="1"/>
-    <col min="7" max="7" width="26.1328125" style="3" customWidth="1"/>
-    <col min="8" max="8" width="6.73046875" style="3" customWidth="1"/>
-    <col min="9" max="9" width="7.265625" style="3" customWidth="1"/>
-    <col min="10" max="16384" width="9.1328125" style="3"/>
+    <col min="3" max="3" width="36.28515625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="16.5703125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" style="3" customWidth="1"/>
+    <col min="7" max="7" width="26.140625" style="3" customWidth="1"/>
+    <col min="8" max="8" width="6.7109375" style="3" customWidth="1"/>
+    <col min="9" max="9" width="7.28515625" style="3" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1685,7 +1694,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="1" customFormat="1">
+    <row r="2" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>81</v>
       </c>
@@ -1712,7 +1721,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>81</v>
       </c>
@@ -1741,7 +1750,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>81</v>
       </c>
@@ -1770,7 +1779,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>81</v>
       </c>
@@ -1799,7 +1808,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>81</v>
       </c>
@@ -1828,7 +1837,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>81</v>
       </c>
@@ -1854,7 +1863,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>81</v>
       </c>
@@ -1883,7 +1892,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>81</v>
       </c>
@@ -1897,7 +1906,7 @@
         <v>16</v>
       </c>
       <c r="E9" s="3">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>98</v>
@@ -1912,7 +1921,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>81</v>
       </c>
@@ -1926,7 +1935,7 @@
         <v>16</v>
       </c>
       <c r="E10" s="3">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>33</v>
@@ -1941,7 +1950,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>81</v>
       </c>
@@ -1967,15 +1976,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>81</v>
       </c>
       <c r="B12" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>236</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>237</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>16</v>
@@ -1984,7 +1993,7 @@
         <v>106</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="G12" s="4" t="s">
         <v>147</v>
@@ -1996,7 +2005,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>81</v>
       </c>
@@ -2022,7 +2031,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>81</v>
       </c>
@@ -2051,7 +2060,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>81</v>
       </c>
@@ -2080,7 +2089,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>81</v>
       </c>
@@ -2106,7 +2115,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>81</v>
       </c>
@@ -2135,15 +2144,15 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>81</v>
       </c>
       <c r="B18" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="C18" s="3" t="s">
         <v>225</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>226</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>16</v>
@@ -2152,10 +2161,10 @@
         <v>130</v>
       </c>
       <c r="F18" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="G18" s="4" t="s">
         <v>227</v>
-      </c>
-      <c r="G18" s="4" t="s">
-        <v>228</v>
       </c>
       <c r="H18" s="3">
         <v>5</v>
@@ -2164,7 +2173,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>81</v>
       </c>
@@ -2193,7 +2202,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>81</v>
       </c>
@@ -2222,7 +2231,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>81</v>
       </c>
@@ -2248,7 +2257,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>81</v>
       </c>
@@ -2265,10 +2274,10 @@
         <v>108</v>
       </c>
       <c r="F22" s="3" t="s">
+        <v>238</v>
+      </c>
+      <c r="G22" s="4" t="s">
         <v>239</v>
-      </c>
-      <c r="G22" s="4" t="s">
-        <v>240</v>
       </c>
       <c r="H22" s="3">
         <v>9</v>
@@ -2277,7 +2286,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>81</v>
       </c>
@@ -2306,7 +2315,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>30</v>
       </c>
@@ -2335,7 +2344,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>30</v>
       </c>
@@ -2364,7 +2373,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>30</v>
       </c>
@@ -2372,7 +2381,7 @@
         <v>221</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>222</v>
+        <v>243</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>16</v>
@@ -2381,11 +2390,11 @@
         <v>147</v>
       </c>
       <c r="F26" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="G26" s="4" t="s">
         <v>223</v>
       </c>
-      <c r="G26" s="4" t="s">
-        <v>224</v>
-      </c>
       <c r="H26" s="3">
         <v>2</v>
       </c>
@@ -2393,53 +2402,53 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:9">
-      <c r="A27" s="3" t="s">
+    <row r="27" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>30</v>
       </c>
-      <c r="B27" s="3" t="s">
-        <v>216</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="E27" s="3">
-        <v>0</v>
-      </c>
-      <c r="F27" s="3" t="s">
-        <v>189</v>
-      </c>
-      <c r="G27" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="H27" s="3">
+      <c r="B27" t="s">
+        <v>242</v>
+      </c>
+      <c r="C27" t="s">
+        <v>241</v>
+      </c>
+      <c r="D27" t="s">
+        <v>16</v>
+      </c>
+      <c r="E27">
+        <v>148</v>
+      </c>
+      <c r="F27" t="s">
+        <v>222</v>
+      </c>
+      <c r="G27" t="s">
+        <v>240</v>
+      </c>
+      <c r="H27">
         <v>3</v>
       </c>
-      <c r="I27" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9">
+      <c r="I27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>50</v>
+        <v>216</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>16</v>
+        <v>190</v>
       </c>
       <c r="E28" s="3">
-        <v>143</v>
+        <v>0</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>52</v>
+        <v>189</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>53</v>
+        <v>76</v>
       </c>
       <c r="H28" s="3">
         <v>4</v>
@@ -2448,27 +2457,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:9">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>153</v>
+        <v>50</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>152</v>
+        <v>51</v>
       </c>
       <c r="D29" s="3" t="s">
         <v>16</v>
       </c>
       <c r="E29" s="3">
-        <v>132</v>
+        <v>143</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>154</v>
+        <v>52</v>
       </c>
       <c r="G29" s="4" t="s">
-        <v>147</v>
+        <v>53</v>
       </c>
       <c r="H29" s="3">
         <v>5</v>
@@ -2477,218 +2486,218 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:9">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>217</v>
+        <v>153</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>218</v>
+        <v>152</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>16</v>
       </c>
       <c r="E30" s="3">
-        <v>0</v>
+        <v>132</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>189</v>
+        <v>154</v>
       </c>
       <c r="G30" s="4" t="s">
-        <v>76</v>
+        <v>147</v>
       </c>
       <c r="H30" s="3">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I30" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:9">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>54</v>
+        <v>217</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D31" s="3" t="s">
-        <v>16</v>
+        <v>218</v>
       </c>
       <c r="E31" s="3">
-        <v>119</v>
+        <v>0</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>8</v>
+        <v>189</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>56</v>
+        <v>76</v>
       </c>
       <c r="H31" s="3">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I31" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:9">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>144</v>
+        <v>54</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>145</v>
+        <v>55</v>
       </c>
       <c r="D32" s="3" t="s">
         <v>16</v>
       </c>
       <c r="E32" s="3">
-        <v>101</v>
+        <v>119</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>146</v>
+        <v>8</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>147</v>
+        <v>56</v>
       </c>
       <c r="H32" s="3">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I32" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:9">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>43</v>
+        <v>144</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>44</v>
+        <v>145</v>
       </c>
       <c r="D33" s="3" t="s">
         <v>16</v>
       </c>
       <c r="E33" s="3">
-        <v>144</v>
+        <v>101</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>33</v>
+        <v>146</v>
       </c>
       <c r="G33" s="4" t="s">
-        <v>45</v>
+        <v>147</v>
       </c>
       <c r="H33" s="3">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="I33" s="3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D34" s="3" t="s">
         <v>16</v>
       </c>
       <c r="E34" s="3">
-        <v>127</v>
+        <v>144</v>
       </c>
       <c r="F34" s="3" t="s">
         <v>33</v>
       </c>
       <c r="G34" s="4" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="H34" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I34" s="3">
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:9">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>220</v>
+        <v>41</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>219</v>
+        <v>42</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>16</v>
       </c>
       <c r="E35" s="3">
-        <v>0</v>
+        <v>127</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>189</v>
+        <v>33</v>
       </c>
       <c r="G35" s="4" t="s">
-        <v>76</v>
+        <v>34</v>
       </c>
       <c r="H35" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I35" s="3">
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:9">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>31</v>
+        <v>220</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D36" s="3" t="s">
-        <v>16</v>
+        <v>219</v>
       </c>
       <c r="E36" s="3">
-        <v>125</v>
+        <v>0</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>33</v>
+        <v>189</v>
       </c>
       <c r="G36" s="4" t="s">
-        <v>34</v>
+        <v>76</v>
       </c>
       <c r="H36" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I36" s="3">
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:9">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>57</v>
+        <v>31</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>58</v>
+        <v>32</v>
       </c>
       <c r="D37" s="3" t="s">
         <v>16</v>
       </c>
       <c r="E37" s="3">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F37" s="3" t="s">
         <v>33</v>
@@ -2697,685 +2706,685 @@
         <v>34</v>
       </c>
       <c r="H37" s="3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I37" s="3">
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:9">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>102</v>
+        <v>57</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>103</v>
+        <v>58</v>
       </c>
       <c r="D38" s="3" t="s">
         <v>16</v>
       </c>
       <c r="E38" s="3">
-        <v>117</v>
+        <v>126</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>104</v>
+        <v>33</v>
       </c>
       <c r="G38" s="4" t="s">
-        <v>105</v>
+        <v>34</v>
       </c>
       <c r="H38" s="3">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="I38" s="3">
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:9">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>191</v>
+        <v>102</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>215</v>
+        <v>103</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>16</v>
       </c>
       <c r="E39" s="3">
-        <v>0</v>
+        <v>117</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>189</v>
+        <v>104</v>
       </c>
       <c r="G39" s="4" t="s">
-        <v>76</v>
+        <v>105</v>
       </c>
       <c r="H39" s="3">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="I39" s="3">
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:9">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>35</v>
+        <v>191</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D40" s="3" t="s">
-        <v>16</v>
+        <v>215</v>
       </c>
       <c r="E40" s="3">
-        <v>136</v>
+        <v>0</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>36</v>
+        <v>189</v>
       </c>
       <c r="G40" s="4" t="s">
-        <v>182</v>
+        <v>76</v>
       </c>
       <c r="H40" s="3">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="I40" s="3">
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:9">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D41" s="3" t="s">
         <v>16</v>
       </c>
       <c r="E41" s="3">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="G41" s="4" t="s">
-        <v>40</v>
+        <v>182</v>
       </c>
       <c r="H41" s="3">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="I41" s="3">
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:9">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>163</v>
+        <v>37</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>164</v>
+        <v>38</v>
       </c>
       <c r="D42" s="3" t="s">
         <v>16</v>
       </c>
       <c r="E42" s="3">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>165</v>
+        <v>39</v>
       </c>
       <c r="G42" s="4" t="s">
-        <v>172</v>
+        <v>40</v>
       </c>
       <c r="H42" s="3">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="I42" s="3">
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:9">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B43" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E43" s="3">
+        <v>134</v>
+      </c>
+      <c r="F43" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="G43" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="H43" s="3">
+        <v>9</v>
+      </c>
+      <c r="I43" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B44" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="C43" s="3" t="s">
+      <c r="C44" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="D43" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E43" s="3">
+      <c r="D44" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E44" s="3">
         <v>102</v>
       </c>
-      <c r="F43" s="3" t="s">
+      <c r="F44" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="G43" s="4" t="s">
+      <c r="G44" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="H43" s="3">
-        <v>11</v>
-      </c>
-      <c r="I43" s="3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9">
-      <c r="A44" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B44" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C44" s="3" t="s">
+      <c r="H44" s="3">
         <v>10</v>
       </c>
-      <c r="D44" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E44" s="3">
-        <v>1</v>
-      </c>
-      <c r="F44" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="G44" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H44" s="3">
-        <v>0</v>
-      </c>
       <c r="I44" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="E45" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>8</v>
+        <v>123</v>
       </c>
       <c r="G45" s="4" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="H45" s="3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I45" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:9">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="E46" s="3">
-        <v>118</v>
+        <v>2</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="G46" s="4" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="H46" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I46" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:9" ht="28.5">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D47" s="3" t="s">
         <v>16</v>
       </c>
       <c r="E47" s="3">
-        <v>5</v>
+        <v>118</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G47" s="5" t="s">
-        <v>122</v>
+        <v>12</v>
+      </c>
+      <c r="G47" s="4" t="s">
+        <v>19</v>
       </c>
       <c r="H47" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I47" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:9">
+    <row r="48" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="D48" s="3" t="s">
         <v>16</v>
       </c>
       <c r="E48" s="3">
+        <v>5</v>
+      </c>
+      <c r="F48" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G48" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="H48" s="3">
         <v>4</v>
       </c>
-      <c r="F48" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G48" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H48" s="3">
-        <v>0</v>
-      </c>
       <c r="I48" s="3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B49" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E49" s="3">
+        <v>4</v>
+      </c>
+      <c r="F49" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G49" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H49" s="3">
+        <v>0</v>
+      </c>
+      <c r="I49" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A50" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B50" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C49" s="3" t="s">
+      <c r="C50" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D49" s="3" t="s">
+      <c r="D50" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="E49" s="3">
+      <c r="E50" s="3">
         <v>3</v>
       </c>
-      <c r="F49" s="3" t="s">
+      <c r="F50" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G49" s="4" t="s">
+      <c r="G50" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="H49" s="3">
-        <v>2</v>
-      </c>
-      <c r="I49" s="3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9">
-      <c r="A50" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="B50" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="C50" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="D50" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="E50" s="3">
-        <v>201</v>
-      </c>
-      <c r="F50" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="G50" s="3" t="s">
-        <v>126</v>
-      </c>
       <c r="H50" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I50" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
         <v>108</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="D51" s="3" t="s">
         <v>121</v>
       </c>
       <c r="E51" s="3">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="F51" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G51" s="4" t="s">
-        <v>56</v>
+        <v>125</v>
+      </c>
+      <c r="G51" s="3" t="s">
+        <v>126</v>
       </c>
       <c r="H51" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I51" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:9">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
         <v>108</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>168</v>
+        <v>119</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>166</v>
+        <v>120</v>
       </c>
       <c r="D52" s="3" t="s">
         <v>121</v>
       </c>
       <c r="E52" s="3">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="F52" s="3" t="s">
-        <v>33</v>
+        <v>8</v>
       </c>
       <c r="G52" s="4" t="s">
-        <v>34</v>
+        <v>56</v>
       </c>
       <c r="H52" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I52" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:9">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
         <v>108</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>194</v>
+        <v>168</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>193</v>
+        <v>166</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>121</v>
       </c>
       <c r="E53" s="3">
-        <v>0</v>
+        <v>202</v>
       </c>
       <c r="F53" s="3" t="s">
-        <v>189</v>
+        <v>33</v>
       </c>
       <c r="G53" s="4" t="s">
-        <v>76</v>
+        <v>34</v>
       </c>
       <c r="H53" s="3">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="I53" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:9">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
         <v>108</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>131</v>
+        <v>194</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="D54" s="3" t="s">
-        <v>130</v>
+        <v>193</v>
       </c>
       <c r="E54" s="3">
-        <v>210</v>
+        <v>0</v>
       </c>
       <c r="F54" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="G54" s="3" t="s">
-        <v>181</v>
+        <v>189</v>
+      </c>
+      <c r="G54" s="4" t="s">
+        <v>76</v>
       </c>
       <c r="H54" s="3">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I54" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:9">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
         <v>108</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D55" s="3" t="s">
         <v>130</v>
       </c>
       <c r="E55" s="3">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F55" s="3" t="s">
         <v>79</v>
       </c>
       <c r="G55" s="3" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="H55" s="3">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I55" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:9">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
         <v>108</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D56" s="3" t="s">
         <v>130</v>
       </c>
       <c r="E56" s="3">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F56" s="3" t="s">
         <v>79</v>
       </c>
       <c r="G56" s="3" t="s">
-        <v>137</v>
+        <v>179</v>
       </c>
       <c r="H56" s="3">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I56" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:9">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
         <v>108</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>192</v>
+        <v>133</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>195</v>
+        <v>136</v>
+      </c>
+      <c r="D57" s="3" t="s">
+        <v>130</v>
       </c>
       <c r="E57" s="3">
-        <v>0</v>
+        <v>212</v>
       </c>
       <c r="F57" s="3" t="s">
-        <v>189</v>
-      </c>
-      <c r="G57" s="4" t="s">
-        <v>76</v>
+        <v>79</v>
+      </c>
+      <c r="G57" s="3" t="s">
+        <v>137</v>
       </c>
       <c r="H57" s="3">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="I57" s="3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
         <v>108</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>128</v>
+        <v>192</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="D58" s="3" t="s">
-        <v>130</v>
+        <v>195</v>
       </c>
       <c r="E58" s="3">
-        <v>213</v>
+        <v>0</v>
       </c>
       <c r="F58" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="G58" s="3" t="s">
-        <v>180</v>
+        <v>189</v>
+      </c>
+      <c r="G58" s="4" t="s">
+        <v>76</v>
       </c>
       <c r="H58" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I58" s="3">
         <v>2</v>
       </c>
     </row>
-    <row r="59" spans="1:9">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
         <v>108</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>109</v>
+        <v>128</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>178</v>
+        <v>129</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="E59" s="3">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="F59" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G59" s="4" t="s">
-        <v>29</v>
+        <v>79</v>
+      </c>
+      <c r="G59" s="3" t="s">
+        <v>180</v>
       </c>
       <c r="H59" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I59" s="3">
         <v>2</v>
       </c>
     </row>
-    <row r="60" spans="1:9">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
         <v>108</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="D60" s="3" t="s">
         <v>110</v>
       </c>
       <c r="E60" s="3">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F60" s="3" t="s">
         <v>8</v>
       </c>
       <c r="G60" s="4" t="s">
-        <v>76</v>
+        <v>29</v>
       </c>
       <c r="H60" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I60" s="3">
         <v>2</v>
       </c>
     </row>
-    <row r="61" spans="1:9">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
         <v>108</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="D61" s="3" t="s">
         <v>110</v>
       </c>
       <c r="E61" s="3">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F61" s="3" t="s">
         <v>8</v>
@@ -3384,27 +3393,27 @@
         <v>76</v>
       </c>
       <c r="H61" s="3">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I61" s="3">
         <v>2</v>
       </c>
     </row>
-    <row r="62" spans="1:9">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
         <v>108</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="D62" s="3" t="s">
         <v>110</v>
       </c>
       <c r="E62" s="3">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F62" s="3" t="s">
         <v>8</v>
@@ -3413,27 +3422,27 @@
         <v>76</v>
       </c>
       <c r="H62" s="3">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I62" s="3">
         <v>2</v>
       </c>
     </row>
-    <row r="63" spans="1:9">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
         <v>108</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="D63" s="3" t="s">
         <v>110</v>
       </c>
       <c r="E63" s="3">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F63" s="3" t="s">
         <v>8</v>
@@ -3442,27 +3451,27 @@
         <v>76</v>
       </c>
       <c r="H63" s="3">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I63" s="3">
         <v>2</v>
       </c>
     </row>
-    <row r="64" spans="1:9">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
         <v>108</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D64" s="3" t="s">
         <v>110</v>
       </c>
       <c r="E64" s="3">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F64" s="3" t="s">
         <v>8</v>
@@ -3471,27 +3480,27 @@
         <v>76</v>
       </c>
       <c r="H64" s="3">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I64" s="3">
         <v>2</v>
       </c>
     </row>
-    <row r="65" spans="1:9">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
         <v>108</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="D65" s="3" t="s">
         <v>110</v>
       </c>
       <c r="E65" s="3">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F65" s="3" t="s">
         <v>8</v>
@@ -3500,27 +3509,27 @@
         <v>76</v>
       </c>
       <c r="H65" s="3">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I65" s="3">
         <v>2</v>
       </c>
     </row>
-    <row r="66" spans="1:9">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
         <v>108</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>117</v>
+        <v>183</v>
       </c>
       <c r="D66" s="3" t="s">
         <v>110</v>
       </c>
       <c r="E66" s="3">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F66" s="3" t="s">
         <v>8</v>
@@ -3529,169 +3538,169 @@
         <v>76</v>
       </c>
       <c r="H66" s="3">
+        <v>9</v>
+      </c>
+      <c r="I66" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A67" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="B67" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="C67" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="D67" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="E67" s="3">
+        <v>227</v>
+      </c>
+      <c r="F67" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G67" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="H67" s="3">
         <v>10</v>
       </c>
-      <c r="I66" s="3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="67" spans="1:9">
-      <c r="A67" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="B67" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="C67" s="3" t="s">
-        <v>209</v>
-      </c>
-      <c r="D67" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E67" s="3">
-        <v>120</v>
-      </c>
-      <c r="F67" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="G67" s="4" t="s">
-        <v>149</v>
-      </c>
-      <c r="H67" s="3">
-        <v>0</v>
-      </c>
       <c r="I67" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" spans="1:9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
         <v>59</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>60</v>
+        <v>73</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>61</v>
+        <v>209</v>
       </c>
       <c r="D68" s="3" t="s">
         <v>16</v>
       </c>
       <c r="E68" s="3">
-        <v>138</v>
+        <v>120</v>
       </c>
       <c r="F68" s="3" t="s">
-        <v>62</v>
+        <v>148</v>
       </c>
       <c r="G68" s="4" t="s">
-        <v>63</v>
+        <v>149</v>
       </c>
       <c r="H68" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I68" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:9">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
         <v>59</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>78</v>
+        <v>61</v>
       </c>
       <c r="D69" s="3" t="s">
         <v>16</v>
       </c>
       <c r="E69" s="3">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="F69" s="3" t="s">
-        <v>127</v>
+        <v>62</v>
       </c>
       <c r="G69" s="4" t="s">
-        <v>80</v>
+        <v>63</v>
       </c>
       <c r="H69" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I69" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:9">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
         <v>59</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>212</v>
+        <v>77</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>213</v>
+        <v>78</v>
+      </c>
+      <c r="D70" s="3" t="s">
+        <v>16</v>
       </c>
       <c r="E70" s="3">
-        <v>0</v>
+        <v>145</v>
       </c>
       <c r="F70" s="3" t="s">
-        <v>189</v>
+        <v>127</v>
       </c>
       <c r="G70" s="4" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="H70" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I70" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:9">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
         <v>59</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>64</v>
+        <v>212</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="D71" s="3" t="s">
-        <v>16</v>
+        <v>213</v>
       </c>
       <c r="E71" s="3">
-        <v>141</v>
+        <v>0</v>
       </c>
       <c r="F71" s="3" t="s">
-        <v>33</v>
+        <v>189</v>
       </c>
       <c r="G71" s="4" t="s">
-        <v>34</v>
+        <v>76</v>
       </c>
       <c r="H71" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I71" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:9">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
         <v>59</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>208</v>
+        <v>65</v>
       </c>
       <c r="D72" s="3" t="s">
         <v>16</v>
       </c>
       <c r="E72" s="3">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="F72" s="3" t="s">
         <v>33</v>
@@ -3700,27 +3709,27 @@
         <v>34</v>
       </c>
       <c r="H72" s="3">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I72" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:9">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
         <v>59</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>70</v>
+        <v>208</v>
       </c>
       <c r="D73" s="3" t="s">
         <v>16</v>
       </c>
       <c r="E73" s="3">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="F73" s="3" t="s">
         <v>33</v>
@@ -3729,27 +3738,27 @@
         <v>34</v>
       </c>
       <c r="H73" s="3">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I73" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:9">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
         <v>59</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="D74" s="3" t="s">
         <v>16</v>
       </c>
       <c r="E74" s="3">
-        <v>122</v>
+        <v>139</v>
       </c>
       <c r="F74" s="3" t="s">
         <v>33</v>
@@ -3758,27 +3767,27 @@
         <v>34</v>
       </c>
       <c r="H74" s="3">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I74" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:9">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
         <v>59</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="D75" s="3" t="s">
         <v>16</v>
       </c>
       <c r="E75" s="3">
-        <v>148</v>
+        <v>122</v>
       </c>
       <c r="F75" s="3" t="s">
         <v>33</v>
@@ -3787,253 +3796,282 @@
         <v>34</v>
       </c>
       <c r="H75" s="3">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I75" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:9">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
         <v>59</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>229</v>
+        <v>74</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>230</v>
+        <v>75</v>
       </c>
       <c r="D76" s="3" t="s">
         <v>16</v>
       </c>
       <c r="E76" s="3">
-        <v>133</v>
+        <v>149</v>
       </c>
       <c r="F76" s="3" t="s">
-        <v>231</v>
+        <v>33</v>
       </c>
       <c r="G76" s="4" t="s">
-        <v>147</v>
+        <v>34</v>
       </c>
       <c r="H76" s="3">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I76" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:9">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="s">
         <v>59</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>155</v>
+        <v>228</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>156</v>
+        <v>229</v>
       </c>
       <c r="D77" s="3" t="s">
         <v>16</v>
       </c>
       <c r="E77" s="3">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="F77" s="3" t="s">
-        <v>157</v>
+        <v>230</v>
       </c>
       <c r="G77" s="4" t="s">
         <v>147</v>
       </c>
       <c r="H77" s="3">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I77" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:9">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="s">
         <v>59</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>187</v>
+        <v>155</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>188</v>
+        <v>156</v>
       </c>
       <c r="D78" s="3" t="s">
         <v>16</v>
       </c>
       <c r="E78" s="3">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="F78" s="3" t="s">
-        <v>8</v>
+        <v>157</v>
       </c>
       <c r="G78" s="4" t="s">
-        <v>76</v>
+        <v>147</v>
       </c>
       <c r="H78" s="3">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I78" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:9">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="s">
         <v>59</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>210</v>
+        <v>187</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>211</v>
+        <v>188</v>
+      </c>
+      <c r="D79" s="3" t="s">
+        <v>16</v>
       </c>
       <c r="E79" s="3">
-        <v>0</v>
+        <v>142</v>
       </c>
       <c r="F79" s="3" t="s">
-        <v>189</v>
+        <v>8</v>
       </c>
       <c r="G79" s="4" t="s">
         <v>76</v>
       </c>
       <c r="H79" s="3">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="I79" s="3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="80" spans="1:9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="s">
         <v>59</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>140</v>
+        <v>210</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="D80" s="3" t="s">
-        <v>16</v>
+        <v>211</v>
       </c>
       <c r="E80" s="3">
-        <v>112</v>
+        <v>0</v>
       </c>
       <c r="F80" s="3" t="s">
-        <v>143</v>
+        <v>189</v>
       </c>
       <c r="G80" s="4" t="s">
-        <v>142</v>
+        <v>76</v>
       </c>
       <c r="H80" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I80" s="3">
         <v>2</v>
       </c>
     </row>
-    <row r="81" spans="1:9">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" s="3" t="s">
         <v>59</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="D81" s="3" t="s">
         <v>16</v>
       </c>
       <c r="E81" s="3">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="F81" s="3" t="s">
-        <v>8</v>
+        <v>143</v>
       </c>
       <c r="G81" s="4" t="s">
-        <v>76</v>
+        <v>142</v>
       </c>
       <c r="H81" s="3">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I81" s="3">
         <v>2</v>
       </c>
     </row>
-    <row r="82" spans="1:9">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" s="3" t="s">
         <v>59</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>169</v>
+        <v>138</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>170</v>
+        <v>139</v>
       </c>
       <c r="D82" s="3" t="s">
         <v>16</v>
       </c>
       <c r="E82" s="3">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F82" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="G82" s="3" t="s">
-        <v>147</v>
+        <v>8</v>
+      </c>
+      <c r="G82" s="4" t="s">
+        <v>76</v>
       </c>
       <c r="H82" s="3">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I82" s="3">
         <v>2</v>
       </c>
     </row>
-    <row r="83" spans="1:9">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" s="3" t="s">
         <v>59</v>
       </c>
       <c r="B83" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="C83" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="D83" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E83" s="3">
+        <v>111</v>
+      </c>
+      <c r="F83" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="G83" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="H83" s="3">
+        <v>6</v>
+      </c>
+      <c r="I83" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A84" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B84" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="C84" s="3" t="s">
         <v>232</v>
       </c>
-      <c r="C83" s="3" t="s">
+      <c r="D84" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E84" s="3">
+        <v>112</v>
+      </c>
+      <c r="F84" s="3" t="s">
         <v>233</v>
       </c>
-      <c r="D83" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E83" s="3">
-        <v>112</v>
-      </c>
-      <c r="F83" s="3" t="s">
+      <c r="G84" s="3" t="s">
         <v>234</v>
       </c>
-      <c r="G83" s="3" t="s">
-        <v>235</v>
-      </c>
-      <c r="H83" s="3">
+      <c r="H84" s="3">
         <v>7</v>
       </c>
-      <c r="I83" s="3">
+      <c r="I84" s="3">
         <v>2</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I83" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I82">
-      <sortCondition ref="A2:A82"/>
-      <sortCondition ref="I2:I82"/>
-      <sortCondition ref="H2:H82"/>
+  <autoFilter ref="A1:I84" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I84">
+      <sortCondition ref="A2:A84"/>
+      <sortCondition ref="I2:I84"/>
+      <sortCondition ref="H2:H84"/>
     </sortState>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:I83">
-    <sortCondition ref="A3:A83"/>
-    <sortCondition ref="I3:I83"/>
-    <sortCondition ref="H3:H83"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:I84">
+    <sortCondition ref="A3:A84"/>
+    <sortCondition ref="I3:I84"/>
+    <sortCondition ref="H3:H84"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Removed default for help_file.
</commit_message>
<xml_diff>
--- a/src/game_params.xlsx
+++ b/src/game_params.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Activity_Data\Mancala_github\MancalaGames\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE20A46C-BACF-4957-BC8F-DFD822755C8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52D085DA-8721-499C-9643-4B0A8975476B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="243">
   <si>
     <t>tab</t>
   </si>
@@ -93,9 +93,6 @@
   </si>
   <si>
     <t>Help File</t>
-  </si>
-  <si>
-    <t>mancala_help.html</t>
   </si>
   <si>
     <t>about</t>
@@ -1647,8 +1644,8 @@
   <dimension ref="A1:I84"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C26" sqref="C26"/>
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G47" sqref="G47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1679,7 +1676,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>4</v>
@@ -1696,23 +1693,23 @@
     </row>
     <row r="2" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>196</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>197</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3">
         <v>0</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H2" s="3">
         <v>0</v>
@@ -1723,13 +1720,13 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>86</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>87</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>16</v>
@@ -1738,10 +1735,10 @@
         <v>114</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H3" s="3">
         <v>1</v>
@@ -1752,13 +1749,13 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>88</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>89</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>16</v>
@@ -1770,7 +1767,7 @@
         <v>8</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H4" s="3">
         <v>2</v>
@@ -1781,13 +1778,13 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>90</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>91</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>16</v>
@@ -1799,7 +1796,7 @@
         <v>8</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H5" s="3">
         <v>3</v>
@@ -1810,13 +1807,13 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>106</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>107</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>16</v>
@@ -1825,10 +1822,10 @@
         <v>107</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H6" s="3">
         <v>4</v>
@@ -1839,22 +1836,22 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>202</v>
-      </c>
       <c r="E7" s="3">
         <v>0</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H7" s="3">
         <v>5</v>
@@ -1865,13 +1862,13 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B8" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>94</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>95</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>16</v>
@@ -1880,10 +1877,10 @@
         <v>113</v>
       </c>
       <c r="F8" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G8" s="4" t="s">
         <v>33</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>34</v>
       </c>
       <c r="H8" s="3">
         <v>6</v>
@@ -1894,13 +1891,13 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B9" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>96</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>97</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>16</v>
@@ -1909,10 +1906,10 @@
         <v>151</v>
       </c>
       <c r="F9" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="G9" s="4" t="s">
         <v>98</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>99</v>
       </c>
       <c r="H9" s="3">
         <v>7</v>
@@ -1923,13 +1920,13 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B10" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>161</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>162</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>16</v>
@@ -1938,10 +1935,10 @@
         <v>150</v>
       </c>
       <c r="F10" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G10" s="4" t="s">
         <v>33</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>34</v>
       </c>
       <c r="H10" s="3">
         <v>8</v>
@@ -1952,22 +1949,22 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B11" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>198</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="E11" s="3">
+        <v>0</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="G11" s="4" t="s">
         <v>199</v>
-      </c>
-      <c r="E11" s="3">
-        <v>0</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>189</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>200</v>
       </c>
       <c r="H11" s="3">
         <v>9</v>
@@ -1978,13 +1975,13 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B12" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>235</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>236</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>16</v>
@@ -1993,10 +1990,10 @@
         <v>106</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H12" s="3">
         <v>10</v>
@@ -2007,22 +2004,22 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E13" s="3">
         <v>0</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H13" s="3">
         <v>0</v>
@@ -2033,13 +2030,13 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B14" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>100</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>101</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>16</v>
@@ -2051,7 +2048,7 @@
         <v>8</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H14" s="3">
         <v>1</v>
@@ -2062,13 +2059,13 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="C15" s="3" t="s">
         <v>82</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>83</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>16</v>
@@ -2077,10 +2074,10 @@
         <v>103</v>
       </c>
       <c r="F15" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G15" s="4" t="s">
         <v>33</v>
-      </c>
-      <c r="G15" s="4" t="s">
-        <v>34</v>
       </c>
       <c r="H15" s="3">
         <v>2</v>
@@ -2091,22 +2088,22 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E16" s="3">
         <v>0</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H16" s="3">
         <v>3</v>
@@ -2117,13 +2114,13 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>16</v>
@@ -2135,7 +2132,7 @@
         <v>8</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H17" s="3">
         <v>4</v>
@@ -2146,13 +2143,13 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B18" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="C18" s="3" t="s">
         <v>224</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>225</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>16</v>
@@ -2161,10 +2158,10 @@
         <v>130</v>
       </c>
       <c r="F18" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="G18" s="4" t="s">
         <v>226</v>
-      </c>
-      <c r="G18" s="4" t="s">
-        <v>227</v>
       </c>
       <c r="H18" s="3">
         <v>5</v>
@@ -2175,13 +2172,13 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B19" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="C19" s="3" t="s">
         <v>92</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>93</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>16</v>
@@ -2190,10 +2187,10 @@
         <v>129</v>
       </c>
       <c r="F19" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G19" s="4" t="s">
         <v>33</v>
-      </c>
-      <c r="G19" s="4" t="s">
-        <v>34</v>
       </c>
       <c r="H19" s="3">
         <v>6</v>
@@ -2204,13 +2201,13 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B20" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C20" s="3" t="s">
         <v>84</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>85</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>16</v>
@@ -2219,10 +2216,10 @@
         <v>123</v>
       </c>
       <c r="F20" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G20" s="4" t="s">
         <v>33</v>
-      </c>
-      <c r="G20" s="4" t="s">
-        <v>34</v>
       </c>
       <c r="H20" s="3">
         <v>7</v>
@@ -2233,22 +2230,22 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B21" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="C21" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="C21" s="3" t="s">
-        <v>206</v>
-      </c>
       <c r="E21" s="3">
         <v>0</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H21" s="3">
         <v>8</v>
@@ -2259,13 +2256,13 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B22" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="C22" s="3" t="s">
         <v>150</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>151</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>16</v>
@@ -2274,10 +2271,10 @@
         <v>108</v>
       </c>
       <c r="F22" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="G22" s="4" t="s">
         <v>238</v>
-      </c>
-      <c r="G22" s="4" t="s">
-        <v>239</v>
       </c>
       <c r="H22" s="3">
         <v>9</v>
@@ -2288,13 +2285,13 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>16</v>
@@ -2303,10 +2300,10 @@
         <v>131</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H23" s="3">
         <v>10</v>
@@ -2317,13 +2314,13 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B24" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C24" s="3" t="s">
         <v>46</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>47</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>16</v>
@@ -2332,10 +2329,10 @@
         <v>115</v>
       </c>
       <c r="F24" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="G24" s="4" t="s">
         <v>48</v>
-      </c>
-      <c r="G24" s="4" t="s">
-        <v>49</v>
       </c>
       <c r="H24" s="3">
         <v>0</v>
@@ -2346,13 +2343,13 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B25" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="C25" s="3" t="s">
         <v>184</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>185</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>16</v>
@@ -2364,7 +2361,7 @@
         <v>8</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H25" s="3">
         <v>1</v>
@@ -2375,13 +2372,13 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>16</v>
@@ -2390,10 +2387,10 @@
         <v>147</v>
       </c>
       <c r="F26" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="G26" s="4" t="s">
         <v>222</v>
-      </c>
-      <c r="G26" s="4" t="s">
-        <v>223</v>
       </c>
       <c r="H26" s="3">
         <v>2</v>
@@ -2404,13 +2401,13 @@
     </row>
     <row r="27" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B27" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C27" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D27" t="s">
         <v>16</v>
@@ -2419,10 +2416,10 @@
         <v>148</v>
       </c>
       <c r="F27" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G27" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="H27">
         <v>3</v>
@@ -2433,22 +2430,22 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E28" s="3">
         <v>0</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H28" s="3">
         <v>4</v>
@@ -2459,13 +2456,13 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B29" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C29" s="3" t="s">
         <v>50</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>51</v>
       </c>
       <c r="D29" s="3" t="s">
         <v>16</v>
@@ -2474,10 +2471,10 @@
         <v>143</v>
       </c>
       <c r="F29" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="G29" s="4" t="s">
         <v>52</v>
-      </c>
-      <c r="G29" s="4" t="s">
-        <v>53</v>
       </c>
       <c r="H29" s="3">
         <v>5</v>
@@ -2488,13 +2485,13 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D30" s="3" t="s">
         <v>16</v>
@@ -2503,10 +2500,10 @@
         <v>132</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G30" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H30" s="3">
         <v>6</v>
@@ -2517,22 +2514,22 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B31" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="C31" s="3" t="s">
         <v>217</v>
       </c>
-      <c r="C31" s="3" t="s">
-        <v>218</v>
-      </c>
       <c r="E31" s="3">
         <v>0</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H31" s="3">
         <v>7</v>
@@ -2543,13 +2540,13 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B32" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C32" s="3" t="s">
         <v>54</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>55</v>
       </c>
       <c r="D32" s="3" t="s">
         <v>16</v>
@@ -2561,7 +2558,7 @@
         <v>8</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H32" s="3">
         <v>8</v>
@@ -2572,13 +2569,13 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B33" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="C33" s="3" t="s">
         <v>144</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>145</v>
       </c>
       <c r="D33" s="3" t="s">
         <v>16</v>
@@ -2587,10 +2584,10 @@
         <v>101</v>
       </c>
       <c r="F33" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="G33" s="4" t="s">
         <v>146</v>
-      </c>
-      <c r="G33" s="4" t="s">
-        <v>147</v>
       </c>
       <c r="H33" s="3">
         <v>9</v>
@@ -2601,13 +2598,13 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B34" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C34" s="3" t="s">
         <v>43</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>44</v>
       </c>
       <c r="D34" s="3" t="s">
         <v>16</v>
@@ -2616,10 +2613,10 @@
         <v>144</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G34" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H34" s="3">
         <v>0</v>
@@ -2630,13 +2627,13 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B35" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C35" s="3" t="s">
         <v>41</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>42</v>
       </c>
       <c r="D35" s="3" t="s">
         <v>16</v>
@@ -2645,10 +2642,10 @@
         <v>127</v>
       </c>
       <c r="F35" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G35" s="4" t="s">
         <v>33</v>
-      </c>
-      <c r="G35" s="4" t="s">
-        <v>34</v>
       </c>
       <c r="H35" s="3">
         <v>1</v>
@@ -2659,22 +2656,22 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E36" s="3">
         <v>0</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G36" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H36" s="3">
         <v>2</v>
@@ -2685,13 +2682,13 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B37" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B37" s="3" t="s">
+      <c r="C37" s="3" t="s">
         <v>31</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>32</v>
       </c>
       <c r="D37" s="3" t="s">
         <v>16</v>
@@ -2700,10 +2697,10 @@
         <v>125</v>
       </c>
       <c r="F37" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G37" s="4" t="s">
         <v>33</v>
-      </c>
-      <c r="G37" s="4" t="s">
-        <v>34</v>
       </c>
       <c r="H37" s="3">
         <v>3</v>
@@ -2714,13 +2711,13 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B38" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C38" s="3" t="s">
         <v>57</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>58</v>
       </c>
       <c r="D38" s="3" t="s">
         <v>16</v>
@@ -2729,10 +2726,10 @@
         <v>126</v>
       </c>
       <c r="F38" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G38" s="4" t="s">
         <v>33</v>
-      </c>
-      <c r="G38" s="4" t="s">
-        <v>34</v>
       </c>
       <c r="H38" s="3">
         <v>4</v>
@@ -2743,13 +2740,13 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B39" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="C39" s="3" t="s">
         <v>102</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>103</v>
       </c>
       <c r="D39" s="3" t="s">
         <v>16</v>
@@ -2758,10 +2755,10 @@
         <v>117</v>
       </c>
       <c r="F39" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="G39" s="4" t="s">
         <v>104</v>
-      </c>
-      <c r="G39" s="4" t="s">
-        <v>105</v>
       </c>
       <c r="H39" s="3">
         <v>5</v>
@@ -2772,22 +2769,22 @@
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E40" s="3">
         <v>0</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G40" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H40" s="3">
         <v>6</v>
@@ -2798,13 +2795,13 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B41" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C41" s="3" t="s">
         <v>35</v>
-      </c>
-      <c r="C41" s="3" t="s">
-        <v>36</v>
       </c>
       <c r="D41" s="3" t="s">
         <v>16</v>
@@ -2813,10 +2810,10 @@
         <v>136</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G41" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="H41" s="3">
         <v>7</v>
@@ -2827,13 +2824,13 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B42" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C42" s="3" t="s">
         <v>37</v>
-      </c>
-      <c r="C42" s="3" t="s">
-        <v>38</v>
       </c>
       <c r="D42" s="3" t="s">
         <v>16</v>
@@ -2842,10 +2839,10 @@
         <v>135</v>
       </c>
       <c r="F42" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G42" s="4" t="s">
         <v>39</v>
-      </c>
-      <c r="G42" s="4" t="s">
-        <v>40</v>
       </c>
       <c r="H42" s="3">
         <v>8</v>
@@ -2856,13 +2853,13 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B43" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="C43" s="3" t="s">
         <v>163</v>
-      </c>
-      <c r="C43" s="3" t="s">
-        <v>164</v>
       </c>
       <c r="D43" s="3" t="s">
         <v>16</v>
@@ -2871,10 +2868,10 @@
         <v>134</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G43" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="H43" s="3">
         <v>9</v>
@@ -2885,13 +2882,13 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B44" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C44" s="3" t="s">
         <v>71</v>
-      </c>
-      <c r="C44" s="3" t="s">
-        <v>72</v>
       </c>
       <c r="D44" s="3" t="s">
         <v>16</v>
@@ -2900,10 +2897,10 @@
         <v>102</v>
       </c>
       <c r="F44" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G44" s="4" t="s">
         <v>33</v>
-      </c>
-      <c r="G44" s="4" t="s">
-        <v>34</v>
       </c>
       <c r="H44" s="3">
         <v>10</v>
@@ -2929,7 +2926,7 @@
         <v>1</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G45" s="4" t="s">
         <v>13</v>
@@ -2946,13 +2943,13 @@
         <v>9</v>
       </c>
       <c r="B46" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C46" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C46" s="3" t="s">
+      <c r="D46" s="3" t="s">
         <v>24</v>
-      </c>
-      <c r="D46" s="3" t="s">
-        <v>25</v>
       </c>
       <c r="E46" s="3">
         <v>2</v>
@@ -2961,7 +2958,7 @@
         <v>8</v>
       </c>
       <c r="G46" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H46" s="3">
         <v>2</v>
@@ -2989,9 +2986,7 @@
       <c r="F47" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G47" s="4" t="s">
-        <v>19</v>
-      </c>
+      <c r="G47" s="4"/>
       <c r="H47" s="3">
         <v>3</v>
       </c>
@@ -3004,10 +2999,10 @@
         <v>9</v>
       </c>
       <c r="B48" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C48" s="3" t="s">
         <v>20</v>
-      </c>
-      <c r="C48" s="3" t="s">
-        <v>21</v>
       </c>
       <c r="D48" s="3" t="s">
         <v>16</v>
@@ -3016,10 +3011,10 @@
         <v>5</v>
       </c>
       <c r="F48" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G48" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H48" s="3">
         <v>4</v>
@@ -3062,13 +3057,13 @@
         <v>9</v>
       </c>
       <c r="B50" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C50" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C50" s="3" t="s">
-        <v>28</v>
-      </c>
       <c r="D50" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E50" s="3">
         <v>3</v>
@@ -3077,7 +3072,7 @@
         <v>8</v>
       </c>
       <c r="G50" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H50" s="3">
         <v>2</v>
@@ -3088,25 +3083,25 @@
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B51" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="C51" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="C51" s="3" t="s">
-        <v>125</v>
-      </c>
       <c r="D51" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E51" s="3">
         <v>201</v>
       </c>
       <c r="F51" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="G51" s="3" t="s">
         <v>125</v>
-      </c>
-      <c r="G51" s="3" t="s">
-        <v>126</v>
       </c>
       <c r="H51" s="3">
         <v>0</v>
@@ -3117,16 +3112,16 @@
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B52" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C52" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="C52" s="3" t="s">
+      <c r="D52" s="3" t="s">
         <v>120</v>
-      </c>
-      <c r="D52" s="3" t="s">
-        <v>121</v>
       </c>
       <c r="E52" s="3">
         <v>203</v>
@@ -3135,7 +3130,7 @@
         <v>8</v>
       </c>
       <c r="G52" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H52" s="3">
         <v>1</v>
@@ -3146,25 +3141,25 @@
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E53" s="3">
         <v>202</v>
       </c>
       <c r="F53" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G53" s="4" t="s">
         <v>33</v>
-      </c>
-      <c r="G53" s="4" t="s">
-        <v>34</v>
       </c>
       <c r="H53" s="3">
         <v>2</v>
@@ -3175,22 +3170,22 @@
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E54" s="3">
         <v>0</v>
       </c>
       <c r="F54" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G54" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H54" s="3">
         <v>5</v>
@@ -3201,25 +3196,25 @@
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E55" s="3">
         <v>210</v>
       </c>
       <c r="F55" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G55" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H55" s="3">
         <v>6</v>
@@ -3230,25 +3225,25 @@
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E56" s="3">
         <v>211</v>
       </c>
       <c r="F56" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G56" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="H56" s="3">
         <v>7</v>
@@ -3259,25 +3254,25 @@
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E57" s="3">
         <v>212</v>
       </c>
       <c r="F57" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G57" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H57" s="3">
         <v>8</v>
@@ -3288,22 +3283,22 @@
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E58" s="3">
         <v>0</v>
       </c>
       <c r="F58" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G58" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H58" s="3">
         <v>1</v>
@@ -3314,25 +3309,25 @@
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B59" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="C59" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="C59" s="3" t="s">
+      <c r="D59" s="3" t="s">
         <v>129</v>
-      </c>
-      <c r="D59" s="3" t="s">
-        <v>130</v>
       </c>
       <c r="E59" s="3">
         <v>213</v>
       </c>
       <c r="F59" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G59" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H59" s="3">
         <v>2</v>
@@ -3343,16 +3338,16 @@
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="B60" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="B60" s="3" t="s">
+      <c r="C60" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="D60" s="3" t="s">
         <v>109</v>
-      </c>
-      <c r="C60" s="3" t="s">
-        <v>178</v>
-      </c>
-      <c r="D60" s="3" t="s">
-        <v>110</v>
       </c>
       <c r="E60" s="3">
         <v>220</v>
@@ -3361,7 +3356,7 @@
         <v>8</v>
       </c>
       <c r="G60" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H60" s="3">
         <v>3</v>
@@ -3372,16 +3367,16 @@
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E61" s="3">
         <v>221</v>
@@ -3390,7 +3385,7 @@
         <v>8</v>
       </c>
       <c r="G61" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H61" s="3">
         <v>4</v>
@@ -3401,16 +3396,16 @@
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E62" s="3">
         <v>222</v>
@@ -3419,7 +3414,7 @@
         <v>8</v>
       </c>
       <c r="G62" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H62" s="3">
         <v>5</v>
@@ -3430,16 +3425,16 @@
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E63" s="3">
         <v>223</v>
@@ -3448,7 +3443,7 @@
         <v>8</v>
       </c>
       <c r="G63" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H63" s="3">
         <v>6</v>
@@ -3459,16 +3454,16 @@
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E64" s="3">
         <v>224</v>
@@ -3477,7 +3472,7 @@
         <v>8</v>
       </c>
       <c r="G64" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H64" s="3">
         <v>7</v>
@@ -3488,16 +3483,16 @@
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E65" s="3">
         <v>225</v>
@@ -3506,7 +3501,7 @@
         <v>8</v>
       </c>
       <c r="G65" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H65" s="3">
         <v>8</v>
@@ -3517,16 +3512,16 @@
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E66" s="3">
         <v>226</v>
@@ -3535,7 +3530,7 @@
         <v>8</v>
       </c>
       <c r="G66" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H66" s="3">
         <v>9</v>
@@ -3546,16 +3541,16 @@
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B67" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C67" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="C67" s="3" t="s">
-        <v>117</v>
-      </c>
       <c r="D67" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E67" s="3">
         <v>227</v>
@@ -3564,7 +3559,7 @@
         <v>8</v>
       </c>
       <c r="G67" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H67" s="3">
         <v>10</v>
@@ -3575,13 +3570,13 @@
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D68" s="3" t="s">
         <v>16</v>
@@ -3590,10 +3585,10 @@
         <v>120</v>
       </c>
       <c r="F68" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="G68" s="4" t="s">
         <v>148</v>
-      </c>
-      <c r="G68" s="4" t="s">
-        <v>149</v>
       </c>
       <c r="H68" s="3">
         <v>0</v>
@@ -3604,13 +3599,13 @@
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B69" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B69" s="3" t="s">
+      <c r="C69" s="3" t="s">
         <v>60</v>
-      </c>
-      <c r="C69" s="3" t="s">
-        <v>61</v>
       </c>
       <c r="D69" s="3" t="s">
         <v>16</v>
@@ -3619,10 +3614,10 @@
         <v>138</v>
       </c>
       <c r="F69" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="G69" s="4" t="s">
         <v>62</v>
-      </c>
-      <c r="G69" s="4" t="s">
-        <v>63</v>
       </c>
       <c r="H69" s="3">
         <v>1</v>
@@ -3633,13 +3628,13 @@
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B70" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C70" s="3" t="s">
         <v>77</v>
-      </c>
-      <c r="C70" s="3" t="s">
-        <v>78</v>
       </c>
       <c r="D70" s="3" t="s">
         <v>16</v>
@@ -3648,10 +3643,10 @@
         <v>145</v>
       </c>
       <c r="F70" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G70" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H70" s="3">
         <v>2</v>
@@ -3662,22 +3657,22 @@
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B71" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="C71" s="3" t="s">
         <v>212</v>
       </c>
-      <c r="C71" s="3" t="s">
-        <v>213</v>
-      </c>
       <c r="E71" s="3">
         <v>0</v>
       </c>
       <c r="F71" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G71" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H71" s="3">
         <v>3</v>
@@ -3688,13 +3683,13 @@
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B72" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C72" s="3" t="s">
         <v>64</v>
-      </c>
-      <c r="C72" s="3" t="s">
-        <v>65</v>
       </c>
       <c r="D72" s="3" t="s">
         <v>16</v>
@@ -3703,10 +3698,10 @@
         <v>141</v>
       </c>
       <c r="F72" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G72" s="4" t="s">
         <v>33</v>
-      </c>
-      <c r="G72" s="4" t="s">
-        <v>34</v>
       </c>
       <c r="H72" s="3">
         <v>4</v>
@@ -3717,13 +3712,13 @@
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D73" s="3" t="s">
         <v>16</v>
@@ -3732,10 +3727,10 @@
         <v>137</v>
       </c>
       <c r="F73" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G73" s="4" t="s">
         <v>33</v>
-      </c>
-      <c r="G73" s="4" t="s">
-        <v>34</v>
       </c>
       <c r="H73" s="3">
         <v>5</v>
@@ -3746,13 +3741,13 @@
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B74" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C74" s="3" t="s">
         <v>69</v>
-      </c>
-      <c r="C74" s="3" t="s">
-        <v>70</v>
       </c>
       <c r="D74" s="3" t="s">
         <v>16</v>
@@ -3761,10 +3756,10 @@
         <v>139</v>
       </c>
       <c r="F74" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G74" s="4" t="s">
         <v>33</v>
-      </c>
-      <c r="G74" s="4" t="s">
-        <v>34</v>
       </c>
       <c r="H74" s="3">
         <v>6</v>
@@ -3775,13 +3770,13 @@
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B75" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C75" s="3" t="s">
         <v>66</v>
-      </c>
-      <c r="C75" s="3" t="s">
-        <v>67</v>
       </c>
       <c r="D75" s="3" t="s">
         <v>16</v>
@@ -3790,10 +3785,10 @@
         <v>122</v>
       </c>
       <c r="F75" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G75" s="4" t="s">
         <v>33</v>
-      </c>
-      <c r="G75" s="4" t="s">
-        <v>34</v>
       </c>
       <c r="H75" s="3">
         <v>7</v>
@@ -3804,13 +3799,13 @@
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B76" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C76" s="3" t="s">
         <v>74</v>
-      </c>
-      <c r="C76" s="3" t="s">
-        <v>75</v>
       </c>
       <c r="D76" s="3" t="s">
         <v>16</v>
@@ -3819,10 +3814,10 @@
         <v>149</v>
       </c>
       <c r="F76" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G76" s="4" t="s">
         <v>33</v>
-      </c>
-      <c r="G76" s="4" t="s">
-        <v>34</v>
       </c>
       <c r="H76" s="3">
         <v>8</v>
@@ -3833,13 +3828,13 @@
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B77" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="C77" s="3" t="s">
         <v>228</v>
-      </c>
-      <c r="C77" s="3" t="s">
-        <v>229</v>
       </c>
       <c r="D77" s="3" t="s">
         <v>16</v>
@@ -3848,10 +3843,10 @@
         <v>133</v>
       </c>
       <c r="F77" s="3" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="G77" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H77" s="3">
         <v>9</v>
@@ -3862,13 +3857,13 @@
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B78" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="C78" s="3" t="s">
         <v>155</v>
-      </c>
-      <c r="C78" s="3" t="s">
-        <v>156</v>
       </c>
       <c r="D78" s="3" t="s">
         <v>16</v>
@@ -3877,10 +3872,10 @@
         <v>140</v>
       </c>
       <c r="F78" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G78" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H78" s="3">
         <v>10</v>
@@ -3891,13 +3886,13 @@
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B79" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="C79" s="3" t="s">
         <v>187</v>
-      </c>
-      <c r="C79" s="3" t="s">
-        <v>188</v>
       </c>
       <c r="D79" s="3" t="s">
         <v>16</v>
@@ -3909,7 +3904,7 @@
         <v>8</v>
       </c>
       <c r="G79" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H79" s="3">
         <v>11</v>
@@ -3920,22 +3915,22 @@
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B80" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="C80" s="3" t="s">
         <v>210</v>
       </c>
-      <c r="C80" s="3" t="s">
-        <v>211</v>
-      </c>
       <c r="E80" s="3">
         <v>0</v>
       </c>
       <c r="F80" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G80" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H80" s="3">
         <v>3</v>
@@ -3946,13 +3941,13 @@
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B81" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="C81" s="3" t="s">
         <v>140</v>
-      </c>
-      <c r="C81" s="3" t="s">
-        <v>141</v>
       </c>
       <c r="D81" s="3" t="s">
         <v>16</v>
@@ -3961,10 +3956,10 @@
         <v>112</v>
       </c>
       <c r="F81" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G81" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H81" s="3">
         <v>4</v>
@@ -3975,13 +3970,13 @@
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B82" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="C82" s="3" t="s">
         <v>138</v>
-      </c>
-      <c r="C82" s="3" t="s">
-        <v>139</v>
       </c>
       <c r="D82" s="3" t="s">
         <v>16</v>
@@ -3993,7 +3988,7 @@
         <v>8</v>
       </c>
       <c r="G82" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H82" s="3">
         <v>5</v>
@@ -4004,13 +3999,13 @@
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B83" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="C83" s="3" t="s">
         <v>169</v>
-      </c>
-      <c r="C83" s="3" t="s">
-        <v>170</v>
       </c>
       <c r="D83" s="3" t="s">
         <v>16</v>
@@ -4019,10 +4014,10 @@
         <v>111</v>
       </c>
       <c r="F83" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G83" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H83" s="3">
         <v>6</v>
@@ -4033,13 +4028,13 @@
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B84" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="C84" s="3" t="s">
         <v>231</v>
-      </c>
-      <c r="C84" s="3" t="s">
-        <v>232</v>
       </c>
       <c r="D84" s="3" t="s">
         <v>16</v>
@@ -4048,10 +4043,10 @@
         <v>112</v>
       </c>
       <c r="F84" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="G84" s="3" t="s">
         <v>233</v>
-      </c>
-      <c r="G84" s="3" t="s">
-        <v>234</v>
       </c>
       <c r="H84" s="3">
         <v>7</v>

</xml_diff>

<commit_message>
Changed capsamedir to capt_dir, made it an enumeration, and added CaptDir.BOTH. Updated required game files for the new name and value.
</commit_message>
<xml_diff>
--- a/src/game_params.xlsx
+++ b/src/game_params.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Activity_Data\Mancala_github\MancalaGames\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52D085DA-8721-499C-9643-4B0A8975476B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C05CD46-FCDE-4AF3-BDFB-094E1C198118}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32820" yWindow="2535" windowWidth="19605" windowHeight="12060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="game_params" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="245">
   <si>
     <t>tab</t>
   </si>
@@ -279,12 +279,6 @@
   </si>
   <si>
     <t>Capture</t>
-  </si>
-  <si>
-    <t>capsamedir</t>
-  </si>
-  <si>
-    <t>Capture in Sow Direction</t>
   </si>
   <si>
     <t>moveunlock</t>
@@ -766,6 +760,18 @@
   </si>
   <si>
     <t>Unclaimed Seeds at End</t>
+  </si>
+  <si>
+    <t>capt_dir</t>
+  </si>
+  <si>
+    <t>CaptDir</t>
+  </si>
+  <si>
+    <t>OPP_SOW</t>
+  </si>
+  <si>
+    <t>Capture Direction</t>
   </si>
 </sst>
 </file>
@@ -1644,8 +1650,8 @@
   <dimension ref="A1:I84"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G47" sqref="G47"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1676,7 +1682,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>4</v>
@@ -1696,17 +1702,17 @@
         <v>80</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3">
         <v>0</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>75</v>
@@ -1723,10 +1729,10 @@
         <v>80</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>16</v>
@@ -1752,10 +1758,10 @@
         <v>80</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>16</v>
@@ -1781,10 +1787,10 @@
         <v>80</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>16</v>
@@ -1810,10 +1816,10 @@
         <v>80</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>16</v>
@@ -1822,7 +1828,7 @@
         <v>107</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>79</v>
@@ -1839,16 +1845,16 @@
         <v>80</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E7" s="3">
         <v>0</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>75</v>
@@ -1865,10 +1871,10 @@
         <v>80</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>16</v>
@@ -1894,10 +1900,10 @@
         <v>80</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>16</v>
@@ -1906,10 +1912,10 @@
         <v>151</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H9" s="3">
         <v>7</v>
@@ -1923,10 +1929,10 @@
         <v>80</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>16</v>
@@ -1952,19 +1958,19 @@
         <v>80</v>
       </c>
       <c r="B11" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="E11" s="3">
+        <v>0</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="G11" s="4" t="s">
         <v>197</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>198</v>
-      </c>
-      <c r="E11" s="3">
-        <v>0</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>199</v>
       </c>
       <c r="H11" s="3">
         <v>9</v>
@@ -1978,10 +1984,10 @@
         <v>80</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>16</v>
@@ -1990,10 +1996,10 @@
         <v>106</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="H12" s="3">
         <v>10</v>
@@ -2007,16 +2013,16 @@
         <v>80</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E13" s="3">
         <v>0</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G13" s="4" t="s">
         <v>75</v>
@@ -2033,10 +2039,10 @@
         <v>80</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>16</v>
@@ -2062,10 +2068,10 @@
         <v>80</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>81</v>
+        <v>241</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>82</v>
+        <v>244</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>16</v>
@@ -2074,10 +2080,10 @@
         <v>103</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>32</v>
+        <v>242</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>33</v>
+        <v>243</v>
       </c>
       <c r="H15" s="3">
         <v>2</v>
@@ -2091,16 +2097,16 @@
         <v>80</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="E16" s="3">
         <v>0</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G16" s="4" t="s">
         <v>75</v>
@@ -2117,10 +2123,10 @@
         <v>80</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>16</v>
@@ -2146,10 +2152,10 @@
         <v>80</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>16</v>
@@ -2158,10 +2164,10 @@
         <v>130</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="H18" s="3">
         <v>5</v>
@@ -2175,10 +2181,10 @@
         <v>80</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>16</v>
@@ -2204,10 +2210,10 @@
         <v>80</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>16</v>
@@ -2233,16 +2239,16 @@
         <v>80</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="E21" s="3">
         <v>0</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G21" s="4" t="s">
         <v>75</v>
@@ -2259,10 +2265,10 @@
         <v>80</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>16</v>
@@ -2271,10 +2277,10 @@
         <v>108</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="H22" s="3">
         <v>9</v>
@@ -2288,10 +2294,10 @@
         <v>80</v>
       </c>
       <c r="B23" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="C23" s="3" t="s">
         <v>157</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>159</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>16</v>
@@ -2300,10 +2306,10 @@
         <v>131</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="H23" s="3">
         <v>10</v>
@@ -2346,10 +2352,10 @@
         <v>29</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>16</v>
@@ -2375,10 +2381,10 @@
         <v>29</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>16</v>
@@ -2387,10 +2393,10 @@
         <v>147</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="H26" s="3">
         <v>2</v>
@@ -2404,10 +2410,10 @@
         <v>29</v>
       </c>
       <c r="B27" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C27" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D27" t="s">
         <v>16</v>
@@ -2416,10 +2422,10 @@
         <v>148</v>
       </c>
       <c r="F27" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="G27" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="H27">
         <v>3</v>
@@ -2433,16 +2439,16 @@
         <v>29</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E28" s="3">
         <v>0</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G28" s="4" t="s">
         <v>75</v>
@@ -2488,10 +2494,10 @@
         <v>29</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D30" s="3" t="s">
         <v>16</v>
@@ -2500,10 +2506,10 @@
         <v>132</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G30" s="4" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="H30" s="3">
         <v>6</v>
@@ -2517,16 +2523,16 @@
         <v>29</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="E31" s="3">
         <v>0</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G31" s="4" t="s">
         <v>75</v>
@@ -2572,10 +2578,10 @@
         <v>29</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D33" s="3" t="s">
         <v>16</v>
@@ -2584,10 +2590,10 @@
         <v>101</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="G33" s="4" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="H33" s="3">
         <v>9</v>
@@ -2659,16 +2665,16 @@
         <v>29</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E36" s="3">
         <v>0</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G36" s="4" t="s">
         <v>75</v>
@@ -2743,10 +2749,10 @@
         <v>29</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D39" s="3" t="s">
         <v>16</v>
@@ -2755,10 +2761,10 @@
         <v>117</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G39" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H39" s="3">
         <v>5</v>
@@ -2772,16 +2778,16 @@
         <v>29</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="E40" s="3">
         <v>0</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G40" s="4" t="s">
         <v>75</v>
@@ -2813,7 +2819,7 @@
         <v>35</v>
       </c>
       <c r="G41" s="4" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="H41" s="3">
         <v>7</v>
@@ -2856,10 +2862,10 @@
         <v>29</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D43" s="3" t="s">
         <v>16</v>
@@ -2868,10 +2874,10 @@
         <v>134</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="G43" s="4" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="H43" s="3">
         <v>9</v>
@@ -2926,7 +2932,7 @@
         <v>1</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="G45" s="4" t="s">
         <v>13</v>
@@ -3014,7 +3020,7 @@
         <v>21</v>
       </c>
       <c r="G48" s="5" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="H48" s="3">
         <v>4</v>
@@ -3083,25 +3089,25 @@
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E51" s="3">
         <v>201</v>
       </c>
       <c r="F51" s="3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="G51" s="3" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="H51" s="3">
         <v>0</v>
@@ -3112,16 +3118,16 @@
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B52" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="D52" s="3" t="s">
         <v>118</v>
-      </c>
-      <c r="C52" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="D52" s="3" t="s">
-        <v>120</v>
       </c>
       <c r="E52" s="3">
         <v>203</v>
@@ -3141,16 +3147,16 @@
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E53" s="3">
         <v>202</v>
@@ -3170,19 +3176,19 @@
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E54" s="3">
         <v>0</v>
       </c>
       <c r="F54" s="3" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G54" s="4" t="s">
         <v>75</v>
@@ -3196,16 +3202,16 @@
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E55" s="3">
         <v>210</v>
@@ -3214,7 +3220,7 @@
         <v>78</v>
       </c>
       <c r="G55" s="3" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="H55" s="3">
         <v>6</v>
@@ -3225,16 +3231,16 @@
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B56" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="C56" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="C56" s="3" t="s">
-        <v>133</v>
-      </c>
       <c r="D56" s="3" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E56" s="3">
         <v>211</v>
@@ -3243,7 +3249,7 @@
         <v>78</v>
       </c>
       <c r="G56" s="3" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="H56" s="3">
         <v>7</v>
@@ -3254,16 +3260,16 @@
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E57" s="3">
         <v>212</v>
@@ -3272,7 +3278,7 @@
         <v>78</v>
       </c>
       <c r="G57" s="3" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="H57" s="3">
         <v>8</v>
@@ -3283,19 +3289,19 @@
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E58" s="3">
         <v>0</v>
       </c>
       <c r="F58" s="3" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G58" s="4" t="s">
         <v>75</v>
@@ -3309,16 +3315,16 @@
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B59" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="D59" s="3" t="s">
         <v>127</v>
-      </c>
-      <c r="C59" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="D59" s="3" t="s">
-        <v>129</v>
       </c>
       <c r="E59" s="3">
         <v>213</v>
@@ -3327,7 +3333,7 @@
         <v>78</v>
       </c>
       <c r="G59" s="3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="H59" s="3">
         <v>2</v>
@@ -3338,16 +3344,16 @@
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="D60" s="3" t="s">
         <v>107</v>
-      </c>
-      <c r="B60" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="C60" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="D60" s="3" t="s">
-        <v>109</v>
       </c>
       <c r="E60" s="3">
         <v>220</v>
@@ -3367,16 +3373,16 @@
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="C61" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="D61" s="3" t="s">
         <v>107</v>
-      </c>
-      <c r="B61" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="C61" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="D61" s="3" t="s">
-        <v>109</v>
       </c>
       <c r="E61" s="3">
         <v>221</v>
@@ -3396,16 +3402,16 @@
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="C62" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="D62" s="3" t="s">
         <v>107</v>
-      </c>
-      <c r="B62" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="C62" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="D62" s="3" t="s">
-        <v>109</v>
       </c>
       <c r="E62" s="3">
         <v>222</v>
@@ -3425,16 +3431,16 @@
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="C63" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="D63" s="3" t="s">
         <v>107</v>
-      </c>
-      <c r="B63" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="C63" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="D63" s="3" t="s">
-        <v>109</v>
       </c>
       <c r="E63" s="3">
         <v>223</v>
@@ -3454,16 +3460,16 @@
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="C64" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="D64" s="3" t="s">
         <v>107</v>
-      </c>
-      <c r="B64" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="C64" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="D64" s="3" t="s">
-        <v>109</v>
       </c>
       <c r="E64" s="3">
         <v>224</v>
@@ -3483,16 +3489,16 @@
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="C65" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="D65" s="3" t="s">
         <v>107</v>
-      </c>
-      <c r="B65" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="C65" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="D65" s="3" t="s">
-        <v>109</v>
       </c>
       <c r="E65" s="3">
         <v>225</v>
@@ -3512,16 +3518,16 @@
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C66" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="D66" s="3" t="s">
         <v>107</v>
-      </c>
-      <c r="B66" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="C66" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="D66" s="3" t="s">
-        <v>109</v>
       </c>
       <c r="E66" s="3">
         <v>226</v>
@@ -3541,16 +3547,16 @@
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="B67" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="C67" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="D67" s="3" t="s">
         <v>107</v>
-      </c>
-      <c r="B67" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="C67" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="D67" s="3" t="s">
-        <v>109</v>
       </c>
       <c r="E67" s="3">
         <v>227</v>
@@ -3576,7 +3582,7 @@
         <v>72</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D68" s="3" t="s">
         <v>16</v>
@@ -3585,10 +3591,10 @@
         <v>120</v>
       </c>
       <c r="F68" s="3" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="G68" s="4" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="H68" s="3">
         <v>0</v>
@@ -3643,7 +3649,7 @@
         <v>145</v>
       </c>
       <c r="F70" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="G70" s="4" t="s">
         <v>79</v>
@@ -3660,16 +3666,16 @@
         <v>58</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="E71" s="3">
         <v>0</v>
       </c>
       <c r="F71" s="3" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G71" s="4" t="s">
         <v>75</v>
@@ -3718,7 +3724,7 @@
         <v>67</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D73" s="3" t="s">
         <v>16</v>
@@ -3831,10 +3837,10 @@
         <v>58</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="D77" s="3" t="s">
         <v>16</v>
@@ -3843,10 +3849,10 @@
         <v>133</v>
       </c>
       <c r="F77" s="3" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="G77" s="4" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="H77" s="3">
         <v>9</v>
@@ -3860,10 +3866,10 @@
         <v>58</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D78" s="3" t="s">
         <v>16</v>
@@ -3872,10 +3878,10 @@
         <v>140</v>
       </c>
       <c r="F78" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="G78" s="4" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="H78" s="3">
         <v>10</v>
@@ -3889,10 +3895,10 @@
         <v>58</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D79" s="3" t="s">
         <v>16</v>
@@ -3918,16 +3924,16 @@
         <v>58</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="E80" s="3">
         <v>0</v>
       </c>
       <c r="F80" s="3" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G80" s="4" t="s">
         <v>75</v>
@@ -3944,10 +3950,10 @@
         <v>58</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D81" s="3" t="s">
         <v>16</v>
@@ -3956,10 +3962,10 @@
         <v>112</v>
       </c>
       <c r="F81" s="3" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="G81" s="4" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="H81" s="3">
         <v>4</v>
@@ -3973,10 +3979,10 @@
         <v>58</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D82" s="3" t="s">
         <v>16</v>
@@ -4002,10 +4008,10 @@
         <v>58</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D83" s="3" t="s">
         <v>16</v>
@@ -4014,10 +4020,10 @@
         <v>111</v>
       </c>
       <c r="F83" s="3" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="G83" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="H83" s="3">
         <v>6</v>
@@ -4031,10 +4037,10 @@
         <v>58</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="D84" s="3" t="s">
         <v>16</v>
@@ -4043,10 +4049,10 @@
         <v>112</v>
       </c>
       <c r="F84" s="3" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="G84" s="3" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="H84" s="3">
         <v>7</v>

</xml_diff>

<commit_message>
Fixed handling of visit_opp - if blocks or children limited sowing, the opposite side could be visited and the lapper would stop when it shouldn't. The game Bao exposed this error. Renamed visit_opp to mlap_cont and moved the lap continuer tests out of sow_rule into mlap_cont enum. The LAP_CONT* rules were not moved because they effect the base sower (could be moved). Added mlap_param for mlap_cont. Renumbered the sow_rule enums. Updated the xlsx format macro for new params. Adjusted games that were effected. csv files are now configure with line ending of LF only.
</commit_message>
<xml_diff>
--- a/src/game_params.xlsx
+++ b/src/game_params.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Activity_Data\Mancala_github\MancalaGames\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C05CD46-FCDE-4AF3-BDFB-094E1C198118}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EFF7A96-8354-4031-8789-883CB43001BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32820" yWindow="2535" windowWidth="19605" windowHeight="12060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="game_params" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">game_params!$A$1:$I$84</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">game_params!$A$1:$I$86</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="250">
   <si>
     <t>tab</t>
   </si>
@@ -255,12 +255,6 @@
   </si>
   <si>
     <t>mlaps</t>
-  </si>
-  <si>
-    <t>visit_opp</t>
-  </si>
-  <si>
-    <t>Visit Opp for Mlaps</t>
   </si>
   <si>
     <t>0</t>
@@ -772,6 +766,27 @@
   </si>
   <si>
     <t>Capture Direction</t>
+  </si>
+  <si>
+    <t>slap_lbl</t>
+  </si>
+  <si>
+    <t>Sow Lap Control</t>
+  </si>
+  <si>
+    <t>Lap Continue Reason</t>
+  </si>
+  <si>
+    <t>SowLapCont</t>
+  </si>
+  <si>
+    <t>mlap_param</t>
+  </si>
+  <si>
+    <t>Lap Continue Param</t>
+  </si>
+  <si>
+    <t>mlap_cont</t>
   </si>
 </sst>
 </file>
@@ -1338,6 +1353,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF7C80"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1647,11 +1667,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:I84"/>
+  <dimension ref="A1:I86"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C15" sqref="C15"/>
+      <pane ySplit="1" topLeftCell="A58" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C80" sqref="C80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1682,7 +1702,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>4</v>
@@ -1699,23 +1719,23 @@
     </row>
     <row r="2" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3">
         <v>0</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="H2" s="3">
         <v>0</v>
@@ -1726,13 +1746,13 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>16</v>
@@ -1755,13 +1775,13 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>16</v>
@@ -1773,7 +1793,7 @@
         <v>8</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="H4" s="3">
         <v>2</v>
@@ -1784,13 +1804,13 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>16</v>
@@ -1802,7 +1822,7 @@
         <v>8</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="H5" s="3">
         <v>3</v>
@@ -1813,13 +1833,13 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>16</v>
@@ -1828,10 +1848,10 @@
         <v>107</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H6" s="3">
         <v>4</v>
@@ -1842,22 +1862,22 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="E7" s="3">
         <v>0</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="H7" s="3">
         <v>5</v>
@@ -1868,13 +1888,13 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>16</v>
@@ -1897,13 +1917,13 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>16</v>
@@ -1912,10 +1932,10 @@
         <v>151</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="H9" s="3">
         <v>7</v>
@@ -1926,13 +1946,13 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>16</v>
@@ -1955,22 +1975,22 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B11" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="E11" s="3">
+        <v>0</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="G11" s="4" t="s">
         <v>195</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>196</v>
-      </c>
-      <c r="E11" s="3">
-        <v>0</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>197</v>
       </c>
       <c r="H11" s="3">
         <v>9</v>
@@ -1981,13 +2001,13 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>16</v>
@@ -1996,10 +2016,10 @@
         <v>106</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="H12" s="3">
         <v>10</v>
@@ -2010,22 +2030,22 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E13" s="3">
         <v>0</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="H13" s="3">
         <v>0</v>
@@ -2036,13 +2056,13 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>16</v>
@@ -2054,7 +2074,7 @@
         <v>8</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="H14" s="3">
         <v>1</v>
@@ -2065,13 +2085,13 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>16</v>
@@ -2080,10 +2100,10 @@
         <v>103</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="H15" s="3">
         <v>2</v>
@@ -2094,22 +2114,22 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="E16" s="3">
         <v>0</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="H16" s="3">
         <v>3</v>
@@ -2120,13 +2140,13 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>16</v>
@@ -2138,7 +2158,7 @@
         <v>8</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="H17" s="3">
         <v>4</v>
@@ -2149,13 +2169,13 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>16</v>
@@ -2164,10 +2184,10 @@
         <v>130</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="H18" s="3">
         <v>5</v>
@@ -2178,13 +2198,13 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>16</v>
@@ -2207,13 +2227,13 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C20" s="3" t="s">
         <v>80</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>82</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>16</v>
@@ -2236,22 +2256,22 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="E21" s="3">
         <v>0</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="H21" s="3">
         <v>8</v>
@@ -2262,13 +2282,13 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>16</v>
@@ -2277,10 +2297,10 @@
         <v>108</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="H22" s="3">
         <v>9</v>
@@ -2291,13 +2311,13 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B23" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="C23" s="3" t="s">
         <v>155</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>157</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>16</v>
@@ -2306,10 +2326,10 @@
         <v>131</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="H23" s="3">
         <v>10</v>
@@ -2352,10 +2372,10 @@
         <v>29</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>16</v>
@@ -2367,7 +2387,7 @@
         <v>8</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="H25" s="3">
         <v>1</v>
@@ -2381,10 +2401,10 @@
         <v>29</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>16</v>
@@ -2393,10 +2413,10 @@
         <v>147</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="H26" s="3">
         <v>2</v>
@@ -2410,10 +2430,10 @@
         <v>29</v>
       </c>
       <c r="B27" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C27" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D27" t="s">
         <v>16</v>
@@ -2422,10 +2442,10 @@
         <v>148</v>
       </c>
       <c r="F27" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="G27" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="H27">
         <v>3</v>
@@ -2439,19 +2459,19 @@
         <v>29</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="E28" s="3">
         <v>0</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="H28" s="3">
         <v>4</v>
@@ -2494,10 +2514,10 @@
         <v>29</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D30" s="3" t="s">
         <v>16</v>
@@ -2506,10 +2526,10 @@
         <v>132</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="G30" s="4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="H30" s="3">
         <v>6</v>
@@ -2523,19 +2543,19 @@
         <v>29</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="E31" s="3">
         <v>0</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="H31" s="3">
         <v>7</v>
@@ -2578,10 +2598,10 @@
         <v>29</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D33" s="3" t="s">
         <v>16</v>
@@ -2590,10 +2610,10 @@
         <v>101</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="G33" s="4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="H33" s="3">
         <v>9</v>
@@ -2665,19 +2685,19 @@
         <v>29</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="E36" s="3">
         <v>0</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="G36" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="H36" s="3">
         <v>2</v>
@@ -2749,10 +2769,10 @@
         <v>29</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D39" s="3" t="s">
         <v>16</v>
@@ -2761,10 +2781,10 @@
         <v>117</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="G39" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="H39" s="3">
         <v>5</v>
@@ -2778,19 +2798,19 @@
         <v>29</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="E40" s="3">
         <v>0</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="G40" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="H40" s="3">
         <v>6</v>
@@ -2819,7 +2839,7 @@
         <v>35</v>
       </c>
       <c r="G41" s="4" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="H41" s="3">
         <v>7</v>
@@ -2862,10 +2882,10 @@
         <v>29</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D43" s="3" t="s">
         <v>16</v>
@@ -2874,10 +2894,10 @@
         <v>134</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="G43" s="4" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="H43" s="3">
         <v>9</v>
@@ -2932,7 +2952,7 @@
         <v>1</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="G45" s="4" t="s">
         <v>13</v>
@@ -3020,7 +3040,7 @@
         <v>21</v>
       </c>
       <c r="G48" s="5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="H48" s="3">
         <v>4</v>
@@ -3089,25 +3109,25 @@
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E51" s="3">
         <v>201</v>
       </c>
       <c r="F51" s="3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="G51" s="3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="H51" s="3">
         <v>0</v>
@@ -3118,16 +3138,16 @@
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B52" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="D52" s="3" t="s">
         <v>116</v>
-      </c>
-      <c r="C52" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="D52" s="3" t="s">
-        <v>118</v>
       </c>
       <c r="E52" s="3">
         <v>203</v>
@@ -3147,16 +3167,16 @@
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E53" s="3">
         <v>202</v>
@@ -3176,22 +3196,22 @@
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="E54" s="3">
         <v>0</v>
       </c>
       <c r="F54" s="3" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="G54" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="H54" s="3">
         <v>5</v>
@@ -3202,25 +3222,25 @@
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E55" s="3">
         <v>210</v>
       </c>
       <c r="F55" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G55" s="3" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="H55" s="3">
         <v>6</v>
@@ -3231,25 +3251,25 @@
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B56" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="C56" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="C56" s="3" t="s">
-        <v>131</v>
-      </c>
       <c r="D56" s="3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E56" s="3">
         <v>211</v>
       </c>
       <c r="F56" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G56" s="3" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="H56" s="3">
         <v>7</v>
@@ -3260,25 +3280,25 @@
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E57" s="3">
         <v>212</v>
       </c>
       <c r="F57" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G57" s="3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="H57" s="3">
         <v>8</v>
@@ -3289,22 +3309,22 @@
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E58" s="3">
         <v>0</v>
       </c>
       <c r="F58" s="3" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="G58" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="H58" s="3">
         <v>1</v>
@@ -3315,25 +3335,25 @@
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B59" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="D59" s="3" t="s">
         <v>125</v>
-      </c>
-      <c r="C59" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="D59" s="3" t="s">
-        <v>127</v>
       </c>
       <c r="E59" s="3">
         <v>213</v>
       </c>
       <c r="F59" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G59" s="3" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="H59" s="3">
         <v>2</v>
@@ -3344,16 +3364,16 @@
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="D60" s="3" t="s">
         <v>105</v>
-      </c>
-      <c r="B60" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="C60" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="D60" s="3" t="s">
-        <v>107</v>
       </c>
       <c r="E60" s="3">
         <v>220</v>
@@ -3373,16 +3393,16 @@
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C61" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="D61" s="3" t="s">
         <v>105</v>
-      </c>
-      <c r="B61" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="C61" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="D61" s="3" t="s">
-        <v>107</v>
       </c>
       <c r="E61" s="3">
         <v>221</v>
@@ -3391,7 +3411,7 @@
         <v>8</v>
       </c>
       <c r="G61" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="H61" s="3">
         <v>4</v>
@@ -3402,16 +3422,16 @@
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="C62" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="D62" s="3" t="s">
         <v>105</v>
-      </c>
-      <c r="B62" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="C62" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="D62" s="3" t="s">
-        <v>107</v>
       </c>
       <c r="E62" s="3">
         <v>222</v>
@@ -3420,7 +3440,7 @@
         <v>8</v>
       </c>
       <c r="G62" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="H62" s="3">
         <v>5</v>
@@ -3431,16 +3451,16 @@
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="C63" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="D63" s="3" t="s">
         <v>105</v>
-      </c>
-      <c r="B63" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="C63" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="D63" s="3" t="s">
-        <v>107</v>
       </c>
       <c r="E63" s="3">
         <v>223</v>
@@ -3449,7 +3469,7 @@
         <v>8</v>
       </c>
       <c r="G63" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="H63" s="3">
         <v>6</v>
@@ -3460,16 +3480,16 @@
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="C64" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="D64" s="3" t="s">
         <v>105</v>
-      </c>
-      <c r="B64" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="C64" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="D64" s="3" t="s">
-        <v>107</v>
       </c>
       <c r="E64" s="3">
         <v>224</v>
@@ -3478,7 +3498,7 @@
         <v>8</v>
       </c>
       <c r="G64" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="H64" s="3">
         <v>7</v>
@@ -3489,16 +3509,16 @@
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="C65" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="D65" s="3" t="s">
         <v>105</v>
-      </c>
-      <c r="B65" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="C65" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="D65" s="3" t="s">
-        <v>107</v>
       </c>
       <c r="E65" s="3">
         <v>225</v>
@@ -3507,7 +3527,7 @@
         <v>8</v>
       </c>
       <c r="G65" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="H65" s="3">
         <v>8</v>
@@ -3518,16 +3538,16 @@
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="C66" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="D66" s="3" t="s">
         <v>105</v>
-      </c>
-      <c r="B66" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="C66" s="3" t="s">
-        <v>180</v>
-      </c>
-      <c r="D66" s="3" t="s">
-        <v>107</v>
       </c>
       <c r="E66" s="3">
         <v>226</v>
@@ -3536,7 +3556,7 @@
         <v>8</v>
       </c>
       <c r="G66" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="H66" s="3">
         <v>9</v>
@@ -3547,16 +3567,16 @@
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B67" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="C67" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="D67" s="3" t="s">
         <v>105</v>
-      </c>
-      <c r="B67" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="C67" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="D67" s="3" t="s">
-        <v>107</v>
       </c>
       <c r="E67" s="3">
         <v>227</v>
@@ -3565,7 +3585,7 @@
         <v>8</v>
       </c>
       <c r="G67" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="H67" s="3">
         <v>10</v>
@@ -3582,7 +3602,7 @@
         <v>72</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D68" s="3" t="s">
         <v>16</v>
@@ -3591,10 +3611,10 @@
         <v>120</v>
       </c>
       <c r="F68" s="3" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="G68" s="4" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="H68" s="3">
         <v>0</v>
@@ -3637,10 +3657,10 @@
         <v>58</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D70" s="3" t="s">
         <v>16</v>
@@ -3649,10 +3669,10 @@
         <v>145</v>
       </c>
       <c r="F70" s="3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="G70" s="4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H70" s="3">
         <v>2</v>
@@ -3666,19 +3686,19 @@
         <v>58</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="E71" s="3">
         <v>0</v>
       </c>
       <c r="F71" s="3" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="G71" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="H71" s="3">
         <v>3</v>
@@ -3724,7 +3744,7 @@
         <v>67</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D73" s="3" t="s">
         <v>16</v>
@@ -3808,25 +3828,25 @@
         <v>58</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>73</v>
+        <v>223</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>74</v>
+        <v>224</v>
       </c>
       <c r="D76" s="3" t="s">
         <v>16</v>
       </c>
       <c r="E76" s="3">
-        <v>149</v>
+        <v>133</v>
       </c>
       <c r="F76" s="3" t="s">
-        <v>32</v>
+        <v>225</v>
       </c>
       <c r="G76" s="4" t="s">
-        <v>33</v>
+        <v>142</v>
       </c>
       <c r="H76" s="3">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="I76" s="3">
         <v>0</v>
@@ -3837,25 +3857,25 @@
         <v>58</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>225</v>
+        <v>150</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>226</v>
+        <v>151</v>
       </c>
       <c r="D77" s="3" t="s">
         <v>16</v>
       </c>
       <c r="E77" s="3">
-        <v>133</v>
+        <v>140</v>
       </c>
       <c r="F77" s="3" t="s">
-        <v>227</v>
+        <v>152</v>
       </c>
       <c r="G77" s="4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="H77" s="3">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I77" s="3">
         <v>0</v>
@@ -3866,25 +3886,25 @@
         <v>58</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>152</v>
+        <v>182</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>153</v>
+        <v>183</v>
       </c>
       <c r="D78" s="3" t="s">
         <v>16</v>
       </c>
       <c r="E78" s="3">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="F78" s="3" t="s">
-        <v>154</v>
+        <v>8</v>
       </c>
       <c r="G78" s="4" t="s">
-        <v>144</v>
+        <v>73</v>
       </c>
       <c r="H78" s="3">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I78" s="3">
         <v>0</v>
@@ -3895,28 +3915,25 @@
         <v>58</v>
       </c>
       <c r="B79" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="C79" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="E79" s="3">
+        <v>0</v>
+      </c>
+      <c r="F79" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="C79" s="3" t="s">
-        <v>185</v>
-      </c>
-      <c r="D79" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E79" s="3">
-        <v>142</v>
-      </c>
-      <c r="F79" s="3" t="s">
-        <v>8</v>
-      </c>
       <c r="G79" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="H79" s="3">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="I79" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.25">
@@ -3924,22 +3941,25 @@
         <v>58</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>207</v>
+        <v>249</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>208</v>
+        <v>245</v>
+      </c>
+      <c r="D80" s="3" t="s">
+        <v>16</v>
       </c>
       <c r="E80" s="3">
-        <v>0</v>
+        <v>150</v>
       </c>
       <c r="F80" s="3" t="s">
-        <v>186</v>
+        <v>246</v>
       </c>
       <c r="G80" s="4" t="s">
-        <v>75</v>
+        <v>142</v>
       </c>
       <c r="H80" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I80" s="3">
         <v>2</v>
@@ -3950,25 +3970,25 @@
         <v>58</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>137</v>
+        <v>247</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>138</v>
+        <v>248</v>
       </c>
       <c r="D81" s="3" t="s">
         <v>16</v>
       </c>
       <c r="E81" s="3">
-        <v>112</v>
+        <v>151</v>
       </c>
       <c r="F81" s="3" t="s">
-        <v>140</v>
+        <v>8</v>
       </c>
       <c r="G81" s="4" t="s">
-        <v>139</v>
+        <v>73</v>
       </c>
       <c r="H81" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I81" s="3">
         <v>2</v>
@@ -3979,25 +3999,22 @@
         <v>58</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>135</v>
+        <v>205</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="D82" s="3" t="s">
-        <v>16</v>
+        <v>206</v>
       </c>
       <c r="E82" s="3">
-        <v>110</v>
+        <v>0</v>
       </c>
       <c r="F82" s="3" t="s">
-        <v>8</v>
+        <v>184</v>
       </c>
       <c r="G82" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="H82" s="3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I82" s="3">
         <v>2</v>
@@ -4008,25 +4025,25 @@
         <v>58</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>166</v>
+        <v>135</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>167</v>
+        <v>136</v>
       </c>
       <c r="D83" s="3" t="s">
         <v>16</v>
       </c>
       <c r="E83" s="3">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F83" s="3" t="s">
-        <v>168</v>
-      </c>
-      <c r="G83" s="3" t="s">
-        <v>144</v>
+        <v>138</v>
+      </c>
+      <c r="G83" s="4" t="s">
+        <v>137</v>
       </c>
       <c r="H83" s="3">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="I83" s="3">
         <v>2</v>
@@ -4037,42 +4054,100 @@
         <v>58</v>
       </c>
       <c r="B84" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="C84" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="D84" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E84" s="3">
+        <v>110</v>
+      </c>
+      <c r="F84" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G84" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="H84" s="3">
+        <v>5</v>
+      </c>
+      <c r="I84" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A85" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B85" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="C85" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="D85" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E85" s="3">
+        <v>111</v>
+      </c>
+      <c r="F85" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="G85" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="H85" s="3">
+        <v>6</v>
+      </c>
+      <c r="I85" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A86" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B86" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="C86" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="D86" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E86" s="3">
+        <v>112</v>
+      </c>
+      <c r="F86" s="3" t="s">
         <v>228</v>
       </c>
-      <c r="C84" s="3" t="s">
+      <c r="G86" s="3" t="s">
         <v>229</v>
       </c>
-      <c r="D84" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E84" s="3">
-        <v>112</v>
-      </c>
-      <c r="F84" s="3" t="s">
-        <v>230</v>
-      </c>
-      <c r="G84" s="3" t="s">
-        <v>231</v>
-      </c>
-      <c r="H84" s="3">
+      <c r="H86" s="3">
         <v>7</v>
       </c>
-      <c r="I84" s="3">
+      <c r="I86" s="3">
         <v>2</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I84" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I84">
-      <sortCondition ref="A2:A84"/>
-      <sortCondition ref="I2:I84"/>
-      <sortCondition ref="H2:H84"/>
+  <autoFilter ref="A1:I86" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I86">
+      <sortCondition ref="A2:A86"/>
+      <sortCondition ref="I2:I86"/>
+      <sortCondition ref="H2:H86"/>
     </sortState>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:I84">
-    <sortCondition ref="A3:A84"/>
-    <sortCondition ref="I3:I84"/>
-    <sortCondition ref="H3:H84"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:I86">
+    <sortCondition ref="A3:A86"/>
+    <sortCondition ref="I3:I86"/>
+    <sortCondition ref="H3:H86"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added the ability to edit the variations from the editor.
</commit_message>
<xml_diff>
--- a/src/game_params.xlsx
+++ b/src/game_params.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Activity_Data\Mancala_github\MancalaGames\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EFF7A96-8354-4031-8789-883CB43001BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC15A28D-5F1B-4B03-8535-FF963F45C84F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32925" yWindow="2415" windowWidth="21180" windowHeight="12060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="game_params" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="513" uniqueCount="257">
   <si>
     <t>tab</t>
   </si>
@@ -787,6 +787,27 @@
   </si>
   <si>
     <t>mlap_cont</t>
+  </si>
+  <si>
+    <t>Variants</t>
+  </si>
+  <si>
+    <t>variants</t>
+  </si>
+  <si>
+    <t>Named Variants</t>
+  </si>
+  <si>
+    <t>_</t>
+  </si>
+  <si>
+    <t>TextDict</t>
+  </si>
+  <si>
+    <t>vari_params</t>
+  </si>
+  <si>
+    <t>Vari Params</t>
   </si>
 </sst>
 </file>
@@ -1667,11 +1688,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:I86"/>
+  <dimension ref="A1:I88"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A58" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C80" sqref="C80"/>
+      <pane ySplit="1" topLeftCell="A73" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A87" sqref="A87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4136,6 +4157,58 @@
         <v>2</v>
       </c>
     </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A87" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="B87" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="C87" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="D87" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="E87" s="3">
+        <v>250</v>
+      </c>
+      <c r="F87" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="H87" s="3">
+        <v>0</v>
+      </c>
+      <c r="I87" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A88" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="B88" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="C88" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="D88" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="E88" s="3">
+        <v>251</v>
+      </c>
+      <c r="F88" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="H88" s="3">
+        <v>0</v>
+      </c>
+      <c r="I88" s="3">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:I86" xr:uid="{00000000-0001-0000-0000-000000000000}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I86">

</xml_diff>

<commit_message>
Allow the multi-line text widgets to grow. Corrected UDIR_HOLES widget so that it changes # of check boxes again, adding variants to the man_games_editor started games broke it, required putting tk var names back in but made them unique for the two apps. Moved the widgets out of the way of the expanding UDIR_HOLES, mlap_continue widgets had been put in the way. Consistent use of tk constants instead of strings.
</commit_message>
<xml_diff>
--- a/src/game_params.xlsx
+++ b/src/game_params.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Activity_Data\Mancala_github\MancalaGames\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC15A28D-5F1B-4B03-8535-FF963F45C84F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5113BD47-FFAD-46B6-8AA3-7715A025633D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32925" yWindow="2415" windowWidth="21180" windowHeight="12060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33615" yWindow="1800" windowWidth="21180" windowHeight="12060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="game_params" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">game_params!$A$1:$I$86</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">game_params!$A$1:$I$88</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -964,7 +964,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1144,6 +1144,12 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -1306,7 +1312,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1324,6 +1330,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -1691,8 +1700,8 @@
   <dimension ref="A1:I88"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A73" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A87" sqref="A87"/>
+      <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H86" sqref="H86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3021,7 +3030,7 @@
       <c r="B47" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C47" s="3" t="s">
+      <c r="C47" s="7" t="s">
         <v>18</v>
       </c>
       <c r="D47" s="3" t="s">
@@ -3048,7 +3057,7 @@
       <c r="B48" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C48" s="3" t="s">
+      <c r="C48" s="7" t="s">
         <v>20</v>
       </c>
       <c r="D48" s="3" t="s">
@@ -3077,7 +3086,7 @@
       <c r="B49" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C49" s="3" t="s">
+      <c r="C49" s="7" t="s">
         <v>15</v>
       </c>
       <c r="D49" s="3" t="s">
@@ -3951,7 +3960,7 @@
         <v>73</v>
       </c>
       <c r="H79" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I79" s="3">
         <v>2</v>
@@ -3980,7 +3989,7 @@
         <v>142</v>
       </c>
       <c r="H80" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I80" s="3">
         <v>2</v>
@@ -4009,7 +4018,7 @@
         <v>73</v>
       </c>
       <c r="H81" s="3">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="I81" s="3">
         <v>2</v>
@@ -4035,7 +4044,7 @@
         <v>73</v>
       </c>
       <c r="H82" s="3">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I82" s="3">
         <v>2</v>
@@ -4064,7 +4073,7 @@
         <v>137</v>
       </c>
       <c r="H83" s="3">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="I83" s="3">
         <v>2</v>
@@ -4093,7 +4102,7 @@
         <v>73</v>
       </c>
       <c r="H84" s="3">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="I84" s="3">
         <v>2</v>
@@ -4122,7 +4131,7 @@
         <v>142</v>
       </c>
       <c r="H85" s="3">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="I85" s="3">
         <v>2</v>
@@ -4151,7 +4160,7 @@
         <v>229</v>
       </c>
       <c r="H86" s="3">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="I86" s="3">
         <v>2</v>
@@ -4164,7 +4173,7 @@
       <c r="B87" s="3" t="s">
         <v>251</v>
       </c>
-      <c r="C87" s="3" t="s">
+      <c r="C87" s="7" t="s">
         <v>252</v>
       </c>
       <c r="D87" s="3" t="s">
@@ -4190,7 +4199,7 @@
       <c r="B88" s="3" t="s">
         <v>255</v>
       </c>
-      <c r="C88" s="3" t="s">
+      <c r="C88" s="7" t="s">
         <v>256</v>
       </c>
       <c r="D88" s="3" t="s">
@@ -4210,13 +4219,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I86" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I86">
-      <sortCondition ref="A2:A86"/>
-      <sortCondition ref="I2:I86"/>
-      <sortCondition ref="H2:H86"/>
-    </sortState>
-  </autoFilter>
+  <autoFilter ref="A1:I88" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:I86">
     <sortCondition ref="A3:A86"/>
     <sortCondition ref="I3:I86"/>

</xml_diff>

<commit_message>
Moved sow parameters in 1st column up after visit_opp/mlap_cont was moved to second col.
</commit_message>
<xml_diff>
--- a/src/game_params.xlsx
+++ b/src/game_params.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Activity_Data\Mancala_github\MancalaGames\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E202C228-00E9-434C-9FE5-D82669AEF1A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2242356-4DCD-41D9-BEFB-A530A17E29BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4650" yWindow="1455" windowWidth="21180" windowHeight="12690" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7845" yWindow="1485" windowWidth="18315" windowHeight="12690" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="game_params" sheetId="1" r:id="rId1"/>
@@ -1306,25 +1306,24 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1688,12 +1687,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr codeName="Sheet1"/>
+  <sheetPr codeName="Sheet1" filterMode="1"/>
   <dimension ref="A1:I88"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B60" sqref="B60:B67"/>
+      <selection pane="bottomLeft" activeCell="H79" sqref="H79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1739,7 +1738,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>78</v>
       </c>
@@ -1766,7 +1765,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>78</v>
       </c>
@@ -1795,7 +1794,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>78</v>
       </c>
@@ -1824,7 +1823,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>78</v>
       </c>
@@ -1853,7 +1852,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>78</v>
       </c>
@@ -1882,7 +1881,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>78</v>
       </c>
@@ -1908,7 +1907,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>78</v>
       </c>
@@ -1937,7 +1936,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>78</v>
       </c>
@@ -1966,7 +1965,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>78</v>
       </c>
@@ -1995,7 +1994,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>78</v>
       </c>
@@ -2021,7 +2020,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>78</v>
       </c>
@@ -2050,7 +2049,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>78</v>
       </c>
@@ -2076,7 +2075,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>78</v>
       </c>
@@ -2105,7 +2104,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>78</v>
       </c>
@@ -2134,7 +2133,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>78</v>
       </c>
@@ -2160,7 +2159,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>78</v>
       </c>
@@ -2189,7 +2188,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>78</v>
       </c>
@@ -2218,7 +2217,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>78</v>
       </c>
@@ -2247,7 +2246,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>78</v>
       </c>
@@ -2276,7 +2275,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>78</v>
       </c>
@@ -2302,7 +2301,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>78</v>
       </c>
@@ -2331,7 +2330,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>78</v>
       </c>
@@ -2360,7 +2359,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>29</v>
       </c>
@@ -2389,7 +2388,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>29</v>
       </c>
@@ -2418,7 +2417,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>29</v>
       </c>
@@ -2447,36 +2446,36 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="6" t="s">
+    <row r="27" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>29</v>
       </c>
-      <c r="B27" s="6" t="s">
+      <c r="B27" t="s">
         <v>229</v>
       </c>
-      <c r="C27" s="6" t="s">
+      <c r="C27" t="s">
         <v>228</v>
       </c>
-      <c r="D27" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="E27" s="6">
+      <c r="D27" t="s">
+        <v>16</v>
+      </c>
+      <c r="E27">
         <v>148</v>
       </c>
-      <c r="F27" s="6" t="s">
+      <c r="F27" t="s">
         <v>209</v>
       </c>
-      <c r="G27" s="6" t="s">
+      <c r="G27" t="s">
         <v>227</v>
       </c>
-      <c r="H27" s="6">
+      <c r="H27">
         <v>3</v>
       </c>
-      <c r="I27" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>29</v>
       </c>
@@ -2502,7 +2501,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>29</v>
       </c>
@@ -2531,7 +2530,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>29</v>
       </c>
@@ -2560,7 +2559,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>29</v>
       </c>
@@ -2586,7 +2585,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>29</v>
       </c>
@@ -2615,7 +2614,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>29</v>
       </c>
@@ -2644,7 +2643,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>29</v>
       </c>
@@ -2673,7 +2672,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>29</v>
       </c>
@@ -2702,7 +2701,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>29</v>
       </c>
@@ -2728,7 +2727,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>29</v>
       </c>
@@ -2757,7 +2756,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>29</v>
       </c>
@@ -2786,7 +2785,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>29</v>
       </c>
@@ -2815,7 +2814,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>29</v>
       </c>
@@ -2841,7 +2840,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>29</v>
       </c>
@@ -2870,7 +2869,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>29</v>
       </c>
@@ -2899,7 +2898,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>29</v>
       </c>
@@ -2928,7 +2927,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>29</v>
       </c>
@@ -2957,7 +2956,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>9</v>
       </c>
@@ -2986,7 +2985,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>9</v>
       </c>
@@ -3015,7 +3014,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>9</v>
       </c>
@@ -3042,7 +3041,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>9</v>
       </c>
@@ -3061,7 +3060,7 @@
       <c r="F48" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="G48" s="7" t="s">
+      <c r="G48" s="6" t="s">
         <v>109</v>
       </c>
       <c r="H48" s="1">
@@ -3071,7 +3070,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>9</v>
       </c>
@@ -3100,7 +3099,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>9</v>
       </c>
@@ -3129,7 +3128,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>103</v>
       </c>
@@ -3158,7 +3157,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>103</v>
       </c>
@@ -3187,7 +3186,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>103</v>
       </c>
@@ -3216,7 +3215,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>103</v>
       </c>
@@ -3242,7 +3241,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>103</v>
       </c>
@@ -3271,7 +3270,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>103</v>
       </c>
@@ -3300,7 +3299,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>103</v>
       </c>
@@ -3329,7 +3328,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>103</v>
       </c>
@@ -3355,7 +3354,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>103</v>
       </c>
@@ -3384,7 +3383,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>103</v>
       </c>
@@ -3413,7 +3412,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>103</v>
       </c>
@@ -3442,7 +3441,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>103</v>
       </c>
@@ -3471,7 +3470,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>103</v>
       </c>
@@ -3500,7 +3499,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>103</v>
       </c>
@@ -3529,7 +3528,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>103</v>
       </c>
@@ -3558,7 +3557,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>103</v>
       </c>
@@ -3587,7 +3586,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>103</v>
       </c>
@@ -3868,7 +3867,7 @@
         <v>134</v>
       </c>
       <c r="H76" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I76" s="1">
         <v>0</v>
@@ -3897,7 +3896,7 @@
         <v>134</v>
       </c>
       <c r="H77" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I77" s="1">
         <v>0</v>
@@ -3926,7 +3925,7 @@
         <v>73</v>
       </c>
       <c r="H78" s="1">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I78" s="1">
         <v>0</v>
@@ -4158,7 +4157,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>242</v>
       </c>
@@ -4184,7 +4183,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>242</v>
       </c>
@@ -4211,7 +4210,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I88" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:I88" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="Sow"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:I86">
     <sortCondition ref="A3:A86"/>
     <sortCondition ref="I3:I86"/>

</xml_diff>

<commit_message>
Added an ability to edit the extra tags in game config files. It's not really user friendly.
</commit_message>
<xml_diff>
--- a/src/game_params.xlsx
+++ b/src/game_params.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Activity_Data\Mancala_github\MancalaGames\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2242356-4DCD-41D9-BEFB-A530A17E29BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85FA91AB-BF80-4D50-9CBF-1C5FCECC0057}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7845" yWindow="1485" windowWidth="18315" windowHeight="12690" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29655" yWindow="1965" windowWidth="18315" windowHeight="12690" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="game_params" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">game_params!$A$1:$I$88</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">game_params!$A$1:$I$89</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="513" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="260">
   <si>
     <t>tab</t>
   </si>
@@ -808,6 +808,15 @@
   </si>
   <si>
     <t>mx_easy_rand_a</t>
+  </si>
+  <si>
+    <t>Tags</t>
+  </si>
+  <si>
+    <t>extra_tops</t>
+  </si>
+  <si>
+    <t>Additional Top Level Tags</t>
   </si>
 </sst>
 </file>
@@ -1687,12 +1696,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr codeName="Sheet1" filterMode="1"/>
-  <dimension ref="A1:I88"/>
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:I89"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H79" sqref="H79"/>
+      <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C89" sqref="C89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1738,7 +1747,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>78</v>
       </c>
@@ -1765,7 +1774,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>78</v>
       </c>
@@ -1794,7 +1803,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>78</v>
       </c>
@@ -1823,7 +1832,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>78</v>
       </c>
@@ -1852,7 +1861,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>78</v>
       </c>
@@ -1881,7 +1890,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>78</v>
       </c>
@@ -1907,7 +1916,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>78</v>
       </c>
@@ -1936,7 +1945,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>78</v>
       </c>
@@ -1965,7 +1974,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>78</v>
       </c>
@@ -1994,7 +2003,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>78</v>
       </c>
@@ -2020,7 +2029,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>78</v>
       </c>
@@ -2049,7 +2058,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>78</v>
       </c>
@@ -2075,7 +2084,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>78</v>
       </c>
@@ -2104,7 +2113,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>78</v>
       </c>
@@ -2133,7 +2142,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>78</v>
       </c>
@@ -2159,7 +2168,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>78</v>
       </c>
@@ -2188,7 +2197,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>78</v>
       </c>
@@ -2217,7 +2226,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>78</v>
       </c>
@@ -2246,7 +2255,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>78</v>
       </c>
@@ -2275,7 +2284,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>78</v>
       </c>
@@ -2301,7 +2310,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>78</v>
       </c>
@@ -2330,7 +2339,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>78</v>
       </c>
@@ -2359,7 +2368,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>29</v>
       </c>
@@ -2388,7 +2397,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>29</v>
       </c>
@@ -2417,7 +2426,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>29</v>
       </c>
@@ -2446,7 +2455,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>29</v>
       </c>
@@ -2475,7 +2484,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>29</v>
       </c>
@@ -2501,7 +2510,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>29</v>
       </c>
@@ -2530,7 +2539,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>29</v>
       </c>
@@ -2559,7 +2568,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>29</v>
       </c>
@@ -2585,7 +2594,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>29</v>
       </c>
@@ -2614,7 +2623,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>29</v>
       </c>
@@ -2643,7 +2652,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>29</v>
       </c>
@@ -2672,7 +2681,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>29</v>
       </c>
@@ -2701,7 +2710,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>29</v>
       </c>
@@ -2727,7 +2736,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>29</v>
       </c>
@@ -2756,7 +2765,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>29</v>
       </c>
@@ -2785,7 +2794,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>29</v>
       </c>
@@ -2814,7 +2823,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>29</v>
       </c>
@@ -2840,7 +2849,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>29</v>
       </c>
@@ -2869,7 +2878,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>29</v>
       </c>
@@ -2898,7 +2907,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>29</v>
       </c>
@@ -2927,7 +2936,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>29</v>
       </c>
@@ -2956,7 +2965,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>9</v>
       </c>
@@ -2985,7 +2994,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>9</v>
       </c>
@@ -3014,7 +3023,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>9</v>
       </c>
@@ -3041,7 +3050,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>9</v>
       </c>
@@ -3070,7 +3079,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>9</v>
       </c>
@@ -3099,7 +3108,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>9</v>
       </c>
@@ -3128,7 +3137,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="51" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>103</v>
       </c>
@@ -3157,7 +3166,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>103</v>
       </c>
@@ -3186,7 +3195,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>103</v>
       </c>
@@ -3215,7 +3224,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>103</v>
       </c>
@@ -3241,7 +3250,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>103</v>
       </c>
@@ -3270,7 +3279,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>103</v>
       </c>
@@ -3299,7 +3308,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>103</v>
       </c>
@@ -3328,7 +3337,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>103</v>
       </c>
@@ -3354,7 +3363,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="59" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>103</v>
       </c>
@@ -3383,7 +3392,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="60" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>103</v>
       </c>
@@ -3412,7 +3421,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="61" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>103</v>
       </c>
@@ -3441,7 +3450,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="62" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>103</v>
       </c>
@@ -3470,7 +3479,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="63" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>103</v>
       </c>
@@ -3499,7 +3508,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="64" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>103</v>
       </c>
@@ -3528,7 +3537,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="65" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>103</v>
       </c>
@@ -3557,7 +3566,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="66" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>103</v>
       </c>
@@ -3586,7 +3595,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="67" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>103</v>
       </c>
@@ -4157,7 +4166,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="87" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>242</v>
       </c>
@@ -4183,7 +4192,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>242</v>
       </c>
@@ -4209,14 +4218,34 @@
         <v>2</v>
       </c>
     </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A89" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="D89" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="E89" s="1">
+        <v>300</v>
+      </c>
+      <c r="F89" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="H89" s="1">
+        <v>0</v>
+      </c>
+      <c r="I89" s="1">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:I88" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="Sow"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:I89" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:I86">
     <sortCondition ref="A3:A86"/>
     <sortCondition ref="I3:I86"/>

</xml_diff>

<commit_message>
Changed sow_own_store to sow_stores, made it an enumeration that now supports sowing both stores.
</commit_message>
<xml_diff>
--- a/src/game_params.xlsx
+++ b/src/game_params.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Activity_Data\Mancala_github\MancalaGames\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85FA91AB-BF80-4D50-9CBF-1C5FCECC0057}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B45410C-65D0-46DB-A361-1C552A1E0C0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29655" yWindow="1965" windowWidth="18315" windowHeight="12690" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32145" yWindow="495" windowWidth="21885" windowHeight="15480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="game_params" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="262">
   <si>
     <t>tab</t>
   </si>
@@ -240,12 +240,6 @@
   </si>
   <si>
     <t>skip_start</t>
-  </si>
-  <si>
-    <t>sow_own_store</t>
-  </si>
-  <si>
-    <t>Sow Own Store</t>
   </si>
   <si>
     <t>blocks</t>
@@ -817,6 +811,18 @@
   </si>
   <si>
     <t>Additional Top Level Tags</t>
+  </si>
+  <si>
+    <t>Sow Store</t>
+  </si>
+  <si>
+    <t>SowStores</t>
+  </si>
+  <si>
+    <t>NEITHER</t>
+  </si>
+  <si>
+    <t>sow_stores</t>
   </si>
 </sst>
 </file>
@@ -1701,7 +1707,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C89" sqref="C89"/>
+      <selection pane="bottomLeft" activeCell="C69" sqref="C69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1732,7 +1738,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>4</v>
@@ -1749,23 +1755,23 @@
     </row>
     <row r="2" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1">
         <v>0</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H2" s="1">
         <v>0</v>
@@ -1776,13 +1782,13 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>16</v>
@@ -1805,13 +1811,13 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>16</v>
@@ -1823,7 +1829,7 @@
         <v>8</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H4" s="1">
         <v>2</v>
@@ -1834,13 +1840,13 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>16</v>
@@ -1852,7 +1858,7 @@
         <v>8</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H5" s="1">
         <v>3</v>
@@ -1863,13 +1869,13 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>16</v>
@@ -1878,10 +1884,10 @@
         <v>107</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="H6" s="1">
         <v>4</v>
@@ -1892,22 +1898,22 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E7" s="1">
         <v>0</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H7" s="1">
         <v>5</v>
@@ -1918,13 +1924,13 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>16</v>
@@ -1947,13 +1953,13 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>16</v>
@@ -1962,10 +1968,10 @@
         <v>151</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="H9" s="1">
         <v>7</v>
@@ -1976,13 +1982,13 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>16</v>
@@ -2005,22 +2011,22 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="E11" s="1">
+        <v>0</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="G11" s="5" t="s">
         <v>185</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="E11" s="1">
-        <v>0</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>187</v>
       </c>
       <c r="H11" s="1">
         <v>9</v>
@@ -2031,13 +2037,13 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>16</v>
@@ -2046,10 +2052,10 @@
         <v>106</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="H12" s="1">
         <v>10</v>
@@ -2060,22 +2066,22 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E13" s="1">
         <v>0</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H13" s="1">
         <v>0</v>
@@ -2086,13 +2092,13 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>16</v>
@@ -2104,7 +2110,7 @@
         <v>8</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H14" s="1">
         <v>1</v>
@@ -2115,13 +2121,13 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>16</v>
@@ -2130,10 +2136,10 @@
         <v>103</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="H15" s="1">
         <v>2</v>
@@ -2144,22 +2150,22 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E16" s="1">
         <v>0</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H16" s="1">
         <v>3</v>
@@ -2170,13 +2176,13 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>16</v>
@@ -2188,7 +2194,7 @@
         <v>8</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H17" s="1">
         <v>4</v>
@@ -2199,13 +2205,13 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>16</v>
@@ -2214,10 +2220,10 @@
         <v>130</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="H18" s="1">
         <v>5</v>
@@ -2228,13 +2234,13 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>16</v>
@@ -2257,13 +2263,13 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>78</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>80</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>16</v>
@@ -2286,22 +2292,22 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E21" s="1">
         <v>0</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H21" s="1">
         <v>8</v>
@@ -2312,13 +2318,13 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>16</v>
@@ -2327,10 +2333,10 @@
         <v>108</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="H22" s="1">
         <v>9</v>
@@ -2341,13 +2347,13 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B23" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C23" s="1" t="s">
         <v>145</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>147</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>16</v>
@@ -2356,10 +2362,10 @@
         <v>131</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="H23" s="1">
         <v>10</v>
@@ -2402,10 +2408,10 @@
         <v>29</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>16</v>
@@ -2417,7 +2423,7 @@
         <v>8</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H25" s="1">
         <v>1</v>
@@ -2431,10 +2437,10 @@
         <v>29</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>16</v>
@@ -2443,10 +2449,10 @@
         <v>147</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="G26" s="5" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="H26" s="1">
         <v>2</v>
@@ -2460,10 +2466,10 @@
         <v>29</v>
       </c>
       <c r="B27" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C27" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="D27" t="s">
         <v>16</v>
@@ -2472,10 +2478,10 @@
         <v>148</v>
       </c>
       <c r="F27" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="G27" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="H27">
         <v>3</v>
@@ -2489,19 +2495,19 @@
         <v>29</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="E28" s="1">
         <v>0</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="G28" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H28" s="1">
         <v>4</v>
@@ -2544,10 +2550,10 @@
         <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>16</v>
@@ -2556,10 +2562,10 @@
         <v>132</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="G30" s="5" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="H30" s="1">
         <v>6</v>
@@ -2573,19 +2579,19 @@
         <v>29</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="E31" s="1">
         <v>0</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="G31" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H31" s="1">
         <v>7</v>
@@ -2628,10 +2634,10 @@
         <v>29</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>16</v>
@@ -2640,10 +2646,10 @@
         <v>101</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="G33" s="5" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="H33" s="1">
         <v>9</v>
@@ -2715,19 +2721,19 @@
         <v>29</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="E36" s="1">
         <v>0</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="G36" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H36" s="1">
         <v>2</v>
@@ -2799,10 +2805,10 @@
         <v>29</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>16</v>
@@ -2811,10 +2817,10 @@
         <v>117</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="G39" s="5" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="H39" s="1">
         <v>5</v>
@@ -2828,19 +2834,19 @@
         <v>29</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E40" s="1">
         <v>0</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="G40" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H40" s="1">
         <v>6</v>
@@ -2869,7 +2875,7 @@
         <v>35</v>
       </c>
       <c r="G41" s="5" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="H41" s="1">
         <v>7</v>
@@ -2912,10 +2918,10 @@
         <v>29</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>16</v>
@@ -2924,10 +2930,10 @@
         <v>134</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="G43" s="5" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="H43" s="1">
         <v>9</v>
@@ -2941,10 +2947,10 @@
         <v>29</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>16</v>
@@ -2982,7 +2988,7 @@
         <v>1</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="G45" s="5" t="s">
         <v>13</v>
@@ -3070,7 +3076,7 @@
         <v>21</v>
       </c>
       <c r="G48" s="6" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="H48" s="1">
         <v>4</v>
@@ -3139,25 +3145,25 @@
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E51" s="1">
         <v>201</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="H51" s="1">
         <v>0</v>
@@ -3168,16 +3174,16 @@
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B52" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D52" s="1" t="s">
         <v>106</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>108</v>
       </c>
       <c r="E52" s="1">
         <v>203</v>
@@ -3197,16 +3203,16 @@
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E53" s="1">
         <v>202</v>
@@ -3226,22 +3232,22 @@
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E54" s="1">
         <v>0</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="G54" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H54" s="1">
         <v>5</v>
@@ -3252,25 +3258,25 @@
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E55" s="1">
         <v>210</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="H55" s="1">
         <v>6</v>
@@ -3281,25 +3287,25 @@
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B56" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C56" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="C56" s="1" t="s">
-        <v>121</v>
-      </c>
       <c r="D56" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E56" s="1">
         <v>211</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="H56" s="1">
         <v>7</v>
@@ -3310,25 +3316,25 @@
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E57" s="1">
         <v>212</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G57" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="H57" s="1">
         <v>8</v>
@@ -3339,22 +3345,22 @@
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E58" s="1">
         <v>0</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="G58" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H58" s="1">
         <v>1</v>
@@ -3365,25 +3371,25 @@
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B59" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D59" s="1" t="s">
         <v>115</v>
-      </c>
-      <c r="C59" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="D59" s="1" t="s">
-        <v>117</v>
       </c>
       <c r="E59" s="1">
         <v>213</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G59" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="H59" s="1">
         <v>2</v>
@@ -3394,16 +3400,16 @@
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E60" s="1">
         <v>220</v>
@@ -3423,16 +3429,16 @@
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E61" s="1">
         <v>221</v>
@@ -3441,7 +3447,7 @@
         <v>8</v>
       </c>
       <c r="G61" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H61" s="1">
         <v>4</v>
@@ -3452,16 +3458,16 @@
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E62" s="1">
         <v>222</v>
@@ -3470,7 +3476,7 @@
         <v>8</v>
       </c>
       <c r="G62" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H62" s="1">
         <v>5</v>
@@ -3481,16 +3487,16 @@
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E63" s="1">
         <v>223</v>
@@ -3499,7 +3505,7 @@
         <v>8</v>
       </c>
       <c r="G63" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H63" s="1">
         <v>6</v>
@@ -3510,16 +3516,16 @@
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E64" s="1">
         <v>224</v>
@@ -3528,7 +3534,7 @@
         <v>8</v>
       </c>
       <c r="G64" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H64" s="1">
         <v>7</v>
@@ -3539,16 +3545,16 @@
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E65" s="1">
         <v>225</v>
@@ -3557,7 +3563,7 @@
         <v>8</v>
       </c>
       <c r="G65" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H65" s="1">
         <v>8</v>
@@ -3568,16 +3574,16 @@
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E66" s="1">
         <v>226</v>
@@ -3586,7 +3592,7 @@
         <v>8</v>
       </c>
       <c r="G66" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H66" s="1">
         <v>9</v>
@@ -3597,16 +3603,16 @@
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="C67" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="B67" s="1" t="s">
-        <v>256</v>
-      </c>
-      <c r="C67" s="1" t="s">
-        <v>105</v>
-      </c>
       <c r="D67" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E67" s="1">
         <v>227</v>
@@ -3615,7 +3621,7 @@
         <v>8</v>
       </c>
       <c r="G67" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H67" s="1">
         <v>10</v>
@@ -3629,10 +3635,10 @@
         <v>58</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>16</v>
@@ -3641,10 +3647,10 @@
         <v>120</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="G68" s="5" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="H68" s="1">
         <v>0</v>
@@ -3687,10 +3693,10 @@
         <v>58</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D70" s="1" t="s">
         <v>16</v>
@@ -3699,10 +3705,10 @@
         <v>145</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G70" s="5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="H70" s="1">
         <v>2</v>
@@ -3716,19 +3722,19 @@
         <v>58</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="E71" s="1">
         <v>0</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="G71" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H71" s="1">
         <v>3</v>
@@ -3774,7 +3780,7 @@
         <v>67</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D73" s="1" t="s">
         <v>16</v>
@@ -3800,16 +3806,16 @@
         <v>58</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D74" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E74" s="1">
-        <v>139</v>
+        <v>122</v>
       </c>
       <c r="F74" s="1" t="s">
         <v>32</v>
@@ -3829,22 +3835,22 @@
         <v>58</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>65</v>
+        <v>261</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>66</v>
+        <v>258</v>
       </c>
       <c r="D75" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E75" s="1">
-        <v>122</v>
+        <v>139</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>32</v>
+        <v>259</v>
       </c>
       <c r="G75" s="5" t="s">
-        <v>33</v>
+        <v>260</v>
       </c>
       <c r="H75" s="1">
         <v>7</v>
@@ -3858,10 +3864,10 @@
         <v>58</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D76" s="1" t="s">
         <v>16</v>
@@ -3870,10 +3876,10 @@
         <v>133</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="G76" s="5" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="H76" s="1">
         <v>8</v>
@@ -3887,10 +3893,10 @@
         <v>58</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D77" s="1" t="s">
         <v>16</v>
@@ -3899,10 +3905,10 @@
         <v>140</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G77" s="5" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="H77" s="1">
         <v>9</v>
@@ -3916,10 +3922,10 @@
         <v>58</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D78" s="1" t="s">
         <v>16</v>
@@ -3931,7 +3937,7 @@
         <v>8</v>
       </c>
       <c r="G78" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H78" s="1">
         <v>10</v>
@@ -3945,19 +3951,19 @@
         <v>58</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="E79" s="1">
         <v>0</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="G79" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H79" s="1">
         <v>3</v>
@@ -3971,10 +3977,10 @@
         <v>58</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="D80" s="1" t="s">
         <v>16</v>
@@ -3983,10 +3989,10 @@
         <v>150</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="G80" s="5" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="H80" s="1">
         <v>4</v>
@@ -4000,10 +4006,10 @@
         <v>58</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D81" s="1" t="s">
         <v>16</v>
@@ -4015,7 +4021,7 @@
         <v>8</v>
       </c>
       <c r="G81" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H81" s="1">
         <v>5</v>
@@ -4029,19 +4035,19 @@
         <v>58</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E82" s="1">
         <v>0</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="G82" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H82" s="1">
         <v>6</v>
@@ -4055,10 +4061,10 @@
         <v>58</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D83" s="1" t="s">
         <v>16</v>
@@ -4067,10 +4073,10 @@
         <v>112</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="G83" s="5" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="H83" s="1">
         <v>7</v>
@@ -4084,10 +4090,10 @@
         <v>58</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D84" s="1" t="s">
         <v>16</v>
@@ -4099,7 +4105,7 @@
         <v>8</v>
       </c>
       <c r="G84" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H84" s="1">
         <v>8</v>
@@ -4113,10 +4119,10 @@
         <v>58</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D85" s="1" t="s">
         <v>16</v>
@@ -4125,10 +4131,10 @@
         <v>111</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="G85" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="H85" s="1">
         <v>9</v>
@@ -4142,10 +4148,10 @@
         <v>58</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D86" s="1" t="s">
         <v>16</v>
@@ -4154,10 +4160,10 @@
         <v>112</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="G86" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="H86" s="1">
         <v>10</v>
@@ -4168,22 +4174,22 @@
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>242</v>
+        <v>255</v>
       </c>
       <c r="B87" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="D87" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="C87" s="1" t="s">
+      <c r="E87" s="1">
+        <v>300</v>
+      </c>
+      <c r="F87" s="1" t="s">
         <v>244</v>
-      </c>
-      <c r="D87" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="E87" s="1">
-        <v>250</v>
-      </c>
-      <c r="F87" s="1" t="s">
-        <v>246</v>
       </c>
       <c r="H87" s="1">
         <v>0</v>
@@ -4194,58 +4200,64 @@
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="C88" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="B88" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="C88" s="1" t="s">
-        <v>248</v>
-      </c>
       <c r="D88" s="1" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="E88" s="1">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="H88" s="1">
         <v>0</v>
       </c>
       <c r="I88" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>257</v>
+        <v>240</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>258</v>
+        <v>245</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>259</v>
+        <v>246</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="E89" s="1">
-        <v>300</v>
+        <v>251</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="H89" s="1">
         <v>0</v>
       </c>
       <c r="I89" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I89" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:I89" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I89">
+      <sortCondition ref="A2:A89"/>
+      <sortCondition ref="I2:I89"/>
+      <sortCondition ref="H2:H89"/>
+    </sortState>
+  </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:I86">
     <sortCondition ref="A3:A86"/>
     <sortCondition ref="I3:I86"/>

</xml_diff>

<commit_message>
Added END_COND and END_PARAM. END_COND adds extra conditions for ending a game; the goal and win conditions do not change. Defined end conditions for cleared own/opp holes, seeds limit, and limit on seeds for each hole. Added the game SimpleCapt. Moved the end game parameters on the editor window and gave them a label. Added a new rules source filter to play_mancala. Updated the excel macro for formatting props_used.csv due to the new parameters.
</commit_message>
<xml_diff>
--- a/src/game_params.xlsx
+++ b/src/game_params.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Activity_Data\Mancala_github\MancalaGames\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B45410C-65D0-46DB-A361-1C552A1E0C0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11FE6958-DDE1-4357-9547-89A7111EA2CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32145" yWindow="495" windowWidth="21885" windowHeight="15480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4665" yWindow="105" windowWidth="21885" windowHeight="15480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="game_params" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">game_params!$A$1:$I$89</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">game_params!$A$1:$I$92</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="535" uniqueCount="270">
   <si>
     <t>tab</t>
   </si>
@@ -823,6 +823,30 @@
   </si>
   <si>
     <t>sow_stores</t>
+  </si>
+  <si>
+    <t>end_cond</t>
+  </si>
+  <si>
+    <t>end_param</t>
+  </si>
+  <si>
+    <t>End Game Condition</t>
+  </si>
+  <si>
+    <t>End Cond Param</t>
+  </si>
+  <si>
+    <t>EndGameCond</t>
+  </si>
+  <si>
+    <t>NO_ADDTL</t>
+  </si>
+  <si>
+    <t>end_lbl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">End Game  </t>
   </si>
 </sst>
 </file>
@@ -1703,11 +1727,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:I89"/>
+  <dimension ref="A1:I92"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C69" sqref="C69"/>
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H24" sqref="H24:H36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1794,7 +1818,7 @@
         <v>16</v>
       </c>
       <c r="E3" s="1">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>32</v>
@@ -1936,7 +1960,7 @@
         <v>16</v>
       </c>
       <c r="E8" s="1">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>32</v>
@@ -1965,7 +1989,7 @@
         <v>16</v>
       </c>
       <c r="E9" s="1">
-        <v>151</v>
+        <v>192</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>91</v>
@@ -1994,7 +2018,7 @@
         <v>16</v>
       </c>
       <c r="E10" s="1">
-        <v>150</v>
+        <v>190</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>32</v>
@@ -2104,7 +2128,7 @@
         <v>16</v>
       </c>
       <c r="E14" s="1">
-        <v>124</v>
+        <v>146</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>8</v>
@@ -2188,7 +2212,7 @@
         <v>16</v>
       </c>
       <c r="E17" s="1">
-        <v>128</v>
+        <v>160</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>8</v>
@@ -2217,7 +2241,7 @@
         <v>16</v>
       </c>
       <c r="E18" s="1">
-        <v>130</v>
+        <v>162</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>211</v>
@@ -2246,7 +2270,7 @@
         <v>16</v>
       </c>
       <c r="E19" s="1">
-        <v>129</v>
+        <v>161</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>32</v>
@@ -2275,7 +2299,7 @@
         <v>16</v>
       </c>
       <c r="E20" s="1">
-        <v>123</v>
+        <v>145</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>32</v>
@@ -2359,7 +2383,7 @@
         <v>16</v>
       </c>
       <c r="E23" s="1">
-        <v>131</v>
+        <v>163</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>144</v>
@@ -2388,7 +2412,7 @@
         <v>16</v>
       </c>
       <c r="E24" s="1">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>47</v>
@@ -2417,7 +2441,7 @@
         <v>16</v>
       </c>
       <c r="E25" s="1">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>8</v>
@@ -2437,22 +2461,19 @@
         <v>29</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>16</v>
+        <v>175</v>
       </c>
       <c r="E26" s="1">
-        <v>147</v>
+        <v>0</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>207</v>
+        <v>174</v>
       </c>
       <c r="G26" s="5" t="s">
-        <v>208</v>
+        <v>71</v>
       </c>
       <c r="H26" s="1">
         <v>2</v>
@@ -2461,32 +2482,32 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B27" t="s">
-        <v>227</v>
-      </c>
-      <c r="C27" t="s">
-        <v>226</v>
-      </c>
-      <c r="D27" t="s">
-        <v>16</v>
-      </c>
-      <c r="E27">
-        <v>148</v>
-      </c>
-      <c r="F27" t="s">
-        <v>207</v>
-      </c>
-      <c r="G27" t="s">
-        <v>225</v>
-      </c>
-      <c r="H27">
+      <c r="B27" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E27" s="1">
+        <v>185</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G27" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="H27" s="1">
         <v>3</v>
       </c>
-      <c r="I27">
+      <c r="I27" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2495,19 +2516,22 @@
         <v>29</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>201</v>
+        <v>138</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>175</v>
+        <v>137</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="E28" s="1">
-        <v>0</v>
+        <v>164</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>174</v>
+        <v>139</v>
       </c>
       <c r="G28" s="5" t="s">
-        <v>71</v>
+        <v>132</v>
       </c>
       <c r="H28" s="1">
         <v>4</v>
@@ -2521,22 +2545,19 @@
         <v>29</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>49</v>
+        <v>202</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>16</v>
+        <v>203</v>
       </c>
       <c r="E29" s="1">
-        <v>143</v>
+        <v>0</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>51</v>
+        <v>174</v>
       </c>
       <c r="G29" s="5" t="s">
-        <v>52</v>
+        <v>71</v>
       </c>
       <c r="H29" s="1">
         <v>5</v>
@@ -2550,22 +2571,22 @@
         <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>138</v>
+        <v>53</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>137</v>
+        <v>54</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E30" s="1">
-        <v>132</v>
+        <v>142</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>139</v>
+        <v>8</v>
       </c>
       <c r="G30" s="5" t="s">
-        <v>132</v>
+        <v>55</v>
       </c>
       <c r="H30" s="1">
         <v>6</v>
@@ -2579,19 +2600,22 @@
         <v>29</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>202</v>
+        <v>129</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>203</v>
+        <v>130</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="E31" s="1">
-        <v>0</v>
+        <v>101</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>174</v>
+        <v>131</v>
       </c>
       <c r="G31" s="5" t="s">
-        <v>71</v>
+        <v>132</v>
       </c>
       <c r="H31" s="1">
         <v>7</v>
@@ -2605,22 +2629,19 @@
         <v>29</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>53</v>
+        <v>268</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>16</v>
+        <v>269</v>
       </c>
       <c r="E32" s="1">
-        <v>119</v>
+        <v>0</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>8</v>
+        <v>174</v>
       </c>
       <c r="G32" s="5" t="s">
-        <v>55</v>
+        <v>71</v>
       </c>
       <c r="H32" s="1">
         <v>8</v>
@@ -2634,22 +2655,22 @@
         <v>29</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>129</v>
+        <v>262</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>130</v>
+        <v>264</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E33" s="1">
-        <v>101</v>
+        <v>118</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>131</v>
+        <v>266</v>
       </c>
       <c r="G33" s="5" t="s">
-        <v>132</v>
+        <v>267</v>
       </c>
       <c r="H33" s="1">
         <v>9</v>
@@ -2663,28 +2684,28 @@
         <v>29</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>42</v>
+        <v>263</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>43</v>
+        <v>265</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E34" s="1">
-        <v>144</v>
+        <v>119</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="G34" s="5" t="s">
-        <v>44</v>
+        <v>71</v>
       </c>
       <c r="H34" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="I34" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
@@ -2692,54 +2713,57 @@
         <v>29</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>40</v>
+        <v>206</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>41</v>
+        <v>228</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E35" s="1">
-        <v>127</v>
+        <v>188</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>32</v>
+        <v>207</v>
       </c>
       <c r="G35" s="5" t="s">
-        <v>33</v>
+        <v>208</v>
       </c>
       <c r="H35" s="1">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="I35" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>29</v>
       </c>
-      <c r="B36" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>204</v>
+      <c r="B36" t="s">
+        <v>227</v>
+      </c>
+      <c r="C36" t="s">
+        <v>226</v>
+      </c>
+      <c r="D36" t="s">
+        <v>16</v>
       </c>
       <c r="E36" s="1">
-        <v>0</v>
-      </c>
-      <c r="F36" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="G36" s="5" t="s">
-        <v>71</v>
+        <v>189</v>
+      </c>
+      <c r="F36" t="s">
+        <v>207</v>
+      </c>
+      <c r="G36" t="s">
+        <v>225</v>
       </c>
       <c r="H36" s="1">
-        <v>2</v>
-      </c>
-      <c r="I36" s="1">
-        <v>2</v>
+        <v>12</v>
+      </c>
+      <c r="I36">
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
@@ -2747,25 +2771,25 @@
         <v>29</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E37" s="1">
-        <v>125</v>
+        <v>186</v>
       </c>
       <c r="F37" s="1" t="s">
         <v>32</v>
       </c>
       <c r="G37" s="5" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="H37" s="1">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I37" s="1">
         <v>2</v>
@@ -2776,16 +2800,16 @@
         <v>29</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E38" s="1">
-        <v>126</v>
+        <v>149</v>
       </c>
       <c r="F38" s="1" t="s">
         <v>32</v>
@@ -2794,7 +2818,7 @@
         <v>33</v>
       </c>
       <c r="H38" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I38" s="1">
         <v>2</v>
@@ -2805,25 +2829,22 @@
         <v>29</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>95</v>
+        <v>205</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>16</v>
+        <v>204</v>
       </c>
       <c r="E39" s="1">
-        <v>117</v>
+        <v>0</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>97</v>
+        <v>174</v>
       </c>
       <c r="G39" s="5" t="s">
-        <v>98</v>
+        <v>71</v>
       </c>
       <c r="H39" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="I39" s="1">
         <v>2</v>
@@ -2834,22 +2855,25 @@
         <v>29</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>176</v>
+        <v>30</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>200</v>
+        <v>31</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="E40" s="1">
-        <v>0</v>
+        <v>147</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>174</v>
+        <v>32</v>
       </c>
       <c r="G40" s="5" t="s">
-        <v>71</v>
+        <v>33</v>
       </c>
       <c r="H40" s="1">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="I40" s="1">
         <v>2</v>
@@ -2860,25 +2884,25 @@
         <v>29</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>34</v>
+        <v>56</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>35</v>
+        <v>57</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E41" s="1">
-        <v>136</v>
+        <v>148</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="G41" s="5" t="s">
-        <v>167</v>
+        <v>33</v>
       </c>
       <c r="H41" s="1">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="I41" s="1">
         <v>2</v>
@@ -2889,25 +2913,25 @@
         <v>29</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>36</v>
+        <v>95</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>37</v>
+        <v>96</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E42" s="1">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>38</v>
+        <v>97</v>
       </c>
       <c r="G42" s="5" t="s">
-        <v>39</v>
+        <v>98</v>
       </c>
       <c r="H42" s="1">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="I42" s="1">
         <v>2</v>
@@ -2918,25 +2942,22 @@
         <v>29</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>148</v>
+        <v>176</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>16</v>
+        <v>200</v>
       </c>
       <c r="E43" s="1">
-        <v>134</v>
+        <v>0</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>150</v>
+        <v>174</v>
       </c>
       <c r="G43" s="5" t="s">
-        <v>157</v>
+        <v>71</v>
       </c>
       <c r="H43" s="1">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="I43" s="1">
         <v>2</v>
@@ -2947,25 +2968,25 @@
         <v>29</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>68</v>
+        <v>34</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>69</v>
+        <v>35</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E44" s="1">
-        <v>102</v>
+        <v>168</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="G44" s="5" t="s">
-        <v>33</v>
+        <v>167</v>
       </c>
       <c r="H44" s="1">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="I44" s="1">
         <v>2</v>
@@ -2973,113 +2994,115 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>10</v>
+        <v>37</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="E45" s="1">
-        <v>1</v>
+        <v>167</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>108</v>
+        <v>38</v>
       </c>
       <c r="G45" s="5" t="s">
-        <v>13</v>
+        <v>39</v>
       </c>
       <c r="H45" s="1">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="I45" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E46" s="1">
+        <v>166</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="G46" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="H46" s="1">
         <v>9</v>
       </c>
-      <c r="B46" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E46" s="1">
-        <v>2</v>
-      </c>
-      <c r="F46" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G46" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="H46" s="1">
-        <v>2</v>
-      </c>
       <c r="I46" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>17</v>
+        <v>68</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>18</v>
+        <v>69</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E47" s="1">
-        <v>118</v>
+        <v>102</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G47" s="5"/>
+        <v>32</v>
+      </c>
+      <c r="G47" s="5" t="s">
+        <v>33</v>
+      </c>
       <c r="H47" s="1">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="I47" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="E48" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G48" s="6" t="s">
-        <v>107</v>
+        <v>108</v>
+      </c>
+      <c r="G48" s="5" t="s">
+        <v>13</v>
       </c>
       <c r="H48" s="1">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I48" s="1">
         <v>0</v>
@@ -3090,28 +3113,28 @@
         <v>9</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="E49" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="G49" s="5" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="H49" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I49" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
@@ -3119,54 +3142,52 @@
         <v>9</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="E50" s="1">
+        <v>141</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G50" s="5"/>
+      <c r="H50" s="1">
         <v>3</v>
       </c>
-      <c r="F50" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G50" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="H50" s="1">
-        <v>2</v>
-      </c>
       <c r="I50" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>101</v>
+        <v>9</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>109</v>
+        <v>19</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>110</v>
+        <v>20</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>106</v>
+        <v>16</v>
       </c>
       <c r="E51" s="1">
-        <v>201</v>
+        <v>5</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="G51" s="1" t="s">
-        <v>111</v>
+        <v>21</v>
+      </c>
+      <c r="G51" s="6" t="s">
+        <v>107</v>
       </c>
       <c r="H51" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I51" s="1">
         <v>0</v>
@@ -3174,60 +3195,60 @@
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>101</v>
+        <v>9</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>104</v>
+        <v>14</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>105</v>
+        <v>15</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>106</v>
+        <v>16</v>
       </c>
       <c r="E52" s="1">
-        <v>203</v>
+        <v>4</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="G52" s="5" t="s">
-        <v>55</v>
+        <v>13</v>
       </c>
       <c r="H52" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I52" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>101</v>
+        <v>9</v>
       </c>
       <c r="B5